<commit_message>
vault backup: 2024-09-18 20:32:39
</commit_message>
<xml_diff>
--- a/_system/Attachments/Portfolio Management.xlsx
+++ b/_system/Attachments/Portfolio Management.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martin/repos/tomesink/obsidian/_system/Attachments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{010C367C-EB6F-BB45-A4A6-FC5EC464A06E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2A66AF8-9D5C-0842-8C8E-8B2C6B2E771A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41600" yWindow="1560" windowWidth="31860" windowHeight="18860" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="39000" yWindow="1720" windowWidth="31860" windowHeight="18860" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Stocks Performance" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
       </extLst>
     </bk>
   </futureMetadata>
-  <futureMetadata name="XLRICHVALUE" count="20">
+  <futureMetadata name="XLRICHVALUE" count="24">
     <bk>
       <extLst>
         <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
@@ -197,13 +197,41 @@
         </ext>
       </extLst>
     </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="61"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="64"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="67"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="70"/>
+        </ext>
+      </extLst>
+    </bk>
   </futureMetadata>
   <cellMetadata count="1">
     <bk>
       <rc t="1" v="0"/>
     </bk>
   </cellMetadata>
-  <valueMetadata count="20">
+  <valueMetadata count="24">
     <bk>
       <rc t="2" v="0"/>
     </bk>
@@ -263,6 +291,18 @@
     </bk>
     <bk>
       <rc t="2" v="19"/>
+    </bk>
+    <bk>
+      <rc t="2" v="20"/>
+    </bk>
+    <bk>
+      <rc t="2" v="21"/>
+    </bk>
+    <bk>
+      <rc t="2" v="22"/>
+    </bk>
+    <bk>
+      <rc t="2" v="23"/>
     </bk>
   </valueMetadata>
 </metadata>
@@ -791,7 +831,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="11">
+  <numFmts count="12">
     <numFmt numFmtId="164" formatCode="[$$-409]\ #,##0.00"/>
     <numFmt numFmtId="165" formatCode="[$£-809]\ #,##0.00"/>
     <numFmt numFmtId="166" formatCode="[$$-409]\ #,##0"/>
@@ -803,6 +843,7 @@
     <numFmt numFmtId="172" formatCode="#,##0.00\ &quot;CZK&quot;"/>
     <numFmt numFmtId="173" formatCode="[$$-409]#,##0.00"/>
     <numFmt numFmtId="174" formatCode="0.0000"/>
+    <numFmt numFmtId="180" formatCode="[$$-409]\ #,##0.0000"/>
   </numFmts>
   <fonts count="14">
     <font>
@@ -891,7 +932,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="30">
+  <fills count="31">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1066,8 +1107,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="41">
+  <borders count="42">
     <border>
       <left/>
       <right/>
@@ -1609,12 +1656,25 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="207">
+  <cellXfs count="219">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -2028,9 +2088,6 @@
     <xf numFmtId="173" fontId="11" fillId="28" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="11" fillId="14" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="1" fontId="9" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2114,92 +2171,51 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="14" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="173" fontId="11" fillId="14" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="30" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="173" fontId="11" fillId="30" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="15" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="29" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="174" fontId="11" fillId="14" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="11" fillId="30" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Per cent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="20">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -2564,6 +2580,86 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0"/>
@@ -4507,7 +4603,7 @@
 </file>
 
 <file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
-<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="59">
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="71">
   <rv s="0">
     <v>https://www.bing.com/financeapi/forcetrigger?t=a1qlnm&amp;q=XNYS%3aCVS&amp;form=skydnc</v>
     <v>Learn more on Bing</v>
@@ -4526,11 +4622,9 @@
     <v>Powered by Refinitiv</v>
     <v>83.25</v>
     <v>52.770499999999998</v>
-    <v>0.52559999999999996</v>
-    <v>0.45</v>
-    <v>7.8220000000000008E-3</v>
-    <v>-0.06</v>
-    <v>-1.0349999999999999E-3</v>
+    <v>0.52610000000000001</v>
+    <v>0.97</v>
+    <v>1.6773E-2</v>
     <v>USD</v>
     <v>CVS Health Corporation is a health solutions company. The Company operates in four segments: Health Care Benefits, Health Services, Pharmacy &amp; Consumer Wellness, and Corporate/Other. Its Health Care Benefits segment offer a range of traditional, voluntary and consumer-directed health insurance products and related services, including medical, pharmacy, dental and behavioral health plans, medical management capabilities, Medicare Advantage and Medicare supplement plans, and Medicaid health care management services. Its Health Services segment provides a full range of pharmacy benefit management solutions, delivers health care services in its medical clinics, virtually, and in the home, and offers provider enablement solutions. The Pharmacy &amp; Consumer Wellness segment dispenses prescriptions in its retail pharmacies and through its infusion operations, provides ancillary pharmacy services, including pharmacy patient care programs, diagnostic testing and vaccination administration.</v>
     <v>300000</v>
@@ -4538,25 +4632,24 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>1 Cvs Dr, WOONSOCKET, RI, 02895-6146 US</v>
-    <v>58.27</v>
+    <v>59.19</v>
     <v>Healthcare Providers &amp; Services</v>
     <v>Stock</v>
-    <v>45548.998426978906</v>
+    <v>45553.772598205469</v>
     <v>0</v>
-    <v>57.1</v>
-    <v>72937640000</v>
+    <v>57.746299999999998</v>
+    <v>73969165200</v>
     <v>CVS HEALTH CORPORATION</v>
     <v>CVS HEALTH CORPORATION</v>
-    <v>57.56</v>
-    <v>10.3178</v>
-    <v>57.53</v>
-    <v>57.98</v>
-    <v>57.92</v>
+    <v>57.93</v>
+    <v>10.2911</v>
+    <v>57.83</v>
+    <v>58.8</v>
     <v>1257979000</v>
     <v>CVS</v>
     <v>CVS HEALTH CORPORATION (XNYS:CVS)</v>
-    <v>7429524</v>
-    <v>8087086</v>
+    <v>2693781</v>
+    <v>7701146</v>
     <v>1996</v>
   </rv>
   <rv s="2">
@@ -4580,11 +4673,9 @@
     <v>Powered by Refinitiv</v>
     <v>165.32</v>
     <v>74</v>
-    <v>2.0085000000000002</v>
-    <v>1.04</v>
-    <v>8.1419999999999999E-3</v>
-    <v>0.81</v>
-    <v>6.2900000000000005E-3</v>
+    <v>2.0015999999999998</v>
+    <v>3.57</v>
+    <v>2.5788999999999999E-2</v>
     <v>USD</v>
     <v>Crocs, Inc. is engaged in the design, development, worldwide marketing, distribution, and sale of casual lifestyle footwear and accessories for women, men, and children. The Company’s segments include Crocs Brand and the HEYDUDE Brand. The Company’s Crocs Brand collection contains Croslite material, a molded footwear technology, delivering extraordinary comfort with each step. Its Croslite materials are formulated to create soft, comfortable, lightweight, non-marking, and odor-resistant footwear. The HEYDUDE Brand offers shoes with a versatile silhouette. It sells its products in more than 80 countries, through two distribution channels: wholesale and direct-to-consumer. Its wholesale channel includes domestic and international multi-brand retailers, mono-branded partner stores, e-tailers, and distributors; its direct-to-consumer channel includes Company-operated retail stores, Company-operated e-commerce sites, and third-party marketplaces.</v>
     <v>7030</v>
@@ -4592,25 +4683,24 @@
     <v>XNAS</v>
     <v>XNAS</v>
     <v>500 Eldorado Boulevard, Building 5, BROOMFIELD, CO, 80021 US</v>
-    <v>131.08000000000001</v>
+    <v>142</v>
     <v>Textiles &amp; Apparel</v>
     <v>Stock</v>
-    <v>45548.963085925781</v>
+    <v>45553.772601642966</v>
     <v>3</v>
-    <v>128.56479999999999</v>
-    <v>7647023000</v>
+    <v>138.2998</v>
+    <v>8432688460</v>
     <v>CROCS, INC.</v>
     <v>CROCS, INC.</v>
-    <v>128.6</v>
-    <v>9.6844999999999999</v>
-    <v>127.73</v>
-    <v>128.77000000000001</v>
-    <v>129.58000000000001</v>
+    <v>138.53</v>
+    <v>10.5366</v>
+    <v>138.43</v>
+    <v>142</v>
     <v>59385130</v>
     <v>CROX</v>
     <v>CROCS, INC. (XNAS:CROX)</v>
-    <v>825808</v>
-    <v>939591</v>
+    <v>442719</v>
+    <v>961370</v>
     <v>2005</v>
   </rv>
   <rv s="2">
@@ -4634,11 +4724,9 @@
     <v>Powered by Refinitiv</v>
     <v>30.07</v>
     <v>17.71</v>
-    <v>1.5169999999999999</v>
-    <v>0.54</v>
-    <v>2.8739000000000001E-2</v>
-    <v>0</v>
-    <v>0</v>
+    <v>1.5156000000000001</v>
+    <v>0.28999999999999998</v>
+    <v>1.4736000000000001E-2</v>
     <v>USD</v>
     <v>Wabash National Corporation provides connected solutions for the transportation, logistics and distribution industries. The Company designs and manufactures products including dry freight and refrigerated trailers, platform trailers, tank trailers, dry and refrigerated truck bodies, structural composite panels and products, transportation, logistics, and distribution industry parts and services, and specialty food grade processing equipment. The Company’s Transportation Solutions (TS) segment comprises the design and manufacturing operations for the Company’s transportation-related equipment and products. This includes dry and refrigerated van trailers, platform trailers, tank trailers and truck-mounted tanks, truck-mounted dry and refrigerated truck bodies and EcoNex technology products. Its Parts &amp; Services (P&amp;S) segment is comprised of the Company’s parts and services businesses as well as the upfitting component of truck bodies business. It also includes DuraPlate composite panels.</v>
     <v>6700</v>
@@ -4646,25 +4734,24 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>3900 Mccarty Lane, LAFAYETTE, IN, 47905 US</v>
-    <v>19.420000000000002</v>
+    <v>20.149699999999999</v>
     <v>Machinery, Equipment &amp; Components</v>
     <v>Stock</v>
-    <v>45548.958333333336</v>
+    <v>45553.772564513281</v>
     <v>6</v>
-    <v>19</v>
-    <v>850505100</v>
+    <v>19.355</v>
+    <v>878664623</v>
     <v>WABASH NATIONAL CORPORATION</v>
     <v>WABASH NATIONAL CORPORATION</v>
-    <v>19.07</v>
-    <v>5.9295999999999998</v>
-    <v>18.79</v>
-    <v>19.329999999999998</v>
-    <v>19.329999999999998</v>
+    <v>19.600000000000001</v>
+    <v>6.0369000000000002</v>
+    <v>19.68</v>
+    <v>19.97</v>
     <v>43999230</v>
     <v>WNC</v>
     <v>WABASH NATIONAL CORPORATION (XNYS:WNC)</v>
-    <v>265192</v>
-    <v>468634</v>
+    <v>204670</v>
+    <v>437924</v>
     <v>1991</v>
   </rv>
   <rv s="2">
@@ -4688,11 +4775,9 @@
     <v>Powered by Refinitiv</v>
     <v>26.4</v>
     <v>16.12</v>
-    <v>1.0354000000000001</v>
-    <v>0.46</v>
-    <v>2.1187999999999999E-2</v>
-    <v>0</v>
-    <v>0</v>
+    <v>1.0365</v>
+    <v>0.18</v>
+    <v>8.2120000000000005E-3</v>
     <v>USD</v>
     <v>Perdoceo Education Corporation, through its academic institutions, offers quality postsecondary education primarily online to a diverse student population, along with campus-based and blended learning programs. The Company's academic institutions include Colorado Technical University (CTU) and the American InterContinental University System (AIUS), which provides degree programs from the associate through doctoral level as well as non-degree seeking and professional development programs. Its academic institutions offer students industry-relevant and career-focused academic programs. CTU offers academic programs in the career-oriented disciplines of business and management, nursing, healthcare management, computer science, engineering, information systems and technology, project management, cybersecurity and criminal justice. AIUS offers academic programs in the career-oriented disciplines of business studies, information technologies, education, health sciences and criminal justice.</v>
     <v>2319</v>
@@ -4700,25 +4785,24 @@
     <v>XNAS</v>
     <v>XNAS</v>
     <v>1750 E. GOLF ROAD, SCHAUMBURG, IL, 60173 US</v>
-    <v>22.3</v>
+    <v>22.11</v>
     <v>Miscellaneous Educational Service Providers</v>
     <v>Stock</v>
-    <v>45548.901013274997</v>
+    <v>45553.772572152346</v>
     <v>9</v>
-    <v>21.73</v>
-    <v>1455980000</v>
+    <v>21.68</v>
+    <v>1451382803</v>
     <v>PERDOCEO EDUCATION CORPORATION</v>
     <v>PERDOCEO EDUCATION CORPORATION</v>
-    <v>21.82</v>
-    <v>10.669499999999999</v>
-    <v>21.71</v>
-    <v>22.17</v>
-    <v>22.17</v>
+    <v>21.87</v>
+    <v>10.7727</v>
+    <v>21.92</v>
+    <v>22.1</v>
     <v>65673430</v>
     <v>PRDO</v>
     <v>PERDOCEO EDUCATION CORPORATION (XNAS:PRDO)</v>
-    <v>388222</v>
-    <v>364633</v>
+    <v>111589</v>
+    <v>378012</v>
     <v>1994</v>
   </rv>
   <rv s="2">
@@ -4742,11 +4826,9 @@
     <v>Powered by Refinitiv</v>
     <v>237.23</v>
     <v>164.07499999999999</v>
-    <v>1.2438</v>
-    <v>-0.27</v>
-    <v>-1.212E-3</v>
-    <v>-0.25</v>
-    <v>-1.124E-3</v>
+    <v>1.2459</v>
+    <v>4.66</v>
+    <v>2.1495E-2</v>
     <v>USD</v>
     <v>Apple Inc. designs, manufactures and markets smartphones, personal computers, tablets, wearables and accessories, and sells a variety of related services. Its product categories include iPhone, Mac, iPad, and Wearables, Home and Accessories. Its software platforms include iOS, iPadOS, macOS, watchOS, and tvOS. Its services include advertising, AppleCare, cloud services, digital content and payment services. It operates various platforms, including the App Store, that allow customers to discover and download applications and digital content, such as books, music, video, games and podcasts. It also offers digital content through subscription-based services, including Apple Arcade, Apple Fitness+, Apple Music, Apple News+ and Apple TV+. Its products include iPhone 15 Pro, iPhone 15, iPhone 14, iPhone 13, MacBook Air, MacBook Pro, iMac, Mac mini, Mac Studio, Mac Pro, and others. It also provides DarwinAI, which specializes in visual quality inspection using its Explainable AI platform.</v>
     <v>161000</v>
@@ -4754,25 +4836,24 @@
     <v>XNAS</v>
     <v>XNAS</v>
     <v>One Apple Park Way, CUPERTINO, CA, 95014 US</v>
-    <v>224.04</v>
+    <v>222.7</v>
     <v>Computers, Phones &amp; Household Electronics</v>
     <v>Stock</v>
-    <v>45548.999825034378</v>
+    <v>45553.772621296092</v>
     <v>12</v>
-    <v>221.91</v>
-    <v>3382921000000</v>
+    <v>217.54</v>
+    <v>3366956803000</v>
     <v>APPLE INC.</v>
     <v>APPLE INC.</v>
-    <v>223.58</v>
-    <v>33.876899999999999</v>
-    <v>222.77</v>
-    <v>222.5</v>
-    <v>222.25</v>
+    <v>217.59</v>
+    <v>33.0075</v>
+    <v>216.79</v>
+    <v>221.45</v>
     <v>15204140000</v>
     <v>AAPL</v>
     <v>APPLE INC. (XNAS:AAPL)</v>
-    <v>36766619</v>
-    <v>43271897</v>
+    <v>36917458</v>
+    <v>43841997</v>
     <v>1977</v>
   </rv>
   <rv s="2">
@@ -4796,11 +4877,9 @@
     <v>Powered by Refinitiv</v>
     <v>92.82</v>
     <v>50.134999999999998</v>
-    <v>0.99360000000000004</v>
-    <v>1.24</v>
-    <v>1.4395E-2</v>
-    <v>0.46</v>
-    <v>5.2639999999999996E-3</v>
+    <v>0.99219999999999997</v>
+    <v>1.21</v>
+    <v>1.3677999999999999E-2</v>
     <v>USD</v>
     <v>Allison Transmission Holdings, Inc. is a designer and manufacturer of propulsion solutions for commercial and defense vehicles. The Company is also a manufacturer of medium-and heavy-duty fully automatic transmissions. Its products are used in a variety of applications, including on-highway trucks, including distribution, refuse, construction, fire and emergency; buses, including school, transit and coach; motorhomes, off-highway vehicles, and equipment, including energy, mining and construction applications; and defense vehicles, including tactical wheeled and tracked. The Company operates in approximately 150 countries. The Company has manufacturing facilities in the United States, Hungary and India, as well as global engineering resources, including electrification engineering centers in Indianapolis, Indiana, Auburn Hills, Michigan and London in the United Kingdom. The Company also has approximately 1,600 independent distributor and dealer locations worldwide.</v>
     <v>3700</v>
@@ -4808,25 +4887,24 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>One Allison Way, INDIANAPOLIS, IN, 46222 US</v>
-    <v>87.92</v>
+    <v>90.064999999999998</v>
     <v>Machinery, Equipment &amp; Components</v>
     <v>Stock</v>
-    <v>45548.997911226565</v>
+    <v>45553.772465751565</v>
     <v>15</v>
-    <v>86.37</v>
-    <v>7614108000</v>
+    <v>88.305000000000007</v>
+    <v>7813653699</v>
     <v>ALLISON TRANSMISSION HOLDINGS, INC.</v>
     <v>ALLISON TRANSMISSION HOLDINGS, INC.</v>
-    <v>86.98</v>
-    <v>11.425800000000001</v>
-    <v>86.14</v>
-    <v>87.38</v>
-    <v>87.84</v>
+    <v>88.305000000000007</v>
+    <v>11.5671</v>
+    <v>88.46</v>
+    <v>89.67</v>
     <v>87137880</v>
     <v>ALSN</v>
     <v>ALLISON TRANSMISSION HOLDINGS, INC. (XNYS:ALSN)</v>
-    <v>479952</v>
-    <v>457093</v>
+    <v>158187</v>
+    <v>484816</v>
     <v>2007</v>
   </rv>
   <rv s="2">
@@ -4850,11 +4928,9 @@
     <v>Powered by Refinitiv</v>
     <v>40.695</v>
     <v>18</v>
-    <v>2.0053999999999998</v>
-    <v>0.35</v>
-    <v>1.9074000000000001E-2</v>
-    <v>0</v>
-    <v>0</v>
+    <v>2.0013999999999998</v>
+    <v>0.4</v>
+    <v>2.0619000000000002E-2</v>
     <v>USD</v>
     <v>Par Pacific Holdings, Inc. is an energy company, which provides both renewable and conventional fuels to the western United States. It owns and operates 125,000 barrels per day of combined refining capacity across three locations and an energy infrastructure network, including 7.6 million barrels of storage, and marine, rail, rack and pipeline assets. The Company has three segments. Refining segment owns and operates four refineries with total operating crude oil throughput capacity of 219 thousand barrels per day (Mbpd). Retail segment operates fuel retail outlets in Hawaii, Washington and Idaho. It operates convenience stores and fuel retail sites under Hele and nomnom brands, 76 branded fuel retail sites and other sites operated by third parties that sell gasoline, diesel, and retail merchandise, such as soft drinks, prepared foods, and other sundries. Logistics segment operates a multi-modal logistics network spanning the Pacific, the Northwest, and the Rocky Mountain regions.</v>
     <v>1814</v>
@@ -4862,25 +4938,24 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>825 Town and Country Ln Ste 1500, HOUSTON, TX, 77024-2235 US</v>
-    <v>19.09</v>
+    <v>19.920000000000002</v>
     <v>Oil &amp; Gas</v>
     <v>Stock</v>
-    <v>45548.958333356248</v>
+    <v>45553.772527106252</v>
     <v>18</v>
-    <v>18.504000000000001</v>
-    <v>1053387000</v>
+    <v>19.215</v>
+    <v>1115351226</v>
     <v>PAR PACIFIC HOLDINGS, INC.</v>
     <v>PAR PACIFIC HOLDINGS, INC.</v>
-    <v>18.57</v>
-    <v>3.2581000000000002</v>
-    <v>18.350000000000001</v>
-    <v>18.7</v>
-    <v>18.7</v>
+    <v>19.47</v>
+    <v>3.3801000000000001</v>
+    <v>19.399999999999999</v>
+    <v>19.8</v>
     <v>56330870</v>
     <v>PARR</v>
     <v>PAR PACIFIC HOLDINGS, INC. (XNYS:PARR)</v>
-    <v>757582</v>
-    <v>950341</v>
+    <v>279093</v>
+    <v>917565</v>
     <v>2005</v>
   </rv>
   <rv s="2">
@@ -4904,11 +4979,9 @@
     <v>Powered by Refinitiv</v>
     <v>84.44</v>
     <v>38.5</v>
-    <v>1.3117000000000001</v>
-    <v>1.93</v>
-    <v>3.3419999999999998E-2</v>
-    <v>0</v>
-    <v>0</v>
+    <v>1.3098000000000001</v>
+    <v>1.78</v>
+    <v>2.9238E-2</v>
     <v>USD</v>
     <v>Hyster-Yale, Inc., formerly Hyster-Yale Materials Handling, Inc., through its wholly owned operating subsidiary, Hyster-Yale Materials Handling, designs, engineers, manufactures, sells, and services a comprehensive line of lift trucks, attachments, aftermarket parts and technology solutions marketed globally primarily under the Hyster and Yale brand names. The Company's business segments include Lift Trucks, Attachments and Fuel Cells. The Hyster-Yale Maximal brand provides trucks for customers requiring fundamental lift truck performance. The Lift Truck segment is focused on fuel cell-powered battery box replacements and integrated fuel cell engine solutions. Hyster- Yale’s attachment subsidiary, Bolzoni S.p.A., is a producer of attachments, forks, and lift tables under the Bolzoni, Auramo and Meyer brand names. The Fuel Cell business, Nuvera Fuel Cells, is an alternative-power technology company focused on fuel cell stacks and engines.</v>
     <v>8600</v>
@@ -4916,25 +4989,24 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>5875 LANDERBROOK DRIVE, SUITE 300, CLEVELAND, OH, 44124 US</v>
-    <v>60.54</v>
+    <v>62.66</v>
     <v>Machinery, Equipment &amp; Components</v>
     <v>Stock</v>
-    <v>45548.958333378905</v>
+    <v>45553.772321087497</v>
     <v>21</v>
-    <v>58.15</v>
-    <v>1044469000</v>
+    <v>59.82</v>
+    <v>1096622059</v>
     <v>HYSTER-YALE, INC.</v>
     <v>HYSTER-YALE, INC.</v>
-    <v>58.78</v>
-    <v>5.9679000000000002</v>
-    <v>57.75</v>
-    <v>59.68</v>
-    <v>59.68</v>
+    <v>60.7</v>
+    <v>6.0879000000000003</v>
+    <v>60.88</v>
+    <v>62.66</v>
     <v>17501150</v>
     <v>HY</v>
     <v>HYSTER-YALE, INC. (XNYS:HY)</v>
-    <v>62412</v>
-    <v>72174</v>
+    <v>23166</v>
+    <v>66473</v>
     <v>1999</v>
   </rv>
   <rv s="2">
@@ -4958,11 +5030,9 @@
     <v>Powered by Refinitiv</v>
     <v>108.02</v>
     <v>71.900000000000006</v>
-    <v>1.5121</v>
-    <v>3.65</v>
-    <v>4.6824999999999999E-2</v>
-    <v>2.2799999999999998</v>
-    <v>2.7940999999999997E-2</v>
+    <v>1.5088999999999999</v>
+    <v>0.41</v>
+    <v>4.8449999999999995E-3</v>
     <v>USD</v>
     <v>Polaris Inc. is engaged in designing, engineering, manufacturing and marketing of powersports vehicles. The Company also designs and manufactures or sources parts, garments and accessories (PG&amp;A), which includes aftermarket accessories and apparel. The Company operates through three segments: Off Road, On Road and Marine. The Off Road segment consists of off-road vehicles and snowmobiles. The On Road segment designs and manufactures motorcycles, moto-roadsters, light duty hauling, and passenger vehicles. The Marine segment designs and manufactures boats that are designed to compete in key segments of the recreational marine industry, specifically pontoon and deck boats. Its product line-up includes the RANGER, RZR and Polaris XPEDITION and GENERAL side-by-side off-road vehicles; Sportsman all-terrain off-road vehicles; military and commercial off-road vehicles; snowmobiles; Indian Motorcycle mid-size and heavyweight motorcycles; Slingshot moto-roadsters, and pontoon and deck boats.</v>
     <v>18500</v>
@@ -4970,25 +5040,24 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>2100 HIGHWAY 55, MEDINA, MN, 55340-9770 US</v>
-    <v>82.7</v>
+    <v>85.47</v>
     <v>Leisure Products</v>
     <v>Stock</v>
-    <v>45548.958333356248</v>
+    <v>45553.772465798436</v>
     <v>24</v>
-    <v>78.39</v>
-    <v>4549040000</v>
+    <v>82.93</v>
+    <v>4740812471</v>
     <v>Polaris Inc.</v>
     <v>Polaris Inc.</v>
-    <v>78.77</v>
-    <v>14.2927</v>
-    <v>77.95</v>
-    <v>81.599999999999994</v>
-    <v>83.88</v>
+    <v>84.9</v>
+    <v>14.6676</v>
+    <v>84.63</v>
+    <v>85.04</v>
     <v>55748030</v>
     <v>PII</v>
     <v>Polaris Inc. (XNYS:PII)</v>
-    <v>779786</v>
-    <v>448085</v>
+    <v>197216</v>
+    <v>473923</v>
     <v>1994</v>
   </rv>
   <rv s="2">
@@ -5012,11 +5081,9 @@
     <v>Powered by Refinitiv</v>
     <v>114.29989999999999</v>
     <v>75.430000000000007</v>
-    <v>1.7417</v>
-    <v>2.78</v>
-    <v>2.9691000000000002E-2</v>
-    <v>-0.68</v>
-    <v>-7.0530000000000002E-3</v>
+    <v>1.7418</v>
+    <v>1.1200000000000001</v>
+    <v>1.1699999999999999E-2</v>
     <v>USD</v>
     <v>CONSOL Energy Inc. is a producer and exporter of high-Btu bituminous thermal coal and metallurgical coal. It owns and operates longwall mining operations in the Northern Appalachian Basin. Its flagship operation is the Pennsylvania Mining Complex, located over 26 miles southwest of Pittsburgh, near the city of Washington and the borough of Waynesburg all in Pennsylvania, and consists of three deep longwall mining operations: the Bailey Mine, the Enlow Fork Mine and the Harvey Mine, as well as a centralized preparation plant. Its segments include the PAMC and the CONSOL Marine Terminal. The PAMC includes the Bailey Mine, the Enlow Fork Mine, the Harvey Mine and a centralized preparation plant. The PAMC segment's principal activities include the mining, preparation and marketing of bituminous coal, sold primarily to industrial end-users, metallurgical end-users and power generators. The CONSOL Marine Terminal segment provides coal export terminal services through the Port of Baltimore.</v>
     <v>2020</v>
@@ -5024,25 +5091,24 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>275 TECHNOLOGY DRIVE, SUITE #101, CANONSBURG, PA, 15317 US</v>
-    <v>97.95</v>
+    <v>96.85</v>
     <v>Coal</v>
     <v>Stock</v>
-    <v>45548.958333356248</v>
+    <v>45553.77259641172</v>
     <v>27</v>
-    <v>94.42</v>
-    <v>2833801000</v>
+    <v>93.41</v>
+    <v>2846734325</v>
     <v>CONSOL ENERGY INC.</v>
     <v>CONSOL ENERGY INC.</v>
-    <v>95</v>
-    <v>7.1966000000000001</v>
-    <v>93.63</v>
-    <v>96.41</v>
+    <v>95.86</v>
+    <v>7.1458000000000004</v>
     <v>95.73</v>
+    <v>96.85</v>
     <v>29393230</v>
     <v>CEIX</v>
     <v>CONSOL ENERGY INC. (XNYS:CEIX)</v>
-    <v>247822</v>
-    <v>512011</v>
+    <v>157351</v>
+    <v>487441</v>
     <v>2017</v>
   </rv>
   <rv s="2">
@@ -5066,11 +5132,9 @@
     <v>Powered by Refinitiv</v>
     <v>127.3484</v>
     <v>84.35</v>
-    <v>1.2484999999999999</v>
-    <v>1.61</v>
-    <v>1.8024999999999999E-2</v>
-    <v>-1.6080000000000001</v>
-    <v>-1.7683999999999998E-2</v>
+    <v>1.2470000000000001</v>
+    <v>2.54</v>
+    <v>2.7397000000000001E-2</v>
     <v>USD</v>
     <v>AGCO Corporation is a designer, manufacturer and distributor of agricultural machinery and precision agriculture technology. The Company sells a range of agricultural equipment, including tractors, combines, self-propelled sprayers, hay tools, forage equipment, seeding and tillage equipment, implements, and grain storage and protein production systems. It provides telemetry-based fleet management tools, including remote monitoring and diagnostics, which help farmers improve uptime, machine and yield optimization, mixed fleet optimization and decision support. The Company's Precision Planting, Headsight and Intelligent Ag Solutions brands provide retrofit solutions to upgrade farmers existing equipment to improve their planting, liquid application and harvest operations. The Company’s Precision Planting, Headsight, JCA and Intelligent Ag Solutions brands also sell precision agriculture solutions around the crop cycle to third party original equipment manufacturers (OEMs).</v>
     <v>27900</v>
@@ -5078,25 +5142,24 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>4205 River Green Pkway, DULUTH, GA, 30096 US</v>
-    <v>91.02</v>
+    <v>95.28</v>
     <v>Machinery, Equipment &amp; Components</v>
     <v>Stock</v>
-    <v>45548.958333356248</v>
+    <v>45553.77254563594</v>
     <v>30</v>
-    <v>89.76</v>
-    <v>6787225000</v>
+    <v>92.734999999999999</v>
+    <v>7109679075</v>
     <v>AGCO CORPORATION</v>
     <v>AGCO CORPORATION</v>
-    <v>90</v>
-    <v>16.197900000000001</v>
-    <v>89.32</v>
-    <v>90.93</v>
-    <v>89.322000000000003</v>
+    <v>92.79</v>
+    <v>16.5151</v>
+    <v>92.71</v>
+    <v>95.25</v>
     <v>74642300</v>
     <v>AGCO</v>
     <v>AGCO CORPORATION (XNYS:AGCO)</v>
-    <v>533652</v>
-    <v>814255</v>
+    <v>208389</v>
+    <v>774131</v>
     <v>1991</v>
   </rv>
   <rv s="2">
@@ -5120,11 +5183,9 @@
     <v>Powered by Refinitiv</v>
     <v>30.1</v>
     <v>24.01</v>
-    <v>1.1546000000000001</v>
-    <v>0.28999999999999998</v>
-    <v>1.0701E-2</v>
-    <v>0</v>
-    <v>0</v>
+    <v>1.1549</v>
+    <v>0.27</v>
+    <v>9.8719999999999988E-3</v>
     <v>USD</v>
     <v>Ituran Location and Control Ltd. is a provider of location-based services, consisting of stolen vehicle recovery (SVR), fleet management services and other tracking services. The Company also provides wireless communication products used in connection with its location-based services and various other applications. Its operations consist of two segments: location-based services and wireless communications products. Its location-based services segment consists of its SVR and tracking services, fleet management and value-added services consisted of personal locater services and concierge services. Its wireless communications products segment consists of short and medium range two-way machine-to-machine wireless communications products that are used for various applications, including automatic vehicle location (AVL) and automatic vehicle identification. It primarily provides its services, as well as sells and leases its products in Israel, Brazil, Argentina and the United States.</v>
     <v>2841</v>
@@ -5132,25 +5193,24 @@
     <v>XNAS</v>
     <v>XNAS</v>
     <v>3 HASHIKMA, A.T AZUR, T.D 163, AZOR, 5800182 IL</v>
-    <v>27.55</v>
+    <v>27.76</v>
     <v>Communications &amp; Networking</v>
     <v>Stock</v>
-    <v>45548.833432360938</v>
+    <v>45553.772053437497</v>
     <v>33</v>
-    <v>27.16</v>
-    <v>544885100</v>
+    <v>27.252500000000001</v>
+    <v>549460679</v>
     <v>ITURAN LOCATION AND CONTROL LTD.</v>
     <v>ITURAN LOCATION AND CONTROL LTD.</v>
-    <v>27.25</v>
-    <v>10.7273</v>
-    <v>27.1</v>
-    <v>27.39</v>
-    <v>27.39</v>
+    <v>27.28</v>
+    <v>10.711499999999999</v>
+    <v>27.35</v>
+    <v>27.62</v>
     <v>19893580</v>
     <v>ITRN</v>
     <v>ITURAN LOCATION AND CONTROL LTD. (XNAS:ITRN)</v>
-    <v>53935</v>
-    <v>84117</v>
+    <v>59626</v>
+    <v>82057</v>
     <v>1994</v>
   </rv>
   <rv s="2">
@@ -5172,13 +5232,11 @@
     <v>268435456</v>
     <v>1</v>
     <v>Powered by Refinitiv</v>
-    <v>49.21</v>
+    <v>49.4</v>
     <v>28.254999999999999</v>
-    <v>1.0374000000000001</v>
-    <v>0.12</v>
-    <v>2.519E-3</v>
-    <v>0</v>
-    <v>0</v>
+    <v>1.0365</v>
+    <v>0.41</v>
+    <v>8.4030000000000007E-3</v>
     <v>USD</v>
     <v>Frontdoor, Inc. is a provider of home warranties in the United States. The Company’s customizable home warranties help customers protect and maintain their homes, typically their assets, from costly and unplanned breakdowns of essential home systems and appliances. The Company operates under the brands American Home Shield, HSA, OneGuard and Landmark Home Warranty. Its annual service subscribe plan covers the repair or replacement of major components of more than 20 home systems and appliances, including electrical, plumbing, heating, ventilation, and air conditioning (HVAC) systems, water heaters, refrigerators, dishwashers, and ranges/ovens/cooktops, as well as optional coverages for electronics, pools, spas, and pumps. Its operations also include its Streem, a technology platform that uses augmented reality, computer vision and machine learning to, among other things, help home service professionals more quickly and accurately diagnose breakdowns and complete repairs.</v>
     <v>1716</v>
@@ -5186,25 +5244,24 @@
     <v>XNAS</v>
     <v>XNAS</v>
     <v>3400 PLAYERS CLUB PARKWAY, STE. 300, MEMPHIS, TN, 38125 US</v>
-    <v>48.31</v>
+    <v>49.4</v>
     <v>Personal &amp; Household Products &amp; Services</v>
     <v>Stock</v>
-    <v>45548.847228506253</v>
+    <v>45553.772605613281</v>
     <v>36</v>
-    <v>47.674999999999997</v>
-    <v>3654047000</v>
+    <v>48.35</v>
+    <v>3765007368</v>
     <v>FRONTDOOR, INC.</v>
     <v>FRONTDOOR, INC.</v>
-    <v>48.1</v>
-    <v>18.4391</v>
-    <v>47.63</v>
-    <v>47.75</v>
-    <v>47.75</v>
+    <v>48.79</v>
+    <v>18.840499999999999</v>
+    <v>48.79</v>
+    <v>49.2</v>
     <v>76524540</v>
     <v>FTDR</v>
     <v>FRONTDOOR, INC. (XNAS:FTDR)</v>
-    <v>496200</v>
-    <v>669040</v>
+    <v>288404</v>
+    <v>633339</v>
     <v>2018</v>
   </rv>
   <rv s="2">
@@ -5228,11 +5285,9 @@
     <v>Powered by Refinitiv</v>
     <v>126.8899</v>
     <v>50.2</v>
-    <v>0.50190000000000001</v>
-    <v>1.52</v>
-    <v>1.4611000000000001E-2</v>
-    <v>-0.43</v>
-    <v>-4.0739999999999995E-3</v>
+    <v>0.50160000000000005</v>
+    <v>3.95</v>
+    <v>3.7427000000000002E-2</v>
     <v>USD</v>
     <v>Lantheus Holdings, Inc. is a radiopharmaceutical-focused company engaged in delivering science to enable clinicians to find, fight and follow disease to deliver patient outcomes. The Company classifies its products in three categories: Radiopharmaceutical Oncology, Precision Diagnostics, and Strategic Partnerships. Its Radiopharmaceutical Oncology diagnostics and therapeutic candidates help healthcare professionals (HCPs) find, fight, and follow cancer, with a focus in prostate cancer. Its pipeline also includes breast and other cancers. Its Precision Diagnostic products assist HCPs to find and follow diseases, with a focus in cardiology. Its Strategic Partnerships focus on enabling precision medicine through the use of biomarkers, digital solutions and pharma solutions platforms. Its commercial products include PYLARIFY, DEFINITY, Ga-DOTA-RM2, and others. Its pipeline includes B amyloid positron emission tomography (PET) imaging agent, NAV-4694, also known as F18-flutafuranol.</v>
     <v>834</v>
@@ -5240,25 +5295,24 @@
     <v>XNAS</v>
     <v>XNAS</v>
     <v>331 Treble Cove Rd, NORTH BILLERICA, MA, 01862 US</v>
-    <v>107</v>
+    <v>109.94</v>
     <v>Healthcare Equipment &amp; Supplies</v>
     <v>Stock</v>
-    <v>45548.906874837499</v>
+    <v>45553.772584316408</v>
     <v>39</v>
-    <v>104.03</v>
-    <v>7328404000</v>
+    <v>104.5</v>
+    <v>7601960773</v>
     <v>LANTHEUS HOLDINGS, INC.</v>
     <v>LANTHEUS HOLDINGS, INC.</v>
-    <v>104.1</v>
-    <v>17.035799999999998</v>
-    <v>104.03</v>
-    <v>105.55</v>
-    <v>105.12</v>
+    <v>104.99</v>
+    <v>17.283100000000001</v>
+    <v>105.54</v>
+    <v>109.49</v>
     <v>69430640</v>
     <v>LNTH</v>
     <v>LANTHEUS HOLDINGS, INC. (XNAS:LNTH)</v>
-    <v>1119849</v>
-    <v>698248</v>
+    <v>286067</v>
+    <v>718116</v>
     <v>2007</v>
   </rv>
   <rv s="2">
@@ -5280,13 +5334,11 @@
     <v>268435456</v>
     <v>1</v>
     <v>Powered by Refinitiv</v>
-    <v>15.13</v>
+    <v>14.91</v>
     <v>6.37</v>
-    <v>2.1507999999999998</v>
-    <v>0.04</v>
-    <v>3.0530000000000002E-3</v>
-    <v>0</v>
-    <v>0</v>
+    <v>2.1511999999999998</v>
+    <v>1.4999999999999999E-2</v>
+    <v>1.142E-3</v>
     <v>USD</v>
     <v>Everi Holdings Inc. develops and offers products and services that provide gaming entertainment, improve its customers’ patron engagement, and help its casino customers operate their businesses. It develops and supplies entertaining game content, gaming machines and gaming systems and services for land-based and iGaming operators. It operates through two segments: Games and Financial Technology Solutions (FinTech). The Games segment provides gaming operators with gaming technology and entertainment products and services, including gaming machines, primarily comprising Class II, Class III and Historic Horse Racing slot machines placed under participation and fixed-fee lease arrangements or sold to casino customers. The FinTech segment provides gaming operators with financial technology products and services, including financial access and related services supporting digital, cashless and physical cash options across mobile, assisted and self-service channels.</v>
     <v>2200</v>
@@ -5297,22 +5349,21 @@
     <v>13.16</v>
     <v>Hotels &amp; Entertainment Services</v>
     <v>Stock</v>
-    <v>45548.958333367969</v>
+    <v>45553.772542522653</v>
     <v>42</v>
-    <v>13.13</v>
-    <v>1121152000</v>
+    <v>13.14</v>
+    <v>1122431694</v>
     <v>EVERI HOLDINGS INC.</v>
     <v>EVERI HOLDINGS INC.</v>
     <v>13.15</v>
-    <v>27.9099</v>
-    <v>13.1</v>
+    <v>27.908200000000001</v>
     <v>13.14</v>
-    <v>13.14</v>
+    <v>13.154999999999999</v>
     <v>85323580</v>
     <v>EVRI</v>
     <v>EVERI HOLDINGS INC. (XNYS:EVRI)</v>
-    <v>462893</v>
-    <v>965533</v>
+    <v>326168</v>
+    <v>863655</v>
     <v>2004</v>
   </rv>
   <rv s="2">
@@ -5333,10 +5384,8 @@
     <v>62.31</v>
     <v>32.14</v>
     <v>2.1230000000000002</v>
-    <v>1.84</v>
-    <v>5.1353999999999997E-2</v>
-    <v>0.32800000000000001</v>
-    <v>8.7069999999999995E-3</v>
+    <v>0.98</v>
+    <v>2.6244999999999997E-2</v>
     <v>USD</v>
     <v>Nextracker Inc. is a provider of integrated solar tracker and software solutions used in utility-scale and ground-mounted distributed generation solar projects. Its products enable solar panels in utility-scale power plants to follow the sun’s movement across the sky and optimize plant performance. Its products include NX Horizon, NX Gemini, TrueCapture, and NX Navigator. Its solutions include Bifacial PV modules, Large Format Modules, and First Solar Series 6 (FSLR6) Modules. NX Horizon is a one-in-portrait (1P) smart solar tracker system that delivers the lowest levelized cost of energy (LCOE). NX Gemini is its two-in-portrait (2P) format tracker which holds two rows of solar panels along the central support beam. TrueCapture is its flagship software offering, which is a self-adjusting tracker control system that uses machine learning to enhance solar power plant energy yield. It has operations in the United States, Brazil, Mexico, Spain, India, Australia, the Middle East and Brazil.</v>
     <v>1050</v>
@@ -5344,24 +5393,23 @@
     <v>XNAS</v>
     <v>XNAS</v>
     <v>6200 Paseo Padre Pkwy, FREMONT, CA, 94555 US</v>
-    <v>37.69</v>
+    <v>38.32</v>
     <v>Renewable Energy</v>
     <v>Stock</v>
-    <v>45548.999650971877</v>
-    <v>36.229999999999997</v>
-    <v>5475238000</v>
+    <v>45553.772578217191</v>
+    <v>36.729999999999997</v>
+    <v>5569712368</v>
     <v>NEXTRACKER INC.</v>
     <v>NEXTRACKER INC.</v>
-    <v>36.28</v>
-    <v>9.9972999999999992</v>
-    <v>35.83</v>
-    <v>37.67</v>
-    <v>37.997999999999998</v>
+    <v>37.340000000000003</v>
+    <v>9.9099000000000004</v>
+    <v>37.340000000000003</v>
+    <v>38.32</v>
     <v>145347400</v>
     <v>NXT</v>
     <v>NEXTRACKER INC. (XNAS:NXT)</v>
-    <v>2972864</v>
-    <v>2855723</v>
+    <v>1947977</v>
+    <v>2850986</v>
     <v>2022</v>
   </rv>
   <rv s="2">
@@ -5385,11 +5433,9 @@
     <v>Powered by Refinitiv</v>
     <v>80.22</v>
     <v>56.25</v>
-    <v>1.7424999999999999</v>
-    <v>0.52</v>
-    <v>6.9479999999999993E-3</v>
-    <v>0</v>
-    <v>0</v>
+    <v>1.7428999999999999</v>
+    <v>1.71</v>
+    <v>2.2438E-2</v>
     <v>USD</v>
     <v>Monarch Casino &amp; Resort, Inc. owns and operates the Atlantis Casino Resort Spa, a hotel and casino in Reno, Nevada (the Atlantis) and the Monarch Casino Resort Spa Black Hawk (the Monarch Black Hawk), a hotel and casino in Black Hawk, Colorado. In addition, it owns separate parcels of land located next to the Atlantis and a parcel of land with an industrial warehouse located between Denver, Colorado, and Monarch Black Hawk. The Atlantis is located approximately three miles south of downtown, which features approximately 61,000 square feet of casino space; 817 guest rooms and suites; eight food outlets; two gourmet coffee and pastry bars and one snack bar; a 30,000 square-foot health spa and salon with an enclosed year-round pool. Monarch Black Hawk features approximately 60,000 square feet of casino space; approximately 1,000 slot machines; approximately 43 table games; a live poker room; a keno counter and a sports book. The resort also includes 10 bars and lounges.</v>
     <v>2900</v>
@@ -5397,25 +5443,24 @@
     <v>XNAS</v>
     <v>XNAS</v>
     <v>Executive Offices, 3800 S Virginia Street, RENO, NV, 89502 US</v>
-    <v>75.86</v>
+    <v>77.92</v>
     <v>Hotels &amp; Entertainment Services</v>
     <v>Stock</v>
-    <v>45548.995103842186</v>
+    <v>45553.772504606248</v>
     <v>47</v>
-    <v>73.844999999999999</v>
-    <v>1390552000</v>
+    <v>75.27</v>
+    <v>1437789190</v>
     <v>MONARCH CASINO &amp; RESORT, INC.</v>
     <v>MONARCH CASINO &amp; RESORT, INC.</v>
-    <v>74.959999999999994</v>
-    <v>17.610800000000001</v>
-    <v>74.84</v>
-    <v>75.36</v>
-    <v>75.36</v>
+    <v>75.98</v>
+    <v>17.8096</v>
+    <v>76.209999999999994</v>
+    <v>77.92</v>
     <v>18452120</v>
     <v>MCRI</v>
     <v>MONARCH CASINO &amp; RESORT, INC. (XNAS:MCRI)</v>
-    <v>89168</v>
-    <v>89974</v>
+    <v>82801</v>
+    <v>100560</v>
     <v>1993</v>
   </rv>
   <rv s="2">
@@ -5439,11 +5484,9 @@
     <v>Powered by Refinitiv</v>
     <v>69.75</v>
     <v>34.96</v>
-    <v>0.97419999999999995</v>
-    <v>0.24</v>
-    <v>4.1520000000000003E-3</v>
-    <v>0.05</v>
-    <v>8.6129999999999996E-4</v>
+    <v>0.97289999999999999</v>
+    <v>1.675</v>
+    <v>2.8496E-2</v>
     <v>USD</v>
     <v>Miller Industries, Inc. is a manufacturer of towing and recovery equipment. The Company designs and manufactures bodies of car carriers and wreckers, which are installed on chassis manufactured by third parties, and sold to its customers. Its products are marketed and sold through a network of distributors that serve all 50 states, Canada, Mexico, and other foreign markets, and through prime contractors to governmental entities. In addition to selling its products, its independent distributors provide end-users with parts and service. Its product line includes car carriers, wreckers, and transport trailers. Car carriers are specialized flat-bed vehicles with hydraulic tilt mechanisms that enable a towing operator to drive or winch a vehicle onto the bed for transport. Its multi-vehicle transport trailers are specialized auto transport trailers with upper and lower decks and hydraulic ramps for loading vehicles. Its brands include Century, Vulcan, Chevron, Holmes, and Challenger.</v>
     <v>1821</v>
@@ -5451,25 +5494,24 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>Ste 100, 8503 Hilltop Dr, OOLTEWAH, TN, 37363 US</v>
-    <v>59.32</v>
+    <v>60.454999999999998</v>
     <v>Automobiles &amp; Auto Parts</v>
     <v>Stock</v>
-    <v>45548.958333344533</v>
+    <v>45553.772410462501</v>
     <v>50</v>
-    <v>57.85</v>
-    <v>664892600</v>
+    <v>58.77</v>
+    <v>692438874</v>
     <v>MILLER INDUSTRIES, INC.</v>
     <v>MILLER INDUSTRIES, INC.</v>
-    <v>58.69</v>
-    <v>9.3452999999999999</v>
-    <v>57.81</v>
-    <v>58.05</v>
-    <v>58.1</v>
+    <v>59.05</v>
+    <v>9.4627999999999997</v>
+    <v>58.78</v>
+    <v>60.454999999999998</v>
     <v>11453790</v>
     <v>MLR</v>
     <v>MILLER INDUSTRIES, INC. (XNYS:MLR)</v>
-    <v>43671</v>
-    <v>90221</v>
+    <v>24625</v>
+    <v>86198</v>
     <v>1994</v>
   </rv>
   <rv s="2">
@@ -5493,11 +5535,9 @@
     <v>Powered by Refinitiv</v>
     <v>15.86</v>
     <v>9.1649999999999991</v>
-    <v>0.89880000000000004</v>
-    <v>0.14000000000000001</v>
-    <v>1.4402999999999999E-2</v>
-    <v>-5.0000000000000001E-3</v>
-    <v>-5.0710000000000002E-4</v>
+    <v>0.89490000000000003</v>
+    <v>0.09</v>
+    <v>8.7720000000000003E-3</v>
     <v>USD</v>
     <v>Janus International Group, Inc. is a global manufacturer and supplier of turn-key self-storage, commercial and industrial building solutions. It operates through two geographic segments: Janus North America and Janus International. The Janus North America segment is comprised of all the other entities, including Janus International Group, LLC, Betco, Inc., Noke, Inc., Asta Industries, Inc., DBCI, LLC, Access Control Technologies, LLC, Janus Door, LLC, and Steel Door Depot.com, LLC. The Janus International segment is comprised of Janus International Europe Holdings Ltd. (UK). Its production and sales are in Europe and Australia. It provides facility and door automation and access control technologies, roll up and swing doors, hallway systems and relocatable storage moveable additional storage structures (MASS) units. It is comprised of three sales channels, including New Construction-Self-storage, R3-Self-storage, and Commercial and Other. It also provides terminal maintenance services.</v>
     <v>1956</v>
@@ -5505,25 +5545,24 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>135 Janus International Blvd., TEMPLE, GA, 30179 US</v>
-    <v>10.005000000000001</v>
+    <v>10.4</v>
     <v>Homebuilding &amp; Construction Supplies</v>
     <v>Stock</v>
-    <v>45548.958333356248</v>
+    <v>45553.772548992965</v>
     <v>53</v>
-    <v>9.75</v>
-    <v>1432877000</v>
+    <v>10.11</v>
+    <v>1504084770</v>
     <v>JANUS INTERNATIONAL GROUP, INC.</v>
     <v>JANUS INTERNATIONAL GROUP, INC.</v>
-    <v>9.85</v>
-    <v>11.0563</v>
-    <v>9.7200000000000006</v>
-    <v>9.86</v>
-    <v>9.8550000000000004</v>
+    <v>10.29</v>
+    <v>11.5047</v>
+    <v>10.26</v>
+    <v>10.35</v>
     <v>145322200</v>
     <v>JBI</v>
     <v>JANUS INTERNATIONAL GROUP, INC. (XNYS:JBI)</v>
-    <v>1466098</v>
-    <v>2451088</v>
+    <v>544015</v>
+    <v>2091493</v>
     <v>2020</v>
   </rv>
   <rv s="2">
@@ -5547,11 +5586,9 @@
     <v>Powered by Refinitiv</v>
     <v>574.76</v>
     <v>318.17</v>
-    <v>1.3039000000000001</v>
-    <v>5.26</v>
-    <v>1.4098999999999999E-2</v>
-    <v>0</v>
-    <v>0</v>
+    <v>1.3</v>
+    <v>8.61</v>
+    <v>2.1687999999999999E-2</v>
     <v>USD</v>
     <v>Ulta Beauty, Inc. is a beauty retailer. The Company's product categories include cosmetics, skincare, haircare products and styling tools, fragrance and bath, services, and accessories and other. The Company has one segment, which includes retail stores, salon services, and e-commerce. It offers a range of beauty services in its stores, focusing on hair, makeup, brow and skin services. Its skin services include a skin treatment room or dedicated skin treatment area on the sales floor. Its Ulta Beauty store prototype includes an open salon area, with most of its stores offering brow services on the salon floor. It offers a new way to shop for beauty - bringing together All Things Beauty, All in One Place. In addition to ship to home order fulfillment, it offers guests Buy Online, Pick-up in Store, Curbside Pickup, and Store 2 Door, which provides the ability for customers to order in-store and have products delivered to their homes. It operates over 1,350 retail stores across 50 states.</v>
     <v>20000</v>
@@ -5559,29 +5596,232 @@
     <v>XNAS</v>
     <v>XNAS</v>
     <v>1000 Remington Blvd, Suite 120, BOLINGBROOK, IL, 60440 US</v>
-    <v>382.84</v>
+    <v>405.87</v>
     <v>Specialty Retailers</v>
     <v>Stock</v>
-    <v>45548.999404108596</v>
+    <v>45553.772602650002</v>
     <v>56</v>
-    <v>375</v>
-    <v>17825390000</v>
+    <v>397.38</v>
+    <v>19110205635</v>
     <v>ULTA BEAUTY, INC.</v>
     <v>ULTA BEAUTY, INC.</v>
-    <v>375.99</v>
-    <v>14.9808</v>
-    <v>373.08</v>
-    <v>378.34</v>
-    <v>378.34</v>
+    <v>398</v>
+    <v>15.9413</v>
+    <v>397</v>
+    <v>405.61</v>
     <v>47114730</v>
     <v>ULTA</v>
     <v>ULTA BEAUTY, INC. (XNAS:ULTA)</v>
-    <v>762495</v>
-    <v>1625657</v>
+    <v>769082</v>
+    <v>1657712</v>
     <v>2016</v>
   </rv>
   <rv s="2">
     <v>57</v>
+  </rv>
+  <rv s="0">
+    <v>https://www.bing.com/financeapi/forcetrigger?t=a1vehw&amp;q=XNYS%3aIGT&amp;form=skydnc</v>
+    <v>Learn more on Bing</v>
+  </rv>
+  <rv s="1">
+    <v>0</v>
+    <v>INTERNATIONAL GAME TECHNOLOGY PLC (XNYS:IGT)</v>
+    <v>2</v>
+    <v>3</v>
+    <v>Finance</v>
+    <v>4</v>
+    <v>en-GB</v>
+    <v>a1vehw</v>
+    <v>268435456</v>
+    <v>1</v>
+    <v>Powered by Refinitiv</v>
+    <v>32.909999999999997</v>
+    <v>18.899999999999999</v>
+    <v>1.9702</v>
+    <v>0.45</v>
+    <v>2.0622999999999999E-2</v>
+    <v>USD</v>
+    <v>International Game Technology PLC is a United Kingdom-based company, which is engaged in gaming. The Company operates and provides an integrated portfolio of gaming technology products and services, including online and instant lottery systems, iLottery, instant ticket printing, lottery management services, commercial services, gaming systems, electronic gaming machines, iGaming, and sports betting. The Company operates through three segments. The Global Lottery segment operates traditional lottery and iLottery businesses across the world, which includes sales, operations, product development, technology, and support, across the world. The Global Gaming segment operates a land-based gaming business across the world, which includes sales, product management, studios, global manufacturing, operation, and technology, across the world. The Digital &amp; Betting segment operates iGaming and sports betting activities across the world.</v>
+    <v>11000</v>
+    <v>New York Stock Exchange</v>
+    <v>XNYS</v>
+    <v>XNYS</v>
+    <v>10 Finsbury Square, Third Floor, LONDON, UNITED KINGDOM-NA, EC2A 1AF GB</v>
+    <v>22.34</v>
+    <v>Hotels &amp; Entertainment Services</v>
+    <v>Stock</v>
+    <v>45553.772503830471</v>
+    <v>59</v>
+    <v>21.78</v>
+    <v>4454000000</v>
+    <v>INTERNATIONAL GAME TECHNOLOGY PLC</v>
+    <v>INTERNATIONAL GAME TECHNOLOGY PLC</v>
+    <v>21.91</v>
+    <v>21.110900000000001</v>
+    <v>21.82</v>
+    <v>22.27</v>
+    <v>200000000</v>
+    <v>IGT</v>
+    <v>INTERNATIONAL GAME TECHNOLOGY PLC (XNYS:IGT)</v>
+    <v>334254</v>
+    <v>635397</v>
+    <v>2014</v>
+  </rv>
+  <rv s="2">
+    <v>60</v>
+  </rv>
+  <rv s="0">
+    <v>https://www.bing.com/financeapi/forcetrigger?t=a1z3ec&amp;q=XNYS%3aODC&amp;form=skydnc</v>
+    <v>Learn more on Bing</v>
+  </rv>
+  <rv s="1">
+    <v>0</v>
+    <v>OIL-DRI CORPORATION OF AMERICA (XNYS:ODC)</v>
+    <v>2</v>
+    <v>3</v>
+    <v>Finance</v>
+    <v>4</v>
+    <v>en-GB</v>
+    <v>a1z3ec</v>
+    <v>268435456</v>
+    <v>1</v>
+    <v>Powered by Refinitiv</v>
+    <v>87.32</v>
+    <v>54.8</v>
+    <v>0.58589999999999998</v>
+    <v>0.87</v>
+    <v>1.2675000000000001E-2</v>
+    <v>USD</v>
+    <v>Oil-Dri Corporation of America is a manufacturer and supplier of specialty sorbent products for pet care, animal health and nutrition, fluid purification, agricultural ingredients, sports field, industrial and automotive markets. Its principal product is cat litter. The Company’s Retail and Wholesale Products Group segment customers include mass merchandisers, the farm and fleet channel, drugstore chains, pet specialty retail outlets, dollar stores, retail grocery stores, distributors of industrial cleanup and automotive products, environmental service companies, sports field product users and marketers of consumer products. Its Business to Business Products Group segment customers include processors and refiners of edible oils, renewable diesel, petroleum-based oils and biodiesel fuel; manufacturers of animal feed and agricultural chemicals; and distributors of animal health and nutrition products. It is also a supplier of silica gel-based crystal cat litter.</v>
+    <v>884</v>
+    <v>New York Stock Exchange</v>
+    <v>XNYS</v>
+    <v>XNYS</v>
+    <v>SUITE 400, 410 NORTH MICHIGAN AVENUE, CHICAGO, IL, 60611 US</v>
+    <v>69.510000000000005</v>
+    <v>Chemicals</v>
+    <v>Stock</v>
+    <v>45553.771617580467</v>
+    <v>62</v>
+    <v>68.459999999999994</v>
+    <v>500133200</v>
+    <v>OIL-DRI CORPORATION OF AMERICA</v>
+    <v>OIL-DRI CORPORATION OF AMERICA</v>
+    <v>68.459999999999994</v>
+    <v>14.085800000000001</v>
+    <v>68.64</v>
+    <v>69.510000000000005</v>
+    <v>7286320</v>
+    <v>ODC</v>
+    <v>OIL-DRI CORPORATION OF AMERICA (XNYS:ODC)</v>
+    <v>5454</v>
+    <v>15891</v>
+    <v>1969</v>
+  </rv>
+  <rv s="2">
+    <v>63</v>
+  </rv>
+  <rv s="0">
+    <v>https://www.bing.com/financeapi/forcetrigger?t=a1mt9c&amp;q=XNAS%3aACLS&amp;form=skydnc</v>
+    <v>Learn more on Bing</v>
+  </rv>
+  <rv s="1">
+    <v>0</v>
+    <v>AXCELIS TECHNOLOGIES, INC. (XNAS:ACLS)</v>
+    <v>2</v>
+    <v>3</v>
+    <v>Finance</v>
+    <v>4</v>
+    <v>en-GB</v>
+    <v>a1mt9c</v>
+    <v>268435456</v>
+    <v>1</v>
+    <v>Powered by Refinitiv</v>
+    <v>170.9692</v>
+    <v>93.77</v>
+    <v>1.5901000000000001</v>
+    <v>1.23</v>
+    <v>1.2327999999999999E-2</v>
+    <v>USD</v>
+    <v>Axcelis Technologies, Inc. designs, manufactures and services ion implantation and other processing equipment used in the fabrication of semiconductor chips. The Company offers a complete line of high energy, high current and medium current implanters for all application requirements. In addition to equipment, the Company provides extensive aftermarket lifecycle products and services, including used tools, spare parts, equipment upgrades, maintenance services and customer training. Its Purion flagship systems are all based on a common platform, which enables a combination of implant purity, precision and productivity. Combining a single wafer end station, with advanced spot beam architectures (that ensures all points across the wafer see the same beam condition at the same beam angle), Purion products enable process control to optimize device performance and yield, at high productivity. The Company sells its products to semiconductor chip manufacturers around the world.</v>
+    <v>1620</v>
+    <v>Nasdaq Stock Market</v>
+    <v>XNAS</v>
+    <v>XNAS</v>
+    <v>108 Cherry Hill Dr, BEVERLY, MA, 01915 US</v>
+    <v>101.82</v>
+    <v>Semiconductors &amp; Semiconductor Equipment</v>
+    <v>Stock</v>
+    <v>45553.772599015625</v>
+    <v>65</v>
+    <v>98.3</v>
+    <v>3294376590</v>
+    <v>AXCELIS TECHNOLOGIES, INC.</v>
+    <v>AXCELIS TECHNOLOGIES, INC.</v>
+    <v>101.01</v>
+    <v>13.784700000000001</v>
+    <v>99.77</v>
+    <v>101</v>
+    <v>32617590</v>
+    <v>ACLS</v>
+    <v>AXCELIS TECHNOLOGIES, INC. (XNAS:ACLS)</v>
+    <v>301555</v>
+    <v>517965</v>
+    <v>1995</v>
+  </rv>
+  <rv s="2">
+    <v>66</v>
+  </rv>
+  <rv s="0">
+    <v>https://www.bing.com/financeapi/forcetrigger?t=a1retc&amp;q=XNYS%3aDELL&amp;form=skydnc</v>
+    <v>Learn more on Bing</v>
+  </rv>
+  <rv s="1">
+    <v>0</v>
+    <v>DELL TECHNOLOGIES INC. (XNYS:DELL)</v>
+    <v>2</v>
+    <v>3</v>
+    <v>Finance</v>
+    <v>4</v>
+    <v>en-GB</v>
+    <v>a1retc</v>
+    <v>268435456</v>
+    <v>1</v>
+    <v>Powered by Refinitiv</v>
+    <v>179.7</v>
+    <v>63.9</v>
+    <v>0.89510000000000001</v>
+    <v>1.681</v>
+    <v>1.439E-2</v>
+    <v>USD</v>
+    <v>Dell Technologies Inc. is engaged in designing, developing, manufacturing, marketing, selling, and supporting a wide range of comprehensive and integrated solutions, products, and services. The Company operates through two segments: Infrastructure Solutions Group (ISG) and Client Solutions Group (CSG). Its ISG segment enables the Company’s customer’s digital transformation with solutions that address artificial intelligence (AI), machine learning, data analytics, and multi cloud environments. Its comprehensive storage portfolio includes modern and traditional storage solutions, including all-flash arrays, scale-out file, object platforms, hyper-converged infrastructure, and software-defined storage. Its CSG segment offers branded personal computers (PCs) including notebooks, desktops, and workstations and branded peripherals that include displays, docking stations, keyboards, mice, and webcam and audio devices, as well as third-party software and peripherals.</v>
+    <v>120000</v>
+    <v>New York Stock Exchange</v>
+    <v>XNYS</v>
+    <v>XNYS</v>
+    <v>ONE DELL WAY, ROUND ROCK, TX, 78682 US</v>
+    <v>119.62</v>
+    <v>Computers, Phones &amp; Household Electronics</v>
+    <v>Stock</v>
+    <v>45553.772594108596</v>
+    <v>68</v>
+    <v>116.57</v>
+    <v>83233301184</v>
+    <v>DELL TECHNOLOGIES INC.</v>
+    <v>DELL TECHNOLOGIES INC.</v>
+    <v>117.56</v>
+    <v>21.6111</v>
+    <v>116.82</v>
+    <v>118.501</v>
+    <v>702384800</v>
+    <v>DELL</v>
+    <v>DELL TECHNOLOGIES INC. (XNYS:DELL)</v>
+    <v>7170560</v>
+    <v>11513168</v>
+    <v>2013</v>
+  </rv>
+  <rv s="2">
+    <v>69</v>
   </rv>
 </rvData>
 </file>
@@ -5609,8 +5849,6 @@
     <k n="Beta"/>
     <k n="Change"/>
     <k n="Change (%)"/>
-    <k n="Change (Extended hours)"/>
-    <k n="Change % (Extended hours)"/>
     <k n="Currency" t="s"/>
     <k n="Description" t="s"/>
     <k n="Employees"/>
@@ -5631,7 +5869,6 @@
     <k n="P/E"/>
     <k n="Previous close"/>
     <k n="Price"/>
-    <k n="Price (Extended hours)"/>
     <k n="Shares outstanding"/>
     <k n="Ticker symbol" t="s"/>
     <k n="UniqueName" t="s"/>
@@ -5659,8 +5896,6 @@
     <k n="Beta"/>
     <k n="Change"/>
     <k n="Change (%)"/>
-    <k n="Change (Extended hours)"/>
-    <k n="Change % (Extended hours)"/>
     <k n="Currency" t="s"/>
     <k n="Description" t="s"/>
     <k n="Employees"/>
@@ -5680,7 +5915,6 @@
     <k n="P/E"/>
     <k n="Previous close"/>
     <k n="Price"/>
-    <k n="Price (Extended hours)"/>
     <k n="Shares outstanding"/>
     <k n="Ticker symbol" t="s"/>
     <k n="UniqueName" t="s"/>
@@ -5694,7 +5928,7 @@
 <file path=xl/richData/rdsupportingpropertybag.xml><?xml version="1.0" encoding="utf-8"?>
 <supportingPropertyBags xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2">
   <spbArrays count="2">
-    <a count="45">
+    <a count="42">
       <v t="s">%EntityServiceId</v>
       <v t="s">_Format</v>
       <v t="s">%IsRefreshable</v>
@@ -5705,16 +5939,13 @@
       <v t="s">Name</v>
       <v t="s">_SubLabel</v>
       <v t="s">Price</v>
-      <v t="s">Price (Extended hours)</v>
       <v t="s">Exchange</v>
       <v t="s">Official name</v>
       <v t="s">Last trade time</v>
       <v t="s">Ticker symbol</v>
       <v t="s">Exchange abbreviation</v>
       <v t="s">Change</v>
-      <v t="s">Change (Extended hours)</v>
       <v t="s">Change (%)</v>
-      <v t="s">Change % (Extended hours)</v>
       <v t="s">Currency</v>
       <v t="s">Previous close</v>
       <v t="s">Open</v>
@@ -5741,7 +5972,7 @@
       <v t="s">ExchangeID</v>
       <v t="s">%ProviderInfo</v>
     </a>
-    <a count="44">
+    <a count="41">
       <v t="s">%EntityServiceId</v>
       <v t="s">_Format</v>
       <v t="s">%IsRefreshable</v>
@@ -5752,16 +5983,13 @@
       <v t="s">Name</v>
       <v t="s">_SubLabel</v>
       <v t="s">Price</v>
-      <v t="s">Price (Extended hours)</v>
       <v t="s">Exchange</v>
       <v t="s">Official name</v>
       <v t="s">Last trade time</v>
       <v t="s">Ticker symbol</v>
       <v t="s">Exchange abbreviation</v>
       <v t="s">Change</v>
-      <v t="s">Change (Extended hours)</v>
       <v t="s">Change (%)</v>
-      <v t="s">Change % (Extended hours)</v>
       <v t="s">Currency</v>
       <v t="s">Previous close</v>
       <v t="s">Open</v>
@@ -5826,19 +6054,13 @@
       <v>8</v>
       <v>9</v>
       <v>4</v>
-      <v>1</v>
-      <v>1</v>
-      <v>5</v>
     </spb>
     <spb s="4">
-      <v>at close</v>
+      <v>Real-Time Nasdaq Last Sale</v>
       <v>from previous close</v>
       <v>from previous close</v>
-      <v>Source: Nasdaq</v>
+      <v>Source: Nasdaq Last Sale</v>
       <v>GMT</v>
-      <v>Delayed 15 minutes</v>
-      <v>from close</v>
-      <v>from close</v>
     </spb>
     <spb s="5">
       <v>1</v>
@@ -5892,9 +6114,6 @@
     <k n="Year incorporated" t="i"/>
     <k n="`%EntityServiceId" t="i"/>
     <k n="Shares outstanding" t="i"/>
-    <k n="Price (Extended hours)" t="i"/>
-    <k n="Change (Extended hours)" t="i"/>
-    <k n="Change % (Extended hours)" t="i"/>
   </s>
   <s>
     <k n="Price" t="s"/>
@@ -5902,9 +6121,6 @@
     <k n="Change (%)" t="s"/>
     <k n="ExchangeID" t="s"/>
     <k n="Last trade time" t="s"/>
-    <k n="Price (Extended hours)" t="s"/>
-    <k n="Change (Extended hours)" t="s"/>
-    <k n="Change % (Extended hours)" t="s"/>
   </s>
   <s>
     <k n="^Order" t="spba"/>
@@ -5976,29 +6192,29 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4AEE35AE-5B0D-FE48-BB2D-FD669C9DCA16}" name="Portfolio" displayName="Portfolio" ref="B2:K22" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
-  <autoFilter ref="B2:K22" xr:uid="{4AEE35AE-5B0D-FE48-BB2D-FD669C9DCA16}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4AEE35AE-5B0D-FE48-BB2D-FD669C9DCA16}" name="Portfolio" displayName="Portfolio" ref="B2:K26" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="B2:K26" xr:uid="{4AEE35AE-5B0D-FE48-BB2D-FD669C9DCA16}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{0445D94A-6FCB-7D4D-96B6-8AA18900F668}" name="Company" dataDxfId="17"/>
-    <tableColumn id="8" xr3:uid="{D4CC5B63-9F41-F843-9F6B-16BF8366EF76}" name="Name" dataDxfId="16">
+    <tableColumn id="1" xr3:uid="{0445D94A-6FCB-7D4D-96B6-8AA18900F668}" name="Company" dataDxfId="9"/>
+    <tableColumn id="8" xr3:uid="{D4CC5B63-9F41-F843-9F6B-16BF8366EF76}" name="Name" dataDxfId="8">
       <calculatedColumnFormula array="1">_FV(Portfolio[[#This Row],[Company]],"Name")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{B02ADEDD-E393-8F47-A86F-790F7D8AC135}" name="Ticker" dataDxfId="15">
+    <tableColumn id="2" xr3:uid="{B02ADEDD-E393-8F47-A86F-790F7D8AC135}" name="Ticker" dataDxfId="7">
       <calculatedColumnFormula array="1">_FV(B3,"Ticker symbol",TRUE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{DAB4D9A1-3A8B-F941-8C60-3B2546DAB540}" name="Industry" dataDxfId="14">
+    <tableColumn id="3" xr3:uid="{DAB4D9A1-3A8B-F941-8C60-3B2546DAB540}" name="Industry" dataDxfId="6">
       <calculatedColumnFormula array="1">_FV(B3,"Industry")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{2480957A-208E-8047-AEFC-5888351C1175}" name="Purchase" dataDxfId="13"/>
-    <tableColumn id="9" xr3:uid="{C19D84FB-40D7-E444-83AC-793DDFB09317}" name="Amount" dataDxfId="12"/>
-    <tableColumn id="10" xr3:uid="{0339281E-B096-D14D-B83F-1032AB2E4CB5}" name="Cost" dataDxfId="11"/>
-    <tableColumn id="6" xr3:uid="{633C3CE6-95BE-E743-869D-E0D6471E5EDB}" name="Current Price" dataDxfId="10">
+    <tableColumn id="4" xr3:uid="{2480957A-208E-8047-AEFC-5888351C1175}" name="Purchase" dataDxfId="5"/>
+    <tableColumn id="9" xr3:uid="{C19D84FB-40D7-E444-83AC-793DDFB09317}" name="Amount" dataDxfId="4"/>
+    <tableColumn id="10" xr3:uid="{0339281E-B096-D14D-B83F-1032AB2E4CB5}" name="Cost" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{633C3CE6-95BE-E743-869D-E0D6471E5EDB}" name="Current Price" dataDxfId="2">
       <calculatedColumnFormula array="1">_FV(B3,"Price")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{0C4F3DBA-8ADF-A44E-971F-127F7DF8311F}" name="Change" dataDxfId="9">
+    <tableColumn id="5" xr3:uid="{0C4F3DBA-8ADF-A44E-971F-127F7DF8311F}" name="Change" dataDxfId="1">
       <calculatedColumnFormula>((I3-F3)/F3)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{A51F63E4-8280-4643-84C4-E673A52345D6}" name="Profit/Loss" dataDxfId="8">
+    <tableColumn id="11" xr3:uid="{A51F63E4-8280-4643-84C4-E673A52345D6}" name="Profit/Loss" dataDxfId="0">
       <calculatedColumnFormula>(I3*G3) - H3</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -40363,7 +40579,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:X1011"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A16" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
@@ -68759,284 +68975,284 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="175"/>
-    <col min="3" max="3" width="20.83203125" style="184" customWidth="1"/>
-    <col min="4" max="4" width="14.5" style="185" customWidth="1"/>
-    <col min="5" max="5" width="13.6640625" style="183" customWidth="1"/>
-    <col min="6" max="16384" width="10.83203125" style="175"/>
+    <col min="1" max="2" width="10.83203125" style="174"/>
+    <col min="3" max="3" width="20.83203125" style="183" customWidth="1"/>
+    <col min="4" max="4" width="14.5" style="184" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" style="182" customWidth="1"/>
+    <col min="6" max="16384" width="10.83203125" style="174"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15">
-      <c r="A1" s="176" t="s">
+      <c r="A1" s="175" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="176" t="s">
+      <c r="B1" s="175" t="s">
         <v>144</v>
       </c>
-      <c r="C1" s="188" t="s">
+      <c r="C1" s="187" t="s">
         <v>145</v>
       </c>
-      <c r="D1" s="189" t="s">
+      <c r="D1" s="188" t="s">
         <v>146</v>
       </c>
-      <c r="E1" s="186" t="s">
+      <c r="E1" s="185" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="177"/>
-      <c r="G1" s="177"/>
-      <c r="H1" s="177"/>
-      <c r="I1" s="177"/>
-      <c r="J1" s="177"/>
-      <c r="K1" s="177"/>
+      <c r="F1" s="176"/>
+      <c r="G1" s="176"/>
+      <c r="H1" s="176"/>
+      <c r="I1" s="176"/>
+      <c r="J1" s="176"/>
+      <c r="K1" s="176"/>
     </row>
     <row r="2" spans="1:13" ht="15">
-      <c r="A2" s="178">
+      <c r="A2" s="177">
         <v>2023</v>
       </c>
-      <c r="B2" s="179">
+      <c r="B2" s="178">
         <v>11</v>
       </c>
-      <c r="C2" s="190">
+      <c r="C2" s="189">
         <v>1E-4</v>
       </c>
-      <c r="D2" s="191">
+      <c r="D2" s="190">
         <f>C2</f>
         <v>1E-4</v>
       </c>
-      <c r="E2" s="187" t="e">
+      <c r="E2" s="186" t="e">
         <f>STDEV($D$2:D2)*SQRT(52)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="F2" s="180"/>
-      <c r="G2" s="181"/>
-      <c r="H2" s="182"/>
-      <c r="I2" s="181"/>
-      <c r="J2" s="181"/>
-      <c r="K2" s="181"/>
+      <c r="F2" s="179"/>
+      <c r="G2" s="180"/>
+      <c r="H2" s="181"/>
+      <c r="I2" s="180"/>
+      <c r="J2" s="180"/>
+      <c r="K2" s="180"/>
     </row>
     <row r="3" spans="1:13" ht="15">
-      <c r="A3" s="178"/>
-      <c r="B3" s="179">
+      <c r="A3" s="177"/>
+      <c r="B3" s="178">
         <v>12</v>
       </c>
-      <c r="C3" s="190">
+      <c r="C3" s="189">
         <v>0</v>
       </c>
-      <c r="D3" s="191">
+      <c r="D3" s="190">
         <f>D2+C3</f>
         <v>1E-4</v>
       </c>
-      <c r="E3" s="187">
+      <c r="E3" s="186">
         <f>STDEV($D$2:D3)*SQRT(52)</f>
         <v>0</v>
       </c>
-      <c r="F3" s="180"/>
-      <c r="G3" s="181"/>
-      <c r="H3" s="181"/>
-      <c r="I3" s="181"/>
-      <c r="J3" s="181"/>
-      <c r="K3" s="181"/>
-      <c r="M3" s="203">
+      <c r="F3" s="179"/>
+      <c r="G3" s="180"/>
+      <c r="H3" s="180"/>
+      <c r="I3" s="180"/>
+      <c r="J3" s="180"/>
+      <c r="K3" s="180"/>
+      <c r="M3" s="202">
         <v>2.0000000000000001E-4</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="15">
-      <c r="A4" s="178">
+      <c r="A4" s="177">
         <v>2024</v>
       </c>
-      <c r="B4" s="179">
+      <c r="B4" s="178">
         <v>1</v>
       </c>
-      <c r="C4" s="190">
+      <c r="C4" s="189">
         <v>1.6000000000000001E-3</v>
       </c>
-      <c r="D4" s="191">
+      <c r="D4" s="190">
         <f>D3+C4</f>
         <v>1.7000000000000001E-3</v>
       </c>
-      <c r="E4" s="187">
+      <c r="E4" s="186">
         <f>STDEV($D$2:D4)*SQRT(52)</f>
         <v>6.6613311982916239E-3</v>
       </c>
-      <c r="F4" s="180"/>
-      <c r="G4" s="181"/>
-      <c r="H4" s="181"/>
-      <c r="I4" s="181"/>
-      <c r="J4" s="181"/>
-      <c r="K4" s="181"/>
+      <c r="F4" s="179"/>
+      <c r="G4" s="180"/>
+      <c r="H4" s="180"/>
+      <c r="I4" s="180"/>
+      <c r="J4" s="180"/>
+      <c r="K4" s="180"/>
     </row>
     <row r="5" spans="1:13" ht="14">
-      <c r="A5" s="192"/>
-      <c r="B5" s="179">
+      <c r="A5" s="191"/>
+      <c r="B5" s="178">
         <v>2</v>
       </c>
-      <c r="C5" s="190">
+      <c r="C5" s="189">
         <v>3.7999999999999999E-2</v>
       </c>
-      <c r="D5" s="191">
+      <c r="D5" s="190">
         <f>D4+C5</f>
         <v>3.9699999999999999E-2</v>
       </c>
-      <c r="E5" s="187">
+      <c r="E5" s="186">
         <f>STDEV($D$2:D5)*SQRT(52)</f>
         <v>0.14096183880752977</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="14">
-      <c r="A6" s="192"/>
-      <c r="B6" s="179">
+      <c r="A6" s="191"/>
+      <c r="B6" s="178">
         <v>3</v>
       </c>
-      <c r="C6" s="190">
+      <c r="C6" s="189">
         <v>3.4200000000000001E-2</v>
       </c>
-      <c r="D6" s="191">
+      <c r="D6" s="190">
         <f t="shared" ref="D6:D11" si="0">D5+C6</f>
         <v>7.3899999999999993E-2</v>
       </c>
-      <c r="E6" s="187">
+      <c r="E6" s="186">
         <f>STDEV($D$2:D6)*SQRT(52)</f>
         <v>0.2384073824360311</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="14">
-      <c r="A7" s="192"/>
-      <c r="B7" s="179">
+      <c r="A7" s="191"/>
+      <c r="B7" s="178">
         <v>4</v>
       </c>
-      <c r="C7" s="190">
+      <c r="C7" s="189">
         <v>-3.0800000000000001E-2</v>
       </c>
-      <c r="D7" s="191">
+      <c r="D7" s="190">
         <f t="shared" si="0"/>
         <v>4.3099999999999992E-2</v>
       </c>
-      <c r="E7" s="187">
+      <c r="E7" s="186">
         <f>STDEV($D$2:D7)*SQRT(52)</f>
         <v>0.22121738328320101</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="14">
-      <c r="A8" s="192"/>
-      <c r="B8" s="179">
+      <c r="A8" s="191"/>
+      <c r="B8" s="178">
         <v>5</v>
       </c>
-      <c r="C8" s="190">
+      <c r="C8" s="189">
         <v>2.5499999999999998E-2</v>
       </c>
-      <c r="D8" s="191">
+      <c r="D8" s="190">
         <f t="shared" si="0"/>
         <v>6.8599999999999994E-2</v>
       </c>
-      <c r="E8" s="187">
+      <c r="E8" s="186">
         <f>STDEV($D$2:D8)*SQRT(52)</f>
         <v>0.23235565104259587</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="14">
-      <c r="A9" s="192"/>
-      <c r="B9" s="179">
+      <c r="A9" s="191"/>
+      <c r="B9" s="178">
         <v>6</v>
       </c>
-      <c r="C9" s="190">
+      <c r="C9" s="189">
         <v>5.5500000000000001E-2</v>
       </c>
-      <c r="D9" s="191">
+      <c r="D9" s="190">
         <f t="shared" si="0"/>
         <v>0.12409999999999999</v>
       </c>
-      <c r="E9" s="187">
+      <c r="E9" s="186">
         <f>STDEV($D$2:D9)*SQRT(52)</f>
         <v>0.31759423685847055</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="14">
-      <c r="A10" s="192"/>
-      <c r="B10" s="174">
+      <c r="A10" s="191"/>
+      <c r="B10" s="173">
         <v>7</v>
       </c>
-      <c r="C10" s="190">
+      <c r="C10" s="189">
         <v>5.8999999999999999E-3</v>
       </c>
-      <c r="D10" s="191">
+      <c r="D10" s="190">
         <f t="shared" si="0"/>
         <v>0.12999999999999998</v>
       </c>
-      <c r="E10" s="187">
+      <c r="E10" s="186">
         <f>STDEV($D$2:D10)*SQRT(52)</f>
         <v>0.36204596546724716</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="14">
-      <c r="A11" s="192"/>
-      <c r="B11" s="174">
+      <c r="A11" s="191"/>
+      <c r="B11" s="173">
         <v>8</v>
       </c>
-      <c r="C11" s="190">
+      <c r="C11" s="189">
         <v>-3.49E-2</v>
       </c>
-      <c r="D11" s="191">
+      <c r="D11" s="190">
         <f t="shared" si="0"/>
         <v>9.5099999999999976E-2</v>
       </c>
-      <c r="E11" s="187">
+      <c r="E11" s="186">
         <f>STDEV($D$2:D11)*SQRT(52)</f>
         <v>0.35429037180758316</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="14">
-      <c r="A12" s="192"/>
-      <c r="B12" s="179">
+      <c r="A12" s="191"/>
+      <c r="B12" s="178">
         <v>3</v>
       </c>
-      <c r="C12" s="190"/>
-      <c r="D12" s="191"/>
-      <c r="E12" s="193"/>
+      <c r="C12" s="189"/>
+      <c r="D12" s="190"/>
+      <c r="E12" s="192"/>
     </row>
     <row r="13" spans="1:13" ht="14">
-      <c r="A13" s="192"/>
-      <c r="B13" s="179">
+      <c r="A13" s="191"/>
+      <c r="B13" s="178">
         <v>4</v>
       </c>
-      <c r="C13" s="190"/>
-      <c r="D13" s="191"/>
-      <c r="E13" s="193"/>
+      <c r="C13" s="189"/>
+      <c r="D13" s="190"/>
+      <c r="E13" s="192"/>
     </row>
     <row r="14" spans="1:13" ht="14">
-      <c r="A14" s="192"/>
-      <c r="B14" s="179">
+      <c r="A14" s="191"/>
+      <c r="B14" s="178">
         <v>5</v>
       </c>
-      <c r="C14" s="190"/>
-      <c r="D14" s="191"/>
-      <c r="E14" s="193"/>
+      <c r="C14" s="189"/>
+      <c r="D14" s="190"/>
+      <c r="E14" s="192"/>
     </row>
     <row r="15" spans="1:13" ht="14">
-      <c r="A15" s="192"/>
-      <c r="B15" s="179">
+      <c r="A15" s="191"/>
+      <c r="B15" s="178">
         <v>6</v>
       </c>
-      <c r="C15" s="190"/>
-      <c r="D15" s="191"/>
-      <c r="E15" s="193"/>
+      <c r="C15" s="189"/>
+      <c r="D15" s="190"/>
+      <c r="E15" s="192"/>
     </row>
     <row r="16" spans="1:13" ht="14">
-      <c r="A16" s="192"/>
-      <c r="B16" s="174">
+      <c r="A16" s="191"/>
+      <c r="B16" s="173">
         <v>7</v>
       </c>
-      <c r="C16" s="190"/>
-      <c r="D16" s="191"/>
-      <c r="E16" s="193"/>
+      <c r="C16" s="189"/>
+      <c r="D16" s="190"/>
+      <c r="E16" s="192"/>
     </row>
     <row r="17" spans="1:5" ht="14">
-      <c r="A17" s="192"/>
-      <c r="B17" s="174">
+      <c r="A17" s="191"/>
+      <c r="B17" s="173">
         <v>8</v>
       </c>
-      <c r="C17" s="190"/>
-      <c r="D17" s="191"/>
-      <c r="E17" s="193"/>
+      <c r="C17" s="189"/>
+      <c r="D17" s="190"/>
+      <c r="E17" s="192"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -69290,29 +69506,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="205" t="s">
+      <c r="A1" s="204" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="B2" s="206">
+      <c r="B2" s="205">
         <v>45537</v>
       </c>
-      <c r="C2" s="204" t="s">
+      <c r="C2" s="203" t="s">
         <v>166</v>
       </c>
       <c r="D2">
         <v>9444</v>
       </c>
-      <c r="E2" s="204" t="s">
+      <c r="E2" s="203" t="s">
         <v>167</v>
       </c>
-      <c r="F2" s="204" t="s">
+      <c r="F2" s="203" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="D6" s="204"/>
+      <c r="D6" s="203"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -69322,10 +69538,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F51CD2FE-0785-5E4C-91F5-512BDFA3DC54}">
-  <dimension ref="B1:L27"/>
+  <dimension ref="B1:L28"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
@@ -69408,15 +69624,15 @@
       </c>
       <c r="I3" s="151" cm="1">
         <f t="array" aca="1" ref="I3" ca="1">_FV(B3,"Price")</f>
-        <v>57.98</v>
+        <v>58.8</v>
       </c>
       <c r="J3" s="131">
-        <f t="shared" ref="J3:J22" ca="1" si="0">((I3-F3)/F3)</f>
-        <v>-0.15665454545454549</v>
+        <f t="shared" ref="J3:J26" ca="1" si="0">((I3-F3)/F3)</f>
+        <v>-0.14472727272727276</v>
       </c>
       <c r="K3" s="172">
-        <f t="shared" ref="K3:K22" ca="1" si="1">(I3*G3) - H3</f>
-        <v>-78.511336000000028</v>
+        <f t="shared" ref="K3:K26" ca="1" si="1">(I3*G3) - H3</f>
+        <v>-72.536159999999995</v>
       </c>
       <c r="L3"/>
     </row>
@@ -69447,15 +69663,15 @@
       </c>
       <c r="I4" s="151" cm="1">
         <f t="array" aca="1" ref="I4" ca="1">_FV(B4,"Price")</f>
-        <v>128.77000000000001</v>
+        <v>142</v>
       </c>
       <c r="J4" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>0.28744251149770061</v>
+        <v>0.41971605678864232</v>
       </c>
       <c r="K4" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>144.00893000000008</v>
+        <v>210.27800000000002</v>
       </c>
       <c r="L4"/>
     </row>
@@ -69486,15 +69702,15 @@
       </c>
       <c r="I5" s="151" cm="1">
         <f t="array" aca="1" ref="I5" ca="1">_FV(B5,"Price")</f>
-        <v>19.329999999999998</v>
+        <v>19.97</v>
       </c>
       <c r="J5" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.11330275229357809</v>
+        <v>-8.3944954128440455E-2</v>
       </c>
       <c r="K5" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>-56.812064000000078</v>
+        <v>-42.105376000000035</v>
       </c>
       <c r="L5"/>
     </row>
@@ -69525,15 +69741,15 @@
       </c>
       <c r="I6" s="151" cm="1">
         <f t="array" aca="1" ref="I6" ca="1">_FV(B6,"Price")</f>
-        <v>22.17</v>
+        <v>22.1</v>
       </c>
       <c r="J6" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>0.26685714285714296</v>
+        <v>0.26285714285714296</v>
       </c>
       <c r="K6" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>147.61438800000008</v>
+        <v>145.56644000000006</v>
       </c>
       <c r="L6"/>
     </row>
@@ -69564,15 +69780,15 @@
       </c>
       <c r="I7" s="153" cm="1">
         <f t="array" aca="1" ref="I7" ca="1">_FV(B7,"Price")</f>
-        <v>222.5</v>
+        <v>221.45</v>
       </c>
       <c r="J7" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>0.26090898787260564</v>
+        <v>0.25495863085118431</v>
       </c>
       <c r="K7" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>130.71974999999998</v>
+        <v>127.73869500000001</v>
       </c>
       <c r="L7"/>
     </row>
@@ -69603,15 +69819,15 @@
       </c>
       <c r="I8" s="153" cm="1">
         <f t="array" aca="1" ref="I8" ca="1">_FV(B8,"Price")</f>
-        <v>87.38</v>
+        <v>89.67</v>
       </c>
       <c r="J8" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>0.55646597791236185</v>
+        <v>0.59725685785536164</v>
       </c>
       <c r="K8" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>278.72669200000007</v>
+        <v>299.16127800000004</v>
       </c>
       <c r="L8"/>
     </row>
@@ -69642,15 +69858,15 @@
       </c>
       <c r="I9" s="153" cm="1">
         <f t="array" aca="1" ref="I9" ca="1">_FV(B9,"Price")</f>
-        <v>18.7</v>
+        <v>19.8</v>
       </c>
       <c r="J9" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.44312090530077425</v>
+        <v>-0.41036331149493743</v>
       </c>
       <c r="K9" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>-221.97917000000001</v>
+        <v>-205.56617999999997</v>
       </c>
       <c r="L9"/>
     </row>
@@ -69681,15 +69897,15 @@
       </c>
       <c r="I10" s="155" cm="1">
         <f t="array" aca="1" ref="I10" ca="1">_FV(B10,"Price")</f>
-        <v>59.68</v>
+        <v>62.66</v>
       </c>
       <c r="J10" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>2.5429553264604755E-2</v>
+        <v>7.6632302405498176E-2</v>
       </c>
       <c r="K10" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>12.76124799999991</v>
+        <v>38.414875999999936</v>
       </c>
       <c r="L10"/>
     </row>
@@ -69720,15 +69936,15 @@
       </c>
       <c r="I11" s="155" cm="1">
         <f t="array" aca="1" ref="I11" ca="1">_FV(B11,"Price")</f>
-        <v>81.599999999999994</v>
+        <v>85.04</v>
       </c>
       <c r="J11" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.10594938095759836</v>
+        <v>-6.825901172345776E-2</v>
       </c>
       <c r="K11" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>-53.097600000000057</v>
+        <v>-34.215440000000001</v>
       </c>
       <c r="L11"/>
     </row>
@@ -69759,15 +69975,15 @@
       </c>
       <c r="I12" s="155" cm="1">
         <f t="array" aca="1" ref="I12" ca="1">_FV(B12,"Price")</f>
-        <v>96.41</v>
+        <v>96.85</v>
       </c>
       <c r="J12" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>0.15185185185185177</v>
+        <v>0.15710872162485054</v>
       </c>
       <c r="K12" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>76.062054999999987</v>
+        <v>78.695674999999937</v>
       </c>
       <c r="L12"/>
     </row>
@@ -69798,15 +70014,15 @@
       </c>
       <c r="I13" s="155" cm="1">
         <f t="array" aca="1" ref="I13" ca="1">_FV(B13,"Price")</f>
-        <v>90.93</v>
+        <v>95.25</v>
       </c>
       <c r="J13" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.22262118491920999</v>
+        <v>-0.18568863811233649</v>
       </c>
       <c r="K13" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>-111.53771699999999</v>
+        <v>-93.03472499999998</v>
       </c>
       <c r="L13"/>
     </row>
@@ -69837,15 +70053,15 @@
       </c>
       <c r="I14" s="157" cm="1">
         <f t="array" aca="1" ref="I14" ca="1">_FV(B14,"Price")</f>
-        <v>27.39</v>
+        <v>27.62</v>
       </c>
       <c r="J14" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>7.4539034915653279E-2</v>
+        <v>8.3562181247548162E-2</v>
       </c>
       <c r="K14" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>37.377839999999992</v>
+        <v>41.898720000000026</v>
       </c>
       <c r="L14"/>
     </row>
@@ -69876,15 +70092,15 @@
       </c>
       <c r="I15" s="157" cm="1">
         <f t="array" aca="1" ref="I15" ca="1">_FV(B15,"Price")</f>
-        <v>47.75</v>
+        <v>49.2</v>
       </c>
       <c r="J15" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>0.60720296196566803</v>
+        <v>0.65600807808818584</v>
       </c>
       <c r="K15" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>304.2416750000001</v>
+        <v>328.69404000000009</v>
       </c>
       <c r="L15"/>
     </row>
@@ -69915,15 +70131,15 @@
       </c>
       <c r="I16" s="157" cm="1">
         <f t="array" aca="1" ref="I16" ca="1">_FV(B16,"Price")</f>
-        <v>105.55</v>
+        <v>109.49</v>
       </c>
       <c r="J16" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>0.69612726980556006</v>
+        <v>0.75944078418769079</v>
       </c>
       <c r="K16" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>348.69861000000003</v>
+        <v>380.41639799999996</v>
       </c>
       <c r="L16"/>
     </row>
@@ -69954,15 +70170,15 @@
       </c>
       <c r="I17" s="157" cm="1">
         <f t="array" aca="1" ref="I17" ca="1">_FV(B17,"Price")</f>
-        <v>13.14</v>
+        <v>13.154999999999999</v>
       </c>
       <c r="J17" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>0.49828962371721791</v>
+        <v>0.5</v>
       </c>
       <c r="K17" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>249.42671400000006</v>
+        <v>250.28336549999995</v>
       </c>
       <c r="L17"/>
     </row>
@@ -69993,15 +70209,15 @@
       </c>
       <c r="I18" s="159" cm="1">
         <f t="array" aca="1" ref="I18" ca="1">_FV(B18,"Price")</f>
-        <v>37.67</v>
+        <v>38.32</v>
       </c>
       <c r="J18" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.2236191261335532</v>
+        <v>-0.21022258862324819</v>
       </c>
       <c r="K18" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>-108.44999999999993</v>
+        <v>-101.94999999999999</v>
       </c>
       <c r="L18"/>
     </row>
@@ -70032,15 +70248,15 @@
       </c>
       <c r="I19" s="159" cm="1">
         <f t="array" aca="1" ref="I19" ca="1">_FV(B19,"Price")</f>
-        <v>75.36</v>
+        <v>77.92</v>
       </c>
       <c r="J19" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>7.7340957827019247E-2</v>
+        <v>0.11393852751965687</v>
       </c>
       <c r="K19" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>37.879999999999995</v>
+        <v>55.800000000000068</v>
       </c>
       <c r="L19"/>
     </row>
@@ -70071,15 +70287,15 @@
       </c>
       <c r="I20" s="159" cm="1">
         <f t="array" aca="1" ref="I20" ca="1">_FV(B20,"Price")</f>
-        <v>58.05</v>
+        <v>60.454999999999998</v>
       </c>
       <c r="J20" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>-6.6420070762303038E-2</v>
+        <v>-2.7742039240913501E-2</v>
       </c>
       <c r="K20" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>-33.04000000000002</v>
+        <v>-13.800000000000011</v>
       </c>
       <c r="L20"/>
     </row>
@@ -70110,93 +70326,245 @@
       </c>
       <c r="I21" s="159" cm="1">
         <f t="array" aca="1" ref="I21" ca="1">_FV(B21,"Price")</f>
-        <v>9.86</v>
+        <v>10.35</v>
       </c>
       <c r="J21" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.264179104477612</v>
+        <v>-0.22761194029850751</v>
       </c>
       <c r="K21" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>-132.40361999999999</v>
+        <v>-114.08594999999997</v>
       </c>
       <c r="L21"/>
     </row>
     <row r="22" spans="2:12">
-      <c r="B22" s="135" t="e" vm="20">
+      <c r="B22" s="206" t="e" vm="20">
         <v>#VALUE!</v>
       </c>
-      <c r="C22" s="148" t="str" cm="1">
+      <c r="C22" s="211" t="str" cm="1">
         <f t="array" aca="1" ref="C22" ca="1">_FV(Portfolio[[#This Row],[Company]],"Name")</f>
         <v>ULTA BEAUTY, INC.</v>
       </c>
-      <c r="D22" s="149" t="str" cm="1">
+      <c r="D22" s="212" t="str" cm="1">
         <f t="array" aca="1" ref="D22" ca="1">_FV(B22,"Ticker symbol",TRUE)</f>
         <v>ULTA</v>
       </c>
-      <c r="E22" s="149" t="str" cm="1">
+      <c r="E22" s="212" t="str" cm="1">
         <f t="array" aca="1" ref="E22" ca="1">_FV(B22,"Industry")</f>
         <v>Specialty Retailers</v>
       </c>
-      <c r="F22" s="158">
+      <c r="F22" s="207">
         <v>393.4</v>
       </c>
-      <c r="G22" s="173">
+      <c r="G22" s="217">
         <v>1.28</v>
       </c>
-      <c r="H22" s="170">
+      <c r="H22" s="208">
         <v>503.56</v>
       </c>
-      <c r="I22" s="159" cm="1">
+      <c r="I22" s="213" cm="1">
         <f t="array" aca="1" ref="I22" ca="1">_FV(B22,"Price")</f>
-        <v>378.34</v>
+        <v>405.61</v>
       </c>
       <c r="J22" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>-3.8281647178444338E-2</v>
+        <v>3.1037112353838426E-2</v>
       </c>
       <c r="K22" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>-19.284800000000018</v>
+        <v>15.620799999999974</v>
       </c>
       <c r="L22"/>
     </row>
-    <row r="27" spans="2:12" ht="13">
-      <c r="K27" s="171">
-        <f ca="1">SUM(K3:K22)</f>
-        <v>952.40159500000016</v>
+    <row r="23" spans="2:12">
+      <c r="B23" s="214" t="e" vm="21">
+        <v>#VALUE!</v>
+      </c>
+      <c r="C23" s="214" t="str" cm="1">
+        <f t="array" aca="1" ref="C23" ca="1">_FV(Portfolio[[#This Row],[Company]],"Name")</f>
+        <v>INTERNATIONAL GAME TECHNOLOGY PLC</v>
+      </c>
+      <c r="D23" s="215" t="str" cm="1">
+        <f t="array" aca="1" ref="D23" ca="1">_FV(B23,"Ticker symbol",TRUE)</f>
+        <v>IGT</v>
+      </c>
+      <c r="E23" s="215" t="str" cm="1">
+        <f t="array" aca="1" ref="E23" ca="1">_FV(B23,"Industry")</f>
+        <v>Hotels &amp; Entertainment Services</v>
+      </c>
+      <c r="F23" s="209">
+        <v>22.26</v>
+      </c>
+      <c r="G23" s="218">
+        <v>22.506499999999999</v>
+      </c>
+      <c r="H23" s="210">
+        <v>501</v>
+      </c>
+      <c r="I23" s="216" cm="1">
+        <f t="array" aca="1" ref="I23" ca="1">_FV(B23,"Price")</f>
+        <v>22.27</v>
+      </c>
+      <c r="J23" s="131">
+        <f t="shared" ca="1" si="0"/>
+        <v>4.4923629829281264E-4</v>
+      </c>
+      <c r="K23" s="172">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.21975499999996373</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12">
+      <c r="B24" s="214" t="e" vm="22">
+        <v>#VALUE!</v>
+      </c>
+      <c r="C24" s="214" t="str" cm="1">
+        <f t="array" aca="1" ref="C24" ca="1">_FV(Portfolio[[#This Row],[Company]],"Name")</f>
+        <v>OIL-DRI CORPORATION OF AMERICA</v>
+      </c>
+      <c r="D24" s="215" t="str" cm="1">
+        <f t="array" aca="1" ref="D24" ca="1">_FV(B24,"Ticker symbol",TRUE)</f>
+        <v>ODC</v>
+      </c>
+      <c r="E24" s="215" t="str" cm="1">
+        <f t="array" aca="1" ref="E24" ca="1">_FV(B24,"Industry")</f>
+        <v>Chemicals</v>
+      </c>
+      <c r="F24" s="209">
+        <v>69.64</v>
+      </c>
+      <c r="G24" s="218">
+        <v>7.2146999999999997</v>
+      </c>
+      <c r="H24" s="210">
+        <v>500.99</v>
+      </c>
+      <c r="I24" s="216" cm="1">
+        <f t="array" aca="1" ref="I24" ca="1">_FV(B24,"Price")</f>
+        <v>69.510000000000005</v>
+      </c>
+      <c r="J24" s="131">
+        <f t="shared" ca="1" si="0"/>
+        <v>-1.8667432510051042E-3</v>
+      </c>
+      <c r="K24" s="172">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.50379700000002003</v>
+      </c>
+    </row>
+    <row r="25" spans="2:12">
+      <c r="B25" s="214" t="e" vm="23">
+        <v>#VALUE!</v>
+      </c>
+      <c r="C25" s="214" t="str" cm="1">
+        <f t="array" aca="1" ref="C25" ca="1">_FV(Portfolio[[#This Row],[Company]],"Name")</f>
+        <v>AXCELIS TECHNOLOGIES, INC.</v>
+      </c>
+      <c r="D25" s="215" t="str" cm="1">
+        <f t="array" aca="1" ref="D25" ca="1">_FV(B25,"Ticker symbol",TRUE)</f>
+        <v>ACLS</v>
+      </c>
+      <c r="E25" s="215" t="str" cm="1">
+        <f t="array" aca="1" ref="E25" ca="1">_FV(B25,"Industry")</f>
+        <v>Semiconductors &amp; Semiconductor Equipment</v>
+      </c>
+      <c r="F25" s="209">
+        <v>101.13</v>
+      </c>
+      <c r="G25" s="218">
+        <v>4.9541000000000004</v>
+      </c>
+      <c r="H25" s="210">
+        <v>500.99</v>
+      </c>
+      <c r="I25" s="216" cm="1">
+        <f t="array" aca="1" ref="I25" ca="1">_FV(B25,"Price")</f>
+        <v>101</v>
+      </c>
+      <c r="J25" s="131">
+        <f t="shared" ca="1" si="0"/>
+        <v>-1.2854741421931717E-3</v>
+      </c>
+      <c r="K25" s="172">
+        <f t="shared" ca="1" si="1"/>
+        <v>-0.62589999999994461</v>
+      </c>
+    </row>
+    <row r="26" spans="2:12">
+      <c r="B26" s="214" t="e" vm="24">
+        <v>#VALUE!</v>
+      </c>
+      <c r="C26" s="214" t="str" cm="1">
+        <f t="array" aca="1" ref="C26" ca="1">_FV(Portfolio[[#This Row],[Company]],"Name")</f>
+        <v>DELL TECHNOLOGIES INC.</v>
+      </c>
+      <c r="D26" s="215" t="str" cm="1">
+        <f t="array" aca="1" ref="D26" ca="1">_FV(B26,"Ticker symbol",TRUE)</f>
+        <v>DELL</v>
+      </c>
+      <c r="E26" s="215" t="str" cm="1">
+        <f t="array" aca="1" ref="E26" ca="1">_FV(B26,"Industry")</f>
+        <v>Computers, Phones &amp; Household Electronics</v>
+      </c>
+      <c r="F26" s="209">
+        <v>118.18</v>
+      </c>
+      <c r="G26" s="218">
+        <v>4.2393999999999998</v>
+      </c>
+      <c r="H26" s="210">
+        <v>501</v>
+      </c>
+      <c r="I26" s="216" cm="1">
+        <f t="array" aca="1" ref="I26" ca="1">_FV(B26,"Price")</f>
+        <v>118.501</v>
+      </c>
+      <c r="J26" s="131">
+        <f t="shared" ca="1" si="0"/>
+        <v>2.7161956337789636E-3</v>
+      </c>
+      <c r="K26" s="172">
+        <f t="shared" ca="1" si="1"/>
+        <v>1.3731394000000137</v>
+      </c>
+    </row>
+    <row r="28" spans="2:12" ht="13">
+      <c r="K28" s="171">
+        <f ca="1">SUM(K3:K26)</f>
+        <v>1296.7452478999999</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="J22">
-    <cfRule type="cellIs" dxfId="7" priority="3" operator="lessThan">
+  <conditionalFormatting sqref="J22:J26">
+    <cfRule type="cellIs" dxfId="13" priority="3" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="12" priority="4" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J3:K21">
-    <cfRule type="cellIs" dxfId="5" priority="7" operator="lessThan">
+    <cfRule type="cellIs" dxfId="19" priority="7" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="18" priority="8" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K22">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="lessThan">
+  <conditionalFormatting sqref="K22:K26">
+    <cfRule type="cellIs" dxfId="17" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="16" priority="2" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K27">
-    <cfRule type="cellIs" dxfId="1" priority="5" operator="lessThan">
+  <conditionalFormatting sqref="K28">
+    <cfRule type="cellIs" dxfId="15" priority="5" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="14" priority="6" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -70568,7 +70936,7 @@
     <col min="3" max="3" width="58.6640625" style="51" customWidth="1"/>
     <col min="4" max="4" width="47.83203125" style="51" customWidth="1"/>
     <col min="5" max="5" width="52.6640625" style="51" customWidth="1"/>
-    <col min="6" max="6" width="26.6640625" style="200" customWidth="1"/>
+    <col min="6" max="6" width="26.6640625" style="199" customWidth="1"/>
     <col min="7" max="16384" width="16.33203125" style="51"/>
   </cols>
   <sheetData>
@@ -70585,10 +70953,10 @@
       <c r="D1" s="52" t="s">
         <v>55</v>
       </c>
-      <c r="E1" s="196" t="s">
+      <c r="E1" s="195" t="s">
         <v>164</v>
       </c>
-      <c r="F1" s="197" t="s">
+      <c r="F1" s="196" t="s">
         <v>163</v>
       </c>
     </row>
@@ -70596,7 +70964,7 @@
       <c r="A2" s="53" t="s">
         <v>56</v>
       </c>
-      <c r="B2" s="195" t="s">
+      <c r="B2" s="194" t="s">
         <v>57</v>
       </c>
       <c r="C2" s="54" t="s">
@@ -70606,7 +70974,7 @@
         <v>58</v>
       </c>
       <c r="E2" s="56"/>
-      <c r="F2" s="198">
+      <c r="F2" s="197">
         <v>1.5E-3</v>
       </c>
     </row>
@@ -70614,7 +70982,7 @@
       <c r="A3" s="57" t="s">
         <v>59</v>
       </c>
-      <c r="B3" s="194" t="s">
+      <c r="B3" s="193" t="s">
         <v>57</v>
       </c>
       <c r="C3" s="59" t="s">
@@ -70624,61 +70992,61 @@
         <v>61</v>
       </c>
       <c r="E3" s="61"/>
-      <c r="F3" s="199"/>
+      <c r="F3" s="198"/>
     </row>
     <row r="4" spans="1:6" ht="24" customHeight="1">
       <c r="A4" s="57" t="s">
         <v>62</v>
       </c>
-      <c r="B4" s="194" t="s">
+      <c r="B4" s="193" t="s">
         <v>57</v>
       </c>
-      <c r="C4" s="194" t="s">
+      <c r="C4" s="193" t="s">
         <v>63</v>
       </c>
       <c r="D4" s="60" t="s">
         <v>64</v>
       </c>
       <c r="E4" s="61"/>
-      <c r="F4" s="199"/>
+      <c r="F4" s="198"/>
     </row>
     <row r="5" spans="1:6" ht="24" customHeight="1">
       <c r="A5" s="57" t="s">
         <v>65</v>
       </c>
-      <c r="B5" s="194" t="s">
+      <c r="B5" s="193" t="s">
         <v>57</v>
       </c>
-      <c r="C5" s="194" t="s">
+      <c r="C5" s="193" t="s">
         <v>66</v>
       </c>
       <c r="D5" s="60" t="s">
         <v>67</v>
       </c>
       <c r="E5" s="61"/>
-      <c r="F5" s="199"/>
+      <c r="F5" s="198"/>
     </row>
     <row r="6" spans="1:6" ht="24" customHeight="1">
       <c r="A6" s="57" t="s">
         <v>68</v>
       </c>
-      <c r="B6" s="194" t="s">
+      <c r="B6" s="193" t="s">
         <v>57</v>
       </c>
-      <c r="C6" s="194" t="s">
+      <c r="C6" s="193" t="s">
         <v>69</v>
       </c>
       <c r="D6" s="60" t="s">
         <v>70</v>
       </c>
       <c r="E6" s="61"/>
-      <c r="F6" s="199"/>
+      <c r="F6" s="198"/>
     </row>
     <row r="7" spans="1:6" ht="24" customHeight="1">
       <c r="A7" s="57" t="s">
         <v>71</v>
       </c>
-      <c r="B7" s="194" t="s">
+      <c r="B7" s="193" t="s">
         <v>57</v>
       </c>
       <c r="C7" s="62" t="s">
@@ -70688,16 +71056,16 @@
         <v>73</v>
       </c>
       <c r="E7" s="61"/>
-      <c r="F7" s="199"/>
+      <c r="F7" s="198"/>
     </row>
     <row r="8" spans="1:6" ht="24" customHeight="1">
       <c r="A8" s="57" t="s">
         <v>74</v>
       </c>
-      <c r="B8" s="194" t="s">
+      <c r="B8" s="193" t="s">
         <v>57</v>
       </c>
-      <c r="C8" s="194" t="s">
+      <c r="C8" s="193" t="s">
         <v>75</v>
       </c>
       <c r="D8" s="60" t="s">
@@ -70706,13 +71074,13 @@
       <c r="E8" s="63" t="s">
         <v>77</v>
       </c>
-      <c r="F8" s="199"/>
+      <c r="F8" s="198"/>
     </row>
     <row r="9" spans="1:6" ht="24" customHeight="1">
       <c r="A9" s="57" t="s">
         <v>78</v>
       </c>
-      <c r="B9" s="194" t="s">
+      <c r="B9" s="193" t="s">
         <v>79</v>
       </c>
       <c r="C9" s="59" t="s">
@@ -70722,16 +71090,16 @@
         <v>81</v>
       </c>
       <c r="E9" s="61"/>
-      <c r="F9" s="199"/>
+      <c r="F9" s="198"/>
     </row>
     <row r="10" spans="1:6" ht="24" customHeight="1">
       <c r="A10" s="57" t="s">
         <v>82</v>
       </c>
-      <c r="B10" s="194" t="s">
+      <c r="B10" s="193" t="s">
         <v>57</v>
       </c>
-      <c r="C10" s="194" t="s">
+      <c r="C10" s="193" t="s">
         <v>83</v>
       </c>
       <c r="D10" s="60" t="s">
@@ -70740,93 +71108,93 @@
       <c r="E10" s="63" t="s">
         <v>85</v>
       </c>
-      <c r="F10" s="199"/>
+      <c r="F10" s="198"/>
     </row>
     <row r="11" spans="1:6" ht="24" customHeight="1">
       <c r="A11" s="57" t="s">
         <v>86</v>
       </c>
-      <c r="B11" s="194" t="s">
+      <c r="B11" s="193" t="s">
         <v>57</v>
       </c>
-      <c r="C11" s="194" t="s">
+      <c r="C11" s="193" t="s">
         <v>87</v>
       </c>
       <c r="D11" s="60" t="s">
         <v>88</v>
       </c>
       <c r="E11" s="61"/>
-      <c r="F11" s="199"/>
+      <c r="F11" s="198"/>
     </row>
     <row r="12" spans="1:6" ht="24" customHeight="1">
       <c r="A12" s="57" t="s">
         <v>89</v>
       </c>
-      <c r="B12" s="194" t="s">
+      <c r="B12" s="193" t="s">
         <v>79</v>
       </c>
-      <c r="C12" s="194" t="s">
+      <c r="C12" s="193" t="s">
         <v>90</v>
       </c>
       <c r="D12" s="60" t="s">
         <v>91</v>
       </c>
       <c r="E12" s="61"/>
-      <c r="F12" s="199"/>
+      <c r="F12" s="198"/>
     </row>
     <row r="13" spans="1:6" ht="24" customHeight="1">
       <c r="A13" s="57" t="s">
         <v>92</v>
       </c>
-      <c r="B13" s="194" t="s">
+      <c r="B13" s="193" t="s">
         <v>57</v>
       </c>
-      <c r="C13" s="194" t="s">
+      <c r="C13" s="193" t="s">
         <v>93</v>
       </c>
       <c r="D13" s="60" t="s">
         <v>94</v>
       </c>
       <c r="E13" s="61"/>
-      <c r="F13" s="199"/>
+      <c r="F13" s="198"/>
     </row>
     <row r="14" spans="1:6" ht="24" customHeight="1">
       <c r="A14" s="57" t="s">
         <v>95</v>
       </c>
-      <c r="B14" s="194" t="s">
+      <c r="B14" s="193" t="s">
         <v>96</v>
       </c>
-      <c r="C14" s="194" t="s">
+      <c r="C14" s="193" t="s">
         <v>97</v>
       </c>
       <c r="D14" s="60" t="s">
         <v>98</v>
       </c>
       <c r="E14" s="61"/>
-      <c r="F14" s="199"/>
+      <c r="F14" s="198"/>
     </row>
     <row r="15" spans="1:6" ht="24" customHeight="1">
       <c r="A15" s="57" t="s">
         <v>99</v>
       </c>
-      <c r="B15" s="194" t="s">
+      <c r="B15" s="193" t="s">
         <v>79</v>
       </c>
-      <c r="C15" s="194" t="s">
+      <c r="C15" s="193" t="s">
         <v>100</v>
       </c>
       <c r="D15" s="60" t="s">
         <v>101</v>
       </c>
       <c r="E15" s="61"/>
-      <c r="F15" s="199"/>
+      <c r="F15" s="198"/>
     </row>
     <row r="16" spans="1:6" ht="24" customHeight="1">
       <c r="A16" s="57" t="s">
         <v>102</v>
       </c>
-      <c r="B16" s="194" t="s">
+      <c r="B16" s="193" t="s">
         <v>57</v>
       </c>
       <c r="C16" s="58" t="s">
@@ -70836,7 +71204,7 @@
         <v>103</v>
       </c>
       <c r="E16" s="56"/>
-      <c r="F16" s="198">
+      <c r="F16" s="197">
         <v>6.9999999999999999E-4</v>
       </c>
     </row>
@@ -70844,39 +71212,39 @@
       <c r="A17" s="57" t="s">
         <v>104</v>
       </c>
-      <c r="B17" s="194" t="s">
+      <c r="B17" s="193" t="s">
         <v>57</v>
       </c>
-      <c r="C17" s="194" t="s">
+      <c r="C17" s="193" t="s">
         <v>105</v>
       </c>
       <c r="D17" s="60" t="s">
         <v>133</v>
       </c>
       <c r="E17" s="61"/>
-      <c r="F17" s="199"/>
+      <c r="F17" s="198"/>
     </row>
     <row r="18" spans="1:6" ht="24" customHeight="1">
       <c r="A18" s="57" t="s">
         <v>147</v>
       </c>
-      <c r="B18" s="194" t="s">
+      <c r="B18" s="193" t="s">
         <v>57</v>
       </c>
-      <c r="C18" s="194" t="s">
+      <c r="C18" s="193" t="s">
         <v>148</v>
       </c>
       <c r="D18" s="60" t="s">
         <v>150</v>
       </c>
       <c r="E18" s="61"/>
-      <c r="F18" s="199"/>
+      <c r="F18" s="198"/>
     </row>
     <row r="19" spans="1:6" ht="24" customHeight="1">
       <c r="A19" s="57" t="s">
         <v>162</v>
       </c>
-      <c r="B19" s="194" t="s">
+      <c r="B19" s="193" t="s">
         <v>79</v>
       </c>
       <c r="C19" s="58" t="s">
@@ -70888,7 +71256,7 @@
       <c r="E19" s="61" t="s">
         <v>157</v>
       </c>
-      <c r="F19" s="199">
+      <c r="F19" s="198">
         <v>1.8E-3</v>
       </c>
     </row>
@@ -70896,7 +71264,7 @@
       <c r="A20" s="57" t="s">
         <v>151</v>
       </c>
-      <c r="B20" s="194" t="s">
+      <c r="B20" s="193" t="s">
         <v>79</v>
       </c>
       <c r="C20" s="58" t="s">
@@ -70906,7 +71274,7 @@
         <v>153</v>
       </c>
       <c r="E20" s="61"/>
-      <c r="F20" s="199">
+      <c r="F20" s="198">
         <v>1.1999999999999999E-3</v>
       </c>
     </row>
@@ -70914,7 +71282,7 @@
       <c r="A21" s="57" t="s">
         <v>159</v>
       </c>
-      <c r="B21" s="194" t="s">
+      <c r="B21" s="193" t="s">
         <v>57</v>
       </c>
       <c r="C21" s="58" t="s">
@@ -70924,12 +71292,12 @@
         <v>161</v>
       </c>
       <c r="E21" s="56"/>
-      <c r="F21" s="201">
+      <c r="F21" s="200">
         <v>6.9999999999999999E-4</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="24" customHeight="1">
-      <c r="F22" s="202">
+      <c r="F22" s="201">
         <f>(AVERAGE(F2:F21))</f>
         <v>1.1800000000000001E-3</v>
       </c>

</xml_diff>

<commit_message>
vault backup: 2024-09-18 20:35:39
</commit_message>
<xml_diff>
--- a/_system/Attachments/Portfolio Management.xlsx
+++ b/_system/Attachments/Portfolio Management.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martin/repos/tomesink/obsidian/_system/Attachments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2A66AF8-9D5C-0842-8C8E-8B2C6B2E771A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85E3B1DC-B524-1F4D-83E9-2128C4F45E20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="39000" yWindow="1720" windowWidth="31860" windowHeight="18860" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -69541,7 +69541,7 @@
   <dimension ref="B1:L28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="L27" sqref="L27"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>

</xml_diff>

<commit_message>
vault backup: 2024-09-19 14:15:02
</commit_message>
<xml_diff>
--- a/_system/Attachments/Portfolio Management.xlsx
+++ b/_system/Attachments/Portfolio Management.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martin/repos/tomesink/obsidian/_system/Attachments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85E3B1DC-B524-1F4D-83E9-2128C4F45E20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3ECE60A-E4F3-6749-AEDF-E91484D5C55C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39000" yWindow="1720" windowWidth="31860" windowHeight="18860" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="35840" yWindow="1360" windowWidth="23320" windowHeight="18860" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Stocks Performance" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
       </extLst>
     </bk>
   </futureMetadata>
-  <futureMetadata name="XLRICHVALUE" count="24">
+  <futureMetadata name="XLRICHVALUE" count="22">
     <bk>
       <extLst>
         <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
@@ -151,14 +151,14 @@
     <bk>
       <extLst>
         <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
-          <xlrd:rvb i="41"/>
+          <xlrd:rvb i="40"/>
         </ext>
       </extLst>
     </bk>
     <bk>
       <extLst>
         <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
-          <xlrd:rvb i="44"/>
+          <xlrd:rvb i="43"/>
         </ext>
       </extLst>
     </bk>
@@ -211,27 +211,13 @@
         </ext>
       </extLst>
     </bk>
-    <bk>
-      <extLst>
-        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
-          <xlrd:rvb i="67"/>
-        </ext>
-      </extLst>
-    </bk>
-    <bk>
-      <extLst>
-        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
-          <xlrd:rvb i="70"/>
-        </ext>
-      </extLst>
-    </bk>
   </futureMetadata>
   <cellMetadata count="1">
     <bk>
       <rc t="1" v="0"/>
     </bk>
   </cellMetadata>
-  <valueMetadata count="24">
+  <valueMetadata count="22">
     <bk>
       <rc t="2" v="0"/>
     </bk>
@@ -297,12 +283,6 @@
     </bk>
     <bk>
       <rc t="2" v="21"/>
-    </bk>
-    <bk>
-      <rc t="2" v="22"/>
-    </bk>
-    <bk>
-      <rc t="2" v="23"/>
     </bk>
   </valueMetadata>
 </metadata>
@@ -2215,7 +2195,67 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Per cent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="20">
+  <dxfs count="18">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -2580,86 +2620,6 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0"/>
@@ -4603,7 +4563,7 @@
 </file>
 
 <file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
-<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="71">
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="65">
   <rv s="0">
     <v>https://www.bing.com/financeapi/forcetrigger?t=a1qlnm&amp;q=XNYS%3aCVS&amp;form=skydnc</v>
     <v>Learn more on Bing</v>
@@ -4622,9 +4582,9 @@
     <v>Powered by Refinitiv</v>
     <v>83.25</v>
     <v>52.770499999999998</v>
-    <v>0.52610000000000001</v>
-    <v>0.97</v>
-    <v>1.6773E-2</v>
+    <v>0.52459999999999996</v>
+    <v>0.59</v>
+    <v>1.0201999999999999E-2</v>
     <v>USD</v>
     <v>CVS Health Corporation is a health solutions company. The Company operates in four segments: Health Care Benefits, Health Services, Pharmacy &amp; Consumer Wellness, and Corporate/Other. Its Health Care Benefits segment offer a range of traditional, voluntary and consumer-directed health insurance products and related services, including medical, pharmacy, dental and behavioral health plans, medical management capabilities, Medicare Advantage and Medicare supplement plans, and Medicaid health care management services. Its Health Services segment provides a full range of pharmacy benefit management solutions, delivers health care services in its medical clinics, virtually, and in the home, and offers provider enablement solutions. The Pharmacy &amp; Consumer Wellness segment dispenses prescriptions in its retail pharmacies and through its infusion operations, provides ancillary pharmacy services, including pharmacy patient care programs, diagnostic testing and vaccination administration.</v>
     <v>300000</v>
@@ -4635,20 +4595,20 @@
     <v>59.19</v>
     <v>Healthcare Providers &amp; Services</v>
     <v>Stock</v>
-    <v>45553.772598205469</v>
+    <v>45553.996098471878</v>
     <v>0</v>
     <v>57.746299999999998</v>
-    <v>73969165200</v>
+    <v>73491133180</v>
     <v>CVS HEALTH CORPORATION</v>
     <v>CVS HEALTH CORPORATION</v>
-    <v>57.93</v>
-    <v>10.2911</v>
+    <v>57.88</v>
+    <v>10.396100000000001</v>
     <v>57.83</v>
-    <v>58.8</v>
+    <v>58.42</v>
     <v>1257979000</v>
     <v>CVS</v>
     <v>CVS HEALTH CORPORATION (XNYS:CVS)</v>
-    <v>2693781</v>
+    <v>2291</v>
     <v>7701146</v>
     <v>1996</v>
   </rv>
@@ -4665,7 +4625,7 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>4</v>
+    <v>5</v>
     <v>en-GB</v>
     <v>a1qclh</v>
     <v>268435456</v>
@@ -4673,9 +4633,9 @@
     <v>Powered by Refinitiv</v>
     <v>165.32</v>
     <v>74</v>
-    <v>2.0015999999999998</v>
-    <v>3.57</v>
-    <v>2.5788999999999999E-2</v>
+    <v>2.0011000000000001</v>
+    <v>1.38</v>
+    <v>9.9690000000000004E-3</v>
     <v>USD</v>
     <v>Crocs, Inc. is engaged in the design, development, worldwide marketing, distribution, and sale of casual lifestyle footwear and accessories for women, men, and children. The Company’s segments include Crocs Brand and the HEYDUDE Brand. The Company’s Crocs Brand collection contains Croslite material, a molded footwear technology, delivering extraordinary comfort with each step. Its Croslite materials are formulated to create soft, comfortable, lightweight, non-marking, and odor-resistant footwear. The HEYDUDE Brand offers shoes with a versatile silhouette. It sells its products in more than 80 countries, through two distribution channels: wholesale and direct-to-consumer. Its wholesale channel includes domestic and international multi-brand retailers, mono-branded partner stores, e-tailers, and distributors; its direct-to-consumer channel includes Company-operated retail stores, Company-operated e-commerce sites, and third-party marketplaces.</v>
     <v>7030</v>
@@ -4683,23 +4643,23 @@
     <v>XNAS</v>
     <v>XNAS</v>
     <v>500 Eldorado Boulevard, Building 5, BROOMFIELD, CO, 80021 US</v>
-    <v>142</v>
+    <v>143</v>
     <v>Textiles &amp; Apparel</v>
     <v>Stock</v>
-    <v>45553.772601642966</v>
+    <v>45553.982780497659</v>
     <v>3</v>
     <v>138.2998</v>
-    <v>8432688460</v>
+    <v>8302635025</v>
     <v>CROCS, INC.</v>
     <v>CROCS, INC.</v>
     <v>138.53</v>
-    <v>10.5366</v>
+    <v>10.514799999999999</v>
     <v>138.43</v>
-    <v>142</v>
+    <v>139.81</v>
     <v>59385130</v>
     <v>CROX</v>
     <v>CROCS, INC. (XNAS:CROX)</v>
-    <v>442719</v>
+    <v>1337</v>
     <v>961370</v>
     <v>2005</v>
   </rv>
@@ -4716,7 +4676,7 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>4</v>
+    <v>5</v>
     <v>en-GB</v>
     <v>a25yfr</v>
     <v>268435456</v>
@@ -4724,9 +4684,9 @@
     <v>Powered by Refinitiv</v>
     <v>30.07</v>
     <v>17.71</v>
-    <v>1.5156000000000001</v>
-    <v>0.28999999999999998</v>
-    <v>1.4736000000000001E-2</v>
+    <v>1.5144</v>
+    <v>0.06</v>
+    <v>3.0490000000000001E-3</v>
     <v>USD</v>
     <v>Wabash National Corporation provides connected solutions for the transportation, logistics and distribution industries. The Company designs and manufactures products including dry freight and refrigerated trailers, platform trailers, tank trailers, dry and refrigerated truck bodies, structural composite panels and products, transportation, logistics, and distribution industry parts and services, and specialty food grade processing equipment. The Company’s Transportation Solutions (TS) segment comprises the design and manufacturing operations for the Company’s transportation-related equipment and products. This includes dry and refrigerated van trailers, platform trailers, tank trailers and truck-mounted tanks, truck-mounted dry and refrigerated truck bodies and EcoNex technology products. Its Parts &amp; Services (P&amp;S) segment is comprised of the Company’s parts and services businesses as well as the upfitting component of truck bodies business. It also includes DuraPlate composite panels.</v>
     <v>6700</v>
@@ -4737,20 +4697,20 @@
     <v>20.149699999999999</v>
     <v>Machinery, Equipment &amp; Components</v>
     <v>Stock</v>
-    <v>45553.772564513281</v>
+    <v>45553.958333333336</v>
     <v>6</v>
     <v>19.355</v>
-    <v>878664623</v>
+    <v>868544800</v>
     <v>WABASH NATIONAL CORPORATION</v>
     <v>WABASH NATIONAL CORPORATION</v>
-    <v>19.600000000000001</v>
-    <v>6.0369000000000002</v>
     <v>19.68</v>
-    <v>19.97</v>
+    <v>6.0552999999999999</v>
+    <v>19.68</v>
+    <v>19.739999999999998</v>
     <v>43999230</v>
     <v>WNC</v>
     <v>WABASH NATIONAL CORPORATION (XNYS:WNC)</v>
-    <v>204670</v>
+    <v>5</v>
     <v>437924</v>
     <v>1991</v>
   </rv>
@@ -4767,7 +4727,7 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>4</v>
+    <v>5</v>
     <v>en-GB</v>
     <v>a1pfoc</v>
     <v>268435456</v>
@@ -4775,9 +4735,9 @@
     <v>Powered by Refinitiv</v>
     <v>26.4</v>
     <v>16.12</v>
-    <v>1.0365</v>
-    <v>0.18</v>
-    <v>8.2120000000000005E-3</v>
+    <v>1.0366</v>
+    <v>-0.01</v>
+    <v>-4.5620000000000003E-4</v>
     <v>USD</v>
     <v>Perdoceo Education Corporation, through its academic institutions, offers quality postsecondary education primarily online to a diverse student population, along with campus-based and blended learning programs. The Company's academic institutions include Colorado Technical University (CTU) and the American InterContinental University System (AIUS), which provides degree programs from the associate through doctoral level as well as non-degree seeking and professional development programs. Its academic institutions offer students industry-relevant and career-focused academic programs. CTU offers academic programs in the career-oriented disciplines of business and management, nursing, healthcare management, computer science, engineering, information systems and technology, project management, cybersecurity and criminal justice. AIUS offers academic programs in the career-oriented disciplines of business studies, information technologies, education, health sciences and criminal justice.</v>
     <v>2319</v>
@@ -4785,23 +4745,23 @@
     <v>XNAS</v>
     <v>XNAS</v>
     <v>1750 E. GOLF ROAD, SCHAUMBURG, IL, 60173 US</v>
-    <v>22.11</v>
+    <v>22.16</v>
     <v>Miscellaneous Educational Service Providers</v>
     <v>Stock</v>
-    <v>45553.772572152346</v>
+    <v>45553.835491724218</v>
     <v>9</v>
-    <v>21.68</v>
-    <v>1451382803</v>
+    <v>21.67</v>
+    <v>1438904851</v>
     <v>PERDOCEO EDUCATION CORPORATION</v>
     <v>PERDOCEO EDUCATION CORPORATION</v>
     <v>21.87</v>
-    <v>10.7727</v>
+    <v>10.7677</v>
     <v>21.92</v>
-    <v>22.1</v>
+    <v>21.91</v>
     <v>65673430</v>
     <v>PRDO</v>
     <v>PERDOCEO EDUCATION CORPORATION (XNAS:PRDO)</v>
-    <v>111589</v>
+    <v>381075</v>
     <v>378012</v>
     <v>1994</v>
   </rv>
@@ -4826,9 +4786,9 @@
     <v>Powered by Refinitiv</v>
     <v>237.23</v>
     <v>164.07499999999999</v>
-    <v>1.2459</v>
-    <v>4.66</v>
-    <v>2.1495E-2</v>
+    <v>1.2446999999999999</v>
+    <v>3.9</v>
+    <v>1.7989999999999999E-2</v>
     <v>USD</v>
     <v>Apple Inc. designs, manufactures and markets smartphones, personal computers, tablets, wearables and accessories, and sells a variety of related services. Its product categories include iPhone, Mac, iPad, and Wearables, Home and Accessories. Its software platforms include iOS, iPadOS, macOS, watchOS, and tvOS. Its services include advertising, AppleCare, cloud services, digital content and payment services. It operates various platforms, including the App Store, that allow customers to discover and download applications and digital content, such as books, music, video, games and podcasts. It also offers digital content through subscription-based services, including Apple Arcade, Apple Fitness+, Apple Music, Apple News+ and Apple TV+. Its products include iPhone 15 Pro, iPhone 15, iPhone 14, iPhone 13, MacBook Air, MacBook Pro, iMac, Mac mini, Mac Studio, Mac Pro, and others. It also provides DarwinAI, which specializes in visual quality inspection using its Explainable AI platform.</v>
     <v>161000</v>
@@ -4836,23 +4796,23 @@
     <v>XNAS</v>
     <v>XNAS</v>
     <v>One Apple Park Way, CUPERTINO, CA, 95014 US</v>
-    <v>222.7</v>
+    <v>222.71</v>
     <v>Computers, Phones &amp; Household Electronics</v>
     <v>Stock</v>
-    <v>45553.772621296092</v>
+    <v>45553.999827233594</v>
     <v>12</v>
     <v>217.54</v>
-    <v>3366956803000</v>
+    <v>3355401656600</v>
     <v>APPLE INC.</v>
     <v>APPLE INC.</v>
-    <v>217.59</v>
-    <v>33.0075</v>
+    <v>217.55</v>
+    <v>33.601300000000002</v>
     <v>216.79</v>
-    <v>221.45</v>
+    <v>220.69</v>
     <v>15204140000</v>
     <v>AAPL</v>
     <v>APPLE INC. (XNAS:AAPL)</v>
-    <v>36917458</v>
+    <v>293419</v>
     <v>43841997</v>
     <v>1977</v>
   </rv>
@@ -4877,9 +4837,9 @@
     <v>Powered by Refinitiv</v>
     <v>92.82</v>
     <v>50.134999999999998</v>
-    <v>0.99219999999999997</v>
-    <v>1.21</v>
-    <v>1.3677999999999999E-2</v>
+    <v>0.99250000000000005</v>
+    <v>0.11</v>
+    <v>1.243E-3</v>
     <v>USD</v>
     <v>Allison Transmission Holdings, Inc. is a designer and manufacturer of propulsion solutions for commercial and defense vehicles. The Company is also a manufacturer of medium-and heavy-duty fully automatic transmissions. Its products are used in a variety of applications, including on-highway trucks, including distribution, refuse, construction, fire and emergency; buses, including school, transit and coach; motorhomes, off-highway vehicles, and equipment, including energy, mining and construction applications; and defense vehicles, including tactical wheeled and tracked. The Company operates in approximately 150 countries. The Company has manufacturing facilities in the United States, Hungary and India, as well as global engineering resources, including electrification engineering centers in Indianapolis, Indiana, Auburn Hills, Michigan and London in the United Kingdom. The Company also has approximately 1,600 independent distributor and dealer locations worldwide.</v>
     <v>3700</v>
@@ -4887,23 +4847,23 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>One Allison Way, INDIANAPOLIS, IN, 46222 US</v>
-    <v>90.064999999999998</v>
+    <v>90.34</v>
     <v>Machinery, Equipment &amp; Components</v>
     <v>Stock</v>
-    <v>45553.772465751565</v>
+    <v>45553.958333367969</v>
     <v>15</v>
-    <v>88.305000000000007</v>
-    <v>7813653699</v>
+    <v>88.35</v>
+    <v>7717802031</v>
     <v>ALLISON TRANSMISSION HOLDINGS, INC.</v>
     <v>ALLISON TRANSMISSION HOLDINGS, INC.</v>
-    <v>88.305000000000007</v>
-    <v>11.5671</v>
+    <v>88.6</v>
+    <v>11.5815</v>
     <v>88.46</v>
-    <v>89.67</v>
+    <v>88.57</v>
     <v>87137880</v>
     <v>ALSN</v>
     <v>ALLISON TRANSMISSION HOLDINGS, INC. (XNYS:ALSN)</v>
-    <v>158187</v>
+    <v>4</v>
     <v>484816</v>
     <v>2007</v>
   </rv>
@@ -4920,7 +4880,7 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>4</v>
+    <v>5</v>
     <v>en-GB</v>
     <v>az23tc</v>
     <v>268435456</v>
@@ -4929,8 +4889,8 @@
     <v>40.695</v>
     <v>18</v>
     <v>2.0013999999999998</v>
-    <v>0.4</v>
-    <v>2.0619000000000002E-2</v>
+    <v>-0.03</v>
+    <v>-1.5459999999999998E-3</v>
     <v>USD</v>
     <v>Par Pacific Holdings, Inc. is an energy company, which provides both renewable and conventional fuels to the western United States. It owns and operates 125,000 barrels per day of combined refining capacity across three locations and an energy infrastructure network, including 7.6 million barrels of storage, and marine, rail, rack and pipeline assets. The Company has three segments. Refining segment owns and operates four refineries with total operating crude oil throughput capacity of 219 thousand barrels per day (Mbpd). Retail segment operates fuel retail outlets in Hawaii, Washington and Idaho. It operates convenience stores and fuel retail sites under Hele and nomnom brands, 76 branded fuel retail sites and other sites operated by third parties that sell gasoline, diesel, and retail merchandise, such as soft drinks, prepared foods, and other sundries. Logistics segment operates a multi-modal logistics network spanning the Pacific, the Northwest, and the Rocky Mountain regions.</v>
     <v>1814</v>
@@ -4941,20 +4901,20 @@
     <v>19.920000000000002</v>
     <v>Oil &amp; Gas</v>
     <v>Stock</v>
-    <v>45553.772527106252</v>
+    <v>45553.958333356248</v>
     <v>18</v>
     <v>19.215</v>
-    <v>1115351226</v>
+    <v>1091128951</v>
     <v>PAR PACIFIC HOLDINGS, INC.</v>
     <v>PAR PACIFIC HOLDINGS, INC.</v>
-    <v>19.47</v>
-    <v>3.3801000000000001</v>
+    <v>19.46</v>
+    <v>3.3748</v>
     <v>19.399999999999999</v>
-    <v>19.8</v>
+    <v>19.37</v>
     <v>56330870</v>
     <v>PARR</v>
     <v>PAR PACIFIC HOLDINGS, INC. (XNYS:PARR)</v>
-    <v>279093</v>
+    <v>700399</v>
     <v>917565</v>
     <v>2005</v>
   </rv>
@@ -4971,7 +4931,7 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>4</v>
+    <v>5</v>
     <v>en-GB</v>
     <v>a1v177</v>
     <v>268435456</v>
@@ -4979,9 +4939,9 @@
     <v>Powered by Refinitiv</v>
     <v>84.44</v>
     <v>38.5</v>
-    <v>1.3098000000000001</v>
-    <v>1.78</v>
-    <v>2.9238E-2</v>
+    <v>1.3108</v>
+    <v>-0.56000000000000005</v>
+    <v>-9.1979999999999996E-3</v>
     <v>USD</v>
     <v>Hyster-Yale, Inc., formerly Hyster-Yale Materials Handling, Inc., through its wholly owned operating subsidiary, Hyster-Yale Materials Handling, designs, engineers, manufactures, sells, and services a comprehensive line of lift trucks, attachments, aftermarket parts and technology solutions marketed globally primarily under the Hyster and Yale brand names. The Company's business segments include Lift Trucks, Attachments and Fuel Cells. The Hyster-Yale Maximal brand provides trucks for customers requiring fundamental lift truck performance. The Lift Truck segment is focused on fuel cell-powered battery box replacements and integrated fuel cell engine solutions. Hyster- Yale’s attachment subsidiary, Bolzoni S.p.A., is a producer of attachments, forks, and lift tables under the Bolzoni, Auramo and Meyer brand names. The Fuel Cell business, Nuvera Fuel Cells, is an alternative-power technology company focused on fuel cell stacks and engines.</v>
     <v>8600</v>
@@ -4989,23 +4949,23 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>5875 LANDERBROOK DRIVE, SUITE 300, CLEVELAND, OH, 44124 US</v>
-    <v>62.66</v>
+    <v>62.87</v>
     <v>Machinery, Equipment &amp; Components</v>
     <v>Stock</v>
-    <v>45553.772321087497</v>
+    <v>45553.958333367969</v>
     <v>21</v>
     <v>59.82</v>
-    <v>1096622059</v>
+    <v>1055669368</v>
     <v>HYSTER-YALE, INC.</v>
     <v>HYSTER-YALE, INC.</v>
-    <v>60.7</v>
-    <v>6.0879000000000003</v>
+    <v>60.57</v>
+    <v>6.0319000000000003</v>
     <v>60.88</v>
-    <v>62.66</v>
+    <v>60.32</v>
     <v>17501150</v>
     <v>HY</v>
     <v>HYSTER-YALE, INC. (XNYS:HY)</v>
-    <v>23166</v>
+    <v>60370</v>
     <v>66473</v>
     <v>1999</v>
   </rv>
@@ -5022,17 +4982,17 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>4</v>
+    <v>5</v>
     <v>en-GB</v>
     <v>a1zvsm</v>
     <v>268435456</v>
     <v>1</v>
     <v>Powered by Refinitiv</v>
-    <v>108.02</v>
+    <v>107.955</v>
     <v>71.900000000000006</v>
     <v>1.5088999999999999</v>
-    <v>0.41</v>
-    <v>4.8449999999999995E-3</v>
+    <v>-1.1499999999999999</v>
+    <v>-1.3589E-2</v>
     <v>USD</v>
     <v>Polaris Inc. is engaged in designing, engineering, manufacturing and marketing of powersports vehicles. The Company also designs and manufactures or sources parts, garments and accessories (PG&amp;A), which includes aftermarket accessories and apparel. The Company operates through three segments: Off Road, On Road and Marine. The Off Road segment consists of off-road vehicles and snowmobiles. The On Road segment designs and manufactures motorcycles, moto-roadsters, light duty hauling, and passenger vehicles. The Marine segment designs and manufactures boats that are designed to compete in key segments of the recreational marine industry, specifically pontoon and deck boats. Its product line-up includes the RANGER, RZR and Polaris XPEDITION and GENERAL side-by-side off-road vehicles; Sportsman all-terrain off-road vehicles; military and commercial off-road vehicles; snowmobiles; Indian Motorcycle mid-size and heavyweight motorcycles; Slingshot moto-roadsters, and pontoon and deck boats.</v>
     <v>18500</v>
@@ -5040,23 +5000,23 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>2100 HIGHWAY 55, MEDINA, MN, 55340-9770 US</v>
-    <v>85.47</v>
+    <v>86.42</v>
     <v>Leisure Products</v>
     <v>Stock</v>
-    <v>45553.772465798436</v>
+    <v>45553.999334409375</v>
     <v>24</v>
-    <v>82.93</v>
-    <v>4740812471</v>
+    <v>82.6</v>
+    <v>4653845544</v>
     <v>Polaris Inc.</v>
     <v>Polaris Inc.</v>
-    <v>84.9</v>
-    <v>14.6676</v>
+    <v>84.92</v>
+    <v>14.6219</v>
     <v>84.63</v>
-    <v>85.04</v>
+    <v>83.48</v>
     <v>55748030</v>
     <v>PII</v>
     <v>Polaris Inc. (XNYS:PII)</v>
-    <v>197216</v>
+    <v>401026</v>
     <v>473923</v>
     <v>1994</v>
   </rv>
@@ -5073,7 +5033,7 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>4</v>
+    <v>5</v>
     <v>en-GB</v>
     <v>aw21cw</v>
     <v>268435456</v>
@@ -5082,8 +5042,8 @@
     <v>114.29989999999999</v>
     <v>75.430000000000007</v>
     <v>1.7418</v>
-    <v>1.1200000000000001</v>
-    <v>1.1699999999999999E-2</v>
+    <v>-1.4</v>
+    <v>-1.4624E-2</v>
     <v>USD</v>
     <v>CONSOL Energy Inc. is a producer and exporter of high-Btu bituminous thermal coal and metallurgical coal. It owns and operates longwall mining operations in the Northern Appalachian Basin. Its flagship operation is the Pennsylvania Mining Complex, located over 26 miles southwest of Pittsburgh, near the city of Washington and the borough of Waynesburg all in Pennsylvania, and consists of three deep longwall mining operations: the Bailey Mine, the Enlow Fork Mine and the Harvey Mine, as well as a centralized preparation plant. Its segments include the PAMC and the CONSOL Marine Terminal. The PAMC includes the Bailey Mine, the Enlow Fork Mine, the Harvey Mine and a centralized preparation plant. The PAMC segment's principal activities include the mining, preparation and marketing of bituminous coal, sold primarily to industrial end-users, metallurgical end-users and power generators. The CONSOL Marine Terminal segment provides coal export terminal services through the Port of Baltimore.</v>
     <v>2020</v>
@@ -5091,23 +5051,23 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>275 TECHNOLOGY DRIVE, SUITE #101, CANONSBURG, PA, 15317 US</v>
-    <v>96.85</v>
+    <v>96.97</v>
     <v>Coal</v>
     <v>Stock</v>
-    <v>45553.77259641172</v>
+    <v>45553.958333356248</v>
     <v>27</v>
     <v>93.41</v>
-    <v>2846734325</v>
+    <v>2772663385</v>
     <v>CONSOL ENERGY INC.</v>
     <v>CONSOL ENERGY INC.</v>
-    <v>95.86</v>
-    <v>7.1458000000000004</v>
+    <v>96.2</v>
+    <v>7.0412999999999997</v>
     <v>95.73</v>
-    <v>96.85</v>
+    <v>94.33</v>
     <v>29393230</v>
     <v>CEIX</v>
     <v>CONSOL ENERGY INC. (XNYS:CEIX)</v>
-    <v>157351</v>
+    <v>20</v>
     <v>487441</v>
     <v>2017</v>
   </rv>
@@ -5132,9 +5092,9 @@
     <v>Powered by Refinitiv</v>
     <v>127.3484</v>
     <v>84.35</v>
-    <v>1.2470000000000001</v>
-    <v>2.54</v>
-    <v>2.7397000000000001E-2</v>
+    <v>1.2448999999999999</v>
+    <v>1.04</v>
+    <v>1.1217999999999999E-2</v>
     <v>USD</v>
     <v>AGCO Corporation is a designer, manufacturer and distributor of agricultural machinery and precision agriculture technology. The Company sells a range of agricultural equipment, including tractors, combines, self-propelled sprayers, hay tools, forage equipment, seeding and tillage equipment, implements, and grain storage and protein production systems. It provides telemetry-based fleet management tools, including remote monitoring and diagnostics, which help farmers improve uptime, machine and yield optimization, mixed fleet optimization and decision support. The Company's Precision Planting, Headsight and Intelligent Ag Solutions brands provide retrofit solutions to upgrade farmers existing equipment to improve their planting, liquid application and harvest operations. The Company’s Precision Planting, Headsight, JCA and Intelligent Ag Solutions brands also sell precision agriculture solutions around the crop cycle to third party original equipment manufacturers (OEMs).</v>
     <v>27900</v>
@@ -5142,23 +5102,23 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>4205 River Green Pkway, DULUTH, GA, 30096 US</v>
-    <v>95.28</v>
+    <v>96</v>
     <v>Machinery, Equipment &amp; Components</v>
     <v>Stock</v>
-    <v>45553.77254563594</v>
+    <v>45553.958333356248</v>
     <v>30</v>
     <v>92.734999999999999</v>
-    <v>7109679075</v>
+    <v>6997715625</v>
     <v>AGCO CORPORATION</v>
     <v>AGCO CORPORATION</v>
-    <v>92.79</v>
-    <v>16.5151</v>
+    <v>92.85</v>
+    <v>16.700299999999999</v>
     <v>92.71</v>
-    <v>95.25</v>
+    <v>93.75</v>
     <v>74642300</v>
     <v>AGCO</v>
     <v>AGCO CORPORATION (XNYS:AGCO)</v>
-    <v>208389</v>
+    <v>362</v>
     <v>774131</v>
     <v>1991</v>
   </rv>
@@ -5175,7 +5135,7 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>4</v>
+    <v>5</v>
     <v>en-GB</v>
     <v>a1vuw7</v>
     <v>268435456</v>
@@ -5183,9 +5143,9 @@
     <v>Powered by Refinitiv</v>
     <v>30.1</v>
     <v>24.01</v>
-    <v>1.1549</v>
-    <v>0.27</v>
-    <v>9.8719999999999988E-3</v>
+    <v>1.1547000000000001</v>
+    <v>0.05</v>
+    <v>1.828E-3</v>
     <v>USD</v>
     <v>Ituran Location and Control Ltd. is a provider of location-based services, consisting of stolen vehicle recovery (SVR), fleet management services and other tracking services. The Company also provides wireless communication products used in connection with its location-based services and various other applications. Its operations consist of two segments: location-based services and wireless communications products. Its location-based services segment consists of its SVR and tracking services, fleet management and value-added services consisted of personal locater services and concierge services. Its wireless communications products segment consists of short and medium range two-way machine-to-machine wireless communications products that are used for various applications, including automatic vehicle location (AVL) and automatic vehicle identification. It primarily provides its services, as well as sells and leases its products in Israel, Brazil, Argentina and the United States.</v>
     <v>2841</v>
@@ -5196,127 +5156,25 @@
     <v>27.76</v>
     <v>Communications &amp; Networking</v>
     <v>Stock</v>
-    <v>45553.772053437497</v>
+    <v>45553.833346967185</v>
     <v>33</v>
     <v>27.252500000000001</v>
-    <v>549460679</v>
+    <v>545084092</v>
     <v>ITURAN LOCATION AND CONTROL LTD.</v>
     <v>ITURAN LOCATION AND CONTROL LTD.</v>
     <v>27.28</v>
-    <v>10.711499999999999</v>
+    <v>10.7311</v>
     <v>27.35</v>
-    <v>27.62</v>
+    <v>27.4</v>
     <v>19893580</v>
     <v>ITRN</v>
     <v>ITURAN LOCATION AND CONTROL LTD. (XNAS:ITRN)</v>
-    <v>59626</v>
+    <v>75499</v>
     <v>82057</v>
     <v>1994</v>
   </rv>
   <rv s="2">
     <v>34</v>
-  </rv>
-  <rv s="0">
-    <v>https://www.bing.com/financeapi/forcetrigger?t=bgowlh&amp;q=XNAS%3aFTDR&amp;form=skydnc</v>
-    <v>Learn more on Bing</v>
-  </rv>
-  <rv s="1">
-    <v>0</v>
-    <v>FRONTDOOR, INC. (XNAS:FTDR)</v>
-    <v>2</v>
-    <v>3</v>
-    <v>Finance</v>
-    <v>4</v>
-    <v>en-GB</v>
-    <v>bgowlh</v>
-    <v>268435456</v>
-    <v>1</v>
-    <v>Powered by Refinitiv</v>
-    <v>49.4</v>
-    <v>28.254999999999999</v>
-    <v>1.0365</v>
-    <v>0.41</v>
-    <v>8.4030000000000007E-3</v>
-    <v>USD</v>
-    <v>Frontdoor, Inc. is a provider of home warranties in the United States. The Company’s customizable home warranties help customers protect and maintain their homes, typically their assets, from costly and unplanned breakdowns of essential home systems and appliances. The Company operates under the brands American Home Shield, HSA, OneGuard and Landmark Home Warranty. Its annual service subscribe plan covers the repair or replacement of major components of more than 20 home systems and appliances, including electrical, plumbing, heating, ventilation, and air conditioning (HVAC) systems, water heaters, refrigerators, dishwashers, and ranges/ovens/cooktops, as well as optional coverages for electronics, pools, spas, and pumps. Its operations also include its Streem, a technology platform that uses augmented reality, computer vision and machine learning to, among other things, help home service professionals more quickly and accurately diagnose breakdowns and complete repairs.</v>
-    <v>1716</v>
-    <v>Nasdaq Stock Market</v>
-    <v>XNAS</v>
-    <v>XNAS</v>
-    <v>3400 PLAYERS CLUB PARKWAY, STE. 300, MEMPHIS, TN, 38125 US</v>
-    <v>49.4</v>
-    <v>Personal &amp; Household Products &amp; Services</v>
-    <v>Stock</v>
-    <v>45553.772605613281</v>
-    <v>36</v>
-    <v>48.35</v>
-    <v>3765007368</v>
-    <v>FRONTDOOR, INC.</v>
-    <v>FRONTDOOR, INC.</v>
-    <v>48.79</v>
-    <v>18.840499999999999</v>
-    <v>48.79</v>
-    <v>49.2</v>
-    <v>76524540</v>
-    <v>FTDR</v>
-    <v>FRONTDOOR, INC. (XNAS:FTDR)</v>
-    <v>288404</v>
-    <v>633339</v>
-    <v>2018</v>
-  </rv>
-  <rv s="2">
-    <v>37</v>
-  </rv>
-  <rv s="0">
-    <v>https://www.bing.com/financeapi/forcetrigger?t=a1x1pr&amp;q=XNAS%3aLNTH&amp;form=skydnc</v>
-    <v>Learn more on Bing</v>
-  </rv>
-  <rv s="1">
-    <v>0</v>
-    <v>LANTHEUS HOLDINGS, INC. (XNAS:LNTH)</v>
-    <v>2</v>
-    <v>3</v>
-    <v>Finance</v>
-    <v>4</v>
-    <v>en-GB</v>
-    <v>a1x1pr</v>
-    <v>268435456</v>
-    <v>1</v>
-    <v>Powered by Refinitiv</v>
-    <v>126.8899</v>
-    <v>50.2</v>
-    <v>0.50160000000000005</v>
-    <v>3.95</v>
-    <v>3.7427000000000002E-2</v>
-    <v>USD</v>
-    <v>Lantheus Holdings, Inc. is a radiopharmaceutical-focused company engaged in delivering science to enable clinicians to find, fight and follow disease to deliver patient outcomes. The Company classifies its products in three categories: Radiopharmaceutical Oncology, Precision Diagnostics, and Strategic Partnerships. Its Radiopharmaceutical Oncology diagnostics and therapeutic candidates help healthcare professionals (HCPs) find, fight, and follow cancer, with a focus in prostate cancer. Its pipeline also includes breast and other cancers. Its Precision Diagnostic products assist HCPs to find and follow diseases, with a focus in cardiology. Its Strategic Partnerships focus on enabling precision medicine through the use of biomarkers, digital solutions and pharma solutions platforms. Its commercial products include PYLARIFY, DEFINITY, Ga-DOTA-RM2, and others. Its pipeline includes B amyloid positron emission tomography (PET) imaging agent, NAV-4694, also known as F18-flutafuranol.</v>
-    <v>834</v>
-    <v>Nasdaq Stock Market</v>
-    <v>XNAS</v>
-    <v>XNAS</v>
-    <v>331 Treble Cove Rd, NORTH BILLERICA, MA, 01862 US</v>
-    <v>109.94</v>
-    <v>Healthcare Equipment &amp; Supplies</v>
-    <v>Stock</v>
-    <v>45553.772584316408</v>
-    <v>39</v>
-    <v>104.5</v>
-    <v>7601960773</v>
-    <v>LANTHEUS HOLDINGS, INC.</v>
-    <v>LANTHEUS HOLDINGS, INC.</v>
-    <v>104.99</v>
-    <v>17.283100000000001</v>
-    <v>105.54</v>
-    <v>109.49</v>
-    <v>69430640</v>
-    <v>LNTH</v>
-    <v>LANTHEUS HOLDINGS, INC. (XNAS:LNTH)</v>
-    <v>286067</v>
-    <v>718116</v>
-    <v>2007</v>
-  </rv>
-  <rv s="2">
-    <v>40</v>
   </rv>
   <rv s="0">
     <v>https://www.bing.com/financeapi/forcetrigger?t=a1sea2&amp;q=XNYS%3aEVRI&amp;form=skydnc</v>
@@ -5328,17 +5186,17 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>4</v>
+    <v>5</v>
     <v>en-GB</v>
     <v>a1sea2</v>
     <v>268435456</v>
     <v>1</v>
     <v>Powered by Refinitiv</v>
-    <v>14.91</v>
+    <v>14.62</v>
     <v>6.37</v>
-    <v>2.1511999999999998</v>
-    <v>1.4999999999999999E-2</v>
-    <v>1.142E-3</v>
+    <v>2.15</v>
+    <v>0.04</v>
+    <v>3.0439999999999998E-3</v>
     <v>USD</v>
     <v>Everi Holdings Inc. develops and offers products and services that provide gaming entertainment, improve its customers’ patron engagement, and help its casino customers operate their businesses. It develops and supplies entertaining game content, gaming machines and gaming systems and services for land-based and iGaming operators. It operates through two segments: Games and Financial Technology Solutions (FinTech). The Games segment provides gaming operators with gaming technology and entertainment products and services, including gaming machines, primarily comprising Class II, Class III and Historic Horse Racing slot machines placed under participation and fixed-fee lease arrangements or sold to casino customers. The FinTech segment provides gaming operators with financial technology products and services, including financial access and related services supporting digital, cashless and physical cash options across mobile, assisted and self-service channels.</v>
     <v>2200</v>
@@ -5346,36 +5204,36 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>7250 S Tenaya Way Ste 100, LAS VEGAS, NV, 89113-2175 US</v>
-    <v>13.16</v>
+    <v>13.19</v>
     <v>Hotels &amp; Entertainment Services</v>
     <v>Stock</v>
-    <v>45553.772542522653</v>
-    <v>42</v>
+    <v>45553.958333367969</v>
+    <v>36</v>
     <v>13.14</v>
-    <v>1122431694</v>
+    <v>1124564784</v>
     <v>EVERI HOLDINGS INC.</v>
     <v>EVERI HOLDINGS INC.</v>
-    <v>13.15</v>
-    <v>27.908200000000001</v>
+    <v>13.16</v>
+    <v>27.993099999999998</v>
     <v>13.14</v>
-    <v>13.154999999999999</v>
+    <v>13.18</v>
     <v>85323580</v>
     <v>EVRI</v>
     <v>EVERI HOLDINGS INC. (XNYS:EVRI)</v>
-    <v>326168</v>
+    <v>499</v>
     <v>863655</v>
     <v>2004</v>
   </rv>
   <rv s="2">
-    <v>43</v>
+    <v>37</v>
   </rv>
   <rv s="3">
-    <v>5</v>
+    <v>6</v>
     <v>NEXTRACKER INC. (XNAS:NXT)</v>
-    <v>6</v>
+    <v>7</v>
     <v>3</v>
     <v>Finance</v>
-    <v>4</v>
+    <v>5</v>
     <v>en-GB</v>
     <v>c8ssgh</v>
     <v>268435456</v>
@@ -5384,8 +5242,8 @@
     <v>62.31</v>
     <v>32.14</v>
     <v>2.1230000000000002</v>
-    <v>0.98</v>
-    <v>2.6244999999999997E-2</v>
+    <v>-0.5</v>
+    <v>-1.3389999999999999E-2</v>
     <v>USD</v>
     <v>Nextracker Inc. is a provider of integrated solar tracker and software solutions used in utility-scale and ground-mounted distributed generation solar projects. Its products enable solar panels in utility-scale power plants to follow the sun’s movement across the sky and optimize plant performance. Its products include NX Horizon, NX Gemini, TrueCapture, and NX Navigator. Its solutions include Bifacial PV modules, Large Format Modules, and First Solar Series 6 (FSLR6) Modules. NX Horizon is a one-in-portrait (1P) smart solar tracker system that delivers the lowest levelized cost of energy (LCOE). NX Gemini is its two-in-portrait (2P) format tracker which holds two rows of solar panels along the central support beam. TrueCapture is its flagship software offering, which is a self-adjusting tracker control system that uses machine learning to enhance solar power plant energy yield. It has operations in the United States, Brazil, Mexico, Spain, India, Australia, the Middle East and Brazil.</v>
     <v>1050</v>
@@ -5393,27 +5251,27 @@
     <v>XNAS</v>
     <v>XNAS</v>
     <v>6200 Paseo Padre Pkwy, FREMONT, CA, 94555 US</v>
-    <v>38.32</v>
+    <v>38.83</v>
     <v>Renewable Energy</v>
     <v>Stock</v>
-    <v>45553.772578217191</v>
-    <v>36.729999999999997</v>
-    <v>5569712368</v>
+    <v>45553.995709883595</v>
+    <v>36.704999999999998</v>
+    <v>5354598216</v>
     <v>NEXTRACKER INC.</v>
     <v>NEXTRACKER INC.</v>
     <v>37.340000000000003</v>
-    <v>9.9099000000000004</v>
+    <v>9.7772000000000006</v>
     <v>37.340000000000003</v>
-    <v>38.32</v>
+    <v>36.840000000000003</v>
     <v>145347400</v>
     <v>NXT</v>
     <v>NEXTRACKER INC. (XNAS:NXT)</v>
-    <v>1947977</v>
+    <v>4254</v>
     <v>2850986</v>
     <v>2022</v>
   </rv>
   <rv s="2">
-    <v>45</v>
+    <v>39</v>
   </rv>
   <rv s="0">
     <v>https://www.bing.com/financeapi/forcetrigger?t=a1xejc&amp;q=XNAS%3aMCRI&amp;form=skydnc</v>
@@ -5425,7 +5283,7 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>4</v>
+    <v>5</v>
     <v>en-GB</v>
     <v>a1xejc</v>
     <v>268435456</v>
@@ -5433,9 +5291,9 @@
     <v>Powered by Refinitiv</v>
     <v>80.22</v>
     <v>56.25</v>
-    <v>1.7428999999999999</v>
-    <v>1.71</v>
-    <v>2.2438E-2</v>
+    <v>1.7425999999999999</v>
+    <v>0.25</v>
+    <v>3.2799999999999999E-3</v>
     <v>USD</v>
     <v>Monarch Casino &amp; Resort, Inc. owns and operates the Atlantis Casino Resort Spa, a hotel and casino in Reno, Nevada (the Atlantis) and the Monarch Casino Resort Spa Black Hawk (the Monarch Black Hawk), a hotel and casino in Black Hawk, Colorado. In addition, it owns separate parcels of land located next to the Atlantis and a parcel of land with an industrial warehouse located between Denver, Colorado, and Monarch Black Hawk. The Atlantis is located approximately three miles south of downtown, which features approximately 61,000 square feet of casino space; 817 guest rooms and suites; eight food outlets; two gourmet coffee and pastry bars and one snack bar; a 30,000 square-foot health spa and salon with an enclosed year-round pool. Monarch Black Hawk features approximately 60,000 square feet of casino space; approximately 1,000 slot machines; approximately 43 table games; a live poker room; a keno counter and a sports book. The resort also includes 10 bars and lounges.</v>
     <v>2900</v>
@@ -5443,28 +5301,28 @@
     <v>XNAS</v>
     <v>XNAS</v>
     <v>Executive Offices, 3800 S Virginia Street, RENO, NV, 89502 US</v>
-    <v>77.92</v>
+    <v>78.16</v>
     <v>Hotels &amp; Entertainment Services</v>
     <v>Stock</v>
-    <v>45553.772504606248</v>
-    <v>47</v>
+    <v>45553.846688113284</v>
+    <v>41</v>
     <v>75.27</v>
-    <v>1437789190</v>
+    <v>1410849095</v>
     <v>MONARCH CASINO &amp; RESORT, INC.</v>
     <v>MONARCH CASINO &amp; RESORT, INC.</v>
     <v>75.98</v>
-    <v>17.8096</v>
+    <v>17.867999999999999</v>
     <v>76.209999999999994</v>
-    <v>77.92</v>
+    <v>76.459999999999994</v>
     <v>18452120</v>
     <v>MCRI</v>
     <v>MONARCH CASINO &amp; RESORT, INC. (XNAS:MCRI)</v>
-    <v>82801</v>
+    <v>141398</v>
     <v>100560</v>
     <v>1993</v>
   </rv>
   <rv s="2">
-    <v>48</v>
+    <v>42</v>
   </rv>
   <rv s="0">
     <v>https://www.bing.com/financeapi/forcetrigger?t=a1xqm7&amp;q=XNYS%3aMLR&amp;form=skydnc</v>
@@ -5476,7 +5334,7 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>4</v>
+    <v>5</v>
     <v>en-GB</v>
     <v>a1xqm7</v>
     <v>268435456</v>
@@ -5484,9 +5342,9 @@
     <v>Powered by Refinitiv</v>
     <v>69.75</v>
     <v>34.96</v>
-    <v>0.97289999999999999</v>
-    <v>1.675</v>
-    <v>2.8496E-2</v>
+    <v>0.97099999999999997</v>
+    <v>1.22</v>
+    <v>2.0754999999999999E-2</v>
     <v>USD</v>
     <v>Miller Industries, Inc. is a manufacturer of towing and recovery equipment. The Company designs and manufactures bodies of car carriers and wreckers, which are installed on chassis manufactured by third parties, and sold to its customers. Its products are marketed and sold through a network of distributors that serve all 50 states, Canada, Mexico, and other foreign markets, and through prime contractors to governmental entities. In addition to selling its products, its independent distributors provide end-users with parts and service. Its product line includes car carriers, wreckers, and transport trailers. Car carriers are specialized flat-bed vehicles with hydraulic tilt mechanisms that enable a towing operator to drive or winch a vehicle onto the bed for transport. Its multi-vehicle transport trailers are specialized auto transport trailers with upper and lower decks and hydraulic ramps for loading vehicles. Its brands include Century, Vulcan, Chevron, Holmes, and Challenger.</v>
     <v>1821</v>
@@ -5494,28 +5352,28 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>Ste 100, 8503 Hilltop Dr, OOLTEWAH, TN, 37363 US</v>
-    <v>60.454999999999998</v>
+    <v>60.91</v>
     <v>Automobiles &amp; Auto Parts</v>
     <v>Stock</v>
-    <v>45553.772410462501</v>
-    <v>50</v>
-    <v>58.77</v>
-    <v>692438874</v>
+    <v>45553.958333356248</v>
+    <v>44</v>
+    <v>58.6</v>
+    <v>687227400</v>
     <v>MILLER INDUSTRIES, INC.</v>
     <v>MILLER INDUSTRIES, INC.</v>
-    <v>59.05</v>
-    <v>9.4627999999999997</v>
+    <v>58.83</v>
+    <v>9.6592000000000002</v>
     <v>58.78</v>
-    <v>60.454999999999998</v>
+    <v>60</v>
     <v>11453790</v>
     <v>MLR</v>
     <v>MILLER INDUSTRIES, INC. (XNYS:MLR)</v>
-    <v>24625</v>
+    <v>80869</v>
     <v>86198</v>
     <v>1994</v>
   </rv>
   <rv s="2">
-    <v>51</v>
+    <v>45</v>
   </rv>
   <rv s="0">
     <v>https://www.bing.com/financeapi/forcetrigger?t=btavh7&amp;q=XNYS%3aJBI&amp;form=skydnc</v>
@@ -5527,7 +5385,7 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>4</v>
+    <v>5</v>
     <v>en-GB</v>
     <v>btavh7</v>
     <v>268435456</v>
@@ -5536,8 +5394,8 @@
     <v>15.86</v>
     <v>9.1649999999999991</v>
     <v>0.89490000000000003</v>
-    <v>0.09</v>
-    <v>8.7720000000000003E-3</v>
+    <v>-0.25</v>
+    <v>-2.4365999999999999E-2</v>
     <v>USD</v>
     <v>Janus International Group, Inc. is a global manufacturer and supplier of turn-key self-storage, commercial and industrial building solutions. It operates through two geographic segments: Janus North America and Janus International. The Janus North America segment is comprised of all the other entities, including Janus International Group, LLC, Betco, Inc., Noke, Inc., Asta Industries, Inc., DBCI, LLC, Access Control Technologies, LLC, Janus Door, LLC, and Steel Door Depot.com, LLC. The Janus International segment is comprised of Janus International Europe Holdings Ltd. (UK). Its production and sales are in Europe and Australia. It provides facility and door automation and access control technologies, roll up and swing doors, hallway systems and relocatable storage moveable additional storage structures (MASS) units. It is comprised of three sales channels, including New Construction-Self-storage, R3-Self-storage, and Commercial and Other. It also provides terminal maintenance services.</v>
     <v>1956</v>
@@ -5545,28 +5403,28 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>135 Janus International Blvd., TEMPLE, GA, 30179 US</v>
-    <v>10.4</v>
+    <v>10.46</v>
     <v>Homebuilding &amp; Construction Supplies</v>
     <v>Stock</v>
-    <v>45553.772548992965</v>
-    <v>53</v>
-    <v>10.11</v>
-    <v>1504084770</v>
+    <v>45553.958333356248</v>
+    <v>47</v>
+    <v>10.01</v>
+    <v>1454675222</v>
     <v>JANUS INTERNATIONAL GROUP, INC.</v>
     <v>JANUS INTERNATIONAL GROUP, INC.</v>
-    <v>10.29</v>
-    <v>11.5047</v>
+    <v>10.3</v>
+    <v>11.224399999999999</v>
     <v>10.26</v>
-    <v>10.35</v>
+    <v>10.01</v>
     <v>145322200</v>
     <v>JBI</v>
     <v>JANUS INTERNATIONAL GROUP, INC. (XNYS:JBI)</v>
-    <v>544015</v>
+    <v>1787162</v>
     <v>2091493</v>
     <v>2020</v>
   </rv>
   <rv s="2">
-    <v>54</v>
+    <v>48</v>
   </rv>
   <rv s="0">
     <v>https://www.bing.com/financeapi/forcetrigger?t=a24war&amp;q=XNAS%3aULTA&amp;form=skydnc</v>
@@ -5578,7 +5436,7 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>4</v>
+    <v>5</v>
     <v>en-GB</v>
     <v>a24war</v>
     <v>268435456</v>
@@ -5586,9 +5444,9 @@
     <v>Powered by Refinitiv</v>
     <v>574.76</v>
     <v>318.17</v>
-    <v>1.3</v>
-    <v>8.61</v>
-    <v>2.1687999999999999E-2</v>
+    <v>1.2955000000000001</v>
+    <v>5.72</v>
+    <v>1.4408000000000001E-2</v>
     <v>USD</v>
     <v>Ulta Beauty, Inc. is a beauty retailer. The Company's product categories include cosmetics, skincare, haircare products and styling tools, fragrance and bath, services, and accessories and other. The Company has one segment, which includes retail stores, salon services, and e-commerce. It offers a range of beauty services in its stores, focusing on hair, makeup, brow and skin services. Its skin services include a skin treatment room or dedicated skin treatment area on the sales floor. Its Ulta Beauty store prototype includes an open salon area, with most of its stores offering brow services on the salon floor. It offers a new way to shop for beauty - bringing together All Things Beauty, All in One Place. In addition to ship to home order fulfillment, it offers guests Buy Online, Pick-up in Store, Curbside Pickup, and Store 2 Door, which provides the ability for customers to order in-store and have products delivered to their homes. It operates over 1,350 retail stores across 50 states.</v>
     <v>20000</v>
@@ -5596,28 +5454,28 @@
     <v>XNAS</v>
     <v>XNAS</v>
     <v>1000 Remington Blvd, Suite 120, BOLINGBROOK, IL, 60440 US</v>
-    <v>405.87</v>
+    <v>408.74</v>
     <v>Specialty Retailers</v>
     <v>Stock</v>
-    <v>45553.772602650002</v>
-    <v>56</v>
+    <v>45553.99901368047</v>
+    <v>50</v>
     <v>397.38</v>
-    <v>19110205635</v>
+    <v>18974044065</v>
     <v>ULTA BEAUTY, INC.</v>
     <v>ULTA BEAUTY, INC.</v>
-    <v>398</v>
-    <v>15.9413</v>
+    <v>397.4</v>
+    <v>16.170999999999999</v>
     <v>397</v>
-    <v>405.61</v>
+    <v>402.72</v>
     <v>47114730</v>
     <v>ULTA</v>
     <v>ULTA BEAUTY, INC. (XNAS:ULTA)</v>
-    <v>769082</v>
+    <v>2626</v>
     <v>1657712</v>
     <v>2016</v>
   </rv>
   <rv s="2">
-    <v>57</v>
+    <v>51</v>
   </rv>
   <rv s="0">
     <v>https://www.bing.com/financeapi/forcetrigger?t=a1vehw&amp;q=XNYS%3aIGT&amp;form=skydnc</v>
@@ -5629,17 +5487,17 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>4</v>
+    <v>5</v>
     <v>en-GB</v>
     <v>a1vehw</v>
     <v>268435456</v>
     <v>1</v>
     <v>Powered by Refinitiv</v>
-    <v>32.909999999999997</v>
+    <v>32.6</v>
     <v>18.899999999999999</v>
     <v>1.9702</v>
-    <v>0.45</v>
-    <v>2.0622999999999999E-2</v>
+    <v>0.09</v>
+    <v>4.1250000000000002E-3</v>
     <v>USD</v>
     <v>International Game Technology PLC is a United Kingdom-based company, which is engaged in gaming. The Company operates and provides an integrated portfolio of gaming technology products and services, including online and instant lottery systems, iLottery, instant ticket printing, lottery management services, commercial services, gaming systems, electronic gaming machines, iGaming, and sports betting. The Company operates through three segments. The Global Lottery segment operates traditional lottery and iLottery businesses across the world, which includes sales, operations, product development, technology, and support, across the world. The Global Gaming segment operates a land-based gaming business across the world, which includes sales, product management, studios, global manufacturing, operation, and technology, across the world. The Digital &amp; Betting segment operates iGaming and sports betting activities across the world.</v>
     <v>11000</v>
@@ -5647,28 +5505,28 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>10 Finsbury Square, Third Floor, LONDON, UNITED KINGDOM-NA, EC2A 1AF GB</v>
-    <v>22.34</v>
+    <v>22.39</v>
     <v>Hotels &amp; Entertainment Services</v>
     <v>Stock</v>
-    <v>45553.772503830471</v>
-    <v>59</v>
+    <v>45553.958333367969</v>
+    <v>53</v>
     <v>21.78</v>
-    <v>4454000000</v>
+    <v>4382000000</v>
     <v>INTERNATIONAL GAME TECHNOLOGY PLC</v>
     <v>INTERNATIONAL GAME TECHNOLOGY PLC</v>
+    <v>21.83</v>
+    <v>21.198</v>
+    <v>21.82</v>
     <v>21.91</v>
-    <v>21.110900000000001</v>
-    <v>21.82</v>
-    <v>22.27</v>
     <v>200000000</v>
     <v>IGT</v>
     <v>INTERNATIONAL GAME TECHNOLOGY PLC (XNYS:IGT)</v>
-    <v>334254</v>
+    <v>816456</v>
     <v>635397</v>
     <v>2014</v>
   </rv>
   <rv s="2">
-    <v>60</v>
+    <v>54</v>
   </rv>
   <rv s="0">
     <v>https://www.bing.com/financeapi/forcetrigger?t=a1z3ec&amp;q=XNYS%3aODC&amp;form=skydnc</v>
@@ -5680,7 +5538,7 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>4</v>
+    <v>5</v>
     <v>en-GB</v>
     <v>a1z3ec</v>
     <v>268435456</v>
@@ -5689,8 +5547,8 @@
     <v>87.32</v>
     <v>54.8</v>
     <v>0.58589999999999998</v>
-    <v>0.87</v>
-    <v>1.2675000000000001E-2</v>
+    <v>-0.79</v>
+    <v>-1.1509E-2</v>
     <v>USD</v>
     <v>Oil-Dri Corporation of America is a manufacturer and supplier of specialty sorbent products for pet care, animal health and nutrition, fluid purification, agricultural ingredients, sports field, industrial and automotive markets. Its principal product is cat litter. The Company’s Retail and Wholesale Products Group segment customers include mass merchandisers, the farm and fleet channel, drugstore chains, pet specialty retail outlets, dollar stores, retail grocery stores, distributors of industrial cleanup and automotive products, environmental service companies, sports field product users and marketers of consumer products. Its Business to Business Products Group segment customers include processors and refiners of edible oils, renewable diesel, petroleum-based oils and biodiesel fuel; manufacturers of animal feed and agricultural chemicals; and distributors of animal health and nutrition products. It is also a supplier of silica gel-based crystal cat litter.</v>
     <v>884</v>
@@ -5701,25 +5559,25 @@
     <v>69.510000000000005</v>
     <v>Chemicals</v>
     <v>Stock</v>
-    <v>45553.771617580467</v>
-    <v>62</v>
-    <v>68.459999999999994</v>
+    <v>45553.958333344533</v>
+    <v>56</v>
+    <v>67.709999999999994</v>
     <v>500133200</v>
     <v>OIL-DRI CORPORATION OF AMERICA</v>
     <v>OIL-DRI CORPORATION OF AMERICA</v>
-    <v>68.459999999999994</v>
-    <v>14.085800000000001</v>
+    <v>68.47</v>
+    <v>13.9237</v>
     <v>68.64</v>
-    <v>69.510000000000005</v>
+    <v>67.849999999999994</v>
     <v>7286320</v>
     <v>ODC</v>
     <v>OIL-DRI CORPORATION OF AMERICA (XNYS:ODC)</v>
-    <v>5454</v>
+    <v>15719</v>
     <v>15891</v>
     <v>1969</v>
   </rv>
   <rv s="2">
-    <v>63</v>
+    <v>57</v>
   </rv>
   <rv s="0">
     <v>https://www.bing.com/financeapi/forcetrigger?t=a1mt9c&amp;q=XNAS%3aACLS&amp;form=skydnc</v>
@@ -5731,7 +5589,7 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>4</v>
+    <v>5</v>
     <v>en-GB</v>
     <v>a1mt9c</v>
     <v>268435456</v>
@@ -5739,9 +5597,9 @@
     <v>Powered by Refinitiv</v>
     <v>170.9692</v>
     <v>93.77</v>
-    <v>1.5901000000000001</v>
-    <v>1.23</v>
-    <v>1.2327999999999999E-2</v>
+    <v>1.5933999999999999</v>
+    <v>-1.93</v>
+    <v>-1.9344E-2</v>
     <v>USD</v>
     <v>Axcelis Technologies, Inc. designs, manufactures and services ion implantation and other processing equipment used in the fabrication of semiconductor chips. The Company offers a complete line of high energy, high current and medium current implanters for all application requirements. In addition to equipment, the Company provides extensive aftermarket lifecycle products and services, including used tools, spare parts, equipment upgrades, maintenance services and customer training. Its Purion flagship systems are all based on a common platform, which enables a combination of implant purity, precision and productivity. Combining a single wafer end station, with advanced spot beam architectures (that ensures all points across the wafer see the same beam condition at the same beam angle), Purion products enable process control to optimize device performance and yield, at high productivity. The Company sells its products to semiconductor chip manufacturers around the world.</v>
     <v>1620</v>
@@ -5752,25 +5610,25 @@
     <v>101.82</v>
     <v>Semiconductors &amp; Semiconductor Equipment</v>
     <v>Stock</v>
-    <v>45553.772599015625</v>
-    <v>65</v>
-    <v>98.3</v>
-    <v>3294376590</v>
+    <v>45553.980763853906</v>
+    <v>59</v>
+    <v>97.64</v>
+    <v>3191305005</v>
     <v>AXCELIS TECHNOLOGIES, INC.</v>
     <v>AXCELIS TECHNOLOGIES, INC.</v>
     <v>101.01</v>
-    <v>13.784700000000001</v>
+    <v>13.4796</v>
     <v>99.77</v>
-    <v>101</v>
+    <v>97.84</v>
     <v>32617590</v>
     <v>ACLS</v>
     <v>AXCELIS TECHNOLOGIES, INC. (XNAS:ACLS)</v>
-    <v>301555</v>
+    <v>121</v>
     <v>517965</v>
     <v>1995</v>
   </rv>
   <rv s="2">
-    <v>66</v>
+    <v>60</v>
   </rv>
   <rv s="0">
     <v>https://www.bing.com/financeapi/forcetrigger?t=a1retc&amp;q=XNYS%3aDELL&amp;form=skydnc</v>
@@ -5790,9 +5648,9 @@
     <v>Powered by Refinitiv</v>
     <v>179.7</v>
     <v>63.9</v>
-    <v>0.89510000000000001</v>
-    <v>1.681</v>
-    <v>1.439E-2</v>
+    <v>0.89570000000000005</v>
+    <v>-0.83</v>
+    <v>-7.1050000000000002E-3</v>
     <v>USD</v>
     <v>Dell Technologies Inc. is engaged in designing, developing, manufacturing, marketing, selling, and supporting a wide range of comprehensive and integrated solutions, products, and services. The Company operates through two segments: Infrastructure Solutions Group (ISG) and Client Solutions Group (CSG). Its ISG segment enables the Company’s customer’s digital transformation with solutions that address artificial intelligence (AI), machine learning, data analytics, and multi cloud environments. Its comprehensive storage portfolio includes modern and traditional storage solutions, including all-flash arrays, scale-out file, object platforms, hyper-converged infrastructure, and software-defined storage. Its CSG segment offers branded personal computers (PCs) including notebooks, desktops, and workstations and branded peripherals that include displays, docking stations, keyboards, mice, and webcam and audio devices, as well as third-party software and peripherals.</v>
     <v>120000</v>
@@ -5803,25 +5661,25 @@
     <v>119.62</v>
     <v>Computers, Phones &amp; Household Electronics</v>
     <v>Stock</v>
-    <v>45553.772594108596</v>
-    <v>68</v>
-    <v>116.57</v>
-    <v>83233301184</v>
+    <v>45553.99987446719</v>
+    <v>62</v>
+    <v>115.94</v>
+    <v>81469612952</v>
     <v>DELL TECHNOLOGIES INC.</v>
     <v>DELL TECHNOLOGIES INC.</v>
-    <v>117.56</v>
-    <v>21.6111</v>
+    <v>117.58</v>
+    <v>21.342400000000001</v>
     <v>116.82</v>
-    <v>118.501</v>
+    <v>115.99</v>
     <v>702384800</v>
     <v>DELL</v>
     <v>DELL TECHNOLOGIES INC. (XNYS:DELL)</v>
-    <v>7170560</v>
+    <v>89231</v>
     <v>11513168</v>
     <v>2013</v>
   </rv>
   <rv s="2">
-    <v>69</v>
+    <v>63</v>
   </rv>
 </rvData>
 </file>
@@ -6016,7 +5874,7 @@
       <v t="s">%ProviderInfo</v>
     </a>
   </spbArrays>
-  <spbData count="7">
+  <spbData count="8">
     <spb s="0">
       <v>0</v>
       <v>Name</v>
@@ -6060,6 +5918,13 @@
       <v>from previous close</v>
       <v>from previous close</v>
       <v>Source: Nasdaq Last Sale</v>
+      <v>GMT</v>
+    </spb>
+    <spb s="4">
+      <v>Delayed 15 minutes</v>
+      <v>from previous close</v>
+      <v>from previous close</v>
+      <v>Source: Nasdaq</v>
       <v>GMT</v>
     </spb>
     <spb s="5">
@@ -6192,29 +6057,29 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4AEE35AE-5B0D-FE48-BB2D-FD669C9DCA16}" name="Portfolio" displayName="Portfolio" ref="B2:K26" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="B2:K26" xr:uid="{4AEE35AE-5B0D-FE48-BB2D-FD669C9DCA16}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4AEE35AE-5B0D-FE48-BB2D-FD669C9DCA16}" name="Portfolio" displayName="Portfolio" ref="B2:K24" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+  <autoFilter ref="B2:K24" xr:uid="{4AEE35AE-5B0D-FE48-BB2D-FD669C9DCA16}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{0445D94A-6FCB-7D4D-96B6-8AA18900F668}" name="Company" dataDxfId="9"/>
-    <tableColumn id="8" xr3:uid="{D4CC5B63-9F41-F843-9F6B-16BF8366EF76}" name="Name" dataDxfId="8">
+    <tableColumn id="1" xr3:uid="{0445D94A-6FCB-7D4D-96B6-8AA18900F668}" name="Company" dataDxfId="15"/>
+    <tableColumn id="8" xr3:uid="{D4CC5B63-9F41-F843-9F6B-16BF8366EF76}" name="Name" dataDxfId="14">
       <calculatedColumnFormula array="1">_FV(Portfolio[[#This Row],[Company]],"Name")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{B02ADEDD-E393-8F47-A86F-790F7D8AC135}" name="Ticker" dataDxfId="7">
+    <tableColumn id="2" xr3:uid="{B02ADEDD-E393-8F47-A86F-790F7D8AC135}" name="Ticker" dataDxfId="13">
       <calculatedColumnFormula array="1">_FV(B3,"Ticker symbol",TRUE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{DAB4D9A1-3A8B-F941-8C60-3B2546DAB540}" name="Industry" dataDxfId="6">
+    <tableColumn id="3" xr3:uid="{DAB4D9A1-3A8B-F941-8C60-3B2546DAB540}" name="Industry" dataDxfId="12">
       <calculatedColumnFormula array="1">_FV(B3,"Industry")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{2480957A-208E-8047-AEFC-5888351C1175}" name="Purchase" dataDxfId="5"/>
-    <tableColumn id="9" xr3:uid="{C19D84FB-40D7-E444-83AC-793DDFB09317}" name="Amount" dataDxfId="4"/>
-    <tableColumn id="10" xr3:uid="{0339281E-B096-D14D-B83F-1032AB2E4CB5}" name="Cost" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{633C3CE6-95BE-E743-869D-E0D6471E5EDB}" name="Current Price" dataDxfId="2">
+    <tableColumn id="4" xr3:uid="{2480957A-208E-8047-AEFC-5888351C1175}" name="Purchase" dataDxfId="11"/>
+    <tableColumn id="9" xr3:uid="{C19D84FB-40D7-E444-83AC-793DDFB09317}" name="Amount" dataDxfId="10"/>
+    <tableColumn id="10" xr3:uid="{0339281E-B096-D14D-B83F-1032AB2E4CB5}" name="Cost" dataDxfId="9"/>
+    <tableColumn id="6" xr3:uid="{633C3CE6-95BE-E743-869D-E0D6471E5EDB}" name="Current Price" dataDxfId="8">
       <calculatedColumnFormula array="1">_FV(B3,"Price")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{0C4F3DBA-8ADF-A44E-971F-127F7DF8311F}" name="Change" dataDxfId="1">
+    <tableColumn id="5" xr3:uid="{0C4F3DBA-8ADF-A44E-971F-127F7DF8311F}" name="Change" dataDxfId="7">
       <calculatedColumnFormula>((I3-F3)/F3)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{A51F63E4-8280-4643-84C4-E673A52345D6}" name="Profit/Loss" dataDxfId="0">
+    <tableColumn id="11" xr3:uid="{A51F63E4-8280-4643-84C4-E673A52345D6}" name="Profit/Loss" dataDxfId="6">
       <calculatedColumnFormula>(I3*G3) - H3</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -69538,10 +69403,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F51CD2FE-0785-5E4C-91F5-512BDFA3DC54}">
-  <dimension ref="B1:L28"/>
+  <dimension ref="B1:L26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
@@ -69624,15 +69489,15 @@
       </c>
       <c r="I3" s="151" cm="1">
         <f t="array" aca="1" ref="I3" ca="1">_FV(B3,"Price")</f>
-        <v>58.8</v>
+        <v>58.42</v>
       </c>
       <c r="J3" s="131">
-        <f t="shared" ref="J3:J26" ca="1" si="0">((I3-F3)/F3)</f>
-        <v>-0.14472727272727276</v>
+        <f t="shared" ref="J3:J24" ca="1" si="0">((I3-F3)/F3)</f>
+        <v>-0.15025454545454542</v>
       </c>
       <c r="K3" s="172">
-        <f t="shared" ref="K3:K26" ca="1" si="1">(I3*G3) - H3</f>
-        <v>-72.536159999999995</v>
+        <f t="shared" ref="K3:K24" ca="1" si="1">(I3*G3) - H3</f>
+        <v>-75.305143999999984</v>
       </c>
       <c r="L3"/>
     </row>
@@ -69663,15 +69528,15 @@
       </c>
       <c r="I4" s="151" cm="1">
         <f t="array" aca="1" ref="I4" ca="1">_FV(B4,"Price")</f>
-        <v>142</v>
+        <v>139.81</v>
       </c>
       <c r="J4" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>0.41971605678864232</v>
+        <v>0.39782043591281752</v>
       </c>
       <c r="K4" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>210.27800000000002</v>
+        <v>199.30829000000006</v>
       </c>
       <c r="L4"/>
     </row>
@@ -69702,15 +69567,15 @@
       </c>
       <c r="I5" s="151" cm="1">
         <f t="array" aca="1" ref="I5" ca="1">_FV(B5,"Price")</f>
-        <v>19.97</v>
+        <v>19.739999999999998</v>
       </c>
       <c r="J5" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>-8.3944954128440455E-2</v>
+        <v>-9.44954128440368E-2</v>
       </c>
       <c r="K5" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>-42.105376000000035</v>
+        <v>-47.390592000000083</v>
       </c>
       <c r="L5"/>
     </row>
@@ -69741,15 +69606,15 @@
       </c>
       <c r="I6" s="151" cm="1">
         <f t="array" aca="1" ref="I6" ca="1">_FV(B6,"Price")</f>
-        <v>22.1</v>
+        <v>21.91</v>
       </c>
       <c r="J6" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>0.26285714285714296</v>
+        <v>0.252</v>
       </c>
       <c r="K6" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>145.56644000000006</v>
+        <v>140.00772399999994</v>
       </c>
       <c r="L6"/>
     </row>
@@ -69780,15 +69645,15 @@
       </c>
       <c r="I7" s="153" cm="1">
         <f t="array" aca="1" ref="I7" ca="1">_FV(B7,"Price")</f>
-        <v>221.45</v>
+        <v>220.69</v>
       </c>
       <c r="J7" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>0.25495863085118431</v>
+        <v>0.25065170576901274</v>
       </c>
       <c r="K7" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>127.73869500000001</v>
+        <v>125.58097900000007</v>
       </c>
       <c r="L7"/>
     </row>
@@ -69819,15 +69684,15 @@
       </c>
       <c r="I8" s="153" cm="1">
         <f t="array" aca="1" ref="I8" ca="1">_FV(B8,"Price")</f>
-        <v>89.67</v>
+        <v>88.57</v>
       </c>
       <c r="J8" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>0.59725685785536164</v>
+        <v>0.57766298539365857</v>
       </c>
       <c r="K8" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>299.16127800000004</v>
+        <v>289.34553800000003</v>
       </c>
       <c r="L8"/>
     </row>
@@ -69858,15 +69723,15 @@
       </c>
       <c r="I9" s="153" cm="1">
         <f t="array" aca="1" ref="I9" ca="1">_FV(B9,"Price")</f>
-        <v>19.8</v>
+        <v>19.37</v>
       </c>
       <c r="J9" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.41036331149493743</v>
+        <v>-0.42316855270994636</v>
       </c>
       <c r="K9" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>-205.56617999999997</v>
+        <v>-211.982167</v>
       </c>
       <c r="L9"/>
     </row>
@@ -69897,15 +69762,15 @@
       </c>
       <c r="I10" s="155" cm="1">
         <f t="array" aca="1" ref="I10" ca="1">_FV(B10,"Price")</f>
-        <v>62.66</v>
+        <v>60.32</v>
       </c>
       <c r="J10" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>7.6632302405498176E-2</v>
+        <v>3.6426116838487926E-2</v>
       </c>
       <c r="K10" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>38.414875999999936</v>
+        <v>18.270751999999902</v>
       </c>
       <c r="L10"/>
     </row>
@@ -69936,15 +69801,15 @@
       </c>
       <c r="I11" s="155" cm="1">
         <f t="array" aca="1" ref="I11" ca="1">_FV(B11,"Price")</f>
-        <v>85.04</v>
+        <v>83.48</v>
       </c>
       <c r="J11" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>-6.825901172345776E-2</v>
+        <v>-8.5351155911033108E-2</v>
       </c>
       <c r="K11" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>-34.215440000000001</v>
+        <v>-42.778279999999995</v>
       </c>
       <c r="L11"/>
     </row>
@@ -69975,15 +69840,15 @@
       </c>
       <c r="I12" s="155" cm="1">
         <f t="array" aca="1" ref="I12" ca="1">_FV(B12,"Price")</f>
-        <v>96.85</v>
+        <v>94.33</v>
       </c>
       <c r="J12" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>0.15710872162485054</v>
+        <v>0.12700119474313018</v>
       </c>
       <c r="K12" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>78.695674999999937</v>
+        <v>63.612214999999992</v>
       </c>
       <c r="L12"/>
     </row>
@@ -70014,15 +69879,15 @@
       </c>
       <c r="I13" s="155" cm="1">
         <f t="array" aca="1" ref="I13" ca="1">_FV(B13,"Price")</f>
-        <v>95.25</v>
+        <v>93.75</v>
       </c>
       <c r="J13" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.18568863811233649</v>
+        <v>-0.19851243908694535</v>
       </c>
       <c r="K13" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>-93.03472499999998</v>
+        <v>-99.459374999999966</v>
       </c>
       <c r="L13"/>
     </row>
@@ -70053,15 +69918,15 @@
       </c>
       <c r="I14" s="157" cm="1">
         <f t="array" aca="1" ref="I14" ca="1">_FV(B14,"Price")</f>
-        <v>27.62</v>
+        <v>27.4</v>
       </c>
       <c r="J14" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>8.3562181247548162E-2</v>
+        <v>7.4931345625735599E-2</v>
       </c>
       <c r="K14" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>41.898720000000026</v>
+        <v>37.574399999999969</v>
       </c>
       <c r="L14"/>
     </row>
@@ -70071,114 +69936,114 @@
       </c>
       <c r="C15" s="146" t="str" cm="1">
         <f t="array" aca="1" ref="C15" ca="1">_FV(Portfolio[[#This Row],[Company]],"Name")</f>
-        <v>FRONTDOOR, INC.</v>
+        <v>EVERI HOLDINGS INC.</v>
       </c>
       <c r="D15" s="147" t="str" cm="1">
         <f t="array" aca="1" ref="D15" ca="1">_FV(B15,"Ticker symbol",TRUE)</f>
-        <v>FTDR</v>
+        <v>EVRI</v>
       </c>
       <c r="E15" s="147" t="str" cm="1">
         <f t="array" aca="1" ref="E15" ca="1">_FV(B15,"Industry")</f>
-        <v>Personal &amp; Household Products &amp; Services</v>
+        <v>Hotels &amp; Entertainment Services</v>
       </c>
       <c r="F15" s="156">
-        <v>29.71</v>
+        <v>8.77</v>
       </c>
       <c r="G15" s="163">
-        <v>16.863700000000001</v>
+        <v>57.110100000000003</v>
       </c>
       <c r="H15" s="169">
         <v>501</v>
       </c>
       <c r="I15" s="157" cm="1">
         <f t="array" aca="1" ref="I15" ca="1">_FV(B15,"Price")</f>
-        <v>49.2</v>
+        <v>13.18</v>
       </c>
       <c r="J15" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>0.65600807808818584</v>
+        <v>0.50285062713797035</v>
       </c>
       <c r="K15" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>328.69404000000009</v>
+        <v>251.71111800000006</v>
       </c>
       <c r="L15"/>
     </row>
     <row r="16" spans="2:12">
-      <c r="B16" s="136" t="e" vm="14">
+      <c r="B16" s="135" t="e" vm="14">
         <v>#VALUE!</v>
       </c>
-      <c r="C16" s="146" t="str" cm="1">
+      <c r="C16" s="148" t="str" cm="1">
         <f t="array" aca="1" ref="C16" ca="1">_FV(Portfolio[[#This Row],[Company]],"Name")</f>
-        <v>LANTHEUS HOLDINGS, INC.</v>
-      </c>
-      <c r="D16" s="147" t="str" cm="1">
+        <v>NEXTRACKER INC.</v>
+      </c>
+      <c r="D16" s="149" t="str" cm="1">
         <f t="array" aca="1" ref="D16" ca="1">_FV(B16,"Ticker symbol",TRUE)</f>
-        <v>LNTH</v>
-      </c>
-      <c r="E16" s="147" t="str" cm="1">
+        <v>NXT</v>
+      </c>
+      <c r="E16" s="149" t="str" cm="1">
         <f t="array" aca="1" ref="E16" ca="1">_FV(B16,"Industry")</f>
-        <v>Healthcare Equipment &amp; Supplies</v>
-      </c>
-      <c r="F16" s="156">
-        <v>62.23</v>
-      </c>
-      <c r="G16" s="163">
-        <v>8.0502000000000002</v>
-      </c>
-      <c r="H16" s="169">
-        <v>501</v>
-      </c>
-      <c r="I16" s="157" cm="1">
+        <v>Renewable Energy</v>
+      </c>
+      <c r="F16" s="158">
+        <v>48.52</v>
+      </c>
+      <c r="G16" s="164">
+        <v>10</v>
+      </c>
+      <c r="H16" s="170">
+        <v>485.15</v>
+      </c>
+      <c r="I16" s="159" cm="1">
         <f t="array" aca="1" ref="I16" ca="1">_FV(B16,"Price")</f>
-        <v>109.49</v>
+        <v>36.840000000000003</v>
       </c>
       <c r="J16" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>0.75944078418769079</v>
+        <v>-0.24072547403132727</v>
       </c>
       <c r="K16" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>380.41639799999996</v>
+        <v>-116.74999999999994</v>
       </c>
       <c r="L16"/>
     </row>
     <row r="17" spans="2:12">
-      <c r="B17" s="136" t="e" vm="15">
+      <c r="B17" s="135" t="e" vm="15">
         <v>#VALUE!</v>
       </c>
-      <c r="C17" s="146" t="str" cm="1">
+      <c r="C17" s="148" t="str" cm="1">
         <f t="array" aca="1" ref="C17" ca="1">_FV(Portfolio[[#This Row],[Company]],"Name")</f>
-        <v>EVERI HOLDINGS INC.</v>
-      </c>
-      <c r="D17" s="147" t="str" cm="1">
+        <v>MONARCH CASINO &amp; RESORT, INC.</v>
+      </c>
+      <c r="D17" s="149" t="str" cm="1">
         <f t="array" aca="1" ref="D17" ca="1">_FV(B17,"Ticker symbol",TRUE)</f>
-        <v>EVRI</v>
-      </c>
-      <c r="E17" s="147" t="str" cm="1">
+        <v>MCRI</v>
+      </c>
+      <c r="E17" s="149" t="str" cm="1">
         <f t="array" aca="1" ref="E17" ca="1">_FV(B17,"Industry")</f>
         <v>Hotels &amp; Entertainment Services</v>
       </c>
-      <c r="F17" s="156">
-        <v>8.77</v>
-      </c>
-      <c r="G17" s="163">
-        <v>57.110100000000003</v>
-      </c>
-      <c r="H17" s="169">
-        <v>501</v>
-      </c>
-      <c r="I17" s="157" cm="1">
+      <c r="F17" s="158">
+        <v>69.95</v>
+      </c>
+      <c r="G17" s="164">
+        <v>7</v>
+      </c>
+      <c r="H17" s="170">
+        <v>489.64</v>
+      </c>
+      <c r="I17" s="159" cm="1">
         <f t="array" aca="1" ref="I17" ca="1">_FV(B17,"Price")</f>
-        <v>13.154999999999999</v>
+        <v>76.459999999999994</v>
       </c>
       <c r="J17" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>0.5</v>
+        <v>9.3066476054324387E-2</v>
       </c>
       <c r="K17" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>250.28336549999995</v>
+        <v>45.579999999999927</v>
       </c>
       <c r="L17"/>
     </row>
@@ -70188,36 +70053,36 @@
       </c>
       <c r="C18" s="148" t="str" cm="1">
         <f t="array" aca="1" ref="C18" ca="1">_FV(Portfolio[[#This Row],[Company]],"Name")</f>
-        <v>NEXTRACKER INC.</v>
+        <v>MILLER INDUSTRIES, INC.</v>
       </c>
       <c r="D18" s="149" t="str" cm="1">
         <f t="array" aca="1" ref="D18" ca="1">_FV(B18,"Ticker symbol",TRUE)</f>
-        <v>NXT</v>
+        <v>MLR</v>
       </c>
       <c r="E18" s="149" t="str" cm="1">
         <f t="array" aca="1" ref="E18" ca="1">_FV(B18,"Industry")</f>
-        <v>Renewable Energy</v>
+        <v>Automobiles &amp; Auto Parts</v>
       </c>
       <c r="F18" s="158">
-        <v>48.52</v>
+        <v>62.18</v>
       </c>
       <c r="G18" s="164">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H18" s="170">
-        <v>485.15</v>
+        <v>497.44</v>
       </c>
       <c r="I18" s="159" cm="1">
         <f t="array" aca="1" ref="I18" ca="1">_FV(B18,"Price")</f>
-        <v>38.32</v>
+        <v>60</v>
       </c>
       <c r="J18" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.21022258862324819</v>
+        <v>-3.5059504663879054E-2</v>
       </c>
       <c r="K18" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>-101.94999999999999</v>
+        <v>-17.439999999999998</v>
       </c>
       <c r="L18"/>
     </row>
@@ -70227,155 +70092,153 @@
       </c>
       <c r="C19" s="148" t="str" cm="1">
         <f t="array" aca="1" ref="C19" ca="1">_FV(Portfolio[[#This Row],[Company]],"Name")</f>
-        <v>MONARCH CASINO &amp; RESORT, INC.</v>
+        <v>JANUS INTERNATIONAL GROUP, INC.</v>
       </c>
       <c r="D19" s="149" t="str" cm="1">
         <f t="array" aca="1" ref="D19" ca="1">_FV(B19,"Ticker symbol",TRUE)</f>
-        <v>MCRI</v>
+        <v>JBI</v>
       </c>
       <c r="E19" s="149" t="str" cm="1">
         <f t="array" aca="1" ref="E19" ca="1">_FV(B19,"Industry")</f>
-        <v>Hotels &amp; Entertainment Services</v>
+        <v>Homebuilding &amp; Construction Supplies</v>
       </c>
       <c r="F19" s="158">
-        <v>69.95</v>
+        <v>13.4</v>
       </c>
       <c r="G19" s="164">
-        <v>7</v>
+        <v>37.383000000000003</v>
       </c>
       <c r="H19" s="170">
-        <v>489.64</v>
+        <v>501</v>
       </c>
       <c r="I19" s="159" cm="1">
         <f t="array" aca="1" ref="I19" ca="1">_FV(B19,"Price")</f>
-        <v>77.92</v>
+        <v>10.01</v>
       </c>
       <c r="J19" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>0.11393852751965687</v>
+        <v>-0.2529850746268657</v>
       </c>
       <c r="K19" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>55.800000000000068</v>
+        <v>-126.79616999999996</v>
       </c>
       <c r="L19"/>
     </row>
     <row r="20" spans="2:12">
-      <c r="B20" s="135" t="e" vm="18">
+      <c r="B20" s="206" t="e" vm="18">
         <v>#VALUE!</v>
       </c>
-      <c r="C20" s="148" t="str" cm="1">
+      <c r="C20" s="211" t="str" cm="1">
         <f t="array" aca="1" ref="C20" ca="1">_FV(Portfolio[[#This Row],[Company]],"Name")</f>
-        <v>MILLER INDUSTRIES, INC.</v>
-      </c>
-      <c r="D20" s="149" t="str" cm="1">
+        <v>ULTA BEAUTY, INC.</v>
+      </c>
+      <c r="D20" s="212" t="str" cm="1">
         <f t="array" aca="1" ref="D20" ca="1">_FV(B20,"Ticker symbol",TRUE)</f>
-        <v>MLR</v>
-      </c>
-      <c r="E20" s="149" t="str" cm="1">
+        <v>ULTA</v>
+      </c>
+      <c r="E20" s="212" t="str" cm="1">
         <f t="array" aca="1" ref="E20" ca="1">_FV(B20,"Industry")</f>
-        <v>Automobiles &amp; Auto Parts</v>
-      </c>
-      <c r="F20" s="158">
-        <v>62.18</v>
-      </c>
-      <c r="G20" s="164">
-        <v>8</v>
-      </c>
-      <c r="H20" s="170">
-        <v>497.44</v>
-      </c>
-      <c r="I20" s="159" cm="1">
+        <v>Specialty Retailers</v>
+      </c>
+      <c r="F20" s="207">
+        <v>393.4</v>
+      </c>
+      <c r="G20" s="217">
+        <v>1.28</v>
+      </c>
+      <c r="H20" s="208">
+        <v>503.56</v>
+      </c>
+      <c r="I20" s="213" cm="1">
         <f t="array" aca="1" ref="I20" ca="1">_FV(B20,"Price")</f>
-        <v>60.454999999999998</v>
+        <v>402.72</v>
       </c>
       <c r="J20" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.7742039240913501E-2</v>
+        <v>2.3690899847483606E-2</v>
       </c>
       <c r="K20" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>-13.800000000000011</v>
+        <v>11.921600000000069</v>
       </c>
       <c r="L20"/>
     </row>
     <row r="21" spans="2:12">
-      <c r="B21" s="135" t="e" vm="19">
+      <c r="B21" s="214" t="e" vm="19">
         <v>#VALUE!</v>
       </c>
-      <c r="C21" s="148" t="str" cm="1">
+      <c r="C21" s="214" t="str" cm="1">
         <f t="array" aca="1" ref="C21" ca="1">_FV(Portfolio[[#This Row],[Company]],"Name")</f>
-        <v>JANUS INTERNATIONAL GROUP, INC.</v>
-      </c>
-      <c r="D21" s="149" t="str" cm="1">
+        <v>INTERNATIONAL GAME TECHNOLOGY PLC</v>
+      </c>
+      <c r="D21" s="215" t="str" cm="1">
         <f t="array" aca="1" ref="D21" ca="1">_FV(B21,"Ticker symbol",TRUE)</f>
-        <v>JBI</v>
-      </c>
-      <c r="E21" s="149" t="str" cm="1">
+        <v>IGT</v>
+      </c>
+      <c r="E21" s="215" t="str" cm="1">
         <f t="array" aca="1" ref="E21" ca="1">_FV(B21,"Industry")</f>
-        <v>Homebuilding &amp; Construction Supplies</v>
-      </c>
-      <c r="F21" s="158">
-        <v>13.4</v>
-      </c>
-      <c r="G21" s="164">
-        <v>37.383000000000003</v>
-      </c>
-      <c r="H21" s="170">
+        <v>Hotels &amp; Entertainment Services</v>
+      </c>
+      <c r="F21" s="209">
+        <v>22.26</v>
+      </c>
+      <c r="G21" s="218">
+        <v>22.506499999999999</v>
+      </c>
+      <c r="H21" s="210">
         <v>501</v>
       </c>
-      <c r="I21" s="159" cm="1">
+      <c r="I21" s="216" cm="1">
         <f t="array" aca="1" ref="I21" ca="1">_FV(B21,"Price")</f>
-        <v>10.35</v>
+        <v>21.91</v>
       </c>
       <c r="J21" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.22761194029850751</v>
+        <v>-1.5723270440251635E-2</v>
       </c>
       <c r="K21" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>-114.08594999999997</v>
-      </c>
-      <c r="L21"/>
+        <v>-7.8825850000000059</v>
+      </c>
     </row>
     <row r="22" spans="2:12">
-      <c r="B22" s="206" t="e" vm="20">
+      <c r="B22" s="214" t="e" vm="20">
         <v>#VALUE!</v>
       </c>
-      <c r="C22" s="211" t="str" cm="1">
+      <c r="C22" s="214" t="str" cm="1">
         <f t="array" aca="1" ref="C22" ca="1">_FV(Portfolio[[#This Row],[Company]],"Name")</f>
-        <v>ULTA BEAUTY, INC.</v>
-      </c>
-      <c r="D22" s="212" t="str" cm="1">
+        <v>OIL-DRI CORPORATION OF AMERICA</v>
+      </c>
+      <c r="D22" s="215" t="str" cm="1">
         <f t="array" aca="1" ref="D22" ca="1">_FV(B22,"Ticker symbol",TRUE)</f>
-        <v>ULTA</v>
-      </c>
-      <c r="E22" s="212" t="str" cm="1">
+        <v>ODC</v>
+      </c>
+      <c r="E22" s="215" t="str" cm="1">
         <f t="array" aca="1" ref="E22" ca="1">_FV(B22,"Industry")</f>
-        <v>Specialty Retailers</v>
-      </c>
-      <c r="F22" s="207">
-        <v>393.4</v>
-      </c>
-      <c r="G22" s="217">
-        <v>1.28</v>
-      </c>
-      <c r="H22" s="208">
-        <v>503.56</v>
-      </c>
-      <c r="I22" s="213" cm="1">
+        <v>Chemicals</v>
+      </c>
+      <c r="F22" s="209">
+        <v>69.64</v>
+      </c>
+      <c r="G22" s="218">
+        <v>7.2146999999999997</v>
+      </c>
+      <c r="H22" s="210">
+        <v>500.99</v>
+      </c>
+      <c r="I22" s="216" cm="1">
         <f t="array" aca="1" ref="I22" ca="1">_FV(B22,"Price")</f>
-        <v>405.61</v>
+        <v>67.849999999999994</v>
       </c>
       <c r="J22" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>3.1037112353838426E-2</v>
+        <v>-2.5703618609994344E-2</v>
       </c>
       <c r="K22" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>15.620799999999974</v>
-      </c>
-      <c r="L22"/>
+        <v>-11.472605000000101</v>
+      </c>
     </row>
     <row r="23" spans="2:12">
       <c r="B23" s="214" t="e" vm="21">
@@ -70383,36 +70246,36 @@
       </c>
       <c r="C23" s="214" t="str" cm="1">
         <f t="array" aca="1" ref="C23" ca="1">_FV(Portfolio[[#This Row],[Company]],"Name")</f>
-        <v>INTERNATIONAL GAME TECHNOLOGY PLC</v>
+        <v>AXCELIS TECHNOLOGIES, INC.</v>
       </c>
       <c r="D23" s="215" t="str" cm="1">
         <f t="array" aca="1" ref="D23" ca="1">_FV(B23,"Ticker symbol",TRUE)</f>
-        <v>IGT</v>
+        <v>ACLS</v>
       </c>
       <c r="E23" s="215" t="str" cm="1">
         <f t="array" aca="1" ref="E23" ca="1">_FV(B23,"Industry")</f>
-        <v>Hotels &amp; Entertainment Services</v>
+        <v>Semiconductors &amp; Semiconductor Equipment</v>
       </c>
       <c r="F23" s="209">
-        <v>22.26</v>
+        <v>101.13</v>
       </c>
       <c r="G23" s="218">
-        <v>22.506499999999999</v>
+        <v>4.9541000000000004</v>
       </c>
       <c r="H23" s="210">
-        <v>501</v>
+        <v>500.99</v>
       </c>
       <c r="I23" s="216" cm="1">
         <f t="array" aca="1" ref="I23" ca="1">_FV(B23,"Price")</f>
-        <v>22.27</v>
+        <v>97.84</v>
       </c>
       <c r="J23" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>4.4923629829281264E-4</v>
+        <v>-3.2532384060120559E-2</v>
       </c>
       <c r="K23" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>0.21975499999996373</v>
+        <v>-16.280855999999972</v>
       </c>
     </row>
     <row r="24" spans="2:12">
@@ -70421,150 +70284,66 @@
       </c>
       <c r="C24" s="214" t="str" cm="1">
         <f t="array" aca="1" ref="C24" ca="1">_FV(Portfolio[[#This Row],[Company]],"Name")</f>
-        <v>OIL-DRI CORPORATION OF AMERICA</v>
+        <v>DELL TECHNOLOGIES INC.</v>
       </c>
       <c r="D24" s="215" t="str" cm="1">
         <f t="array" aca="1" ref="D24" ca="1">_FV(B24,"Ticker symbol",TRUE)</f>
-        <v>ODC</v>
+        <v>DELL</v>
       </c>
       <c r="E24" s="215" t="str" cm="1">
         <f t="array" aca="1" ref="E24" ca="1">_FV(B24,"Industry")</f>
-        <v>Chemicals</v>
+        <v>Computers, Phones &amp; Household Electronics</v>
       </c>
       <c r="F24" s="209">
-        <v>69.64</v>
+        <v>118.18</v>
       </c>
       <c r="G24" s="218">
-        <v>7.2146999999999997</v>
+        <v>4.2393999999999998</v>
       </c>
       <c r="H24" s="210">
-        <v>500.99</v>
+        <v>501</v>
       </c>
       <c r="I24" s="216" cm="1">
         <f t="array" aca="1" ref="I24" ca="1">_FV(B24,"Price")</f>
-        <v>69.510000000000005</v>
+        <v>115.99</v>
       </c>
       <c r="J24" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.8667432510051042E-3</v>
+        <v>-1.8531054323912777E-2</v>
       </c>
       <c r="K24" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>0.50379700000002003</v>
-      </c>
-    </row>
-    <row r="25" spans="2:12">
-      <c r="B25" s="214" t="e" vm="23">
-        <v>#VALUE!</v>
-      </c>
-      <c r="C25" s="214" t="str" cm="1">
-        <f t="array" aca="1" ref="C25" ca="1">_FV(Portfolio[[#This Row],[Company]],"Name")</f>
-        <v>AXCELIS TECHNOLOGIES, INC.</v>
-      </c>
-      <c r="D25" s="215" t="str" cm="1">
-        <f t="array" aca="1" ref="D25" ca="1">_FV(B25,"Ticker symbol",TRUE)</f>
-        <v>ACLS</v>
-      </c>
-      <c r="E25" s="215" t="str" cm="1">
-        <f t="array" aca="1" ref="E25" ca="1">_FV(B25,"Industry")</f>
-        <v>Semiconductors &amp; Semiconductor Equipment</v>
-      </c>
-      <c r="F25" s="209">
-        <v>101.13</v>
-      </c>
-      <c r="G25" s="218">
-        <v>4.9541000000000004</v>
-      </c>
-      <c r="H25" s="210">
-        <v>500.99</v>
-      </c>
-      <c r="I25" s="216" cm="1">
-        <f t="array" aca="1" ref="I25" ca="1">_FV(B25,"Price")</f>
-        <v>101</v>
-      </c>
-      <c r="J25" s="131">
-        <f t="shared" ca="1" si="0"/>
-        <v>-1.2854741421931717E-3</v>
-      </c>
-      <c r="K25" s="172">
-        <f t="shared" ca="1" si="1"/>
-        <v>-0.62589999999994461</v>
-      </c>
-    </row>
-    <row r="26" spans="2:12">
-      <c r="B26" s="214" t="e" vm="24">
-        <v>#VALUE!</v>
-      </c>
-      <c r="C26" s="214" t="str" cm="1">
-        <f t="array" aca="1" ref="C26" ca="1">_FV(Portfolio[[#This Row],[Company]],"Name")</f>
-        <v>DELL TECHNOLOGIES INC.</v>
-      </c>
-      <c r="D26" s="215" t="str" cm="1">
-        <f t="array" aca="1" ref="D26" ca="1">_FV(B26,"Ticker symbol",TRUE)</f>
-        <v>DELL</v>
-      </c>
-      <c r="E26" s="215" t="str" cm="1">
-        <f t="array" aca="1" ref="E26" ca="1">_FV(B26,"Industry")</f>
-        <v>Computers, Phones &amp; Household Electronics</v>
-      </c>
-      <c r="F26" s="209">
-        <v>118.18</v>
-      </c>
-      <c r="G26" s="218">
-        <v>4.2393999999999998</v>
-      </c>
-      <c r="H26" s="210">
-        <v>501</v>
-      </c>
-      <c r="I26" s="216" cm="1">
-        <f t="array" aca="1" ref="I26" ca="1">_FV(B26,"Price")</f>
-        <v>118.501</v>
-      </c>
-      <c r="J26" s="131">
-        <f t="shared" ca="1" si="0"/>
-        <v>2.7161956337789636E-3</v>
-      </c>
-      <c r="K26" s="172">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.3731394000000137</v>
-      </c>
-    </row>
-    <row r="28" spans="2:12" ht="13">
-      <c r="K28" s="171">
-        <f ca="1">SUM(K3:K26)</f>
-        <v>1296.7452478999999</v>
+        <v>-9.2719940000000634</v>
+      </c>
+    </row>
+    <row r="26" spans="2:12" ht="13">
+      <c r="K26" s="171">
+        <f ca="1">SUM(K3:K24)</f>
+        <v>400.10284799999971</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="J22:J26">
-    <cfRule type="cellIs" dxfId="13" priority="3" operator="lessThan">
+  <conditionalFormatting sqref="J20:J24 J3:K19">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J3:K21">
-    <cfRule type="cellIs" dxfId="19" priority="7" operator="lessThan">
+  <conditionalFormatting sqref="K20:K24">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K22:K26">
-    <cfRule type="cellIs" dxfId="17" priority="1" operator="lessThan">
+  <conditionalFormatting sqref="K26">
+    <cfRule type="cellIs" dxfId="1" priority="5" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="2" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K28">
-    <cfRule type="cellIs" dxfId="15" priority="5" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="6" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
vault backup: 2024-09-19 18:29:35
</commit_message>
<xml_diff>
--- a/_system/Attachments/Portfolio Management.xlsx
+++ b/_system/Attachments/Portfolio Management.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martin/repos/tomesink/obsidian/_system/Attachments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3ECE60A-E4F3-6749-AEDF-E91484D5C55C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE2FF8F1-0296-1C43-91F9-2ACAFD2A8421}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35840" yWindow="1360" windowWidth="23320" windowHeight="18860" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3300" yWindow="980" windowWidth="33800" windowHeight="18860" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Stocks Performance" sheetId="1" r:id="rId1"/>
@@ -811,7 +811,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="12">
+  <numFmts count="11">
     <numFmt numFmtId="164" formatCode="[$$-409]\ #,##0.00"/>
     <numFmt numFmtId="165" formatCode="[$£-809]\ #,##0.00"/>
     <numFmt numFmtId="166" formatCode="[$$-409]\ #,##0"/>
@@ -823,7 +823,6 @@
     <numFmt numFmtId="172" formatCode="#,##0.00\ &quot;CZK&quot;"/>
     <numFmt numFmtId="173" formatCode="[$$-409]#,##0.00"/>
     <numFmt numFmtId="174" formatCode="0.0000"/>
-    <numFmt numFmtId="180" formatCode="[$$-409]\ #,##0.0000"/>
   </numFmts>
   <fonts count="14">
     <font>
@@ -2187,7 +2186,7 @@
     <xf numFmtId="174" fontId="11" fillId="14" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="180" fontId="11" fillId="30" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="174" fontId="11" fillId="30" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -4583,8 +4582,8 @@
     <v>83.25</v>
     <v>52.770499999999998</v>
     <v>0.52459999999999996</v>
-    <v>0.59</v>
-    <v>1.0201999999999999E-2</v>
+    <v>-0.1079</v>
+    <v>-1.8470000000000001E-3</v>
     <v>USD</v>
     <v>CVS Health Corporation is a health solutions company. The Company operates in four segments: Health Care Benefits, Health Services, Pharmacy &amp; Consumer Wellness, and Corporate/Other. Its Health Care Benefits segment offer a range of traditional, voluntary and consumer-directed health insurance products and related services, including medical, pharmacy, dental and behavioral health plans, medical management capabilities, Medicare Advantage and Medicare supplement plans, and Medicaid health care management services. Its Health Services segment provides a full range of pharmacy benefit management solutions, delivers health care services in its medical clinics, virtually, and in the home, and offers provider enablement solutions. The Pharmacy &amp; Consumer Wellness segment dispenses prescriptions in its retail pharmacies and through its infusion operations, provides ancillary pharmacy services, including pharmacy patient care programs, diagnostic testing and vaccination administration.</v>
     <v>300000</v>
@@ -4592,24 +4591,24 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>1 Cvs Dr, WOONSOCKET, RI, 02895-6146 US</v>
-    <v>59.19</v>
+    <v>59.1</v>
     <v>Healthcare Providers &amp; Services</v>
     <v>Stock</v>
-    <v>45553.996098471878</v>
+    <v>45554.683699687499</v>
     <v>0</v>
-    <v>57.746299999999998</v>
-    <v>73491133180</v>
+    <v>58.12</v>
+    <v>73355397245</v>
     <v>CVS HEALTH CORPORATION</v>
     <v>CVS HEALTH CORPORATION</v>
-    <v>57.88</v>
-    <v>10.396100000000001</v>
-    <v>57.83</v>
+    <v>58.87</v>
+    <v>10.3926</v>
     <v>58.42</v>
+    <v>58.312100000000001</v>
     <v>1257979000</v>
     <v>CVS</v>
     <v>CVS HEALTH CORPORATION (XNYS:CVS)</v>
-    <v>2291</v>
-    <v>7701146</v>
+    <v>1754217</v>
+    <v>7591748</v>
     <v>1996</v>
   </rv>
   <rv s="2">
@@ -4625,7 +4624,7 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>5</v>
+    <v>4</v>
     <v>en-GB</v>
     <v>a1qclh</v>
     <v>268435456</v>
@@ -4634,8 +4633,8 @@
     <v>165.32</v>
     <v>74</v>
     <v>2.0011000000000001</v>
-    <v>1.38</v>
-    <v>9.9690000000000004E-3</v>
+    <v>0.94</v>
+    <v>6.7229999999999998E-3</v>
     <v>USD</v>
     <v>Crocs, Inc. is engaged in the design, development, worldwide marketing, distribution, and sale of casual lifestyle footwear and accessories for women, men, and children. The Company’s segments include Crocs Brand and the HEYDUDE Brand. The Company’s Crocs Brand collection contains Croslite material, a molded footwear technology, delivering extraordinary comfort with each step. Its Croslite materials are formulated to create soft, comfortable, lightweight, non-marking, and odor-resistant footwear. The HEYDUDE Brand offers shoes with a versatile silhouette. It sells its products in more than 80 countries, through two distribution channels: wholesale and direct-to-consumer. Its wholesale channel includes domestic and international multi-brand retailers, mono-branded partner stores, e-tailers, and distributors; its direct-to-consumer channel includes Company-operated retail stores, Company-operated e-commerce sites, and third-party marketplaces.</v>
     <v>7030</v>
@@ -4643,24 +4642,24 @@
     <v>XNAS</v>
     <v>XNAS</v>
     <v>500 Eldorado Boulevard, Building 5, BROOMFIELD, CO, 80021 US</v>
-    <v>143</v>
+    <v>144.32</v>
     <v>Textiles &amp; Apparel</v>
     <v>Stock</v>
-    <v>45553.982780497659</v>
+    <v>45554.683689594531</v>
     <v>3</v>
-    <v>138.2998</v>
-    <v>8302635025</v>
+    <v>140.1</v>
+    <v>8358457047</v>
     <v>CROCS, INC.</v>
     <v>CROCS, INC.</v>
-    <v>138.53</v>
+    <v>142.94999999999999</v>
     <v>10.514799999999999</v>
-    <v>138.43</v>
     <v>139.81</v>
+    <v>140.75</v>
     <v>59385130</v>
     <v>CROX</v>
     <v>CROCS, INC. (XNAS:CROX)</v>
-    <v>1337</v>
-    <v>961370</v>
+    <v>268511</v>
+    <v>937487</v>
     <v>2005</v>
   </rv>
   <rv s="2">
@@ -4676,7 +4675,7 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>5</v>
+    <v>4</v>
     <v>en-GB</v>
     <v>a25yfr</v>
     <v>268435456</v>
@@ -4685,8 +4684,8 @@
     <v>30.07</v>
     <v>17.71</v>
     <v>1.5144</v>
-    <v>0.06</v>
-    <v>3.0490000000000001E-3</v>
+    <v>0.2</v>
+    <v>1.0132E-2</v>
     <v>USD</v>
     <v>Wabash National Corporation provides connected solutions for the transportation, logistics and distribution industries. The Company designs and manufactures products including dry freight and refrigerated trailers, platform trailers, tank trailers, dry and refrigerated truck bodies, structural composite panels and products, transportation, logistics, and distribution industry parts and services, and specialty food grade processing equipment. The Company’s Transportation Solutions (TS) segment comprises the design and manufacturing operations for the Company’s transportation-related equipment and products. This includes dry and refrigerated van trailers, platform trailers, tank trailers and truck-mounted tanks, truck-mounted dry and refrigerated truck bodies and EcoNex technology products. Its Parts &amp; Services (P&amp;S) segment is comprised of the Company’s parts and services businesses as well as the upfitting component of truck bodies business. It also includes DuraPlate composite panels.</v>
     <v>6700</v>
@@ -4694,24 +4693,24 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>3900 Mccarty Lane, LAFAYETTE, IN, 47905 US</v>
-    <v>20.149699999999999</v>
+    <v>20.14</v>
     <v>Machinery, Equipment &amp; Components</v>
     <v>Stock</v>
-    <v>45553.958333333336</v>
+    <v>45554.683655717185</v>
     <v>6</v>
-    <v>19.355</v>
-    <v>868544800</v>
+    <v>19.79</v>
+    <v>877344646</v>
     <v>WABASH NATIONAL CORPORATION</v>
     <v>WABASH NATIONAL CORPORATION</v>
-    <v>19.68</v>
+    <v>20.059999999999999</v>
     <v>6.0552999999999999</v>
-    <v>19.68</v>
     <v>19.739999999999998</v>
+    <v>19.940000000000001</v>
     <v>43999230</v>
     <v>WNC</v>
     <v>WABASH NATIONAL CORPORATION (XNYS:WNC)</v>
-    <v>5</v>
-    <v>437924</v>
+    <v>118349</v>
+    <v>435088</v>
     <v>1991</v>
   </rv>
   <rv s="2">
@@ -4727,7 +4726,7 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>5</v>
+    <v>4</v>
     <v>en-GB</v>
     <v>a1pfoc</v>
     <v>268435456</v>
@@ -4736,8 +4735,8 @@
     <v>26.4</v>
     <v>16.12</v>
     <v>1.0366</v>
-    <v>-0.01</v>
-    <v>-4.5620000000000003E-4</v>
+    <v>0.17499999999999999</v>
+    <v>7.9869999999999993E-3</v>
     <v>USD</v>
     <v>Perdoceo Education Corporation, through its academic institutions, offers quality postsecondary education primarily online to a diverse student population, along with campus-based and blended learning programs. The Company's academic institutions include Colorado Technical University (CTU) and the American InterContinental University System (AIUS), which provides degree programs from the associate through doctoral level as well as non-degree seeking and professional development programs. Its academic institutions offer students industry-relevant and career-focused academic programs. CTU offers academic programs in the career-oriented disciplines of business and management, nursing, healthcare management, computer science, engineering, information systems and technology, project management, cybersecurity and criminal justice. AIUS offers academic programs in the career-oriented disciplines of business studies, information technologies, education, health sciences and criminal justice.</v>
     <v>2319</v>
@@ -4745,24 +4744,24 @@
     <v>XNAS</v>
     <v>XNAS</v>
     <v>1750 E. GOLF ROAD, SCHAUMBURG, IL, 60173 US</v>
-    <v>22.16</v>
+    <v>22.34</v>
     <v>Miscellaneous Educational Service Providers</v>
     <v>Stock</v>
-    <v>45553.835491724218</v>
+    <v>45554.683665995311</v>
     <v>9</v>
-    <v>21.67</v>
-    <v>1438904851</v>
+    <v>21.840599999999998</v>
+    <v>1450397701</v>
     <v>PERDOCEO EDUCATION CORPORATION</v>
     <v>PERDOCEO EDUCATION CORPORATION</v>
-    <v>21.87</v>
+    <v>22.25</v>
     <v>10.7677</v>
-    <v>21.92</v>
     <v>21.91</v>
+    <v>22.085000000000001</v>
     <v>65673430</v>
     <v>PRDO</v>
     <v>PERDOCEO EDUCATION CORPORATION (XNAS:PRDO)</v>
-    <v>381075</v>
-    <v>378012</v>
+    <v>73088</v>
+    <v>383603</v>
     <v>1994</v>
   </rv>
   <rv s="2">
@@ -4787,8 +4786,8 @@
     <v>237.23</v>
     <v>164.07499999999999</v>
     <v>1.2446999999999999</v>
-    <v>3.9</v>
-    <v>1.7989999999999999E-2</v>
+    <v>8.3015000000000008</v>
+    <v>3.7616000000000004E-2</v>
     <v>USD</v>
     <v>Apple Inc. designs, manufactures and markets smartphones, personal computers, tablets, wearables and accessories, and sells a variety of related services. Its product categories include iPhone, Mac, iPad, and Wearables, Home and Accessories. Its software platforms include iOS, iPadOS, macOS, watchOS, and tvOS. Its services include advertising, AppleCare, cloud services, digital content and payment services. It operates various platforms, including the App Store, that allow customers to discover and download applications and digital content, such as books, music, video, games and podcasts. It also offers digital content through subscription-based services, including Apple Arcade, Apple Fitness+, Apple Music, Apple News+ and Apple TV+. Its products include iPhone 15 Pro, iPhone 15, iPhone 14, iPhone 13, MacBook Air, MacBook Pro, iMac, Mac mini, Mac Studio, Mac Pro, and others. It also provides DarwinAI, which specializes in visual quality inspection using its Explainable AI platform.</v>
     <v>161000</v>
@@ -4796,24 +4795,24 @@
     <v>XNAS</v>
     <v>XNAS</v>
     <v>One Apple Park Way, CUPERTINO, CA, 95014 US</v>
-    <v>222.71</v>
+    <v>229.82</v>
     <v>Computers, Phones &amp; Household Electronics</v>
     <v>Stock</v>
-    <v>45553.999827233594</v>
+    <v>45554.683719258595</v>
     <v>12</v>
-    <v>217.54</v>
-    <v>3355401656600</v>
+    <v>224.64</v>
+    <v>3481618824810</v>
     <v>APPLE INC.</v>
     <v>APPLE INC.</v>
-    <v>217.55</v>
+    <v>225.01</v>
     <v>33.601300000000002</v>
-    <v>216.79</v>
     <v>220.69</v>
+    <v>228.9915</v>
     <v>15204140000</v>
     <v>AAPL</v>
     <v>APPLE INC. (XNAS:AAPL)</v>
-    <v>293419</v>
-    <v>43841997</v>
+    <v>32376781</v>
+    <v>44471580</v>
     <v>1977</v>
   </rv>
   <rv s="2">
@@ -4838,8 +4837,8 @@
     <v>92.82</v>
     <v>50.134999999999998</v>
     <v>0.99250000000000005</v>
-    <v>0.11</v>
-    <v>1.243E-3</v>
+    <v>2.2000000000000002</v>
+    <v>2.4839000000000003E-2</v>
     <v>USD</v>
     <v>Allison Transmission Holdings, Inc. is a designer and manufacturer of propulsion solutions for commercial and defense vehicles. The Company is also a manufacturer of medium-and heavy-duty fully automatic transmissions. Its products are used in a variety of applications, including on-highway trucks, including distribution, refuse, construction, fire and emergency; buses, including school, transit and coach; motorhomes, off-highway vehicles, and equipment, including energy, mining and construction applications; and defense vehicles, including tactical wheeled and tracked. The Company operates in approximately 150 countries. The Company has manufacturing facilities in the United States, Hungary and India, as well as global engineering resources, including electrification engineering centers in Indianapolis, Indiana, Auburn Hills, Michigan and London in the United Kingdom. The Company also has approximately 1,600 independent distributor and dealer locations worldwide.</v>
     <v>3700</v>
@@ -4847,24 +4846,24 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>One Allison Way, INDIANAPOLIS, IN, 46222 US</v>
-    <v>90.34</v>
+    <v>90.91</v>
     <v>Machinery, Equipment &amp; Components</v>
     <v>Stock</v>
-    <v>45553.958333367969</v>
+    <v>45554.683676793749</v>
     <v>15</v>
-    <v>88.35</v>
-    <v>7717802031</v>
+    <v>89.39</v>
+    <v>7909505367</v>
     <v>ALLISON TRANSMISSION HOLDINGS, INC.</v>
     <v>ALLISON TRANSMISSION HOLDINGS, INC.</v>
-    <v>88.6</v>
+    <v>89.95</v>
     <v>11.5815</v>
-    <v>88.46</v>
     <v>88.57</v>
+    <v>90.77</v>
     <v>87137880</v>
     <v>ALSN</v>
     <v>ALLISON TRANSMISSION HOLDINGS, INC. (XNYS:ALSN)</v>
-    <v>4</v>
-    <v>484816</v>
+    <v>145905</v>
+    <v>483317</v>
     <v>2007</v>
   </rv>
   <rv s="2">
@@ -4880,7 +4879,7 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>5</v>
+    <v>4</v>
     <v>en-GB</v>
     <v>az23tc</v>
     <v>268435456</v>
@@ -4888,9 +4887,9 @@
     <v>Powered by Refinitiv</v>
     <v>40.695</v>
     <v>18</v>
-    <v>2.0013999999999998</v>
-    <v>-0.03</v>
-    <v>-1.5459999999999998E-3</v>
+    <v>2.0030999999999999</v>
+    <v>0.35099999999999998</v>
+    <v>1.8121000000000002E-2</v>
     <v>USD</v>
     <v>Par Pacific Holdings, Inc. is an energy company, which provides both renewable and conventional fuels to the western United States. It owns and operates 125,000 barrels per day of combined refining capacity across three locations and an energy infrastructure network, including 7.6 million barrels of storage, and marine, rail, rack and pipeline assets. The Company has three segments. Refining segment owns and operates four refineries with total operating crude oil throughput capacity of 219 thousand barrels per day (Mbpd). Retail segment operates fuel retail outlets in Hawaii, Washington and Idaho. It operates convenience stores and fuel retail sites under Hele and nomnom brands, 76 branded fuel retail sites and other sites operated by third parties that sell gasoline, diesel, and retail merchandise, such as soft drinks, prepared foods, and other sundries. Logistics segment operates a multi-modal logistics network spanning the Pacific, the Northwest, and the Rocky Mountain regions.</v>
     <v>1814</v>
@@ -4898,24 +4897,24 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>825 Town and Country Ln Ste 1500, HOUSTON, TX, 77024-2235 US</v>
-    <v>19.920000000000002</v>
+    <v>20.2</v>
     <v>Oil &amp; Gas</v>
     <v>Stock</v>
-    <v>45553.958333356248</v>
+    <v>45554.683513923439</v>
     <v>18</v>
-    <v>19.215</v>
-    <v>1091128951</v>
+    <v>19.555</v>
+    <v>1110901087</v>
     <v>PAR PACIFIC HOLDINGS, INC.</v>
     <v>PAR PACIFIC HOLDINGS, INC.</v>
-    <v>19.46</v>
+    <v>19.98</v>
     <v>3.3748</v>
-    <v>19.399999999999999</v>
     <v>19.37</v>
+    <v>19.721</v>
     <v>56330870</v>
     <v>PARR</v>
     <v>PAR PACIFIC HOLDINGS, INC. (XNYS:PARR)</v>
-    <v>700399</v>
-    <v>917565</v>
+    <v>191838</v>
+    <v>911057</v>
     <v>2005</v>
   </rv>
   <rv s="2">
@@ -4931,7 +4930,7 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>5</v>
+    <v>4</v>
     <v>en-GB</v>
     <v>a1v177</v>
     <v>268435456</v>
@@ -4940,8 +4939,8 @@
     <v>84.44</v>
     <v>38.5</v>
     <v>1.3108</v>
-    <v>-0.56000000000000005</v>
-    <v>-9.1979999999999996E-3</v>
+    <v>1.34</v>
+    <v>2.2214999999999999E-2</v>
     <v>USD</v>
     <v>Hyster-Yale, Inc., formerly Hyster-Yale Materials Handling, Inc., through its wholly owned operating subsidiary, Hyster-Yale Materials Handling, designs, engineers, manufactures, sells, and services a comprehensive line of lift trucks, attachments, aftermarket parts and technology solutions marketed globally primarily under the Hyster and Yale brand names. The Company's business segments include Lift Trucks, Attachments and Fuel Cells. The Hyster-Yale Maximal brand provides trucks for customers requiring fundamental lift truck performance. The Lift Truck segment is focused on fuel cell-powered battery box replacements and integrated fuel cell engine solutions. Hyster- Yale’s attachment subsidiary, Bolzoni S.p.A., is a producer of attachments, forks, and lift tables under the Bolzoni, Auramo and Meyer brand names. The Fuel Cell business, Nuvera Fuel Cells, is an alternative-power technology company focused on fuel cell stacks and engines.</v>
     <v>8600</v>
@@ -4949,24 +4948,24 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>5875 LANDERBROOK DRIVE, SUITE 300, CLEVELAND, OH, 44124 US</v>
-    <v>62.87</v>
+    <v>61.994999999999997</v>
     <v>Machinery, Equipment &amp; Components</v>
     <v>Stock</v>
-    <v>45553.958333367969</v>
+    <v>45554.682903772657</v>
     <v>21</v>
-    <v>59.82</v>
-    <v>1055669368</v>
+    <v>61.01</v>
+    <v>1079120909</v>
     <v>HYSTER-YALE, INC.</v>
     <v>HYSTER-YALE, INC.</v>
-    <v>60.57</v>
+    <v>61.57</v>
     <v>6.0319000000000003</v>
-    <v>60.88</v>
     <v>60.32</v>
+    <v>61.66</v>
     <v>17501150</v>
     <v>HY</v>
     <v>HYSTER-YALE, INC. (XNYS:HY)</v>
-    <v>60370</v>
-    <v>66473</v>
+    <v>12610</v>
+    <v>66109</v>
     <v>1999</v>
   </rv>
   <rv s="2">
@@ -4982,7 +4981,7 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>5</v>
+    <v>4</v>
     <v>en-GB</v>
     <v>a1zvsm</v>
     <v>268435456</v>
@@ -4990,9 +4989,9 @@
     <v>Powered by Refinitiv</v>
     <v>107.955</v>
     <v>71.900000000000006</v>
-    <v>1.5088999999999999</v>
-    <v>-1.1499999999999999</v>
-    <v>-1.3589E-2</v>
+    <v>1.5097</v>
+    <v>1.91</v>
+    <v>2.2879999999999998E-2</v>
     <v>USD</v>
     <v>Polaris Inc. is engaged in designing, engineering, manufacturing and marketing of powersports vehicles. The Company also designs and manufactures or sources parts, garments and accessories (PG&amp;A), which includes aftermarket accessories and apparel. The Company operates through three segments: Off Road, On Road and Marine. The Off Road segment consists of off-road vehicles and snowmobiles. The On Road segment designs and manufactures motorcycles, moto-roadsters, light duty hauling, and passenger vehicles. The Marine segment designs and manufactures boats that are designed to compete in key segments of the recreational marine industry, specifically pontoon and deck boats. Its product line-up includes the RANGER, RZR and Polaris XPEDITION and GENERAL side-by-side off-road vehicles; Sportsman all-terrain off-road vehicles; military and commercial off-road vehicles; snowmobiles; Indian Motorcycle mid-size and heavyweight motorcycles; Slingshot moto-roadsters, and pontoon and deck boats.</v>
     <v>18500</v>
@@ -5000,24 +4999,24 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>2100 HIGHWAY 55, MEDINA, MN, 55340-9770 US</v>
-    <v>86.42</v>
+    <v>85.59</v>
     <v>Leisure Products</v>
     <v>Stock</v>
-    <v>45553.999334409375</v>
+    <v>45554.683616782029</v>
     <v>24</v>
-    <v>82.6</v>
-    <v>4653845544</v>
+    <v>84.364999999999995</v>
+    <v>4760324281</v>
     <v>Polaris Inc.</v>
     <v>Polaris Inc.</v>
-    <v>84.92</v>
+    <v>85.59</v>
     <v>14.6219</v>
-    <v>84.63</v>
     <v>83.48</v>
+    <v>85.39</v>
     <v>55748030</v>
     <v>PII</v>
     <v>Polaris Inc. (XNYS:PII)</v>
-    <v>401026</v>
-    <v>473923</v>
+    <v>109467</v>
+    <v>461892</v>
     <v>1994</v>
   </rv>
   <rv s="2">
@@ -5033,7 +5032,7 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>5</v>
+    <v>4</v>
     <v>en-GB</v>
     <v>aw21cw</v>
     <v>268435456</v>
@@ -5041,9 +5040,9 @@
     <v>Powered by Refinitiv</v>
     <v>114.29989999999999</v>
     <v>75.430000000000007</v>
-    <v>1.7418</v>
-    <v>-1.4</v>
-    <v>-1.4624E-2</v>
+    <v>1.7444</v>
+    <v>1.82</v>
+    <v>1.9293999999999999E-2</v>
     <v>USD</v>
     <v>CONSOL Energy Inc. is a producer and exporter of high-Btu bituminous thermal coal and metallurgical coal. It owns and operates longwall mining operations in the Northern Appalachian Basin. Its flagship operation is the Pennsylvania Mining Complex, located over 26 miles southwest of Pittsburgh, near the city of Washington and the borough of Waynesburg all in Pennsylvania, and consists of three deep longwall mining operations: the Bailey Mine, the Enlow Fork Mine and the Harvey Mine, as well as a centralized preparation plant. Its segments include the PAMC and the CONSOL Marine Terminal. The PAMC includes the Bailey Mine, the Enlow Fork Mine, the Harvey Mine and a centralized preparation plant. The PAMC segment's principal activities include the mining, preparation and marketing of bituminous coal, sold primarily to industrial end-users, metallurgical end-users and power generators. The CONSOL Marine Terminal segment provides coal export terminal services through the Port of Baltimore.</v>
     <v>2020</v>
@@ -5051,24 +5050,24 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>275 TECHNOLOGY DRIVE, SUITE #101, CANONSBURG, PA, 15317 US</v>
-    <v>96.97</v>
+    <v>96.94</v>
     <v>Coal</v>
     <v>Stock</v>
-    <v>45553.958333356248</v>
+    <v>45554.68352082109</v>
     <v>27</v>
-    <v>93.41</v>
-    <v>2772663385</v>
+    <v>95.04</v>
+    <v>2826159064</v>
     <v>CONSOL ENERGY INC.</v>
     <v>CONSOL ENERGY INC.</v>
     <v>96.2</v>
     <v>7.0412999999999997</v>
-    <v>95.73</v>
     <v>94.33</v>
+    <v>96.15</v>
     <v>29393230</v>
     <v>CEIX</v>
     <v>CONSOL ENERGY INC. (XNYS:CEIX)</v>
-    <v>20</v>
-    <v>487441</v>
+    <v>90477</v>
+    <v>492196</v>
     <v>2017</v>
   </rv>
   <rv s="2">
@@ -5093,8 +5092,8 @@
     <v>127.3484</v>
     <v>84.35</v>
     <v>1.2448999999999999</v>
-    <v>1.04</v>
-    <v>1.1217999999999999E-2</v>
+    <v>2.1349999999999998</v>
+    <v>2.2772999999999998E-2</v>
     <v>USD</v>
     <v>AGCO Corporation is a designer, manufacturer and distributor of agricultural machinery and precision agriculture technology. The Company sells a range of agricultural equipment, including tractors, combines, self-propelled sprayers, hay tools, forage equipment, seeding and tillage equipment, implements, and grain storage and protein production systems. It provides telemetry-based fleet management tools, including remote monitoring and diagnostics, which help farmers improve uptime, machine and yield optimization, mixed fleet optimization and decision support. The Company's Precision Planting, Headsight and Intelligent Ag Solutions brands provide retrofit solutions to upgrade farmers existing equipment to improve their planting, liquid application and harvest operations. The Company’s Precision Planting, Headsight, JCA and Intelligent Ag Solutions brands also sell precision agriculture solutions around the crop cycle to third party original equipment manufacturers (OEMs).</v>
     <v>27900</v>
@@ -5102,24 +5101,24 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>4205 River Green Pkway, DULUTH, GA, 30096 US</v>
-    <v>96</v>
+    <v>95.96</v>
     <v>Machinery, Equipment &amp; Components</v>
     <v>Stock</v>
-    <v>45553.958333356248</v>
+    <v>45554.683582985941</v>
     <v>30</v>
-    <v>92.734999999999999</v>
-    <v>6997715625</v>
+    <v>94.64</v>
+    <v>7157076935</v>
     <v>AGCO CORPORATION</v>
     <v>AGCO CORPORATION</v>
-    <v>92.85</v>
+    <v>95.36</v>
     <v>16.700299999999999</v>
-    <v>92.71</v>
     <v>93.75</v>
+    <v>95.885000000000005</v>
     <v>74642300</v>
     <v>AGCO</v>
     <v>AGCO CORPORATION (XNYS:AGCO)</v>
-    <v>362</v>
-    <v>774131</v>
+    <v>134692</v>
+    <v>739418</v>
     <v>1991</v>
   </rv>
   <rv s="2">
@@ -5135,7 +5134,7 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>5</v>
+    <v>4</v>
     <v>en-GB</v>
     <v>a1vuw7</v>
     <v>268435456</v>
@@ -5145,7 +5144,7 @@
     <v>24.01</v>
     <v>1.1547000000000001</v>
     <v>0.05</v>
-    <v>1.828E-3</v>
+    <v>1.825E-3</v>
     <v>USD</v>
     <v>Ituran Location and Control Ltd. is a provider of location-based services, consisting of stolen vehicle recovery (SVR), fleet management services and other tracking services. The Company also provides wireless communication products used in connection with its location-based services and various other applications. Its operations consist of two segments: location-based services and wireless communications products. Its location-based services segment consists of its SVR and tracking services, fleet management and value-added services consisted of personal locater services and concierge services. Its wireless communications products segment consists of short and medium range two-way machine-to-machine wireless communications products that are used for various applications, including automatic vehicle location (AVL) and automatic vehicle identification. It primarily provides its services, as well as sells and leases its products in Israel, Brazil, Argentina and the United States.</v>
     <v>2841</v>
@@ -5153,24 +5152,24 @@
     <v>XNAS</v>
     <v>XNAS</v>
     <v>3 HASHIKMA, A.T AZUR, T.D 163, AZOR, 5800182 IL</v>
-    <v>27.76</v>
+    <v>28</v>
     <v>Communications &amp; Networking</v>
     <v>Stock</v>
-    <v>45553.833346967185</v>
+    <v>45554.682208680468</v>
     <v>33</v>
-    <v>27.252500000000001</v>
-    <v>545084092</v>
+    <v>27.38</v>
+    <v>546078771</v>
     <v>ITURAN LOCATION AND CONTROL LTD.</v>
     <v>ITURAN LOCATION AND CONTROL LTD.</v>
-    <v>27.28</v>
+    <v>27.78</v>
     <v>10.7311</v>
-    <v>27.35</v>
     <v>27.4</v>
+    <v>27.45</v>
     <v>19893580</v>
     <v>ITRN</v>
     <v>ITURAN LOCATION AND CONTROL LTD. (XNAS:ITRN)</v>
-    <v>75499</v>
-    <v>82057</v>
+    <v>12952</v>
+    <v>82373</v>
     <v>1994</v>
   </rv>
   <rv s="2">
@@ -5186,7 +5185,7 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>5</v>
+    <v>4</v>
     <v>en-GB</v>
     <v>a1sea2</v>
     <v>268435456</v>
@@ -5195,8 +5194,8 @@
     <v>14.62</v>
     <v>6.37</v>
     <v>2.15</v>
-    <v>0.04</v>
-    <v>3.0439999999999998E-3</v>
+    <v>0</v>
+    <v>0</v>
     <v>USD</v>
     <v>Everi Holdings Inc. develops and offers products and services that provide gaming entertainment, improve its customers’ patron engagement, and help its casino customers operate their businesses. It develops and supplies entertaining game content, gaming machines and gaming systems and services for land-based and iGaming operators. It operates through two segments: Games and Financial Technology Solutions (FinTech). The Games segment provides gaming operators with gaming technology and entertainment products and services, including gaming machines, primarily comprising Class II, Class III and Historic Horse Racing slot machines placed under participation and fixed-fee lease arrangements or sold to casino customers. The FinTech segment provides gaming operators with financial technology products and services, including financial access and related services supporting digital, cashless and physical cash options across mobile, assisted and self-service channels.</v>
     <v>2200</v>
@@ -5204,36 +5203,36 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>7250 S Tenaya Way Ste 100, LAS VEGAS, NV, 89113-2175 US</v>
-    <v>13.19</v>
+    <v>13.219900000000001</v>
     <v>Hotels &amp; Entertainment Services</v>
     <v>Stock</v>
-    <v>45553.958333367969</v>
+    <v>45554.683597499999</v>
     <v>36</v>
-    <v>13.14</v>
+    <v>13.18</v>
     <v>1124564784</v>
     <v>EVERI HOLDINGS INC.</v>
     <v>EVERI HOLDINGS INC.</v>
-    <v>13.16</v>
+    <v>13.2</v>
     <v>27.993099999999998</v>
-    <v>13.14</v>
+    <v>13.18</v>
     <v>13.18</v>
     <v>85323580</v>
     <v>EVRI</v>
     <v>EVERI HOLDINGS INC. (XNYS:EVRI)</v>
-    <v>499</v>
-    <v>863655</v>
+    <v>126966</v>
+    <v>844929</v>
     <v>2004</v>
   </rv>
   <rv s="2">
     <v>37</v>
   </rv>
   <rv s="3">
+    <v>5</v>
+    <v>NEXTRACKER INC. (XNAS:NXT)</v>
     <v>6</v>
-    <v>NEXTRACKER INC. (XNAS:NXT)</v>
-    <v>7</v>
     <v>3</v>
     <v>Finance</v>
-    <v>5</v>
+    <v>4</v>
     <v>en-GB</v>
     <v>c8ssgh</v>
     <v>268435456</v>
@@ -5241,9 +5240,9 @@
     <v>Powered by Refinitiv</v>
     <v>62.31</v>
     <v>32.14</v>
-    <v>2.1230000000000002</v>
-    <v>-0.5</v>
-    <v>-1.3389999999999999E-2</v>
+    <v>2.1349999999999998</v>
+    <v>0.36</v>
+    <v>9.7719999999999994E-3</v>
     <v>USD</v>
     <v>Nextracker Inc. is a provider of integrated solar tracker and software solutions used in utility-scale and ground-mounted distributed generation solar projects. Its products enable solar panels in utility-scale power plants to follow the sun’s movement across the sky and optimize plant performance. Its products include NX Horizon, NX Gemini, TrueCapture, and NX Navigator. Its solutions include Bifacial PV modules, Large Format Modules, and First Solar Series 6 (FSLR6) Modules. NX Horizon is a one-in-portrait (1P) smart solar tracker system that delivers the lowest levelized cost of energy (LCOE). NX Gemini is its two-in-portrait (2P) format tracker which holds two rows of solar panels along the central support beam. TrueCapture is its flagship software offering, which is a self-adjusting tracker control system that uses machine learning to enhance solar power plant energy yield. It has operations in the United States, Brazil, Mexico, Spain, India, Australia, the Middle East and Brazil.</v>
     <v>1050</v>
@@ -5251,23 +5250,23 @@
     <v>XNAS</v>
     <v>XNAS</v>
     <v>6200 Paseo Padre Pkwy, FREMONT, CA, 94555 US</v>
-    <v>38.83</v>
+    <v>38.49</v>
     <v>Renewable Energy</v>
     <v>Stock</v>
-    <v>45553.995709883595</v>
-    <v>36.704999999999998</v>
-    <v>5354598216</v>
+    <v>45554.683675253909</v>
+    <v>36.549999999999997</v>
+    <v>5406923280</v>
     <v>NEXTRACKER INC.</v>
     <v>NEXTRACKER INC.</v>
-    <v>37.340000000000003</v>
+    <v>38.49</v>
     <v>9.7772000000000006</v>
-    <v>37.340000000000003</v>
     <v>36.840000000000003</v>
+    <v>37.200000000000003</v>
     <v>145347400</v>
     <v>NXT</v>
     <v>NEXTRACKER INC. (XNAS:NXT)</v>
-    <v>4254</v>
-    <v>2850986</v>
+    <v>1185014</v>
+    <v>2855707</v>
     <v>2022</v>
   </rv>
   <rv s="2">
@@ -5283,7 +5282,7 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>5</v>
+    <v>4</v>
     <v>en-GB</v>
     <v>a1xejc</v>
     <v>268435456</v>
@@ -5292,8 +5291,8 @@
     <v>80.22</v>
     <v>56.25</v>
     <v>1.7425999999999999</v>
-    <v>0.25</v>
-    <v>3.2799999999999999E-3</v>
+    <v>0.45</v>
+    <v>5.8850000000000005E-3</v>
     <v>USD</v>
     <v>Monarch Casino &amp; Resort, Inc. owns and operates the Atlantis Casino Resort Spa, a hotel and casino in Reno, Nevada (the Atlantis) and the Monarch Casino Resort Spa Black Hawk (the Monarch Black Hawk), a hotel and casino in Black Hawk, Colorado. In addition, it owns separate parcels of land located next to the Atlantis and a parcel of land with an industrial warehouse located between Denver, Colorado, and Monarch Black Hawk. The Atlantis is located approximately three miles south of downtown, which features approximately 61,000 square feet of casino space; 817 guest rooms and suites; eight food outlets; two gourmet coffee and pastry bars and one snack bar; a 30,000 square-foot health spa and salon with an enclosed year-round pool. Monarch Black Hawk features approximately 60,000 square feet of casino space; approximately 1,000 slot machines; approximately 43 table games; a live poker room; a keno counter and a sports book. The resort also includes 10 bars and lounges.</v>
     <v>2900</v>
@@ -5301,24 +5300,24 @@
     <v>XNAS</v>
     <v>XNAS</v>
     <v>Executive Offices, 3800 S Virginia Street, RENO, NV, 89502 US</v>
-    <v>78.16</v>
+    <v>77.89</v>
     <v>Hotels &amp; Entertainment Services</v>
     <v>Stock</v>
-    <v>45553.846688113284</v>
+    <v>45554.683548125002</v>
     <v>41</v>
-    <v>75.27</v>
-    <v>1410849095</v>
+    <v>76.25</v>
+    <v>1419152549</v>
     <v>MONARCH CASINO &amp; RESORT, INC.</v>
     <v>MONARCH CASINO &amp; RESORT, INC.</v>
-    <v>75.98</v>
+    <v>77.739999999999995</v>
     <v>17.867999999999999</v>
-    <v>76.209999999999994</v>
     <v>76.459999999999994</v>
+    <v>76.91</v>
     <v>18452120</v>
     <v>MCRI</v>
     <v>MONARCH CASINO &amp; RESORT, INC. (XNAS:MCRI)</v>
-    <v>141398</v>
-    <v>100560</v>
+    <v>32713</v>
+    <v>101934</v>
     <v>1993</v>
   </rv>
   <rv s="2">
@@ -5334,7 +5333,7 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>5</v>
+    <v>4</v>
     <v>en-GB</v>
     <v>a1xqm7</v>
     <v>268435456</v>
@@ -5343,8 +5342,8 @@
     <v>69.75</v>
     <v>34.96</v>
     <v>0.97099999999999997</v>
-    <v>1.22</v>
-    <v>2.0754999999999999E-2</v>
+    <v>1.06</v>
+    <v>1.7666999999999999E-2</v>
     <v>USD</v>
     <v>Miller Industries, Inc. is a manufacturer of towing and recovery equipment. The Company designs and manufactures bodies of car carriers and wreckers, which are installed on chassis manufactured by third parties, and sold to its customers. Its products are marketed and sold through a network of distributors that serve all 50 states, Canada, Mexico, and other foreign markets, and through prime contractors to governmental entities. In addition to selling its products, its independent distributors provide end-users with parts and service. Its product line includes car carriers, wreckers, and transport trailers. Car carriers are specialized flat-bed vehicles with hydraulic tilt mechanisms that enable a towing operator to drive or winch a vehicle onto the bed for transport. Its multi-vehicle transport trailers are specialized auto transport trailers with upper and lower decks and hydraulic ramps for loading vehicles. Its brands include Century, Vulcan, Chevron, Holmes, and Challenger.</v>
     <v>1821</v>
@@ -5352,24 +5351,24 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>Ste 100, 8503 Hilltop Dr, OOLTEWAH, TN, 37363 US</v>
-    <v>60.91</v>
+    <v>61.999899999999997</v>
     <v>Automobiles &amp; Auto Parts</v>
     <v>Stock</v>
-    <v>45553.958333356248</v>
+    <v>45554.683621689066</v>
     <v>44</v>
-    <v>58.6</v>
-    <v>687227400</v>
+    <v>60.08</v>
+    <v>699368417</v>
     <v>MILLER INDUSTRIES, INC.</v>
     <v>MILLER INDUSTRIES, INC.</v>
-    <v>58.83</v>
+    <v>61.3</v>
     <v>9.6592000000000002</v>
-    <v>58.78</v>
     <v>60</v>
+    <v>61.06</v>
     <v>11453790</v>
     <v>MLR</v>
     <v>MILLER INDUSTRIES, INC. (XNYS:MLR)</v>
-    <v>80869</v>
-    <v>86198</v>
+    <v>39189</v>
+    <v>85821</v>
     <v>1994</v>
   </rv>
   <rv s="2">
@@ -5385,7 +5384,7 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>5</v>
+    <v>4</v>
     <v>en-GB</v>
     <v>btavh7</v>
     <v>268435456</v>
@@ -5393,9 +5392,9 @@
     <v>Powered by Refinitiv</v>
     <v>15.86</v>
     <v>9.1649999999999991</v>
-    <v>0.89490000000000003</v>
-    <v>-0.25</v>
-    <v>-2.4365999999999999E-2</v>
+    <v>0.89800000000000002</v>
+    <v>0.16</v>
+    <v>1.5984000000000002E-2</v>
     <v>USD</v>
     <v>Janus International Group, Inc. is a global manufacturer and supplier of turn-key self-storage, commercial and industrial building solutions. It operates through two geographic segments: Janus North America and Janus International. The Janus North America segment is comprised of all the other entities, including Janus International Group, LLC, Betco, Inc., Noke, Inc., Asta Industries, Inc., DBCI, LLC, Access Control Technologies, LLC, Janus Door, LLC, and Steel Door Depot.com, LLC. The Janus International segment is comprised of Janus International Europe Holdings Ltd. (UK). Its production and sales are in Europe and Australia. It provides facility and door automation and access control technologies, roll up and swing doors, hallway systems and relocatable storage moveable additional storage structures (MASS) units. It is comprised of three sales channels, including New Construction-Self-storage, R3-Self-storage, and Commercial and Other. It also provides terminal maintenance services.</v>
     <v>1956</v>
@@ -5403,24 +5402,24 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>135 Janus International Blvd., TEMPLE, GA, 30179 US</v>
-    <v>10.46</v>
+    <v>10.3</v>
     <v>Homebuilding &amp; Construction Supplies</v>
     <v>Stock</v>
-    <v>45553.958333356248</v>
+    <v>45554.683642974218</v>
     <v>47</v>
-    <v>10.01</v>
-    <v>1454675222</v>
+    <v>10.07</v>
+    <v>1454676000</v>
     <v>JANUS INTERNATIONAL GROUP, INC.</v>
     <v>JANUS INTERNATIONAL GROUP, INC.</v>
-    <v>10.3</v>
+    <v>10.23</v>
     <v>11.224399999999999</v>
-    <v>10.26</v>
     <v>10.01</v>
+    <v>10.17</v>
     <v>145322200</v>
     <v>JBI</v>
     <v>JANUS INTERNATIONAL GROUP, INC. (XNYS:JBI)</v>
-    <v>1787162</v>
-    <v>2091493</v>
+    <v>457418</v>
+    <v>2025718</v>
     <v>2020</v>
   </rv>
   <rv s="2">
@@ -5436,7 +5435,7 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>5</v>
+    <v>4</v>
     <v>en-GB</v>
     <v>a24war</v>
     <v>268435456</v>
@@ -5445,8 +5444,8 @@
     <v>574.76</v>
     <v>318.17</v>
     <v>1.2955000000000001</v>
-    <v>5.72</v>
-    <v>1.4408000000000001E-2</v>
+    <v>-0.24</v>
+    <v>-5.9590000000000001E-4</v>
     <v>USD</v>
     <v>Ulta Beauty, Inc. is a beauty retailer. The Company's product categories include cosmetics, skincare, haircare products and styling tools, fragrance and bath, services, and accessories and other. The Company has one segment, which includes retail stores, salon services, and e-commerce. It offers a range of beauty services in its stores, focusing on hair, makeup, brow and skin services. Its skin services include a skin treatment room or dedicated skin treatment area on the sales floor. Its Ulta Beauty store prototype includes an open salon area, with most of its stores offering brow services on the salon floor. It offers a new way to shop for beauty - bringing together All Things Beauty, All in One Place. In addition to ship to home order fulfillment, it offers guests Buy Online, Pick-up in Store, Curbside Pickup, and Store 2 Door, which provides the ability for customers to order in-store and have products delivered to their homes. It operates over 1,350 retail stores across 50 states.</v>
     <v>20000</v>
@@ -5454,24 +5453,24 @@
     <v>XNAS</v>
     <v>XNAS</v>
     <v>1000 Remington Blvd, Suite 120, BOLINGBROOK, IL, 60440 US</v>
-    <v>408.74</v>
+    <v>409.59</v>
     <v>Specialty Retailers</v>
     <v>Stock</v>
-    <v>45553.99901368047</v>
+    <v>45554.683703714843</v>
     <v>50</v>
-    <v>397.38</v>
-    <v>18974044065</v>
+    <v>400.3</v>
+    <v>18962736530</v>
     <v>ULTA BEAUTY, INC.</v>
     <v>ULTA BEAUTY, INC.</v>
-    <v>397.4</v>
-    <v>16.170999999999999</v>
-    <v>397</v>
+    <v>408.75</v>
+    <v>16.134</v>
     <v>402.72</v>
+    <v>402.48</v>
     <v>47114730</v>
     <v>ULTA</v>
     <v>ULTA BEAUTY, INC. (XNAS:ULTA)</v>
-    <v>2626</v>
-    <v>1657712</v>
+    <v>405263</v>
+    <v>1668245</v>
     <v>2016</v>
   </rv>
   <rv s="2">
@@ -5487,7 +5486,7 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>5</v>
+    <v>4</v>
     <v>en-GB</v>
     <v>a1vehw</v>
     <v>268435456</v>
@@ -5495,9 +5494,9 @@
     <v>Powered by Refinitiv</v>
     <v>32.6</v>
     <v>18.899999999999999</v>
-    <v>1.9702</v>
-    <v>0.09</v>
-    <v>4.1250000000000002E-3</v>
+    <v>1.9695</v>
+    <v>0.04</v>
+    <v>1.8260000000000001E-3</v>
     <v>USD</v>
     <v>International Game Technology PLC is a United Kingdom-based company, which is engaged in gaming. The Company operates and provides an integrated portfolio of gaming technology products and services, including online and instant lottery systems, iLottery, instant ticket printing, lottery management services, commercial services, gaming systems, electronic gaming machines, iGaming, and sports betting. The Company operates through three segments. The Global Lottery segment operates traditional lottery and iLottery businesses across the world, which includes sales, operations, product development, technology, and support, across the world. The Global Gaming segment operates a land-based gaming business across the world, which includes sales, product management, studios, global manufacturing, operation, and technology, across the world. The Digital &amp; Betting segment operates iGaming and sports betting activities across the world.</v>
     <v>11000</v>
@@ -5505,24 +5504,24 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>10 Finsbury Square, Third Floor, LONDON, UNITED KINGDOM-NA, EC2A 1AF GB</v>
-    <v>22.39</v>
+    <v>22.37</v>
     <v>Hotels &amp; Entertainment Services</v>
     <v>Stock</v>
-    <v>45553.958333367969</v>
+    <v>45554.68371833281</v>
     <v>53</v>
-    <v>21.78</v>
-    <v>4382000000</v>
+    <v>21.930800000000001</v>
+    <v>4390000000</v>
     <v>INTERNATIONAL GAME TECHNOLOGY PLC</v>
     <v>INTERNATIONAL GAME TECHNOLOGY PLC</v>
-    <v>21.83</v>
+    <v>22.27</v>
     <v>21.198</v>
-    <v>21.82</v>
     <v>21.91</v>
+    <v>21.95</v>
     <v>200000000</v>
     <v>IGT</v>
     <v>INTERNATIONAL GAME TECHNOLOGY PLC (XNYS:IGT)</v>
-    <v>816456</v>
-    <v>635397</v>
+    <v>139046</v>
+    <v>634451</v>
     <v>2014</v>
   </rv>
   <rv s="2">
@@ -5538,7 +5537,7 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>5</v>
+    <v>4</v>
     <v>en-GB</v>
     <v>a1z3ec</v>
     <v>268435456</v>
@@ -5546,9 +5545,9 @@
     <v>Powered by Refinitiv</v>
     <v>87.32</v>
     <v>54.8</v>
-    <v>0.58589999999999998</v>
-    <v>-0.79</v>
-    <v>-1.1509E-2</v>
+    <v>0.58699999999999997</v>
+    <v>0.12</v>
+    <v>1.769E-3</v>
     <v>USD</v>
     <v>Oil-Dri Corporation of America is a manufacturer and supplier of specialty sorbent products for pet care, animal health and nutrition, fluid purification, agricultural ingredients, sports field, industrial and automotive markets. Its principal product is cat litter. The Company’s Retail and Wholesale Products Group segment customers include mass merchandisers, the farm and fleet channel, drugstore chains, pet specialty retail outlets, dollar stores, retail grocery stores, distributors of industrial cleanup and automotive products, environmental service companies, sports field product users and marketers of consumer products. Its Business to Business Products Group segment customers include processors and refiners of edible oils, renewable diesel, petroleum-based oils and biodiesel fuel; manufacturers of animal feed and agricultural chemicals; and distributors of animal health and nutrition products. It is also a supplier of silica gel-based crystal cat litter.</v>
     <v>884</v>
@@ -5556,24 +5555,24 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>SUITE 400, 410 NORTH MICHIGAN AVENUE, CHICAGO, IL, 60611 US</v>
-    <v>69.510000000000005</v>
+    <v>68.5</v>
     <v>Chemicals</v>
     <v>Stock</v>
-    <v>45553.958333344533</v>
+    <v>45554.683460346874</v>
     <v>56</v>
-    <v>67.709999999999994</v>
-    <v>500133200</v>
+    <v>67.694999999999993</v>
+    <v>494377000</v>
     <v>OIL-DRI CORPORATION OF AMERICA</v>
     <v>OIL-DRI CORPORATION OF AMERICA</v>
-    <v>68.47</v>
+    <v>68.5</v>
     <v>13.9237</v>
-    <v>68.64</v>
     <v>67.849999999999994</v>
+    <v>67.97</v>
     <v>7286320</v>
     <v>ODC</v>
     <v>OIL-DRI CORPORATION OF AMERICA (XNYS:ODC)</v>
-    <v>15719</v>
-    <v>15891</v>
+    <v>3758</v>
+    <v>16047</v>
     <v>1969</v>
   </rv>
   <rv s="2">
@@ -5589,7 +5588,7 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>5</v>
+    <v>4</v>
     <v>en-GB</v>
     <v>a1mt9c</v>
     <v>268435456</v>
@@ -5598,8 +5597,8 @@
     <v>170.9692</v>
     <v>93.77</v>
     <v>1.5933999999999999</v>
-    <v>-1.93</v>
-    <v>-1.9344E-2</v>
+    <v>4.16</v>
+    <v>4.2518E-2</v>
     <v>USD</v>
     <v>Axcelis Technologies, Inc. designs, manufactures and services ion implantation and other processing equipment used in the fabrication of semiconductor chips. The Company offers a complete line of high energy, high current and medium current implanters for all application requirements. In addition to equipment, the Company provides extensive aftermarket lifecycle products and services, including used tools, spare parts, equipment upgrades, maintenance services and customer training. Its Purion flagship systems are all based on a common platform, which enables a combination of implant purity, precision and productivity. Combining a single wafer end station, with advanced spot beam architectures (that ensures all points across the wafer see the same beam condition at the same beam angle), Purion products enable process control to optimize device performance and yield, at high productivity. The Company sells its products to semiconductor chip manufacturers around the world.</v>
     <v>1620</v>
@@ -5607,24 +5606,24 @@
     <v>XNAS</v>
     <v>XNAS</v>
     <v>108 Cherry Hill Dr, BEVERLY, MA, 01915 US</v>
-    <v>101.82</v>
+    <v>102.27</v>
     <v>Semiconductors &amp; Semiconductor Equipment</v>
     <v>Stock</v>
-    <v>45553.980763853906</v>
+    <v>45554.68356297422</v>
     <v>59</v>
-    <v>97.64</v>
-    <v>3191305005</v>
+    <v>100.07</v>
+    <v>3326994180</v>
     <v>AXCELIS TECHNOLOGIES, INC.</v>
     <v>AXCELIS TECHNOLOGIES, INC.</v>
-    <v>101.01</v>
+    <v>102.27</v>
     <v>13.4796</v>
-    <v>99.77</v>
     <v>97.84</v>
+    <v>102</v>
     <v>32617590</v>
     <v>ACLS</v>
     <v>AXCELIS TECHNOLOGIES, INC. (XNAS:ACLS)</v>
-    <v>121</v>
-    <v>517965</v>
+    <v>202914</v>
+    <v>521482</v>
     <v>1995</v>
   </rv>
   <rv s="2">
@@ -5649,8 +5648,8 @@
     <v>179.7</v>
     <v>63.9</v>
     <v>0.89570000000000005</v>
-    <v>-0.83</v>
-    <v>-7.1050000000000002E-3</v>
+    <v>2.0750000000000002</v>
+    <v>1.7888999999999999E-2</v>
     <v>USD</v>
     <v>Dell Technologies Inc. is engaged in designing, developing, manufacturing, marketing, selling, and supporting a wide range of comprehensive and integrated solutions, products, and services. The Company operates through two segments: Infrastructure Solutions Group (ISG) and Client Solutions Group (CSG). Its ISG segment enables the Company’s customer’s digital transformation with solutions that address artificial intelligence (AI), machine learning, data analytics, and multi cloud environments. Its comprehensive storage portfolio includes modern and traditional storage solutions, including all-flash arrays, scale-out file, object platforms, hyper-converged infrastructure, and software-defined storage. Its CSG segment offers branded personal computers (PCs) including notebooks, desktops, and workstations and branded peripherals that include displays, docking stations, keyboards, mice, and webcam and audio devices, as well as third-party software and peripherals.</v>
     <v>120000</v>
@@ -5658,24 +5657,24 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>ONE DELL WAY, ROUND ROCK, TX, 78682 US</v>
-    <v>119.62</v>
+    <v>120.07</v>
     <v>Computers, Phones &amp; Household Electronics</v>
     <v>Stock</v>
-    <v>45553.99987446719</v>
+    <v>45554.683723935159</v>
     <v>62</v>
-    <v>115.94</v>
-    <v>81469612952</v>
+    <v>117.49</v>
+    <v>82927061412</v>
     <v>DELL TECHNOLOGIES INC.</v>
     <v>DELL TECHNOLOGIES INC.</v>
-    <v>117.58</v>
+    <v>120.07</v>
     <v>21.342400000000001</v>
-    <v>116.82</v>
     <v>115.99</v>
+    <v>118.065</v>
     <v>702384800</v>
     <v>DELL</v>
     <v>DELL TECHNOLOGIES INC. (XNYS:DELL)</v>
-    <v>89231</v>
-    <v>11513168</v>
+    <v>5658715</v>
+    <v>11347373</v>
     <v>2013</v>
   </rv>
   <rv s="2">
@@ -5874,7 +5873,7 @@
       <v t="s">%ProviderInfo</v>
     </a>
   </spbArrays>
-  <spbData count="8">
+  <spbData count="7">
     <spb s="0">
       <v>0</v>
       <v>Name</v>
@@ -5918,13 +5917,6 @@
       <v>from previous close</v>
       <v>from previous close</v>
       <v>Source: Nasdaq Last Sale</v>
-      <v>GMT</v>
-    </spb>
-    <spb s="4">
-      <v>Delayed 15 minutes</v>
-      <v>from previous close</v>
-      <v>from previous close</v>
-      <v>Source: Nasdaq</v>
       <v>GMT</v>
     </spb>
     <spb s="5">
@@ -69133,7 +69125,7 @@
   <dimension ref="B1:K13"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.6640625" defaultRowHeight="21.75" customHeight="1"/>
@@ -69405,8 +69397,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F51CD2FE-0785-5E4C-91F5-512BDFA3DC54}">
   <dimension ref="B1:L26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
+    <sheetView tabSelected="1" topLeftCell="C4" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
@@ -69489,15 +69481,15 @@
       </c>
       <c r="I3" s="151" cm="1">
         <f t="array" aca="1" ref="I3" ca="1">_FV(B3,"Price")</f>
-        <v>58.42</v>
+        <v>58.312100000000001</v>
       </c>
       <c r="J3" s="131">
         <f t="shared" ref="J3:J24" ca="1" si="0">((I3-F3)/F3)</f>
-        <v>-0.15025454545454542</v>
+        <v>-0.15182399999999999</v>
       </c>
       <c r="K3" s="172">
         <f t="shared" ref="K3:K24" ca="1" si="1">(I3*G3) - H3</f>
-        <v>-75.305143999999984</v>
+        <v>-76.091389719999995</v>
       </c>
       <c r="L3"/>
     </row>
@@ -69528,15 +69520,15 @@
       </c>
       <c r="I4" s="151" cm="1">
         <f t="array" aca="1" ref="I4" ca="1">_FV(B4,"Price")</f>
-        <v>139.81</v>
+        <v>140.75</v>
       </c>
       <c r="J4" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>0.39782043591281752</v>
+        <v>0.40721855628874232</v>
       </c>
       <c r="K4" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>199.30829000000006</v>
+        <v>204.01675</v>
       </c>
       <c r="L4"/>
     </row>
@@ -69567,15 +69559,15 @@
       </c>
       <c r="I5" s="151" cm="1">
         <f t="array" aca="1" ref="I5" ca="1">_FV(B5,"Price")</f>
-        <v>19.739999999999998</v>
+        <v>19.940000000000001</v>
       </c>
       <c r="J5" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>-9.44954128440368E-2</v>
+        <v>-8.532110091743117E-2</v>
       </c>
       <c r="K5" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>-47.390592000000083</v>
+        <v>-42.794752000000017</v>
       </c>
       <c r="L5"/>
     </row>
@@ -69606,15 +69598,15 @@
       </c>
       <c r="I6" s="151" cm="1">
         <f t="array" aca="1" ref="I6" ca="1">_FV(B6,"Price")</f>
-        <v>21.91</v>
+        <v>22.085000000000001</v>
       </c>
       <c r="J6" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>0.252</v>
+        <v>0.26200000000000007</v>
       </c>
       <c r="K6" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>140.00772399999994</v>
+        <v>145.12759400000004</v>
       </c>
       <c r="L6"/>
     </row>
@@ -69645,15 +69637,15 @@
       </c>
       <c r="I7" s="153" cm="1">
         <f t="array" aca="1" ref="I7" ca="1">_FV(B7,"Price")</f>
-        <v>220.69</v>
+        <v>228.9915</v>
       </c>
       <c r="J7" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>0.25065170576901274</v>
+        <v>0.29769636178170683</v>
       </c>
       <c r="K7" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>125.58097900000007</v>
+        <v>149.14976765000006</v>
       </c>
       <c r="L7"/>
     </row>
@@ -69684,15 +69676,15 @@
       </c>
       <c r="I8" s="153" cm="1">
         <f t="array" aca="1" ref="I8" ca="1">_FV(B8,"Price")</f>
-        <v>88.57</v>
+        <v>90.77</v>
       </c>
       <c r="J8" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>0.57766298539365857</v>
+        <v>0.61685073031706439</v>
       </c>
       <c r="K8" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>289.34553800000003</v>
+        <v>308.97701800000004</v>
       </c>
       <c r="L8"/>
     </row>
@@ -69723,15 +69715,15 @@
       </c>
       <c r="I9" s="153" cm="1">
         <f t="array" aca="1" ref="I9" ca="1">_FV(B9,"Price")</f>
-        <v>19.37</v>
+        <v>19.721</v>
       </c>
       <c r="J9" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.42316855270994636</v>
+        <v>-0.41271590232281119</v>
       </c>
       <c r="K9" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>-211.982167</v>
+        <v>-206.74493110000003</v>
       </c>
       <c r="L9"/>
     </row>
@@ -69762,15 +69754,15 @@
       </c>
       <c r="I10" s="155" cm="1">
         <f t="array" aca="1" ref="I10" ca="1">_FV(B10,"Price")</f>
-        <v>60.32</v>
+        <v>61.66</v>
       </c>
       <c r="J10" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>3.6426116838487926E-2</v>
+        <v>5.9450171821305735E-2</v>
       </c>
       <c r="K10" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>18.270751999999902</v>
+        <v>29.806275999999912</v>
       </c>
       <c r="L10"/>
     </row>
@@ -69801,15 +69793,15 @@
       </c>
       <c r="I11" s="155" cm="1">
         <f t="array" aca="1" ref="I11" ca="1">_FV(B11,"Price")</f>
-        <v>83.48</v>
+        <v>85.39</v>
       </c>
       <c r="J11" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>-8.5351155911033108E-2</v>
+        <v>-6.4424235783937717E-2</v>
       </c>
       <c r="K11" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>-42.778279999999995</v>
+        <v>-32.29428999999999</v>
       </c>
       <c r="L11"/>
     </row>
@@ -69840,15 +69832,15 @@
       </c>
       <c r="I12" s="155" cm="1">
         <f t="array" aca="1" ref="I12" ca="1">_FV(B12,"Price")</f>
-        <v>94.33</v>
+        <v>96.15</v>
       </c>
       <c r="J12" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>0.12700119474313018</v>
+        <v>0.14874551971326166</v>
       </c>
       <c r="K12" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>63.612214999999992</v>
+        <v>74.505825000000073</v>
       </c>
       <c r="L12"/>
     </row>
@@ -69879,15 +69871,15 @@
       </c>
       <c r="I13" s="155" cm="1">
         <f t="array" aca="1" ref="I13" ca="1">_FV(B13,"Price")</f>
-        <v>93.75</v>
+        <v>95.885000000000005</v>
       </c>
       <c r="J13" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.19851243908694535</v>
+        <v>-0.18025989569975201</v>
       </c>
       <c r="K13" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>-99.459374999999966</v>
+        <v>-90.314956499999994</v>
       </c>
       <c r="L13"/>
     </row>
@@ -69918,15 +69910,15 @@
       </c>
       <c r="I14" s="157" cm="1">
         <f t="array" aca="1" ref="I14" ca="1">_FV(B14,"Price")</f>
-        <v>27.4</v>
+        <v>27.45</v>
       </c>
       <c r="J14" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>7.4931345625735599E-2</v>
+        <v>7.6892899176147542E-2</v>
       </c>
       <c r="K14" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>37.574399999999969</v>
+        <v>38.557199999999966</v>
       </c>
       <c r="L14"/>
     </row>
@@ -69996,15 +69988,15 @@
       </c>
       <c r="I16" s="159" cm="1">
         <f t="array" aca="1" ref="I16" ca="1">_FV(B16,"Price")</f>
-        <v>36.840000000000003</v>
+        <v>37.200000000000003</v>
       </c>
       <c r="J16" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.24072547403132727</v>
+        <v>-0.23330585325638911</v>
       </c>
       <c r="K16" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>-116.74999999999994</v>
+        <v>-113.14999999999998</v>
       </c>
       <c r="L16"/>
     </row>
@@ -70035,15 +70027,15 @@
       </c>
       <c r="I17" s="159" cm="1">
         <f t="array" aca="1" ref="I17" ca="1">_FV(B17,"Price")</f>
-        <v>76.459999999999994</v>
+        <v>76.91</v>
       </c>
       <c r="J17" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>9.3066476054324387E-2</v>
+        <v>9.9499642601858382E-2</v>
       </c>
       <c r="K17" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>45.579999999999927</v>
+        <v>48.730000000000018</v>
       </c>
       <c r="L17"/>
     </row>
@@ -70074,15 +70066,15 @@
       </c>
       <c r="I18" s="159" cm="1">
         <f t="array" aca="1" ref="I18" ca="1">_FV(B18,"Price")</f>
-        <v>60</v>
+        <v>61.06</v>
       </c>
       <c r="J18" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>-3.5059504663879054E-2</v>
+        <v>-1.8012222579607551E-2</v>
       </c>
       <c r="K18" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>-17.439999999999998</v>
+        <v>-8.9599999999999795</v>
       </c>
       <c r="L18"/>
     </row>
@@ -70113,15 +70105,15 @@
       </c>
       <c r="I19" s="159" cm="1">
         <f t="array" aca="1" ref="I19" ca="1">_FV(B19,"Price")</f>
-        <v>10.01</v>
+        <v>10.17</v>
       </c>
       <c r="J19" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.2529850746268657</v>
+        <v>-0.241044776119403</v>
       </c>
       <c r="K19" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>-126.79616999999996</v>
+        <v>-120.81488999999999</v>
       </c>
       <c r="L19"/>
     </row>
@@ -70152,15 +70144,15 @@
       </c>
       <c r="I20" s="213" cm="1">
         <f t="array" aca="1" ref="I20" ca="1">_FV(B20,"Price")</f>
-        <v>402.72</v>
+        <v>402.48</v>
       </c>
       <c r="J20" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>2.3690899847483606E-2</v>
+        <v>2.3080833756990445E-2</v>
       </c>
       <c r="K20" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>11.921600000000069</v>
+        <v>11.614399999999989</v>
       </c>
       <c r="L20"/>
     </row>
@@ -70191,15 +70183,15 @@
       </c>
       <c r="I21" s="216" cm="1">
         <f t="array" aca="1" ref="I21" ca="1">_FV(B21,"Price")</f>
-        <v>21.91</v>
+        <v>21.95</v>
       </c>
       <c r="J21" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.5723270440251635E-2</v>
+        <v>-1.3926325247080065E-2</v>
       </c>
       <c r="K21" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>-7.8825850000000059</v>
+        <v>-6.9823250000000598</v>
       </c>
     </row>
     <row r="22" spans="2:12">
@@ -70229,15 +70221,15 @@
       </c>
       <c r="I22" s="216" cm="1">
         <f t="array" aca="1" ref="I22" ca="1">_FV(B22,"Price")</f>
-        <v>67.849999999999994</v>
+        <v>67.97</v>
       </c>
       <c r="J22" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.5703618609994344E-2</v>
+        <v>-2.3980470993681818E-2</v>
       </c>
       <c r="K22" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>-11.472605000000101</v>
+        <v>-10.606841000000031</v>
       </c>
     </row>
     <row r="23" spans="2:12">
@@ -70267,15 +70259,15 @@
       </c>
       <c r="I23" s="216" cm="1">
         <f t="array" aca="1" ref="I23" ca="1">_FV(B23,"Price")</f>
-        <v>97.84</v>
+        <v>102</v>
       </c>
       <c r="J23" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>-3.2532384060120559E-2</v>
+        <v>8.6027884900623415E-3</v>
       </c>
       <c r="K23" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>-16.280855999999972</v>
+        <v>4.328200000000038</v>
       </c>
     </row>
     <row r="24" spans="2:12">
@@ -70305,25 +70297,25 @@
       </c>
       <c r="I24" s="216" cm="1">
         <f t="array" aca="1" ref="I24" ca="1">_FV(B24,"Price")</f>
-        <v>115.99</v>
+        <v>118.065</v>
       </c>
       <c r="J24" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.8531054323912777E-2</v>
+        <v>-9.7309189372151881E-4</v>
       </c>
       <c r="K24" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>-9.2719940000000634</v>
+        <v>-0.4752390000000446</v>
       </c>
     </row>
     <row r="26" spans="2:12" ht="13">
       <c r="K26" s="171">
         <f ca="1">SUM(K3:K24)</f>
-        <v>400.10284799999971</v>
+        <v>557.29453433000003</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="J20:J24 J3:K19">
+  <conditionalFormatting sqref="J3:K19 J20:J24">
     <cfRule type="cellIs" dxfId="5" priority="3" operator="lessThan">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
vault backup: 2024-09-20 11:47:27
</commit_message>
<xml_diff>
--- a/_system/Attachments/Portfolio Management.xlsx
+++ b/_system/Attachments/Portfolio Management.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martin/repos/tomesink/obsidian/_system/Attachments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE2FF8F1-0296-1C43-91F9-2ACAFD2A8421}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C66517AD-F217-FF4B-9C0E-B364BEEE3B57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3300" yWindow="980" windowWidth="33800" windowHeight="18860" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3300" yWindow="980" windowWidth="33800" windowHeight="18860" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Stocks Performance" sheetId="1" r:id="rId1"/>
@@ -4582,8 +4582,8 @@
     <v>83.25</v>
     <v>52.770499999999998</v>
     <v>0.52459999999999996</v>
-    <v>-0.1079</v>
-    <v>-1.8470000000000001E-3</v>
+    <v>-0.02</v>
+    <v>-3.4229999999999997E-4</v>
     <v>USD</v>
     <v>CVS Health Corporation is a health solutions company. The Company operates in four segments: Health Care Benefits, Health Services, Pharmacy &amp; Consumer Wellness, and Corporate/Other. Its Health Care Benefits segment offer a range of traditional, voluntary and consumer-directed health insurance products and related services, including medical, pharmacy, dental and behavioral health plans, medical management capabilities, Medicare Advantage and Medicare supplement plans, and Medicaid health care management services. Its Health Services segment provides a full range of pharmacy benefit management solutions, delivers health care services in its medical clinics, virtually, and in the home, and offers provider enablement solutions. The Pharmacy &amp; Consumer Wellness segment dispenses prescriptions in its retail pharmacies and through its infusion operations, provides ancillary pharmacy services, including pharmacy patient care programs, diagnostic testing and vaccination administration.</v>
     <v>300000</v>
@@ -4594,20 +4594,20 @@
     <v>59.1</v>
     <v>Healthcare Providers &amp; Services</v>
     <v>Stock</v>
-    <v>45554.683699687499</v>
+    <v>45554.99989664297</v>
     <v>0</v>
     <v>58.12</v>
-    <v>73355397245</v>
+    <v>73465973600</v>
     <v>CVS HEALTH CORPORATION</v>
     <v>CVS HEALTH CORPORATION</v>
-    <v>58.87</v>
+    <v>58.7</v>
     <v>10.3926</v>
     <v>58.42</v>
-    <v>58.312100000000001</v>
+    <v>58.4</v>
     <v>1257979000</v>
     <v>CVS</v>
     <v>CVS HEALTH CORPORATION (XNYS:CVS)</v>
-    <v>1754217</v>
+    <v>788</v>
     <v>7591748</v>
     <v>1996</v>
   </rv>
@@ -4624,7 +4624,7 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>4</v>
+    <v>5</v>
     <v>en-GB</v>
     <v>a1qclh</v>
     <v>268435456</v>
@@ -4633,8 +4633,8 @@
     <v>165.32</v>
     <v>74</v>
     <v>2.0011000000000001</v>
-    <v>0.94</v>
-    <v>6.7229999999999998E-3</v>
+    <v>-1.89</v>
+    <v>-1.3517999999999999E-2</v>
     <v>USD</v>
     <v>Crocs, Inc. is engaged in the design, development, worldwide marketing, distribution, and sale of casual lifestyle footwear and accessories for women, men, and children. The Company’s segments include Crocs Brand and the HEYDUDE Brand. The Company’s Crocs Brand collection contains Croslite material, a molded footwear technology, delivering extraordinary comfort with each step. Its Croslite materials are formulated to create soft, comfortable, lightweight, non-marking, and odor-resistant footwear. The HEYDUDE Brand offers shoes with a versatile silhouette. It sells its products in more than 80 countries, through two distribution channels: wholesale and direct-to-consumer. Its wholesale channel includes domestic and international multi-brand retailers, mono-branded partner stores, e-tailers, and distributors; its direct-to-consumer channel includes Company-operated retail stores, Company-operated e-commerce sites, and third-party marketplaces.</v>
     <v>7030</v>
@@ -4645,20 +4645,20 @@
     <v>144.32</v>
     <v>Textiles &amp; Apparel</v>
     <v>Stock</v>
-    <v>45554.683689594531</v>
+    <v>45554.991820578121</v>
     <v>3</v>
-    <v>140.1</v>
-    <v>8358457047</v>
+    <v>134.44499999999999</v>
+    <v>8190397129</v>
     <v>CROCS, INC.</v>
     <v>CROCS, INC.</v>
     <v>142.94999999999999</v>
-    <v>10.514799999999999</v>
+    <v>10.3727</v>
     <v>139.81</v>
-    <v>140.75</v>
+    <v>137.91999999999999</v>
     <v>59385130</v>
     <v>CROX</v>
     <v>CROCS, INC. (XNAS:CROX)</v>
-    <v>268511</v>
+    <v>354</v>
     <v>937487</v>
     <v>2005</v>
   </rv>
@@ -4675,7 +4675,7 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>4</v>
+    <v>5</v>
     <v>en-GB</v>
     <v>a25yfr</v>
     <v>268435456</v>
@@ -4684,8 +4684,8 @@
     <v>30.07</v>
     <v>17.71</v>
     <v>1.5144</v>
-    <v>0.2</v>
-    <v>1.0132E-2</v>
+    <v>0.23</v>
+    <v>1.1651E-2</v>
     <v>USD</v>
     <v>Wabash National Corporation provides connected solutions for the transportation, logistics and distribution industries. The Company designs and manufactures products including dry freight and refrigerated trailers, platform trailers, tank trailers, dry and refrigerated truck bodies, structural composite panels and products, transportation, logistics, and distribution industry parts and services, and specialty food grade processing equipment. The Company’s Transportation Solutions (TS) segment comprises the design and manufacturing operations for the Company’s transportation-related equipment and products. This includes dry and refrigerated van trailers, platform trailers, tank trailers and truck-mounted tanks, truck-mounted dry and refrigerated truck bodies and EcoNex technology products. Its Parts &amp; Services (P&amp;S) segment is comprised of the Company’s parts and services businesses as well as the upfitting component of truck bodies business. It also includes DuraPlate composite panels.</v>
     <v>6700</v>
@@ -4693,23 +4693,23 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>3900 Mccarty Lane, LAFAYETTE, IN, 47905 US</v>
-    <v>20.14</v>
+    <v>20.2</v>
     <v>Machinery, Equipment &amp; Components</v>
     <v>Stock</v>
-    <v>45554.683655717185</v>
+    <v>45554.958333333336</v>
     <v>6</v>
     <v>19.79</v>
-    <v>877344646</v>
+    <v>878664623</v>
     <v>WABASH NATIONAL CORPORATION</v>
     <v>WABASH NATIONAL CORPORATION</v>
-    <v>20.059999999999999</v>
-    <v>6.0552999999999999</v>
+    <v>20.2</v>
+    <v>6.1258999999999997</v>
     <v>19.739999999999998</v>
-    <v>19.940000000000001</v>
+    <v>19.97</v>
     <v>43999230</v>
     <v>WNC</v>
     <v>WABASH NATIONAL CORPORATION (XNYS:WNC)</v>
-    <v>118349</v>
+    <v>410448</v>
     <v>435088</v>
     <v>1991</v>
   </rv>
@@ -4726,7 +4726,7 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>4</v>
+    <v>5</v>
     <v>en-GB</v>
     <v>a1pfoc</v>
     <v>268435456</v>
@@ -4735,8 +4735,8 @@
     <v>26.4</v>
     <v>16.12</v>
     <v>1.0366</v>
-    <v>0.17499999999999999</v>
-    <v>7.9869999999999993E-3</v>
+    <v>0.44</v>
+    <v>2.0081999999999999E-2</v>
     <v>USD</v>
     <v>Perdoceo Education Corporation, through its academic institutions, offers quality postsecondary education primarily online to a diverse student population, along with campus-based and blended learning programs. The Company's academic institutions include Colorado Technical University (CTU) and the American InterContinental University System (AIUS), which provides degree programs from the associate through doctoral level as well as non-degree seeking and professional development programs. Its academic institutions offer students industry-relevant and career-focused academic programs. CTU offers academic programs in the career-oriented disciplines of business and management, nursing, healthcare management, computer science, engineering, information systems and technology, project management, cybersecurity and criminal justice. AIUS offers academic programs in the career-oriented disciplines of business studies, information technologies, education, health sciences and criminal justice.</v>
     <v>2319</v>
@@ -4744,23 +4744,23 @@
     <v>XNAS</v>
     <v>XNAS</v>
     <v>1750 E. GOLF ROAD, SCHAUMBURG, IL, 60173 US</v>
-    <v>22.34</v>
+    <v>22.36</v>
     <v>Miscellaneous Educational Service Providers</v>
     <v>Stock</v>
-    <v>45554.683665995311</v>
+    <v>45554.904691469528</v>
     <v>9</v>
     <v>21.840599999999998</v>
-    <v>1450397701</v>
+    <v>1467801160</v>
     <v>PERDOCEO EDUCATION CORPORATION</v>
     <v>PERDOCEO EDUCATION CORPORATION</v>
     <v>22.25</v>
-    <v>10.7677</v>
+    <v>10.984</v>
     <v>21.91</v>
-    <v>22.085000000000001</v>
+    <v>22.35</v>
     <v>65673430</v>
     <v>PRDO</v>
     <v>PERDOCEO EDUCATION CORPORATION (XNAS:PRDO)</v>
-    <v>73088</v>
+    <v>284119</v>
     <v>383603</v>
     <v>1994</v>
   </rv>
@@ -4786,8 +4786,8 @@
     <v>237.23</v>
     <v>164.07499999999999</v>
     <v>1.2446999999999999</v>
-    <v>8.3015000000000008</v>
-    <v>3.7616000000000004E-2</v>
+    <v>8.18</v>
+    <v>3.7066000000000002E-2</v>
     <v>USD</v>
     <v>Apple Inc. designs, manufactures and markets smartphones, personal computers, tablets, wearables and accessories, and sells a variety of related services. Its product categories include iPhone, Mac, iPad, and Wearables, Home and Accessories. Its software platforms include iOS, iPadOS, macOS, watchOS, and tvOS. Its services include advertising, AppleCare, cloud services, digital content and payment services. It operates various platforms, including the App Store, that allow customers to discover and download applications and digital content, such as books, music, video, games and podcasts. It also offers digital content through subscription-based services, including Apple Arcade, Apple Fitness+, Apple Music, Apple News+ and Apple TV+. Its products include iPhone 15 Pro, iPhone 15, iPhone 14, iPhone 13, MacBook Air, MacBook Pro, iMac, Mac mini, Mac Studio, Mac Pro, and others. It also provides DarwinAI, which specializes in visual quality inspection using its Explainable AI platform.</v>
     <v>161000</v>
@@ -4798,20 +4798,20 @@
     <v>229.82</v>
     <v>Computers, Phones &amp; Household Electronics</v>
     <v>Stock</v>
-    <v>45554.683719258595</v>
+    <v>45554.999953321094</v>
     <v>12</v>
-    <v>224.64</v>
-    <v>3481618824810</v>
+    <v>224.63</v>
+    <v>3479771521800</v>
     <v>APPLE INC.</v>
     <v>APPLE INC.</v>
-    <v>225.01</v>
-    <v>33.601300000000002</v>
+    <v>224.99</v>
+    <v>34.846699999999998</v>
     <v>220.69</v>
-    <v>228.9915</v>
+    <v>228.87</v>
     <v>15204140000</v>
     <v>AAPL</v>
     <v>APPLE INC. (XNAS:AAPL)</v>
-    <v>32376781</v>
+    <v>73844</v>
     <v>44471580</v>
     <v>1977</v>
   </rv>
@@ -4828,7 +4828,7 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>4</v>
+    <v>5</v>
     <v>en-GB</v>
     <v>a1ncgh</v>
     <v>268435456</v>
@@ -4837,8 +4837,8 @@
     <v>92.82</v>
     <v>50.134999999999998</v>
     <v>0.99250000000000005</v>
-    <v>2.2000000000000002</v>
-    <v>2.4839000000000003E-2</v>
+    <v>2.42</v>
+    <v>2.7323E-2</v>
     <v>USD</v>
     <v>Allison Transmission Holdings, Inc. is a designer and manufacturer of propulsion solutions for commercial and defense vehicles. The Company is also a manufacturer of medium-and heavy-duty fully automatic transmissions. Its products are used in a variety of applications, including on-highway trucks, including distribution, refuse, construction, fire and emergency; buses, including school, transit and coach; motorhomes, off-highway vehicles, and equipment, including energy, mining and construction applications; and defense vehicles, including tactical wheeled and tracked. The Company operates in approximately 150 countries. The Company has manufacturing facilities in the United States, Hungary and India, as well as global engineering resources, including electrification engineering centers in Indianapolis, Indiana, Auburn Hills, Michigan and London in the United Kingdom. The Company also has approximately 1,600 independent distributor and dealer locations worldwide.</v>
     <v>3700</v>
@@ -4846,23 +4846,23 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>One Allison Way, INDIANAPOLIS, IN, 46222 US</v>
-    <v>90.91</v>
+    <v>91.22</v>
     <v>Machinery, Equipment &amp; Components</v>
     <v>Stock</v>
-    <v>45554.683676793749</v>
+    <v>45554.958333378905</v>
     <v>15</v>
     <v>89.39</v>
-    <v>7909505367</v>
+    <v>7928675701</v>
     <v>ALLISON TRANSMISSION HOLDINGS, INC.</v>
     <v>ALLISON TRANSMISSION HOLDINGS, INC.</v>
-    <v>89.95</v>
-    <v>11.5815</v>
+    <v>90.1</v>
+    <v>11.8979</v>
     <v>88.57</v>
-    <v>90.77</v>
+    <v>90.99</v>
     <v>87137880</v>
     <v>ALSN</v>
     <v>ALLISON TRANSMISSION HOLDINGS, INC. (XNYS:ALSN)</v>
-    <v>145905</v>
+    <v>571135</v>
     <v>483317</v>
     <v>2007</v>
   </rv>
@@ -4879,7 +4879,7 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>4</v>
+    <v>5</v>
     <v>en-GB</v>
     <v>az23tc</v>
     <v>268435456</v>
@@ -4888,8 +4888,8 @@
     <v>40.695</v>
     <v>18</v>
     <v>2.0030999999999999</v>
-    <v>0.35099999999999998</v>
-    <v>1.8121000000000002E-2</v>
+    <v>0.32</v>
+    <v>1.652E-2</v>
     <v>USD</v>
     <v>Par Pacific Holdings, Inc. is an energy company, which provides both renewable and conventional fuels to the western United States. It owns and operates 125,000 barrels per day of combined refining capacity across three locations and an energy infrastructure network, including 7.6 million barrels of storage, and marine, rail, rack and pipeline assets. The Company has three segments. Refining segment owns and operates four refineries with total operating crude oil throughput capacity of 219 thousand barrels per day (Mbpd). Retail segment operates fuel retail outlets in Hawaii, Washington and Idaho. It operates convenience stores and fuel retail sites under Hele and nomnom brands, 76 branded fuel retail sites and other sites operated by third parties that sell gasoline, diesel, and retail merchandise, such as soft drinks, prepared foods, and other sundries. Logistics segment operates a multi-modal logistics network spanning the Pacific, the Northwest, and the Rocky Mountain regions.</v>
     <v>1814</v>
@@ -4900,20 +4900,20 @@
     <v>20.2</v>
     <v>Oil &amp; Gas</v>
     <v>Stock</v>
-    <v>45554.683513923439</v>
+    <v>45554.958333356248</v>
     <v>18</v>
     <v>19.555</v>
-    <v>1110901087</v>
+    <v>1109154830</v>
     <v>PAR PACIFIC HOLDINGS, INC.</v>
     <v>PAR PACIFIC HOLDINGS, INC.</v>
-    <v>19.98</v>
-    <v>3.3748</v>
+    <v>19.809999999999999</v>
+    <v>3.4306000000000001</v>
     <v>19.37</v>
-    <v>19.721</v>
+    <v>19.690000000000001</v>
     <v>56330870</v>
     <v>PARR</v>
     <v>PAR PACIFIC HOLDINGS, INC. (XNYS:PARR)</v>
-    <v>191838</v>
+    <v>737114</v>
     <v>911057</v>
     <v>2005</v>
   </rv>
@@ -4930,7 +4930,7 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>4</v>
+    <v>5</v>
     <v>en-GB</v>
     <v>a1v177</v>
     <v>268435456</v>
@@ -4939,8 +4939,8 @@
     <v>84.44</v>
     <v>38.5</v>
     <v>1.3108</v>
-    <v>1.34</v>
-    <v>2.2214999999999999E-2</v>
+    <v>2.11</v>
+    <v>3.4980000000000004E-2</v>
     <v>USD</v>
     <v>Hyster-Yale, Inc., formerly Hyster-Yale Materials Handling, Inc., through its wholly owned operating subsidiary, Hyster-Yale Materials Handling, designs, engineers, manufactures, sells, and services a comprehensive line of lift trucks, attachments, aftermarket parts and technology solutions marketed globally primarily under the Hyster and Yale brand names. The Company's business segments include Lift Trucks, Attachments and Fuel Cells. The Hyster-Yale Maximal brand provides trucks for customers requiring fundamental lift truck performance. The Lift Truck segment is focused on fuel cell-powered battery box replacements and integrated fuel cell engine solutions. Hyster- Yale’s attachment subsidiary, Bolzoni S.p.A., is a producer of attachments, forks, and lift tables under the Bolzoni, Auramo and Meyer brand names. The Fuel Cell business, Nuvera Fuel Cells, is an alternative-power technology company focused on fuel cell stacks and engines.</v>
     <v>8600</v>
@@ -4948,23 +4948,23 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>5875 LANDERBROOK DRIVE, SUITE 300, CLEVELAND, OH, 44124 US</v>
-    <v>61.994999999999997</v>
+    <v>62.65</v>
     <v>Machinery, Equipment &amp; Components</v>
     <v>Stock</v>
-    <v>45554.682903772657</v>
+    <v>45554.958333378905</v>
     <v>21</v>
     <v>61.01</v>
-    <v>1079120909</v>
+    <v>1092596794</v>
     <v>HYSTER-YALE, INC.</v>
     <v>HYSTER-YALE, INC.</v>
-    <v>61.57</v>
-    <v>6.0319000000000003</v>
+    <v>61.8</v>
+    <v>6.2428999999999997</v>
     <v>60.32</v>
-    <v>61.66</v>
+    <v>62.43</v>
     <v>17501150</v>
     <v>HY</v>
     <v>HYSTER-YALE, INC. (XNYS:HY)</v>
-    <v>12610</v>
+    <v>61542</v>
     <v>66109</v>
     <v>1999</v>
   </rv>
@@ -4975,13 +4975,13 @@
     <v>https://www.bing.com/financeapi/forcetrigger?t=a1zvsm&amp;q=XNYS%3aPII&amp;form=skydnc</v>
     <v>Learn more on Bing</v>
   </rv>
-  <rv s="1">
-    <v>0</v>
+  <rv s="3">
+    <v>6</v>
     <v>Polaris Inc. (XNYS:PII)</v>
     <v>2</v>
-    <v>3</v>
+    <v>7</v>
     <v>Finance</v>
-    <v>4</v>
+    <v>8</v>
     <v>en-GB</v>
     <v>a1zvsm</v>
     <v>268435456</v>
@@ -4990,8 +4990,8 @@
     <v>107.955</v>
     <v>71.900000000000006</v>
     <v>1.5097</v>
-    <v>1.91</v>
-    <v>2.2879999999999998E-2</v>
+    <v>2.38</v>
+    <v>2.8510000000000001E-2</v>
     <v>USD</v>
     <v>Polaris Inc. is engaged in designing, engineering, manufacturing and marketing of powersports vehicles. The Company also designs and manufactures or sources parts, garments and accessories (PG&amp;A), which includes aftermarket accessories and apparel. The Company operates through three segments: Off Road, On Road and Marine. The Off Road segment consists of off-road vehicles and snowmobiles. The On Road segment designs and manufactures motorcycles, moto-roadsters, light duty hauling, and passenger vehicles. The Marine segment designs and manufactures boats that are designed to compete in key segments of the recreational marine industry, specifically pontoon and deck boats. Its product line-up includes the RANGER, RZR and Polaris XPEDITION and GENERAL side-by-side off-road vehicles; Sportsman all-terrain off-road vehicles; military and commercial off-road vehicles; snowmobiles; Indian Motorcycle mid-size and heavyweight motorcycles; Slingshot moto-roadsters, and pontoon and deck boats.</v>
     <v>18500</v>
@@ -4999,23 +4999,24 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>2100 HIGHWAY 55, MEDINA, MN, 55340-9770 US</v>
-    <v>85.59</v>
+    <v>85.9</v>
     <v>Leisure Products</v>
     <v>Stock</v>
-    <v>45554.683616782029</v>
+    <v>45554.958333356248</v>
     <v>24</v>
     <v>84.364999999999995</v>
-    <v>4760324281</v>
+    <v>4786525855</v>
     <v>Polaris Inc.</v>
     <v>Polaris Inc.</v>
-    <v>85.59</v>
-    <v>14.6219</v>
+    <v>85.55</v>
+    <v>15.0388</v>
     <v>83.48</v>
-    <v>85.39</v>
+    <v>85.86</v>
+    <v>85.86</v>
     <v>55748030</v>
     <v>PII</v>
     <v>Polaris Inc. (XNYS:PII)</v>
-    <v>109467</v>
+    <v>107</v>
     <v>461892</v>
     <v>1994</v>
   </rv>
@@ -5032,7 +5033,7 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>4</v>
+    <v>5</v>
     <v>en-GB</v>
     <v>aw21cw</v>
     <v>268435456</v>
@@ -5041,8 +5042,8 @@
     <v>114.29989999999999</v>
     <v>75.430000000000007</v>
     <v>1.7444</v>
-    <v>1.82</v>
-    <v>1.9293999999999999E-2</v>
+    <v>3.37</v>
+    <v>3.5726000000000001E-2</v>
     <v>USD</v>
     <v>CONSOL Energy Inc. is a producer and exporter of high-Btu bituminous thermal coal and metallurgical coal. It owns and operates longwall mining operations in the Northern Appalachian Basin. Its flagship operation is the Pennsylvania Mining Complex, located over 26 miles southwest of Pittsburgh, near the city of Washington and the borough of Waynesburg all in Pennsylvania, and consists of three deep longwall mining operations: the Bailey Mine, the Enlow Fork Mine and the Harvey Mine, as well as a centralized preparation plant. Its segments include the PAMC and the CONSOL Marine Terminal. The PAMC includes the Bailey Mine, the Enlow Fork Mine, the Harvey Mine and a centralized preparation plant. The PAMC segment's principal activities include the mining, preparation and marketing of bituminous coal, sold primarily to industrial end-users, metallurgical end-users and power generators. The CONSOL Marine Terminal segment provides coal export terminal services through the Port of Baltimore.</v>
     <v>2020</v>
@@ -5050,23 +5051,23 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>275 TECHNOLOGY DRIVE, SUITE #101, CANONSBURG, PA, 15317 US</v>
-    <v>96.94</v>
+    <v>97.91</v>
     <v>Coal</v>
     <v>Stock</v>
-    <v>45554.68352082109</v>
+    <v>45554.958333367969</v>
     <v>27</v>
     <v>95.04</v>
-    <v>2826159064</v>
+    <v>2871718571</v>
     <v>CONSOL ENERGY INC.</v>
     <v>CONSOL ENERGY INC.</v>
-    <v>96.2</v>
-    <v>7.0412999999999997</v>
+    <v>96.94</v>
+    <v>7.2929000000000004</v>
     <v>94.33</v>
-    <v>96.15</v>
+    <v>97.7</v>
     <v>29393230</v>
     <v>CEIX</v>
     <v>CONSOL ENERGY INC. (XNYS:CEIX)</v>
-    <v>90477</v>
+    <v>6</v>
     <v>492196</v>
     <v>2017</v>
   </rv>
@@ -5083,7 +5084,7 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>4</v>
+    <v>5</v>
     <v>en-GB</v>
     <v>a1n1r7</v>
     <v>268435456</v>
@@ -5092,8 +5093,8 @@
     <v>127.3484</v>
     <v>84.35</v>
     <v>1.2448999999999999</v>
-    <v>2.1349999999999998</v>
-    <v>2.2772999999999998E-2</v>
+    <v>2.08</v>
+    <v>2.2187000000000002E-2</v>
     <v>USD</v>
     <v>AGCO Corporation is a designer, manufacturer and distributor of agricultural machinery and precision agriculture technology. The Company sells a range of agricultural equipment, including tractors, combines, self-propelled sprayers, hay tools, forage equipment, seeding and tillage equipment, implements, and grain storage and protein production systems. It provides telemetry-based fleet management tools, including remote monitoring and diagnostics, which help farmers improve uptime, machine and yield optimization, mixed fleet optimization and decision support. The Company's Precision Planting, Headsight and Intelligent Ag Solutions brands provide retrofit solutions to upgrade farmers existing equipment to improve their planting, liquid application and harvest operations. The Company’s Precision Planting, Headsight, JCA and Intelligent Ag Solutions brands also sell precision agriculture solutions around the crop cycle to third party original equipment manufacturers (OEMs).</v>
     <v>27900</v>
@@ -5101,23 +5102,23 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>4205 River Green Pkway, DULUTH, GA, 30096 US</v>
-    <v>95.96</v>
+    <v>96.49</v>
     <v>Machinery, Equipment &amp; Components</v>
     <v>Stock</v>
-    <v>45554.683582985941</v>
+    <v>45554.958333356248</v>
     <v>30</v>
-    <v>94.64</v>
-    <v>7157076935</v>
+    <v>94.62</v>
+    <v>7152971609</v>
     <v>AGCO CORPORATION</v>
     <v>AGCO CORPORATION</v>
-    <v>95.36</v>
-    <v>16.700299999999999</v>
+    <v>95.59</v>
+    <v>17.070900000000002</v>
     <v>93.75</v>
-    <v>95.885000000000005</v>
+    <v>95.83</v>
     <v>74642300</v>
     <v>AGCO</v>
     <v>AGCO CORPORATION (XNYS:AGCO)</v>
-    <v>134692</v>
+    <v>569964</v>
     <v>739418</v>
     <v>1991</v>
   </rv>
@@ -5134,7 +5135,7 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>4</v>
+    <v>5</v>
     <v>en-GB</v>
     <v>a1vuw7</v>
     <v>268435456</v>
@@ -5143,8 +5144,8 @@
     <v>30.1</v>
     <v>24.01</v>
     <v>1.1547000000000001</v>
-    <v>0.05</v>
-    <v>1.825E-3</v>
+    <v>-0.09</v>
+    <v>-3.2850000000000002E-3</v>
     <v>USD</v>
     <v>Ituran Location and Control Ltd. is a provider of location-based services, consisting of stolen vehicle recovery (SVR), fleet management services and other tracking services. The Company also provides wireless communication products used in connection with its location-based services and various other applications. Its operations consist of two segments: location-based services and wireless communications products. Its location-based services segment consists of its SVR and tracking services, fleet management and value-added services consisted of personal locater services and concierge services. Its wireless communications products segment consists of short and medium range two-way machine-to-machine wireless communications products that are used for various applications, including automatic vehicle location (AVL) and automatic vehicle identification. It primarily provides its services, as well as sells and leases its products in Israel, Brazil, Argentina and the United States.</v>
     <v>2841</v>
@@ -5155,20 +5156,20 @@
     <v>28</v>
     <v>Communications &amp; Networking</v>
     <v>Stock</v>
-    <v>45554.682208680468</v>
+    <v>45554.996892245312</v>
     <v>33</v>
-    <v>27.38</v>
-    <v>546078771</v>
+    <v>27.31</v>
+    <v>543293669</v>
     <v>ITURAN LOCATION AND CONTROL LTD.</v>
     <v>ITURAN LOCATION AND CONTROL LTD.</v>
     <v>27.78</v>
-    <v>10.7311</v>
+    <v>10.6959</v>
     <v>27.4</v>
-    <v>27.45</v>
+    <v>27.31</v>
     <v>19893580</v>
     <v>ITRN</v>
     <v>ITURAN LOCATION AND CONTROL LTD. (XNAS:ITRN)</v>
-    <v>12952</v>
+    <v>37008</v>
     <v>82373</v>
     <v>1994</v>
   </rv>
@@ -5185,17 +5186,17 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>4</v>
+    <v>5</v>
     <v>en-GB</v>
     <v>a1sea2</v>
     <v>268435456</v>
     <v>1</v>
     <v>Powered by Refinitiv</v>
-    <v>14.62</v>
+    <v>14.475</v>
     <v>6.37</v>
     <v>2.15</v>
-    <v>0</v>
-    <v>0</v>
+    <v>-0.03</v>
+    <v>-2.2759999999999998E-3</v>
     <v>USD</v>
     <v>Everi Holdings Inc. develops and offers products and services that provide gaming entertainment, improve its customers’ patron engagement, and help its casino customers operate their businesses. It develops and supplies entertaining game content, gaming machines and gaming systems and services for land-based and iGaming operators. It operates through two segments: Games and Financial Technology Solutions (FinTech). The Games segment provides gaming operators with gaming technology and entertainment products and services, including gaming machines, primarily comprising Class II, Class III and Historic Horse Racing slot machines placed under participation and fixed-fee lease arrangements or sold to casino customers. The FinTech segment provides gaming operators with financial technology products and services, including financial access and related services supporting digital, cashless and physical cash options across mobile, assisted and self-service channels.</v>
     <v>2200</v>
@@ -5203,36 +5204,36 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>7250 S Tenaya Way Ste 100, LAS VEGAS, NV, 89113-2175 US</v>
-    <v>13.219900000000001</v>
+    <v>13.22</v>
     <v>Hotels &amp; Entertainment Services</v>
     <v>Stock</v>
-    <v>45554.683597499999</v>
+    <v>45554.958333367969</v>
     <v>36</v>
-    <v>13.18</v>
-    <v>1124564784</v>
+    <v>13.14</v>
+    <v>1122005077</v>
     <v>EVERI HOLDINGS INC.</v>
     <v>EVERI HOLDINGS INC.</v>
-    <v>13.2</v>
-    <v>27.993099999999998</v>
     <v>13.18</v>
+    <v>27.929400000000001</v>
     <v>13.18</v>
+    <v>13.15</v>
     <v>85323580</v>
     <v>EVRI</v>
     <v>EVERI HOLDINGS INC. (XNYS:EVRI)</v>
-    <v>126966</v>
+    <v>521172</v>
     <v>844929</v>
     <v>2004</v>
   </rv>
   <rv s="2">
     <v>37</v>
   </rv>
-  <rv s="3">
-    <v>5</v>
+  <rv s="4">
+    <v>9</v>
     <v>NEXTRACKER INC. (XNAS:NXT)</v>
-    <v>6</v>
+    <v>10</v>
     <v>3</v>
     <v>Finance</v>
-    <v>4</v>
+    <v>5</v>
     <v>en-GB</v>
     <v>c8ssgh</v>
     <v>268435456</v>
@@ -5241,8 +5242,8 @@
     <v>62.31</v>
     <v>32.14</v>
     <v>2.1349999999999998</v>
-    <v>0.36</v>
-    <v>9.7719999999999994E-3</v>
+    <v>-0.38</v>
+    <v>-1.0315000000000001E-2</v>
     <v>USD</v>
     <v>Nextracker Inc. is a provider of integrated solar tracker and software solutions used in utility-scale and ground-mounted distributed generation solar projects. Its products enable solar panels in utility-scale power plants to follow the sun’s movement across the sky and optimize plant performance. Its products include NX Horizon, NX Gemini, TrueCapture, and NX Navigator. Its solutions include Bifacial PV modules, Large Format Modules, and First Solar Series 6 (FSLR6) Modules. NX Horizon is a one-in-portrait (1P) smart solar tracker system that delivers the lowest levelized cost of energy (LCOE). NX Gemini is its two-in-portrait (2P) format tracker which holds two rows of solar panels along the central support beam. TrueCapture is its flagship software offering, which is a self-adjusting tracker control system that uses machine learning to enhance solar power plant energy yield. It has operations in the United States, Brazil, Mexico, Spain, India, Australia, the Middle East and Brazil.</v>
     <v>1050</v>
@@ -5253,19 +5254,19 @@
     <v>38.49</v>
     <v>Renewable Energy</v>
     <v>Stock</v>
-    <v>45554.683675253909</v>
-    <v>36.549999999999997</v>
-    <v>5406923280</v>
+    <v>45554.977939142969</v>
+    <v>36.159999999999997</v>
+    <v>5299366204</v>
     <v>NEXTRACKER INC.</v>
     <v>NEXTRACKER INC.</v>
     <v>38.49</v>
-    <v>9.7772000000000006</v>
+    <v>9.6762999999999995</v>
     <v>36.840000000000003</v>
-    <v>37.200000000000003</v>
+    <v>36.46</v>
     <v>145347400</v>
     <v>NXT</v>
     <v>NEXTRACKER INC. (XNAS:NXT)</v>
-    <v>1185014</v>
+    <v>601</v>
     <v>2855707</v>
     <v>2022</v>
   </rv>
@@ -5282,7 +5283,7 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>4</v>
+    <v>5</v>
     <v>en-GB</v>
     <v>a1xejc</v>
     <v>268435456</v>
@@ -5291,8 +5292,8 @@
     <v>80.22</v>
     <v>56.25</v>
     <v>1.7425999999999999</v>
-    <v>0.45</v>
-    <v>5.8850000000000005E-3</v>
+    <v>0.19</v>
+    <v>2.4849999999999998E-3</v>
     <v>USD</v>
     <v>Monarch Casino &amp; Resort, Inc. owns and operates the Atlantis Casino Resort Spa, a hotel and casino in Reno, Nevada (the Atlantis) and the Monarch Casino Resort Spa Black Hawk (the Monarch Black Hawk), a hotel and casino in Black Hawk, Colorado. In addition, it owns separate parcels of land located next to the Atlantis and a parcel of land with an industrial warehouse located between Denver, Colorado, and Monarch Black Hawk. The Atlantis is located approximately three miles south of downtown, which features approximately 61,000 square feet of casino space; 817 guest rooms and suites; eight food outlets; two gourmet coffee and pastry bars and one snack bar; a 30,000 square-foot health spa and salon with an enclosed year-round pool. Monarch Black Hawk features approximately 60,000 square feet of casino space; approximately 1,000 slot machines; approximately 43 table games; a live poker room; a keno counter and a sports book. The resort also includes 10 bars and lounges.</v>
     <v>2900</v>
@@ -5303,20 +5304,20 @@
     <v>77.89</v>
     <v>Hotels &amp; Entertainment Services</v>
     <v>Stock</v>
-    <v>45554.683548125002</v>
+    <v>45554.85904797422</v>
     <v>41</v>
-    <v>76.25</v>
-    <v>1419152549</v>
+    <v>75.87</v>
+    <v>1414354998</v>
     <v>MONARCH CASINO &amp; RESORT, INC.</v>
     <v>MONARCH CASINO &amp; RESORT, INC.</v>
     <v>77.739999999999995</v>
-    <v>17.867999999999999</v>
+    <v>17.912400000000002</v>
     <v>76.459999999999994</v>
-    <v>76.91</v>
+    <v>76.650000000000006</v>
     <v>18452120</v>
     <v>MCRI</v>
     <v>MONARCH CASINO &amp; RESORT, INC. (XNAS:MCRI)</v>
-    <v>32713</v>
+    <v>139155</v>
     <v>101934</v>
     <v>1993</v>
   </rv>
@@ -5333,7 +5334,7 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>4</v>
+    <v>5</v>
     <v>en-GB</v>
     <v>a1xqm7</v>
     <v>268435456</v>
@@ -5342,8 +5343,8 @@
     <v>69.75</v>
     <v>34.96</v>
     <v>0.97099999999999997</v>
-    <v>1.06</v>
-    <v>1.7666999999999999E-2</v>
+    <v>1.5</v>
+    <v>2.5000000000000001E-2</v>
     <v>USD</v>
     <v>Miller Industries, Inc. is a manufacturer of towing and recovery equipment. The Company designs and manufactures bodies of car carriers and wreckers, which are installed on chassis manufactured by third parties, and sold to its customers. Its products are marketed and sold through a network of distributors that serve all 50 states, Canada, Mexico, and other foreign markets, and through prime contractors to governmental entities. In addition to selling its products, its independent distributors provide end-users with parts and service. Its product line includes car carriers, wreckers, and transport trailers. Car carriers are specialized flat-bed vehicles with hydraulic tilt mechanisms that enable a towing operator to drive or winch a vehicle onto the bed for transport. Its multi-vehicle transport trailers are specialized auto transport trailers with upper and lower decks and hydraulic ramps for loading vehicles. Its brands include Century, Vulcan, Chevron, Holmes, and Challenger.</v>
     <v>1821</v>
@@ -5354,20 +5355,20 @@
     <v>61.999899999999997</v>
     <v>Automobiles &amp; Auto Parts</v>
     <v>Stock</v>
-    <v>45554.683621689066</v>
+    <v>45554.958333344533</v>
     <v>44</v>
     <v>60.08</v>
-    <v>699368417</v>
+    <v>704408085</v>
     <v>MILLER INDUSTRIES, INC.</v>
     <v>MILLER INDUSTRIES, INC.</v>
-    <v>61.3</v>
-    <v>9.6592000000000002</v>
+    <v>61.25</v>
+    <v>9.9006000000000007</v>
     <v>60</v>
-    <v>61.06</v>
+    <v>61.5</v>
     <v>11453790</v>
     <v>MLR</v>
     <v>MILLER INDUSTRIES, INC. (XNYS:MLR)</v>
-    <v>39189</v>
+    <v>102467</v>
     <v>85821</v>
     <v>1994</v>
   </rv>
@@ -5384,7 +5385,7 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>4</v>
+    <v>5</v>
     <v>en-GB</v>
     <v>btavh7</v>
     <v>268435456</v>
@@ -5393,8 +5394,8 @@
     <v>15.86</v>
     <v>9.1649999999999991</v>
     <v>0.89800000000000002</v>
-    <v>0.16</v>
-    <v>1.5984000000000002E-2</v>
+    <v>0.11</v>
+    <v>1.0989000000000001E-2</v>
     <v>USD</v>
     <v>Janus International Group, Inc. is a global manufacturer and supplier of turn-key self-storage, commercial and industrial building solutions. It operates through two geographic segments: Janus North America and Janus International. The Janus North America segment is comprised of all the other entities, including Janus International Group, LLC, Betco, Inc., Noke, Inc., Asta Industries, Inc., DBCI, LLC, Access Control Technologies, LLC, Janus Door, LLC, and Steel Door Depot.com, LLC. The Janus International segment is comprised of Janus International Europe Holdings Ltd. (UK). Its production and sales are in Europe and Australia. It provides facility and door automation and access control technologies, roll up and swing doors, hallway systems and relocatable storage moveable additional storage structures (MASS) units. It is comprised of three sales channels, including New Construction-Self-storage, R3-Self-storage, and Commercial and Other. It also provides terminal maintenance services.</v>
     <v>1956</v>
@@ -5405,20 +5406,20 @@
     <v>10.3</v>
     <v>Homebuilding &amp; Construction Supplies</v>
     <v>Stock</v>
-    <v>45554.683642974218</v>
+    <v>45554.958333356248</v>
     <v>47</v>
-    <v>10.07</v>
+    <v>10.06</v>
     <v>1454676000</v>
     <v>JANUS INTERNATIONAL GROUP, INC.</v>
     <v>JANUS INTERNATIONAL GROUP, INC.</v>
-    <v>10.23</v>
-    <v>11.224399999999999</v>
+    <v>10.24</v>
+    <v>11.3477</v>
     <v>10.01</v>
-    <v>10.17</v>
+    <v>10.119999999999999</v>
     <v>145322200</v>
     <v>JBI</v>
     <v>JANUS INTERNATIONAL GROUP, INC. (XNYS:JBI)</v>
-    <v>457418</v>
+    <v>1702699</v>
     <v>2025718</v>
     <v>2020</v>
   </rv>
@@ -5444,8 +5445,8 @@
     <v>574.76</v>
     <v>318.17</v>
     <v>1.2955000000000001</v>
-    <v>-0.24</v>
-    <v>-5.9590000000000001E-4</v>
+    <v>0.56999999999999995</v>
+    <v>1.4149999999999998E-3</v>
     <v>USD</v>
     <v>Ulta Beauty, Inc. is a beauty retailer. The Company's product categories include cosmetics, skincare, haircare products and styling tools, fragrance and bath, services, and accessories and other. The Company has one segment, which includes retail stores, salon services, and e-commerce. It offers a range of beauty services in its stores, focusing on hair, makeup, brow and skin services. Its skin services include a skin treatment room or dedicated skin treatment area on the sales floor. Its Ulta Beauty store prototype includes an open salon area, with most of its stores offering brow services on the salon floor. It offers a new way to shop for beauty - bringing together All Things Beauty, All in One Place. In addition to ship to home order fulfillment, it offers guests Buy Online, Pick-up in Store, Curbside Pickup, and Store 2 Door, which provides the ability for customers to order in-store and have products delivered to their homes. It operates over 1,350 retail stores across 50 states.</v>
     <v>20000</v>
@@ -5456,20 +5457,20 @@
     <v>409.59</v>
     <v>Specialty Retailers</v>
     <v>Stock</v>
-    <v>45554.683703714843</v>
+    <v>45554.995565786718</v>
     <v>50</v>
     <v>400.3</v>
-    <v>18962736530</v>
+    <v>19000899461</v>
     <v>ULTA BEAUTY, INC.</v>
     <v>ULTA BEAUTY, INC.</v>
     <v>408.75</v>
-    <v>16.134</v>
+    <v>16.193899999999999</v>
     <v>402.72</v>
-    <v>402.48</v>
+    <v>403.29</v>
     <v>47114730</v>
     <v>ULTA</v>
     <v>ULTA BEAUTY, INC. (XNAS:ULTA)</v>
-    <v>405263</v>
+    <v>132</v>
     <v>1668245</v>
     <v>2016</v>
   </rv>
@@ -5486,17 +5487,17 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>4</v>
+    <v>5</v>
     <v>en-GB</v>
     <v>a1vehw</v>
     <v>268435456</v>
     <v>1</v>
     <v>Powered by Refinitiv</v>
-    <v>32.6</v>
+    <v>32.24</v>
     <v>18.899999999999999</v>
     <v>1.9695</v>
-    <v>0.04</v>
-    <v>1.8260000000000001E-3</v>
+    <v>0.02</v>
+    <v>9.1279999999999996E-4</v>
     <v>USD</v>
     <v>International Game Technology PLC is a United Kingdom-based company, which is engaged in gaming. The Company operates and provides an integrated portfolio of gaming technology products and services, including online and instant lottery systems, iLottery, instant ticket printing, lottery management services, commercial services, gaming systems, electronic gaming machines, iGaming, and sports betting. The Company operates through three segments. The Global Lottery segment operates traditional lottery and iLottery businesses across the world, which includes sales, operations, product development, technology, and support, across the world. The Global Gaming segment operates a land-based gaming business across the world, which includes sales, product management, studios, global manufacturing, operation, and technology, across the world. The Digital &amp; Betting segment operates iGaming and sports betting activities across the world.</v>
     <v>11000</v>
@@ -5504,23 +5505,23 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>10 Finsbury Square, Third Floor, LONDON, UNITED KINGDOM-NA, EC2A 1AF GB</v>
-    <v>22.37</v>
+    <v>22.52</v>
     <v>Hotels &amp; Entertainment Services</v>
     <v>Stock</v>
-    <v>45554.68371833281</v>
+    <v>45554.958333356248</v>
     <v>53</v>
-    <v>21.930800000000001</v>
-    <v>4390000000</v>
+    <v>21.89</v>
+    <v>4386000000</v>
     <v>INTERNATIONAL GAME TECHNOLOGY PLC</v>
     <v>INTERNATIONAL GAME TECHNOLOGY PLC</v>
-    <v>22.27</v>
-    <v>21.198</v>
+    <v>22.52</v>
+    <v>21.217300000000002</v>
     <v>21.91</v>
-    <v>21.95</v>
+    <v>21.93</v>
     <v>200000000</v>
     <v>IGT</v>
     <v>INTERNATIONAL GAME TECHNOLOGY PLC (XNYS:IGT)</v>
-    <v>139046</v>
+    <v>578995</v>
     <v>634451</v>
     <v>2014</v>
   </rv>
@@ -5537,7 +5538,7 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>4</v>
+    <v>5</v>
     <v>en-GB</v>
     <v>a1z3ec</v>
     <v>268435456</v>
@@ -5546,8 +5547,8 @@
     <v>87.32</v>
     <v>54.8</v>
     <v>0.58699999999999997</v>
-    <v>0.12</v>
-    <v>1.769E-3</v>
+    <v>0.86</v>
+    <v>1.2675000000000001E-2</v>
     <v>USD</v>
     <v>Oil-Dri Corporation of America is a manufacturer and supplier of specialty sorbent products for pet care, animal health and nutrition, fluid purification, agricultural ingredients, sports field, industrial and automotive markets. Its principal product is cat litter. The Company’s Retail and Wholesale Products Group segment customers include mass merchandisers, the farm and fleet channel, drugstore chains, pet specialty retail outlets, dollar stores, retail grocery stores, distributors of industrial cleanup and automotive products, environmental service companies, sports field product users and marketers of consumer products. Its Business to Business Products Group segment customers include processors and refiners of edible oils, renewable diesel, petroleum-based oils and biodiesel fuel; manufacturers of animal feed and agricultural chemicals; and distributors of animal health and nutrition products. It is also a supplier of silica gel-based crystal cat litter.</v>
     <v>884</v>
@@ -5555,23 +5556,23 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>SUITE 400, 410 NORTH MICHIGAN AVENUE, CHICAGO, IL, 60611 US</v>
-    <v>68.5</v>
+    <v>69.31</v>
     <v>Chemicals</v>
     <v>Stock</v>
-    <v>45554.683460346874</v>
+    <v>45554.958333344533</v>
     <v>56</v>
     <v>67.694999999999993</v>
     <v>494377000</v>
     <v>OIL-DRI CORPORATION OF AMERICA</v>
     <v>OIL-DRI CORPORATION OF AMERICA</v>
-    <v>68.5</v>
-    <v>13.9237</v>
+    <v>69.13</v>
+    <v>14.100099999999999</v>
     <v>67.849999999999994</v>
-    <v>67.97</v>
+    <v>68.709999999999994</v>
     <v>7286320</v>
     <v>ODC</v>
     <v>OIL-DRI CORPORATION OF AMERICA (XNYS:ODC)</v>
-    <v>3758</v>
+    <v>17825</v>
     <v>16047</v>
     <v>1969</v>
   </rv>
@@ -5588,7 +5589,7 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>4</v>
+    <v>5</v>
     <v>en-GB</v>
     <v>a1mt9c</v>
     <v>268435456</v>
@@ -5597,8 +5598,8 @@
     <v>170.9692</v>
     <v>93.77</v>
     <v>1.5933999999999999</v>
-    <v>4.16</v>
-    <v>4.2518E-2</v>
+    <v>4.3899999999999997</v>
+    <v>4.4869000000000006E-2</v>
     <v>USD</v>
     <v>Axcelis Technologies, Inc. designs, manufactures and services ion implantation and other processing equipment used in the fabrication of semiconductor chips. The Company offers a complete line of high energy, high current and medium current implanters for all application requirements. In addition to equipment, the Company provides extensive aftermarket lifecycle products and services, including used tools, spare parts, equipment upgrades, maintenance services and customer training. Its Purion flagship systems are all based on a common platform, which enables a combination of implant purity, precision and productivity. Combining a single wafer end station, with advanced spot beam architectures (that ensures all points across the wafer see the same beam condition at the same beam angle), Purion products enable process control to optimize device performance and yield, at high productivity. The Company sells its products to semiconductor chip manufacturers around the world.</v>
     <v>1620</v>
@@ -5606,23 +5607,23 @@
     <v>XNAS</v>
     <v>XNAS</v>
     <v>108 Cherry Hill Dr, BEVERLY, MA, 01915 US</v>
-    <v>102.27</v>
+    <v>102.99</v>
     <v>Semiconductors &amp; Semiconductor Equipment</v>
     <v>Stock</v>
-    <v>45554.68356297422</v>
+    <v>45554.99339609922</v>
     <v>59</v>
     <v>100.07</v>
-    <v>3326994180</v>
+    <v>3334496225</v>
     <v>AXCELIS TECHNOLOGIES, INC.</v>
     <v>AXCELIS TECHNOLOGIES, INC.</v>
     <v>102.27</v>
-    <v>13.4796</v>
+    <v>14.0844</v>
     <v>97.84</v>
-    <v>102</v>
+    <v>102.23</v>
     <v>32617590</v>
     <v>ACLS</v>
     <v>AXCELIS TECHNOLOGIES, INC. (XNAS:ACLS)</v>
-    <v>202914</v>
+    <v>15</v>
     <v>521482</v>
     <v>1995</v>
   </rv>
@@ -5639,7 +5640,7 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>4</v>
+    <v>5</v>
     <v>en-GB</v>
     <v>a1retc</v>
     <v>268435456</v>
@@ -5648,8 +5649,8 @@
     <v>179.7</v>
     <v>63.9</v>
     <v>0.89570000000000005</v>
-    <v>2.0750000000000002</v>
-    <v>1.7888999999999999E-2</v>
+    <v>1.78</v>
+    <v>1.5346E-2</v>
     <v>USD</v>
     <v>Dell Technologies Inc. is engaged in designing, developing, manufacturing, marketing, selling, and supporting a wide range of comprehensive and integrated solutions, products, and services. The Company operates through two segments: Infrastructure Solutions Group (ISG) and Client Solutions Group (CSG). Its ISG segment enables the Company’s customer’s digital transformation with solutions that address artificial intelligence (AI), machine learning, data analytics, and multi cloud environments. Its comprehensive storage portfolio includes modern and traditional storage solutions, including all-flash arrays, scale-out file, object platforms, hyper-converged infrastructure, and software-defined storage. Its CSG segment offers branded personal computers (PCs) including notebooks, desktops, and workstations and branded peripherals that include displays, docking stations, keyboards, mice, and webcam and audio devices, as well as third-party software and peripherals.</v>
     <v>120000</v>
@@ -5660,20 +5661,20 @@
     <v>120.07</v>
     <v>Computers, Phones &amp; Household Electronics</v>
     <v>Stock</v>
-    <v>45554.683723935159</v>
+    <v>45554.99945133047</v>
     <v>62</v>
-    <v>117.49</v>
-    <v>82927061412</v>
+    <v>117.36</v>
+    <v>82719857896</v>
     <v>DELL TECHNOLOGIES INC.</v>
     <v>DELL TECHNOLOGIES INC.</v>
     <v>120.07</v>
-    <v>21.342400000000001</v>
+    <v>21.669899999999998</v>
     <v>115.99</v>
-    <v>118.065</v>
+    <v>117.77</v>
     <v>702384800</v>
     <v>DELL</v>
     <v>DELL TECHNOLOGIES INC. (XNYS:DELL)</v>
-    <v>5658715</v>
+    <v>8004</v>
     <v>11347373</v>
     <v>2013</v>
   </rv>
@@ -5684,7 +5685,7 @@
 </file>
 
 <file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
-<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="4">
+<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="5">
   <s t="_hyperlink">
     <k n="Address" t="s"/>
     <k n="Text" t="s"/>
@@ -5764,6 +5765,51 @@
     <k n="Industry" t="s"/>
     <k n="Instrument type" t="s"/>
     <k n="Last trade time"/>
+    <k n="LearnMoreOnLink" t="r"/>
+    <k n="Low"/>
+    <k n="Market cap"/>
+    <k n="Name" t="s"/>
+    <k n="Official name" t="s"/>
+    <k n="Open"/>
+    <k n="P/E"/>
+    <k n="Previous close"/>
+    <k n="Price"/>
+    <k n="Price (Extended hours)"/>
+    <k n="Shares outstanding"/>
+    <k n="Ticker symbol" t="s"/>
+    <k n="UniqueName" t="s"/>
+    <k n="Volume"/>
+    <k n="Volume average"/>
+    <k n="Year incorporated"/>
+  </s>
+  <s t="_linkedentitycore">
+    <k n="_Display" t="spb"/>
+    <k n="_DisplayString" t="s"/>
+    <k n="_Flags" t="spb"/>
+    <k n="_Format" t="spb"/>
+    <k n="_Icon" t="s"/>
+    <k n="_SubLabel" t="spb"/>
+    <k n="%EntityCulture" t="s"/>
+    <k n="%EntityId" t="s"/>
+    <k n="%EntityServiceId"/>
+    <k n="%IsRefreshable" t="b"/>
+    <k n="%ProviderInfo" t="s"/>
+    <k n="52 week high"/>
+    <k n="52 week low"/>
+    <k n="Beta"/>
+    <k n="Change"/>
+    <k n="Change (%)"/>
+    <k n="Currency" t="s"/>
+    <k n="Description" t="s"/>
+    <k n="Employees"/>
+    <k n="Exchange" t="s"/>
+    <k n="Exchange abbreviation" t="s"/>
+    <k n="ExchangeID" t="s"/>
+    <k n="Headquarters" t="s"/>
+    <k n="High"/>
+    <k n="Industry" t="s"/>
+    <k n="Instrument type" t="s"/>
+    <k n="Last trade time"/>
     <k n="Low"/>
     <k n="Market cap"/>
     <k n="Name" t="s"/>
@@ -5784,7 +5830,7 @@
 
 <file path=xl/richData/rdsupportingpropertybag.xml><?xml version="1.0" encoding="utf-8"?>
 <supportingPropertyBags xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2">
-  <spbArrays count="2">
+  <spbArrays count="3">
     <a count="42">
       <v t="s">%EntityServiceId</v>
       <v t="s">_Format</v>
@@ -5796,6 +5842,51 @@
       <v t="s">Name</v>
       <v t="s">_SubLabel</v>
       <v t="s">Price</v>
+      <v t="s">Exchange</v>
+      <v t="s">Official name</v>
+      <v t="s">Last trade time</v>
+      <v t="s">Ticker symbol</v>
+      <v t="s">Exchange abbreviation</v>
+      <v t="s">Change</v>
+      <v t="s">Change (%)</v>
+      <v t="s">Currency</v>
+      <v t="s">Previous close</v>
+      <v t="s">Open</v>
+      <v t="s">High</v>
+      <v t="s">Low</v>
+      <v t="s">52 week high</v>
+      <v t="s">52 week low</v>
+      <v t="s">Volume</v>
+      <v t="s">Volume average</v>
+      <v t="s">Market cap</v>
+      <v t="s">Beta</v>
+      <v t="s">P/E</v>
+      <v t="s">Shares outstanding</v>
+      <v t="s">Description</v>
+      <v t="s">Employees</v>
+      <v t="s">Headquarters</v>
+      <v t="s">Industry</v>
+      <v t="s">Instrument type</v>
+      <v t="s">Year incorporated</v>
+      <v t="s">_Flags</v>
+      <v t="s">UniqueName</v>
+      <v t="s">_DisplayString</v>
+      <v t="s">LearnMoreOnLink</v>
+      <v t="s">ExchangeID</v>
+      <v t="s">%ProviderInfo</v>
+    </a>
+    <a count="43">
+      <v t="s">%EntityServiceId</v>
+      <v t="s">_Format</v>
+      <v t="s">%IsRefreshable</v>
+      <v t="s">%EntityCulture</v>
+      <v t="s">%EntityId</v>
+      <v t="s">_Icon</v>
+      <v t="s">_Display</v>
+      <v t="s">Name</v>
+      <v t="s">_SubLabel</v>
+      <v t="s">Price</v>
+      <v t="s">Price (Extended hours)</v>
       <v t="s">Exchange</v>
       <v t="s">Official name</v>
       <v t="s">Last trade time</v>
@@ -5873,7 +5964,7 @@
       <v t="s">%ProviderInfo</v>
     </a>
   </spbArrays>
-  <spbData count="7">
+  <spbData count="11">
     <spb s="0">
       <v>0</v>
       <v>Name</v>
@@ -5919,11 +6010,54 @@
       <v>Source: Nasdaq Last Sale</v>
       <v>GMT</v>
     </spb>
+    <spb s="4">
+      <v>Delayed 15 minutes</v>
+      <v>from previous close</v>
+      <v>from previous close</v>
+      <v>Source: Nasdaq</v>
+      <v>GMT</v>
+    </spb>
+    <spb s="0">
+      <v>1</v>
+      <v>Name</v>
+      <v>LearnMoreOnLink</v>
+    </spb>
     <spb s="5">
       <v>1</v>
+      <v>2</v>
+      <v>2</v>
+      <v>1</v>
+      <v>3</v>
+      <v>1</v>
+      <v>1</v>
+      <v>1</v>
+      <v>4</v>
+      <v>4</v>
+      <v>5</v>
+      <v>6</v>
+      <v>1</v>
+      <v>1</v>
+      <v>1</v>
+      <v>4</v>
+      <v>7</v>
+      <v>8</v>
+      <v>9</v>
+      <v>4</v>
+      <v>1</v>
+    </spb>
+    <spb s="6">
+      <v>at close</v>
+      <v>from previous close</v>
+      <v>from previous close</v>
+      <v>Source: Nasdaq</v>
+      <v>GMT</v>
+      <v>Delayed 15 minutes</v>
+    </spb>
+    <spb s="7">
+      <v>2</v>
       <v>Name</v>
     </spb>
-    <spb s="6">
+    <spb s="8">
       <v>1</v>
       <v>1</v>
       <v>1</v>
@@ -5933,7 +6067,7 @@
 </file>
 
 <file path=xl/richData/rdsupportingpropertybagstructure.xml><?xml version="1.0" encoding="utf-8"?>
-<spbStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" count="7">
+<spbStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" count="9">
   <s>
     <k n="^Order" t="spba"/>
     <k n="TitleProperty" t="s"/>
@@ -5978,6 +6112,37 @@
     <k n="Change (%)" t="s"/>
     <k n="ExchangeID" t="s"/>
     <k n="Last trade time" t="s"/>
+  </s>
+  <s>
+    <k n="Low" t="i"/>
+    <k n="P/E" t="i"/>
+    <k n="Beta" t="i"/>
+    <k n="High" t="i"/>
+    <k n="Name" t="i"/>
+    <k n="Open" t="i"/>
+    <k n="Price" t="i"/>
+    <k n="Change" t="i"/>
+    <k n="Volume" t="i"/>
+    <k n="Employees" t="i"/>
+    <k n="Change (%)" t="i"/>
+    <k n="Market cap" t="i"/>
+    <k n="52 week low" t="i"/>
+    <k n="52 week high" t="i"/>
+    <k n="Previous close" t="i"/>
+    <k n="Volume average" t="i"/>
+    <k n="Last trade time" t="i"/>
+    <k n="Year incorporated" t="i"/>
+    <k n="`%EntityServiceId" t="i"/>
+    <k n="Shares outstanding" t="i"/>
+    <k n="Price (Extended hours)" t="i"/>
+  </s>
+  <s>
+    <k n="Price" t="s"/>
+    <k n="Change" t="s"/>
+    <k n="Change (%)" t="s"/>
+    <k n="ExchangeID" t="s"/>
+    <k n="Last trade time" t="s"/>
+    <k n="Price (Extended hours)" t="s"/>
   </s>
   <s>
     <k n="^Order" t="spba"/>
@@ -69397,7 +69562,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F51CD2FE-0785-5E4C-91F5-512BDFA3DC54}">
   <dimension ref="B1:L26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C4" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView topLeftCell="C4" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
@@ -69481,15 +69646,15 @@
       </c>
       <c r="I3" s="151" cm="1">
         <f t="array" aca="1" ref="I3" ca="1">_FV(B3,"Price")</f>
-        <v>58.312100000000001</v>
+        <v>58.4</v>
       </c>
       <c r="J3" s="131">
         <f t="shared" ref="J3:J24" ca="1" si="0">((I3-F3)/F3)</f>
-        <v>-0.15182399999999999</v>
+        <v>-0.15054545454545457</v>
       </c>
       <c r="K3" s="172">
         <f t="shared" ref="K3:K24" ca="1" si="1">(I3*G3) - H3</f>
-        <v>-76.091389719999995</v>
+        <v>-75.450879999999984</v>
       </c>
       <c r="L3"/>
     </row>
@@ -69520,15 +69685,15 @@
       </c>
       <c r="I4" s="151" cm="1">
         <f t="array" aca="1" ref="I4" ca="1">_FV(B4,"Price")</f>
-        <v>140.75</v>
+        <v>137.91999999999999</v>
       </c>
       <c r="J4" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>0.40721855628874232</v>
+        <v>0.37892421515696856</v>
       </c>
       <c r="K4" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>204.01675</v>
+        <v>189.84127999999998</v>
       </c>
       <c r="L4"/>
     </row>
@@ -69559,15 +69724,15 @@
       </c>
       <c r="I5" s="151" cm="1">
         <f t="array" aca="1" ref="I5" ca="1">_FV(B5,"Price")</f>
-        <v>19.940000000000001</v>
+        <v>19.97</v>
       </c>
       <c r="J5" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>-8.532110091743117E-2</v>
+        <v>-8.3944954128440455E-2</v>
       </c>
       <c r="K5" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>-42.794752000000017</v>
+        <v>-42.105376000000035</v>
       </c>
       <c r="L5"/>
     </row>
@@ -69598,15 +69763,15 @@
       </c>
       <c r="I6" s="151" cm="1">
         <f t="array" aca="1" ref="I6" ca="1">_FV(B6,"Price")</f>
-        <v>22.085000000000001</v>
+        <v>22.35</v>
       </c>
       <c r="J6" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>0.26200000000000007</v>
+        <v>0.27714285714285725</v>
       </c>
       <c r="K6" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>145.12759400000004</v>
+        <v>152.88054</v>
       </c>
       <c r="L6"/>
     </row>
@@ -69637,15 +69802,15 @@
       </c>
       <c r="I7" s="153" cm="1">
         <f t="array" aca="1" ref="I7" ca="1">_FV(B7,"Price")</f>
-        <v>228.9915</v>
+        <v>228.87</v>
       </c>
       <c r="J7" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>0.29769636178170683</v>
+        <v>0.29700782046922813</v>
       </c>
       <c r="K7" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>149.14976765000006</v>
+        <v>148.80481700000007</v>
       </c>
       <c r="L7"/>
     </row>
@@ -69676,15 +69841,15 @@
       </c>
       <c r="I8" s="153" cm="1">
         <f t="array" aca="1" ref="I8" ca="1">_FV(B8,"Price")</f>
-        <v>90.77</v>
+        <v>90.99</v>
       </c>
       <c r="J8" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>0.61685073031706439</v>
+        <v>0.62076950480940496</v>
       </c>
       <c r="K8" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>308.97701800000004</v>
+        <v>310.94016600000009</v>
       </c>
       <c r="L8"/>
     </row>
@@ -69715,15 +69880,15 @@
       </c>
       <c r="I9" s="153" cm="1">
         <f t="array" aca="1" ref="I9" ca="1">_FV(B9,"Price")</f>
-        <v>19.721</v>
+        <v>19.690000000000001</v>
       </c>
       <c r="J9" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.41271590232281119</v>
+        <v>-0.4136390708755211</v>
       </c>
       <c r="K9" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>-206.74493110000003</v>
+        <v>-207.20747899999998</v>
       </c>
       <c r="L9"/>
     </row>
@@ -69754,15 +69919,15 @@
       </c>
       <c r="I10" s="155" cm="1">
         <f t="array" aca="1" ref="I10" ca="1">_FV(B10,"Price")</f>
-        <v>61.66</v>
+        <v>62.43</v>
       </c>
       <c r="J10" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>5.9450171821305735E-2</v>
+        <v>7.2680412371133957E-2</v>
       </c>
       <c r="K10" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>29.806275999999912</v>
+        <v>36.434897999999976</v>
       </c>
       <c r="L10"/>
     </row>
@@ -69793,15 +69958,15 @@
       </c>
       <c r="I11" s="155" cm="1">
         <f t="array" aca="1" ref="I11" ca="1">_FV(B11,"Price")</f>
-        <v>85.39</v>
+        <v>85.86</v>
       </c>
       <c r="J11" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>-6.4424235783937717E-2</v>
+        <v>-5.9274679522296446E-2</v>
       </c>
       <c r="K11" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>-32.29428999999999</v>
+        <v>-29.714460000000031</v>
       </c>
       <c r="L11"/>
     </row>
@@ -69832,15 +69997,15 @@
       </c>
       <c r="I12" s="155" cm="1">
         <f t="array" aca="1" ref="I12" ca="1">_FV(B12,"Price")</f>
-        <v>96.15</v>
+        <v>97.7</v>
       </c>
       <c r="J12" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>0.14874551971326166</v>
+        <v>0.16726403823178015</v>
       </c>
       <c r="K12" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>74.505825000000073</v>
+        <v>83.783350000000041</v>
       </c>
       <c r="L12"/>
     </row>
@@ -69871,15 +70036,15 @@
       </c>
       <c r="I13" s="155" cm="1">
         <f t="array" aca="1" ref="I13" ca="1">_FV(B13,"Price")</f>
-        <v>95.885000000000005</v>
+        <v>95.83</v>
       </c>
       <c r="J13" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.18025989569975201</v>
+        <v>-0.18073010173548773</v>
       </c>
       <c r="K13" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>-90.314956499999994</v>
+        <v>-90.550526999999988</v>
       </c>
       <c r="L13"/>
     </row>
@@ -69910,15 +70075,15 @@
       </c>
       <c r="I14" s="157" cm="1">
         <f t="array" aca="1" ref="I14" ca="1">_FV(B14,"Price")</f>
-        <v>27.45</v>
+        <v>27.31</v>
       </c>
       <c r="J14" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>7.6892899176147542E-2</v>
+        <v>7.1400549234994129E-2</v>
       </c>
       <c r="K14" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>38.557199999999966</v>
+        <v>35.805359999999951</v>
       </c>
       <c r="L14"/>
     </row>
@@ -69949,15 +70114,15 @@
       </c>
       <c r="I15" s="157" cm="1">
         <f t="array" aca="1" ref="I15" ca="1">_FV(B15,"Price")</f>
-        <v>13.18</v>
+        <v>13.15</v>
       </c>
       <c r="J15" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>0.50285062713797035</v>
+        <v>0.49942987457240606</v>
       </c>
       <c r="K15" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>251.71111800000006</v>
+        <v>249.99781500000006</v>
       </c>
       <c r="L15"/>
     </row>
@@ -69988,15 +70153,15 @@
       </c>
       <c r="I16" s="159" cm="1">
         <f t="array" aca="1" ref="I16" ca="1">_FV(B16,"Price")</f>
-        <v>37.200000000000003</v>
+        <v>36.46</v>
       </c>
       <c r="J16" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.23330585325638911</v>
+        <v>-0.24855729596042872</v>
       </c>
       <c r="K16" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>-113.14999999999998</v>
+        <v>-120.54999999999995</v>
       </c>
       <c r="L16"/>
     </row>
@@ -70027,15 +70192,15 @@
       </c>
       <c r="I17" s="159" cm="1">
         <f t="array" aca="1" ref="I17" ca="1">_FV(B17,"Price")</f>
-        <v>76.91</v>
+        <v>76.650000000000006</v>
       </c>
       <c r="J17" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>9.9499642601858382E-2</v>
+        <v>9.5782701929950004E-2</v>
       </c>
       <c r="K17" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>48.730000000000018</v>
+        <v>46.910000000000082</v>
       </c>
       <c r="L17"/>
     </row>
@@ -70066,15 +70231,15 @@
       </c>
       <c r="I18" s="159" cm="1">
         <f t="array" aca="1" ref="I18" ca="1">_FV(B18,"Price")</f>
-        <v>61.06</v>
+        <v>61.5</v>
       </c>
       <c r="J18" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.8012222579607551E-2</v>
+        <v>-1.0935992280476033E-2</v>
       </c>
       <c r="K18" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>-8.9599999999999795</v>
+        <v>-5.4399999999999977</v>
       </c>
       <c r="L18"/>
     </row>
@@ -70105,15 +70270,15 @@
       </c>
       <c r="I19" s="159" cm="1">
         <f t="array" aca="1" ref="I19" ca="1">_FV(B19,"Price")</f>
-        <v>10.17</v>
+        <v>10.119999999999999</v>
       </c>
       <c r="J19" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.241044776119403</v>
+        <v>-0.24477611940298516</v>
       </c>
       <c r="K19" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>-120.81488999999999</v>
+        <v>-122.68403999999998</v>
       </c>
       <c r="L19"/>
     </row>
@@ -70144,15 +70309,15 @@
       </c>
       <c r="I20" s="213" cm="1">
         <f t="array" aca="1" ref="I20" ca="1">_FV(B20,"Price")</f>
-        <v>402.48</v>
+        <v>403.29</v>
       </c>
       <c r="J20" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>2.3080833756990445E-2</v>
+        <v>2.513980681240479E-2</v>
       </c>
       <c r="K20" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>11.614399999999989</v>
+        <v>12.651200000000074</v>
       </c>
       <c r="L20"/>
     </row>
@@ -70183,15 +70348,15 @@
       </c>
       <c r="I21" s="216" cm="1">
         <f t="array" aca="1" ref="I21" ca="1">_FV(B21,"Price")</f>
-        <v>21.95</v>
+        <v>21.93</v>
       </c>
       <c r="J21" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.3926325247080065E-2</v>
+        <v>-1.482479784366585E-2</v>
       </c>
       <c r="K21" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>-6.9823250000000598</v>
+        <v>-7.4324550000000045</v>
       </c>
     </row>
     <row r="22" spans="2:12">
@@ -70221,15 +70386,15 @@
       </c>
       <c r="I22" s="216" cm="1">
         <f t="array" aca="1" ref="I22" ca="1">_FV(B22,"Price")</f>
-        <v>67.97</v>
+        <v>68.709999999999994</v>
       </c>
       <c r="J22" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.3980470993681818E-2</v>
+        <v>-1.3354394026421695E-2</v>
       </c>
       <c r="K22" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>-10.606841000000031</v>
+        <v>-5.2679630000000657</v>
       </c>
     </row>
     <row r="23" spans="2:12">
@@ -70259,15 +70424,15 @@
       </c>
       <c r="I23" s="216" cm="1">
         <f t="array" aca="1" ref="I23" ca="1">_FV(B23,"Price")</f>
-        <v>102</v>
+        <v>102.23</v>
       </c>
       <c r="J23" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>8.6027884900623415E-3</v>
+        <v>1.0877088895481149E-2</v>
       </c>
       <c r="K23" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>4.328200000000038</v>
+        <v>5.4676430000000664</v>
       </c>
     </row>
     <row r="24" spans="2:12">
@@ -70297,21 +70462,21 @@
       </c>
       <c r="I24" s="216" cm="1">
         <f t="array" aca="1" ref="I24" ca="1">_FV(B24,"Price")</f>
-        <v>118.065</v>
+        <v>117.77</v>
       </c>
       <c r="J24" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>-9.7309189372151881E-4</v>
+        <v>-3.4692841428330579E-3</v>
       </c>
       <c r="K24" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.4752390000000446</v>
+        <v>-1.7258620000000633</v>
       </c>
     </row>
     <row r="26" spans="2:12" ht="13">
       <c r="K26" s="171">
         <f ca="1">SUM(K3:K24)</f>
-        <v>557.29453433000003</v>
+        <v>565.38802700000042</v>
       </c>
     </row>
   </sheetData>
@@ -70693,7 +70858,7 @@
   </sheetPr>
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>

</xml_diff>

<commit_message>
vault backup: 2024-09-22 16:51:26
</commit_message>
<xml_diff>
--- a/_system/Attachments/Portfolio Management.xlsx
+++ b/_system/Attachments/Portfolio Management.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martin/repos/tomesink/obsidian/_system/Attachments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C66517AD-F217-FF4B-9C0E-B364BEEE3B57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{549939C1-0008-4E43-95DA-4B14F967A023}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3300" yWindow="980" windowWidth="33800" windowHeight="18860" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4581,9 +4581,11 @@
     <v>Powered by Refinitiv</v>
     <v>83.25</v>
     <v>52.770499999999998</v>
-    <v>0.52459999999999996</v>
-    <v>-0.02</v>
-    <v>-3.4229999999999997E-4</v>
+    <v>0.52759999999999996</v>
+    <v>-0.89</v>
+    <v>-1.524E-2</v>
+    <v>0.01</v>
+    <v>1.739E-4</v>
     <v>USD</v>
     <v>CVS Health Corporation is a health solutions company. The Company operates in four segments: Health Care Benefits, Health Services, Pharmacy &amp; Consumer Wellness, and Corporate/Other. Its Health Care Benefits segment offer a range of traditional, voluntary and consumer-directed health insurance products and related services, including medical, pharmacy, dental and behavioral health plans, medical management capabilities, Medicare Advantage and Medicare supplement plans, and Medicaid health care management services. Its Health Services segment provides a full range of pharmacy benefit management solutions, delivers health care services in its medical clinics, virtually, and in the home, and offers provider enablement solutions. The Pharmacy &amp; Consumer Wellness segment dispenses prescriptions in its retail pharmacies and through its infusion operations, provides ancillary pharmacy services, including pharmacy patient care programs, diagnostic testing and vaccination administration.</v>
     <v>300000</v>
@@ -4591,24 +4593,25 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>1 Cvs Dr, WOONSOCKET, RI, 02895-6146 US</v>
-    <v>59.1</v>
+    <v>58.08</v>
     <v>Healthcare Providers &amp; Services</v>
     <v>Stock</v>
-    <v>45554.99989664297</v>
+    <v>45555.999544455466</v>
     <v>0</v>
-    <v>58.12</v>
-    <v>73465973600</v>
+    <v>57.13</v>
+    <v>72346390000</v>
     <v>CVS HEALTH CORPORATION</v>
     <v>CVS HEALTH CORPORATION</v>
-    <v>58.7</v>
-    <v>10.3926</v>
-    <v>58.42</v>
+    <v>58</v>
+    <v>10.2342</v>
     <v>58.4</v>
+    <v>57.51</v>
+    <v>57.52</v>
     <v>1257979000</v>
     <v>CVS</v>
     <v>CVS HEALTH CORPORATION (XNYS:CVS)</v>
-    <v>788</v>
-    <v>7591748</v>
+    <v>10239966</v>
+    <v>7552236</v>
     <v>1996</v>
   </rv>
   <rv s="2">
@@ -4624,7 +4627,7 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>5</v>
+    <v>4</v>
     <v>en-GB</v>
     <v>a1qclh</v>
     <v>268435456</v>
@@ -4632,9 +4635,11 @@
     <v>Powered by Refinitiv</v>
     <v>165.32</v>
     <v>74</v>
-    <v>2.0011000000000001</v>
-    <v>-1.89</v>
-    <v>-1.3517999999999999E-2</v>
+    <v>1.9970000000000001</v>
+    <v>1.1299999999999999</v>
+    <v>8.1930000000000006E-3</v>
+    <v>-0.52</v>
+    <v>-3.7399999999999998E-3</v>
     <v>USD</v>
     <v>Crocs, Inc. is engaged in the design, development, worldwide marketing, distribution, and sale of casual lifestyle footwear and accessories for women, men, and children. The Company’s segments include Crocs Brand and the HEYDUDE Brand. The Company’s Crocs Brand collection contains Croslite material, a molded footwear technology, delivering extraordinary comfort with each step. Its Croslite materials are formulated to create soft, comfortable, lightweight, non-marking, and odor-resistant footwear. The HEYDUDE Brand offers shoes with a versatile silhouette. It sells its products in more than 80 countries, through two distribution channels: wholesale and direct-to-consumer. Its wholesale channel includes domestic and international multi-brand retailers, mono-branded partner stores, e-tailers, and distributors; its direct-to-consumer channel includes Company-operated retail stores, Company-operated e-commerce sites, and third-party marketplaces.</v>
     <v>7030</v>
@@ -4642,24 +4647,25 @@
     <v>XNAS</v>
     <v>XNAS</v>
     <v>500 Eldorado Boulevard, Building 5, BROOMFIELD, CO, 80021 US</v>
-    <v>144.32</v>
+    <v>140.34</v>
     <v>Textiles &amp; Apparel</v>
     <v>Stock</v>
-    <v>45554.991820578121</v>
+    <v>45555.99378098359</v>
     <v>3</v>
-    <v>134.44499999999999</v>
-    <v>8190397129</v>
+    <v>137.63499999999999</v>
+    <v>8257503000</v>
     <v>CROCS, INC.</v>
     <v>CROCS, INC.</v>
-    <v>142.94999999999999</v>
-    <v>10.3727</v>
-    <v>139.81</v>
+    <v>138.16</v>
+    <v>10.457599999999999</v>
     <v>137.91999999999999</v>
+    <v>139.05000000000001</v>
+    <v>138.53</v>
     <v>59385130</v>
     <v>CROX</v>
     <v>CROCS, INC. (XNAS:CROX)</v>
-    <v>354</v>
-    <v>937487</v>
+    <v>1491867</v>
+    <v>946750</v>
     <v>2005</v>
   </rv>
   <rv s="2">
@@ -4675,7 +4681,7 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>5</v>
+    <v>4</v>
     <v>en-GB</v>
     <v>a25yfr</v>
     <v>268435456</v>
@@ -4683,9 +4689,11 @@
     <v>Powered by Refinitiv</v>
     <v>30.07</v>
     <v>17.71</v>
-    <v>1.5144</v>
-    <v>0.23</v>
-    <v>1.1651E-2</v>
+    <v>1.5177</v>
+    <v>-0.59</v>
+    <v>-2.9544000000000001E-2</v>
+    <v>-5.0000000000000001E-4</v>
+    <v>-2.5799999999999997E-5</v>
     <v>USD</v>
     <v>Wabash National Corporation provides connected solutions for the transportation, logistics and distribution industries. The Company designs and manufactures products including dry freight and refrigerated trailers, platform trailers, tank trailers, dry and refrigerated truck bodies, structural composite panels and products, transportation, logistics, and distribution industry parts and services, and specialty food grade processing equipment. The Company’s Transportation Solutions (TS) segment comprises the design and manufacturing operations for the Company’s transportation-related equipment and products. This includes dry and refrigerated van trailers, platform trailers, tank trailers and truck-mounted tanks, truck-mounted dry and refrigerated truck bodies and EcoNex technology products. Its Parts &amp; Services (P&amp;S) segment is comprised of the Company’s parts and services businesses as well as the upfitting component of truck bodies business. It also includes DuraPlate composite panels.</v>
     <v>6700</v>
@@ -4693,24 +4701,25 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>3900 Mccarty Lane, LAFAYETTE, IN, 47905 US</v>
-    <v>20.2</v>
+    <v>19.760000000000002</v>
     <v>Machinery, Equipment &amp; Components</v>
     <v>Stock</v>
-    <v>45554.958333333336</v>
+    <v>45555.958333333336</v>
     <v>6</v>
-    <v>19.79</v>
-    <v>878664623</v>
+    <v>19.190000000000001</v>
+    <v>852705100</v>
     <v>WABASH NATIONAL CORPORATION</v>
     <v>WABASH NATIONAL CORPORATION</v>
-    <v>20.2</v>
-    <v>6.1258999999999997</v>
-    <v>19.739999999999998</v>
+    <v>19.73</v>
+    <v>5.9450000000000003</v>
     <v>19.97</v>
+    <v>19.38</v>
+    <v>19.3795</v>
     <v>43999230</v>
     <v>WNC</v>
     <v>WABASH NATIONAL CORPORATION (XNYS:WNC)</v>
-    <v>410448</v>
-    <v>435088</v>
+    <v>3587244</v>
+    <v>423715</v>
     <v>1991</v>
   </rv>
   <rv s="2">
@@ -4726,7 +4735,7 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>5</v>
+    <v>4</v>
     <v>en-GB</v>
     <v>a1pfoc</v>
     <v>268435456</v>
@@ -4734,9 +4743,11 @@
     <v>Powered by Refinitiv</v>
     <v>26.4</v>
     <v>16.12</v>
-    <v>1.0366</v>
-    <v>0.44</v>
-    <v>2.0081999999999999E-2</v>
+    <v>1.0349999999999999</v>
+    <v>-0.12</v>
+    <v>-5.3690000000000005E-3</v>
+    <v>0</v>
+    <v>0</v>
     <v>USD</v>
     <v>Perdoceo Education Corporation, through its academic institutions, offers quality postsecondary education primarily online to a diverse student population, along with campus-based and blended learning programs. The Company's academic institutions include Colorado Technical University (CTU) and the American InterContinental University System (AIUS), which provides degree programs from the associate through doctoral level as well as non-degree seeking and professional development programs. Its academic institutions offer students industry-relevant and career-focused academic programs. CTU offers academic programs in the career-oriented disciplines of business and management, nursing, healthcare management, computer science, engineering, information systems and technology, project management, cybersecurity and criminal justice. AIUS offers academic programs in the career-oriented disciplines of business studies, information technologies, education, health sciences and criminal justice.</v>
     <v>2319</v>
@@ -4744,24 +4755,25 @@
     <v>XNAS</v>
     <v>XNAS</v>
     <v>1750 E. GOLF ROAD, SCHAUMBURG, IL, 60173 US</v>
-    <v>22.36</v>
+    <v>22.64</v>
     <v>Miscellaneous Educational Service Providers</v>
     <v>Stock</v>
-    <v>45554.904691469528</v>
+    <v>45555.90269422422</v>
     <v>9</v>
-    <v>21.840599999999998</v>
-    <v>1467801160</v>
+    <v>22.01</v>
+    <v>1459920000</v>
     <v>PERDOCEO EDUCATION CORPORATION</v>
     <v>PERDOCEO EDUCATION CORPORATION</v>
-    <v>22.25</v>
-    <v>10.984</v>
-    <v>21.91</v>
+    <v>22.2</v>
+    <v>10.924899999999999</v>
     <v>22.35</v>
+    <v>22.23</v>
+    <v>22.23</v>
     <v>65673430</v>
     <v>PRDO</v>
     <v>PERDOCEO EDUCATION CORPORATION (XNAS:PRDO)</v>
-    <v>284119</v>
-    <v>383603</v>
+    <v>2494424</v>
+    <v>386595</v>
     <v>1994</v>
   </rv>
   <rv s="2">
@@ -4785,9 +4797,11 @@
     <v>Powered by Refinitiv</v>
     <v>237.23</v>
     <v>164.07499999999999</v>
-    <v>1.2446999999999999</v>
-    <v>8.18</v>
-    <v>3.7066000000000002E-2</v>
+    <v>1.2405999999999999</v>
+    <v>-0.67</v>
+    <v>-2.9270000000000003E-3</v>
+    <v>-0.43359999999999999</v>
+    <v>-1.9E-3</v>
     <v>USD</v>
     <v>Apple Inc. designs, manufactures and markets smartphones, personal computers, tablets, wearables and accessories, and sells a variety of related services. Its product categories include iPhone, Mac, iPad, and Wearables, Home and Accessories. Its software platforms include iOS, iPadOS, macOS, watchOS, and tvOS. Its services include advertising, AppleCare, cloud services, digital content and payment services. It operates various platforms, including the App Store, that allow customers to discover and download applications and digital content, such as books, music, video, games and podcasts. It also offers digital content through subscription-based services, including Apple Arcade, Apple Fitness+, Apple Music, Apple News+ and Apple TV+. Its products include iPhone 15 Pro, iPhone 15, iPhone 14, iPhone 13, MacBook Air, MacBook Pro, iMac, Mac mini, Mac Studio, Mac Pro, and others. It also provides DarwinAI, which specializes in visual quality inspection using its Explainable AI platform.</v>
     <v>161000</v>
@@ -4795,24 +4809,25 @@
     <v>XNAS</v>
     <v>XNAS</v>
     <v>One Apple Park Way, CUPERTINO, CA, 95014 US</v>
-    <v>229.82</v>
+    <v>233.09</v>
     <v>Computers, Phones &amp; Household Electronics</v>
     <v>Stock</v>
-    <v>45554.999953321094</v>
+    <v>45555.999911909377</v>
     <v>12</v>
-    <v>224.63</v>
-    <v>3479771521800</v>
+    <v>227.62</v>
+    <v>3469584000000</v>
     <v>APPLE INC.</v>
     <v>APPLE INC.</v>
-    <v>224.99</v>
-    <v>34.846699999999998</v>
-    <v>220.69</v>
+    <v>229.97</v>
+    <v>34.744700000000002</v>
     <v>228.87</v>
+    <v>228.2</v>
+    <v>227.7664</v>
     <v>15204140000</v>
     <v>AAPL</v>
     <v>APPLE INC. (XNAS:AAPL)</v>
-    <v>73844</v>
-    <v>44471580</v>
+    <v>318679888</v>
+    <v>45464410</v>
     <v>1977</v>
   </rv>
   <rv s="2">
@@ -4828,7 +4843,7 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>5</v>
+    <v>4</v>
     <v>en-GB</v>
     <v>a1ncgh</v>
     <v>268435456</v>
@@ -4836,9 +4851,11 @@
     <v>Powered by Refinitiv</v>
     <v>92.82</v>
     <v>50.134999999999998</v>
-    <v>0.99250000000000005</v>
-    <v>2.42</v>
-    <v>2.7323E-2</v>
+    <v>0.98839999999999995</v>
+    <v>7.0000000000000007E-2</v>
+    <v>7.693E-4</v>
+    <v>-0.32</v>
+    <v>-3.5139999999999998E-3</v>
     <v>USD</v>
     <v>Allison Transmission Holdings, Inc. is a designer and manufacturer of propulsion solutions for commercial and defense vehicles. The Company is also a manufacturer of medium-and heavy-duty fully automatic transmissions. Its products are used in a variety of applications, including on-highway trucks, including distribution, refuse, construction, fire and emergency; buses, including school, transit and coach; motorhomes, off-highway vehicles, and equipment, including energy, mining and construction applications; and defense vehicles, including tactical wheeled and tracked. The Company operates in approximately 150 countries. The Company has manufacturing facilities in the United States, Hungary and India, as well as global engineering resources, including electrification engineering centers in Indianapolis, Indiana, Auburn Hills, Michigan and London in the United Kingdom. The Company also has approximately 1,600 independent distributor and dealer locations worldwide.</v>
     <v>3700</v>
@@ -4846,24 +4863,25 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>One Allison Way, INDIANAPOLIS, IN, 46222 US</v>
-    <v>91.22</v>
+    <v>91.32</v>
     <v>Machinery, Equipment &amp; Components</v>
     <v>Stock</v>
-    <v>45554.958333378905</v>
+    <v>45555.97244203672</v>
     <v>15</v>
-    <v>89.39</v>
-    <v>7928675701</v>
+    <v>89.15</v>
+    <v>7934775000</v>
     <v>ALLISON TRANSMISSION HOLDINGS, INC.</v>
     <v>ALLISON TRANSMISSION HOLDINGS, INC.</v>
-    <v>90.1</v>
-    <v>11.8979</v>
-    <v>88.57</v>
+    <v>90.42</v>
+    <v>11.907</v>
     <v>90.99</v>
+    <v>91.06</v>
+    <v>90.74</v>
     <v>87137880</v>
     <v>ALSN</v>
     <v>ALLISON TRANSMISSION HOLDINGS, INC. (XNYS:ALSN)</v>
-    <v>571135</v>
-    <v>483317</v>
+    <v>1483495</v>
+    <v>489823</v>
     <v>2007</v>
   </rv>
   <rv s="2">
@@ -4879,7 +4897,7 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>5</v>
+    <v>4</v>
     <v>en-GB</v>
     <v>az23tc</v>
     <v>268435456</v>
@@ -4887,9 +4905,11 @@
     <v>Powered by Refinitiv</v>
     <v>40.695</v>
     <v>18</v>
-    <v>2.0030999999999999</v>
-    <v>0.32</v>
-    <v>1.652E-2</v>
+    <v>1.9927999999999999</v>
+    <v>-0.34</v>
+    <v>-1.7267999999999999E-2</v>
+    <v>-7.0000000000000007E-2</v>
+    <v>-3.6180000000000001E-3</v>
     <v>USD</v>
     <v>Par Pacific Holdings, Inc. is an energy company, which provides both renewable and conventional fuels to the western United States. It owns and operates 125,000 barrels per day of combined refining capacity across three locations and an energy infrastructure network, including 7.6 million barrels of storage, and marine, rail, rack and pipeline assets. The Company has three segments. Refining segment owns and operates four refineries with total operating crude oil throughput capacity of 219 thousand barrels per day (Mbpd). Retail segment operates fuel retail outlets in Hawaii, Washington and Idaho. It operates convenience stores and fuel retail sites under Hele and nomnom brands, 76 branded fuel retail sites and other sites operated by third parties that sell gasoline, diesel, and retail merchandise, such as soft drinks, prepared foods, and other sundries. Logistics segment operates a multi-modal logistics network spanning the Pacific, the Northwest, and the Rocky Mountain regions.</v>
     <v>1814</v>
@@ -4897,24 +4917,25 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>825 Town and Country Ln Ste 1500, HOUSTON, TX, 77024-2235 US</v>
-    <v>20.2</v>
+    <v>19.555</v>
     <v>Oil &amp; Gas</v>
     <v>Stock</v>
-    <v>45554.958333356248</v>
+    <v>45555.958333356248</v>
     <v>18</v>
-    <v>19.555</v>
-    <v>1109154830</v>
+    <v>18.440000000000001</v>
+    <v>1090002000</v>
     <v>PAR PACIFIC HOLDINGS, INC.</v>
     <v>PAR PACIFIC HOLDINGS, INC.</v>
-    <v>19.809999999999999</v>
-    <v>3.4306000000000001</v>
-    <v>19.37</v>
+    <v>19.16</v>
+    <v>3.3714</v>
     <v>19.690000000000001</v>
+    <v>19.350000000000001</v>
+    <v>19.28</v>
     <v>56330870</v>
     <v>PARR</v>
     <v>PAR PACIFIC HOLDINGS, INC. (XNYS:PARR)</v>
-    <v>737114</v>
-    <v>911057</v>
+    <v>5755229</v>
+    <v>903736</v>
     <v>2005</v>
   </rv>
   <rv s="2">
@@ -4930,7 +4951,7 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>5</v>
+    <v>4</v>
     <v>en-GB</v>
     <v>a1v177</v>
     <v>268435456</v>
@@ -4938,9 +4959,11 @@
     <v>Powered by Refinitiv</v>
     <v>84.44</v>
     <v>38.5</v>
-    <v>1.3108</v>
-    <v>2.11</v>
-    <v>3.4980000000000004E-2</v>
+    <v>1.3077000000000001</v>
+    <v>-0.63</v>
+    <v>-1.0091000000000001E-2</v>
+    <v>0</v>
+    <v>0</v>
     <v>USD</v>
     <v>Hyster-Yale, Inc., formerly Hyster-Yale Materials Handling, Inc., through its wholly owned operating subsidiary, Hyster-Yale Materials Handling, designs, engineers, manufactures, sells, and services a comprehensive line of lift trucks, attachments, aftermarket parts and technology solutions marketed globally primarily under the Hyster and Yale brand names. The Company's business segments include Lift Trucks, Attachments and Fuel Cells. The Hyster-Yale Maximal brand provides trucks for customers requiring fundamental lift truck performance. The Lift Truck segment is focused on fuel cell-powered battery box replacements and integrated fuel cell engine solutions. Hyster- Yale’s attachment subsidiary, Bolzoni S.p.A., is a producer of attachments, forks, and lift tables under the Bolzoni, Auramo and Meyer brand names. The Fuel Cell business, Nuvera Fuel Cells, is an alternative-power technology company focused on fuel cell stacks and engines.</v>
     <v>8600</v>
@@ -4948,24 +4971,25 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>5875 LANDERBROOK DRIVE, SUITE 300, CLEVELAND, OH, 44124 US</v>
-    <v>62.65</v>
+    <v>62.47</v>
     <v>Machinery, Equipment &amp; Components</v>
     <v>Stock</v>
-    <v>45554.958333378905</v>
+    <v>45555.958333378905</v>
     <v>21</v>
-    <v>61.01</v>
-    <v>1092596794</v>
+    <v>60.734999999999999</v>
+    <v>1081571000</v>
     <v>HYSTER-YALE, INC.</v>
     <v>HYSTER-YALE, INC.</v>
+    <v>61.81</v>
+    <v>6.1798999999999999</v>
+    <v>62.43</v>
     <v>61.8</v>
-    <v>6.2428999999999997</v>
-    <v>60.32</v>
-    <v>62.43</v>
+    <v>61.8</v>
     <v>17501150</v>
     <v>HY</v>
     <v>HYSTER-YALE, INC. (XNYS:HY)</v>
-    <v>61542</v>
-    <v>66109</v>
+    <v>152802</v>
+    <v>64494</v>
     <v>1999</v>
   </rv>
   <rv s="2">
@@ -4975,13 +4999,13 @@
     <v>https://www.bing.com/financeapi/forcetrigger?t=a1zvsm&amp;q=XNYS%3aPII&amp;form=skydnc</v>
     <v>Learn more on Bing</v>
   </rv>
-  <rv s="3">
-    <v>6</v>
+  <rv s="1">
+    <v>0</v>
     <v>Polaris Inc. (XNYS:PII)</v>
     <v>2</v>
-    <v>7</v>
+    <v>3</v>
     <v>Finance</v>
-    <v>8</v>
+    <v>5</v>
     <v>en-GB</v>
     <v>a1zvsm</v>
     <v>268435456</v>
@@ -4989,9 +5013,11 @@
     <v>Powered by Refinitiv</v>
     <v>107.955</v>
     <v>71.900000000000006</v>
-    <v>1.5097</v>
-    <v>2.38</v>
-    <v>2.8510000000000001E-2</v>
+    <v>1.5104</v>
+    <v>-1.56</v>
+    <v>-1.8169000000000001E-2</v>
+    <v>0</v>
+    <v>0</v>
     <v>USD</v>
     <v>Polaris Inc. is engaged in designing, engineering, manufacturing and marketing of powersports vehicles. The Company also designs and manufactures or sources parts, garments and accessories (PG&amp;A), which includes aftermarket accessories and apparel. The Company operates through three segments: Off Road, On Road and Marine. The Off Road segment consists of off-road vehicles and snowmobiles. The On Road segment designs and manufactures motorcycles, moto-roadsters, light duty hauling, and passenger vehicles. The Marine segment designs and manufactures boats that are designed to compete in key segments of the recreational marine industry, specifically pontoon and deck boats. Its product line-up includes the RANGER, RZR and Polaris XPEDITION and GENERAL side-by-side off-road vehicles; Sportsman all-terrain off-road vehicles; military and commercial off-road vehicles; snowmobiles; Indian Motorcycle mid-size and heavyweight motorcycles; Slingshot moto-roadsters, and pontoon and deck boats.</v>
     <v>18500</v>
@@ -4999,25 +5025,25 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>2100 HIGHWAY 55, MEDINA, MN, 55340-9770 US</v>
-    <v>85.9</v>
+    <v>85.73</v>
     <v>Leisure Products</v>
     <v>Stock</v>
-    <v>45554.958333356248</v>
+    <v>45555.847227696097</v>
     <v>24</v>
-    <v>84.364999999999995</v>
-    <v>4786525855</v>
+    <v>83.36</v>
+    <v>4701231000</v>
     <v>Polaris Inc.</v>
     <v>Polaris Inc.</v>
-    <v>85.55</v>
+    <v>85.73</v>
     <v>15.0388</v>
-    <v>83.48</v>
     <v>85.86</v>
-    <v>85.86</v>
+    <v>84.3</v>
+    <v>84.33</v>
     <v>55748030</v>
     <v>PII</v>
     <v>Polaris Inc. (XNYS:PII)</v>
-    <v>107</v>
-    <v>461892</v>
+    <v>1113065</v>
+    <v>460857</v>
     <v>1994</v>
   </rv>
   <rv s="2">
@@ -5033,7 +5059,7 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>5</v>
+    <v>4</v>
     <v>en-GB</v>
     <v>aw21cw</v>
     <v>268435456</v>
@@ -5041,9 +5067,11 @@
     <v>Powered by Refinitiv</v>
     <v>114.29989999999999</v>
     <v>75.430000000000007</v>
-    <v>1.7444</v>
-    <v>3.37</v>
-    <v>3.5726000000000001E-2</v>
+    <v>1.7347999999999999</v>
+    <v>-0.37</v>
+    <v>-3.787E-3</v>
+    <v>-2.3199999999999998</v>
+    <v>-2.3836E-2</v>
     <v>USD</v>
     <v>CONSOL Energy Inc. is a producer and exporter of high-Btu bituminous thermal coal and metallurgical coal. It owns and operates longwall mining operations in the Northern Appalachian Basin. Its flagship operation is the Pennsylvania Mining Complex, located over 26 miles southwest of Pittsburgh, near the city of Washington and the borough of Waynesburg all in Pennsylvania, and consists of three deep longwall mining operations: the Bailey Mine, the Enlow Fork Mine and the Harvey Mine, as well as a centralized preparation plant. Its segments include the PAMC and the CONSOL Marine Terminal. The PAMC includes the Bailey Mine, the Enlow Fork Mine, the Harvey Mine and a centralized preparation plant. The PAMC segment's principal activities include the mining, preparation and marketing of bituminous coal, sold primarily to industrial end-users, metallurgical end-users and power generators. The CONSOL Marine Terminal segment provides coal export terminal services through the Port of Baltimore.</v>
     <v>2020</v>
@@ -5051,24 +5079,25 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>275 TECHNOLOGY DRIVE, SUITE #101, CANONSBURG, PA, 15317 US</v>
-    <v>97.91</v>
+    <v>99.21</v>
     <v>Coal</v>
     <v>Stock</v>
-    <v>45554.958333367969</v>
+    <v>45555.958333367969</v>
     <v>27</v>
-    <v>95.04</v>
-    <v>2871718571</v>
+    <v>96.56</v>
+    <v>2860843000</v>
     <v>CONSOL ENERGY INC.</v>
     <v>CONSOL ENERGY INC.</v>
-    <v>96.94</v>
-    <v>7.2929000000000004</v>
-    <v>94.33</v>
+    <v>97.53</v>
+    <v>7.2652999999999999</v>
     <v>97.7</v>
+    <v>97.33</v>
+    <v>95.01</v>
     <v>29393230</v>
     <v>CEIX</v>
     <v>CONSOL ENERGY INC. (XNYS:CEIX)</v>
-    <v>6</v>
-    <v>492196</v>
+    <v>1215282</v>
+    <v>494365</v>
     <v>2017</v>
   </rv>
   <rv s="2">
@@ -5084,7 +5113,7 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>5</v>
+    <v>4</v>
     <v>en-GB</v>
     <v>a1n1r7</v>
     <v>268435456</v>
@@ -5092,9 +5121,11 @@
     <v>Powered by Refinitiv</v>
     <v>127.3484</v>
     <v>84.35</v>
-    <v>1.2448999999999999</v>
-    <v>2.08</v>
-    <v>2.2187000000000002E-2</v>
+    <v>1.2488999999999999</v>
+    <v>-1.0900000000000001</v>
+    <v>-1.1374E-2</v>
+    <v>-0.6</v>
+    <v>-6.3330000000000001E-3</v>
     <v>USD</v>
     <v>AGCO Corporation is a designer, manufacturer and distributor of agricultural machinery and precision agriculture technology. The Company sells a range of agricultural equipment, including tractors, combines, self-propelled sprayers, hay tools, forage equipment, seeding and tillage equipment, implements, and grain storage and protein production systems. It provides telemetry-based fleet management tools, including remote monitoring and diagnostics, which help farmers improve uptime, machine and yield optimization, mixed fleet optimization and decision support. The Company's Precision Planting, Headsight and Intelligent Ag Solutions brands provide retrofit solutions to upgrade farmers existing equipment to improve their planting, liquid application and harvest operations. The Company’s Precision Planting, Headsight, JCA and Intelligent Ag Solutions brands also sell precision agriculture solutions around the crop cycle to third party original equipment manufacturers (OEMs).</v>
     <v>27900</v>
@@ -5102,24 +5133,25 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>4205 River Green Pkway, DULUTH, GA, 30096 US</v>
-    <v>96.49</v>
+    <v>95.61</v>
     <v>Machinery, Equipment &amp; Components</v>
     <v>Stock</v>
-    <v>45554.958333356248</v>
+    <v>45555.96684641172</v>
     <v>30</v>
-    <v>94.62</v>
-    <v>7152971609</v>
+    <v>93.655000000000001</v>
+    <v>7071612000</v>
     <v>AGCO CORPORATION</v>
     <v>AGCO CORPORATION</v>
-    <v>95.59</v>
-    <v>17.070900000000002</v>
-    <v>93.75</v>
+    <v>95.29</v>
+    <v>16.8766</v>
     <v>95.83</v>
+    <v>94.74</v>
+    <v>94.14</v>
     <v>74642300</v>
     <v>AGCO</v>
     <v>AGCO CORPORATION (XNYS:AGCO)</v>
-    <v>569964</v>
-    <v>739418</v>
+    <v>1623030</v>
+    <v>735783</v>
     <v>1991</v>
   </rv>
   <rv s="2">
@@ -5135,7 +5167,7 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>5</v>
+    <v>4</v>
     <v>en-GB</v>
     <v>a1vuw7</v>
     <v>268435456</v>
@@ -5143,9 +5175,11 @@
     <v>Powered by Refinitiv</v>
     <v>30.1</v>
     <v>24.01</v>
-    <v>1.1547000000000001</v>
-    <v>-0.09</v>
-    <v>-3.2850000000000002E-3</v>
+    <v>1.1538999999999999</v>
+    <v>-0.73</v>
+    <v>-2.673E-2</v>
+    <v>-0.55020000000000002</v>
+    <v>-2.07E-2</v>
     <v>USD</v>
     <v>Ituran Location and Control Ltd. is a provider of location-based services, consisting of stolen vehicle recovery (SVR), fleet management services and other tracking services. The Company also provides wireless communication products used in connection with its location-based services and various other applications. Its operations consist of two segments: location-based services and wireless communications products. Its location-based services segment consists of its SVR and tracking services, fleet management and value-added services consisted of personal locater services and concierge services. Its wireless communications products segment consists of short and medium range two-way machine-to-machine wireless communications products that are used for various applications, including automatic vehicle location (AVL) and automatic vehicle identification. It primarily provides its services, as well as sells and leases its products in Israel, Brazil, Argentina and the United States.</v>
     <v>2841</v>
@@ -5153,24 +5187,25 @@
     <v>XNAS</v>
     <v>XNAS</v>
     <v>3 HASHIKMA, A.T AZUR, T.D 163, AZOR, 5800182 IL</v>
-    <v>28</v>
+    <v>26.99</v>
     <v>Communications &amp; Networking</v>
     <v>Stock</v>
-    <v>45554.996892245312</v>
+    <v>45555.917770381253</v>
     <v>33</v>
-    <v>27.31</v>
-    <v>543293669</v>
+    <v>26.08</v>
+    <v>528771400</v>
     <v>ITURAN LOCATION AND CONTROL LTD.</v>
     <v>ITURAN LOCATION AND CONTROL LTD.</v>
-    <v>27.78</v>
-    <v>10.6959</v>
-    <v>27.4</v>
+    <v>26.5</v>
+    <v>10.4101</v>
     <v>27.31</v>
+    <v>26.58</v>
+    <v>26.029800000000002</v>
     <v>19893580</v>
     <v>ITRN</v>
     <v>ITURAN LOCATION AND CONTROL LTD. (XNAS:ITRN)</v>
-    <v>37008</v>
-    <v>82373</v>
+    <v>184508</v>
+    <v>81754</v>
     <v>1994</v>
   </rv>
   <rv s="2">
@@ -5186,7 +5221,7 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>5</v>
+    <v>4</v>
     <v>en-GB</v>
     <v>a1sea2</v>
     <v>268435456</v>
@@ -5194,9 +5229,11 @@
     <v>Powered by Refinitiv</v>
     <v>14.475</v>
     <v>6.37</v>
-    <v>2.15</v>
-    <v>-0.03</v>
-    <v>-2.2759999999999998E-3</v>
+    <v>2.1524000000000001</v>
+    <v>-0.01</v>
+    <v>-7.6050000000000011E-4</v>
+    <v>0.11</v>
+    <v>8.371E-3</v>
     <v>USD</v>
     <v>Everi Holdings Inc. develops and offers products and services that provide gaming entertainment, improve its customers’ patron engagement, and help its casino customers operate their businesses. It develops and supplies entertaining game content, gaming machines and gaming systems and services for land-based and iGaming operators. It operates through two segments: Games and Financial Technology Solutions (FinTech). The Games segment provides gaming operators with gaming technology and entertainment products and services, including gaming machines, primarily comprising Class II, Class III and Historic Horse Racing slot machines placed under participation and fixed-fee lease arrangements or sold to casino customers. The FinTech segment provides gaming operators with financial technology products and services, including financial access and related services supporting digital, cashless and physical cash options across mobile, assisted and self-service channels.</v>
     <v>2200</v>
@@ -5204,36 +5241,37 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>7250 S Tenaya Way Ste 100, LAS VEGAS, NV, 89113-2175 US</v>
-    <v>13.22</v>
+    <v>13.19</v>
     <v>Hotels &amp; Entertainment Services</v>
     <v>Stock</v>
-    <v>45554.958333367969</v>
+    <v>45555.967937928122</v>
     <v>36</v>
-    <v>13.14</v>
-    <v>1122005077</v>
+    <v>13.13</v>
+    <v>1121152000</v>
     <v>EVERI HOLDINGS INC.</v>
     <v>EVERI HOLDINGS INC.</v>
-    <v>13.18</v>
-    <v>27.929400000000001</v>
-    <v>13.18</v>
+    <v>13.19</v>
+    <v>27.9099</v>
     <v>13.15</v>
+    <v>13.14</v>
+    <v>13.25</v>
     <v>85323580</v>
     <v>EVRI</v>
     <v>EVERI HOLDINGS INC. (XNYS:EVRI)</v>
-    <v>521172</v>
-    <v>844929</v>
+    <v>1441199</v>
+    <v>834251</v>
     <v>2004</v>
   </rv>
   <rv s="2">
     <v>37</v>
   </rv>
-  <rv s="4">
-    <v>9</v>
+  <rv s="3">
+    <v>6</v>
     <v>NEXTRACKER INC. (XNAS:NXT)</v>
-    <v>10</v>
+    <v>7</v>
     <v>3</v>
     <v>Finance</v>
-    <v>5</v>
+    <v>4</v>
     <v>en-GB</v>
     <v>c8ssgh</v>
     <v>268435456</v>
@@ -5242,8 +5280,10 @@
     <v>62.31</v>
     <v>32.14</v>
     <v>2.1349999999999998</v>
-    <v>-0.38</v>
-    <v>-1.0315000000000001E-2</v>
+    <v>0.2</v>
+    <v>5.4850000000000003E-3</v>
+    <v>0.01</v>
+    <v>2.7279999999999996E-4</v>
     <v>USD</v>
     <v>Nextracker Inc. is a provider of integrated solar tracker and software solutions used in utility-scale and ground-mounted distributed generation solar projects. Its products enable solar panels in utility-scale power plants to follow the sun’s movement across the sky and optimize plant performance. Its products include NX Horizon, NX Gemini, TrueCapture, and NX Navigator. Its solutions include Bifacial PV modules, Large Format Modules, and First Solar Series 6 (FSLR6) Modules. NX Horizon is a one-in-portrait (1P) smart solar tracker system that delivers the lowest levelized cost of energy (LCOE). NX Gemini is its two-in-portrait (2P) format tracker which holds two rows of solar panels along the central support beam. TrueCapture is its flagship software offering, which is a self-adjusting tracker control system that uses machine learning to enhance solar power plant energy yield. It has operations in the United States, Brazil, Mexico, Spain, India, Australia, the Middle East and Brazil.</v>
     <v>1050</v>
@@ -5251,23 +5291,24 @@
     <v>XNAS</v>
     <v>XNAS</v>
     <v>6200 Paseo Padre Pkwy, FREMONT, CA, 94555 US</v>
-    <v>38.49</v>
+    <v>36.950000000000003</v>
     <v>Renewable Energy</v>
     <v>Stock</v>
-    <v>45554.977939142969</v>
-    <v>36.159999999999997</v>
-    <v>5299366204</v>
+    <v>45555.991244664059</v>
+    <v>35.86</v>
+    <v>5328437000</v>
     <v>NEXTRACKER INC.</v>
     <v>NEXTRACKER INC.</v>
-    <v>38.49</v>
-    <v>9.6762999999999995</v>
-    <v>36.840000000000003</v>
+    <v>36.36</v>
+    <v>9.7293000000000003</v>
     <v>36.46</v>
+    <v>36.659999999999997</v>
+    <v>36.67</v>
     <v>145347400</v>
     <v>NXT</v>
     <v>NEXTRACKER INC. (XNAS:NXT)</v>
-    <v>601</v>
-    <v>2855707</v>
+    <v>11221138</v>
+    <v>2881718</v>
     <v>2022</v>
   </rv>
   <rv s="2">
@@ -5283,7 +5324,7 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>5</v>
+    <v>4</v>
     <v>en-GB</v>
     <v>a1xejc</v>
     <v>268435456</v>
@@ -5291,9 +5332,11 @@
     <v>Powered by Refinitiv</v>
     <v>80.22</v>
     <v>56.25</v>
-    <v>1.7425999999999999</v>
-    <v>0.19</v>
-    <v>2.4849999999999998E-3</v>
+    <v>1.7439</v>
+    <v>-0.39</v>
+    <v>-5.0880000000000005E-3</v>
+    <v>-0.04</v>
+    <v>-5.2450000000000001E-4</v>
     <v>USD</v>
     <v>Monarch Casino &amp; Resort, Inc. owns and operates the Atlantis Casino Resort Spa, a hotel and casino in Reno, Nevada (the Atlantis) and the Monarch Casino Resort Spa Black Hawk (the Monarch Black Hawk), a hotel and casino in Black Hawk, Colorado. In addition, it owns separate parcels of land located next to the Atlantis and a parcel of land with an industrial warehouse located between Denver, Colorado, and Monarch Black Hawk. The Atlantis is located approximately three miles south of downtown, which features approximately 61,000 square feet of casino space; 817 guest rooms and suites; eight food outlets; two gourmet coffee and pastry bars and one snack bar; a 30,000 square-foot health spa and salon with an enclosed year-round pool. Monarch Black Hawk features approximately 60,000 square feet of casino space; approximately 1,000 slot machines; approximately 43 table games; a live poker room; a keno counter and a sports book. The resort also includes 10 bars and lounges.</v>
     <v>2900</v>
@@ -5301,24 +5344,25 @@
     <v>XNAS</v>
     <v>XNAS</v>
     <v>Executive Offices, 3800 S Virginia Street, RENO, NV, 89502 US</v>
-    <v>77.89</v>
+    <v>77.28</v>
     <v>Hotels &amp; Entertainment Services</v>
     <v>Stock</v>
-    <v>45554.85904797422</v>
+    <v>45555.903181411719</v>
     <v>41</v>
-    <v>75.87</v>
-    <v>1414354998</v>
+    <v>75.349999999999994</v>
+    <v>1407158000</v>
     <v>MONARCH CASINO &amp; RESORT, INC.</v>
     <v>MONARCH CASINO &amp; RESORT, INC.</v>
-    <v>77.739999999999995</v>
-    <v>17.912400000000002</v>
-    <v>76.459999999999994</v>
+    <v>76.36</v>
+    <v>17.821100000000001</v>
     <v>76.650000000000006</v>
+    <v>76.260000000000005</v>
+    <v>76.22</v>
     <v>18452120</v>
     <v>MCRI</v>
     <v>MONARCH CASINO &amp; RESORT, INC. (XNAS:MCRI)</v>
-    <v>139155</v>
-    <v>101934</v>
+    <v>1349469</v>
+    <v>104726</v>
     <v>1993</v>
   </rv>
   <rv s="2">
@@ -5342,9 +5386,11 @@
     <v>Powered by Refinitiv</v>
     <v>69.75</v>
     <v>34.96</v>
-    <v>0.97099999999999997</v>
-    <v>1.5</v>
-    <v>2.5000000000000001E-2</v>
+    <v>0.97</v>
+    <v>0.19</v>
+    <v>3.0890000000000002E-3</v>
+    <v>0</v>
+    <v>0</v>
     <v>USD</v>
     <v>Miller Industries, Inc. is a manufacturer of towing and recovery equipment. The Company designs and manufactures bodies of car carriers and wreckers, which are installed on chassis manufactured by third parties, and sold to its customers. Its products are marketed and sold through a network of distributors that serve all 50 states, Canada, Mexico, and other foreign markets, and through prime contractors to governmental entities. In addition to selling its products, its independent distributors provide end-users with parts and service. Its product line includes car carriers, wreckers, and transport trailers. Car carriers are specialized flat-bed vehicles with hydraulic tilt mechanisms that enable a towing operator to drive or winch a vehicle onto the bed for transport. Its multi-vehicle transport trailers are specialized auto transport trailers with upper and lower decks and hydraulic ramps for loading vehicles. Its brands include Century, Vulcan, Chevron, Holmes, and Challenger.</v>
     <v>1821</v>
@@ -5352,24 +5398,25 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>Ste 100, 8503 Hilltop Dr, OOLTEWAH, TN, 37363 US</v>
-    <v>61.999899999999997</v>
+    <v>61.99</v>
     <v>Automobiles &amp; Auto Parts</v>
     <v>Stock</v>
-    <v>45554.958333344533</v>
+    <v>45555.84722947891</v>
     <v>44</v>
-    <v>60.08</v>
-    <v>704408085</v>
+    <v>60.064999999999998</v>
+    <v>706584305</v>
     <v>MILLER INDUSTRIES, INC.</v>
     <v>MILLER INDUSTRIES, INC.</v>
-    <v>61.25</v>
+    <v>60.7</v>
     <v>9.9006000000000007</v>
-    <v>60</v>
+    <v>61.5</v>
+    <v>61.69</v>
     <v>61.5</v>
     <v>11453790</v>
     <v>MLR</v>
     <v>MILLER INDUSTRIES, INC. (XNYS:MLR)</v>
-    <v>102467</v>
-    <v>85821</v>
+    <v>338551</v>
+    <v>86786</v>
     <v>1994</v>
   </rv>
   <rv s="2">
@@ -5385,7 +5432,7 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>5</v>
+    <v>4</v>
     <v>en-GB</v>
     <v>btavh7</v>
     <v>268435456</v>
@@ -5393,9 +5440,11 @@
     <v>Powered by Refinitiv</v>
     <v>15.86</v>
     <v>9.1649999999999991</v>
-    <v>0.89800000000000002</v>
-    <v>0.11</v>
-    <v>1.0989000000000001E-2</v>
+    <v>0.89059999999999995</v>
+    <v>-0.02</v>
+    <v>-1.9759999999999999E-3</v>
+    <v>-0.01</v>
+    <v>-9.9010000000000005E-4</v>
     <v>USD</v>
     <v>Janus International Group, Inc. is a global manufacturer and supplier of turn-key self-storage, commercial and industrial building solutions. It operates through two geographic segments: Janus North America and Janus International. The Janus North America segment is comprised of all the other entities, including Janus International Group, LLC, Betco, Inc., Noke, Inc., Asta Industries, Inc., DBCI, LLC, Access Control Technologies, LLC, Janus Door, LLC, and Steel Door Depot.com, LLC. The Janus International segment is comprised of Janus International Europe Holdings Ltd. (UK). Its production and sales are in Europe and Australia. It provides facility and door automation and access control technologies, roll up and swing doors, hallway systems and relocatable storage moveable additional storage structures (MASS) units. It is comprised of three sales channels, including New Construction-Self-storage, R3-Self-storage, and Commercial and Other. It also provides terminal maintenance services.</v>
     <v>1956</v>
@@ -5403,24 +5452,25 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>135 Janus International Blvd., TEMPLE, GA, 30179 US</v>
-    <v>10.3</v>
+    <v>10.385</v>
     <v>Homebuilding &amp; Construction Supplies</v>
     <v>Stock</v>
-    <v>45554.958333356248</v>
+    <v>45555.958333356248</v>
     <v>47</v>
-    <v>10.06</v>
-    <v>1454676000</v>
+    <v>10.02</v>
+    <v>1467755000</v>
     <v>JANUS INTERNATIONAL GROUP, INC.</v>
     <v>JANUS INTERNATIONAL GROUP, INC.</v>
-    <v>10.24</v>
-    <v>11.3477</v>
-    <v>10.01</v>
+    <v>10.19</v>
+    <v>11.3254</v>
     <v>10.119999999999999</v>
+    <v>10.1</v>
+    <v>10.09</v>
     <v>145322200</v>
     <v>JBI</v>
     <v>JANUS INTERNATIONAL GROUP, INC. (XNYS:JBI)</v>
-    <v>1702699</v>
-    <v>2025718</v>
+    <v>5522079</v>
+    <v>1977907</v>
     <v>2020</v>
   </rv>
   <rv s="2">
@@ -5444,9 +5494,11 @@
     <v>Powered by Refinitiv</v>
     <v>574.76</v>
     <v>318.17</v>
-    <v>1.2955000000000001</v>
-    <v>0.56999999999999995</v>
-    <v>1.4149999999999998E-3</v>
+    <v>1.3098000000000001</v>
+    <v>-1.28</v>
+    <v>-3.1740000000000002E-3</v>
+    <v>-0.23</v>
+    <v>-5.7209999999999997E-4</v>
     <v>USD</v>
     <v>Ulta Beauty, Inc. is a beauty retailer. The Company's product categories include cosmetics, skincare, haircare products and styling tools, fragrance and bath, services, and accessories and other. The Company has one segment, which includes retail stores, salon services, and e-commerce. It offers a range of beauty services in its stores, focusing on hair, makeup, brow and skin services. Its skin services include a skin treatment room or dedicated skin treatment area on the sales floor. Its Ulta Beauty store prototype includes an open salon area, with most of its stores offering brow services on the salon floor. It offers a new way to shop for beauty - bringing together All Things Beauty, All in One Place. In addition to ship to home order fulfillment, it offers guests Buy Online, Pick-up in Store, Curbside Pickup, and Store 2 Door, which provides the ability for customers to order in-store and have products delivered to their homes. It operates over 1,350 retail stores across 50 states.</v>
     <v>20000</v>
@@ -5454,24 +5506,25 @@
     <v>XNAS</v>
     <v>XNAS</v>
     <v>1000 Remington Blvd, Suite 120, BOLINGBROOK, IL, 60440 US</v>
-    <v>409.59</v>
+    <v>408</v>
     <v>Specialty Retailers</v>
     <v>Stock</v>
-    <v>45554.995565786718</v>
+    <v>45555.999797256249</v>
     <v>50</v>
-    <v>400.3</v>
-    <v>19000899461</v>
+    <v>400.2</v>
+    <v>18940590000</v>
     <v>ULTA BEAUTY, INC.</v>
     <v>ULTA BEAUTY, INC.</v>
-    <v>408.75</v>
-    <v>16.193899999999999</v>
-    <v>402.72</v>
+    <v>402</v>
+    <v>16.142499999999998</v>
     <v>403.29</v>
+    <v>402.01</v>
+    <v>401.78</v>
     <v>47114730</v>
     <v>ULTA</v>
     <v>ULTA BEAUTY, INC. (XNAS:ULTA)</v>
-    <v>132</v>
-    <v>1668245</v>
+    <v>1451394</v>
+    <v>1665189</v>
     <v>2016</v>
   </rv>
   <rv s="2">
@@ -5487,7 +5540,7 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>5</v>
+    <v>4</v>
     <v>en-GB</v>
     <v>a1vehw</v>
     <v>268435456</v>
@@ -5495,9 +5548,11 @@
     <v>Powered by Refinitiv</v>
     <v>32.24</v>
     <v>18.899999999999999</v>
-    <v>1.9695</v>
-    <v>0.02</v>
-    <v>9.1279999999999996E-4</v>
+    <v>1.9694</v>
+    <v>-0.26</v>
+    <v>-1.1856E-2</v>
+    <v>-0.26</v>
+    <v>-1.1998E-2</v>
     <v>USD</v>
     <v>International Game Technology PLC is a United Kingdom-based company, which is engaged in gaming. The Company operates and provides an integrated portfolio of gaming technology products and services, including online and instant lottery systems, iLottery, instant ticket printing, lottery management services, commercial services, gaming systems, electronic gaming machines, iGaming, and sports betting. The Company operates through three segments. The Global Lottery segment operates traditional lottery and iLottery businesses across the world, which includes sales, operations, product development, technology, and support, across the world. The Global Gaming segment operates a land-based gaming business across the world, which includes sales, product management, studios, global manufacturing, operation, and technology, across the world. The Digital &amp; Betting segment operates iGaming and sports betting activities across the world.</v>
     <v>11000</v>
@@ -5505,24 +5560,25 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>10 Finsbury Square, Third Floor, LONDON, UNITED KINGDOM-NA, EC2A 1AF GB</v>
-    <v>22.52</v>
+    <v>21.88</v>
     <v>Hotels &amp; Entertainment Services</v>
     <v>Stock</v>
-    <v>45554.958333356248</v>
+    <v>45555.999513726565</v>
     <v>53</v>
-    <v>21.89</v>
-    <v>4386000000</v>
+    <v>21.46</v>
+    <v>4334000000</v>
     <v>INTERNATIONAL GAME TECHNOLOGY PLC</v>
     <v>INTERNATIONAL GAME TECHNOLOGY PLC</v>
-    <v>22.52</v>
-    <v>21.217300000000002</v>
-    <v>21.91</v>
+    <v>21.84</v>
+    <v>20.965599999999998</v>
     <v>21.93</v>
+    <v>21.67</v>
+    <v>21.41</v>
     <v>200000000</v>
     <v>IGT</v>
     <v>INTERNATIONAL GAME TECHNOLOGY PLC (XNYS:IGT)</v>
-    <v>578995</v>
-    <v>634451</v>
+    <v>1539803</v>
+    <v>628576</v>
     <v>2014</v>
   </rv>
   <rv s="2">
@@ -5546,9 +5602,11 @@
     <v>Powered by Refinitiv</v>
     <v>87.32</v>
     <v>54.8</v>
-    <v>0.58699999999999997</v>
-    <v>0.86</v>
-    <v>1.2675000000000001E-2</v>
+    <v>0.58579999999999999</v>
+    <v>0.34</v>
+    <v>4.9480000000000001E-3</v>
+    <v>0</v>
+    <v>0</v>
     <v>USD</v>
     <v>Oil-Dri Corporation of America is a manufacturer and supplier of specialty sorbent products for pet care, animal health and nutrition, fluid purification, agricultural ingredients, sports field, industrial and automotive markets. Its principal product is cat litter. The Company’s Retail and Wholesale Products Group segment customers include mass merchandisers, the farm and fleet channel, drugstore chains, pet specialty retail outlets, dollar stores, retail grocery stores, distributors of industrial cleanup and automotive products, environmental service companies, sports field product users and marketers of consumer products. Its Business to Business Products Group segment customers include processors and refiners of edible oils, renewable diesel, petroleum-based oils and biodiesel fuel; manufacturers of animal feed and agricultural chemicals; and distributors of animal health and nutrition products. It is also a supplier of silica gel-based crystal cat litter.</v>
     <v>884</v>
@@ -5556,24 +5614,25 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>SUITE 400, 410 NORTH MICHIGAN AVENUE, CHICAGO, IL, 60611 US</v>
-    <v>69.31</v>
+    <v>69.84</v>
     <v>Chemicals</v>
     <v>Stock</v>
-    <v>45554.958333344533</v>
+    <v>45555.850474733597</v>
     <v>56</v>
-    <v>67.694999999999993</v>
-    <v>494377000</v>
+    <v>68</v>
+    <v>502902000</v>
     <v>OIL-DRI CORPORATION OF AMERICA</v>
     <v>OIL-DRI CORPORATION OF AMERICA</v>
-    <v>69.13</v>
+    <v>68.239999999999995</v>
     <v>14.100099999999999</v>
-    <v>67.849999999999994</v>
     <v>68.709999999999994</v>
+    <v>69.05</v>
+    <v>69.02</v>
     <v>7286320</v>
     <v>ODC</v>
     <v>OIL-DRI CORPORATION OF AMERICA (XNYS:ODC)</v>
-    <v>17825</v>
-    <v>16047</v>
+    <v>49361</v>
+    <v>16177</v>
     <v>1969</v>
   </rv>
   <rv s="2">
@@ -5589,7 +5648,7 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>5</v>
+    <v>4</v>
     <v>en-GB</v>
     <v>a1mt9c</v>
     <v>268435456</v>
@@ -5597,9 +5656,11 @@
     <v>Powered by Refinitiv</v>
     <v>170.9692</v>
     <v>93.77</v>
-    <v>1.5933999999999999</v>
-    <v>4.3899999999999997</v>
-    <v>4.4869000000000006E-2</v>
+    <v>1.5822000000000001</v>
+    <v>-0.94</v>
+    <v>-9.195E-3</v>
+    <v>0.67</v>
+    <v>6.6149999999999994E-3</v>
     <v>USD</v>
     <v>Axcelis Technologies, Inc. designs, manufactures and services ion implantation and other processing equipment used in the fabrication of semiconductor chips. The Company offers a complete line of high energy, high current and medium current implanters for all application requirements. In addition to equipment, the Company provides extensive aftermarket lifecycle products and services, including used tools, spare parts, equipment upgrades, maintenance services and customer training. Its Purion flagship systems are all based on a common platform, which enables a combination of implant purity, precision and productivity. Combining a single wafer end station, with advanced spot beam architectures (that ensures all points across the wafer see the same beam condition at the same beam angle), Purion products enable process control to optimize device performance and yield, at high productivity. The Company sells its products to semiconductor chip manufacturers around the world.</v>
     <v>1620</v>
@@ -5607,24 +5668,25 @@
     <v>XNAS</v>
     <v>XNAS</v>
     <v>108 Cherry Hill Dr, BEVERLY, MA, 01915 US</v>
-    <v>102.99</v>
+    <v>101.87350000000001</v>
     <v>Semiconductors &amp; Semiconductor Equipment</v>
     <v>Stock</v>
-    <v>45554.99339609922</v>
+    <v>45555.992803159374</v>
     <v>59</v>
-    <v>100.07</v>
-    <v>3334496225</v>
+    <v>98.59</v>
+    <v>3303835000</v>
     <v>AXCELIS TECHNOLOGIES, INC.</v>
     <v>AXCELIS TECHNOLOGIES, INC.</v>
-    <v>102.27</v>
-    <v>14.0844</v>
-    <v>97.84</v>
+    <v>100.32</v>
+    <v>13.9549</v>
     <v>102.23</v>
+    <v>101.29</v>
+    <v>101.96</v>
     <v>32617590</v>
     <v>ACLS</v>
     <v>AXCELIS TECHNOLOGIES, INC. (XNAS:ACLS)</v>
-    <v>15</v>
-    <v>521482</v>
+    <v>3094950</v>
+    <v>524505</v>
     <v>1995</v>
   </rv>
   <rv s="2">
@@ -5640,7 +5702,7 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>5</v>
+    <v>4</v>
     <v>en-GB</v>
     <v>a1retc</v>
     <v>268435456</v>
@@ -5648,9 +5710,11 @@
     <v>Powered by Refinitiv</v>
     <v>179.7</v>
     <v>63.9</v>
-    <v>0.89570000000000005</v>
-    <v>1.78</v>
-    <v>1.5346E-2</v>
+    <v>0.89480000000000004</v>
+    <v>-0.27</v>
+    <v>-2.2929999999999999E-3</v>
+    <v>-0.56999999999999995</v>
+    <v>-4.8509999999999994E-3</v>
     <v>USD</v>
     <v>Dell Technologies Inc. is engaged in designing, developing, manufacturing, marketing, selling, and supporting a wide range of comprehensive and integrated solutions, products, and services. The Company operates through two segments: Infrastructure Solutions Group (ISG) and Client Solutions Group (CSG). Its ISG segment enables the Company’s customer’s digital transformation with solutions that address artificial intelligence (AI), machine learning, data analytics, and multi cloud environments. Its comprehensive storage portfolio includes modern and traditional storage solutions, including all-flash arrays, scale-out file, object platforms, hyper-converged infrastructure, and software-defined storage. Its CSG segment offers branded personal computers (PCs) including notebooks, desktops, and workstations and branded peripherals that include displays, docking stations, keyboards, mice, and webcam and audio devices, as well as third-party software and peripherals.</v>
     <v>120000</v>
@@ -5658,24 +5722,25 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>ONE DELL WAY, ROUND ROCK, TX, 78682 US</v>
-    <v>120.07</v>
+    <v>119.05</v>
     <v>Computers, Phones &amp; Household Electronics</v>
     <v>Stock</v>
-    <v>45554.99945133047</v>
+    <v>45555.999838610936</v>
     <v>62</v>
-    <v>117.36</v>
-    <v>82719857896</v>
+    <v>115.08</v>
+    <v>82484580000</v>
     <v>DELL TECHNOLOGIES INC.</v>
     <v>DELL TECHNOLOGIES INC.</v>
-    <v>120.07</v>
-    <v>21.669899999999998</v>
-    <v>115.99</v>
+    <v>116.5</v>
+    <v>21.629899999999999</v>
     <v>117.77</v>
-    <v>702384800</v>
+    <v>117.5</v>
+    <v>116.93</v>
+    <v>701996500</v>
     <v>DELL</v>
     <v>DELL TECHNOLOGIES INC. (XNYS:DELL)</v>
-    <v>8004</v>
-    <v>11347373</v>
+    <v>75332831</v>
+    <v>11286953</v>
     <v>2013</v>
   </rv>
   <rv s="2">
@@ -5685,7 +5750,7 @@
 </file>
 
 <file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
-<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="5">
+<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="4">
   <s t="_hyperlink">
     <k n="Address" t="s"/>
     <k n="Text" t="s"/>
@@ -5707,53 +5772,8 @@
     <k n="Beta"/>
     <k n="Change"/>
     <k n="Change (%)"/>
-    <k n="Currency" t="s"/>
-    <k n="Description" t="s"/>
-    <k n="Employees"/>
-    <k n="Exchange" t="s"/>
-    <k n="Exchange abbreviation" t="s"/>
-    <k n="ExchangeID" t="s"/>
-    <k n="Headquarters" t="s"/>
-    <k n="High"/>
-    <k n="Industry" t="s"/>
-    <k n="Instrument type" t="s"/>
-    <k n="Last trade time"/>
-    <k n="LearnMoreOnLink" t="r"/>
-    <k n="Low"/>
-    <k n="Market cap"/>
-    <k n="Name" t="s"/>
-    <k n="Official name" t="s"/>
-    <k n="Open"/>
-    <k n="P/E"/>
-    <k n="Previous close"/>
-    <k n="Price"/>
-    <k n="Shares outstanding"/>
-    <k n="Ticker symbol" t="s"/>
-    <k n="UniqueName" t="s"/>
-    <k n="Volume"/>
-    <k n="Volume average"/>
-    <k n="Year incorporated"/>
-  </s>
-  <s t="_linkedentity">
-    <k n="%cvi" t="r"/>
-  </s>
-  <s t="_linkedentitycore">
-    <k n="_Display" t="spb"/>
-    <k n="_DisplayString" t="s"/>
-    <k n="_Flags" t="spb"/>
-    <k n="_Format" t="spb"/>
-    <k n="_Icon" t="s"/>
-    <k n="_SubLabel" t="spb"/>
-    <k n="%EntityCulture" t="s"/>
-    <k n="%EntityId" t="s"/>
-    <k n="%EntityServiceId"/>
-    <k n="%IsRefreshable" t="b"/>
-    <k n="%ProviderInfo" t="s"/>
-    <k n="52 week high"/>
-    <k n="52 week low"/>
-    <k n="Beta"/>
-    <k n="Change"/>
-    <k n="Change (%)"/>
+    <k n="Change (Extended hours)"/>
+    <k n="Change % (Extended hours)"/>
     <k n="Currency" t="s"/>
     <k n="Description" t="s"/>
     <k n="Employees"/>
@@ -5782,6 +5802,9 @@
     <k n="Volume average"/>
     <k n="Year incorporated"/>
   </s>
+  <s t="_linkedentity">
+    <k n="%cvi" t="r"/>
+  </s>
   <s t="_linkedentitycore">
     <k n="_Display" t="spb"/>
     <k n="_DisplayString" t="s"/>
@@ -5799,6 +5822,8 @@
     <k n="Beta"/>
     <k n="Change"/>
     <k n="Change (%)"/>
+    <k n="Change (Extended hours)"/>
+    <k n="Change % (Extended hours)"/>
     <k n="Currency" t="s"/>
     <k n="Description" t="s"/>
     <k n="Employees"/>
@@ -5818,6 +5843,7 @@
     <k n="P/E"/>
     <k n="Previous close"/>
     <k n="Price"/>
+    <k n="Price (Extended hours)"/>
     <k n="Shares outstanding"/>
     <k n="Ticker symbol" t="s"/>
     <k n="UniqueName" t="s"/>
@@ -5830,8 +5856,8 @@
 
 <file path=xl/richData/rdsupportingpropertybag.xml><?xml version="1.0" encoding="utf-8"?>
 <supportingPropertyBags xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2">
-  <spbArrays count="3">
-    <a count="42">
+  <spbArrays count="2">
+    <a count="45">
       <v t="s">%EntityServiceId</v>
       <v t="s">_Format</v>
       <v t="s">%IsRefreshable</v>
@@ -5842,13 +5868,16 @@
       <v t="s">Name</v>
       <v t="s">_SubLabel</v>
       <v t="s">Price</v>
+      <v t="s">Price (Extended hours)</v>
       <v t="s">Exchange</v>
       <v t="s">Official name</v>
       <v t="s">Last trade time</v>
       <v t="s">Ticker symbol</v>
       <v t="s">Exchange abbreviation</v>
       <v t="s">Change</v>
+      <v t="s">Change (Extended hours)</v>
       <v t="s">Change (%)</v>
+      <v t="s">Change % (Extended hours)</v>
       <v t="s">Currency</v>
       <v t="s">Previous close</v>
       <v t="s">Open</v>
@@ -5875,7 +5904,7 @@
       <v t="s">ExchangeID</v>
       <v t="s">%ProviderInfo</v>
     </a>
-    <a count="43">
+    <a count="44">
       <v t="s">%EntityServiceId</v>
       <v t="s">_Format</v>
       <v t="s">%IsRefreshable</v>
@@ -5893,51 +5922,9 @@
       <v t="s">Ticker symbol</v>
       <v t="s">Exchange abbreviation</v>
       <v t="s">Change</v>
+      <v t="s">Change (Extended hours)</v>
       <v t="s">Change (%)</v>
-      <v t="s">Currency</v>
-      <v t="s">Previous close</v>
-      <v t="s">Open</v>
-      <v t="s">High</v>
-      <v t="s">Low</v>
-      <v t="s">52 week high</v>
-      <v t="s">52 week low</v>
-      <v t="s">Volume</v>
-      <v t="s">Volume average</v>
-      <v t="s">Market cap</v>
-      <v t="s">Beta</v>
-      <v t="s">P/E</v>
-      <v t="s">Shares outstanding</v>
-      <v t="s">Description</v>
-      <v t="s">Employees</v>
-      <v t="s">Headquarters</v>
-      <v t="s">Industry</v>
-      <v t="s">Instrument type</v>
-      <v t="s">Year incorporated</v>
-      <v t="s">_Flags</v>
-      <v t="s">UniqueName</v>
-      <v t="s">_DisplayString</v>
-      <v t="s">LearnMoreOnLink</v>
-      <v t="s">ExchangeID</v>
-      <v t="s">%ProviderInfo</v>
-    </a>
-    <a count="41">
-      <v t="s">%EntityServiceId</v>
-      <v t="s">_Format</v>
-      <v t="s">%IsRefreshable</v>
-      <v t="s">%EntityCulture</v>
-      <v t="s">%EntityId</v>
-      <v t="s">_Icon</v>
-      <v t="s">_Display</v>
-      <v t="s">Name</v>
-      <v t="s">_SubLabel</v>
-      <v t="s">Price</v>
-      <v t="s">Exchange</v>
-      <v t="s">Official name</v>
-      <v t="s">Last trade time</v>
-      <v t="s">Ticker symbol</v>
-      <v t="s">Exchange abbreviation</v>
-      <v t="s">Change</v>
-      <v t="s">Change (%)</v>
+      <v t="s">Change % (Extended hours)</v>
       <v t="s">Currency</v>
       <v t="s">Previous close</v>
       <v t="s">Open</v>
@@ -5964,7 +5951,7 @@
       <v t="s">%ProviderInfo</v>
     </a>
   </spbArrays>
-  <spbData count="11">
+  <spbData count="8">
     <spb s="0">
       <v>0</v>
       <v>Name</v>
@@ -6002,62 +5989,35 @@
       <v>8</v>
       <v>9</v>
       <v>4</v>
+      <v>1</v>
+      <v>1</v>
+      <v>5</v>
     </spb>
     <spb s="4">
-      <v>Real-Time Nasdaq Last Sale</v>
-      <v>from previous close</v>
-      <v>from previous close</v>
-      <v>Source: Nasdaq Last Sale</v>
-      <v>GMT</v>
-    </spb>
-    <spb s="4">
-      <v>Delayed 15 minutes</v>
-      <v>from previous close</v>
-      <v>from previous close</v>
-      <v>Source: Nasdaq</v>
-      <v>GMT</v>
-    </spb>
-    <spb s="0">
-      <v>1</v>
-      <v>Name</v>
-      <v>LearnMoreOnLink</v>
-    </spb>
-    <spb s="5">
-      <v>1</v>
-      <v>2</v>
-      <v>2</v>
-      <v>1</v>
-      <v>3</v>
-      <v>1</v>
-      <v>1</v>
-      <v>1</v>
-      <v>4</v>
-      <v>4</v>
-      <v>5</v>
-      <v>6</v>
-      <v>1</v>
-      <v>1</v>
-      <v>1</v>
-      <v>4</v>
-      <v>7</v>
-      <v>8</v>
-      <v>9</v>
-      <v>4</v>
-      <v>1</v>
-    </spb>
-    <spb s="6">
       <v>at close</v>
       <v>from previous close</v>
       <v>from previous close</v>
       <v>Source: Nasdaq</v>
       <v>GMT</v>
       <v>Delayed 15 minutes</v>
+      <v>from close</v>
+      <v>from close</v>
     </spb>
-    <spb s="7">
-      <v>2</v>
+    <spb s="4">
+      <v>at close</v>
+      <v>from previous close</v>
+      <v>from previous close</v>
+      <v>Source: Nasdaq Last Sale</v>
+      <v>GMT</v>
+      <v>Real-Time Nasdaq Last Sale</v>
+      <v>from close</v>
+      <v>from close</v>
+    </spb>
+    <spb s="5">
+      <v>1</v>
       <v>Name</v>
     </spb>
-    <spb s="8">
+    <spb s="6">
       <v>1</v>
       <v>1</v>
       <v>1</v>
@@ -6067,7 +6027,7 @@
 </file>
 
 <file path=xl/richData/rdsupportingpropertybagstructure.xml><?xml version="1.0" encoding="utf-8"?>
-<spbStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" count="9">
+<spbStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" count="7">
   <s>
     <k n="^Order" t="spba"/>
     <k n="TitleProperty" t="s"/>
@@ -6105,36 +6065,9 @@
     <k n="Year incorporated" t="i"/>
     <k n="`%EntityServiceId" t="i"/>
     <k n="Shares outstanding" t="i"/>
-  </s>
-  <s>
-    <k n="Price" t="s"/>
-    <k n="Change" t="s"/>
-    <k n="Change (%)" t="s"/>
-    <k n="ExchangeID" t="s"/>
-    <k n="Last trade time" t="s"/>
-  </s>
-  <s>
-    <k n="Low" t="i"/>
-    <k n="P/E" t="i"/>
-    <k n="Beta" t="i"/>
-    <k n="High" t="i"/>
-    <k n="Name" t="i"/>
-    <k n="Open" t="i"/>
-    <k n="Price" t="i"/>
-    <k n="Change" t="i"/>
-    <k n="Volume" t="i"/>
-    <k n="Employees" t="i"/>
-    <k n="Change (%)" t="i"/>
-    <k n="Market cap" t="i"/>
-    <k n="52 week low" t="i"/>
-    <k n="52 week high" t="i"/>
-    <k n="Previous close" t="i"/>
-    <k n="Volume average" t="i"/>
-    <k n="Last trade time" t="i"/>
-    <k n="Year incorporated" t="i"/>
-    <k n="`%EntityServiceId" t="i"/>
-    <k n="Shares outstanding" t="i"/>
     <k n="Price (Extended hours)" t="i"/>
+    <k n="Change (Extended hours)" t="i"/>
+    <k n="Change % (Extended hours)" t="i"/>
   </s>
   <s>
     <k n="Price" t="s"/>
@@ -6143,6 +6076,8 @@
     <k n="ExchangeID" t="s"/>
     <k n="Last trade time" t="s"/>
     <k n="Price (Extended hours)" t="s"/>
+    <k n="Change (Extended hours)" t="s"/>
+    <k n="Change % (Extended hours)" t="s"/>
   </s>
   <s>
     <k n="^Order" t="spba"/>
@@ -69646,15 +69581,15 @@
       </c>
       <c r="I3" s="151" cm="1">
         <f t="array" aca="1" ref="I3" ca="1">_FV(B3,"Price")</f>
-        <v>58.4</v>
+        <v>57.51</v>
       </c>
       <c r="J3" s="131">
         <f t="shared" ref="J3:J24" ca="1" si="0">((I3-F3)/F3)</f>
-        <v>-0.15054545454545457</v>
+        <v>-0.16349090909090913</v>
       </c>
       <c r="K3" s="172">
         <f t="shared" ref="K3:K24" ca="1" si="1">(I3*G3) - H3</f>
-        <v>-75.450879999999984</v>
+        <v>-81.936131999999986</v>
       </c>
       <c r="L3"/>
     </row>
@@ -69685,15 +69620,15 @@
       </c>
       <c r="I4" s="151" cm="1">
         <f t="array" aca="1" ref="I4" ca="1">_FV(B4,"Price")</f>
-        <v>137.91999999999999</v>
+        <v>139.05000000000001</v>
       </c>
       <c r="J4" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>0.37892421515696856</v>
+        <v>0.3902219556088784</v>
       </c>
       <c r="K4" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>189.84127999999998</v>
+        <v>195.50145000000009</v>
       </c>
       <c r="L4"/>
     </row>
@@ -69724,15 +69659,15 @@
       </c>
       <c r="I5" s="151" cm="1">
         <f t="array" aca="1" ref="I5" ca="1">_FV(B5,"Price")</f>
-        <v>19.97</v>
+        <v>19.38</v>
       </c>
       <c r="J5" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>-8.3944954128440455E-2</v>
+        <v>-0.11100917431192668</v>
       </c>
       <c r="K5" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>-42.105376000000035</v>
+        <v>-55.663104000000033</v>
       </c>
       <c r="L5"/>
     </row>
@@ -69763,15 +69698,15 @@
       </c>
       <c r="I6" s="151" cm="1">
         <f t="array" aca="1" ref="I6" ca="1">_FV(B6,"Price")</f>
-        <v>22.35</v>
+        <v>22.23</v>
       </c>
       <c r="J6" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>0.27714285714285725</v>
+        <v>0.2702857142857143</v>
       </c>
       <c r="K6" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>152.88054</v>
+        <v>149.36977200000001</v>
       </c>
       <c r="L6"/>
     </row>
@@ -69802,15 +69737,15 @@
       </c>
       <c r="I7" s="153" cm="1">
         <f t="array" aca="1" ref="I7" ca="1">_FV(B7,"Price")</f>
-        <v>228.87</v>
+        <v>228.2</v>
       </c>
       <c r="J7" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>0.29700782046922813</v>
+        <v>0.29321092598889253</v>
       </c>
       <c r="K7" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>148.80481700000007</v>
+        <v>146.90261999999996</v>
       </c>
       <c r="L7"/>
     </row>
@@ -69841,15 +69776,15 @@
       </c>
       <c r="I8" s="153" cm="1">
         <f t="array" aca="1" ref="I8" ca="1">_FV(B8,"Price")</f>
-        <v>90.99</v>
+        <v>91.06</v>
       </c>
       <c r="J8" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>0.62076950480940496</v>
+        <v>0.6220163876024225</v>
       </c>
       <c r="K8" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>310.94016600000009</v>
+        <v>311.56480400000009</v>
       </c>
       <c r="L8"/>
     </row>
@@ -69880,15 +69815,15 @@
       </c>
       <c r="I9" s="153" cm="1">
         <f t="array" aca="1" ref="I9" ca="1">_FV(B9,"Price")</f>
-        <v>19.690000000000001</v>
+        <v>19.350000000000001</v>
       </c>
       <c r="J9" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.4136390708755211</v>
+        <v>-0.42376414532459789</v>
       </c>
       <c r="K9" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>-207.20747899999998</v>
+        <v>-212.28058499999997</v>
       </c>
       <c r="L9"/>
     </row>
@@ -69919,15 +69854,15 @@
       </c>
       <c r="I10" s="155" cm="1">
         <f t="array" aca="1" ref="I10" ca="1">_FV(B10,"Price")</f>
-        <v>62.43</v>
+        <v>61.8</v>
       </c>
       <c r="J10" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>7.2680412371133957E-2</v>
+        <v>6.1855670103092682E-2</v>
       </c>
       <c r="K10" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>36.434897999999976</v>
+        <v>31.011479999999892</v>
       </c>
       <c r="L10"/>
     </row>
@@ -69958,15 +69893,15 @@
       </c>
       <c r="I11" s="155" cm="1">
         <f t="array" aca="1" ref="I11" ca="1">_FV(B11,"Price")</f>
-        <v>85.86</v>
+        <v>84.3</v>
       </c>
       <c r="J11" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>-5.9274679522296446E-2</v>
+        <v>-7.6366823709871801E-2</v>
       </c>
       <c r="K11" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>-29.714460000000031</v>
+        <v>-38.277300000000025</v>
       </c>
       <c r="L11"/>
     </row>
@@ -69997,15 +69932,15 @@
       </c>
       <c r="I12" s="155" cm="1">
         <f t="array" aca="1" ref="I12" ca="1">_FV(B12,"Price")</f>
-        <v>97.7</v>
+        <v>97.33</v>
       </c>
       <c r="J12" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>0.16726403823178015</v>
+        <v>0.16284348864994019</v>
       </c>
       <c r="K12" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>83.783350000000041</v>
+        <v>81.568714999999997</v>
       </c>
       <c r="L12"/>
     </row>
@@ -70036,15 +69971,15 @@
       </c>
       <c r="I13" s="155" cm="1">
         <f t="array" aca="1" ref="I13" ca="1">_FV(B13,"Price")</f>
-        <v>95.83</v>
+        <v>94.74</v>
       </c>
       <c r="J13" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.18073010173548773</v>
+        <v>-0.19004873044370355</v>
       </c>
       <c r="K13" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>-90.550526999999988</v>
+        <v>-95.219106000000011</v>
       </c>
       <c r="L13"/>
     </row>
@@ -70075,15 +70010,15 @@
       </c>
       <c r="I14" s="157" cm="1">
         <f t="array" aca="1" ref="I14" ca="1">_FV(B14,"Price")</f>
-        <v>27.31</v>
+        <v>26.58</v>
       </c>
       <c r="J14" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>7.1400549234994129E-2</v>
+        <v>4.276186739897999E-2</v>
       </c>
       <c r="K14" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>35.805359999999951</v>
+        <v>21.456479999999942</v>
       </c>
       <c r="L14"/>
     </row>
@@ -70114,15 +70049,15 @@
       </c>
       <c r="I15" s="157" cm="1">
         <f t="array" aca="1" ref="I15" ca="1">_FV(B15,"Price")</f>
-        <v>13.15</v>
+        <v>13.14</v>
       </c>
       <c r="J15" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>0.49942987457240606</v>
+        <v>0.49828962371721791</v>
       </c>
       <c r="K15" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>249.99781500000006</v>
+        <v>249.42671400000006</v>
       </c>
       <c r="L15"/>
     </row>
@@ -70153,15 +70088,15 @@
       </c>
       <c r="I16" s="159" cm="1">
         <f t="array" aca="1" ref="I16" ca="1">_FV(B16,"Price")</f>
-        <v>36.46</v>
+        <v>36.659999999999997</v>
       </c>
       <c r="J16" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.24855729596042872</v>
+        <v>-0.2444352844187965</v>
       </c>
       <c r="K16" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>-120.54999999999995</v>
+        <v>-118.55000000000001</v>
       </c>
       <c r="L16"/>
     </row>
@@ -70192,15 +70127,15 @@
       </c>
       <c r="I17" s="159" cm="1">
         <f t="array" aca="1" ref="I17" ca="1">_FV(B17,"Price")</f>
-        <v>76.650000000000006</v>
+        <v>76.260000000000005</v>
       </c>
       <c r="J17" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>9.5782701929950004E-2</v>
+        <v>9.0207290922087235E-2</v>
       </c>
       <c r="K17" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>46.910000000000082</v>
+        <v>44.180000000000064</v>
       </c>
       <c r="L17"/>
     </row>
@@ -70231,15 +70166,15 @@
       </c>
       <c r="I18" s="159" cm="1">
         <f t="array" aca="1" ref="I18" ca="1">_FV(B18,"Price")</f>
-        <v>61.5</v>
+        <v>61.69</v>
       </c>
       <c r="J18" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.0935992280476033E-2</v>
+        <v>-7.8803473785783538E-3</v>
       </c>
       <c r="K18" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>-5.4399999999999977</v>
+        <v>-3.9200000000000159</v>
       </c>
       <c r="L18"/>
     </row>
@@ -70270,15 +70205,15 @@
       </c>
       <c r="I19" s="159" cm="1">
         <f t="array" aca="1" ref="I19" ca="1">_FV(B19,"Price")</f>
-        <v>10.119999999999999</v>
+        <v>10.1</v>
       </c>
       <c r="J19" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.24477611940298516</v>
+        <v>-0.24626865671641796</v>
       </c>
       <c r="K19" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>-122.68403999999998</v>
+        <v>-123.43169999999998</v>
       </c>
       <c r="L19"/>
     </row>
@@ -70309,15 +70244,15 @@
       </c>
       <c r="I20" s="213" cm="1">
         <f t="array" aca="1" ref="I20" ca="1">_FV(B20,"Price")</f>
-        <v>403.29</v>
+        <v>402.01</v>
       </c>
       <c r="J20" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>2.513980681240479E-2</v>
+        <v>2.1886120996441317E-2</v>
       </c>
       <c r="K20" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>12.651200000000074</v>
+        <v>11.012800000000027</v>
       </c>
       <c r="L20"/>
     </row>
@@ -70348,15 +70283,15 @@
       </c>
       <c r="I21" s="216" cm="1">
         <f t="array" aca="1" ref="I21" ca="1">_FV(B21,"Price")</f>
-        <v>21.93</v>
+        <v>21.67</v>
       </c>
       <c r="J21" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.482479784366585E-2</v>
+        <v>-2.6504941599281212E-2</v>
       </c>
       <c r="K21" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>-7.4324550000000045</v>
+        <v>-13.284144999999967</v>
       </c>
     </row>
     <row r="22" spans="2:12">
@@ -70386,15 +70321,15 @@
       </c>
       <c r="I22" s="216" cm="1">
         <f t="array" aca="1" ref="I22" ca="1">_FV(B22,"Price")</f>
-        <v>68.709999999999994</v>
+        <v>69.05</v>
       </c>
       <c r="J22" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.3354394026421695E-2</v>
+        <v>-8.4721424468696648E-3</v>
       </c>
       <c r="K22" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>-5.2679630000000657</v>
+        <v>-2.8149650000000292</v>
       </c>
     </row>
     <row r="23" spans="2:12">
@@ -70424,15 +70359,15 @@
       </c>
       <c r="I23" s="216" cm="1">
         <f t="array" aca="1" ref="I23" ca="1">_FV(B23,"Price")</f>
-        <v>102.23</v>
+        <v>101.29</v>
       </c>
       <c r="J23" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>1.0877088895481149E-2</v>
+        <v>1.5821220211609888E-3</v>
       </c>
       <c r="K23" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>5.4676430000000664</v>
+        <v>0.8107890000000566</v>
       </c>
     </row>
     <row r="24" spans="2:12">
@@ -70462,21 +70397,21 @@
       </c>
       <c r="I24" s="216" cm="1">
         <f t="array" aca="1" ref="I24" ca="1">_FV(B24,"Price")</f>
-        <v>117.77</v>
+        <v>117.5</v>
       </c>
       <c r="J24" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>-3.4692841428330579E-3</v>
+        <v>-5.7539346759181483E-3</v>
       </c>
       <c r="K24" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>-1.7258620000000633</v>
+        <v>-2.8704999999999927</v>
       </c>
     </row>
     <row r="26" spans="2:12" ht="13">
       <c r="K26" s="171">
         <f ca="1">SUM(K3:K24)</f>
-        <v>565.38802700000042</v>
+        <v>494.55808700000017</v>
       </c>
     </row>
   </sheetData>
@@ -70862,7 +70797,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C17" sqref="C17"/>
+      <selection pane="bottomRight" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="24" customHeight="1"/>

</xml_diff>

<commit_message>
vault backup: 2024-09-26 10:34:45
</commit_message>
<xml_diff>
--- a/_system/Attachments/Portfolio Management.xlsx
+++ b/_system/Attachments/Portfolio Management.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martin/repos/tomesink/obsidian/_system/Attachments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{549939C1-0008-4E43-95DA-4B14F967A023}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FDBA237-E197-6847-86AF-7A92E8D91CA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3300" yWindow="980" windowWidth="33800" windowHeight="18860" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3300" yWindow="980" windowWidth="33800" windowHeight="18860" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Stocks Performance" sheetId="1" r:id="rId1"/>
@@ -4581,11 +4581,9 @@
     <v>Powered by Refinitiv</v>
     <v>83.25</v>
     <v>52.770499999999998</v>
-    <v>0.52759999999999996</v>
-    <v>-0.89</v>
-    <v>-1.524E-2</v>
-    <v>0.01</v>
-    <v>1.739E-4</v>
+    <v>0.52790000000000004</v>
+    <v>0.56000000000000005</v>
+    <v>9.6419999999999995E-3</v>
     <v>USD</v>
     <v>CVS Health Corporation is a health solutions company. The Company operates in four segments: Health Care Benefits, Health Services, Pharmacy &amp; Consumer Wellness, and Corporate/Other. Its Health Care Benefits segment offer a range of traditional, voluntary and consumer-directed health insurance products and related services, including medical, pharmacy, dental and behavioral health plans, medical management capabilities, Medicare Advantage and Medicare supplement plans, and Medicaid health care management services. Its Health Services segment provides a full range of pharmacy benefit management solutions, delivers health care services in its medical clinics, virtually, and in the home, and offers provider enablement solutions. The Pharmacy &amp; Consumer Wellness segment dispenses prescriptions in its retail pharmacies and through its infusion operations, provides ancillary pharmacy services, including pharmacy patient care programs, diagnostic testing and vaccination administration.</v>
     <v>300000</v>
@@ -4593,25 +4591,24 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>1 Cvs Dr, WOONSOCKET, RI, 02895-6146 US</v>
-    <v>58.08</v>
+    <v>59.33</v>
     <v>Healthcare Providers &amp; Services</v>
     <v>Stock</v>
-    <v>45555.999544455466</v>
+    <v>45560.99967543906</v>
     <v>0</v>
-    <v>57.13</v>
-    <v>72346390000</v>
+    <v>58.32</v>
+    <v>73767888560</v>
     <v>CVS HEALTH CORPORATION</v>
     <v>CVS HEALTH CORPORATION</v>
-    <v>58</v>
-    <v>10.2342</v>
-    <v>58.4</v>
-    <v>57.51</v>
-    <v>57.52</v>
+    <v>58.82</v>
+    <v>10.4353</v>
+    <v>58.08</v>
+    <v>58.64</v>
     <v>1257979000</v>
     <v>CVS</v>
     <v>CVS HEALTH CORPORATION (XNYS:CVS)</v>
-    <v>10239966</v>
-    <v>7552236</v>
+    <v>131</v>
+    <v>7652552</v>
     <v>1996</v>
   </rv>
   <rv s="2">
@@ -4627,7 +4624,7 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>4</v>
+    <v>5</v>
     <v>en-GB</v>
     <v>a1qclh</v>
     <v>268435456</v>
@@ -4635,11 +4632,9 @@
     <v>Powered by Refinitiv</v>
     <v>165.32</v>
     <v>74</v>
-    <v>1.9970000000000001</v>
-    <v>1.1299999999999999</v>
-    <v>8.1930000000000006E-3</v>
-    <v>-0.52</v>
-    <v>-3.7399999999999998E-3</v>
+    <v>1.9946999999999999</v>
+    <v>-1.79</v>
+    <v>-1.2359E-2</v>
     <v>USD</v>
     <v>Crocs, Inc. is engaged in the design, development, worldwide marketing, distribution, and sale of casual lifestyle footwear and accessories for women, men, and children. The Company’s segments include Crocs Brand and the HEYDUDE Brand. The Company’s Crocs Brand collection contains Croslite material, a molded footwear technology, delivering extraordinary comfort with each step. Its Croslite materials are formulated to create soft, comfortable, lightweight, non-marking, and odor-resistant footwear. The HEYDUDE Brand offers shoes with a versatile silhouette. It sells its products in more than 80 countries, through two distribution channels: wholesale and direct-to-consumer. Its wholesale channel includes domestic and international multi-brand retailers, mono-branded partner stores, e-tailers, and distributors; its direct-to-consumer channel includes Company-operated retail stores, Company-operated e-commerce sites, and third-party marketplaces.</v>
     <v>7030</v>
@@ -4647,25 +4642,24 @@
     <v>XNAS</v>
     <v>XNAS</v>
     <v>500 Eldorado Boulevard, Building 5, BROOMFIELD, CO, 80021 US</v>
-    <v>140.34</v>
+    <v>146.44999999999999</v>
     <v>Textiles &amp; Apparel</v>
     <v>Stock</v>
-    <v>45555.99378098359</v>
+    <v>45560.995847939063</v>
     <v>3</v>
-    <v>137.63499999999999</v>
-    <v>8257503000</v>
+    <v>141.81</v>
+    <v>8494448995</v>
     <v>CROCS, INC.</v>
     <v>CROCS, INC.</v>
-    <v>138.16</v>
-    <v>10.457599999999999</v>
-    <v>137.91999999999999</v>
-    <v>139.05000000000001</v>
-    <v>138.53</v>
+    <v>145.36000000000001</v>
+    <v>10.7577</v>
+    <v>144.83000000000001</v>
+    <v>143.04</v>
     <v>59385130</v>
     <v>CROX</v>
     <v>CROCS, INC. (XNAS:CROX)</v>
-    <v>1491867</v>
-    <v>946750</v>
+    <v>116</v>
+    <v>989539</v>
     <v>2005</v>
   </rv>
   <rv s="2">
@@ -4681,7 +4675,7 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>4</v>
+    <v>5</v>
     <v>en-GB</v>
     <v>a25yfr</v>
     <v>268435456</v>
@@ -4689,11 +4683,9 @@
     <v>Powered by Refinitiv</v>
     <v>30.07</v>
     <v>17.71</v>
-    <v>1.5177</v>
-    <v>-0.59</v>
-    <v>-2.9544000000000001E-2</v>
-    <v>-5.0000000000000001E-4</v>
-    <v>-2.5799999999999997E-5</v>
+    <v>1.5168999999999999</v>
+    <v>-0.46</v>
+    <v>-2.4146999999999998E-2</v>
     <v>USD</v>
     <v>Wabash National Corporation provides connected solutions for the transportation, logistics and distribution industries. The Company designs and manufactures products including dry freight and refrigerated trailers, platform trailers, tank trailers, dry and refrigerated truck bodies, structural composite panels and products, transportation, logistics, and distribution industry parts and services, and specialty food grade processing equipment. The Company’s Transportation Solutions (TS) segment comprises the design and manufacturing operations for the Company’s transportation-related equipment and products. This includes dry and refrigerated van trailers, platform trailers, tank trailers and truck-mounted tanks, truck-mounted dry and refrigerated truck bodies and EcoNex technology products. Its Parts &amp; Services (P&amp;S) segment is comprised of the Company’s parts and services businesses as well as the upfitting component of truck bodies business. It also includes DuraPlate composite panels.</v>
     <v>6700</v>
@@ -4701,25 +4693,24 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>3900 Mccarty Lane, LAFAYETTE, IN, 47905 US</v>
-    <v>19.760000000000002</v>
+    <v>19.100000000000001</v>
     <v>Machinery, Equipment &amp; Components</v>
     <v>Stock</v>
-    <v>45555.958333333336</v>
+    <v>45560.958333333336</v>
     <v>6</v>
-    <v>19.190000000000001</v>
-    <v>852705100</v>
+    <v>18.46</v>
+    <v>817945685</v>
     <v>WABASH NATIONAL CORPORATION</v>
     <v>WABASH NATIONAL CORPORATION</v>
-    <v>19.73</v>
-    <v>5.9450000000000003</v>
-    <v>19.97</v>
-    <v>19.38</v>
-    <v>19.3795</v>
+    <v>19.079999999999998</v>
+    <v>5.7026000000000003</v>
+    <v>19.05</v>
+    <v>18.59</v>
     <v>43999230</v>
     <v>WNC</v>
     <v>WABASH NATIONAL CORPORATION (XNYS:WNC)</v>
-    <v>3587244</v>
-    <v>423715</v>
+    <v>731224</v>
+    <v>568548</v>
     <v>1991</v>
   </rv>
   <rv s="2">
@@ -4735,7 +4726,7 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>4</v>
+    <v>5</v>
     <v>en-GB</v>
     <v>a1pfoc</v>
     <v>268435456</v>
@@ -4743,11 +4734,9 @@
     <v>Powered by Refinitiv</v>
     <v>26.4</v>
     <v>16.12</v>
-    <v>1.0349999999999999</v>
-    <v>-0.12</v>
-    <v>-5.3690000000000005E-3</v>
-    <v>0</v>
-    <v>0</v>
+    <v>1.0347</v>
+    <v>-0.08</v>
+    <v>-3.6380000000000002E-3</v>
     <v>USD</v>
     <v>Perdoceo Education Corporation, through its academic institutions, offers quality postsecondary education primarily online to a diverse student population, along with campus-based and blended learning programs. The Company's academic institutions include Colorado Technical University (CTU) and the American InterContinental University System (AIUS), which provides degree programs from the associate through doctoral level as well as non-degree seeking and professional development programs. Its academic institutions offer students industry-relevant and career-focused academic programs. CTU offers academic programs in the career-oriented disciplines of business and management, nursing, healthcare management, computer science, engineering, information systems and technology, project management, cybersecurity and criminal justice. AIUS offers academic programs in the career-oriented disciplines of business studies, information technologies, education, health sciences and criminal justice.</v>
     <v>2319</v>
@@ -4755,25 +4744,24 @@
     <v>XNAS</v>
     <v>XNAS</v>
     <v>1750 E. GOLF ROAD, SCHAUMBURG, IL, 60173 US</v>
-    <v>22.64</v>
+    <v>22.245000000000001</v>
     <v>Miscellaneous Educational Service Providers</v>
     <v>Stock</v>
-    <v>45555.90269422422</v>
+    <v>45560.879044455469</v>
     <v>9</v>
-    <v>22.01</v>
-    <v>1459920000</v>
+    <v>21.79</v>
+    <v>1438904851</v>
     <v>PERDOCEO EDUCATION CORPORATION</v>
     <v>PERDOCEO EDUCATION CORPORATION</v>
-    <v>22.2</v>
-    <v>10.924899999999999</v>
-    <v>22.35</v>
-    <v>22.23</v>
-    <v>22.23</v>
+    <v>22.06</v>
+    <v>10.7677</v>
+    <v>21.99</v>
+    <v>21.91</v>
     <v>65673430</v>
     <v>PRDO</v>
     <v>PERDOCEO EDUCATION CORPORATION (XNAS:PRDO)</v>
-    <v>2494424</v>
-    <v>386595</v>
+    <v>304010</v>
+    <v>482038</v>
     <v>1994</v>
   </rv>
   <rv s="2">
@@ -4797,11 +4785,9 @@
     <v>Powered by Refinitiv</v>
     <v>237.23</v>
     <v>164.07499999999999</v>
-    <v>1.2405999999999999</v>
-    <v>-0.67</v>
-    <v>-2.9270000000000003E-3</v>
-    <v>-0.43359999999999999</v>
-    <v>-1.9E-3</v>
+    <v>1.2396</v>
+    <v>-1</v>
+    <v>-4.398E-3</v>
     <v>USD</v>
     <v>Apple Inc. designs, manufactures and markets smartphones, personal computers, tablets, wearables and accessories, and sells a variety of related services. Its product categories include iPhone, Mac, iPad, and Wearables, Home and Accessories. Its software platforms include iOS, iPadOS, macOS, watchOS, and tvOS. Its services include advertising, AppleCare, cloud services, digital content and payment services. It operates various platforms, including the App Store, that allow customers to discover and download applications and digital content, such as books, music, video, games and podcasts. It also offers digital content through subscription-based services, including Apple Arcade, Apple Fitness+, Apple Music, Apple News+ and Apple TV+. Its products include iPhone 15 Pro, iPhone 15, iPhone 14, iPhone 13, MacBook Air, MacBook Pro, iMac, Mac mini, Mac Studio, Mac Pro, and others. It also provides DarwinAI, which specializes in visual quality inspection using its Explainable AI platform.</v>
     <v>161000</v>
@@ -4809,25 +4795,24 @@
     <v>XNAS</v>
     <v>XNAS</v>
     <v>One Apple Park Way, CUPERTINO, CA, 95014 US</v>
-    <v>233.09</v>
+    <v>227.29</v>
     <v>Computers, Phones &amp; Household Electronics</v>
     <v>Stock</v>
-    <v>45555.999911909377</v>
+    <v>45560.999899212497</v>
     <v>12</v>
-    <v>227.62</v>
-    <v>3469584000000</v>
+    <v>224.02</v>
+    <v>3441761171800</v>
     <v>APPLE INC.</v>
     <v>APPLE INC.</v>
-    <v>229.97</v>
-    <v>34.744700000000002</v>
-    <v>228.87</v>
-    <v>228.2</v>
-    <v>227.7664</v>
+    <v>224.93</v>
+    <v>34.466099999999997</v>
+    <v>227.37</v>
+    <v>226.37</v>
     <v>15204140000</v>
     <v>AAPL</v>
     <v>APPLE INC. (XNAS:AAPL)</v>
-    <v>318679888</v>
-    <v>45464410</v>
+    <v>48420</v>
+    <v>56862007</v>
     <v>1977</v>
   </rv>
   <rv s="2">
@@ -4843,19 +4828,17 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>4</v>
+    <v>5</v>
     <v>en-GB</v>
     <v>a1ncgh</v>
     <v>268435456</v>
     <v>1</v>
     <v>Powered by Refinitiv</v>
-    <v>92.82</v>
+    <v>93.44</v>
     <v>50.134999999999998</v>
-    <v>0.98839999999999995</v>
-    <v>7.0000000000000007E-2</v>
-    <v>7.693E-4</v>
-    <v>-0.32</v>
-    <v>-3.5139999999999998E-3</v>
+    <v>0.98760000000000003</v>
+    <v>0.2</v>
+    <v>2.1510000000000001E-3</v>
     <v>USD</v>
     <v>Allison Transmission Holdings, Inc. is a designer and manufacturer of propulsion solutions for commercial and defense vehicles. The Company is also a manufacturer of medium-and heavy-duty fully automatic transmissions. Its products are used in a variety of applications, including on-highway trucks, including distribution, refuse, construction, fire and emergency; buses, including school, transit and coach; motorhomes, off-highway vehicles, and equipment, including energy, mining and construction applications; and defense vehicles, including tactical wheeled and tracked. The Company operates in approximately 150 countries. The Company has manufacturing facilities in the United States, Hungary and India, as well as global engineering resources, including electrification engineering centers in Indianapolis, Indiana, Auburn Hills, Michigan and London in the United Kingdom. The Company also has approximately 1,600 independent distributor and dealer locations worldwide.</v>
     <v>3700</v>
@@ -4863,25 +4846,24 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>One Allison Way, INDIANAPOLIS, IN, 46222 US</v>
-    <v>91.32</v>
+    <v>93.44</v>
     <v>Machinery, Equipment &amp; Components</v>
     <v>Stock</v>
-    <v>45555.97244203672</v>
+    <v>45560.996451700783</v>
     <v>15</v>
-    <v>89.15</v>
-    <v>7934775000</v>
+    <v>92.35</v>
+    <v>8119507658</v>
     <v>ALLISON TRANSMISSION HOLDINGS, INC.</v>
     <v>ALLISON TRANSMISSION HOLDINGS, INC.</v>
-    <v>90.42</v>
-    <v>11.907</v>
-    <v>90.99</v>
-    <v>91.06</v>
-    <v>90.74</v>
+    <v>93.29</v>
+    <v>12.1843</v>
+    <v>92.98</v>
+    <v>93.18</v>
     <v>87137880</v>
     <v>ALSN</v>
     <v>ALLISON TRANSMISSION HOLDINGS, INC. (XNYS:ALSN)</v>
-    <v>1483495</v>
-    <v>489823</v>
+    <v>553433</v>
+    <v>545628</v>
     <v>2007</v>
   </rv>
   <rv s="2">
@@ -4897,19 +4879,17 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>4</v>
+    <v>5</v>
     <v>en-GB</v>
     <v>az23tc</v>
     <v>268435456</v>
     <v>1</v>
     <v>Powered by Refinitiv</v>
     <v>40.695</v>
-    <v>18</v>
-    <v>1.9927999999999999</v>
-    <v>-0.34</v>
-    <v>-1.7267999999999999E-2</v>
-    <v>-7.0000000000000007E-2</v>
-    <v>-3.6180000000000001E-3</v>
+    <v>17.28</v>
+    <v>1.9867999999999999</v>
+    <v>-0.94</v>
+    <v>-5.1562999999999998E-2</v>
     <v>USD</v>
     <v>Par Pacific Holdings, Inc. is an energy company, which provides both renewable and conventional fuels to the western United States. It owns and operates 125,000 barrels per day of combined refining capacity across three locations and an energy infrastructure network, including 7.6 million barrels of storage, and marine, rail, rack and pipeline assets. The Company has three segments. Refining segment owns and operates four refineries with total operating crude oil throughput capacity of 219 thousand barrels per day (Mbpd). Retail segment operates fuel retail outlets in Hawaii, Washington and Idaho. It operates convenience stores and fuel retail sites under Hele and nomnom brands, 76 branded fuel retail sites and other sites operated by third parties that sell gasoline, diesel, and retail merchandise, such as soft drinks, prepared foods, and other sundries. Logistics segment operates a multi-modal logistics network spanning the Pacific, the Northwest, and the Rocky Mountain regions.</v>
     <v>1814</v>
@@ -4917,25 +4897,24 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>825 Town and Country Ln Ste 1500, HOUSTON, TX, 77024-2235 US</v>
-    <v>19.555</v>
+    <v>18.260000000000002</v>
     <v>Oil &amp; Gas</v>
     <v>Stock</v>
-    <v>45555.958333356248</v>
+    <v>45560.984654571097</v>
     <v>18</v>
-    <v>18.440000000000001</v>
-    <v>1090002000</v>
+    <v>17.28</v>
+    <v>973960742</v>
     <v>PAR PACIFIC HOLDINGS, INC.</v>
     <v>PAR PACIFIC HOLDINGS, INC.</v>
-    <v>19.16</v>
-    <v>3.3714</v>
-    <v>19.690000000000001</v>
-    <v>19.350000000000001</v>
-    <v>19.28</v>
+    <v>18.21</v>
+    <v>3.0124</v>
+    <v>18.23</v>
+    <v>17.29</v>
     <v>56330870</v>
     <v>PARR</v>
     <v>PAR PACIFIC HOLDINGS, INC. (XNYS:PARR)</v>
-    <v>5755229</v>
-    <v>903736</v>
+    <v>88</v>
+    <v>1136885</v>
     <v>2005</v>
   </rv>
   <rv s="2">
@@ -4951,7 +4930,7 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>4</v>
+    <v>5</v>
     <v>en-GB</v>
     <v>a1v177</v>
     <v>268435456</v>
@@ -4959,11 +4938,9 @@
     <v>Powered by Refinitiv</v>
     <v>84.44</v>
     <v>38.5</v>
-    <v>1.3077000000000001</v>
-    <v>-0.63</v>
-    <v>-1.0091000000000001E-2</v>
-    <v>0</v>
-    <v>0</v>
+    <v>1.3067</v>
+    <v>-1.1000000000000001</v>
+    <v>-1.7710999999999998E-2</v>
     <v>USD</v>
     <v>Hyster-Yale, Inc., formerly Hyster-Yale Materials Handling, Inc., through its wholly owned operating subsidiary, Hyster-Yale Materials Handling, designs, engineers, manufactures, sells, and services a comprehensive line of lift trucks, attachments, aftermarket parts and technology solutions marketed globally primarily under the Hyster and Yale brand names. The Company's business segments include Lift Trucks, Attachments and Fuel Cells. The Hyster-Yale Maximal brand provides trucks for customers requiring fundamental lift truck performance. The Lift Truck segment is focused on fuel cell-powered battery box replacements and integrated fuel cell engine solutions. Hyster- Yale’s attachment subsidiary, Bolzoni S.p.A., is a producer of attachments, forks, and lift tables under the Bolzoni, Auramo and Meyer brand names. The Fuel Cell business, Nuvera Fuel Cells, is an alternative-power technology company focused on fuel cell stacks and engines.</v>
     <v>8600</v>
@@ -4971,25 +4948,24 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>5875 LANDERBROOK DRIVE, SUITE 300, CLEVELAND, OH, 44124 US</v>
-    <v>62.47</v>
+    <v>62.45</v>
     <v>Machinery, Equipment &amp; Components</v>
     <v>Stock</v>
-    <v>45555.958333378905</v>
+    <v>45560.958333378905</v>
     <v>21</v>
-    <v>60.734999999999999</v>
-    <v>1081571000</v>
+    <v>60.88</v>
+    <v>1086996000</v>
     <v>HYSTER-YALE, INC.</v>
     <v>HYSTER-YALE, INC.</v>
-    <v>61.81</v>
-    <v>6.1798999999999999</v>
-    <v>62.43</v>
-    <v>61.8</v>
-    <v>61.8</v>
+    <v>62.45</v>
+    <v>6.1009000000000002</v>
+    <v>62.11</v>
+    <v>61.01</v>
     <v>17501150</v>
     <v>HY</v>
     <v>HYSTER-YALE, INC. (XNYS:HY)</v>
-    <v>152802</v>
-    <v>64494</v>
+    <v>53347</v>
+    <v>67208</v>
     <v>1999</v>
   </rv>
   <rv s="2">
@@ -5011,13 +4987,11 @@
     <v>268435456</v>
     <v>1</v>
     <v>Powered by Refinitiv</v>
-    <v>107.955</v>
+    <v>106.17</v>
     <v>71.900000000000006</v>
-    <v>1.5104</v>
+    <v>1.5101</v>
     <v>-1.56</v>
-    <v>-1.8169000000000001E-2</v>
-    <v>0</v>
-    <v>0</v>
+    <v>-1.8364000000000002E-2</v>
     <v>USD</v>
     <v>Polaris Inc. is engaged in designing, engineering, manufacturing and marketing of powersports vehicles. The Company also designs and manufactures or sources parts, garments and accessories (PG&amp;A), which includes aftermarket accessories and apparel. The Company operates through three segments: Off Road, On Road and Marine. The Off Road segment consists of off-road vehicles and snowmobiles. The On Road segment designs and manufactures motorcycles, moto-roadsters, light duty hauling, and passenger vehicles. The Marine segment designs and manufactures boats that are designed to compete in key segments of the recreational marine industry, specifically pontoon and deck boats. Its product line-up includes the RANGER, RZR and Polaris XPEDITION and GENERAL side-by-side off-road vehicles; Sportsman all-terrain off-road vehicles; military and commercial off-road vehicles; snowmobiles; Indian Motorcycle mid-size and heavyweight motorcycles; Slingshot moto-roadsters, and pontoon and deck boats.</v>
     <v>18500</v>
@@ -5025,25 +4999,24 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>2100 HIGHWAY 55, MEDINA, MN, 55340-9770 US</v>
-    <v>85.73</v>
+    <v>85.38</v>
     <v>Leisure Products</v>
     <v>Stock</v>
-    <v>45555.847227696097</v>
+    <v>45560.958333356248</v>
     <v>24</v>
-    <v>83.36</v>
-    <v>4701231000</v>
+    <v>83.2</v>
+    <v>4648828221</v>
     <v>Polaris Inc.</v>
     <v>Polaris Inc.</v>
-    <v>85.73</v>
-    <v>15.0388</v>
-    <v>85.86</v>
-    <v>84.3</v>
-    <v>84.33</v>
+    <v>85.01</v>
+    <v>14.6061</v>
+    <v>84.95</v>
+    <v>83.39</v>
     <v>55748030</v>
     <v>PII</v>
     <v>Polaris Inc. (XNYS:PII)</v>
-    <v>1113065</v>
-    <v>460857</v>
+    <v>371113</v>
+    <v>496466</v>
     <v>1994</v>
   </rv>
   <rv s="2">
@@ -5059,7 +5032,7 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>4</v>
+    <v>5</v>
     <v>en-GB</v>
     <v>aw21cw</v>
     <v>268435456</v>
@@ -5067,11 +5040,9 @@
     <v>Powered by Refinitiv</v>
     <v>114.29989999999999</v>
     <v>75.430000000000007</v>
-    <v>1.7347999999999999</v>
-    <v>-0.37</v>
-    <v>-3.787E-3</v>
-    <v>-2.3199999999999998</v>
-    <v>-2.3836E-2</v>
+    <v>1.7321</v>
+    <v>-1.52</v>
+    <v>-1.485E-2</v>
     <v>USD</v>
     <v>CONSOL Energy Inc. is a producer and exporter of high-Btu bituminous thermal coal and metallurgical coal. It owns and operates longwall mining operations in the Northern Appalachian Basin. Its flagship operation is the Pennsylvania Mining Complex, located over 26 miles southwest of Pittsburgh, near the city of Washington and the borough of Waynesburg all in Pennsylvania, and consists of three deep longwall mining operations: the Bailey Mine, the Enlow Fork Mine and the Harvey Mine, as well as a centralized preparation plant. Its segments include the PAMC and the CONSOL Marine Terminal. The PAMC includes the Bailey Mine, the Enlow Fork Mine, the Harvey Mine and a centralized preparation plant. The PAMC segment's principal activities include the mining, preparation and marketing of bituminous coal, sold primarily to industrial end-users, metallurgical end-users and power generators. The CONSOL Marine Terminal segment provides coal export terminal services through the Port of Baltimore.</v>
     <v>2020</v>
@@ -5079,25 +5050,24 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>275 TECHNOLOGY DRIVE, SUITE #101, CANONSBURG, PA, 15317 US</v>
-    <v>99.21</v>
+    <v>102.14</v>
     <v>Coal</v>
     <v>Stock</v>
-    <v>45555.958333367969</v>
+    <v>45560.958333356248</v>
     <v>27</v>
-    <v>96.56</v>
-    <v>2860843000</v>
+    <v>100.31</v>
+    <v>2964013313</v>
     <v>CONSOL ENERGY INC.</v>
     <v>CONSOL ENERGY INC.</v>
-    <v>97.53</v>
-    <v>7.2652999999999999</v>
-    <v>97.7</v>
-    <v>97.33</v>
-    <v>95.01</v>
+    <v>102.02</v>
+    <v>7.5273000000000003</v>
+    <v>102.36</v>
+    <v>100.84</v>
     <v>29393230</v>
     <v>CEIX</v>
     <v>CONSOL ENERGY INC. (XNYS:CEIX)</v>
-    <v>1215282</v>
-    <v>494365</v>
+    <v>472722</v>
+    <v>560119</v>
     <v>2017</v>
   </rv>
   <rv s="2">
@@ -5113,7 +5083,7 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>4</v>
+    <v>5</v>
     <v>en-GB</v>
     <v>a1n1r7</v>
     <v>268435456</v>
@@ -5121,11 +5091,9 @@
     <v>Powered by Refinitiv</v>
     <v>127.3484</v>
     <v>84.35</v>
-    <v>1.2488999999999999</v>
-    <v>-1.0900000000000001</v>
-    <v>-1.1374E-2</v>
-    <v>-0.6</v>
-    <v>-6.3330000000000001E-3</v>
+    <v>1.2501</v>
+    <v>-1.91</v>
+    <v>-1.9827999999999998E-2</v>
     <v>USD</v>
     <v>AGCO Corporation is a designer, manufacturer and distributor of agricultural machinery and precision agriculture technology. The Company sells a range of agricultural equipment, including tractors, combines, self-propelled sprayers, hay tools, forage equipment, seeding and tillage equipment, implements, and grain storage and protein production systems. It provides telemetry-based fleet management tools, including remote monitoring and diagnostics, which help farmers improve uptime, machine and yield optimization, mixed fleet optimization and decision support. The Company's Precision Planting, Headsight and Intelligent Ag Solutions brands provide retrofit solutions to upgrade farmers existing equipment to improve their planting, liquid application and harvest operations. The Company’s Precision Planting, Headsight, JCA and Intelligent Ag Solutions brands also sell precision agriculture solutions around the crop cycle to third party original equipment manufacturers (OEMs).</v>
     <v>27900</v>
@@ -5133,25 +5101,24 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>4205 River Green Pkway, DULUTH, GA, 30096 US</v>
-    <v>95.61</v>
+    <v>96.6</v>
     <v>Machinery, Equipment &amp; Components</v>
     <v>Stock</v>
-    <v>45555.96684641172</v>
+    <v>45560.96577725625</v>
     <v>30</v>
-    <v>93.655000000000001</v>
-    <v>7071612000</v>
+    <v>93.9</v>
+    <v>7047725966</v>
     <v>AGCO CORPORATION</v>
     <v>AGCO CORPORATION</v>
-    <v>95.29</v>
-    <v>16.8766</v>
-    <v>95.83</v>
-    <v>94.74</v>
-    <v>94.14</v>
+    <v>96.53</v>
+    <v>16.819700000000001</v>
+    <v>96.33</v>
+    <v>94.42</v>
     <v>74642300</v>
     <v>AGCO</v>
     <v>AGCO CORPORATION (XNYS:AGCO)</v>
-    <v>1623030</v>
-    <v>735783</v>
+    <v>747354</v>
+    <v>725815</v>
     <v>1991</v>
   </rv>
   <rv s="2">
@@ -5167,7 +5134,7 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>4</v>
+    <v>5</v>
     <v>en-GB</v>
     <v>a1vuw7</v>
     <v>268435456</v>
@@ -5175,11 +5142,9 @@
     <v>Powered by Refinitiv</v>
     <v>30.1</v>
     <v>24.01</v>
-    <v>1.1538999999999999</v>
-    <v>-0.73</v>
-    <v>-2.673E-2</v>
-    <v>-0.55020000000000002</v>
-    <v>-2.07E-2</v>
+    <v>1.1527000000000001</v>
+    <v>0.33</v>
+    <v>1.2495000000000001E-2</v>
     <v>USD</v>
     <v>Ituran Location and Control Ltd. is a provider of location-based services, consisting of stolen vehicle recovery (SVR), fleet management services and other tracking services. The Company also provides wireless communication products used in connection with its location-based services and various other applications. Its operations consist of two segments: location-based services and wireless communications products. Its location-based services segment consists of its SVR and tracking services, fleet management and value-added services consisted of personal locater services and concierge services. Its wireless communications products segment consists of short and medium range two-way machine-to-machine wireless communications products that are used for various applications, including automatic vehicle location (AVL) and automatic vehicle identification. It primarily provides its services, as well as sells and leases its products in Israel, Brazil, Argentina and the United States.</v>
     <v>2841</v>
@@ -5187,25 +5152,24 @@
     <v>XNAS</v>
     <v>XNAS</v>
     <v>3 HASHIKMA, A.T AZUR, T.D 163, AZOR, 5800182 IL</v>
-    <v>26.99</v>
+    <v>26.885000000000002</v>
     <v>Communications &amp; Networking</v>
     <v>Stock</v>
-    <v>45555.917770381253</v>
+    <v>45560.946889432809</v>
     <v>33</v>
-    <v>26.08</v>
-    <v>528771400</v>
+    <v>26.35</v>
+    <v>531954329</v>
     <v>ITURAN LOCATION AND CONTROL LTD.</v>
     <v>ITURAN LOCATION AND CONTROL LTD.</v>
-    <v>26.5</v>
-    <v>10.4101</v>
-    <v>27.31</v>
-    <v>26.58</v>
-    <v>26.029800000000002</v>
+    <v>26.35</v>
+    <v>10.4727</v>
+    <v>26.41</v>
+    <v>26.74</v>
     <v>19893580</v>
     <v>ITRN</v>
     <v>ITURAN LOCATION AND CONTROL LTD. (XNAS:ITRN)</v>
-    <v>184508</v>
-    <v>81754</v>
+    <v>65641</v>
+    <v>80767</v>
     <v>1994</v>
   </rv>
   <rv s="2">
@@ -5221,19 +5185,17 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>4</v>
+    <v>5</v>
     <v>en-GB</v>
     <v>a1sea2</v>
     <v>268435456</v>
     <v>1</v>
     <v>Powered by Refinitiv</v>
-    <v>14.475</v>
+    <v>13.755000000000001</v>
     <v>6.37</v>
-    <v>2.1524000000000001</v>
-    <v>-0.01</v>
-    <v>-7.6050000000000011E-4</v>
-    <v>0.11</v>
-    <v>8.371E-3</v>
+    <v>2.1516999999999999</v>
+    <v>-0.02</v>
+    <v>-1.5219999999999999E-3</v>
     <v>USD</v>
     <v>Everi Holdings Inc. develops and offers products and services that provide gaming entertainment, improve its customers’ patron engagement, and help its casino customers operate their businesses. It develops and supplies entertaining game content, gaming machines and gaming systems and services for land-based and iGaming operators. It operates through two segments: Games and Financial Technology Solutions (FinTech). The Games segment provides gaming operators with gaming technology and entertainment products and services, including gaming machines, primarily comprising Class II, Class III and Historic Horse Racing slot machines placed under participation and fixed-fee lease arrangements or sold to casino customers. The FinTech segment provides gaming operators with financial technology products and services, including financial access and related services supporting digital, cashless and physical cash options across mobile, assisted and self-service channels.</v>
     <v>2200</v>
@@ -5241,25 +5203,24 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>7250 S Tenaya Way Ste 100, LAS VEGAS, NV, 89113-2175 US</v>
-    <v>13.19</v>
+    <v>13.16</v>
     <v>Hotels &amp; Entertainment Services</v>
     <v>Stock</v>
-    <v>45555.967937928122</v>
+    <v>45560.958333367969</v>
     <v>36</v>
-    <v>13.13</v>
-    <v>1121152000</v>
+    <v>13.12</v>
+    <v>1119445369</v>
     <v>EVERI HOLDINGS INC.</v>
     <v>EVERI HOLDINGS INC.</v>
-    <v>13.19</v>
-    <v>27.9099</v>
-    <v>13.15</v>
     <v>13.14</v>
-    <v>13.25</v>
+    <v>27.8657</v>
+    <v>13.14</v>
+    <v>13.12</v>
     <v>85323580</v>
     <v>EVRI</v>
     <v>EVERI HOLDINGS INC. (XNYS:EVRI)</v>
-    <v>1441199</v>
-    <v>834251</v>
+    <v>957009</v>
+    <v>800625</v>
     <v>2004</v>
   </rv>
   <rv s="2">
@@ -5269,9 +5230,9 @@
     <v>6</v>
     <v>NEXTRACKER INC. (XNAS:NXT)</v>
     <v>7</v>
-    <v>3</v>
+    <v>8</v>
     <v>Finance</v>
-    <v>4</v>
+    <v>9</v>
     <v>en-GB</v>
     <v>c8ssgh</v>
     <v>268435456</v>
@@ -5280,10 +5241,8 @@
     <v>62.31</v>
     <v>32.14</v>
     <v>2.1349999999999998</v>
-    <v>0.2</v>
-    <v>5.4850000000000003E-3</v>
-    <v>0.01</v>
-    <v>2.7279999999999996E-4</v>
+    <v>-0.32</v>
+    <v>-8.7119999999999993E-3</v>
     <v>USD</v>
     <v>Nextracker Inc. is a provider of integrated solar tracker and software solutions used in utility-scale and ground-mounted distributed generation solar projects. Its products enable solar panels in utility-scale power plants to follow the sun’s movement across the sky and optimize plant performance. Its products include NX Horizon, NX Gemini, TrueCapture, and NX Navigator. Its solutions include Bifacial PV modules, Large Format Modules, and First Solar Series 6 (FSLR6) Modules. NX Horizon is a one-in-portrait (1P) smart solar tracker system that delivers the lowest levelized cost of energy (LCOE). NX Gemini is its two-in-portrait (2P) format tracker which holds two rows of solar panels along the central support beam. TrueCapture is its flagship software offering, which is a self-adjusting tracker control system that uses machine learning to enhance solar power plant energy yield. It has operations in the United States, Brazil, Mexico, Spain, India, Australia, the Middle East and Brazil.</v>
     <v>1050</v>
@@ -5291,24 +5250,24 @@
     <v>XNAS</v>
     <v>XNAS</v>
     <v>6200 Paseo Padre Pkwy, FREMONT, CA, 94555 US</v>
-    <v>36.950000000000003</v>
+    <v>37.18</v>
     <v>Renewable Energy</v>
     <v>Stock</v>
-    <v>45555.991244664059</v>
-    <v>35.86</v>
-    <v>5328437000</v>
+    <v>45560.965945392971</v>
+    <v>36.241</v>
+    <v>5292098833</v>
     <v>NEXTRACKER INC.</v>
     <v>NEXTRACKER INC.</v>
-    <v>36.36</v>
-    <v>9.7293000000000003</v>
-    <v>36.46</v>
-    <v>36.659999999999997</v>
-    <v>36.67</v>
+    <v>36.75</v>
+    <v>9.6631</v>
+    <v>36.729999999999997</v>
+    <v>36.409999999999997</v>
+    <v>36.450000000000003</v>
     <v>145347400</v>
     <v>NXT</v>
     <v>NEXTRACKER INC. (XNAS:NXT)</v>
-    <v>11221138</v>
-    <v>2881718</v>
+    <v>108</v>
+    <v>3149150</v>
     <v>2022</v>
   </rv>
   <rv s="2">
@@ -5332,11 +5291,9 @@
     <v>Powered by Refinitiv</v>
     <v>80.22</v>
     <v>56.25</v>
-    <v>1.7439</v>
-    <v>-0.39</v>
-    <v>-5.0880000000000005E-3</v>
-    <v>-0.04</v>
-    <v>-5.2450000000000001E-4</v>
+    <v>1.7438</v>
+    <v>-0.44</v>
+    <v>-5.6879999999999995E-3</v>
     <v>USD</v>
     <v>Monarch Casino &amp; Resort, Inc. owns and operates the Atlantis Casino Resort Spa, a hotel and casino in Reno, Nevada (the Atlantis) and the Monarch Casino Resort Spa Black Hawk (the Monarch Black Hawk), a hotel and casino in Black Hawk, Colorado. In addition, it owns separate parcels of land located next to the Atlantis and a parcel of land with an industrial warehouse located between Denver, Colorado, and Monarch Black Hawk. The Atlantis is located approximately three miles south of downtown, which features approximately 61,000 square feet of casino space; 817 guest rooms and suites; eight food outlets; two gourmet coffee and pastry bars and one snack bar; a 30,000 square-foot health spa and salon with an enclosed year-round pool. Monarch Black Hawk features approximately 60,000 square feet of casino space; approximately 1,000 slot machines; approximately 43 table games; a live poker room; a keno counter and a sports book. The resort also includes 10 bars and lounges.</v>
     <v>2900</v>
@@ -5344,25 +5301,24 @@
     <v>XNAS</v>
     <v>XNAS</v>
     <v>Executive Offices, 3800 S Virginia Street, RENO, NV, 89502 US</v>
-    <v>77.28</v>
+    <v>78.010000000000005</v>
     <v>Hotels &amp; Entertainment Services</v>
     <v>Stock</v>
-    <v>45555.903181411719</v>
+    <v>45560.896590589844</v>
     <v>41</v>
-    <v>75.349999999999994</v>
-    <v>1407158000</v>
+    <v>76.819999999999993</v>
+    <v>1419337070</v>
     <v>MONARCH CASINO &amp; RESORT, INC.</v>
     <v>MONARCH CASINO &amp; RESORT, INC.</v>
-    <v>76.36</v>
-    <v>17.821100000000001</v>
-    <v>76.650000000000006</v>
-    <v>76.260000000000005</v>
-    <v>76.22</v>
+    <v>77.67</v>
+    <v>17.9755</v>
+    <v>77.36</v>
+    <v>76.92</v>
     <v>18452120</v>
     <v>MCRI</v>
     <v>MONARCH CASINO &amp; RESORT, INC. (XNAS:MCRI)</v>
-    <v>1349469</v>
-    <v>104726</v>
+    <v>188996</v>
+    <v>159838</v>
     <v>1993</v>
   </rv>
   <rv s="2">
@@ -5386,11 +5342,9 @@
     <v>Powered by Refinitiv</v>
     <v>69.75</v>
     <v>34.96</v>
-    <v>0.97</v>
-    <v>0.19</v>
-    <v>3.0890000000000002E-3</v>
-    <v>0</v>
-    <v>0</v>
+    <v>0.96970000000000001</v>
+    <v>-0.23</v>
+    <v>-3.7990000000000003E-3</v>
     <v>USD</v>
     <v>Miller Industries, Inc. is a manufacturer of towing and recovery equipment. The Company designs and manufactures bodies of car carriers and wreckers, which are installed on chassis manufactured by third parties, and sold to its customers. Its products are marketed and sold through a network of distributors that serve all 50 states, Canada, Mexico, and other foreign markets, and through prime contractors to governmental entities. In addition to selling its products, its independent distributors provide end-users with parts and service. Its product line includes car carriers, wreckers, and transport trailers. Car carriers are specialized flat-bed vehicles with hydraulic tilt mechanisms that enable a towing operator to drive or winch a vehicle onto the bed for transport. Its multi-vehicle transport trailers are specialized auto transport trailers with upper and lower decks and hydraulic ramps for loading vehicles. Its brands include Century, Vulcan, Chevron, Holmes, and Challenger.</v>
     <v>1821</v>
@@ -5398,25 +5352,24 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>Ste 100, 8503 Hilltop Dr, OOLTEWAH, TN, 37363 US</v>
-    <v>61.99</v>
+    <v>61.26</v>
     <v>Automobiles &amp; Auto Parts</v>
     <v>Stock</v>
-    <v>45555.84722947891</v>
+    <v>45560.958333367969</v>
     <v>44</v>
-    <v>60.064999999999998</v>
-    <v>706584305</v>
+    <v>60.090800000000002</v>
+    <v>690892612</v>
     <v>MILLER INDUSTRIES, INC.</v>
     <v>MILLER INDUSTRIES, INC.</v>
-    <v>60.7</v>
-    <v>9.9006000000000007</v>
-    <v>61.5</v>
-    <v>61.69</v>
-    <v>61.5</v>
+    <v>60.49</v>
+    <v>9.7106999999999992</v>
+    <v>60.55</v>
+    <v>60.32</v>
     <v>11453790</v>
     <v>MLR</v>
     <v>MILLER INDUSTRIES, INC. (XNYS:MLR)</v>
-    <v>338551</v>
-    <v>86786</v>
+    <v>66932</v>
+    <v>97096</v>
     <v>1994</v>
   </rv>
   <rv s="2">
@@ -5432,7 +5385,7 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>4</v>
+    <v>5</v>
     <v>en-GB</v>
     <v>btavh7</v>
     <v>268435456</v>
@@ -5440,11 +5393,9 @@
     <v>Powered by Refinitiv</v>
     <v>15.86</v>
     <v>9.1649999999999991</v>
-    <v>0.89059999999999995</v>
-    <v>-0.02</v>
-    <v>-1.9759999999999999E-3</v>
-    <v>-0.01</v>
-    <v>-9.9010000000000005E-4</v>
+    <v>0.88749999999999996</v>
+    <v>-0.11</v>
+    <v>-1.0945E-2</v>
     <v>USD</v>
     <v>Janus International Group, Inc. is a global manufacturer and supplier of turn-key self-storage, commercial and industrial building solutions. It operates through two geographic segments: Janus North America and Janus International. The Janus North America segment is comprised of all the other entities, including Janus International Group, LLC, Betco, Inc., Noke, Inc., Asta Industries, Inc., DBCI, LLC, Access Control Technologies, LLC, Janus Door, LLC, and Steel Door Depot.com, LLC. The Janus International segment is comprised of Janus International Europe Holdings Ltd. (UK). Its production and sales are in Europe and Australia. It provides facility and door automation and access control technologies, roll up and swing doors, hallway systems and relocatable storage moveable additional storage structures (MASS) units. It is comprised of three sales channels, including New Construction-Self-storage, R3-Self-storage, and Commercial and Other. It also provides terminal maintenance services.</v>
     <v>1956</v>
@@ -5452,25 +5403,24 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>135 Janus International Blvd., TEMPLE, GA, 30179 US</v>
-    <v>10.385</v>
+    <v>10.055</v>
     <v>Homebuilding &amp; Construction Supplies</v>
     <v>Stock</v>
-    <v>45555.958333356248</v>
+    <v>45560.958333367969</v>
     <v>47</v>
-    <v>10.02</v>
-    <v>1467755000</v>
+    <v>9.8849999999999998</v>
+    <v>1444502668</v>
     <v>JANUS INTERNATIONAL GROUP, INC.</v>
     <v>JANUS INTERNATIONAL GROUP, INC.</v>
-    <v>10.19</v>
-    <v>11.3254</v>
-    <v>10.119999999999999</v>
-    <v>10.1</v>
-    <v>10.09</v>
+    <v>10.039999999999999</v>
+    <v>11.145899999999999</v>
+    <v>10.050000000000001</v>
+    <v>9.94</v>
     <v>145322200</v>
     <v>JBI</v>
     <v>JANUS INTERNATIONAL GROUP, INC. (XNYS:JBI)</v>
-    <v>5522079</v>
-    <v>1977907</v>
+    <v>1607027</v>
+    <v>2071883</v>
     <v>2020</v>
   </rv>
   <rv s="2">
@@ -5494,11 +5444,9 @@
     <v>Powered by Refinitiv</v>
     <v>574.76</v>
     <v>318.17</v>
-    <v>1.3098000000000001</v>
-    <v>-1.28</v>
-    <v>-3.1740000000000002E-3</v>
-    <v>-0.23</v>
-    <v>-5.7209999999999997E-4</v>
+    <v>1.3141</v>
+    <v>-0.24</v>
+    <v>-5.9630000000000002E-4</v>
     <v>USD</v>
     <v>Ulta Beauty, Inc. is a beauty retailer. The Company's product categories include cosmetics, skincare, haircare products and styling tools, fragrance and bath, services, and accessories and other. The Company has one segment, which includes retail stores, salon services, and e-commerce. It offers a range of beauty services in its stores, focusing on hair, makeup, brow and skin services. Its skin services include a skin treatment room or dedicated skin treatment area on the sales floor. Its Ulta Beauty store prototype includes an open salon area, with most of its stores offering brow services on the salon floor. It offers a new way to shop for beauty - bringing together All Things Beauty, All in One Place. In addition to ship to home order fulfillment, it offers guests Buy Online, Pick-up in Store, Curbside Pickup, and Store 2 Door, which provides the ability for customers to order in-store and have products delivered to their homes. It operates over 1,350 retail stores across 50 states.</v>
     <v>20000</v>
@@ -5506,25 +5454,24 @@
     <v>XNAS</v>
     <v>XNAS</v>
     <v>1000 Remington Blvd, Suite 120, BOLINGBROOK, IL, 60440 US</v>
-    <v>408</v>
+    <v>402.82</v>
     <v>Specialty Retailers</v>
     <v>Stock</v>
-    <v>45555.999797256249</v>
+    <v>45560.998693414062</v>
     <v>50</v>
-    <v>400.2</v>
-    <v>18940590000</v>
+    <v>395.11</v>
+    <v>18952371289</v>
     <v>ULTA BEAUTY, INC.</v>
     <v>ULTA BEAUTY, INC.</v>
-    <v>402</v>
-    <v>16.142499999999998</v>
-    <v>403.29</v>
-    <v>402.01</v>
-    <v>401.78</v>
+    <v>401.63</v>
+    <v>16.1525</v>
+    <v>402.5</v>
+    <v>402.26</v>
     <v>47114730</v>
     <v>ULTA</v>
     <v>ULTA BEAUTY, INC. (XNAS:ULTA)</v>
-    <v>1451394</v>
-    <v>1665189</v>
+    <v>2270</v>
+    <v>1425839</v>
     <v>2016</v>
   </rv>
   <rv s="2">
@@ -5540,19 +5487,17 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>4</v>
+    <v>5</v>
     <v>en-GB</v>
     <v>a1vehw</v>
     <v>268435456</v>
     <v>1</v>
     <v>Powered by Refinitiv</v>
-    <v>32.24</v>
+    <v>31.85</v>
     <v>18.899999999999999</v>
-    <v>1.9694</v>
-    <v>-0.26</v>
-    <v>-1.1856E-2</v>
-    <v>-0.26</v>
-    <v>-1.1998E-2</v>
+    <v>1.9673</v>
+    <v>-0.12</v>
+    <v>-5.6389999999999999E-3</v>
     <v>USD</v>
     <v>International Game Technology PLC is a United Kingdom-based company, which is engaged in gaming. The Company operates and provides an integrated portfolio of gaming technology products and services, including online and instant lottery systems, iLottery, instant ticket printing, lottery management services, commercial services, gaming systems, electronic gaming machines, iGaming, and sports betting. The Company operates through three segments. The Global Lottery segment operates traditional lottery and iLottery businesses across the world, which includes sales, operations, product development, technology, and support, across the world. The Global Gaming segment operates a land-based gaming business across the world, which includes sales, product management, studios, global manufacturing, operation, and technology, across the world. The Digital &amp; Betting segment operates iGaming and sports betting activities across the world.</v>
     <v>11000</v>
@@ -5560,25 +5505,24 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>10 Finsbury Square, Third Floor, LONDON, UNITED KINGDOM-NA, EC2A 1AF GB</v>
-    <v>21.88</v>
+    <v>21.42</v>
     <v>Hotels &amp; Entertainment Services</v>
     <v>Stock</v>
-    <v>45555.999513726565</v>
+    <v>45560.959838032031</v>
     <v>53</v>
-    <v>21.46</v>
-    <v>4334000000</v>
+    <v>21.15</v>
+    <v>4232000000</v>
     <v>INTERNATIONAL GAME TECHNOLOGY PLC</v>
     <v>INTERNATIONAL GAME TECHNOLOGY PLC</v>
-    <v>21.84</v>
-    <v>20.965599999999998</v>
-    <v>21.93</v>
-    <v>21.67</v>
-    <v>21.41</v>
+    <v>21.42</v>
+    <v>20.472100000000001</v>
+    <v>21.28</v>
+    <v>21.16</v>
     <v>200000000</v>
     <v>IGT</v>
     <v>INTERNATIONAL GAME TECHNOLOGY PLC (XNYS:IGT)</v>
-    <v>1539803</v>
-    <v>628576</v>
+    <v>646284</v>
+    <v>656802</v>
     <v>2014</v>
   </rv>
   <rv s="2">
@@ -5602,11 +5546,9 @@
     <v>Powered by Refinitiv</v>
     <v>87.32</v>
     <v>54.8</v>
-    <v>0.58579999999999999</v>
-    <v>0.34</v>
-    <v>4.9480000000000001E-3</v>
-    <v>0</v>
-    <v>0</v>
+    <v>0.58540000000000003</v>
+    <v>-0.24</v>
+    <v>-3.519E-3</v>
     <v>USD</v>
     <v>Oil-Dri Corporation of America is a manufacturer and supplier of specialty sorbent products for pet care, animal health and nutrition, fluid purification, agricultural ingredients, sports field, industrial and automotive markets. Its principal product is cat litter. The Company’s Retail and Wholesale Products Group segment customers include mass merchandisers, the farm and fleet channel, drugstore chains, pet specialty retail outlets, dollar stores, retail grocery stores, distributors of industrial cleanup and automotive products, environmental service companies, sports field product users and marketers of consumer products. Its Business to Business Products Group segment customers include processors and refiners of edible oils, renewable diesel, petroleum-based oils and biodiesel fuel; manufacturers of animal feed and agricultural chemicals; and distributors of animal health and nutrition products. It is also a supplier of silica gel-based crystal cat litter.</v>
     <v>884</v>
@@ -5614,25 +5556,24 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>SUITE 400, 410 NORTH MICHIGAN AVENUE, CHICAGO, IL, 60611 US</v>
-    <v>69.84</v>
+    <v>68.58</v>
     <v>Chemicals</v>
     <v>Stock</v>
-    <v>45555.850474733597</v>
+    <v>45560.963326110941</v>
     <v>56</v>
-    <v>68</v>
-    <v>502902000</v>
+    <v>67.945599999999999</v>
+    <v>497000100</v>
     <v>OIL-DRI CORPORATION OF AMERICA</v>
     <v>OIL-DRI CORPORATION OF AMERICA</v>
-    <v>68.239999999999995</v>
-    <v>14.100099999999999</v>
-    <v>68.709999999999994</v>
-    <v>69.05</v>
-    <v>69.02</v>
+    <v>68.33</v>
+    <v>13.9483</v>
+    <v>68.209999999999994</v>
+    <v>67.97</v>
     <v>7286320</v>
     <v>ODC</v>
     <v>OIL-DRI CORPORATION OF AMERICA (XNYS:ODC)</v>
-    <v>49361</v>
-    <v>16177</v>
+    <v>12951</v>
+    <v>17074</v>
     <v>1969</v>
   </rv>
   <rv s="2">
@@ -5648,7 +5589,7 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>4</v>
+    <v>5</v>
     <v>en-GB</v>
     <v>a1mt9c</v>
     <v>268435456</v>
@@ -5656,11 +5597,9 @@
     <v>Powered by Refinitiv</v>
     <v>170.9692</v>
     <v>93.77</v>
-    <v>1.5822000000000001</v>
-    <v>-0.94</v>
-    <v>-9.195E-3</v>
-    <v>0.67</v>
-    <v>6.6149999999999994E-3</v>
+    <v>1.5787</v>
+    <v>-1.8</v>
+    <v>-1.7382999999999999E-2</v>
     <v>USD</v>
     <v>Axcelis Technologies, Inc. designs, manufactures and services ion implantation and other processing equipment used in the fabrication of semiconductor chips. The Company offers a complete line of high energy, high current and medium current implanters for all application requirements. In addition to equipment, the Company provides extensive aftermarket lifecycle products and services, including used tools, spare parts, equipment upgrades, maintenance services and customer training. Its Purion flagship systems are all based on a common platform, which enables a combination of implant purity, precision and productivity. Combining a single wafer end station, with advanced spot beam architectures (that ensures all points across the wafer see the same beam condition at the same beam angle), Purion products enable process control to optimize device performance and yield, at high productivity. The Company sells its products to semiconductor chip manufacturers around the world.</v>
     <v>1620</v>
@@ -5668,25 +5607,24 @@
     <v>XNAS</v>
     <v>XNAS</v>
     <v>108 Cherry Hill Dr, BEVERLY, MA, 01915 US</v>
-    <v>101.87350000000001</v>
+    <v>104.1532</v>
     <v>Semiconductors &amp; Semiconductor Equipment</v>
     <v>Stock</v>
-    <v>45555.992803159374</v>
+    <v>45560.978875543748</v>
     <v>59</v>
-    <v>98.59</v>
-    <v>3303835000</v>
+    <v>101.54</v>
+    <v>3318839782</v>
     <v>AXCELIS TECHNOLOGIES, INC.</v>
     <v>AXCELIS TECHNOLOGIES, INC.</v>
-    <v>100.32</v>
-    <v>13.9549</v>
-    <v>102.23</v>
-    <v>101.29</v>
-    <v>101.96</v>
+    <v>103.42</v>
+    <v>14.0182</v>
+    <v>103.55</v>
+    <v>101.75</v>
     <v>32617590</v>
     <v>ACLS</v>
     <v>AXCELIS TECHNOLOGIES, INC. (XNAS:ACLS)</v>
-    <v>3094950</v>
-    <v>524505</v>
+    <v>212</v>
+    <v>630199</v>
     <v>1995</v>
   </rv>
   <rv s="2">
@@ -5710,11 +5648,9 @@
     <v>Powered by Refinitiv</v>
     <v>179.7</v>
     <v>63.9</v>
-    <v>0.89480000000000004</v>
-    <v>-0.27</v>
-    <v>-2.2929999999999999E-3</v>
-    <v>-0.56999999999999995</v>
-    <v>-4.8509999999999994E-3</v>
+    <v>0.89439999999999997</v>
+    <v>2.86</v>
+    <v>2.4380000000000002E-2</v>
     <v>USD</v>
     <v>Dell Technologies Inc. is engaged in designing, developing, manufacturing, marketing, selling, and supporting a wide range of comprehensive and integrated solutions, products, and services. The Company operates through two segments: Infrastructure Solutions Group (ISG) and Client Solutions Group (CSG). Its ISG segment enables the Company’s customer’s digital transformation with solutions that address artificial intelligence (AI), machine learning, data analytics, and multi cloud environments. Its comprehensive storage portfolio includes modern and traditional storage solutions, including all-flash arrays, scale-out file, object platforms, hyper-converged infrastructure, and software-defined storage. Its CSG segment offers branded personal computers (PCs) including notebooks, desktops, and workstations and branded peripherals that include displays, docking stations, keyboards, mice, and webcam and audio devices, as well as third-party software and peripherals.</v>
     <v>120000</v>
@@ -5722,25 +5658,24 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>ONE DELL WAY, ROUND ROCK, TX, 78682 US</v>
-    <v>119.05</v>
+    <v>120.24</v>
     <v>Computers, Phones &amp; Household Electronics</v>
     <v>Stock</v>
-    <v>45555.999838610936</v>
+    <v>45560.999978298438</v>
     <v>62</v>
-    <v>115.08</v>
-    <v>82484580000</v>
+    <v>117.07</v>
+    <v>84358919405</v>
     <v>DELL TECHNOLOGIES INC.</v>
     <v>DELL TECHNOLOGIES INC.</v>
-    <v>116.5</v>
-    <v>21.629899999999999</v>
-    <v>117.77</v>
-    <v>117.5</v>
-    <v>116.93</v>
+    <v>117.27</v>
+    <v>22.111499999999999</v>
+    <v>117.31</v>
+    <v>120.17</v>
     <v>701996500</v>
     <v>DELL</v>
     <v>DELL TECHNOLOGIES INC. (XNYS:DELL)</v>
-    <v>75332831</v>
-    <v>11286953</v>
+    <v>12622</v>
+    <v>13388222</v>
     <v>2013</v>
   </rv>
   <rv s="2">
@@ -5772,8 +5707,6 @@
     <k n="Beta"/>
     <k n="Change"/>
     <k n="Change (%)"/>
-    <k n="Change (Extended hours)"/>
-    <k n="Change % (Extended hours)"/>
     <k n="Currency" t="s"/>
     <k n="Description" t="s"/>
     <k n="Employees"/>
@@ -5794,7 +5727,6 @@
     <k n="P/E"/>
     <k n="Previous close"/>
     <k n="Price"/>
-    <k n="Price (Extended hours)"/>
     <k n="Shares outstanding"/>
     <k n="Ticker symbol" t="s"/>
     <k n="UniqueName" t="s"/>
@@ -5822,8 +5754,6 @@
     <k n="Beta"/>
     <k n="Change"/>
     <k n="Change (%)"/>
-    <k n="Change (Extended hours)"/>
-    <k n="Change % (Extended hours)"/>
     <k n="Currency" t="s"/>
     <k n="Description" t="s"/>
     <k n="Employees"/>
@@ -5857,7 +5787,7 @@
 <file path=xl/richData/rdsupportingpropertybag.xml><?xml version="1.0" encoding="utf-8"?>
 <supportingPropertyBags xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2">
   <spbArrays count="2">
-    <a count="45">
+    <a count="42">
       <v t="s">%EntityServiceId</v>
       <v t="s">_Format</v>
       <v t="s">%IsRefreshable</v>
@@ -5868,16 +5798,13 @@
       <v t="s">Name</v>
       <v t="s">_SubLabel</v>
       <v t="s">Price</v>
-      <v t="s">Price (Extended hours)</v>
       <v t="s">Exchange</v>
       <v t="s">Official name</v>
       <v t="s">Last trade time</v>
       <v t="s">Ticker symbol</v>
       <v t="s">Exchange abbreviation</v>
       <v t="s">Change</v>
-      <v t="s">Change (Extended hours)</v>
       <v t="s">Change (%)</v>
-      <v t="s">Change % (Extended hours)</v>
       <v t="s">Currency</v>
       <v t="s">Previous close</v>
       <v t="s">Open</v>
@@ -5904,7 +5831,7 @@
       <v t="s">ExchangeID</v>
       <v t="s">%ProviderInfo</v>
     </a>
-    <a count="44">
+    <a count="42">
       <v t="s">%EntityServiceId</v>
       <v t="s">_Format</v>
       <v t="s">%IsRefreshable</v>
@@ -5922,9 +5849,7 @@
       <v t="s">Ticker symbol</v>
       <v t="s">Exchange abbreviation</v>
       <v t="s">Change</v>
-      <v t="s">Change (Extended hours)</v>
       <v t="s">Change (%)</v>
-      <v t="s">Change % (Extended hours)</v>
       <v t="s">Currency</v>
       <v t="s">Previous close</v>
       <v t="s">Open</v>
@@ -5951,7 +5876,7 @@
       <v t="s">%ProviderInfo</v>
     </a>
   </spbArrays>
-  <spbData count="8">
+  <spbData count="10">
     <spb s="0">
       <v>0</v>
       <v>Name</v>
@@ -5989,29 +5914,20 @@
       <v>8</v>
       <v>9</v>
       <v>4</v>
-      <v>1</v>
-      <v>1</v>
-      <v>5</v>
     </spb>
     <spb s="4">
-      <v>at close</v>
+      <v>Real-Time Nasdaq Last Sale</v>
+      <v>from previous close</v>
+      <v>from previous close</v>
+      <v>Source: Nasdaq Last Sale</v>
+      <v>GMT</v>
+    </spb>
+    <spb s="4">
+      <v>Delayed 15 minutes</v>
       <v>from previous close</v>
       <v>from previous close</v>
       <v>Source: Nasdaq</v>
       <v>GMT</v>
-      <v>Delayed 15 minutes</v>
-      <v>from close</v>
-      <v>from close</v>
-    </spb>
-    <spb s="4">
-      <v>at close</v>
-      <v>from previous close</v>
-      <v>from previous close</v>
-      <v>Source: Nasdaq Last Sale</v>
-      <v>GMT</v>
-      <v>Real-Time Nasdaq Last Sale</v>
-      <v>from close</v>
-      <v>from close</v>
     </spb>
     <spb s="5">
       <v>1</v>
@@ -6022,12 +5938,43 @@
       <v>1</v>
       <v>1</v>
     </spb>
+    <spb s="7">
+      <v>1</v>
+      <v>2</v>
+      <v>2</v>
+      <v>1</v>
+      <v>3</v>
+      <v>1</v>
+      <v>1</v>
+      <v>1</v>
+      <v>4</v>
+      <v>4</v>
+      <v>5</v>
+      <v>6</v>
+      <v>1</v>
+      <v>1</v>
+      <v>1</v>
+      <v>4</v>
+      <v>7</v>
+      <v>8</v>
+      <v>9</v>
+      <v>4</v>
+      <v>1</v>
+    </spb>
+    <spb s="8">
+      <v>at close</v>
+      <v>from previous close</v>
+      <v>from previous close</v>
+      <v>Source: Nasdaq</v>
+      <v>GMT</v>
+      <v>Delayed 15 minutes</v>
+    </spb>
   </spbData>
 </supportingPropertyBags>
 </file>
 
 <file path=xl/richData/rdsupportingpropertybagstructure.xml><?xml version="1.0" encoding="utf-8"?>
-<spbStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" count="7">
+<spbStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" count="9">
   <s>
     <k n="^Order" t="spba"/>
     <k n="TitleProperty" t="s"/>
@@ -6065,9 +6012,6 @@
     <k n="Year incorporated" t="i"/>
     <k n="`%EntityServiceId" t="i"/>
     <k n="Shares outstanding" t="i"/>
-    <k n="Price (Extended hours)" t="i"/>
-    <k n="Change (Extended hours)" t="i"/>
-    <k n="Change % (Extended hours)" t="i"/>
   </s>
   <s>
     <k n="Price" t="s"/>
@@ -6075,9 +6019,6 @@
     <k n="Change (%)" t="s"/>
     <k n="ExchangeID" t="s"/>
     <k n="Last trade time" t="s"/>
-    <k n="Price (Extended hours)" t="s"/>
-    <k n="Change (Extended hours)" t="s"/>
-    <k n="Change % (Extended hours)" t="s"/>
   </s>
   <s>
     <k n="^Order" t="spba"/>
@@ -6087,6 +6028,37 @@
     <k n="ExchangeID" t="spb"/>
     <k n="UniqueName" t="spb"/>
     <k n="`%ProviderInfo" t="spb"/>
+  </s>
+  <s>
+    <k n="Low" t="i"/>
+    <k n="P/E" t="i"/>
+    <k n="Beta" t="i"/>
+    <k n="High" t="i"/>
+    <k n="Name" t="i"/>
+    <k n="Open" t="i"/>
+    <k n="Price" t="i"/>
+    <k n="Change" t="i"/>
+    <k n="Volume" t="i"/>
+    <k n="Employees" t="i"/>
+    <k n="Change (%)" t="i"/>
+    <k n="Market cap" t="i"/>
+    <k n="52 week low" t="i"/>
+    <k n="52 week high" t="i"/>
+    <k n="Previous close" t="i"/>
+    <k n="Volume average" t="i"/>
+    <k n="Last trade time" t="i"/>
+    <k n="Year incorporated" t="i"/>
+    <k n="`%EntityServiceId" t="i"/>
+    <k n="Shares outstanding" t="i"/>
+    <k n="Price (Extended hours)" t="i"/>
+  </s>
+  <s>
+    <k n="Price" t="s"/>
+    <k n="Change" t="s"/>
+    <k n="Change (%)" t="s"/>
+    <k n="ExchangeID" t="s"/>
+    <k n="Last trade time" t="s"/>
+    <k n="Price (Extended hours)" t="s"/>
   </s>
 </spbStructures>
 </file>
@@ -69497,8 +69469,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F51CD2FE-0785-5E4C-91F5-512BDFA3DC54}">
   <dimension ref="B1:L26"/>
   <sheetViews>
-    <sheetView topLeftCell="C4" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="K28" sqref="K28"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
@@ -69581,15 +69553,15 @@
       </c>
       <c r="I3" s="151" cm="1">
         <f t="array" aca="1" ref="I3" ca="1">_FV(B3,"Price")</f>
-        <v>57.51</v>
+        <v>58.64</v>
       </c>
       <c r="J3" s="131">
         <f t="shared" ref="J3:J24" ca="1" si="0">((I3-F3)/F3)</f>
-        <v>-0.16349090909090913</v>
+        <v>-0.14705454545454544</v>
       </c>
       <c r="K3" s="172">
         <f t="shared" ref="K3:K24" ca="1" si="1">(I3*G3) - H3</f>
-        <v>-81.936131999999986</v>
+        <v>-73.702047999999991</v>
       </c>
       <c r="L3"/>
     </row>
@@ -69620,15 +69592,15 @@
       </c>
       <c r="I4" s="151" cm="1">
         <f t="array" aca="1" ref="I4" ca="1">_FV(B4,"Price")</f>
-        <v>139.05000000000001</v>
+        <v>143.04</v>
       </c>
       <c r="J4" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>0.3902219556088784</v>
+        <v>0.43011397720455907</v>
       </c>
       <c r="K4" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>195.50145000000009</v>
+        <v>215.48735999999997</v>
       </c>
       <c r="L4"/>
     </row>
@@ -69659,15 +69631,15 @@
       </c>
       <c r="I5" s="151" cm="1">
         <f t="array" aca="1" ref="I5" ca="1">_FV(B5,"Price")</f>
-        <v>19.38</v>
+        <v>18.59</v>
       </c>
       <c r="J5" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.11100917431192668</v>
+        <v>-0.14724770642201837</v>
       </c>
       <c r="K5" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>-55.663104000000033</v>
+        <v>-73.81667200000004</v>
       </c>
       <c r="L5"/>
     </row>
@@ -69698,15 +69670,15 @@
       </c>
       <c r="I6" s="151" cm="1">
         <f t="array" aca="1" ref="I6" ca="1">_FV(B6,"Price")</f>
-        <v>22.23</v>
+        <v>21.91</v>
       </c>
       <c r="J6" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>0.2702857142857143</v>
+        <v>0.252</v>
       </c>
       <c r="K6" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>149.36977200000001</v>
+        <v>140.00772399999994</v>
       </c>
       <c r="L6"/>
     </row>
@@ -69737,15 +69709,15 @@
       </c>
       <c r="I7" s="153" cm="1">
         <f t="array" aca="1" ref="I7" ca="1">_FV(B7,"Price")</f>
-        <v>228.2</v>
+        <v>226.37</v>
       </c>
       <c r="J7" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>0.29321092598889253</v>
+        <v>0.28284030375155839</v>
       </c>
       <c r="K7" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>146.90261999999996</v>
+        <v>141.70706700000005</v>
       </c>
       <c r="L7"/>
     </row>
@@ -69776,15 +69748,15 @@
       </c>
       <c r="I8" s="153" cm="1">
         <f t="array" aca="1" ref="I8" ca="1">_FV(B8,"Price")</f>
-        <v>91.06</v>
+        <v>93.18</v>
       </c>
       <c r="J8" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>0.6220163876024225</v>
+        <v>0.65977912361952273</v>
       </c>
       <c r="K8" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>311.56480400000009</v>
+        <v>330.48241200000018</v>
       </c>
       <c r="L8"/>
     </row>
@@ -69815,15 +69787,15 @@
       </c>
       <c r="I9" s="153" cm="1">
         <f t="array" aca="1" ref="I9" ca="1">_FV(B9,"Price")</f>
-        <v>19.350000000000001</v>
+        <v>17.29</v>
       </c>
       <c r="J9" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.42376414532459789</v>
+        <v>-0.48511018463371053</v>
       </c>
       <c r="K9" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>-212.28058499999997</v>
+        <v>-243.01763900000003</v>
       </c>
       <c r="L9"/>
     </row>
@@ -69854,15 +69826,15 @@
       </c>
       <c r="I10" s="155" cm="1">
         <f t="array" aca="1" ref="I10" ca="1">_FV(B10,"Price")</f>
-        <v>61.8</v>
+        <v>61.01</v>
       </c>
       <c r="J10" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>6.1855670103092682E-2</v>
+        <v>4.8281786941580668E-2</v>
       </c>
       <c r="K10" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>31.011479999999892</v>
+        <v>24.210685999999896</v>
       </c>
       <c r="L10"/>
     </row>
@@ -69893,15 +69865,15 @@
       </c>
       <c r="I11" s="155" cm="1">
         <f t="array" aca="1" ref="I11" ca="1">_FV(B11,"Price")</f>
-        <v>84.3</v>
+        <v>83.39</v>
       </c>
       <c r="J11" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>-7.6366823709871801E-2</v>
+        <v>-8.6337241152624034E-2</v>
       </c>
       <c r="K11" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>-38.277300000000025</v>
+        <v>-43.272289999999998</v>
       </c>
       <c r="L11"/>
     </row>
@@ -69932,15 +69904,15 @@
       </c>
       <c r="I12" s="155" cm="1">
         <f t="array" aca="1" ref="I12" ca="1">_FV(B12,"Price")</f>
-        <v>97.33</v>
+        <v>100.84</v>
       </c>
       <c r="J12" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>0.16284348864994019</v>
+        <v>0.20477897252090801</v>
       </c>
       <c r="K12" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>81.568714999999997</v>
+        <v>102.57781999999997</v>
       </c>
       <c r="L12"/>
     </row>
@@ -69971,15 +69943,15 @@
       </c>
       <c r="I13" s="155" cm="1">
         <f t="array" aca="1" ref="I13" ca="1">_FV(B13,"Price")</f>
-        <v>94.74</v>
+        <v>94.42</v>
       </c>
       <c r="J13" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.19004873044370355</v>
+        <v>-0.19278447465162005</v>
       </c>
       <c r="K13" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>-95.219106000000011</v>
+        <v>-96.589697999999999</v>
       </c>
       <c r="L13"/>
     </row>
@@ -70010,15 +69982,15 @@
       </c>
       <c r="I14" s="157" cm="1">
         <f t="array" aca="1" ref="I14" ca="1">_FV(B14,"Price")</f>
-        <v>26.58</v>
+        <v>26.74</v>
       </c>
       <c r="J14" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>4.276186739897999E-2</v>
+        <v>4.9038838760298159E-2</v>
       </c>
       <c r="K14" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>21.456479999999942</v>
+        <v>24.601439999999911</v>
       </c>
       <c r="L14"/>
     </row>
@@ -70049,15 +70021,15 @@
       </c>
       <c r="I15" s="157" cm="1">
         <f t="array" aca="1" ref="I15" ca="1">_FV(B15,"Price")</f>
-        <v>13.14</v>
+        <v>13.12</v>
       </c>
       <c r="J15" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>0.49828962371721791</v>
+        <v>0.4960091220068415</v>
       </c>
       <c r="K15" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>249.42671400000006</v>
+        <v>248.28451199999995</v>
       </c>
       <c r="L15"/>
     </row>
@@ -70088,15 +70060,15 @@
       </c>
       <c r="I16" s="159" cm="1">
         <f t="array" aca="1" ref="I16" ca="1">_FV(B16,"Price")</f>
-        <v>36.659999999999997</v>
+        <v>36.409999999999997</v>
       </c>
       <c r="J16" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.2444352844187965</v>
+        <v>-0.2495877988458369</v>
       </c>
       <c r="K16" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>-118.55000000000001</v>
+        <v>-121.05000000000001</v>
       </c>
       <c r="L16"/>
     </row>
@@ -70127,15 +70099,15 @@
       </c>
       <c r="I17" s="159" cm="1">
         <f t="array" aca="1" ref="I17" ca="1">_FV(B17,"Price")</f>
-        <v>76.260000000000005</v>
+        <v>76.92</v>
       </c>
       <c r="J17" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>9.0207290922087235E-2</v>
+        <v>9.964260185847032E-2</v>
       </c>
       <c r="K17" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>44.180000000000064</v>
+        <v>48.800000000000068</v>
       </c>
       <c r="L17"/>
     </row>
@@ -70166,15 +70138,15 @@
       </c>
       <c r="I18" s="159" cm="1">
         <f t="array" aca="1" ref="I18" ca="1">_FV(B18,"Price")</f>
-        <v>61.69</v>
+        <v>60.32</v>
       </c>
       <c r="J18" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>-7.8803473785783538E-3</v>
+        <v>-2.9913155355419739E-2</v>
       </c>
       <c r="K18" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>-3.9200000000000159</v>
+        <v>-14.879999999999995</v>
       </c>
       <c r="L18"/>
     </row>
@@ -70205,15 +70177,15 @@
       </c>
       <c r="I19" s="159" cm="1">
         <f t="array" aca="1" ref="I19" ca="1">_FV(B19,"Price")</f>
-        <v>10.1</v>
+        <v>9.94</v>
       </c>
       <c r="J19" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.24626865671641796</v>
+        <v>-0.25820895522388065</v>
       </c>
       <c r="K19" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>-123.43169999999998</v>
+        <v>-129.41298</v>
       </c>
       <c r="L19"/>
     </row>
@@ -70244,15 +70216,15 @@
       </c>
       <c r="I20" s="213" cm="1">
         <f t="array" aca="1" ref="I20" ca="1">_FV(B20,"Price")</f>
-        <v>402.01</v>
+        <v>402.26</v>
       </c>
       <c r="J20" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>2.1886120996441317E-2</v>
+        <v>2.2521606507371669E-2</v>
       </c>
       <c r="K20" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>11.012800000000027</v>
+        <v>11.332799999999963</v>
       </c>
       <c r="L20"/>
     </row>
@@ -70283,15 +70255,15 @@
       </c>
       <c r="I21" s="216" cm="1">
         <f t="array" aca="1" ref="I21" ca="1">_FV(B21,"Price")</f>
-        <v>21.67</v>
+        <v>21.16</v>
       </c>
       <c r="J21" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.6504941599281212E-2</v>
+        <v>-4.9415992812219291E-2</v>
       </c>
       <c r="K21" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>-13.284144999999967</v>
+        <v>-24.762460000000033</v>
       </c>
     </row>
     <row r="22" spans="2:12">
@@ -70321,15 +70293,15 @@
       </c>
       <c r="I22" s="216" cm="1">
         <f t="array" aca="1" ref="I22" ca="1">_FV(B22,"Price")</f>
-        <v>69.05</v>
+        <v>67.97</v>
       </c>
       <c r="J22" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>-8.4721424468696648E-3</v>
+        <v>-2.3980470993681818E-2</v>
       </c>
       <c r="K22" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>-2.8149650000000292</v>
+        <v>-10.606841000000031</v>
       </c>
     </row>
     <row r="23" spans="2:12">
@@ -70359,15 +70331,15 @@
       </c>
       <c r="I23" s="216" cm="1">
         <f t="array" aca="1" ref="I23" ca="1">_FV(B23,"Price")</f>
-        <v>101.29</v>
+        <v>101.75</v>
       </c>
       <c r="J23" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>1.5821220211609888E-3</v>
+        <v>6.1307228319984631E-3</v>
       </c>
       <c r="K23" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>0.8107890000000566</v>
+        <v>3.0896750000000566</v>
       </c>
     </row>
     <row r="24" spans="2:12">
@@ -70397,21 +70369,21 @@
       </c>
       <c r="I24" s="216" cm="1">
         <f t="array" aca="1" ref="I24" ca="1">_FV(B24,"Price")</f>
-        <v>117.5</v>
+        <v>120.17</v>
       </c>
       <c r="J24" s="131">
         <f t="shared" ca="1" si="0"/>
-        <v>-5.7539346759181483E-3</v>
+        <v>1.6838720595701427E-2</v>
       </c>
       <c r="K24" s="172">
         <f t="shared" ca="1" si="1"/>
-        <v>-2.8704999999999927</v>
+        <v>8.4486979999999789</v>
       </c>
     </row>
     <row r="26" spans="2:12" ht="13">
       <c r="K26" s="171">
         <f ca="1">SUM(K3:K24)</f>
-        <v>494.55808700000017</v>
+        <v>467.91956599999975</v>
       </c>
     </row>
   </sheetData>
@@ -70793,7 +70765,7 @@
   </sheetPr>
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>

</xml_diff>

<commit_message>
vault backup: 2024-09-30 09:13:22
</commit_message>
<xml_diff>
--- a/_system/Attachments/Portfolio Management.xlsx
+++ b/_system/Attachments/Portfolio Management.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martin/repos/tomesink/obsidian/_system/Attachments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF3EE26A-95B1-7548-BA82-C1E4A125B8EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2EEE7EA-4F86-EF46-BF0F-CF730356E1A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3300" yWindow="980" windowWidth="33800" windowHeight="18860" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2120" yWindow="500" windowWidth="34980" windowHeight="19340" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Stocks Performance" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
       </extLst>
     </bk>
   </futureMetadata>
-  <futureMetadata name="XLRICHVALUE" count="22">
+  <futureMetadata name="XLRICHVALUE" count="25">
     <bk>
       <extLst>
         <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
@@ -211,13 +211,34 @@
         </ext>
       </extLst>
     </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="67"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="70"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="73"/>
+        </ext>
+      </extLst>
+    </bk>
   </futureMetadata>
   <cellMetadata count="1">
     <bk>
       <rc t="1" v="0"/>
     </bk>
   </cellMetadata>
-  <valueMetadata count="22">
+  <valueMetadata count="25">
     <bk>
       <rc t="2" v="0"/>
     </bk>
@@ -283,6 +304,15 @@
     </bk>
     <bk>
       <rc t="2" v="21"/>
+    </bk>
+    <bk>
+      <rc t="2" v="22"/>
+    </bk>
+    <bk>
+      <rc t="2" v="23"/>
+    </bk>
+    <bk>
+      <rc t="2" v="24"/>
     </bk>
   </valueMetadata>
 </metadata>
@@ -824,7 +854,7 @@
     <numFmt numFmtId="173" formatCode="[$$-409]#,##0.00"/>
     <numFmt numFmtId="174" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="16">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -910,8 +940,20 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="31">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1092,8 +1134,26 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="42">
+  <borders count="43">
     <border>
       <left/>
       <right/>
@@ -1648,12 +1708,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="219">
+  <cellXfs count="225">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -2193,10 +2264,28 @@
     <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="10" fontId="9" fillId="31" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="33" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="173" fontId="15" fillId="33" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="32" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Per cent" xfId="1" builtinId="5"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="18">
     <dxf>
@@ -2708,7 +2797,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <c:style val="2"/>
   <c:chart>
@@ -2995,7 +3084,7 @@
                 <a:latin typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-CZ"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2094734553"/>
@@ -3047,7 +3136,7 @@
                 <a:latin typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-CZ"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2094734552"/>
@@ -3093,7 +3182,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <c:style val="2"/>
   <c:chart>
@@ -3380,7 +3469,7 @@
                 <a:latin typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-CZ"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2094734553"/>
@@ -3432,7 +3521,7 @@
                 <a:latin typeface="Arial"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-CZ"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2094734552"/>
@@ -3478,7 +3567,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3548,7 +3637,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-CZ"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -3733,7 +3822,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-CZ"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -3770,7 +3859,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-CZ"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -4566,7 +4655,7 @@
 </file>
 
 <file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
-<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="65">
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="74">
   <rv s="0">
     <v>https://www.bing.com/financeapi/forcetrigger?t=a1qlnm&amp;q=XNYS%3aCVS&amp;form=skydnc</v>
     <v>Learn more on Bing</v>
@@ -4585,9 +4674,11 @@
     <v>Powered by Refinitiv</v>
     <v>83.25</v>
     <v>52.770499999999998</v>
-    <v>0.52780000000000005</v>
-    <v>0.15</v>
-    <v>2.5580000000000004E-3</v>
+    <v>0.5292</v>
+    <v>2.37</v>
+    <v>4.0163000000000004E-2</v>
+    <v>0.1</v>
+    <v>1.6289999999999998E-3</v>
     <v>USD</v>
     <v>CVS Health Corporation is a health solutions company. The Company operates in four segments: Health Care Benefits, Health Services, Pharmacy &amp; Consumer Wellness, and Corporate/Other. Its Health Care Benefits segment offer a range of traditional, voluntary and consumer-directed health insurance products and related services, including medical, pharmacy, dental and behavioral health plans, medical management capabilities, Medicare Advantage and Medicare supplement plans, and Medicaid health care management services. Its Health Services segment provides a full range of pharmacy benefit management solutions, delivers health care services in its medical clinics, virtually, and in the home, and offers provider enablement solutions. The Pharmacy &amp; Consumer Wellness segment dispenses prescriptions in its retail pharmacies and through its infusion operations, provides ancillary pharmacy services, including pharmacy patient care programs, diagnostic testing and vaccination administration.</v>
     <v>300000</v>
@@ -4595,24 +4686,25 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>1 Cvs Dr, WOONSOCKET, RI, 02895-6146 US</v>
-    <v>58.914999999999999</v>
+    <v>61.86</v>
     <v>Healthcare Providers &amp; Services</v>
     <v>Stock</v>
-    <v>45561.566948957814</v>
+    <v>45562.996976296097</v>
     <v>0</v>
-    <v>58.64</v>
-    <v>73956585410</v>
+    <v>59.29</v>
+    <v>73428250000</v>
     <v>CVS HEALTH CORPORATION</v>
     <v>CVS HEALTH CORPORATION</v>
-    <v>58.64</v>
-    <v>10.4353</v>
-    <v>58.64</v>
-    <v>58.79</v>
+    <v>59.45</v>
+    <v>10.926399999999999</v>
+    <v>59.01</v>
+    <v>61.38</v>
+    <v>61.48</v>
     <v>1257979000</v>
     <v>CVS</v>
     <v>CVS HEALTH CORPORATION (XNYS:CVS)</v>
-    <v>143986</v>
-    <v>7936235</v>
+    <v>12510217</v>
+    <v>8081310</v>
     <v>1996</v>
   </rv>
   <rv s="2">
@@ -4636,9 +4728,11 @@
     <v>Powered by Refinitiv</v>
     <v>165.32</v>
     <v>74</v>
-    <v>1.9953000000000001</v>
-    <v>6.0774999999999997</v>
-    <v>4.2487999999999998E-2</v>
+    <v>1.9942</v>
+    <v>-3.09</v>
+    <v>-2.0962999999999999E-2</v>
+    <v>0.2505</v>
+    <v>1.7360000000000001E-3</v>
     <v>USD</v>
     <v>Crocs, Inc. is engaged in the design, development, worldwide marketing, distribution, and sale of casual lifestyle footwear and accessories for women, men, and children. The Company’s segments include Crocs Brand and the HEYDUDE Brand. The Company’s Crocs Brand collection contains Croslite material, a molded footwear technology, delivering extraordinary comfort with each step. Its Croslite materials are formulated to create soft, comfortable, lightweight, non-marking, and odor-resistant footwear. The HEYDUDE Brand offers shoes with a versatile silhouette. It sells its products in more than 80 countries, through two distribution channels: wholesale and direct-to-consumer. Its wholesale channel includes domestic and international multi-brand retailers, mono-branded partner stores, e-tailers, and distributors; its direct-to-consumer channel includes Company-operated retail stores, Company-operated e-commerce sites, and third-party marketplaces.</v>
     <v>7030</v>
@@ -4646,24 +4740,25 @@
     <v>XNAS</v>
     <v>XNAS</v>
     <v>500 Eldorado Boulevard, Building 5, BROOMFIELD, CO, 80021 US</v>
-    <v>150</v>
+    <v>148.25</v>
     <v>Textiles &amp; Apparel</v>
     <v>Stock</v>
-    <v>45561.566964803125</v>
+    <v>45562.968765265628</v>
     <v>3</v>
-    <v>147.1</v>
-    <v>8855362122</v>
+    <v>143.9</v>
+    <v>7647023000</v>
     <v>CROCS, INC.</v>
     <v>CROCS, INC.</v>
-    <v>147.5</v>
-    <v>10.7577</v>
-    <v>143.04</v>
-    <v>149.11750000000001</v>
+    <v>148.01</v>
+    <v>10.853199999999999</v>
+    <v>147.4</v>
+    <v>144.31</v>
+    <v>144.56049999999999</v>
     <v>59385130</v>
     <v>CROX</v>
     <v>CROCS, INC. (XNAS:CROX)</v>
-    <v>76365</v>
-    <v>993344</v>
+    <v>975883</v>
+    <v>978550</v>
     <v>2005</v>
   </rv>
   <rv s="2">
@@ -4687,9 +4782,11 @@
     <v>Powered by Refinitiv</v>
     <v>30.07</v>
     <v>17.71</v>
-    <v>1.5172000000000001</v>
-    <v>0.44</v>
-    <v>2.3668999999999999E-2</v>
+    <v>1.5166999999999999</v>
+    <v>0.2</v>
+    <v>1.0582000000000001E-2</v>
+    <v>0</v>
+    <v>0</v>
     <v>USD</v>
     <v>Wabash National Corporation provides connected solutions for the transportation, logistics and distribution industries. The Company designs and manufactures products including dry freight and refrigerated trailers, platform trailers, tank trailers, dry and refrigerated truck bodies, structural composite panels and products, transportation, logistics, and distribution industry parts and services, and specialty food grade processing equipment. The Company’s Transportation Solutions (TS) segment comprises the design and manufacturing operations for the Company’s transportation-related equipment and products. This includes dry and refrigerated van trailers, platform trailers, tank trailers and truck-mounted tanks, truck-mounted dry and refrigerated truck bodies and EcoNex technology products. Its Parts &amp; Services (P&amp;S) segment is comprised of the Company’s parts and services businesses as well as the upfitting component of truck bodies business. It also includes DuraPlate composite panels.</v>
     <v>6700</v>
@@ -4697,24 +4794,25 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>3900 Mccarty Lane, LAFAYETTE, IN, 47905 US</v>
-    <v>19.03</v>
+    <v>19.57</v>
     <v>Machinery, Equipment &amp; Components</v>
     <v>Stock</v>
-    <v>45561.566820601562</v>
+    <v>45562.958333333336</v>
     <v>6</v>
-    <v>18.86</v>
-    <v>837305346</v>
+    <v>18.920000000000002</v>
+    <v>857985000</v>
     <v>WABASH NATIONAL CORPORATION</v>
     <v>WABASH NATIONAL CORPORATION</v>
-    <v>18.86</v>
-    <v>5.7026000000000003</v>
-    <v>18.59</v>
-    <v>19.03</v>
+    <v>19.22</v>
+    <v>5.8559999999999999</v>
+    <v>18.899999999999999</v>
+    <v>19.100000000000001</v>
+    <v>19.100000000000001</v>
     <v>43999230</v>
     <v>WNC</v>
     <v>WABASH NATIONAL CORPORATION (XNYS:WNC)</v>
-    <v>16421</v>
-    <v>576318</v>
+    <v>253868</v>
+    <v>580646</v>
     <v>1991</v>
   </rv>
   <rv s="2">
@@ -4738,9 +4836,11 @@
     <v>Powered by Refinitiv</v>
     <v>26.4</v>
     <v>16.12</v>
-    <v>1.0346</v>
-    <v>0.2</v>
-    <v>9.127999999999999E-3</v>
+    <v>1.0341</v>
+    <v>0.33</v>
+    <v>1.5109999999999998E-2</v>
+    <v>0</v>
+    <v>0</v>
     <v>USD</v>
     <v>Perdoceo Education Corporation, through its academic institutions, offers quality postsecondary education primarily online to a diverse student population, along with campus-based and blended learning programs. The Company's academic institutions include Colorado Technical University (CTU) and the American InterContinental University System (AIUS), which provides degree programs from the associate through doctoral level as well as non-degree seeking and professional development programs. Its academic institutions offer students industry-relevant and career-focused academic programs. CTU offers academic programs in the career-oriented disciplines of business and management, nursing, healthcare management, computer science, engineering, information systems and technology, project management, cybersecurity and criminal justice. AIUS offers academic programs in the career-oriented disciplines of business studies, information technologies, education, health sciences and criminal justice.</v>
     <v>2319</v>
@@ -4748,24 +4848,25 @@
     <v>XNAS</v>
     <v>XNAS</v>
     <v>1750 E. GOLF ROAD, SCHAUMBURG, IL, 60173 US</v>
-    <v>22.13</v>
+    <v>22.48</v>
     <v>Miscellaneous Educational Service Providers</v>
     <v>Stock</v>
-    <v>45561.566841087501</v>
+    <v>45562.908084085153</v>
     <v>9</v>
-    <v>22.11</v>
-    <v>1452039537</v>
+    <v>21.99</v>
+    <v>1455980000</v>
     <v>PERDOCEO EDUCATION CORPORATION</v>
     <v>PERDOCEO EDUCATION CORPORATION</v>
-    <v>22.13</v>
-    <v>10.7677</v>
-    <v>21.91</v>
-    <v>22.11</v>
+    <v>22.07</v>
+    <v>10.8954</v>
+    <v>21.84</v>
+    <v>22.17</v>
+    <v>22.17</v>
     <v>65673430</v>
     <v>PRDO</v>
     <v>PERDOCEO EDUCATION CORPORATION (XNAS:PRDO)</v>
-    <v>3567</v>
-    <v>483214</v>
+    <v>219658</v>
+    <v>485108</v>
     <v>1994</v>
   </rv>
   <rv s="2">
@@ -4789,9 +4890,11 @@
     <v>Powered by Refinitiv</v>
     <v>237.23</v>
     <v>164.07499999999999</v>
-    <v>1.24</v>
-    <v>0.5</v>
-    <v>2.209E-3</v>
+    <v>1.2394000000000001</v>
+    <v>0.27</v>
+    <v>1.1869999999999999E-3</v>
+    <v>-0.28999999999999998</v>
+    <v>-1.273E-3</v>
     <v>USD</v>
     <v>Apple Inc. designs, manufactures and markets smartphones, personal computers, tablets, wearables and accessories, and sells a variety of related services. Its product categories include iPhone, Mac, iPad, and Wearables, Home and Accessories. Its software platforms include iOS, iPadOS, macOS, watchOS, and tvOS. Its services include advertising, AppleCare, cloud services, digital content and payment services. It operates various platforms, including the App Store, that allow customers to discover and download applications and digital content, such as books, music, video, games and podcasts. It also offers digital content through subscription-based services, including Apple Arcade, Apple Fitness+, Apple Music, Apple News+ and Apple TV+. Its products include iPhone 15 Pro, iPhone 15, iPhone 14, iPhone 13, MacBook Air, MacBook Pro, iMac, Mac mini, Mac Studio, Mac Pro, and others. It also provides DarwinAI, which specializes in visual quality inspection using its Explainable AI platform.</v>
     <v>161000</v>
@@ -4799,24 +4902,25 @@
     <v>XNAS</v>
     <v>XNAS</v>
     <v>One Apple Park Way, CUPERTINO, CA, 95014 US</v>
-    <v>227.62</v>
+    <v>229.52</v>
     <v>Computers, Phones &amp; Household Electronics</v>
     <v>Stock</v>
-    <v>45561.566976318747</v>
+    <v>45562.999957418753</v>
     <v>12</v>
-    <v>226.46</v>
-    <v>3449363241800</v>
+    <v>227.3</v>
+    <v>3382921000000</v>
     <v>APPLE INC.</v>
     <v>APPLE INC.</v>
-    <v>227.31</v>
-    <v>34.466099999999997</v>
-    <v>226.37</v>
-    <v>226.87</v>
+    <v>228.46</v>
+    <v>34.672400000000003</v>
+    <v>227.52</v>
+    <v>227.79</v>
+    <v>227.5</v>
     <v>15204140000</v>
     <v>AAPL</v>
     <v>APPLE INC. (XNAS:AAPL)</v>
-    <v>2754909</v>
-    <v>57342394</v>
+    <v>34025967</v>
+    <v>57417243</v>
     <v>1977</v>
   </rv>
   <rv s="2">
@@ -4838,11 +4942,13 @@
     <v>268435456</v>
     <v>1</v>
     <v>Powered by Refinitiv</v>
-    <v>95.4</v>
+    <v>97.25</v>
     <v>50.134999999999998</v>
-    <v>0.98780000000000001</v>
-    <v>2.2200000000000002</v>
-    <v>2.3824999999999999E-2</v>
+    <v>0.98839999999999995</v>
+    <v>0.61</v>
+    <v>6.3610000000000003E-3</v>
+    <v>-1.1599999999999999</v>
+    <v>-1.2020999999999999E-2</v>
     <v>USD</v>
     <v>Allison Transmission Holdings, Inc. is a designer and manufacturer of propulsion solutions for commercial and defense vehicles. The Company is also a manufacturer of medium-and heavy-duty fully automatic transmissions. Its products are used in a variety of applications, including on-highway trucks, including distribution, refuse, construction, fire and emergency; buses, including school, transit and coach; motorhomes, off-highway vehicles, and equipment, including energy, mining and construction applications; and defense vehicles, including tactical wheeled and tracked. The Company operates in approximately 150 countries. The Company has manufacturing facilities in the United States, Hungary and India, as well as global engineering resources, including electrification engineering centers in Indianapolis, Indiana, Auburn Hills, Michigan and London in the United Kingdom. The Company also has approximately 1,600 independent distributor and dealer locations worldwide.</v>
     <v>3700</v>
@@ -4850,24 +4956,25 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>One Allison Way, INDIANAPOLIS, IN, 46222 US</v>
-    <v>95.4</v>
+    <v>97.25</v>
     <v>Machinery, Equipment &amp; Components</v>
     <v>Stock</v>
-    <v>45561.566761110938</v>
+    <v>45562.958333356248</v>
     <v>15</v>
-    <v>94.194999999999993</v>
-    <v>8102080000</v>
+    <v>95.3</v>
+    <v>7679461000</v>
     <v>ALLISON TRANSMISSION HOLDINGS, INC.</v>
     <v>ALLISON TRANSMISSION HOLDINGS, INC.</v>
-    <v>94.72</v>
-    <v>12.1843</v>
-    <v>93.18</v>
-    <v>95.4</v>
+    <v>96</v>
+    <v>12.621</v>
+    <v>95.89</v>
+    <v>96.5</v>
+    <v>95.34</v>
     <v>87137880</v>
     <v>ALSN</v>
     <v>ALLISON TRANSMISSION HOLDINGS, INC. (XNYS:ALSN)</v>
-    <v>11273</v>
-    <v>554943</v>
+    <v>952149</v>
+    <v>568414</v>
     <v>2007</v>
   </rv>
   <rv s="2">
@@ -4891,9 +4998,11 @@
     <v>Powered by Refinitiv</v>
     <v>40.695</v>
     <v>17.063600000000001</v>
-    <v>1.9891000000000001</v>
-    <v>0.47</v>
-    <v>2.7183000000000002E-2</v>
+    <v>1.9852000000000001</v>
+    <v>0.28000000000000003</v>
+    <v>1.5927E-2</v>
+    <v>0</v>
+    <v>0</v>
     <v>USD</v>
     <v>Par Pacific Holdings, Inc. is an energy company, which provides both renewable and conventional fuels to the western United States. It owns and operates 125,000 barrels per day of combined refining capacity across three locations and an energy infrastructure network, including 7.6 million barrels of storage, and marine, rail, rack and pipeline assets. The Company has three segments. Refining segment owns and operates four refineries with total operating crude oil throughput capacity of 219 thousand barrels per day (Mbpd). Retail segment operates fuel retail outlets in Hawaii, Washington and Idaho. It operates convenience stores and fuel retail sites under Hele and nomnom brands, 76 branded fuel retail sites and other sites operated by third parties that sell gasoline, diesel, and retail merchandise, such as soft drinks, prepared foods, and other sundries. Logistics segment operates a multi-modal logistics network spanning the Pacific, the Northwest, and the Rocky Mountain regions.</v>
     <v>1814</v>
@@ -4901,24 +5010,25 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>825 Town and Country Ln Ste 1500, HOUSTON, TX, 77024-2235 US</v>
-    <v>17.760000000000002</v>
+    <v>17.93</v>
     <v>Oil &amp; Gas</v>
     <v>Stock</v>
-    <v>45561.566935231247</v>
+    <v>45562.958333378905</v>
     <v>18</v>
-    <v>17.063600000000001</v>
-    <v>1000436251</v>
+    <v>17.41</v>
+    <v>1067470000</v>
     <v>PAR PACIFIC HOLDINGS, INC.</v>
     <v>PAR PACIFIC HOLDINGS, INC.</v>
-    <v>17.23</v>
-    <v>3.0124</v>
-    <v>17.29</v>
-    <v>17.760000000000002</v>
+    <v>17.88</v>
+    <v>3.1082999999999998</v>
+    <v>17.579999999999998</v>
+    <v>17.86</v>
+    <v>17.86</v>
     <v>56330870</v>
     <v>PARR</v>
     <v>PAR PACIFIC HOLDINGS, INC. (XNYS:PARR)</v>
-    <v>78265</v>
-    <v>1174527</v>
+    <v>1200796</v>
+    <v>1212458</v>
     <v>2005</v>
   </rv>
   <rv s="2">
@@ -4942,9 +5052,11 @@
     <v>Powered by Refinitiv</v>
     <v>84.44</v>
     <v>38.5</v>
-    <v>1.3069999999999999</v>
-    <v>-1.1000000000000001</v>
-    <v>-1.7710999999999998E-2</v>
+    <v>1.3070999999999999</v>
+    <v>1.99</v>
+    <v>3.2231999999999997E-2</v>
+    <v>0</v>
+    <v>0</v>
     <v>USD</v>
     <v>Hyster-Yale, Inc., formerly Hyster-Yale Materials Handling, Inc., through its wholly owned operating subsidiary, Hyster-Yale Materials Handling, designs, engineers, manufactures, sells, and services a comprehensive line of lift trucks, attachments, aftermarket parts and technology solutions marketed globally primarily under the Hyster and Yale brand names. The Company's business segments include Lift Trucks, Attachments and Fuel Cells. The Hyster-Yale Maximal brand provides trucks for customers requiring fundamental lift truck performance. The Lift Truck segment is focused on fuel cell-powered battery box replacements and integrated fuel cell engine solutions. Hyster- Yale’s attachment subsidiary, Bolzoni S.p.A., is a producer of attachments, forks, and lift tables under the Bolzoni, Auramo and Meyer brand names. The Fuel Cell business, Nuvera Fuel Cells, is an alternative-power technology company focused on fuel cell stacks and engines.</v>
     <v>8600</v>
@@ -4952,24 +5064,25 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>5875 LANDERBROOK DRIVE, SUITE 300, CLEVELAND, OH, 44124 US</v>
-    <v>62.45</v>
+    <v>63.93</v>
     <v>Machinery, Equipment &amp; Components</v>
     <v>Stock</v>
-    <v>45560.958333378905</v>
+    <v>45562.958333378905</v>
     <v>21</v>
-    <v>60.88</v>
-    <v>1086996000</v>
+    <v>61.24</v>
+    <v>1046044000</v>
     <v>HYSTER-YALE, INC.</v>
     <v>HYSTER-YALE, INC.</v>
-    <v>62.45</v>
-    <v>6.1009000000000002</v>
-    <v>62.11</v>
-    <v>61.01</v>
+    <v>62.65</v>
+    <v>6.3749000000000002</v>
+    <v>61.74</v>
+    <v>63.73</v>
+    <v>63.73</v>
     <v>17501150</v>
     <v>HY</v>
     <v>HYSTER-YALE, INC. (XNYS:HY)</v>
-    <v>830</v>
-    <v>66910</v>
+    <v>70316</v>
+    <v>65223</v>
     <v>1999</v>
   </rv>
   <rv s="2">
@@ -4993,9 +5106,11 @@
     <v>Powered by Refinitiv</v>
     <v>106.17</v>
     <v>71.900000000000006</v>
-    <v>1.5101</v>
-    <v>2.13</v>
-    <v>2.5543E-2</v>
+    <v>1.51</v>
+    <v>0.43</v>
+    <v>5.0880000000000005E-3</v>
+    <v>-0.94</v>
+    <v>-1.1065E-2</v>
     <v>USD</v>
     <v>Polaris Inc. is engaged in designing, engineering, manufacturing and marketing of powersports vehicles. The Company also designs and manufactures or sources parts, garments and accessories (PG&amp;A), which includes aftermarket accessories and apparel. The Company operates through three segments: Off Road, On Road and Marine. The Off Road segment consists of off-road vehicles and snowmobiles. The On Road segment designs and manufactures motorcycles, moto-roadsters, light duty hauling, and passenger vehicles. The Marine segment designs and manufactures boats that are designed to compete in key segments of the recreational marine industry, specifically pontoon and deck boats. Its product line-up includes the RANGER, RZR and Polaris XPEDITION and GENERAL side-by-side off-road vehicles; Sportsman all-terrain off-road vehicles; military and commercial off-road vehicles; snowmobiles; Indian Motorcycle mid-size and heavyweight motorcycles; Slingshot moto-roadsters, and pontoon and deck boats.</v>
     <v>18500</v>
@@ -5003,24 +5118,25 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>2100 HIGHWAY 55, MEDINA, MN, 55340-9770 US</v>
-    <v>85.52</v>
+    <v>86.51</v>
     <v>Leisure Products</v>
     <v>Stock</v>
-    <v>45561.566923437502</v>
+    <v>45562.958333344533</v>
     <v>24</v>
-    <v>85.05</v>
-    <v>4767571525</v>
+    <v>84.25</v>
+    <v>4656076000</v>
     <v>Polaris Inc.</v>
     <v>Polaris Inc.</v>
-    <v>85.05</v>
-    <v>14.6061</v>
-    <v>83.39</v>
-    <v>85.52</v>
+    <v>85.73</v>
+    <v>14.877700000000001</v>
+    <v>84.52</v>
+    <v>84.95</v>
+    <v>84.01</v>
     <v>55748030</v>
     <v>PII</v>
     <v>Polaris Inc. (XNYS:PII)</v>
-    <v>8105</v>
-    <v>498409</v>
+    <v>497634</v>
+    <v>492414</v>
     <v>1994</v>
   </rv>
   <rv s="2">
@@ -5044,9 +5160,11 @@
     <v>Powered by Refinitiv</v>
     <v>114.29989999999999</v>
     <v>75.430000000000007</v>
-    <v>1.7326999999999999</v>
-    <v>3.76</v>
-    <v>3.7287000000000001E-2</v>
+    <v>1.7321</v>
+    <v>0.2</v>
+    <v>1.921E-3</v>
+    <v>0.01</v>
+    <v>9.5849999999999999E-5</v>
     <v>USD</v>
     <v>CONSOL Energy Inc. is a producer and exporter of high-Btu bituminous thermal coal and metallurgical coal. It owns and operates longwall mining operations in the Northern Appalachian Basin. Its flagship operation is the Pennsylvania Mining Complex, located over 26 miles southwest of Pittsburgh, near the city of Washington and the borough of Waynesburg all in Pennsylvania, and consists of three deep longwall mining operations: the Bailey Mine, the Enlow Fork Mine and the Harvey Mine, as well as a centralized preparation plant. Its segments include the PAMC and the CONSOL Marine Terminal. The PAMC includes the Bailey Mine, the Enlow Fork Mine, the Harvey Mine and a centralized preparation plant. The PAMC segment's principal activities include the mining, preparation and marketing of bituminous coal, sold primarily to industrial end-users, metallurgical end-users and power generators. The CONSOL Marine Terminal segment provides coal export terminal services through the Port of Baltimore.</v>
     <v>2020</v>
@@ -5054,24 +5172,25 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>275 TECHNOLOGY DRIVE, SUITE #101, CANONSBURG, PA, 15317 US</v>
-    <v>104.6</v>
+    <v>106.58</v>
     <v>Coal</v>
     <v>Stock</v>
-    <v>45561.566885763285</v>
+    <v>45562.958333378905</v>
     <v>27</v>
-    <v>102.86</v>
-    <v>3074531858</v>
+    <v>104.14</v>
+    <v>2852319000</v>
     <v>CONSOL ENERGY INC.</v>
     <v>CONSOL ENERGY INC.</v>
-    <v>102.86</v>
-    <v>7.5273000000000003</v>
-    <v>100.84</v>
-    <v>104.6</v>
+    <v>104.8</v>
+    <v>7.79</v>
+    <v>104.13</v>
+    <v>104.33</v>
+    <v>104.34</v>
     <v>29393230</v>
     <v>CEIX</v>
     <v>CONSOL ENERGY INC. (XNYS:CEIX)</v>
-    <v>12332</v>
-    <v>565985</v>
+    <v>370038</v>
+    <v>498359</v>
     <v>2017</v>
   </rv>
   <rv s="2">
@@ -5095,9 +5214,11 @@
     <v>Powered by Refinitiv</v>
     <v>127.3484</v>
     <v>84.35</v>
-    <v>1.2495000000000001</v>
-    <v>1.31</v>
-    <v>1.3873999999999999E-2</v>
+    <v>1.2508999999999999</v>
+    <v>1.58</v>
+    <v>1.6334000000000001E-2</v>
+    <v>-0.7</v>
+    <v>-7.1199999999999996E-3</v>
     <v>USD</v>
     <v>AGCO Corporation is a designer, manufacturer and distributor of agricultural machinery and precision agriculture technology. The Company sells a range of agricultural equipment, including tractors, combines, self-propelled sprayers, hay tools, forage equipment, seeding and tillage equipment, implements, and grain storage and protein production systems. It provides telemetry-based fleet management tools, including remote monitoring and diagnostics, which help farmers improve uptime, machine and yield optimization, mixed fleet optimization and decision support. The Company's Precision Planting, Headsight and Intelligent Ag Solutions brands provide retrofit solutions to upgrade farmers existing equipment to improve their planting, liquid application and harvest operations. The Company’s Precision Planting, Headsight, JCA and Intelligent Ag Solutions brands also sell precision agriculture solutions around the crop cycle to third party original equipment manufacturers (OEMs).</v>
     <v>27900</v>
@@ -5105,24 +5226,25 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>4205 River Green Pkway, DULUTH, GA, 30096 US</v>
-    <v>96.42</v>
+    <v>99.26</v>
     <v>Machinery, Equipment &amp; Components</v>
     <v>Stock</v>
-    <v>45561.566652719528</v>
+    <v>45562.966145635939</v>
     <v>30</v>
-    <v>95.65</v>
-    <v>7145507379</v>
+    <v>97.575000000000003</v>
+    <v>6804393000</v>
     <v>AGCO CORPORATION</v>
     <v>AGCO CORPORATION</v>
-    <v>96.1</v>
-    <v>16.819700000000001</v>
-    <v>94.42</v>
-    <v>95.73</v>
+    <v>97.71</v>
+    <v>17.5214</v>
+    <v>96.73</v>
+    <v>98.31</v>
+    <v>97.61</v>
     <v>74642300</v>
     <v>AGCO</v>
     <v>AGCO CORPORATION (XNYS:AGCO)</v>
-    <v>7249</v>
-    <v>731422</v>
+    <v>659164</v>
+    <v>736119</v>
     <v>1991</v>
   </rv>
   <rv s="2">
@@ -5146,9 +5268,11 @@
     <v>Powered by Refinitiv</v>
     <v>30.1</v>
     <v>24.01</v>
-    <v>1.1525000000000001</v>
-    <v>0.435</v>
-    <v>1.6508999999999999E-2</v>
+    <v>1.1512</v>
+    <v>-0.34</v>
+    <v>-1.2663000000000001E-2</v>
+    <v>0.09</v>
+    <v>3.3950000000000004E-3</v>
     <v>USD</v>
     <v>Ituran Location and Control Ltd. is a provider of location-based services, consisting of stolen vehicle recovery (SVR), fleet management services and other tracking services. The Company also provides wireless communication products used in connection with its location-based services and various other applications. Its operations consist of two segments: location-based services and wireless communications products. Its location-based services segment consists of its SVR and tracking services, fleet management and value-added services consisted of personal locater services and concierge services. Its wireless communications products segment consists of short and medium range two-way machine-to-machine wireless communications products that are used for various applications, including automatic vehicle location (AVL) and automatic vehicle identification. It primarily provides its services, as well as sells and leases its products in Israel, Brazil, Argentina and the United States.</v>
     <v>2841</v>
@@ -5156,24 +5280,25 @@
     <v>XNAS</v>
     <v>XNAS</v>
     <v>3 HASHIKMA, A.T AZUR, T.D 163, AZOR, 5800182 IL</v>
-    <v>26.85</v>
+    <v>26.87</v>
     <v>Communications &amp; Networking</v>
     <v>Stock</v>
-    <v>45561.566941157034</v>
+    <v>45562.910048032034</v>
     <v>33</v>
-    <v>26.67</v>
-    <v>531954300</v>
+    <v>26.2</v>
+    <v>544885100</v>
     <v>ITURAN LOCATION AND CONTROL LTD.</v>
     <v>ITURAN LOCATION AND CONTROL LTD.</v>
-    <v>26.67</v>
-    <v>10.319900000000001</v>
-    <v>26.35</v>
-    <v>26.785</v>
+    <v>26.87</v>
+    <v>10.3826</v>
+    <v>26.85</v>
+    <v>26.51</v>
+    <v>26.6</v>
     <v>19893580</v>
     <v>ITRN</v>
     <v>ITURAN LOCATION AND CONTROL LTD. (XNAS:ITRN)</v>
-    <v>1852</v>
-    <v>77259</v>
+    <v>105256</v>
+    <v>76889</v>
     <v>1994</v>
   </rv>
   <rv s="2">
@@ -5195,11 +5320,13 @@
     <v>268435456</v>
     <v>1</v>
     <v>Powered by Refinitiv</v>
-    <v>13.755000000000001</v>
+    <v>13.67</v>
     <v>6.37</v>
-    <v>2.1520000000000001</v>
-    <v>4.4999999999999998E-2</v>
-    <v>3.4300000000000003E-3</v>
+    <v>2.1515</v>
+    <v>0.01</v>
+    <v>7.6160000000000008E-4</v>
+    <v>-0.04</v>
+    <v>-3.0439999999999998E-3</v>
     <v>USD</v>
     <v>Everi Holdings Inc. develops and offers products and services that provide gaming entertainment, improve its customers’ patron engagement, and help its casino customers operate their businesses. It develops and supplies entertaining game content, gaming machines and gaming systems and services for land-based and iGaming operators. It operates through two segments: Games and Financial Technology Solutions (FinTech). The Games segment provides gaming operators with gaming technology and entertainment products and services, including gaming machines, primarily comprising Class II, Class III and Historic Horse Racing slot machines placed under participation and fixed-fee lease arrangements or sold to casino customers. The FinTech segment provides gaming operators with financial technology products and services, including financial access and related services supporting digital, cashless and physical cash options across mobile, assisted and self-service channels.</v>
     <v>2200</v>
@@ -5207,24 +5334,25 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>7250 S Tenaya Way Ste 100, LAS VEGAS, NV, 89113-2175 US</v>
-    <v>13.164999999999999</v>
+    <v>13.16</v>
     <v>Hotels &amp; Entertainment Services</v>
     <v>Stock</v>
-    <v>45561.566910253903</v>
+    <v>45562.96055133047</v>
     <v>36</v>
-    <v>13.135</v>
-    <v>1123284930</v>
+    <v>13.13</v>
+    <v>1120299000</v>
     <v>EVERI HOLDINGS INC.</v>
     <v>EVERI HOLDINGS INC.</v>
+    <v>13.15</v>
+    <v>27.9312</v>
+    <v>13.13</v>
     <v>13.14</v>
-    <v>27.8657</v>
-    <v>13.12</v>
-    <v>13.164999999999999</v>
+    <v>13.1</v>
     <v>85323580</v>
     <v>EVRI</v>
     <v>EVERI HOLDINGS INC. (XNYS:EVRI)</v>
-    <v>43283</v>
-    <v>813826</v>
+    <v>708697</v>
+    <v>798529</v>
     <v>2004</v>
   </rv>
   <rv s="2">
@@ -5245,8 +5373,10 @@
     <v>62.31</v>
     <v>32.14</v>
     <v>2.1160000000000001</v>
-    <v>1.925</v>
-    <v>5.287E-2</v>
+    <v>1.34</v>
+    <v>3.5675999999999999E-2</v>
+    <v>-2.5999999999999999E-2</v>
+    <v>-6.6839999999999998E-4</v>
     <v>USD</v>
     <v>Nextracker Inc. is a provider of integrated solar tracker and software solutions used in utility-scale and ground-mounted distributed generation solar projects. Its products enable solar panels in utility-scale power plants to follow the sun’s movement across the sky and optimize plant performance. Its products include NX Horizon, NX Gemini, TrueCapture, and NX Navigator. Its solutions include Bifacial PV modules, Large Format Modules, and First Solar Series 6 (FSLR6) Modules. NX Horizon is a one-in-portrait (1P) smart solar tracker system that delivers the lowest levelized cost of energy (LCOE). NX Gemini is its two-in-portrait (2P) format tracker which holds two rows of solar panels along the central support beam. TrueCapture is its flagship software offering, which is a self-adjusting tracker control system that uses machine learning to enhance solar power plant energy yield. It has operations in the United States, Brazil, Mexico, Spain, India, Australia, the Middle East and Brazil.</v>
     <v>1050</v>
@@ -5254,23 +5384,24 @@
     <v>XNAS</v>
     <v>XNAS</v>
     <v>6200 Paseo Padre Pkwy, FREMONT, CA, 94555 US</v>
-    <v>38.659999999999997</v>
+    <v>39.090000000000003</v>
     <v>Renewable Energy</v>
     <v>Stock</v>
-    <v>45561.566915613279</v>
-    <v>37.49</v>
-    <v>5571892579</v>
+    <v>45562.998350902344</v>
+    <v>38.08</v>
+    <v>5475238000</v>
     <v>NEXTRACKER INC.</v>
     <v>NEXTRACKER INC.</v>
-    <v>37.76</v>
-    <v>9.6631</v>
-    <v>36.409999999999997</v>
-    <v>38.335000000000001</v>
+    <v>38.15</v>
+    <v>10.3238</v>
+    <v>37.56</v>
+    <v>38.9</v>
+    <v>38.874000000000002</v>
     <v>145347400</v>
     <v>NXT</v>
     <v>NEXTRACKER INC. (XNAS:NXT)</v>
-    <v>155544</v>
-    <v>3140478</v>
+    <v>1949793</v>
+    <v>3165195</v>
     <v>2022</v>
   </rv>
   <rv s="2">
@@ -5294,9 +5425,11 @@
     <v>Powered by Refinitiv</v>
     <v>80.22</v>
     <v>56.25</v>
-    <v>1.7437</v>
-    <v>0.77</v>
-    <v>1.0009999999999998E-2</v>
+    <v>1.744</v>
+    <v>-0.02</v>
+    <v>-2.5340000000000003E-4</v>
+    <v>0.28000000000000003</v>
+    <v>3.5479999999999999E-3</v>
     <v>USD</v>
     <v>Monarch Casino &amp; Resort, Inc. owns and operates the Atlantis Casino Resort Spa, a hotel and casino in Reno, Nevada (the Atlantis) and the Monarch Casino Resort Spa Black Hawk (the Monarch Black Hawk), a hotel and casino in Black Hawk, Colorado. In addition, it owns separate parcels of land located next to the Atlantis and a parcel of land with an industrial warehouse located between Denver, Colorado, and Monarch Black Hawk. The Atlantis is located approximately three miles south of downtown, which features approximately 61,000 square feet of casino space; 817 guest rooms and suites; eight food outlets; two gourmet coffee and pastry bars and one snack bar; a 30,000 square-foot health spa and salon with an enclosed year-round pool. Monarch Black Hawk features approximately 60,000 square feet of casino space; approximately 1,000 slot machines; approximately 43 table games; a live poker room; a keno counter and a sports book. The resort also includes 10 bars and lounges.</v>
     <v>2900</v>
@@ -5304,24 +5437,25 @@
     <v>XNAS</v>
     <v>XNAS</v>
     <v>Executive Offices, 3800 S Virginia Street, RENO, NV, 89502 US</v>
-    <v>77.69</v>
+    <v>79.94</v>
     <v>Hotels &amp; Entertainment Services</v>
     <v>Stock</v>
-    <v>45561.56663599531</v>
+    <v>45562.87143851797</v>
     <v>41</v>
-    <v>77.69</v>
-    <v>1433545202</v>
+    <v>78.685000000000002</v>
+    <v>1390552000</v>
     <v>MONARCH CASINO &amp; RESORT, INC.</v>
     <v>MONARCH CASINO &amp; RESORT, INC.</v>
-    <v>77.69</v>
-    <v>17.9755</v>
-    <v>76.92</v>
-    <v>77.69</v>
+    <v>79.44</v>
+    <v>18.442699999999999</v>
+    <v>78.94</v>
+    <v>78.92</v>
+    <v>79.2</v>
     <v>18452120</v>
     <v>MCRI</v>
     <v>MONARCH CASINO &amp; RESORT, INC. (XNAS:MCRI)</v>
-    <v>750</v>
-    <v>163285</v>
+    <v>102323</v>
+    <v>165173</v>
     <v>1993</v>
   </rv>
   <rv s="2">
@@ -5345,9 +5479,11 @@
     <v>Powered by Refinitiv</v>
     <v>69.75</v>
     <v>34.96</v>
-    <v>0.96989999999999998</v>
-    <v>0.67</v>
-    <v>1.1107000000000001E-2</v>
+    <v>0.96940000000000004</v>
+    <v>0.55000000000000004</v>
+    <v>9.2200000000000008E-3</v>
+    <v>0.05</v>
+    <v>8.3059999999999991E-4</v>
     <v>USD</v>
     <v>Miller Industries, Inc. is a manufacturer of towing and recovery equipment. The Company designs and manufactures bodies of car carriers and wreckers, which are installed on chassis manufactured by third parties, and sold to its customers. Its products are marketed and sold through a network of distributors that serve all 50 states, Canada, Mexico, and other foreign markets, and through prime contractors to governmental entities. In addition to selling its products, its independent distributors provide end-users with parts and service. Its product line includes car carriers, wreckers, and transport trailers. Car carriers are specialized flat-bed vehicles with hydraulic tilt mechanisms that enable a towing operator to drive or winch a vehicle onto the bed for transport. Its multi-vehicle transport trailers are specialized auto transport trailers with upper and lower decks and hydraulic ramps for loading vehicles. Its brands include Century, Vulcan, Chevron, Holmes, and Challenger.</v>
     <v>1821</v>
@@ -5355,24 +5491,25 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>Ste 100, 8503 Hilltop Dr, OOLTEWAH, TN, 37363 US</v>
-    <v>61.034999999999997</v>
+    <v>61.16</v>
     <v>Automobiles &amp; Auto Parts</v>
     <v>Stock</v>
-    <v>45561.566298517966</v>
+    <v>45562.958333356248</v>
     <v>44</v>
-    <v>60.99</v>
-    <v>698566652</v>
+    <v>59.552500000000002</v>
+    <v>665923500</v>
     <v>MILLER INDUSTRIES, INC.</v>
     <v>MILLER INDUSTRIES, INC.</v>
-    <v>61.034999999999997</v>
-    <v>9.7106999999999992</v>
-    <v>60.32</v>
-    <v>60.99</v>
+    <v>60.34</v>
+    <v>9.6929999999999996</v>
+    <v>59.65</v>
+    <v>60.2</v>
+    <v>60.25</v>
     <v>11453790</v>
     <v>MLR</v>
     <v>MILLER INDUSTRIES, INC. (XNYS:MLR)</v>
-    <v>1231</v>
-    <v>96715</v>
+    <v>41910</v>
+    <v>96145</v>
     <v>1994</v>
   </rv>
   <rv s="2">
@@ -5396,9 +5533,11 @@
     <v>Powered by Refinitiv</v>
     <v>15.86</v>
     <v>9.1649999999999991</v>
-    <v>0.88849999999999996</v>
-    <v>0.09</v>
-    <v>9.0539999999999995E-3</v>
+    <v>0.88749999999999996</v>
+    <v>0.1</v>
+    <v>9.8329999999999997E-3</v>
+    <v>0</v>
+    <v>0</v>
     <v>USD</v>
     <v>Janus International Group, Inc. is a global manufacturer and supplier of turn-key self-storage, commercial and industrial building solutions. It operates through two geographic segments: Janus North America and Janus International. The Janus North America segment is comprised of all the other entities, including Janus International Group, LLC, Betco, Inc., Noke, Inc., Asta Industries, Inc., DBCI, LLC, Access Control Technologies, LLC, Janus Door, LLC, and Steel Door Depot.com, LLC. The Janus International segment is comprised of Janus International Europe Holdings Ltd. (UK). Its production and sales are in Europe and Australia. It provides facility and door automation and access control technologies, roll up and swing doors, hallway systems and relocatable storage moveable additional storage structures (MASS) units. It is comprised of three sales channels, including New Construction-Self-storage, R3-Self-storage, and Commercial and Other. It also provides terminal maintenance services.</v>
     <v>1956</v>
@@ -5406,24 +5545,25 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>135 Janus International Blvd., TEMPLE, GA, 30179 US</v>
-    <v>10.07</v>
+    <v>10.525</v>
     <v>Homebuilding &amp; Construction Supplies</v>
     <v>Stock</v>
-    <v>45561.566884293752</v>
+    <v>45562.958333356248</v>
     <v>47</v>
-    <v>10.01</v>
-    <v>1457581666</v>
+    <v>10.23</v>
+    <v>1437237000</v>
     <v>JANUS INTERNATIONAL GROUP, INC.</v>
     <v>JANUS INTERNATIONAL GROUP, INC.</v>
-    <v>10.07</v>
-    <v>11.145899999999999</v>
-    <v>9.94</v>
-    <v>10.029999999999999</v>
+    <v>10.32</v>
+    <v>11.510400000000001</v>
+    <v>10.17</v>
+    <v>10.27</v>
+    <v>10.27</v>
     <v>145322200</v>
     <v>JBI</v>
     <v>JANUS INTERNATIONAL GROUP, INC. (XNYS:JBI)</v>
-    <v>18099</v>
-    <v>2031490</v>
+    <v>1925147</v>
+    <v>1998433</v>
     <v>2020</v>
   </rv>
   <rv s="2">
@@ -5447,9 +5587,11 @@
     <v>Powered by Refinitiv</v>
     <v>574.76</v>
     <v>318.17</v>
-    <v>1.3126</v>
-    <v>7.74</v>
-    <v>1.9240999999999998E-2</v>
+    <v>1.3149</v>
+    <v>-2.1</v>
+    <v>-5.1710000000000002E-3</v>
+    <v>-0.02</v>
+    <v>-4.9500000000000004E-5</v>
     <v>USD</v>
     <v>Ulta Beauty, Inc. is a beauty retailer. The Company's product categories include cosmetics, skincare, haircare products and styling tools, fragrance and bath, services, and accessories and other. The Company has one segment, which includes retail stores, salon services, and e-commerce. It offers a range of beauty services in its stores, focusing on hair, makeup, brow and skin services. Its skin services include a skin treatment room or dedicated skin treatment area on the sales floor. Its Ulta Beauty store prototype includes an open salon area, with most of its stores offering brow services on the salon floor. It offers a new way to shop for beauty - bringing together All Things Beauty, All in One Place. In addition to ship to home order fulfillment, it offers guests Buy Online, Pick-up in Store, Curbside Pickup, and Store 2 Door, which provides the ability for customers to order in-store and have products delivered to their homes. It operates over 1,350 retail stores across 50 states.</v>
     <v>20000</v>
@@ -5457,24 +5599,25 @@
     <v>XNAS</v>
     <v>XNAS</v>
     <v>1000 Remington Blvd, Suite 120, BOLINGBROOK, IL, 60440 US</v>
-    <v>410</v>
+    <v>411.79</v>
     <v>Specialty Retailers</v>
     <v>Stock</v>
-    <v>45561.56696653906</v>
+    <v>45562.990797661718</v>
     <v>50</v>
-    <v>406.44</v>
-    <v>19317039300</v>
+    <v>402.51499999999999</v>
+    <v>17825390000</v>
     <v>ULTA BEAUTY, INC.</v>
     <v>ULTA BEAUTY, INC.</v>
-    <v>407.32</v>
-    <v>16.1525</v>
-    <v>402.26</v>
-    <v>410</v>
+    <v>407.63</v>
+    <v>16.222799999999999</v>
+    <v>406.11</v>
+    <v>404.01</v>
+    <v>403.99</v>
     <v>47114730</v>
     <v>ULTA</v>
     <v>ULTA BEAUTY, INC. (XNAS:ULTA)</v>
-    <v>44434</v>
-    <v>1416758</v>
+    <v>1060882</v>
+    <v>1401709</v>
     <v>2016</v>
   </rv>
   <rv s="2">
@@ -5498,9 +5641,11 @@
     <v>Powered by Refinitiv</v>
     <v>31.85</v>
     <v>18.899999999999999</v>
-    <v>1.9681999999999999</v>
-    <v>0.68</v>
-    <v>3.2135999999999998E-2</v>
+    <v>1.9673</v>
+    <v>-0.01</v>
+    <v>-4.6000000000000001E-4</v>
+    <v>0</v>
+    <v>0</v>
     <v>USD</v>
     <v>International Game Technology PLC is a United Kingdom-based company, which is engaged in gaming. The Company operates and provides an integrated portfolio of gaming technology products and services, including online and instant lottery systems, iLottery, instant ticket printing, lottery management services, commercial services, gaming systems, electronic gaming machines, iGaming, and sports betting. The Company operates through three segments. The Global Lottery segment operates traditional lottery and iLottery businesses across the world, which includes sales, operations, product development, technology, and support, across the world. The Global Gaming segment operates a land-based gaming business across the world, which includes sales, product management, studios, global manufacturing, operation, and technology, across the world. The Digital &amp; Betting segment operates iGaming and sports betting activities across the world.</v>
     <v>11000</v>
@@ -5508,24 +5653,25 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>10 Finsbury Square, Third Floor, LONDON, UNITED KINGDOM-NA, EC2A 1AF GB</v>
-    <v>21.878399999999999</v>
+    <v>22.06</v>
     <v>Hotels &amp; Entertainment Services</v>
     <v>Stock</v>
-    <v>45561.566936515628</v>
+    <v>45562.958333344533</v>
     <v>53</v>
-    <v>21.57</v>
-    <v>4368000000</v>
+    <v>21.675000000000001</v>
+    <v>4338000000</v>
     <v>INTERNATIONAL GAME TECHNOLOGY PLC</v>
     <v>INTERNATIONAL GAME TECHNOLOGY PLC</v>
-    <v>21.58</v>
-    <v>20.472300000000001</v>
-    <v>21.16</v>
-    <v>21.84</v>
+    <v>22.06</v>
+    <v>21.0139</v>
+    <v>21.74</v>
+    <v>21.73</v>
+    <v>21.73</v>
     <v>200000000</v>
     <v>IGT</v>
     <v>INTERNATIONAL GAME TECHNOLOGY PLC (XNYS:IGT)</v>
-    <v>31106</v>
-    <v>653800</v>
+    <v>848970</v>
+    <v>658113</v>
     <v>2014</v>
   </rv>
   <rv s="2">
@@ -5549,9 +5695,11 @@
     <v>Powered by Refinitiv</v>
     <v>87.32</v>
     <v>54.8</v>
-    <v>0.58560000000000001</v>
-    <v>-0.24</v>
-    <v>-3.519E-3</v>
+    <v>0.58540000000000003</v>
+    <v>0.08</v>
+    <v>1.1709999999999999E-3</v>
+    <v>0.02</v>
+    <v>2.9240000000000001E-4</v>
     <v>USD</v>
     <v>Oil-Dri Corporation of America is a manufacturer and supplier of specialty sorbent products for pet care, animal health and nutrition, fluid purification, agricultural ingredients, sports field, industrial and automotive markets. Its principal product is cat litter. The Company’s Retail and Wholesale Products Group segment customers include mass merchandisers, the farm and fleet channel, drugstore chains, pet specialty retail outlets, dollar stores, retail grocery stores, distributors of industrial cleanup and automotive products, environmental service companies, sports field product users and marketers of consumer products. Its Business to Business Products Group segment customers include processors and refiners of edible oils, renewable diesel, petroleum-based oils and biodiesel fuel; manufacturers of animal feed and agricultural chemicals; and distributors of animal health and nutrition products. It is also a supplier of silica gel-based crystal cat litter.</v>
     <v>884</v>
@@ -5559,24 +5707,25 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>SUITE 400, 410 NORTH MICHIGAN AVENUE, CHICAGO, IL, 60611 US</v>
-    <v>68.58</v>
+    <v>69.370500000000007</v>
     <v>Chemicals</v>
     <v>Stock</v>
-    <v>45560.963326110941</v>
+    <v>45562.958333356248</v>
     <v>56</v>
-    <v>67.945599999999999</v>
-    <v>497000100</v>
+    <v>68.41</v>
+    <v>495251400</v>
     <v>OIL-DRI CORPORATION OF AMERICA</v>
     <v>OIL-DRI CORPORATION OF AMERICA</v>
+    <v>69.370500000000007</v>
+    <v>14.067299999999999</v>
     <v>68.33</v>
-    <v>13.9483</v>
-    <v>68.209999999999994</v>
-    <v>67.97</v>
+    <v>68.41</v>
+    <v>68.430000000000007</v>
     <v>7286320</v>
     <v>ODC</v>
     <v>OIL-DRI CORPORATION OF AMERICA (XNYS:ODC)</v>
-    <v>308</v>
-    <v>16969</v>
+    <v>6063</v>
+    <v>17000</v>
     <v>1969</v>
   </rv>
   <rv s="2">
@@ -5600,9 +5749,11 @@
     <v>Powered by Refinitiv</v>
     <v>170.9692</v>
     <v>93.77</v>
-    <v>1.5798000000000001</v>
-    <v>5.03</v>
-    <v>4.9435E-2</v>
+    <v>1.5789</v>
+    <v>-0.68</v>
+    <v>-6.293E-3</v>
+    <v>-0.70699999999999996</v>
+    <v>-6.5849999999999997E-3</v>
     <v>USD</v>
     <v>Axcelis Technologies, Inc. designs, manufactures and services ion implantation and other processing equipment used in the fabrication of semiconductor chips. The Company offers a complete line of high energy, high current and medium current implanters for all application requirements. In addition to equipment, the Company provides extensive aftermarket lifecycle products and services, including used tools, spare parts, equipment upgrades, maintenance services and customer training. Its Purion flagship systems are all based on a common platform, which enables a combination of implant purity, precision and productivity. Combining a single wafer end station, with advanced spot beam architectures (that ensures all points across the wafer see the same beam condition at the same beam angle), Purion products enable process control to optimize device performance and yield, at high productivity. The Company sells its products to semiconductor chip manufacturers around the world.</v>
     <v>1620</v>
@@ -5610,24 +5761,25 @@
     <v>XNAS</v>
     <v>XNAS</v>
     <v>108 Cherry Hill Dr, BEVERLY, MA, 01915 US</v>
-    <v>108.68</v>
+    <v>109.47</v>
     <v>Semiconductors &amp; Semiconductor Equipment</v>
     <v>Stock</v>
-    <v>45561.566945786719</v>
+    <v>45562.923512430469</v>
     <v>59</v>
-    <v>106.42319999999999</v>
-    <v>3482906260</v>
+    <v>106.76</v>
+    <v>3368418000</v>
     <v>AXCELIS TECHNOLOGIES, INC.</v>
     <v>AXCELIS TECHNOLOGIES, INC.</v>
-    <v>108.68</v>
-    <v>14.0182</v>
-    <v>101.75</v>
-    <v>106.78</v>
+    <v>109.01</v>
+    <v>14.7925</v>
+    <v>108.05</v>
+    <v>107.37</v>
+    <v>106.663</v>
     <v>32617590</v>
     <v>ACLS</v>
     <v>AXCELIS TECHNOLOGIES, INC. (XNAS:ACLS)</v>
-    <v>72145</v>
-    <v>632167</v>
+    <v>360862</v>
+    <v>652750</v>
     <v>1995</v>
   </rv>
   <rv s="2">
@@ -5651,9 +5803,11 @@
     <v>Powered by Refinitiv</v>
     <v>179.7</v>
     <v>63.9</v>
-    <v>0.89470000000000005</v>
-    <v>2.86</v>
-    <v>2.3799999999999998E-2</v>
+    <v>0.89480000000000004</v>
+    <v>-6.27</v>
+    <v>-4.9569000000000002E-2</v>
+    <v>-0.06</v>
+    <v>-4.9910000000000004E-4</v>
     <v>USD</v>
     <v>Dell Technologies Inc. is engaged in designing, developing, manufacturing, marketing, selling, and supporting a wide range of comprehensive and integrated solutions, products, and services. The Company operates through two segments: Infrastructure Solutions Group (ISG) and Client Solutions Group (CSG). Its ISG segment enables the Company’s customer’s digital transformation with solutions that address artificial intelligence (AI), machine learning, data analytics, and multi cloud environments. Its comprehensive storage portfolio includes modern and traditional storage solutions, including all-flash arrays, scale-out file, object platforms, hyper-converged infrastructure, and software-defined storage. Its CSG segment offers branded personal computers (PCs) including notebooks, desktops, and workstations and branded peripherals that include displays, docking stations, keyboards, mice, and webcam and audio devices, as well as third-party software and peripherals.</v>
     <v>120000</v>
@@ -5661,34 +5815,196 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>ONE DELL WAY, ROUND ROCK, TX, 78682 US</v>
-    <v>123.25</v>
+    <v>124.41</v>
     <v>Computers, Phones &amp; Household Electronics</v>
     <v>Stock</v>
-    <v>45561.566955532035</v>
+    <v>45562.999857407034</v>
     <v>62</v>
-    <v>122.17</v>
-    <v>82351200000</v>
+    <v>120.07</v>
+    <v>81055200000</v>
     <v>DELL TECHNOLOGIES INC.</v>
     <v>DELL TECHNOLOGIES INC.</v>
-    <v>122.17</v>
-    <v>22.111499999999999</v>
-    <v>120.17</v>
-    <v>123.03</v>
-    <v>701996500</v>
+    <v>124</v>
+    <v>22.131900000000002</v>
+    <v>126.49</v>
+    <v>120.22</v>
+    <v>120.16</v>
+    <v>702384800</v>
     <v>DELL</v>
     <v>DELL TECHNOLOGIES INC. (XNYS:DELL)</v>
-    <v>895414</v>
-    <v>13482060</v>
+    <v>13544967</v>
+    <v>13750305</v>
     <v>2013</v>
   </rv>
   <rv s="2">
     <v>63</v>
   </rv>
+  <rv s="0">
+    <v>https://www.bing.com/financeapi/forcetrigger?t=a1zqnm&amp;q=XNYS%3aPFE&amp;form=skydnc</v>
+    <v>Learn more on Bing</v>
+  </rv>
+  <rv s="4">
+    <v>7</v>
+    <v>PFIZER INC. (XNYS:PFE)</v>
+    <v>2</v>
+    <v>8</v>
+    <v>Finance</v>
+    <v>4</v>
+    <v>en-GB</v>
+    <v>a1zqnm</v>
+    <v>268435456</v>
+    <v>1</v>
+    <v>Powered by Refinitiv</v>
+    <v>34.11</v>
+    <v>25.2</v>
+    <v>0.65259999999999996</v>
+    <v>0.12</v>
+    <v>4.1419999999999998E-3</v>
+    <v>0.02</v>
+    <v>6.8750000000000007E-4</v>
+    <v>USD</v>
+    <v>Pfizer Inc. is a research-based global biopharmaceutical company. The Company is engaged in the discovery, development, manufacture, marketing, sale and distribution of biopharmaceutical products worldwide. Its Biopharma segment is engaged in the science-based biopharmaceutical business. Its Biopharma segment includes the Pfizer Oncology Division, the Pfizer U.S. Commercial Division, and the Pfizer International Commercial Division. Its product categories include oncology, primary care and specialty care. Its Oncology products include Ibrance, Xtandi, Inlyta, Bosulif, Lorbrena, Braftovi, Mektovi, Padcev, Adcetris, Talzenna, Tukysa, Elrexfio and Tivdak. Its primary care products include Eliquis, Nurtec ODT/Vydura, Comirnaty, the Prevnar family, Abrysvo, FSME/IMMUN-TicoVac, Paxlovid and Lucira by Pfizer. Its specialty care products include Xeljanz, Enbrel (outside the U.S. and Canada), Inflectra, Cibinqo, Litfulo, Vyndaqel family, Genotropin, Sulperazon, Zavicefta, Medrol and Panzyga.</v>
+    <v>88000</v>
+    <v>New York Stock Exchange</v>
+    <v>XNYS</v>
+    <v>XNYS</v>
+    <v>66 HUDSON BOULEVARD EAST, NEW YORK, NY, 10001-2192 US</v>
+    <v>29.23</v>
+    <v>Pharmaceuticals</v>
+    <v>Stock</v>
+    <v>45562.999659779685</v>
+    <v>65</v>
+    <v>28.92</v>
+    <v>170397500000</v>
+    <v>PFIZER INC.</v>
+    <v>PFIZER INC.</v>
+    <v>29.02</v>
+    <v>28.97</v>
+    <v>29.09</v>
+    <v>29.11</v>
+    <v>5666695000</v>
+    <v>PFE</v>
+    <v>PFIZER INC. (XNYS:PFE)</v>
+    <v>25013039</v>
+    <v>27953342</v>
+    <v>1942</v>
+  </rv>
+  <rv s="2">
+    <v>66</v>
+  </rv>
+  <rv s="0">
+    <v>https://www.bing.com/financeapi/forcetrigger?t=a1odgh&amp;q=XNYS%3aBEN&amp;form=skydnc</v>
+    <v>Learn more on Bing</v>
+  </rv>
+  <rv s="1">
+    <v>0</v>
+    <v>FRANKLIN RESOURCES, INC. (XNYS:BEN)</v>
+    <v>2</v>
+    <v>3</v>
+    <v>Finance</v>
+    <v>4</v>
+    <v>en-GB</v>
+    <v>a1odgh</v>
+    <v>268435456</v>
+    <v>1</v>
+    <v>Powered by Refinitiv</v>
+    <v>30.32</v>
+    <v>18.945</v>
+    <v>1.4086000000000001</v>
+    <v>0.14000000000000001</v>
+    <v>6.7800000000000004E-3</v>
+    <v>0.22</v>
+    <v>1.0582000000000001E-2</v>
+    <v>USD</v>
+    <v>Franklin Resources, Inc. is a global investment management company with subsidiaries operating as Franklin Templeton and serving clients in over 150 countries. It offers specialization on a global scale, bringing capabilities in fixed income, equity, alternatives and multi-asset solutions. The Company provides its investment management and related services to retail, institutional and high-net-worth investors in jurisdictions worldwide. Its investment products include sponsored funds, as well as institutional and high-net-worth separate accounts, retail separately managed account programs, sub-advised products, and other investment vehicles. Its funds include registered funds (including exchange-traded funds or ETFs) and unregistered funds. The Company offers its services and products under its various brand names, including Alcentra, K2, Benefit Street Partners, ClearBridge Investments, Martin Currie, O’Shaughnessy, and Lexington Partners. It also focuses on the retirement sector.</v>
+    <v>10300</v>
+    <v>New York Stock Exchange</v>
+    <v>XNYS</v>
+    <v>XNYS</v>
+    <v>One Franklin Parkway, Building 920/2, SAN MATEO, CA, 94403 US</v>
+    <v>21.065000000000001</v>
+    <v>Investment Banking &amp; Investment Services</v>
+    <v>Stock</v>
+    <v>45562.970611793753</v>
+    <v>68</v>
+    <v>20.68</v>
+    <v>10517500000</v>
+    <v>FRANKLIN RESOURCES, INC.</v>
+    <v>FRANKLIN RESOURCES, INC.</v>
+    <v>20.88</v>
+    <v>12.9894</v>
+    <v>20.65</v>
+    <v>20.79</v>
+    <v>21.01</v>
+    <v>522998400</v>
+    <v>BEN</v>
+    <v>FRANKLIN RESOURCES, INC. (XNYS:BEN)</v>
+    <v>2791502</v>
+    <v>5369841</v>
+    <v>1969</v>
+  </rv>
+  <rv s="2">
+    <v>69</v>
+  </rv>
+  <rv s="0">
+    <v>https://www.bing.com/financeapi/forcetrigger?t=a24uqh&amp;q=XNYS%3aUGI&amp;form=skydnc</v>
+    <v>Learn more on Bing</v>
+  </rv>
+  <rv s="1">
+    <v>0</v>
+    <v>UGI CORPORATION (XNYS:UGI)</v>
+    <v>2</v>
+    <v>3</v>
+    <v>Finance</v>
+    <v>4</v>
+    <v>en-GB</v>
+    <v>a24uqh</v>
+    <v>268435456</v>
+    <v>1</v>
+    <v>Powered by Refinitiv</v>
+    <v>26.15</v>
+    <v>20.190000000000001</v>
+    <v>1.1435</v>
+    <v>0.3</v>
+    <v>1.218E-2</v>
+    <v>0.02</v>
+    <v>8.0219999999999998E-4</v>
+    <v>USD</v>
+    <v>UGI Corporation is a holding company, which distributes, stores, transports and markets energy products and related services. In the United States, the Company owns and operates a retail propane marketing and distribution business, natural gas and electric distribution utilities, and energy marketing, midstream infrastructure, storage, natural gas gathering and processing, natural gas production, electricity generation and energy services businesses. In Europe, the Company markets and distributes propane and other liquified petroleum gas (LPG), and market other energy products and services. It operates through four segments: AmeriGas Propane, UGI International, Midstream &amp; Marketing, and Utilities. The AmeriGas Propane segment operates propane distribution business. The UGI International segment consists of LPG distribution businesses in Austria, Belgium, the Czech Republic, Denmark, Finland, France, Hungary, Italy, Luxembourg, the Netherlands, Norway, Poland, Romania and others.</v>
+    <v>5160</v>
+    <v>New York Stock Exchange</v>
+    <v>XNYS</v>
+    <v>XNYS</v>
+    <v>500 N GULPH RD, P O BOX 858, KING OF PRUSSIA, PA, 19406 US</v>
+    <v>25.085000000000001</v>
+    <v>Natural Gas Utilities</v>
+    <v>Stock</v>
+    <v>45562.958333333336</v>
+    <v>71</v>
+    <v>24.8</v>
+    <v>5158968000</v>
+    <v>UGI CORPORATION</v>
+    <v>UGI CORPORATION</v>
+    <v>24.84</v>
+    <v>7.9371999999999998</v>
+    <v>24.63</v>
+    <v>24.93</v>
+    <v>24.95</v>
+    <v>214688600</v>
+    <v>UGI</v>
+    <v>UGI CORPORATION (XNYS:UGI)</v>
+    <v>2134381</v>
+    <v>2047453</v>
+    <v>1991</v>
+  </rv>
+  <rv s="2">
+    <v>72</v>
+  </rv>
 </rvData>
 </file>
 
 <file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
-<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="4">
+<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="5">
   <s t="_hyperlink">
     <k n="Address" t="s"/>
     <k n="Text" t="s"/>
@@ -5710,6 +6026,8 @@
     <k n="Beta"/>
     <k n="Change"/>
     <k n="Change (%)"/>
+    <k n="Change (Extended hours)"/>
+    <k n="Change % (Extended hours)"/>
     <k n="Currency" t="s"/>
     <k n="Description" t="s"/>
     <k n="Employees"/>
@@ -5730,6 +6048,7 @@
     <k n="P/E"/>
     <k n="Previous close"/>
     <k n="Price"/>
+    <k n="Price (Extended hours)"/>
     <k n="Shares outstanding"/>
     <k n="Ticker symbol" t="s"/>
     <k n="UniqueName" t="s"/>
@@ -5757,6 +6076,8 @@
     <k n="Beta"/>
     <k n="Change"/>
     <k n="Change (%)"/>
+    <k n="Change (Extended hours)"/>
+    <k n="Change % (Extended hours)"/>
     <k n="Currency" t="s"/>
     <k n="Description" t="s"/>
     <k n="Employees"/>
@@ -5776,6 +6097,53 @@
     <k n="P/E"/>
     <k n="Previous close"/>
     <k n="Price"/>
+    <k n="Price (Extended hours)"/>
+    <k n="Shares outstanding"/>
+    <k n="Ticker symbol" t="s"/>
+    <k n="UniqueName" t="s"/>
+    <k n="Volume"/>
+    <k n="Volume average"/>
+    <k n="Year incorporated"/>
+  </s>
+  <s t="_linkedentitycore">
+    <k n="_Display" t="spb"/>
+    <k n="_DisplayString" t="s"/>
+    <k n="_Flags" t="spb"/>
+    <k n="_Format" t="spb"/>
+    <k n="_Icon" t="s"/>
+    <k n="_SubLabel" t="spb"/>
+    <k n="%EntityCulture" t="s"/>
+    <k n="%EntityId" t="s"/>
+    <k n="%EntityServiceId"/>
+    <k n="%IsRefreshable" t="b"/>
+    <k n="%ProviderInfo" t="s"/>
+    <k n="52 week high"/>
+    <k n="52 week low"/>
+    <k n="Beta"/>
+    <k n="Change"/>
+    <k n="Change (%)"/>
+    <k n="Change (Extended hours)"/>
+    <k n="Change % (Extended hours)"/>
+    <k n="Currency" t="s"/>
+    <k n="Description" t="s"/>
+    <k n="Employees"/>
+    <k n="Exchange" t="s"/>
+    <k n="Exchange abbreviation" t="s"/>
+    <k n="ExchangeID" t="s"/>
+    <k n="Headquarters" t="s"/>
+    <k n="High"/>
+    <k n="Industry" t="s"/>
+    <k n="Instrument type" t="s"/>
+    <k n="Last trade time"/>
+    <k n="LearnMoreOnLink" t="r"/>
+    <k n="Low"/>
+    <k n="Market cap"/>
+    <k n="Name" t="s"/>
+    <k n="Official name" t="s"/>
+    <k n="Open"/>
+    <k n="Previous close"/>
+    <k n="Price"/>
+    <k n="Price (Extended hours)"/>
     <k n="Shares outstanding"/>
     <k n="Ticker symbol" t="s"/>
     <k n="UniqueName" t="s"/>
@@ -5788,8 +6156,8 @@
 
 <file path=xl/richData/rdsupportingpropertybag.xml><?xml version="1.0" encoding="utf-8"?>
 <supportingPropertyBags xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2">
-  <spbArrays count="2">
-    <a count="42">
+  <spbArrays count="3">
+    <a count="45">
       <v t="s">%EntityServiceId</v>
       <v t="s">_Format</v>
       <v t="s">%IsRefreshable</v>
@@ -5800,13 +6168,16 @@
       <v t="s">Name</v>
       <v t="s">_SubLabel</v>
       <v t="s">Price</v>
+      <v t="s">Price (Extended hours)</v>
       <v t="s">Exchange</v>
       <v t="s">Official name</v>
       <v t="s">Last trade time</v>
       <v t="s">Ticker symbol</v>
       <v t="s">Exchange abbreviation</v>
       <v t="s">Change</v>
+      <v t="s">Change (Extended hours)</v>
       <v t="s">Change (%)</v>
+      <v t="s">Change % (Extended hours)</v>
       <v t="s">Currency</v>
       <v t="s">Previous close</v>
       <v t="s">Open</v>
@@ -5833,7 +6204,7 @@
       <v t="s">ExchangeID</v>
       <v t="s">%ProviderInfo</v>
     </a>
-    <a count="41">
+    <a count="44">
       <v t="s">%EntityServiceId</v>
       <v t="s">_Format</v>
       <v t="s">%IsRefreshable</v>
@@ -5844,13 +6215,16 @@
       <v t="s">Name</v>
       <v t="s">_SubLabel</v>
       <v t="s">Price</v>
+      <v t="s">Price (Extended hours)</v>
       <v t="s">Exchange</v>
       <v t="s">Official name</v>
       <v t="s">Last trade time</v>
       <v t="s">Ticker symbol</v>
       <v t="s">Exchange abbreviation</v>
       <v t="s">Change</v>
+      <v t="s">Change (Extended hours)</v>
       <v t="s">Change (%)</v>
+      <v t="s">Change % (Extended hours)</v>
       <v t="s">Currency</v>
       <v t="s">Previous close</v>
       <v t="s">Open</v>
@@ -5876,8 +6250,54 @@
       <v t="s">ExchangeID</v>
       <v t="s">%ProviderInfo</v>
     </a>
+    <a count="44">
+      <v t="s">%EntityServiceId</v>
+      <v t="s">_Format</v>
+      <v t="s">%IsRefreshable</v>
+      <v t="s">%EntityCulture</v>
+      <v t="s">%EntityId</v>
+      <v t="s">_Icon</v>
+      <v t="s">_Display</v>
+      <v t="s">Name</v>
+      <v t="s">_SubLabel</v>
+      <v t="s">Price</v>
+      <v t="s">Price (Extended hours)</v>
+      <v t="s">Exchange</v>
+      <v t="s">Official name</v>
+      <v t="s">Last trade time</v>
+      <v t="s">Ticker symbol</v>
+      <v t="s">Exchange abbreviation</v>
+      <v t="s">Change</v>
+      <v t="s">Change (Extended hours)</v>
+      <v t="s">Change (%)</v>
+      <v t="s">Change % (Extended hours)</v>
+      <v t="s">Currency</v>
+      <v t="s">Previous close</v>
+      <v t="s">Open</v>
+      <v t="s">High</v>
+      <v t="s">Low</v>
+      <v t="s">52 week high</v>
+      <v t="s">52 week low</v>
+      <v t="s">Volume</v>
+      <v t="s">Volume average</v>
+      <v t="s">Market cap</v>
+      <v t="s">Beta</v>
+      <v t="s">Shares outstanding</v>
+      <v t="s">Description</v>
+      <v t="s">Employees</v>
+      <v t="s">Headquarters</v>
+      <v t="s">Industry</v>
+      <v t="s">Instrument type</v>
+      <v t="s">Year incorporated</v>
+      <v t="s">_Flags</v>
+      <v t="s">UniqueName</v>
+      <v t="s">_DisplayString</v>
+      <v t="s">LearnMoreOnLink</v>
+      <v t="s">ExchangeID</v>
+      <v t="s">%ProviderInfo</v>
+    </a>
   </spbArrays>
-  <spbData count="7">
+  <spbData count="9">
     <spb s="0">
       <v>0</v>
       <v>Name</v>
@@ -5915,13 +6335,19 @@
       <v>8</v>
       <v>9</v>
       <v>4</v>
+      <v>1</v>
+      <v>1</v>
+      <v>5</v>
     </spb>
     <spb s="4">
-      <v>Real-Time Nasdaq Last Sale</v>
+      <v>at close</v>
       <v>from previous close</v>
       <v>from previous close</v>
       <v>Source: Nasdaq Last Sale</v>
       <v>GMT</v>
+      <v>Real-Time Nasdaq Last Sale</v>
+      <v>from close</v>
+      <v>from close</v>
     </spb>
     <spb s="5">
       <v>1</v>
@@ -5932,12 +6358,41 @@
       <v>1</v>
       <v>1</v>
     </spb>
+    <spb s="0">
+      <v>2</v>
+      <v>Name</v>
+      <v>LearnMoreOnLink</v>
+    </spb>
+    <spb s="7">
+      <v>1</v>
+      <v>2</v>
+      <v>1</v>
+      <v>3</v>
+      <v>1</v>
+      <v>1</v>
+      <v>1</v>
+      <v>4</v>
+      <v>4</v>
+      <v>5</v>
+      <v>6</v>
+      <v>1</v>
+      <v>1</v>
+      <v>1</v>
+      <v>4</v>
+      <v>7</v>
+      <v>8</v>
+      <v>9</v>
+      <v>4</v>
+      <v>1</v>
+      <v>1</v>
+      <v>5</v>
+    </spb>
   </spbData>
 </supportingPropertyBags>
 </file>
 
 <file path=xl/richData/rdsupportingpropertybagstructure.xml><?xml version="1.0" encoding="utf-8"?>
-<spbStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" count="7">
+<spbStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" count="8">
   <s>
     <k n="^Order" t="spba"/>
     <k n="TitleProperty" t="s"/>
@@ -5975,6 +6430,9 @@
     <k n="Year incorporated" t="i"/>
     <k n="`%EntityServiceId" t="i"/>
     <k n="Shares outstanding" t="i"/>
+    <k n="Price (Extended hours)" t="i"/>
+    <k n="Change (Extended hours)" t="i"/>
+    <k n="Change % (Extended hours)" t="i"/>
   </s>
   <s>
     <k n="Price" t="s"/>
@@ -5982,6 +6440,9 @@
     <k n="Change (%)" t="s"/>
     <k n="ExchangeID" t="s"/>
     <k n="Last trade time" t="s"/>
+    <k n="Price (Extended hours)" t="s"/>
+    <k n="Change (Extended hours)" t="s"/>
+    <k n="Change % (Extended hours)" t="s"/>
   </s>
   <s>
     <k n="^Order" t="spba"/>
@@ -5991,6 +6452,30 @@
     <k n="ExchangeID" t="spb"/>
     <k n="UniqueName" t="spb"/>
     <k n="`%ProviderInfo" t="spb"/>
+  </s>
+  <s>
+    <k n="Low" t="i"/>
+    <k n="Beta" t="i"/>
+    <k n="High" t="i"/>
+    <k n="Name" t="i"/>
+    <k n="Open" t="i"/>
+    <k n="Price" t="i"/>
+    <k n="Change" t="i"/>
+    <k n="Volume" t="i"/>
+    <k n="Employees" t="i"/>
+    <k n="Change (%)" t="i"/>
+    <k n="Market cap" t="i"/>
+    <k n="52 week low" t="i"/>
+    <k n="52 week high" t="i"/>
+    <k n="Previous close" t="i"/>
+    <k n="Volume average" t="i"/>
+    <k n="Last trade time" t="i"/>
+    <k n="Year incorporated" t="i"/>
+    <k n="`%EntityServiceId" t="i"/>
+    <k n="Shares outstanding" t="i"/>
+    <k n="Price (Extended hours)" t="i"/>
+    <k n="Change (Extended hours)" t="i"/>
+    <k n="Change % (Extended hours)" t="i"/>
   </s>
 </spbStructures>
 </file>
@@ -6005,7 +6490,7 @@
       <x:numFmt numFmtId="0" formatCode="General"/>
     </x:dxf>
     <x:dxf>
-      <x:numFmt numFmtId="27" formatCode="dd/mm/yyyy\ h:mm"/>
+      <x:numFmt numFmtId="27" formatCode="m/d/yy\ h:mm"/>
     </x:dxf>
     <x:dxf>
       <x:numFmt numFmtId="14" formatCode="0.00%"/>
@@ -6053,8 +6538,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4AEE35AE-5B0D-FE48-BB2D-FD669C9DCA16}" name="Portfolio" displayName="Portfolio" ref="B2:K24" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
-  <autoFilter ref="B2:K24" xr:uid="{4AEE35AE-5B0D-FE48-BB2D-FD669C9DCA16}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4AEE35AE-5B0D-FE48-BB2D-FD669C9DCA16}" name="Portfolio" displayName="Portfolio" ref="B2:K27" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+  <autoFilter ref="B2:K27" xr:uid="{4AEE35AE-5B0D-FE48-BB2D-FD669C9DCA16}"/>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{0445D94A-6FCB-7D4D-96B6-8AA18900F668}" name="Company" dataDxfId="15"/>
     <tableColumn id="8" xr3:uid="{D4CC5B63-9F41-F843-9F6B-16BF8366EF76}" name="Name" dataDxfId="14">
@@ -40442,7 +40927,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:X1011"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A16" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
@@ -69405,10 +69890,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F51CD2FE-0785-5E4C-91F5-512BDFA3DC54}">
-  <dimension ref="B1:L26"/>
+  <dimension ref="B1:L30"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
@@ -69491,15 +69976,15 @@
       </c>
       <c r="I3" s="149" cm="1">
         <f t="array" aca="1" ref="I3" ca="1">_FV(B3,"Price")</f>
-        <v>58.79</v>
+        <v>61.38</v>
       </c>
       <c r="J3" s="129">
         <f t="shared" ref="J3:J24" ca="1" si="0">((I3-F3)/F3)</f>
-        <v>-0.14487272727272729</v>
+        <v>-0.10719999999999996</v>
       </c>
       <c r="K3" s="170">
         <f t="shared" ref="K3:K24" ca="1" si="1">(I3*G3) - H3</f>
-        <v>-72.609027999999967</v>
+        <v>-53.736215999999956</v>
       </c>
       <c r="L3"/>
     </row>
@@ -69530,15 +70015,15 @@
       </c>
       <c r="I4" s="149" cm="1">
         <f t="array" aca="1" ref="I4" ca="1">_FV(B4,"Price")</f>
-        <v>149.11750000000001</v>
+        <v>144.31</v>
       </c>
       <c r="J4" s="129">
         <f t="shared" ca="1" si="0"/>
-        <v>0.49087682463507309</v>
+        <v>0.44281143771245757</v>
       </c>
       <c r="K4" s="170">
         <f t="shared" ca="1" si="1"/>
-        <v>245.9295575000001</v>
+        <v>221.84879000000001</v>
       </c>
       <c r="L4"/>
     </row>
@@ -69569,15 +70054,15 @@
       </c>
       <c r="I5" s="149" cm="1">
         <f t="array" aca="1" ref="I5" ca="1">_FV(B5,"Price")</f>
-        <v>19.03</v>
+        <v>19.100000000000001</v>
       </c>
       <c r="J5" s="129">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.1270642201834862</v>
+        <v>-0.12385321100917428</v>
       </c>
       <c r="K5" s="170">
         <f t="shared" ca="1" si="1"/>
-        <v>-63.705824000000007</v>
+        <v>-62.097280000000012</v>
       </c>
       <c r="L5"/>
     </row>
@@ -69608,15 +70093,15 @@
       </c>
       <c r="I6" s="149" cm="1">
         <f t="array" aca="1" ref="I6" ca="1">_FV(B6,"Price")</f>
-        <v>22.11</v>
+        <v>22.17</v>
       </c>
       <c r="J6" s="129">
         <f t="shared" ca="1" si="0"/>
-        <v>0.2634285714285714</v>
+        <v>0.26685714285714296</v>
       </c>
       <c r="K6" s="170">
         <f t="shared" ca="1" si="1"/>
-        <v>145.85900399999991</v>
+        <v>147.61438800000008</v>
       </c>
       <c r="L6"/>
     </row>
@@ -69647,15 +70132,15 @@
       </c>
       <c r="I7" s="151" cm="1">
         <f t="array" aca="1" ref="I7" ca="1">_FV(B7,"Price")</f>
-        <v>226.87</v>
+        <v>227.79</v>
       </c>
       <c r="J7" s="129">
         <f t="shared" ca="1" si="0"/>
-        <v>0.28567380709509232</v>
+        <v>0.29088745324719473</v>
       </c>
       <c r="K7" s="170">
         <f t="shared" ca="1" si="1"/>
-        <v>143.12661700000001</v>
+        <v>145.73858900000005</v>
       </c>
       <c r="L7"/>
     </row>
@@ -69686,15 +70171,15 @@
       </c>
       <c r="I8" s="151" cm="1">
         <f t="array" aca="1" ref="I8" ca="1">_FV(B8,"Price")</f>
-        <v>95.4</v>
+        <v>96.5</v>
       </c>
       <c r="J8" s="129">
         <f t="shared" ca="1" si="0"/>
-        <v>0.69932312076950487</v>
+        <v>0.71891699323120772</v>
       </c>
       <c r="K8" s="170">
         <f t="shared" ca="1" si="1"/>
-        <v>350.29236000000014</v>
+        <v>360.10810000000004</v>
       </c>
       <c r="L8"/>
     </row>
@@ -69725,15 +70210,15 @@
       </c>
       <c r="I9" s="151" cm="1">
         <f t="array" aca="1" ref="I9" ca="1">_FV(B9,"Price")</f>
-        <v>17.760000000000002</v>
+        <v>17.86</v>
       </c>
       <c r="J9" s="129">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.47111375818939838</v>
+        <v>-0.46813579511614056</v>
       </c>
       <c r="K9" s="170">
         <f t="shared" ca="1" si="1"/>
-        <v>-236.00481600000001</v>
+        <v>-234.51272600000004</v>
       </c>
       <c r="L9"/>
     </row>
@@ -69764,15 +70249,15 @@
       </c>
       <c r="I10" s="153" cm="1">
         <f t="array" aca="1" ref="I10" ca="1">_FV(B10,"Price")</f>
-        <v>61.01</v>
+        <v>63.73</v>
       </c>
       <c r="J10" s="129">
         <f t="shared" ca="1" si="0"/>
-        <v>4.8281786941580668E-2</v>
+        <v>9.5017182130584091E-2</v>
       </c>
       <c r="K10" s="170">
         <f t="shared" ca="1" si="1"/>
-        <v>24.210685999999896</v>
+        <v>47.626077999999893</v>
       </c>
       <c r="L10"/>
     </row>
@@ -69803,15 +70288,15 @@
       </c>
       <c r="I11" s="153" cm="1">
         <f t="array" aca="1" ref="I11" ca="1">_FV(B11,"Price")</f>
-        <v>85.52</v>
+        <v>84.95</v>
       </c>
       <c r="J11" s="129">
         <f t="shared" ca="1" si="0"/>
-        <v>-6.2999890434973158E-2</v>
+        <v>-6.9245096965048686E-2</v>
       </c>
       <c r="K11" s="170">
         <f t="shared" ca="1" si="1"/>
-        <v>-31.580720000000042</v>
+        <v>-34.709450000000004</v>
       </c>
       <c r="L11"/>
     </row>
@@ -69842,15 +70327,15 @@
       </c>
       <c r="I12" s="153" cm="1">
         <f t="array" aca="1" ref="I12" ca="1">_FV(B12,"Price")</f>
-        <v>104.6</v>
+        <v>104.33</v>
       </c>
       <c r="J12" s="129">
         <f t="shared" ca="1" si="0"/>
-        <v>0.24970131421744313</v>
+        <v>0.24647550776583027</v>
       </c>
       <c r="K12" s="170">
         <f t="shared" ca="1" si="1"/>
-        <v>125.08330000000001</v>
+        <v>123.46721500000001</v>
       </c>
       <c r="L12"/>
     </row>
@@ -69881,15 +70366,15 @@
       </c>
       <c r="I13" s="153" cm="1">
         <f t="array" aca="1" ref="I13" ca="1">_FV(B13,"Price")</f>
-        <v>95.73</v>
+        <v>98.31</v>
       </c>
       <c r="J13" s="129">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.18158502180046163</v>
+        <v>-0.15952808412413436</v>
       </c>
       <c r="K13" s="170">
         <f t="shared" ca="1" si="1"/>
-        <v>-90.978836999999999</v>
+        <v>-79.928438999999969</v>
       </c>
       <c r="L13"/>
     </row>
@@ -69920,15 +70405,15 @@
       </c>
       <c r="I14" s="155" cm="1">
         <f t="array" aca="1" ref="I14" ca="1">_FV(B14,"Price")</f>
-        <v>26.785</v>
+        <v>26.51</v>
       </c>
       <c r="J14" s="129">
         <f t="shared" ca="1" si="0"/>
-        <v>5.0804236955668956E-2</v>
+        <v>4.0015692428403422E-2</v>
       </c>
       <c r="K14" s="170">
         <f t="shared" ca="1" si="1"/>
-        <v>25.485959999999977</v>
+        <v>20.080559999999991</v>
       </c>
       <c r="L14"/>
     </row>
@@ -69959,15 +70444,15 @@
       </c>
       <c r="I15" s="155" cm="1">
         <f t="array" aca="1" ref="I15" ca="1">_FV(B15,"Price")</f>
-        <v>13.164999999999999</v>
+        <v>13.14</v>
       </c>
       <c r="J15" s="129">
         <f t="shared" ca="1" si="0"/>
-        <v>0.5011402508551881</v>
+        <v>0.49828962371721791</v>
       </c>
       <c r="K15" s="170">
         <f t="shared" ca="1" si="1"/>
-        <v>250.85446649999994</v>
+        <v>249.42671400000006</v>
       </c>
       <c r="L15"/>
     </row>
@@ -69998,15 +70483,15 @@
       </c>
       <c r="I16" s="157" cm="1">
         <f t="array" aca="1" ref="I16" ca="1">_FV(B16,"Price")</f>
-        <v>38.335000000000001</v>
+        <v>38.9</v>
       </c>
       <c r="J16" s="129">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.20991343775762575</v>
+        <v>-0.19826875515251452</v>
       </c>
       <c r="K16" s="170">
         <f t="shared" ca="1" si="1"/>
-        <v>-101.79999999999995</v>
+        <v>-96.149999999999977</v>
       </c>
       <c r="L16"/>
     </row>
@@ -70037,15 +70522,15 @@
       </c>
       <c r="I17" s="157" cm="1">
         <f t="array" aca="1" ref="I17" ca="1">_FV(B17,"Price")</f>
-        <v>77.69</v>
+        <v>78.92</v>
       </c>
       <c r="J17" s="129">
         <f t="shared" ca="1" si="0"/>
-        <v>0.1106504646175839</v>
+        <v>0.12823445318084345</v>
       </c>
       <c r="K17" s="170">
         <f t="shared" ca="1" si="1"/>
-        <v>54.189999999999941</v>
+        <v>62.800000000000068</v>
       </c>
       <c r="L17"/>
     </row>
@@ -70076,15 +70561,15 @@
       </c>
       <c r="I18" s="157" cm="1">
         <f t="array" aca="1" ref="I18" ca="1">_FV(B18,"Price")</f>
-        <v>60.99</v>
+        <v>60.2</v>
       </c>
       <c r="J18" s="129">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.913798649083303E-2</v>
+        <v>-3.1843036346091938E-2</v>
       </c>
       <c r="K18" s="170">
         <f t="shared" ca="1" si="1"/>
-        <v>-9.5199999999999818</v>
+        <v>-15.839999999999975</v>
       </c>
       <c r="L18"/>
     </row>
@@ -70115,15 +70600,15 @@
       </c>
       <c r="I19" s="157" cm="1">
         <f t="array" aca="1" ref="I19" ca="1">_FV(B19,"Price")</f>
-        <v>10.029999999999999</v>
+        <v>10.27</v>
       </c>
       <c r="J19" s="129">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.25149253731343291</v>
+        <v>-0.23358208955223886</v>
       </c>
       <c r="K19" s="170">
         <f t="shared" ca="1" si="1"/>
-        <v>-126.04851000000002</v>
+        <v>-117.07659000000001</v>
       </c>
       <c r="L19"/>
     </row>
@@ -70154,15 +70639,15 @@
       </c>
       <c r="I20" s="211" cm="1">
         <f t="array" aca="1" ref="I20" ca="1">_FV(B20,"Price")</f>
-        <v>410</v>
+        <v>404.01</v>
       </c>
       <c r="J20" s="129">
         <f t="shared" ca="1" si="0"/>
-        <v>4.219623792577535E-2</v>
+        <v>2.6970005083884124E-2</v>
       </c>
       <c r="K20" s="170">
         <f t="shared" ca="1" si="1"/>
-        <v>21.239999999999952</v>
+        <v>13.572799999999972</v>
       </c>
       <c r="L20"/>
     </row>
@@ -70193,15 +70678,15 @@
       </c>
       <c r="I21" s="214" cm="1">
         <f t="array" aca="1" ref="I21" ca="1">_FV(B21,"Price")</f>
-        <v>21.84</v>
+        <v>21.73</v>
       </c>
       <c r="J21" s="129">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.8867924528301962E-2</v>
+        <v>-2.380952380952386E-2</v>
       </c>
       <c r="K21" s="170">
         <f t="shared" ca="1" si="1"/>
-        <v>-9.4580400000000395</v>
+        <v>-11.933755000000019</v>
       </c>
     </row>
     <row r="22" spans="2:12">
@@ -70231,15 +70716,15 @@
       </c>
       <c r="I22" s="214" cm="1">
         <f t="array" aca="1" ref="I22" ca="1">_FV(B22,"Price")</f>
-        <v>67.97</v>
+        <v>68.41</v>
       </c>
       <c r="J22" s="129">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.3980470993681818E-2</v>
+        <v>-1.7662263067202814E-2</v>
       </c>
       <c r="K22" s="170">
         <f t="shared" ca="1" si="1"/>
-        <v>-10.606841000000031</v>
+        <v>-7.432373000000041</v>
       </c>
     </row>
     <row r="23" spans="2:12">
@@ -70269,15 +70754,15 @@
       </c>
       <c r="I23" s="214" cm="1">
         <f t="array" aca="1" ref="I23" ca="1">_FV(B23,"Price")</f>
-        <v>106.78</v>
+        <v>107.37</v>
       </c>
       <c r="J23" s="129">
         <f t="shared" ca="1" si="0"/>
-        <v>5.5868683872243703E-2</v>
+        <v>6.1702758825274491E-2</v>
       </c>
       <c r="K23" s="170">
         <f t="shared" ca="1" si="1"/>
-        <v>28.00879800000007</v>
+        <v>30.931717000000049</v>
       </c>
     </row>
     <row r="24" spans="2:12">
@@ -70307,21 +70792,117 @@
       </c>
       <c r="I24" s="214" cm="1">
         <f t="array" aca="1" ref="I24" ca="1">_FV(B24,"Price")</f>
-        <v>123.03</v>
+        <v>120.22</v>
       </c>
       <c r="J24" s="129">
         <f t="shared" ca="1" si="0"/>
-        <v>4.1039092909121631E-2</v>
+        <v>1.7261804027754204E-2</v>
       </c>
       <c r="K24" s="170">
         <f t="shared" ca="1" si="1"/>
-        <v>20.573382000000038</v>
-      </c>
-    </row>
-    <row r="26" spans="2:12" ht="13">
-      <c r="K26" s="169">
-        <f ca="1">SUM(K3:K24)</f>
-        <v>682.54151500000012</v>
+        <v>8.6606679999999869</v>
+      </c>
+    </row>
+    <row r="25" spans="2:12">
+      <c r="B25" s="220" t="e" vm="23">
+        <v>#VALUE!</v>
+      </c>
+      <c r="C25" s="220" t="str" cm="1">
+        <f t="array" aca="1" ref="C25" ca="1">_FV(Portfolio[[#This Row],[Company]],"Name")</f>
+        <v>PFIZER INC.</v>
+      </c>
+      <c r="D25" s="221" t="str" cm="1">
+        <f t="array" aca="1" ref="D25" ca="1">_FV(B25,"Ticker symbol",TRUE)</f>
+        <v>PFE</v>
+      </c>
+      <c r="E25" s="221" t="str" cm="1">
+        <f t="array" aca="1" ref="E25" ca="1">_FV(B25,"Industry")</f>
+        <v>Pharmaceuticals</v>
+      </c>
+      <c r="F25" s="222"/>
+      <c r="G25" s="222"/>
+      <c r="H25" s="223"/>
+      <c r="I25" s="224" cm="1">
+        <f t="array" aca="1" ref="I25" ca="1">_FV(B25,"Price")</f>
+        <v>29.09</v>
+      </c>
+      <c r="J25" s="219" t="e">
+        <f ca="1">((I25-F25)/F25)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K25" s="206">
+        <f ca="1">(I25*G25) - H25</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="2:12">
+      <c r="B26" s="220" t="e" vm="24">
+        <v>#VALUE!</v>
+      </c>
+      <c r="C26" s="220" t="str" cm="1">
+        <f t="array" aca="1" ref="C26" ca="1">_FV(Portfolio[[#This Row],[Company]],"Name")</f>
+        <v>FRANKLIN RESOURCES, INC.</v>
+      </c>
+      <c r="D26" s="221" t="str" cm="1">
+        <f t="array" aca="1" ref="D26" ca="1">_FV(B26,"Ticker symbol",TRUE)</f>
+        <v>BEN</v>
+      </c>
+      <c r="E26" s="221" t="str" cm="1">
+        <f t="array" aca="1" ref="E26" ca="1">_FV(B26,"Industry")</f>
+        <v>Investment Banking &amp; Investment Services</v>
+      </c>
+      <c r="F26" s="222"/>
+      <c r="G26" s="222"/>
+      <c r="H26" s="223"/>
+      <c r="I26" s="224" cm="1">
+        <f t="array" aca="1" ref="I26" ca="1">_FV(B26,"Price")</f>
+        <v>20.79</v>
+      </c>
+      <c r="J26" s="219" t="e">
+        <f ca="1">((I26-F26)/F26)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K26" s="206">
+        <f ca="1">(I26*G26) - H26</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="2:12">
+      <c r="B27" s="220" t="e" vm="25">
+        <v>#VALUE!</v>
+      </c>
+      <c r="C27" s="220" t="str" cm="1">
+        <f t="array" aca="1" ref="C27" ca="1">_FV(Portfolio[[#This Row],[Company]],"Name")</f>
+        <v>UGI CORPORATION</v>
+      </c>
+      <c r="D27" s="221" t="str" cm="1">
+        <f t="array" aca="1" ref="D27" ca="1">_FV(B27,"Ticker symbol",TRUE)</f>
+        <v>UGI</v>
+      </c>
+      <c r="E27" s="221" t="str" cm="1">
+        <f t="array" aca="1" ref="E27" ca="1">_FV(B27,"Industry")</f>
+        <v>Natural Gas Utilities</v>
+      </c>
+      <c r="F27" s="222"/>
+      <c r="G27" s="222"/>
+      <c r="H27" s="223"/>
+      <c r="I27" s="224" cm="1">
+        <f t="array" aca="1" ref="I27" ca="1">_FV(B27,"Price")</f>
+        <v>24.93</v>
+      </c>
+      <c r="J27" s="219" t="e">
+        <f ca="1">((I27-F27)/F27)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K27" s="206">
+        <f ca="1">(I27*G27) - H27</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="2:12" ht="13">
+      <c r="K30" s="169">
+        <f ca="1">SUM(K3:K27)</f>
+        <v>718.45879000000025</v>
       </c>
     </row>
   </sheetData>
@@ -70341,7 +70922,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K26">
+  <conditionalFormatting sqref="K30">
     <cfRule type="cellIs" dxfId="1" priority="5" operator="lessThan">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
vault backup: 2024-09-30 14:29:22
</commit_message>
<xml_diff>
--- a/_system/Attachments/Portfolio Management.xlsx
+++ b/_system/Attachments/Portfolio Management.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martin/repos/tomesink/obsidian/_system/Attachments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2EEE7EA-4F86-EF46-BF0F-CF730356E1A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{175DB0B3-41FA-464D-80D2-959ED039FBF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2120" yWindow="500" windowWidth="34980" windowHeight="19340" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="39400" yWindow="900" windowWidth="34980" windowHeight="19340" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Stocks Performance" sheetId="1" r:id="rId1"/>
@@ -841,7 +841,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="11">
+  <numFmts count="12">
     <numFmt numFmtId="164" formatCode="[$$-409]\ #,##0.00"/>
     <numFmt numFmtId="165" formatCode="[$£-809]\ #,##0.00"/>
     <numFmt numFmtId="166" formatCode="[$$-409]\ #,##0"/>
@@ -853,6 +853,7 @@
     <numFmt numFmtId="172" formatCode="#,##0.00\ &quot;CZK&quot;"/>
     <numFmt numFmtId="173" formatCode="[$$-409]#,##0.00"/>
     <numFmt numFmtId="174" formatCode="0.0000"/>
+    <numFmt numFmtId="180" formatCode="[$$-409]\ #,##0.0000"/>
   </numFmts>
   <fonts count="16">
     <font>
@@ -953,7 +954,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1136,12 +1137,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF7030A0"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1153,7 +1148,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="43">
+  <borders count="42">
     <border>
       <left/>
       <right/>
@@ -1708,23 +1703,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="225">
+  <cellXfs count="226">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -2264,22 +2248,25 @@
     <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="10" fontId="9" fillId="31" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="31" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="33" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="173" fontId="15" fillId="33" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="31" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="15" fillId="32" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="173" fontId="15" fillId="32" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="31" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="15" fillId="32" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="174" fontId="15" fillId="32" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -4677,8 +4664,6 @@
     <v>0.5292</v>
     <v>2.37</v>
     <v>4.0163000000000004E-2</v>
-    <v>0.1</v>
-    <v>1.6289999999999998E-3</v>
     <v>USD</v>
     <v>CVS Health Corporation is a health solutions company. The Company operates in four segments: Health Care Benefits, Health Services, Pharmacy &amp; Consumer Wellness, and Corporate/Other. Its Health Care Benefits segment offer a range of traditional, voluntary and consumer-directed health insurance products and related services, including medical, pharmacy, dental and behavioral health plans, medical management capabilities, Medicare Advantage and Medicare supplement plans, and Medicaid health care management services. Its Health Services segment provides a full range of pharmacy benefit management solutions, delivers health care services in its medical clinics, virtually, and in the home, and offers provider enablement solutions. The Pharmacy &amp; Consumer Wellness segment dispenses prescriptions in its retail pharmacies and through its infusion operations, provides ancillary pharmacy services, including pharmacy patient care programs, diagnostic testing and vaccination administration.</v>
     <v>300000</v>
@@ -4696,14 +4681,13 @@
     <v>CVS HEALTH CORPORATION</v>
     <v>CVS HEALTH CORPORATION</v>
     <v>59.45</v>
-    <v>10.926399999999999</v>
+    <v>10.9229</v>
     <v>59.01</v>
     <v>61.38</v>
-    <v>61.48</v>
     <v>1257979000</v>
     <v>CVS</v>
     <v>CVS HEALTH CORPORATION (XNYS:CVS)</v>
-    <v>12510217</v>
+    <v>134971</v>
     <v>8081310</v>
     <v>1996</v>
   </rv>
@@ -4731,8 +4715,6 @@
     <v>1.9942</v>
     <v>-3.09</v>
     <v>-2.0962999999999999E-2</v>
-    <v>0.2505</v>
-    <v>1.7360000000000001E-3</v>
     <v>USD</v>
     <v>Crocs, Inc. is engaged in the design, development, worldwide marketing, distribution, and sale of casual lifestyle footwear and accessories for women, men, and children. The Company’s segments include Crocs Brand and the HEYDUDE Brand. The Company’s Crocs Brand collection contains Croslite material, a molded footwear technology, delivering extraordinary comfort with each step. Its Croslite materials are formulated to create soft, comfortable, lightweight, non-marking, and odor-resistant footwear. The HEYDUDE Brand offers shoes with a versatile silhouette. It sells its products in more than 80 countries, through two distribution channels: wholesale and direct-to-consumer. Its wholesale channel includes domestic and international multi-brand retailers, mono-branded partner stores, e-tailers, and distributors; its direct-to-consumer channel includes Company-operated retail stores, Company-operated e-commerce sites, and third-party marketplaces.</v>
     <v>7030</v>
@@ -4750,14 +4732,13 @@
     <v>CROCS, INC.</v>
     <v>CROCS, INC.</v>
     <v>148.01</v>
-    <v>10.853199999999999</v>
+    <v>10.853300000000001</v>
     <v>147.4</v>
     <v>144.31</v>
-    <v>144.56049999999999</v>
     <v>59385130</v>
     <v>CROX</v>
     <v>CROCS, INC. (XNAS:CROX)</v>
-    <v>975883</v>
+    <v>262</v>
     <v>978550</v>
     <v>2005</v>
   </rv>
@@ -4774,7 +4755,7 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>4</v>
+    <v>5</v>
     <v>en-GB</v>
     <v>a25yfr</v>
     <v>268435456</v>
@@ -4785,8 +4766,6 @@
     <v>1.5166999999999999</v>
     <v>0.2</v>
     <v>1.0582000000000001E-2</v>
-    <v>0</v>
-    <v>0</v>
     <v>USD</v>
     <v>Wabash National Corporation provides connected solutions for the transportation, logistics and distribution industries. The Company designs and manufactures products including dry freight and refrigerated trailers, platform trailers, tank trailers, dry and refrigerated truck bodies, structural composite panels and products, transportation, logistics, and distribution industry parts and services, and specialty food grade processing equipment. The Company’s Transportation Solutions (TS) segment comprises the design and manufacturing operations for the Company’s transportation-related equipment and products. This includes dry and refrigerated van trailers, platform trailers, tank trailers and truck-mounted tanks, truck-mounted dry and refrigerated truck bodies and EcoNex technology products. Its Parts &amp; Services (P&amp;S) segment is comprised of the Company’s parts and services businesses as well as the upfitting component of truck bodies business. It also includes DuraPlate composite panels.</v>
     <v>6700</v>
@@ -4804,14 +4783,13 @@
     <v>WABASH NATIONAL CORPORATION</v>
     <v>WABASH NATIONAL CORPORATION</v>
     <v>19.22</v>
-    <v>5.8559999999999999</v>
+    <v>5.8590999999999998</v>
     <v>18.899999999999999</v>
-    <v>19.100000000000001</v>
     <v>19.100000000000001</v>
     <v>43999230</v>
     <v>WNC</v>
     <v>WABASH NATIONAL CORPORATION (XNYS:WNC)</v>
-    <v>253868</v>
+    <v>10</v>
     <v>580646</v>
     <v>1991</v>
   </rv>
@@ -4839,8 +4817,6 @@
     <v>1.0341</v>
     <v>0.33</v>
     <v>1.5109999999999998E-2</v>
-    <v>0</v>
-    <v>0</v>
     <v>USD</v>
     <v>Perdoceo Education Corporation, through its academic institutions, offers quality postsecondary education primarily online to a diverse student population, along with campus-based and blended learning programs. The Company's academic institutions include Colorado Technical University (CTU) and the American InterContinental University System (AIUS), which provides degree programs from the associate through doctoral level as well as non-degree seeking and professional development programs. Its academic institutions offer students industry-relevant and career-focused academic programs. CTU offers academic programs in the career-oriented disciplines of business and management, nursing, healthcare management, computer science, engineering, information systems and technology, project management, cybersecurity and criminal justice. AIUS offers academic programs in the career-oriented disciplines of business studies, information technologies, education, health sciences and criminal justice.</v>
     <v>2319</v>
@@ -4858,9 +4834,8 @@
     <v>PERDOCEO EDUCATION CORPORATION</v>
     <v>PERDOCEO EDUCATION CORPORATION</v>
     <v>22.07</v>
-    <v>10.8954</v>
+    <v>10.8955</v>
     <v>21.84</v>
-    <v>22.17</v>
     <v>22.17</v>
     <v>65673430</v>
     <v>PRDO</v>
@@ -4893,8 +4868,6 @@
     <v>1.2394000000000001</v>
     <v>0.27</v>
     <v>1.1869999999999999E-3</v>
-    <v>-0.28999999999999998</v>
-    <v>-1.273E-3</v>
     <v>USD</v>
     <v>Apple Inc. designs, manufactures and markets smartphones, personal computers, tablets, wearables and accessories, and sells a variety of related services. Its product categories include iPhone, Mac, iPad, and Wearables, Home and Accessories. Its software platforms include iOS, iPadOS, macOS, watchOS, and tvOS. Its services include advertising, AppleCare, cloud services, digital content and payment services. It operates various platforms, including the App Store, that allow customers to discover and download applications and digital content, such as books, music, video, games and podcasts. It also offers digital content through subscription-based services, including Apple Arcade, Apple Fitness+, Apple Music, Apple News+ and Apple TV+. Its products include iPhone 15 Pro, iPhone 15, iPhone 14, iPhone 13, MacBook Air, MacBook Pro, iMac, Mac mini, Mac Studio, Mac Pro, and others. It also provides DarwinAI, which specializes in visual quality inspection using its Explainable AI platform.</v>
     <v>161000</v>
@@ -4915,11 +4888,10 @@
     <v>34.672400000000003</v>
     <v>227.52</v>
     <v>227.79</v>
-    <v>227.5</v>
     <v>15204140000</v>
     <v>AAPL</v>
     <v>APPLE INC. (XNAS:AAPL)</v>
-    <v>34025967</v>
+    <v>549516</v>
     <v>57417243</v>
     <v>1977</v>
   </rv>
@@ -4936,7 +4908,7 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>4</v>
+    <v>5</v>
     <v>en-GB</v>
     <v>a1ncgh</v>
     <v>268435456</v>
@@ -4947,8 +4919,6 @@
     <v>0.98839999999999995</v>
     <v>0.61</v>
     <v>6.3610000000000003E-3</v>
-    <v>-1.1599999999999999</v>
-    <v>-1.2020999999999999E-2</v>
     <v>USD</v>
     <v>Allison Transmission Holdings, Inc. is a designer and manufacturer of propulsion solutions for commercial and defense vehicles. The Company is also a manufacturer of medium-and heavy-duty fully automatic transmissions. Its products are used in a variety of applications, including on-highway trucks, including distribution, refuse, construction, fire and emergency; buses, including school, transit and coach; motorhomes, off-highway vehicles, and equipment, including energy, mining and construction applications; and defense vehicles, including tactical wheeled and tracked. The Company operates in approximately 150 countries. The Company has manufacturing facilities in the United States, Hungary and India, as well as global engineering resources, including electrification engineering centers in Indianapolis, Indiana, Auburn Hills, Michigan and London in the United Kingdom. The Company also has approximately 1,600 independent distributor and dealer locations worldwide.</v>
     <v>3700</v>
@@ -4966,14 +4936,13 @@
     <v>ALLISON TRANSMISSION HOLDINGS, INC.</v>
     <v>ALLISON TRANSMISSION HOLDINGS, INC.</v>
     <v>96</v>
-    <v>12.621</v>
+    <v>12.6183</v>
     <v>95.89</v>
     <v>96.5</v>
-    <v>95.34</v>
     <v>87137880</v>
     <v>ALSN</v>
     <v>ALLISON TRANSMISSION HOLDINGS, INC. (XNYS:ALSN)</v>
-    <v>952149</v>
+    <v>213</v>
     <v>568414</v>
     <v>2007</v>
   </rv>
@@ -5001,8 +4970,6 @@
     <v>1.9852000000000001</v>
     <v>0.28000000000000003</v>
     <v>1.5927E-2</v>
-    <v>0</v>
-    <v>0</v>
     <v>USD</v>
     <v>Par Pacific Holdings, Inc. is an energy company, which provides both renewable and conventional fuels to the western United States. It owns and operates 125,000 barrels per day of combined refining capacity across three locations and an energy infrastructure network, including 7.6 million barrels of storage, and marine, rail, rack and pipeline assets. The Company has three segments. Refining segment owns and operates four refineries with total operating crude oil throughput capacity of 219 thousand barrels per day (Mbpd). Retail segment operates fuel retail outlets in Hawaii, Washington and Idaho. It operates convenience stores and fuel retail sites under Hele and nomnom brands, 76 branded fuel retail sites and other sites operated by third parties that sell gasoline, diesel, and retail merchandise, such as soft drinks, prepared foods, and other sundries. Logistics segment operates a multi-modal logistics network spanning the Pacific, the Northwest, and the Rocky Mountain regions.</v>
     <v>1814</v>
@@ -5023,11 +4990,10 @@
     <v>3.1082999999999998</v>
     <v>17.579999999999998</v>
     <v>17.86</v>
-    <v>17.86</v>
     <v>56330870</v>
     <v>PARR</v>
     <v>PAR PACIFIC HOLDINGS, INC. (XNYS:PARR)</v>
-    <v>1200796</v>
+    <v>87</v>
     <v>1212458</v>
     <v>2005</v>
   </rv>
@@ -5055,8 +5021,6 @@
     <v>1.3070999999999999</v>
     <v>1.99</v>
     <v>3.2231999999999997E-2</v>
-    <v>0</v>
-    <v>0</v>
     <v>USD</v>
     <v>Hyster-Yale, Inc., formerly Hyster-Yale Materials Handling, Inc., through its wholly owned operating subsidiary, Hyster-Yale Materials Handling, designs, engineers, manufactures, sells, and services a comprehensive line of lift trucks, attachments, aftermarket parts and technology solutions marketed globally primarily under the Hyster and Yale brand names. The Company's business segments include Lift Trucks, Attachments and Fuel Cells. The Hyster-Yale Maximal brand provides trucks for customers requiring fundamental lift truck performance. The Lift Truck segment is focused on fuel cell-powered battery box replacements and integrated fuel cell engine solutions. Hyster- Yale’s attachment subsidiary, Bolzoni S.p.A., is a producer of attachments, forks, and lift tables under the Bolzoni, Auramo and Meyer brand names. The Fuel Cell business, Nuvera Fuel Cells, is an alternative-power technology company focused on fuel cell stacks and engines.</v>
     <v>8600</v>
@@ -5074,9 +5038,8 @@
     <v>HYSTER-YALE, INC.</v>
     <v>HYSTER-YALE, INC.</v>
     <v>62.65</v>
-    <v>6.3749000000000002</v>
+    <v>6.3728999999999996</v>
     <v>61.74</v>
-    <v>63.73</v>
     <v>63.73</v>
     <v>17501150</v>
     <v>HY</v>
@@ -5098,19 +5061,17 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>4</v>
+    <v>5</v>
     <v>en-GB</v>
     <v>a1zvsm</v>
     <v>268435456</v>
     <v>1</v>
     <v>Powered by Refinitiv</v>
-    <v>106.17</v>
+    <v>104.315</v>
     <v>71.900000000000006</v>
     <v>1.51</v>
     <v>0.43</v>
     <v>5.0880000000000005E-3</v>
-    <v>-0.94</v>
-    <v>-1.1065E-2</v>
     <v>USD</v>
     <v>Polaris Inc. is engaged in designing, engineering, manufacturing and marketing of powersports vehicles. The Company also designs and manufactures or sources parts, garments and accessories (PG&amp;A), which includes aftermarket accessories and apparel. The Company operates through three segments: Off Road, On Road and Marine. The Off Road segment consists of off-road vehicles and snowmobiles. The On Road segment designs and manufactures motorcycles, moto-roadsters, light duty hauling, and passenger vehicles. The Marine segment designs and manufactures boats that are designed to compete in key segments of the recreational marine industry, specifically pontoon and deck boats. Its product line-up includes the RANGER, RZR and Polaris XPEDITION and GENERAL side-by-side off-road vehicles; Sportsman all-terrain off-road vehicles; military and commercial off-road vehicles; snowmobiles; Indian Motorcycle mid-size and heavyweight motorcycles; Slingshot moto-roadsters, and pontoon and deck boats.</v>
     <v>18500</v>
@@ -5128,14 +5089,13 @@
     <v>Polaris Inc.</v>
     <v>Polaris Inc.</v>
     <v>85.73</v>
-    <v>14.877700000000001</v>
+    <v>14.8795</v>
     <v>84.52</v>
     <v>84.95</v>
-    <v>84.01</v>
     <v>55748030</v>
     <v>PII</v>
     <v>Polaris Inc. (XNYS:PII)</v>
-    <v>497634</v>
+    <v>11</v>
     <v>492414</v>
     <v>1994</v>
   </rv>
@@ -5152,7 +5112,7 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>4</v>
+    <v>5</v>
     <v>en-GB</v>
     <v>aw21cw</v>
     <v>268435456</v>
@@ -5163,8 +5123,6 @@
     <v>1.7321</v>
     <v>0.2</v>
     <v>1.921E-3</v>
-    <v>0.01</v>
-    <v>9.5849999999999999E-5</v>
     <v>USD</v>
     <v>CONSOL Energy Inc. is a producer and exporter of high-Btu bituminous thermal coal and metallurgical coal. It owns and operates longwall mining operations in the Northern Appalachian Basin. Its flagship operation is the Pennsylvania Mining Complex, located over 26 miles southwest of Pittsburgh, near the city of Washington and the borough of Waynesburg all in Pennsylvania, and consists of three deep longwall mining operations: the Bailey Mine, the Enlow Fork Mine and the Harvey Mine, as well as a centralized preparation plant. Its segments include the PAMC and the CONSOL Marine Terminal. The PAMC includes the Bailey Mine, the Enlow Fork Mine, the Harvey Mine and a centralized preparation plant. The PAMC segment's principal activities include the mining, preparation and marketing of bituminous coal, sold primarily to industrial end-users, metallurgical end-users and power generators. The CONSOL Marine Terminal segment provides coal export terminal services through the Port of Baltimore.</v>
     <v>2020</v>
@@ -5182,10 +5140,9 @@
     <v>CONSOL ENERGY INC.</v>
     <v>CONSOL ENERGY INC.</v>
     <v>104.8</v>
-    <v>7.79</v>
+    <v>7.7877999999999998</v>
     <v>104.13</v>
     <v>104.33</v>
-    <v>104.34</v>
     <v>29393230</v>
     <v>CEIX</v>
     <v>CONSOL ENERGY INC. (XNYS:CEIX)</v>
@@ -5217,8 +5174,6 @@
     <v>1.2508999999999999</v>
     <v>1.58</v>
     <v>1.6334000000000001E-2</v>
-    <v>-0.7</v>
-    <v>-7.1199999999999996E-3</v>
     <v>USD</v>
     <v>AGCO Corporation is a designer, manufacturer and distributor of agricultural machinery and precision agriculture technology. The Company sells a range of agricultural equipment, including tractors, combines, self-propelled sprayers, hay tools, forage equipment, seeding and tillage equipment, implements, and grain storage and protein production systems. It provides telemetry-based fleet management tools, including remote monitoring and diagnostics, which help farmers improve uptime, machine and yield optimization, mixed fleet optimization and decision support. The Company's Precision Planting, Headsight and Intelligent Ag Solutions brands provide retrofit solutions to upgrade farmers existing equipment to improve their planting, liquid application and harvest operations. The Company’s Precision Planting, Headsight, JCA and Intelligent Ag Solutions brands also sell precision agriculture solutions around the crop cycle to third party original equipment manufacturers (OEMs).</v>
     <v>27900</v>
@@ -5239,11 +5194,10 @@
     <v>17.5214</v>
     <v>96.73</v>
     <v>98.31</v>
-    <v>97.61</v>
     <v>74642300</v>
     <v>AGCO</v>
     <v>AGCO CORPORATION (XNYS:AGCO)</v>
-    <v>659164</v>
+    <v>1755</v>
     <v>736119</v>
     <v>1991</v>
   </rv>
@@ -5271,8 +5225,6 @@
     <v>1.1512</v>
     <v>-0.34</v>
     <v>-1.2663000000000001E-2</v>
-    <v>0.09</v>
-    <v>3.3950000000000004E-3</v>
     <v>USD</v>
     <v>Ituran Location and Control Ltd. is a provider of location-based services, consisting of stolen vehicle recovery (SVR), fleet management services and other tracking services. The Company also provides wireless communication products used in connection with its location-based services and various other applications. Its operations consist of two segments: location-based services and wireless communications products. Its location-based services segment consists of its SVR and tracking services, fleet management and value-added services consisted of personal locater services and concierge services. Its wireless communications products segment consists of short and medium range two-way machine-to-machine wireless communications products that are used for various applications, including automatic vehicle location (AVL) and automatic vehicle identification. It primarily provides its services, as well as sells and leases its products in Israel, Brazil, Argentina and the United States.</v>
     <v>2841</v>
@@ -5293,11 +5245,10 @@
     <v>10.3826</v>
     <v>26.85</v>
     <v>26.51</v>
-    <v>26.6</v>
     <v>19893580</v>
     <v>ITRN</v>
     <v>ITURAN LOCATION AND CONTROL LTD. (XNAS:ITRN)</v>
-    <v>105256</v>
+    <v>958</v>
     <v>76889</v>
     <v>1994</v>
   </rv>
@@ -5314,19 +5265,17 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>4</v>
+    <v>5</v>
     <v>en-GB</v>
     <v>a1sea2</v>
     <v>268435456</v>
     <v>1</v>
     <v>Powered by Refinitiv</v>
-    <v>13.67</v>
+    <v>13.345000000000001</v>
     <v>6.37</v>
     <v>2.1515</v>
     <v>0.01</v>
     <v>7.6160000000000008E-4</v>
-    <v>-0.04</v>
-    <v>-3.0439999999999998E-3</v>
     <v>USD</v>
     <v>Everi Holdings Inc. develops and offers products and services that provide gaming entertainment, improve its customers’ patron engagement, and help its casino customers operate their businesses. It develops and supplies entertaining game content, gaming machines and gaming systems and services for land-based and iGaming operators. It operates through two segments: Games and Financial Technology Solutions (FinTech). The Games segment provides gaming operators with gaming technology and entertainment products and services, including gaming machines, primarily comprising Class II, Class III and Historic Horse Racing slot machines placed under participation and fixed-fee lease arrangements or sold to casino customers. The FinTech segment provides gaming operators with financial technology products and services, including financial access and related services supporting digital, cashless and physical cash options across mobile, assisted and self-service channels.</v>
     <v>2200</v>
@@ -5344,14 +5293,13 @@
     <v>EVERI HOLDINGS INC.</v>
     <v>EVERI HOLDINGS INC.</v>
     <v>13.15</v>
-    <v>27.9312</v>
+    <v>27.9099</v>
     <v>13.13</v>
     <v>13.14</v>
-    <v>13.1</v>
     <v>85323580</v>
     <v>EVRI</v>
     <v>EVERI HOLDINGS INC. (XNYS:EVRI)</v>
-    <v>708697</v>
+    <v>5</v>
     <v>798529</v>
     <v>2004</v>
   </rv>
@@ -5359,9 +5307,9 @@
     <v>37</v>
   </rv>
   <rv s="3">
-    <v>5</v>
+    <v>6</v>
     <v>NEXTRACKER INC. (XNAS:NXT)</v>
-    <v>6</v>
+    <v>7</v>
     <v>3</v>
     <v>Finance</v>
     <v>4</v>
@@ -5375,8 +5323,6 @@
     <v>2.1160000000000001</v>
     <v>1.34</v>
     <v>3.5675999999999999E-2</v>
-    <v>-2.5999999999999999E-2</v>
-    <v>-6.6839999999999998E-4</v>
     <v>USD</v>
     <v>Nextracker Inc. is a provider of integrated solar tracker and software solutions used in utility-scale and ground-mounted distributed generation solar projects. Its products enable solar panels in utility-scale power plants to follow the sun’s movement across the sky and optimize plant performance. Its products include NX Horizon, NX Gemini, TrueCapture, and NX Navigator. Its solutions include Bifacial PV modules, Large Format Modules, and First Solar Series 6 (FSLR6) Modules. NX Horizon is a one-in-portrait (1P) smart solar tracker system that delivers the lowest levelized cost of energy (LCOE). NX Gemini is its two-in-portrait (2P) format tracker which holds two rows of solar panels along the central support beam. TrueCapture is its flagship software offering, which is a self-adjusting tracker control system that uses machine learning to enhance solar power plant energy yield. It has operations in the United States, Brazil, Mexico, Spain, India, Australia, the Middle East and Brazil.</v>
     <v>1050</v>
@@ -5396,11 +5342,10 @@
     <v>10.3238</v>
     <v>37.56</v>
     <v>38.9</v>
-    <v>38.874000000000002</v>
     <v>145347400</v>
     <v>NXT</v>
     <v>NEXTRACKER INC. (XNAS:NXT)</v>
-    <v>1949793</v>
+    <v>1714</v>
     <v>3165195</v>
     <v>2022</v>
   </rv>
@@ -5417,7 +5362,7 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>4</v>
+    <v>5</v>
     <v>en-GB</v>
     <v>a1xejc</v>
     <v>268435456</v>
@@ -5428,8 +5373,6 @@
     <v>1.744</v>
     <v>-0.02</v>
     <v>-2.5340000000000003E-4</v>
-    <v>0.28000000000000003</v>
-    <v>3.5479999999999999E-3</v>
     <v>USD</v>
     <v>Monarch Casino &amp; Resort, Inc. owns and operates the Atlantis Casino Resort Spa, a hotel and casino in Reno, Nevada (the Atlantis) and the Monarch Casino Resort Spa Black Hawk (the Monarch Black Hawk), a hotel and casino in Black Hawk, Colorado. In addition, it owns separate parcels of land located next to the Atlantis and a parcel of land with an industrial warehouse located between Denver, Colorado, and Monarch Black Hawk. The Atlantis is located approximately three miles south of downtown, which features approximately 61,000 square feet of casino space; 817 guest rooms and suites; eight food outlets; two gourmet coffee and pastry bars and one snack bar; a 30,000 square-foot health spa and salon with an enclosed year-round pool. Monarch Black Hawk features approximately 60,000 square feet of casino space; approximately 1,000 slot machines; approximately 43 table games; a live poker room; a keno counter and a sports book. The resort also includes 10 bars and lounges.</v>
     <v>2900</v>
@@ -5450,7 +5393,6 @@
     <v>18.442699999999999</v>
     <v>78.94</v>
     <v>78.92</v>
-    <v>79.2</v>
     <v>18452120</v>
     <v>MCRI</v>
     <v>MONARCH CASINO &amp; RESORT, INC. (XNAS:MCRI)</v>
@@ -5471,7 +5413,7 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>4</v>
+    <v>5</v>
     <v>en-GB</v>
     <v>a1xqm7</v>
     <v>268435456</v>
@@ -5482,8 +5424,6 @@
     <v>0.96940000000000004</v>
     <v>0.55000000000000004</v>
     <v>9.2200000000000008E-3</v>
-    <v>0.05</v>
-    <v>8.3059999999999991E-4</v>
     <v>USD</v>
     <v>Miller Industries, Inc. is a manufacturer of towing and recovery equipment. The Company designs and manufactures bodies of car carriers and wreckers, which are installed on chassis manufactured by third parties, and sold to its customers. Its products are marketed and sold through a network of distributors that serve all 50 states, Canada, Mexico, and other foreign markets, and through prime contractors to governmental entities. In addition to selling its products, its independent distributors provide end-users with parts and service. Its product line includes car carriers, wreckers, and transport trailers. Car carriers are specialized flat-bed vehicles with hydraulic tilt mechanisms that enable a towing operator to drive or winch a vehicle onto the bed for transport. Its multi-vehicle transport trailers are specialized auto transport trailers with upper and lower decks and hydraulic ramps for loading vehicles. Its brands include Century, Vulcan, Chevron, Holmes, and Challenger.</v>
     <v>1821</v>
@@ -5501,14 +5441,13 @@
     <v>MILLER INDUSTRIES, INC.</v>
     <v>MILLER INDUSTRIES, INC.</v>
     <v>60.34</v>
-    <v>9.6929999999999996</v>
+    <v>9.6913999999999998</v>
     <v>59.65</v>
     <v>60.2</v>
-    <v>60.25</v>
     <v>11453790</v>
     <v>MLR</v>
     <v>MILLER INDUSTRIES, INC. (XNYS:MLR)</v>
-    <v>41910</v>
+    <v>6</v>
     <v>96145</v>
     <v>1994</v>
   </rv>
@@ -5525,7 +5464,7 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>4</v>
+    <v>5</v>
     <v>en-GB</v>
     <v>btavh7</v>
     <v>268435456</v>
@@ -5536,8 +5475,6 @@
     <v>0.88749999999999996</v>
     <v>0.1</v>
     <v>9.8329999999999997E-3</v>
-    <v>0</v>
-    <v>0</v>
     <v>USD</v>
     <v>Janus International Group, Inc. is a global manufacturer and supplier of turn-key self-storage, commercial and industrial building solutions. It operates through two geographic segments: Janus North America and Janus International. The Janus North America segment is comprised of all the other entities, including Janus International Group, LLC, Betco, Inc., Noke, Inc., Asta Industries, Inc., DBCI, LLC, Access Control Technologies, LLC, Janus Door, LLC, and Steel Door Depot.com, LLC. The Janus International segment is comprised of Janus International Europe Holdings Ltd. (UK). Its production and sales are in Europe and Australia. It provides facility and door automation and access control technologies, roll up and swing doors, hallway systems and relocatable storage moveable additional storage structures (MASS) units. It is comprised of three sales channels, including New Construction-Self-storage, R3-Self-storage, and Commercial and Other. It also provides terminal maintenance services.</v>
     <v>1956</v>
@@ -5555,9 +5492,8 @@
     <v>JANUS INTERNATIONAL GROUP, INC.</v>
     <v>JANUS INTERNATIONAL GROUP, INC.</v>
     <v>10.32</v>
-    <v>11.510400000000001</v>
+    <v>11.516</v>
     <v>10.17</v>
-    <v>10.27</v>
     <v>10.27</v>
     <v>145322200</v>
     <v>JBI</v>
@@ -5590,8 +5526,6 @@
     <v>1.3149</v>
     <v>-2.1</v>
     <v>-5.1710000000000002E-3</v>
-    <v>-0.02</v>
-    <v>-4.9500000000000004E-5</v>
     <v>USD</v>
     <v>Ulta Beauty, Inc. is a beauty retailer. The Company's product categories include cosmetics, skincare, haircare products and styling tools, fragrance and bath, services, and accessories and other. The Company has one segment, which includes retail stores, salon services, and e-commerce. It offers a range of beauty services in its stores, focusing on hair, makeup, brow and skin services. Its skin services include a skin treatment room or dedicated skin treatment area on the sales floor. Its Ulta Beauty store prototype includes an open salon area, with most of its stores offering brow services on the salon floor. It offers a new way to shop for beauty - bringing together All Things Beauty, All in One Place. In addition to ship to home order fulfillment, it offers guests Buy Online, Pick-up in Store, Curbside Pickup, and Store 2 Door, which provides the ability for customers to order in-store and have products delivered to their homes. It operates over 1,350 retail stores across 50 states.</v>
     <v>20000</v>
@@ -5612,11 +5546,10 @@
     <v>16.222799999999999</v>
     <v>406.11</v>
     <v>404.01</v>
-    <v>403.99</v>
     <v>47114730</v>
     <v>ULTA</v>
     <v>ULTA BEAUTY, INC. (XNAS:ULTA)</v>
-    <v>1060882</v>
+    <v>2015</v>
     <v>1401709</v>
     <v>2016</v>
   </rv>
@@ -5633,7 +5566,7 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>4</v>
+    <v>5</v>
     <v>en-GB</v>
     <v>a1vehw</v>
     <v>268435456</v>
@@ -5644,8 +5577,6 @@
     <v>1.9673</v>
     <v>-0.01</v>
     <v>-4.6000000000000001E-4</v>
-    <v>0</v>
-    <v>0</v>
     <v>USD</v>
     <v>International Game Technology PLC is a United Kingdom-based company, which is engaged in gaming. The Company operates and provides an integrated portfolio of gaming technology products and services, including online and instant lottery systems, iLottery, instant ticket printing, lottery management services, commercial services, gaming systems, electronic gaming machines, iGaming, and sports betting. The Company operates through three segments. The Global Lottery segment operates traditional lottery and iLottery businesses across the world, which includes sales, operations, product development, technology, and support, across the world. The Global Gaming segment operates a land-based gaming business across the world, which includes sales, product management, studios, global manufacturing, operation, and technology, across the world. The Digital &amp; Betting segment operates iGaming and sports betting activities across the world.</v>
     <v>11000</v>
@@ -5663,14 +5594,13 @@
     <v>INTERNATIONAL GAME TECHNOLOGY PLC</v>
     <v>INTERNATIONAL GAME TECHNOLOGY PLC</v>
     <v>22.06</v>
-    <v>21.0139</v>
+    <v>21.023599999999998</v>
     <v>21.74</v>
-    <v>21.73</v>
     <v>21.73</v>
     <v>200000000</v>
     <v>IGT</v>
     <v>INTERNATIONAL GAME TECHNOLOGY PLC (XNYS:IGT)</v>
-    <v>848970</v>
+    <v>925</v>
     <v>658113</v>
     <v>2014</v>
   </rv>
@@ -5698,8 +5628,6 @@
     <v>0.58540000000000003</v>
     <v>0.08</v>
     <v>1.1709999999999999E-3</v>
-    <v>0.02</v>
-    <v>2.9240000000000001E-4</v>
     <v>USD</v>
     <v>Oil-Dri Corporation of America is a manufacturer and supplier of specialty sorbent products for pet care, animal health and nutrition, fluid purification, agricultural ingredients, sports field, industrial and automotive markets. Its principal product is cat litter. The Company’s Retail and Wholesale Products Group segment customers include mass merchandisers, the farm and fleet channel, drugstore chains, pet specialty retail outlets, dollar stores, retail grocery stores, distributors of industrial cleanup and automotive products, environmental service companies, sports field product users and marketers of consumer products. Its Business to Business Products Group segment customers include processors and refiners of edible oils, renewable diesel, petroleum-based oils and biodiesel fuel; manufacturers of animal feed and agricultural chemicals; and distributors of animal health and nutrition products. It is also a supplier of silica gel-based crystal cat litter.</v>
     <v>884</v>
@@ -5717,10 +5645,9 @@
     <v>OIL-DRI CORPORATION OF AMERICA</v>
     <v>OIL-DRI CORPORATION OF AMERICA</v>
     <v>69.370500000000007</v>
-    <v>14.067299999999999</v>
+    <v>14.038600000000001</v>
     <v>68.33</v>
     <v>68.41</v>
-    <v>68.430000000000007</v>
     <v>7286320</v>
     <v>ODC</v>
     <v>OIL-DRI CORPORATION OF AMERICA (XNYS:ODC)</v>
@@ -5741,7 +5668,7 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>4</v>
+    <v>5</v>
     <v>en-GB</v>
     <v>a1mt9c</v>
     <v>268435456</v>
@@ -5752,8 +5679,6 @@
     <v>1.5789</v>
     <v>-0.68</v>
     <v>-6.293E-3</v>
-    <v>-0.70699999999999996</v>
-    <v>-6.5849999999999997E-3</v>
     <v>USD</v>
     <v>Axcelis Technologies, Inc. designs, manufactures and services ion implantation and other processing equipment used in the fabrication of semiconductor chips. The Company offers a complete line of high energy, high current and medium current implanters for all application requirements. In addition to equipment, the Company provides extensive aftermarket lifecycle products and services, including used tools, spare parts, equipment upgrades, maintenance services and customer training. Its Purion flagship systems are all based on a common platform, which enables a combination of implant purity, precision and productivity. Combining a single wafer end station, with advanced spot beam architectures (that ensures all points across the wafer see the same beam condition at the same beam angle), Purion products enable process control to optimize device performance and yield, at high productivity. The Company sells its products to semiconductor chip manufacturers around the world.</v>
     <v>1620</v>
@@ -5771,14 +5696,13 @@
     <v>AXCELIS TECHNOLOGIES, INC.</v>
     <v>AXCELIS TECHNOLOGIES, INC.</v>
     <v>109.01</v>
-    <v>14.7925</v>
+    <v>14.7926</v>
     <v>108.05</v>
     <v>107.37</v>
-    <v>106.663</v>
     <v>32617590</v>
     <v>ACLS</v>
     <v>AXCELIS TECHNOLOGIES, INC. (XNAS:ACLS)</v>
-    <v>360862</v>
+    <v>2602</v>
     <v>652750</v>
     <v>1995</v>
   </rv>
@@ -5806,8 +5730,6 @@
     <v>0.89480000000000004</v>
     <v>-6.27</v>
     <v>-4.9569000000000002E-2</v>
-    <v>-0.06</v>
-    <v>-4.9910000000000004E-4</v>
     <v>USD</v>
     <v>Dell Technologies Inc. is engaged in designing, developing, manufacturing, marketing, selling, and supporting a wide range of comprehensive and integrated solutions, products, and services. The Company operates through two segments: Infrastructure Solutions Group (ISG) and Client Solutions Group (CSG). Its ISG segment enables the Company’s customer’s digital transformation with solutions that address artificial intelligence (AI), machine learning, data analytics, and multi cloud environments. Its comprehensive storage portfolio includes modern and traditional storage solutions, including all-flash arrays, scale-out file, object platforms, hyper-converged infrastructure, and software-defined storage. Its CSG segment offers branded personal computers (PCs) including notebooks, desktops, and workstations and branded peripherals that include displays, docking stations, keyboards, mice, and webcam and audio devices, as well as third-party software and peripherals.</v>
     <v>120000</v>
@@ -5828,11 +5750,10 @@
     <v>22.131900000000002</v>
     <v>126.49</v>
     <v>120.22</v>
-    <v>120.16</v>
     <v>702384800</v>
     <v>DELL</v>
     <v>DELL TECHNOLOGIES INC. (XNYS:DELL)</v>
-    <v>13544967</v>
+    <v>95690</v>
     <v>13750305</v>
     <v>2013</v>
   </rv>
@@ -5844,10 +5765,10 @@
     <v>Learn more on Bing</v>
   </rv>
   <rv s="4">
-    <v>7</v>
+    <v>8</v>
     <v>PFIZER INC. (XNYS:PFE)</v>
     <v>2</v>
-    <v>8</v>
+    <v>9</v>
     <v>Finance</v>
     <v>4</v>
     <v>en-GB</v>
@@ -5860,8 +5781,6 @@
     <v>0.65259999999999996</v>
     <v>0.12</v>
     <v>4.1419999999999998E-3</v>
-    <v>0.02</v>
-    <v>6.8750000000000007E-4</v>
     <v>USD</v>
     <v>Pfizer Inc. is a research-based global biopharmaceutical company. The Company is engaged in the discovery, development, manufacture, marketing, sale and distribution of biopharmaceutical products worldwide. Its Biopharma segment is engaged in the science-based biopharmaceutical business. Its Biopharma segment includes the Pfizer Oncology Division, the Pfizer U.S. Commercial Division, and the Pfizer International Commercial Division. Its product categories include oncology, primary care and specialty care. Its Oncology products include Ibrance, Xtandi, Inlyta, Bosulif, Lorbrena, Braftovi, Mektovi, Padcev, Adcetris, Talzenna, Tukysa, Elrexfio and Tivdak. Its primary care products include Eliquis, Nurtec ODT/Vydura, Comirnaty, the Prevnar family, Abrysvo, FSME/IMMUN-TicoVac, Paxlovid and Lucira by Pfizer. Its specialty care products include Xeljanz, Enbrel (outside the U.S. and Canada), Inflectra, Cibinqo, Litfulo, Vyndaqel family, Genotropin, Sulperazon, Zavicefta, Medrol and Panzyga.</v>
     <v>88000</v>
@@ -5881,11 +5800,10 @@
     <v>29.02</v>
     <v>28.97</v>
     <v>29.09</v>
-    <v>29.11</v>
     <v>5666695000</v>
     <v>PFE</v>
     <v>PFIZER INC. (XNYS:PFE)</v>
-    <v>25013039</v>
+    <v>61818</v>
     <v>27953342</v>
     <v>1942</v>
   </rv>
@@ -5902,7 +5820,7 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>4</v>
+    <v>5</v>
     <v>en-GB</v>
     <v>a1odgh</v>
     <v>268435456</v>
@@ -5913,8 +5831,6 @@
     <v>1.4086000000000001</v>
     <v>0.14000000000000001</v>
     <v>6.7800000000000004E-3</v>
-    <v>0.22</v>
-    <v>1.0582000000000001E-2</v>
     <v>USD</v>
     <v>Franklin Resources, Inc. is a global investment management company with subsidiaries operating as Franklin Templeton and serving clients in over 150 countries. It offers specialization on a global scale, bringing capabilities in fixed income, equity, alternatives and multi-asset solutions. The Company provides its investment management and related services to retail, institutional and high-net-worth investors in jurisdictions worldwide. Its investment products include sponsored funds, as well as institutional and high-net-worth separate accounts, retail separately managed account programs, sub-advised products, and other investment vehicles. Its funds include registered funds (including exchange-traded funds or ETFs) and unregistered funds. The Company offers its services and products under its various brand names, including Alcentra, K2, Benefit Street Partners, ClearBridge Investments, Martin Currie, O’Shaughnessy, and Lexington Partners. It also focuses on the retirement sector.</v>
     <v>10300</v>
@@ -5932,14 +5848,13 @@
     <v>FRANKLIN RESOURCES, INC.</v>
     <v>FRANKLIN RESOURCES, INC.</v>
     <v>20.88</v>
-    <v>12.9894</v>
+    <v>12.9832</v>
     <v>20.65</v>
     <v>20.79</v>
-    <v>21.01</v>
     <v>522998400</v>
     <v>BEN</v>
     <v>FRANKLIN RESOURCES, INC. (XNYS:BEN)</v>
-    <v>2791502</v>
+    <v>2943</v>
     <v>5369841</v>
     <v>1969</v>
   </rv>
@@ -5967,8 +5882,6 @@
     <v>1.1435</v>
     <v>0.3</v>
     <v>1.218E-2</v>
-    <v>0.02</v>
-    <v>8.0219999999999998E-4</v>
     <v>USD</v>
     <v>UGI Corporation is a holding company, which distributes, stores, transports and markets energy products and related services. In the United States, the Company owns and operates a retail propane marketing and distribution business, natural gas and electric distribution utilities, and energy marketing, midstream infrastructure, storage, natural gas gathering and processing, natural gas production, electricity generation and energy services businesses. In Europe, the Company markets and distributes propane and other liquified petroleum gas (LPG), and market other energy products and services. It operates through four segments: AmeriGas Propane, UGI International, Midstream &amp; Marketing, and Utilities. The AmeriGas Propane segment operates propane distribution business. The UGI International segment consists of LPG distribution businesses in Austria, Belgium, the Czech Republic, Denmark, Finland, France, Hungary, Italy, Luxembourg, the Netherlands, Norway, Poland, Romania and others.</v>
     <v>5160</v>
@@ -5989,11 +5902,10 @@
     <v>7.9371999999999998</v>
     <v>24.63</v>
     <v>24.93</v>
-    <v>24.95</v>
     <v>214688600</v>
     <v>UGI</v>
     <v>UGI CORPORATION (XNYS:UGI)</v>
-    <v>2134381</v>
+    <v>3101</v>
     <v>2047453</v>
     <v>1991</v>
   </rv>
@@ -6026,8 +5938,6 @@
     <k n="Beta"/>
     <k n="Change"/>
     <k n="Change (%)"/>
-    <k n="Change (Extended hours)"/>
-    <k n="Change % (Extended hours)"/>
     <k n="Currency" t="s"/>
     <k n="Description" t="s"/>
     <k n="Employees"/>
@@ -6048,7 +5958,6 @@
     <k n="P/E"/>
     <k n="Previous close"/>
     <k n="Price"/>
-    <k n="Price (Extended hours)"/>
     <k n="Shares outstanding"/>
     <k n="Ticker symbol" t="s"/>
     <k n="UniqueName" t="s"/>
@@ -6076,8 +5985,6 @@
     <k n="Beta"/>
     <k n="Change"/>
     <k n="Change (%)"/>
-    <k n="Change (Extended hours)"/>
-    <k n="Change % (Extended hours)"/>
     <k n="Currency" t="s"/>
     <k n="Description" t="s"/>
     <k n="Employees"/>
@@ -6097,7 +6004,6 @@
     <k n="P/E"/>
     <k n="Previous close"/>
     <k n="Price"/>
-    <k n="Price (Extended hours)"/>
     <k n="Shares outstanding"/>
     <k n="Ticker symbol" t="s"/>
     <k n="UniqueName" t="s"/>
@@ -6122,8 +6028,6 @@
     <k n="Beta"/>
     <k n="Change"/>
     <k n="Change (%)"/>
-    <k n="Change (Extended hours)"/>
-    <k n="Change % (Extended hours)"/>
     <k n="Currency" t="s"/>
     <k n="Description" t="s"/>
     <k n="Employees"/>
@@ -6143,7 +6047,6 @@
     <k n="Open"/>
     <k n="Previous close"/>
     <k n="Price"/>
-    <k n="Price (Extended hours)"/>
     <k n="Shares outstanding"/>
     <k n="Ticker symbol" t="s"/>
     <k n="UniqueName" t="s"/>
@@ -6157,7 +6060,7 @@
 <file path=xl/richData/rdsupportingpropertybag.xml><?xml version="1.0" encoding="utf-8"?>
 <supportingPropertyBags xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2">
   <spbArrays count="3">
-    <a count="45">
+    <a count="42">
       <v t="s">%EntityServiceId</v>
       <v t="s">_Format</v>
       <v t="s">%IsRefreshable</v>
@@ -6168,16 +6071,13 @@
       <v t="s">Name</v>
       <v t="s">_SubLabel</v>
       <v t="s">Price</v>
-      <v t="s">Price (Extended hours)</v>
       <v t="s">Exchange</v>
       <v t="s">Official name</v>
       <v t="s">Last trade time</v>
       <v t="s">Ticker symbol</v>
       <v t="s">Exchange abbreviation</v>
       <v t="s">Change</v>
-      <v t="s">Change (Extended hours)</v>
       <v t="s">Change (%)</v>
-      <v t="s">Change % (Extended hours)</v>
       <v t="s">Currency</v>
       <v t="s">Previous close</v>
       <v t="s">Open</v>
@@ -6204,7 +6104,7 @@
       <v t="s">ExchangeID</v>
       <v t="s">%ProviderInfo</v>
     </a>
-    <a count="44">
+    <a count="41">
       <v t="s">%EntityServiceId</v>
       <v t="s">_Format</v>
       <v t="s">%IsRefreshable</v>
@@ -6215,16 +6115,13 @@
       <v t="s">Name</v>
       <v t="s">_SubLabel</v>
       <v t="s">Price</v>
-      <v t="s">Price (Extended hours)</v>
       <v t="s">Exchange</v>
       <v t="s">Official name</v>
       <v t="s">Last trade time</v>
       <v t="s">Ticker symbol</v>
       <v t="s">Exchange abbreviation</v>
       <v t="s">Change</v>
-      <v t="s">Change (Extended hours)</v>
       <v t="s">Change (%)</v>
-      <v t="s">Change % (Extended hours)</v>
       <v t="s">Currency</v>
       <v t="s">Previous close</v>
       <v t="s">Open</v>
@@ -6250,7 +6147,7 @@
       <v t="s">ExchangeID</v>
       <v t="s">%ProviderInfo</v>
     </a>
-    <a count="44">
+    <a count="41">
       <v t="s">%EntityServiceId</v>
       <v t="s">_Format</v>
       <v t="s">%IsRefreshable</v>
@@ -6261,16 +6158,13 @@
       <v t="s">Name</v>
       <v t="s">_SubLabel</v>
       <v t="s">Price</v>
-      <v t="s">Price (Extended hours)</v>
       <v t="s">Exchange</v>
       <v t="s">Official name</v>
       <v t="s">Last trade time</v>
       <v t="s">Ticker symbol</v>
       <v t="s">Exchange abbreviation</v>
       <v t="s">Change</v>
-      <v t="s">Change (Extended hours)</v>
       <v t="s">Change (%)</v>
-      <v t="s">Change % (Extended hours)</v>
       <v t="s">Currency</v>
       <v t="s">Previous close</v>
       <v t="s">Open</v>
@@ -6297,7 +6191,7 @@
       <v t="s">%ProviderInfo</v>
     </a>
   </spbArrays>
-  <spbData count="9">
+  <spbData count="10">
     <spb s="0">
       <v>0</v>
       <v>Name</v>
@@ -6335,19 +6229,20 @@
       <v>8</v>
       <v>9</v>
       <v>4</v>
-      <v>1</v>
-      <v>1</v>
-      <v>5</v>
     </spb>
     <spb s="4">
-      <v>at close</v>
+      <v>Real-Time Nasdaq Last Sale</v>
       <v>from previous close</v>
       <v>from previous close</v>
       <v>Source: Nasdaq Last Sale</v>
       <v>GMT</v>
-      <v>Real-Time Nasdaq Last Sale</v>
-      <v>from close</v>
-      <v>from close</v>
+    </spb>
+    <spb s="4">
+      <v>Delayed 15 minutes</v>
+      <v>from previous close</v>
+      <v>from previous close</v>
+      <v>Source: Nasdaq</v>
+      <v>GMT</v>
     </spb>
     <spb s="5">
       <v>1</v>
@@ -6383,9 +6278,6 @@
       <v>8</v>
       <v>9</v>
       <v>4</v>
-      <v>1</v>
-      <v>1</v>
-      <v>5</v>
     </spb>
   </spbData>
 </supportingPropertyBags>
@@ -6430,9 +6322,6 @@
     <k n="Year incorporated" t="i"/>
     <k n="`%EntityServiceId" t="i"/>
     <k n="Shares outstanding" t="i"/>
-    <k n="Price (Extended hours)" t="i"/>
-    <k n="Change (Extended hours)" t="i"/>
-    <k n="Change % (Extended hours)" t="i"/>
   </s>
   <s>
     <k n="Price" t="s"/>
@@ -6440,9 +6329,6 @@
     <k n="Change (%)" t="s"/>
     <k n="ExchangeID" t="s"/>
     <k n="Last trade time" t="s"/>
-    <k n="Price (Extended hours)" t="s"/>
-    <k n="Change (Extended hours)" t="s"/>
-    <k n="Change % (Extended hours)" t="s"/>
   </s>
   <s>
     <k n="^Order" t="spba"/>
@@ -6473,9 +6359,6 @@
     <k n="Year incorporated" t="i"/>
     <k n="`%EntityServiceId" t="i"/>
     <k n="Shares outstanding" t="i"/>
-    <k n="Price (Extended hours)" t="i"/>
-    <k n="Change (Extended hours)" t="i"/>
-    <k n="Change % (Extended hours)" t="i"/>
   </s>
 </spbStructures>
 </file>
@@ -69893,7 +69776,7 @@
   <dimension ref="B1:L30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+      <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
@@ -69979,11 +69862,11 @@
         <v>61.38</v>
       </c>
       <c r="J3" s="129">
-        <f t="shared" ref="J3:J24" ca="1" si="0">((I3-F3)/F3)</f>
+        <f t="shared" ref="J3:J27" ca="1" si="0">((I3-F3)/F3)</f>
         <v>-0.10719999999999996</v>
       </c>
       <c r="K3" s="170">
-        <f t="shared" ref="K3:K24" ca="1" si="1">(I3*G3) - H3</f>
+        <f t="shared" ref="K3:K27" ca="1" si="1">(I3*G3) - H3</f>
         <v>-53.736215999999956</v>
       </c>
       <c r="L3"/>
@@ -70804,109 +70687,127 @@
       </c>
     </row>
     <row r="25" spans="2:12">
-      <c r="B25" s="220" t="e" vm="23">
+      <c r="B25" s="219" t="e" vm="23">
         <v>#VALUE!</v>
       </c>
-      <c r="C25" s="220" t="str" cm="1">
+      <c r="C25" s="219" t="str" cm="1">
         <f t="array" aca="1" ref="C25" ca="1">_FV(Portfolio[[#This Row],[Company]],"Name")</f>
         <v>PFIZER INC.</v>
       </c>
-      <c r="D25" s="221" t="str" cm="1">
+      <c r="D25" s="220" t="str" cm="1">
         <f t="array" aca="1" ref="D25" ca="1">_FV(B25,"Ticker symbol",TRUE)</f>
         <v>PFE</v>
       </c>
-      <c r="E25" s="221" t="str" cm="1">
+      <c r="E25" s="220" t="str" cm="1">
         <f t="array" aca="1" ref="E25" ca="1">_FV(B25,"Industry")</f>
         <v>Pharmaceuticals</v>
       </c>
-      <c r="F25" s="222"/>
-      <c r="G25" s="222"/>
-      <c r="H25" s="223"/>
-      <c r="I25" s="224" cm="1">
+      <c r="F25" s="221">
+        <v>29.22</v>
+      </c>
+      <c r="G25" s="225">
+        <v>17.143799999999999</v>
+      </c>
+      <c r="H25" s="222">
+        <v>501</v>
+      </c>
+      <c r="I25" s="223" cm="1">
         <f t="array" aca="1" ref="I25" ca="1">_FV(B25,"Price")</f>
         <v>29.09</v>
       </c>
-      <c r="J25" s="219" t="e">
-        <f ca="1">((I25-F25)/F25)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K25" s="206">
-        <f ca="1">(I25*G25) - H25</f>
-        <v>0</v>
+      <c r="J25" s="129">
+        <f t="shared" ca="1" si="0"/>
+        <v>-4.4490075290896311E-3</v>
+      </c>
+      <c r="K25" s="170">
+        <f t="shared" ca="1" si="1"/>
+        <v>-2.286858000000052</v>
       </c>
     </row>
     <row r="26" spans="2:12">
-      <c r="B26" s="220" t="e" vm="24">
+      <c r="B26" s="219" t="e" vm="24">
         <v>#VALUE!</v>
       </c>
-      <c r="C26" s="220" t="str" cm="1">
+      <c r="C26" s="219" t="str" cm="1">
         <f t="array" aca="1" ref="C26" ca="1">_FV(Portfolio[[#This Row],[Company]],"Name")</f>
         <v>FRANKLIN RESOURCES, INC.</v>
       </c>
-      <c r="D26" s="221" t="str" cm="1">
+      <c r="D26" s="220" t="str" cm="1">
         <f t="array" aca="1" ref="D26" ca="1">_FV(B26,"Ticker symbol",TRUE)</f>
         <v>BEN</v>
       </c>
-      <c r="E26" s="221" t="str" cm="1">
+      <c r="E26" s="220" t="str" cm="1">
         <f t="array" aca="1" ref="E26" ca="1">_FV(B26,"Industry")</f>
         <v>Investment Banking &amp; Investment Services</v>
       </c>
-      <c r="F26" s="222"/>
-      <c r="G26" s="222"/>
-      <c r="H26" s="223"/>
-      <c r="I26" s="224" cm="1">
+      <c r="F26" s="221">
+        <v>20.9</v>
+      </c>
+      <c r="G26" s="225">
+        <v>24.023</v>
+      </c>
+      <c r="H26" s="222">
+        <v>502</v>
+      </c>
+      <c r="I26" s="223" cm="1">
         <f t="array" aca="1" ref="I26" ca="1">_FV(B26,"Price")</f>
         <v>20.79</v>
       </c>
-      <c r="J26" s="219" t="e">
-        <f ca="1">((I26-F26)/F26)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K26" s="206">
-        <f ca="1">(I26*G26) - H26</f>
-        <v>0</v>
+      <c r="J26" s="129">
+        <f t="shared" ca="1" si="0"/>
+        <v>-5.2631578947368151E-3</v>
+      </c>
+      <c r="K26" s="170">
+        <f t="shared" ca="1" si="1"/>
+        <v>-2.5618300000000431</v>
       </c>
     </row>
     <row r="27" spans="2:12">
-      <c r="B27" s="220" t="e" vm="25">
+      <c r="B27" s="219" t="e" vm="25">
         <v>#VALUE!</v>
       </c>
-      <c r="C27" s="220" t="str" cm="1">
+      <c r="C27" s="219" t="str" cm="1">
         <f t="array" aca="1" ref="C27" ca="1">_FV(Portfolio[[#This Row],[Company]],"Name")</f>
         <v>UGI CORPORATION</v>
       </c>
-      <c r="D27" s="221" t="str" cm="1">
+      <c r="D27" s="220" t="str" cm="1">
         <f t="array" aca="1" ref="D27" ca="1">_FV(B27,"Ticker symbol",TRUE)</f>
         <v>UGI</v>
       </c>
-      <c r="E27" s="221" t="str" cm="1">
+      <c r="E27" s="220" t="str" cm="1">
         <f t="array" aca="1" ref="E27" ca="1">_FV(B27,"Industry")</f>
         <v>Natural Gas Utilities</v>
       </c>
-      <c r="F27" s="222"/>
-      <c r="G27" s="222"/>
-      <c r="H27" s="223"/>
-      <c r="I27" s="224" cm="1">
+      <c r="F27" s="221">
+        <v>24.94</v>
+      </c>
+      <c r="G27" s="224">
+        <v>20.084299999999999</v>
+      </c>
+      <c r="H27" s="222">
+        <v>501</v>
+      </c>
+      <c r="I27" s="223" cm="1">
         <f t="array" aca="1" ref="I27" ca="1">_FV(B27,"Price")</f>
         <v>24.93</v>
       </c>
-      <c r="J27" s="219" t="e">
-        <f ca="1">((I27-F27)/F27)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K27" s="206">
-        <f ca="1">(I27*G27) - H27</f>
-        <v>0</v>
+      <c r="J27" s="129">
+        <f t="shared" ca="1" si="0"/>
+        <v>-4.0096230954296563E-4</v>
+      </c>
+      <c r="K27" s="170">
+        <f t="shared" ca="1" si="1"/>
+        <v>-0.29840100000001257</v>
       </c>
     </row>
     <row r="30" spans="2:12" ht="13">
       <c r="K30" s="169">
         <f ca="1">SUM(K3:K27)</f>
-        <v>718.45879000000025</v>
+        <v>713.31170100000008</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="J3:K19 J20:J24">
+  <conditionalFormatting sqref="J3:K19 J20:J27">
     <cfRule type="cellIs" dxfId="5" priority="3" operator="lessThan">
       <formula>0</formula>
     </cfRule>
@@ -70914,7 +70815,7 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K20:K24">
+  <conditionalFormatting sqref="K20:K27">
     <cfRule type="cellIs" dxfId="3" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
vault backup: 2024-09-30 14:39:21
</commit_message>
<xml_diff>
--- a/_system/Attachments/Portfolio Management.xlsx
+++ b/_system/Attachments/Portfolio Management.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martin/repos/tomesink/obsidian/_system/Attachments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{175DB0B3-41FA-464D-80D2-959ED039FBF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AF4F463-2472-3649-AE4C-2E9E5D53CCFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="39400" yWindow="900" windowWidth="34980" windowHeight="19340" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4687,7 +4687,7 @@
     <v>1257979000</v>
     <v>CVS</v>
     <v>CVS HEALTH CORPORATION (XNYS:CVS)</v>
-    <v>134971</v>
+    <v>147313</v>
     <v>8081310</v>
     <v>1996</v>
   </rv>
@@ -4738,7 +4738,7 @@
     <v>59385130</v>
     <v>CROX</v>
     <v>CROCS, INC. (XNAS:CROX)</v>
-    <v>262</v>
+    <v>316</v>
     <v>978550</v>
     <v>2005</v>
   </rv>
@@ -4891,7 +4891,7 @@
     <v>15204140000</v>
     <v>AAPL</v>
     <v>APPLE INC. (XNAS:AAPL)</v>
-    <v>549516</v>
+    <v>641419</v>
     <v>57417243</v>
     <v>1977</v>
   </rv>
@@ -4959,7 +4959,7 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>4</v>
+    <v>5</v>
     <v>en-GB</v>
     <v>az23tc</v>
     <v>268435456</v>
@@ -4987,13 +4987,13 @@
     <v>PAR PACIFIC HOLDINGS, INC.</v>
     <v>PAR PACIFIC HOLDINGS, INC.</v>
     <v>17.88</v>
-    <v>3.1082999999999998</v>
+    <v>3.1118000000000001</v>
     <v>17.579999999999998</v>
     <v>17.86</v>
     <v>56330870</v>
     <v>PARR</v>
     <v>PAR PACIFIC HOLDINGS, INC. (XNYS:PARR)</v>
-    <v>87</v>
+    <v>97</v>
     <v>1212458</v>
     <v>2005</v>
   </rv>
@@ -5010,7 +5010,7 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>4</v>
+    <v>5</v>
     <v>en-GB</v>
     <v>a1v177</v>
     <v>268435456</v>
@@ -5095,7 +5095,7 @@
     <v>55748030</v>
     <v>PII</v>
     <v>Polaris Inc. (XNYS:PII)</v>
-    <v>11</v>
+    <v>211</v>
     <v>492414</v>
     <v>1994</v>
   </rv>
@@ -5163,7 +5163,7 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>4</v>
+    <v>5</v>
     <v>en-GB</v>
     <v>a1n1r7</v>
     <v>268435456</v>
@@ -5191,7 +5191,7 @@
     <v>AGCO CORPORATION</v>
     <v>AGCO CORPORATION</v>
     <v>97.71</v>
-    <v>17.5214</v>
+    <v>17.512499999999999</v>
     <v>96.73</v>
     <v>98.31</v>
     <v>74642300</v>
@@ -5312,7 +5312,7 @@
     <v>7</v>
     <v>3</v>
     <v>Finance</v>
-    <v>4</v>
+    <v>5</v>
     <v>en-GB</v>
     <v>c8ssgh</v>
     <v>268435456</v>
@@ -5447,7 +5447,7 @@
     <v>11453790</v>
     <v>MLR</v>
     <v>MILLER INDUSTRIES, INC. (XNYS:MLR)</v>
-    <v>6</v>
+    <v>22</v>
     <v>96145</v>
     <v>1994</v>
   </rv>
@@ -5549,7 +5549,7 @@
     <v>47114730</v>
     <v>ULTA</v>
     <v>ULTA BEAUTY, INC. (XNAS:ULTA)</v>
-    <v>2015</v>
+    <v>2016</v>
     <v>1401709</v>
     <v>2016</v>
   </rv>
@@ -5617,7 +5617,7 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>4</v>
+    <v>5</v>
     <v>en-GB</v>
     <v>a1z3ec</v>
     <v>268435456</v>
@@ -5753,7 +5753,7 @@
     <v>702384800</v>
     <v>DELL</v>
     <v>DELL TECHNOLOGIES INC. (XNYS:DELL)</v>
-    <v>95690</v>
+    <v>100374</v>
     <v>13750305</v>
     <v>2013</v>
   </rv>
@@ -5803,7 +5803,7 @@
     <v>5666695000</v>
     <v>PFE</v>
     <v>PFIZER INC. (XNYS:PFE)</v>
-    <v>61818</v>
+    <v>63412</v>
     <v>27953342</v>
     <v>1942</v>
   </rv>
@@ -5820,7 +5820,7 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>5</v>
+    <v>4</v>
     <v>en-GB</v>
     <v>a1odgh</v>
     <v>268435456</v>
@@ -5848,13 +5848,13 @@
     <v>FRANKLIN RESOURCES, INC.</v>
     <v>FRANKLIN RESOURCES, INC.</v>
     <v>20.88</v>
-    <v>12.9832</v>
+    <v>12.9894</v>
     <v>20.65</v>
     <v>20.79</v>
     <v>522998400</v>
     <v>BEN</v>
     <v>FRANKLIN RESOURCES, INC. (XNYS:BEN)</v>
-    <v>2943</v>
+    <v>2954</v>
     <v>5369841</v>
     <v>1969</v>
   </rv>

</xml_diff>

<commit_message>
vault backup: 2024-10-05 14:26:48
</commit_message>
<xml_diff>
--- a/_system/Attachments/Portfolio Management.xlsx
+++ b/_system/Attachments/Portfolio Management.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martin/repos/tomesink/obsidian/_system/Attachments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D39D448F-774A-E942-92A3-A075A2AAC4FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E11B357A-7188-7244-93B4-7A5D52B5DC9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39400" yWindow="900" windowWidth="34980" windowHeight="19340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3860" yWindow="1520" windowWidth="34980" windowHeight="19340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Stocks Performance" sheetId="1" r:id="rId1"/>
@@ -854,7 +854,7 @@
     <numFmt numFmtId="173" formatCode="[$$-409]#,##0.00"/>
     <numFmt numFmtId="174" formatCode="0.0000"/>
     <numFmt numFmtId="175" formatCode="[$$-409]\ #,##0.0000"/>
-    <numFmt numFmtId="180" formatCode="[$CZK]\ #,##0.00"/>
+    <numFmt numFmtId="176" formatCode="[$CZK]\ #,##0.00"/>
   </numFmts>
   <fonts count="16">
     <font>
@@ -2274,7 +2274,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -4669,11 +4669,11 @@
     <v>Powered by Refinitiv</v>
     <v>83.25</v>
     <v>52.770499999999998</v>
-    <v>0.5323</v>
-    <v>-1.34</v>
-    <v>-2.1309999999999999E-2</v>
-    <v>0.02</v>
-    <v>3.2499999999999999E-4</v>
+    <v>0.52700000000000002</v>
+    <v>1.67</v>
+    <v>2.6542E-2</v>
+    <v>-0.2</v>
+    <v>-3.0959999999999998E-3</v>
     <v>USD</v>
     <v>CVS Health Corporation is a health solutions company. The Company operates in four segments: Health Care Benefits, Health Services, Pharmacy &amp; Consumer Wellness, and Corporate/Other. Its Health Care Benefits segment offer a range of traditional, voluntary and consumer-directed health insurance products and related services, including medical, pharmacy, dental and behavioral health plans, medical management capabilities, Medicare Advantage and Medicare supplement plans, and Medicaid health care management services. Its Health Services segment provides a full range of pharmacy benefit management solutions, delivers health care services in its medical clinics, virtually, and in the home, and offers provider enablement solutions. The Pharmacy &amp; Consumer Wellness segment dispenses prescriptions in its retail pharmacies and through its infusion operations, provides ancillary pharmacy services, including pharmacy patient care programs, diagnostic testing and vaccination administration.</v>
     <v>300000</v>
@@ -4681,25 +4681,25 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>1 Cvs Dr, WOONSOCKET, RI, 02895-6146 US</v>
-    <v>63.18</v>
+    <v>65.569999999999993</v>
     <v>Healthcare Providers &amp; Services</v>
     <v>Stock</v>
-    <v>45566.998780578127</v>
+    <v>45569.999667777345</v>
     <v>0</v>
-    <v>60.76</v>
-    <v>77416027660</v>
+    <v>63.664299999999997</v>
+    <v>81252863610</v>
     <v>CVS HEALTH CORPORATION</v>
     <v>CVS HEALTH CORPORATION</v>
-    <v>63</v>
-    <v>10.9513</v>
-    <v>62.88</v>
-    <v>61.54</v>
-    <v>61.56</v>
+    <v>63.72</v>
+    <v>11.4941</v>
+    <v>62.92</v>
+    <v>64.59</v>
+    <v>64.39</v>
     <v>1257979000</v>
     <v>CVS</v>
     <v>CVS HEALTH CORPORATION (XNYS:CVS)</v>
-    <v>16285914</v>
-    <v>8524212</v>
+    <v>16313877</v>
+    <v>9631744</v>
     <v>1996</v>
   </rv>
   <rv s="2">
@@ -4723,11 +4723,11 @@
     <v>Powered by Refinitiv</v>
     <v>165.32</v>
     <v>74</v>
-    <v>1.9923</v>
-    <v>-3.18</v>
-    <v>-2.196E-2</v>
-    <v>-1.51</v>
-    <v>-1.0662E-2</v>
+    <v>1.9844999999999999</v>
+    <v>3.94</v>
+    <v>2.8553000000000002E-2</v>
+    <v>-0.13</v>
+    <v>-9.1590000000000009E-4</v>
     <v>USD</v>
     <v>Crocs, Inc. is engaged in the design, development, worldwide marketing, distribution, and sale of casual lifestyle footwear and accessories for women, men, and children. The Company’s segments include Crocs Brand and the HEYDUDE Brand. The Company’s Crocs Brand collection contains Croslite material, a molded footwear technology, delivering extraordinary comfort with each step. Its Croslite materials are formulated to create soft, comfortable, lightweight, non-marking, and odor-resistant footwear. The HEYDUDE Brand offers shoes with a versatile silhouette. It sells its products in more than 80 countries, through two distribution channels: wholesale and direct-to-consumer. Its wholesale channel includes domestic and international multi-brand retailers, mono-branded partner stores, e-tailers, and distributors; its direct-to-consumer channel includes Company-operated retail stores, Company-operated e-commerce sites, and third-party marketplaces.</v>
     <v>7030</v>
@@ -4735,25 +4735,25 @@
     <v>XNAS</v>
     <v>XNAS</v>
     <v>500 Eldorado Boulevard, Building 5, BROOMFIELD, CO, 80021 US</v>
-    <v>144.44</v>
+    <v>142.74</v>
     <v>Textiles &amp; Apparel</v>
     <v>Stock</v>
-    <v>45566.999929652346</v>
+    <v>45569.974103135937</v>
     <v>3</v>
-    <v>139.41999999999999</v>
-    <v>8410715961</v>
+    <v>140.28</v>
+    <v>8428531500</v>
     <v>CROCS, INC.</v>
     <v>CROCS, INC.</v>
-    <v>144.1</v>
-    <v>10.6517</v>
-    <v>144.81</v>
-    <v>141.63</v>
-    <v>140.12</v>
+    <v>140.86000000000001</v>
+    <v>10.3779</v>
+    <v>137.99</v>
+    <v>141.93</v>
+    <v>141.80000000000001</v>
     <v>59385130</v>
     <v>CROX</v>
     <v>CROCS, INC. (XNAS:CROX)</v>
-    <v>877037</v>
-    <v>967362</v>
+    <v>813650</v>
+    <v>972930</v>
     <v>2005</v>
   </rv>
   <rv s="2">
@@ -4777,9 +4777,9 @@
     <v>Powered by Refinitiv</v>
     <v>30.07</v>
     <v>17.71</v>
-    <v>1.5156000000000001</v>
-    <v>-0.47</v>
-    <v>-2.4492E-2</v>
+    <v>1.5218</v>
+    <v>-0.13</v>
+    <v>-7.1189999999999995E-3</v>
     <v>0</v>
     <v>0</v>
     <v>USD</v>
@@ -4789,25 +4789,25 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>3900 Mccarty Lane, LAFAYETTE, IN, 47905 US</v>
-    <v>19.07</v>
+    <v>18.66</v>
     <v>Machinery, Equipment &amp; Components</v>
     <v>Stock</v>
-    <v>45566.958333356248</v>
+    <v>45569.958333333336</v>
     <v>6</v>
-    <v>18.694600000000001</v>
-    <v>823665585</v>
+    <v>17.989999999999998</v>
+    <v>797706039</v>
     <v>WABASH NATIONAL CORPORATION</v>
     <v>WABASH NATIONAL CORPORATION</v>
-    <v>19.07</v>
-    <v>5.7424999999999997</v>
-    <v>19.190000000000001</v>
-    <v>18.72</v>
-    <v>18.72</v>
+    <v>18.579999999999998</v>
+    <v>5.5614999999999997</v>
+    <v>18.260000000000002</v>
+    <v>18.13</v>
+    <v>18.13</v>
     <v>43999230</v>
     <v>WNC</v>
     <v>WABASH NATIONAL CORPORATION (XNYS:WNC)</v>
-    <v>311272</v>
-    <v>584761</v>
+    <v>294144</v>
+    <v>598279</v>
     <v>1991</v>
   </rv>
   <rv s="2">
@@ -4831,11 +4831,11 @@
     <v>Powered by Refinitiv</v>
     <v>26.4</v>
     <v>16.12</v>
-    <v>1.0342</v>
-    <v>-0.63</v>
-    <v>-2.8327000000000001E-2</v>
-    <v>0.42</v>
-    <v>1.9435000000000001E-2</v>
+    <v>1.0426</v>
+    <v>0.57999999999999996</v>
+    <v>2.7618999999999998E-2</v>
+    <v>0</v>
+    <v>0</v>
     <v>USD</v>
     <v>Perdoceo Education Corporation, through its academic institutions, offers quality postsecondary education primarily online to a diverse student population, along with campus-based and blended learning programs. The Company's academic institutions include Colorado Technical University (CTU) and the American InterContinental University System (AIUS), which provides degree programs from the associate through doctoral level as well as non-degree seeking and professional development programs. Its academic institutions offer students industry-relevant and career-focused academic programs. CTU offers academic programs in the career-oriented disciplines of business and management, nursing, healthcare management, computer science, engineering, information systems and technology, project management, cybersecurity and criminal justice. AIUS offers academic programs in the career-oriented disciplines of business studies, information technologies, education, health sciences and criminal justice.</v>
     <v>2319</v>
@@ -4843,25 +4843,25 @@
     <v>XNAS</v>
     <v>XNAS</v>
     <v>1750 E. GOLF ROAD, SCHAUMBURG, IL, 60173 US</v>
-    <v>22.25</v>
+    <v>21.78</v>
     <v>Miscellaneous Educational Service Providers</v>
     <v>Stock</v>
-    <v>45566.894468356251</v>
+    <v>45569.834787939064</v>
     <v>9</v>
-    <v>21.46</v>
-    <v>1419202822</v>
+    <v>21.27</v>
+    <v>1417232619</v>
     <v>PERDOCEO EDUCATION CORPORATION</v>
     <v>PERDOCEO EDUCATION CORPORATION</v>
-    <v>22.25</v>
-    <v>10.6203</v>
-    <v>22.24</v>
-    <v>21.61</v>
-    <v>22.03</v>
+    <v>21.28</v>
+    <v>10.320499999999999</v>
+    <v>21</v>
+    <v>21.58</v>
+    <v>21.58</v>
     <v>65673430</v>
     <v>PRDO</v>
     <v>PERDOCEO EDUCATION CORPORATION (XNAS:PRDO)</v>
-    <v>563861</v>
-    <v>457958</v>
+    <v>342126</v>
+    <v>468802</v>
     <v>1994</v>
   </rv>
   <rv s="2">
@@ -4885,11 +4885,11 @@
     <v>Powered by Refinitiv</v>
     <v>237.23</v>
     <v>164.07499999999999</v>
-    <v>1.2392000000000001</v>
-    <v>-6.79</v>
-    <v>-2.9142000000000001E-2</v>
-    <v>-0.54</v>
-    <v>-2.3869999999999998E-3</v>
+    <v>1.2384999999999999</v>
+    <v>1.1299999999999999</v>
+    <v>5.0070000000000002E-3</v>
+    <v>-0.38500000000000001</v>
+    <v>-1.6980000000000001E-3</v>
     <v>USD</v>
     <v>Apple Inc. designs, manufactures and markets smartphones, personal computers, tablets, wearables and accessories, and sells a variety of related services. Its product categories include iPhone, Mac, iPad, and Wearables, Home and Accessories. Its software platforms include iOS, iPadOS, macOS, watchOS, and tvOS. Its services include advertising, AppleCare, cloud services, digital content and payment services. It operates various platforms, including the App Store, that allow customers to discover and download applications and digital content, such as books, music, video, games and podcasts. It also offers digital content through subscription-based services, including Apple Arcade, Apple Fitness+, Apple Music, Apple News+ and Apple TV+. Its products include iPhone 15 Pro, iPhone 15, iPhone 14, iPhone 13, MacBook Air, MacBook Pro, iMac, Mac mini, Mac Studio, Mac Pro, and others. It also provides DarwinAI, which specializes in visual quality inspection using its Explainable AI platform.</v>
     <v>161000</v>
@@ -4897,25 +4897,25 @@
     <v>XNAS</v>
     <v>XNAS</v>
     <v>One Apple Park Way, CUPERTINO, CA, 95014 US</v>
-    <v>229.65</v>
+    <v>228</v>
     <v>Computers, Phones &amp; Household Electronics</v>
     <v>Stock</v>
-    <v>45566.999953286722</v>
+    <v>45569.999978448439</v>
     <v>12</v>
-    <v>223.74</v>
-    <v>3439328509400</v>
+    <v>224.13</v>
+    <v>3448298952000</v>
     <v>APPLE INC.</v>
     <v>APPLE INC.</v>
-    <v>229.52</v>
-    <v>34.441699999999997</v>
-    <v>233</v>
-    <v>226.21</v>
+    <v>227.9</v>
+    <v>34.220999999999997</v>
     <v>225.67</v>
+    <v>226.8</v>
+    <v>226.41499999999999</v>
     <v>15204140000</v>
     <v>AAPL</v>
     <v>APPLE INC. (XNAS:AAPL)</v>
-    <v>63285048</v>
-    <v>57675114</v>
+    <v>37345098</v>
+    <v>58699950</v>
     <v>1977</v>
   </rv>
   <rv s="2">
@@ -4937,13 +4937,13 @@
     <v>268435456</v>
     <v>1</v>
     <v>Powered by Refinitiv</v>
-    <v>98</v>
+    <v>99.08</v>
     <v>50.134999999999998</v>
-    <v>0.98850000000000005</v>
-    <v>1.39</v>
-    <v>1.4469000000000001E-2</v>
-    <v>-0.46</v>
-    <v>-4.7199999999999994E-3</v>
+    <v>0.99099999999999999</v>
+    <v>1.96</v>
+    <v>2.0187E-2</v>
+    <v>-3.2500000000000001E-2</v>
+    <v>-3.2810000000000001E-4</v>
     <v>USD</v>
     <v>Allison Transmission Holdings, Inc. is a designer and manufacturer of propulsion solutions for commercial and defense vehicles. The Company is also a manufacturer of medium-and heavy-duty fully automatic transmissions. Its products are used in a variety of applications, including on-highway trucks, including distribution, refuse, construction, fire and emergency; buses, including school, transit and coach; motorhomes, off-highway vehicles, and equipment, including energy, mining and construction applications; and defense vehicles, including tactical wheeled and tracked. The Company operates in approximately 150 countries. The Company has manufacturing facilities in the United States, Hungary and India, as well as global engineering resources, including electrification engineering centers in Indianapolis, Indiana, Auburn Hills, Michigan and London in the United Kingdom. The Company also has approximately 1,600 independent distributor and dealer locations worldwide.</v>
     <v>3700</v>
@@ -4951,25 +4951,25 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>One Allison Way, INDIANAPOLIS, IN, 46222 US</v>
-    <v>98</v>
+    <v>99.08</v>
     <v>Machinery, Equipment &amp; Components</v>
     <v>Stock</v>
-    <v>45566.958333378905</v>
+    <v>45569.983881921093</v>
     <v>15</v>
-    <v>94.85</v>
-    <v>8492457784</v>
+    <v>97.35</v>
+    <v>8631007014</v>
     <v>ALLISON TRANSMISSION HOLDINGS, INC.</v>
     <v>ALLISON TRANSMISSION HOLDINGS, INC.</v>
-    <v>96.2</v>
-    <v>12.7439</v>
-    <v>96.07</v>
-    <v>97.46</v>
-    <v>97</v>
+    <v>98.36</v>
+    <v>12.9518</v>
+    <v>97.09</v>
+    <v>99.05</v>
+    <v>99.017499999999998</v>
     <v>87137880</v>
     <v>ALSN</v>
     <v>ALLISON TRANSMISSION HOLDINGS, INC. (XNYS:ALSN)</v>
-    <v>1012337</v>
-    <v>592905</v>
+    <v>385259</v>
+    <v>635069</v>
     <v>2007</v>
   </rv>
   <rv s="2">
@@ -4993,11 +4993,11 @@
     <v>Powered by Refinitiv</v>
     <v>40.695</v>
     <v>17.063600000000001</v>
-    <v>1.9782</v>
-    <v>-7.0000000000000007E-2</v>
-    <v>-3.9769999999999996E-3</v>
-    <v>0.97</v>
-    <v>5.5334000000000001E-2</v>
+    <v>1.972</v>
+    <v>-0.35</v>
+    <v>-1.8116E-2</v>
+    <v>0</v>
+    <v>0</v>
     <v>USD</v>
     <v>Par Pacific Holdings, Inc. is an energy company, which provides both renewable and conventional fuels to the western United States. It owns and operates 125,000 barrels per day of combined refining capacity across three locations and an energy infrastructure network, including 7.6 million barrels of storage, and marine, rail, rack and pipeline assets. The Company has three segments. Refining segment owns and operates four refineries with total operating crude oil throughput capacity of 219 thousand barrels per day (Mbpd). Retail segment operates fuel retail outlets in Hawaii, Washington and Idaho. It operates convenience stores and fuel retail sites under Hele and nomnom brands, 76 branded fuel retail sites and other sites operated by third parties that sell gasoline, diesel, and retail merchandise, such as soft drinks, prepared foods, and other sundries. Logistics segment operates a multi-modal logistics network spanning the Pacific, the Northwest, and the Rocky Mountain regions.</v>
     <v>1814</v>
@@ -5005,25 +5005,25 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>825 Town and Country Ln Ste 1500, HOUSTON, TX, 77024-2235 US</v>
-    <v>17.72</v>
+    <v>19.71</v>
     <v>Oil &amp; Gas</v>
     <v>Stock</v>
-    <v>45566.958333378905</v>
+    <v>45569.958333356248</v>
     <v>18</v>
-    <v>17.22</v>
-    <v>987480151</v>
+    <v>18.64</v>
+    <v>1088312000</v>
     <v>PAR PACIFIC HOLDINGS, INC.</v>
     <v>PAR PACIFIC HOLDINGS, INC.</v>
-    <v>17.28</v>
-    <v>3.0541999999999998</v>
-    <v>17.600000000000001</v>
-    <v>17.53</v>
-    <v>18.5</v>
+    <v>19.55</v>
+    <v>3.3052000000000001</v>
+    <v>19.32</v>
+    <v>18.97</v>
+    <v>18.97</v>
     <v>56330870</v>
     <v>PARR</v>
     <v>PAR PACIFIC HOLDINGS, INC. (XNYS:PARR)</v>
-    <v>1150512</v>
-    <v>1257869</v>
+    <v>961414</v>
+    <v>1306497</v>
     <v>2005</v>
   </rv>
   <rv s="2">
@@ -5047,9 +5047,9 @@
     <v>Powered by Refinitiv</v>
     <v>84.44</v>
     <v>38.5</v>
-    <v>1.3066</v>
-    <v>-1.07</v>
-    <v>-1.6778999999999999E-2</v>
+    <v>1.3087</v>
+    <v>3.38</v>
+    <v>5.4218999999999996E-2</v>
     <v>0</v>
     <v>0</v>
     <v>USD</v>
@@ -5059,25 +5059,25 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>5875 LANDERBROOK DRIVE, SUITE 300, CLEVELAND, OH, 44124 US</v>
-    <v>63.629199999999997</v>
+    <v>65.760000000000005</v>
     <v>Machinery, Equipment &amp; Components</v>
     <v>Stock</v>
-    <v>45566.958333378905</v>
+    <v>45569.958333378905</v>
     <v>21</v>
-    <v>61.65</v>
-    <v>1097322105</v>
+    <v>63.31</v>
+    <v>1091021000</v>
     <v>HYSTER-YALE, INC.</v>
     <v>HYSTER-YALE, INC.</v>
-    <v>63.6</v>
-    <v>6.2698999999999998</v>
-    <v>63.77</v>
-    <v>62.7</v>
-    <v>62.7</v>
+    <v>63.62</v>
+    <v>6.5719000000000003</v>
+    <v>62.34</v>
+    <v>65.72</v>
+    <v>65.72</v>
     <v>17501150</v>
     <v>HY</v>
     <v>HYSTER-YALE, INC. (XNYS:HY)</v>
-    <v>50676</v>
-    <v>68037</v>
+    <v>83022</v>
+    <v>66357</v>
     <v>1999</v>
   </rv>
   <rv s="2">
@@ -5099,13 +5099,13 @@
     <v>268435456</v>
     <v>1</v>
     <v>Powered by Refinitiv</v>
-    <v>104.315</v>
+    <v>100.91</v>
     <v>71.900000000000006</v>
-    <v>1.5085</v>
-    <v>-0.47</v>
-    <v>-5.646E-3</v>
-    <v>1.79</v>
-    <v>2.1625999999999999E-2</v>
+    <v>1.5028999999999999</v>
+    <v>0.4</v>
+    <v>4.8869999999999999E-3</v>
+    <v>0.39</v>
+    <v>4.7419999999999997E-3</v>
     <v>USD</v>
     <v>Polaris Inc. is engaged in designing, engineering, manufacturing and marketing of powersports vehicles. The Company also designs and manufactures or sources parts, garments and accessories (PG&amp;A), which includes aftermarket accessories and apparel. The Company operates through three segments: Off Road, On Road and Marine. The Off Road segment consists of off-road vehicles and snowmobiles. The On Road segment designs and manufactures motorcycles, moto-roadsters, light duty hauling, and passenger vehicles. The Marine segment designs and manufactures boats that are designed to compete in key segments of the recreational marine industry, specifically pontoon and deck boats. Its product line-up includes the RANGER, RZR and Polaris XPEDITION and GENERAL side-by-side off-road vehicles; Sportsman all-terrain off-road vehicles; military and commercial off-road vehicles; snowmobiles; Indian Motorcycle mid-size and heavyweight motorcycles; Slingshot moto-roadsters, and pontoon and deck boats.</v>
     <v>18500</v>
@@ -5113,25 +5113,25 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>2100 HIGHWAY 55, MEDINA, MN, 55340-9770 US</v>
-    <v>83.46</v>
+    <v>83.07</v>
     <v>Leisure Products</v>
     <v>Stock</v>
-    <v>45566.992872904688</v>
+    <v>45569.958333344533</v>
     <v>24</v>
-    <v>81.650000000000006</v>
-    <v>4614264443</v>
+    <v>81.75</v>
+    <v>4585275467</v>
     <v>Polaris Inc.</v>
     <v>Polaris Inc.</v>
-    <v>82.72</v>
-    <v>14.4976</v>
-    <v>83.24</v>
-    <v>82.77</v>
-    <v>84.56</v>
+    <v>82.92</v>
+    <v>14.406599999999999</v>
+    <v>81.849999999999994</v>
+    <v>82.25</v>
+    <v>82.64</v>
     <v>55748030</v>
     <v>PII</v>
     <v>Polaris Inc. (XNYS:PII)</v>
-    <v>420897</v>
-    <v>489231</v>
+    <v>347818</v>
+    <v>497431</v>
     <v>1994</v>
   </rv>
   <rv s="2">
@@ -5155,11 +5155,11 @@
     <v>Powered by Refinitiv</v>
     <v>114.29989999999999</v>
     <v>75.430000000000007</v>
-    <v>1.7306999999999999</v>
-    <v>-1.66</v>
-    <v>-1.5862000000000001E-2</v>
-    <v>2.0099999999999998</v>
-    <v>1.9515999999999999E-2</v>
+    <v>1.7454000000000001</v>
+    <v>2.4500000000000002</v>
+    <v>2.3990999999999998E-2</v>
+    <v>-0.01</v>
+    <v>-9.5630000000000004E-5</v>
     <v>USD</v>
     <v>CONSOL Energy Inc. is a producer and exporter of high-Btu bituminous thermal coal and metallurgical coal. It owns and operates longwall mining operations in the Northern Appalachian Basin. Its flagship operation is the Pennsylvania Mining Complex, located over 26 miles southwest of Pittsburgh, near the city of Washington and the borough of Waynesburg all in Pennsylvania, and consists of three deep longwall mining operations: the Bailey Mine, the Enlow Fork Mine and the Harvey Mine, as well as a centralized preparation plant. Its segments include the PAMC and the CONSOL Marine Terminal. The PAMC includes the Bailey Mine, the Enlow Fork Mine, the Harvey Mine and a centralized preparation plant. The PAMC segment's principal activities include the mining, preparation and marketing of bituminous coal, sold primarily to industrial end-users, metallurgical end-users and power generators. The CONSOL Marine Terminal segment provides coal export terminal services through the Port of Baltimore.</v>
     <v>2020</v>
@@ -5167,25 +5167,25 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>275 TECHNOLOGY DRIVE, SUITE #101, CANONSBURG, PA, 15317 US</v>
-    <v>104.825</v>
+    <v>105.1344</v>
     <v>Coal</v>
     <v>Stock</v>
-    <v>45566.958333378905</v>
+    <v>45569.969649536717</v>
     <v>27</v>
-    <v>102.45</v>
-    <v>3027208757</v>
+    <v>102.51</v>
+    <v>3073650061</v>
     <v>CONSOL ENERGY INC.</v>
     <v>CONSOL ENERGY INC.</v>
-    <v>104.37</v>
-    <v>7.6877000000000004</v>
-    <v>104.65</v>
-    <v>102.99</v>
-    <v>105</v>
+    <v>103.03</v>
+    <v>7.8056999999999999</v>
+    <v>102.12</v>
+    <v>104.57</v>
+    <v>104.56</v>
     <v>29393230</v>
     <v>CEIX</v>
     <v>CONSOL ENERGY INC. (XNYS:CEIX)</v>
-    <v>241471</v>
-    <v>446739</v>
+    <v>311631</v>
+    <v>424376</v>
     <v>2017</v>
   </rv>
   <rv s="2">
@@ -5209,11 +5209,11 @@
     <v>Powered by Refinitiv</v>
     <v>127.3484</v>
     <v>84.35</v>
-    <v>1.2521</v>
-    <v>0.64</v>
-    <v>6.5400000000000007E-3</v>
-    <v>0.3</v>
-    <v>3.0459999999999997E-3</v>
+    <v>1.2523</v>
+    <v>1.18</v>
+    <v>1.2257000000000001E-2</v>
+    <v>-1.31</v>
+    <v>-1.3443E-2</v>
     <v>USD</v>
     <v>AGCO Corporation is a designer, manufacturer and distributor of agricultural machinery and precision agriculture technology. The Company sells a range of agricultural equipment, including tractors, combines, self-propelled sprayers, hay tools, forage equipment, seeding and tillage equipment, implements, and grain storage and protein production systems. It provides telemetry-based fleet management tools, including remote monitoring and diagnostics, which help farmers improve uptime, machine and yield optimization, mixed fleet optimization and decision support. The Company's Precision Planting, Headsight and Intelligent Ag Solutions brands provide retrofit solutions to upgrade farmers existing equipment to improve their planting, liquid application and harvest operations. The Company’s Precision Planting, Headsight, JCA and Intelligent Ag Solutions brands also sell precision agriculture solutions around the crop cycle to third party original equipment manufacturers (OEMs).</v>
     <v>27900</v>
@@ -5221,25 +5221,25 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>4205 River Green Pkway, DULUTH, GA, 30096 US</v>
-    <v>99.11</v>
+    <v>97.65</v>
     <v>Machinery, Equipment &amp; Components</v>
     <v>Stock</v>
-    <v>45566.958333356248</v>
+    <v>45569.999739073435</v>
     <v>30</v>
-    <v>95.99</v>
-    <v>7352266550</v>
+    <v>96.65</v>
+    <v>7273892135</v>
     <v>AGCO CORPORATION</v>
     <v>AGCO CORPORATION</v>
-    <v>97.68</v>
-    <v>17.546500000000002</v>
-    <v>97.86</v>
-    <v>98.5</v>
-    <v>98.8</v>
+    <v>97.52</v>
+    <v>17.359300000000001</v>
+    <v>96.27</v>
+    <v>97.45</v>
+    <v>96.14</v>
     <v>74642300</v>
     <v>AGCO</v>
     <v>AGCO CORPORATION (XNYS:AGCO)</v>
-    <v>816477</v>
-    <v>736562</v>
+    <v>450825</v>
+    <v>743528</v>
     <v>1991</v>
   </rv>
   <rv s="2">
@@ -5261,11 +5261,11 @@
     <v>268435456</v>
     <v>1</v>
     <v>Powered by Refinitiv</v>
-    <v>30.1</v>
+    <v>30.07</v>
     <v>24.01</v>
-    <v>1.149</v>
-    <v>-0.01</v>
-    <v>-3.768E-4</v>
+    <v>1.1493</v>
+    <v>0.2</v>
+    <v>7.6829999999999997E-3</v>
     <v>0</v>
     <v>0</v>
     <v>USD</v>
@@ -5275,25 +5275,25 @@
     <v>XNAS</v>
     <v>XNAS</v>
     <v>3 HASHIKMA, A.T AZUR, T.D 163, AZOR, 5800182 IL</v>
-    <v>26.6449</v>
+    <v>26.234999999999999</v>
     <v>Communications &amp; Networking</v>
     <v>Stock</v>
-    <v>45566.834569791405</v>
+    <v>45569.833445775002</v>
     <v>33</v>
-    <v>26.132300000000001</v>
-    <v>527776677</v>
+    <v>25.864999999999998</v>
+    <v>521808603</v>
     <v>ITURAN LOCATION AND CONTROL LTD.</v>
     <v>ITURAN LOCATION AND CONTROL LTD.</v>
-    <v>26.46</v>
-    <v>10.3904</v>
-    <v>26.54</v>
-    <v>26.53</v>
-    <v>26.53</v>
+    <v>26.13</v>
+    <v>10.273</v>
+    <v>26.03</v>
+    <v>26.23</v>
+    <v>26.23</v>
     <v>19893580</v>
     <v>ITRN</v>
     <v>ITURAN LOCATION AND CONTROL LTD. (XNAS:ITRN)</v>
-    <v>77503</v>
-    <v>75796</v>
+    <v>45013</v>
+    <v>73923</v>
     <v>1994</v>
   </rv>
   <rv s="2">
@@ -5317,11 +5317,11 @@
     <v>Powered by Refinitiv</v>
     <v>13.345000000000001</v>
     <v>6.37</v>
-    <v>2.1503000000000001</v>
+    <v>2.1423999999999999</v>
     <v>0</v>
     <v>0</v>
-    <v>0</v>
-    <v>0</v>
+    <v>-0.01</v>
+    <v>-7.6050000000000011E-4</v>
     <v>USD</v>
     <v>Everi Holdings Inc. develops and offers products and services that provide gaming entertainment, improve its customers’ patron engagement, and help its casino customers operate their businesses. It develops and supplies entertaining game content, gaming machines and gaming systems and services for land-based and iGaming operators. It operates through two segments: Games and Financial Technology Solutions (FinTech). The Games segment provides gaming operators with gaming technology and entertainment products and services, including gaming machines, primarily comprising Class II, Class III and Historic Horse Racing slot machines placed under participation and fixed-fee lease arrangements or sold to casino customers. The FinTech segment provides gaming operators with financial technology products and services, including financial access and related services supporting digital, cashless and physical cash options across mobile, assisted and self-service channels.</v>
     <v>2200</v>
@@ -5329,25 +5329,25 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>7250 S Tenaya Way Ste 100, LAS VEGAS, NV, 89113-2175 US</v>
-    <v>13.164999999999999</v>
+    <v>13.19</v>
     <v>Hotels &amp; Entertainment Services</v>
     <v>Stock</v>
-    <v>45566.958333367969</v>
+    <v>45569.98723153906</v>
     <v>36</v>
-    <v>13.13</v>
-    <v>1121151841</v>
+    <v>13.14</v>
+    <v>1122005077</v>
     <v>EVERI HOLDINGS INC.</v>
     <v>EVERI HOLDINGS INC.</v>
-    <v>13.13</v>
-    <v>27.9206</v>
-    <v>13.14</v>
-    <v>13.14</v>
+    <v>13.19</v>
+    <v>27.9312</v>
+    <v>13.15</v>
+    <v>13.15</v>
     <v>13.14</v>
     <v>85323580</v>
     <v>EVRI</v>
     <v>EVERI HOLDINGS INC. (XNYS:EVRI)</v>
-    <v>879914</v>
-    <v>793186</v>
+    <v>756393</v>
+    <v>852168</v>
     <v>2004</v>
   </rv>
   <rv s="2">
@@ -5367,11 +5367,11 @@
     <v>Powered by Refinitiv</v>
     <v>62.31</v>
     <v>32.14</v>
-    <v>2.1160000000000001</v>
-    <v>0.55000000000000004</v>
-    <v>1.4674E-2</v>
-    <v>-0.03</v>
-    <v>-7.8890000000000004E-4</v>
+    <v>2.1190000000000002</v>
+    <v>0.23</v>
+    <v>6.3260000000000009E-3</v>
+    <v>0.13</v>
+    <v>3.5530000000000002E-3</v>
     <v>USD</v>
     <v>Nextracker Inc. is a provider of integrated solar tracker and software solutions used in utility-scale and ground-mounted distributed generation solar projects. Its products enable solar panels in utility-scale power plants to follow the sun’s movement across the sky and optimize plant performance. Its products include NX Horizon, NX Gemini, TrueCapture, and NX Navigator. Its solutions include Bifacial PV modules, Large Format Modules, and First Solar Series 6 (FSLR6) Modules. NX Horizon is a one-in-portrait (1P) smart solar tracker system that delivers the lowest levelized cost of energy (LCOE). NX Gemini is its two-in-portrait (2P) format tracker which holds two rows of solar panels along the central support beam. TrueCapture is its flagship software offering, which is a self-adjusting tracker control system that uses machine learning to enhance solar power plant energy yield. It has operations in the United States, Brazil, Mexico, Spain, India, Australia, the Middle East and Brazil.</v>
     <v>1050</v>
@@ -5379,24 +5379,24 @@
     <v>XNAS</v>
     <v>XNAS</v>
     <v>6200 Paseo Padre Pkwy, FREMONT, CA, 94555 US</v>
-    <v>38.64</v>
+    <v>37.450000000000003</v>
     <v>Renewable Energy</v>
     <v>Stock</v>
-    <v>45566.997395682811</v>
-    <v>35.909999999999997</v>
-    <v>5527561622</v>
+    <v>45569.998900821091</v>
+    <v>36.36</v>
+    <v>5318261366</v>
     <v>NEXTRACKER INC.</v>
     <v>NEXTRACKER INC.</v>
-    <v>37.24</v>
-    <v>10.093</v>
-    <v>37.479999999999997</v>
-    <v>38.03</v>
-    <v>38</v>
+    <v>37.39</v>
+    <v>9.6498000000000008</v>
+    <v>36.36</v>
+    <v>36.590000000000003</v>
+    <v>36.72</v>
     <v>145347400</v>
     <v>NXT</v>
     <v>NEXTRACKER INC. (XNAS:NXT)</v>
-    <v>4746083</v>
-    <v>3197317</v>
+    <v>1974573</v>
+    <v>3290102</v>
     <v>2022</v>
   </rv>
   <rv s="2">
@@ -5420,11 +5420,11 @@
     <v>Powered by Refinitiv</v>
     <v>80.22</v>
     <v>56.25</v>
-    <v>1.7441</v>
-    <v>-1.79</v>
-    <v>-2.2581000000000004E-2</v>
-    <v>0</v>
-    <v>0</v>
+    <v>1.7453000000000001</v>
+    <v>0.86</v>
+    <v>1.1153999999999999E-2</v>
+    <v>-0.08</v>
+    <v>-1.026E-3</v>
     <v>USD</v>
     <v>Monarch Casino &amp; Resort, Inc. owns and operates the Atlantis Casino Resort Spa, a hotel and casino in Reno, Nevada (the Atlantis) and the Monarch Casino Resort Spa Black Hawk (the Monarch Black Hawk), a hotel and casino in Black Hawk, Colorado. In addition, it owns separate parcels of land located next to the Atlantis and a parcel of land with an industrial warehouse located between Denver, Colorado, and Monarch Black Hawk. The Atlantis is located approximately three miles south of downtown, which features approximately 61,000 square feet of casino space; 817 guest rooms and suites; eight food outlets; two gourmet coffee and pastry bars and one snack bar; a 30,000 square-foot health spa and salon with an enclosed year-round pool. Monarch Black Hawk features approximately 60,000 square feet of casino space; approximately 1,000 slot machines; approximately 43 table games; a live poker room; a keno counter and a sports book. The resort also includes 10 bars and lounges.</v>
     <v>2900</v>
@@ -5432,25 +5432,25 @@
     <v>XNAS</v>
     <v>XNAS</v>
     <v>Executive Offices, 3800 S Virginia Street, RENO, NV, 89502 US</v>
-    <v>79.010000000000005</v>
+    <v>77.968999999999994</v>
     <v>Hotels &amp; Entertainment Services</v>
     <v>Stock</v>
-    <v>45566.8492548375</v>
+    <v>45569.888832661716</v>
     <v>41</v>
-    <v>77.209999999999994</v>
-    <v>1462699000</v>
+    <v>76.95</v>
+    <v>1438527275</v>
     <v>MONARCH CASINO &amp; RESORT, INC.</v>
     <v>MONARCH CASINO &amp; RESORT, INC.</v>
-    <v>79.010000000000005</v>
-    <v>18.106400000000001</v>
-    <v>79.27</v>
-    <v>77.48</v>
-    <v>77.48</v>
+    <v>77.78</v>
+    <v>18.017600000000002</v>
+    <v>77.099999999999994</v>
+    <v>77.959999999999994</v>
+    <v>77.88</v>
     <v>18452120</v>
     <v>MCRI</v>
     <v>MONARCH CASINO &amp; RESORT, INC. (XNAS:MCRI)</v>
-    <v>91136</v>
-    <v>156956</v>
+    <v>117758</v>
+    <v>156287</v>
     <v>1993</v>
   </rv>
   <rv s="2">
@@ -5474,11 +5474,11 @@
     <v>Powered by Refinitiv</v>
     <v>69.75</v>
     <v>34.96</v>
-    <v>0.96919999999999995</v>
-    <v>-1.1399999999999999</v>
-    <v>-1.8689000000000001E-2</v>
-    <v>-0.02</v>
-    <v>-3.3410000000000004E-4</v>
+    <v>0.9647</v>
+    <v>0.15</v>
+    <v>2.4260000000000002E-3</v>
+    <v>0.04</v>
+    <v>6.4530000000000002E-4</v>
     <v>USD</v>
     <v>Miller Industries, Inc. is a manufacturer of towing and recovery equipment. The Company designs and manufactures bodies of car carriers and wreckers, which are installed on chassis manufactured by third parties, and sold to its customers. Its products are marketed and sold through a network of distributors that serve all 50 states, Canada, Mexico, and other foreign markets, and through prime contractors to governmental entities. In addition to selling its products, its independent distributors provide end-users with parts and service. Its product line includes car carriers, wreckers, and transport trailers. Car carriers are specialized flat-bed vehicles with hydraulic tilt mechanisms that enable a towing operator to drive or winch a vehicle onto the bed for transport. Its multi-vehicle transport trailers are specialized auto transport trailers with upper and lower decks and hydraulic ramps for loading vehicles. Its brands include Century, Vulcan, Chevron, Holmes, and Challenger.</v>
     <v>1821</v>
@@ -5486,25 +5486,25 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>Ste 100, 8503 Hilltop Dr, OOLTEWAH, TN, 37363 US</v>
-    <v>60.91</v>
+    <v>63.13</v>
     <v>Automobiles &amp; Auto Parts</v>
     <v>Stock</v>
-    <v>45566.958333356248</v>
+    <v>45569.960431250001</v>
     <v>44</v>
-    <v>58.68</v>
-    <v>685623869</v>
+    <v>61.52</v>
+    <v>710020442</v>
     <v>MILLER INDUSTRIES, INC.</v>
     <v>MILLER INDUSTRIES, INC.</v>
-    <v>60.91</v>
-    <v>9.6365999999999996</v>
-    <v>61</v>
-    <v>59.86</v>
-    <v>59.84</v>
+    <v>63.13</v>
+    <v>9.9795999999999996</v>
+    <v>61.84</v>
+    <v>61.99</v>
+    <v>62.03</v>
     <v>11453790</v>
     <v>MLR</v>
     <v>MILLER INDUSTRIES, INC. (XNYS:MLR)</v>
-    <v>85975</v>
-    <v>93982</v>
+    <v>68823</v>
+    <v>101679</v>
     <v>1994</v>
   </rv>
   <rv s="2">
@@ -5528,11 +5528,11 @@
     <v>Powered by Refinitiv</v>
     <v>15.86</v>
     <v>9.1649999999999991</v>
-    <v>0.88439999999999996</v>
-    <v>-0.44</v>
-    <v>-4.3521000000000004E-2</v>
-    <v>0.12</v>
-    <v>1.2410000000000001E-2</v>
+    <v>0.88660000000000005</v>
+    <v>0.18</v>
+    <v>1.873E-2</v>
+    <v>0.02</v>
+    <v>2.0430000000000001E-3</v>
     <v>USD</v>
     <v>Janus International Group, Inc. is a global manufacturer and supplier of turn-key self-storage, commercial and industrial building solutions. It operates through two geographic segments: Janus North America and Janus International. The Janus North America segment is comprised of all the other entities, including Janus International Group, LLC, Betco, Inc., Noke, Inc., Asta Industries, Inc., DBCI, LLC, Access Control Technologies, LLC, Janus Door, LLC, and Steel Door Depot.com, LLC. The Janus International segment is comprised of Janus International Europe Holdings Ltd. (UK). Its production and sales are in Europe and Australia. It provides facility and door automation and access control technologies, roll up and swing doors, hallway systems and relocatable storage moveable additional storage structures (MASS) units. It is comprised of three sales channels, including New Construction-Self-storage, R3-Self-storage, and Commercial and Other. It also provides terminal maintenance services.</v>
     <v>1956</v>
@@ -5540,25 +5540,25 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>135 Janus International Blvd., TEMPLE, GA, 30179 US</v>
-    <v>10.11</v>
+    <v>9.8149999999999995</v>
     <v>Homebuilding &amp; Construction Supplies</v>
     <v>Stock</v>
-    <v>45566.958333367969</v>
+    <v>45569.958333367969</v>
     <v>47</v>
-    <v>9.6</v>
-    <v>1469208000</v>
+    <v>9.43</v>
+    <v>1396547000</v>
     <v>JANUS INTERNATIONAL GROUP, INC.</v>
     <v>JANUS INTERNATIONAL GROUP, INC.</v>
-    <v>10.09</v>
-    <v>10.8431</v>
-    <v>10.11</v>
-    <v>9.67</v>
+    <v>9.6999999999999993</v>
+    <v>10.9778</v>
+    <v>9.61</v>
     <v>9.7899999999999991</v>
+    <v>9.81</v>
     <v>145322200</v>
     <v>JBI</v>
     <v>JANUS INTERNATIONAL GROUP, INC. (XNYS:JBI)</v>
-    <v>2615441</v>
-    <v>2054349</v>
+    <v>1675210</v>
+    <v>2130654</v>
     <v>2020</v>
   </rv>
   <rv s="2">
@@ -5582,11 +5582,11 @@
     <v>Powered by Refinitiv</v>
     <v>574.76</v>
     <v>318.17</v>
-    <v>1.3159000000000001</v>
-    <v>-9.99</v>
-    <v>-2.5672999999999998E-2</v>
-    <v>-0.63</v>
-    <v>-1.6619999999999998E-3</v>
+    <v>1.3221000000000001</v>
+    <v>9.08</v>
+    <v>2.4361000000000001E-2</v>
+    <v>-11.86</v>
+    <v>-3.1063E-2</v>
     <v>USD</v>
     <v>Ulta Beauty, Inc. is a beauty retailer. The Company's product categories include cosmetics, skincare, haircare products and styling tools, fragrance and bath, services, and accessories and other. The Company has one segment, which includes retail stores, salon services, and e-commerce. It offers a range of beauty services in its stores, focusing on hair, makeup, brow and skin services. Its skin services include a skin treatment room or dedicated skin treatment area on the sales floor. Its Ulta Beauty store prototype includes an open salon area, with most of its stores offering brow services on the salon floor. It offers a new way to shop for beauty - bringing together All Things Beauty, All in One Place. In addition to ship to home order fulfillment, it offers guests Buy Online, Pick-up in Store, Curbside Pickup, and Store 2 Door, which provides the ability for customers to order in-store and have products delivered to their homes. It operates over 1,350 retail stores across 50 states.</v>
     <v>20000</v>
@@ -5594,25 +5594,25 @@
     <v>XNAS</v>
     <v>XNAS</v>
     <v>1000 Remington Blvd, Suite 120, BOLINGBROOK, IL, 60440 US</v>
-    <v>386.755</v>
+    <v>384.61</v>
     <v>Specialty Retailers</v>
     <v>Stock</v>
-    <v>45566.999979687498</v>
+    <v>45569.998672001566</v>
     <v>50</v>
-    <v>377.07</v>
-    <v>17862607584</v>
+    <v>377.01</v>
+    <v>17988403914</v>
     <v>ULTA BEAUTY, INC.</v>
     <v>ULTA BEAUTY, INC.</v>
-    <v>386.17</v>
-    <v>15.223800000000001</v>
-    <v>389.12</v>
-    <v>379.13</v>
-    <v>378.5</v>
+    <v>380.59</v>
+    <v>15.2249</v>
+    <v>372.72</v>
+    <v>381.8</v>
+    <v>369.94</v>
     <v>47114730</v>
     <v>ULTA</v>
     <v>ULTA BEAUTY, INC. (XNAS:ULTA)</v>
-    <v>1175859</v>
-    <v>1430015</v>
+    <v>1158971</v>
+    <v>1427579</v>
     <v>2016</v>
   </rv>
   <rv s="2">
@@ -5636,11 +5636,11 @@
     <v>Powered by Refinitiv</v>
     <v>31.85</v>
     <v>18.899999999999999</v>
-    <v>1.9643999999999999</v>
-    <v>-0.32</v>
-    <v>-1.5023E-2</v>
-    <v>0.02</v>
-    <v>9.5330000000000002E-4</v>
+    <v>1.9713000000000001</v>
+    <v>0.17</v>
+    <v>8.2480000000000001E-3</v>
+    <v>0.04</v>
+    <v>1.9250000000000001E-3</v>
     <v>USD</v>
     <v>International Game Technology PLC is a United Kingdom-based company, which is engaged in gaming. The Company operates and provides an integrated portfolio of gaming technology products and services, including online and instant lottery systems, iLottery, instant ticket printing, lottery management services, commercial services, gaming systems, electronic gaming machines, iGaming, and sports betting. The Company operates through three segments. The Global Lottery segment operates traditional lottery and iLottery businesses across the world, which includes sales, operations, product development, technology, and support, across the world. The Global Gaming segment operates a land-based gaming business across the world, which includes sales, product management, studios, global manufacturing, operation, and technology, across the world. The Digital &amp; Betting segment operates iGaming and sports betting activities across the world.</v>
     <v>11000</v>
@@ -5648,25 +5648,25 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>10 Finsbury Square, Third Floor, LONDON, UNITED KINGDOM-NA, EC2A 1AF GB</v>
-    <v>21.285</v>
+    <v>21.03</v>
     <v>Hotels &amp; Entertainment Services</v>
     <v>Stock</v>
-    <v>45566.958333367969</v>
+    <v>45569.958333356248</v>
     <v>53</v>
-    <v>20.9</v>
-    <v>4196000000</v>
+    <v>20.73</v>
+    <v>4156000000</v>
     <v>INTERNATIONAL GAME TECHNOLOGY PLC</v>
     <v>INTERNATIONAL GAME TECHNOLOGY PLC</v>
-    <v>21.23</v>
-    <v>20.298200000000001</v>
-    <v>21.3</v>
     <v>20.98</v>
-    <v>21</v>
+    <v>20.104500000000002</v>
+    <v>20.61</v>
+    <v>20.78</v>
+    <v>20.82</v>
     <v>200000000</v>
     <v>IGT</v>
     <v>INTERNATIONAL GAME TECHNOLOGY PLC (XNYS:IGT)</v>
-    <v>1439886</v>
-    <v>675009</v>
+    <v>559848</v>
+    <v>725396</v>
     <v>2014</v>
   </rv>
   <rv s="2">
@@ -5690,9 +5690,9 @@
     <v>Powered by Refinitiv</v>
     <v>87.32</v>
     <v>54.8</v>
-    <v>0.58520000000000005</v>
-    <v>0.27</v>
-    <v>3.9139999999999999E-3</v>
+    <v>0.58860000000000001</v>
+    <v>0.92</v>
+    <v>1.3990000000000001E-2</v>
     <v>0</v>
     <v>0</v>
     <v>USD</v>
@@ -5702,25 +5702,25 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>SUITE 400, 410 NORTH MICHIGAN AVENUE, CHICAGO, IL, 60611 US</v>
-    <v>69.989999999999995</v>
+    <v>66.959999999999994</v>
     <v>Chemicals</v>
     <v>Stock</v>
-    <v>45566.958333344533</v>
+    <v>45569.958333344533</v>
     <v>56</v>
-    <v>68.235399999999998</v>
-    <v>502683400</v>
+    <v>66.25</v>
+    <v>479148600</v>
     <v>OIL-DRI CORPORATION OF AMERICA</v>
     <v>OIL-DRI CORPORATION OF AMERICA</v>
-    <v>68.989999999999995</v>
-    <v>14.212999999999999</v>
-    <v>68.989999999999995</v>
-    <v>69.260000000000005</v>
-    <v>69.260000000000005</v>
+    <v>66.75</v>
+    <v>13.6836</v>
+    <v>65.760000000000005</v>
+    <v>66.680000000000007</v>
+    <v>66.680000000000007</v>
     <v>7286320</v>
     <v>ODC</v>
     <v>OIL-DRI CORPORATION OF AMERICA (XNYS:ODC)</v>
-    <v>19358</v>
-    <v>16307</v>
+    <v>14802</v>
+    <v>16359</v>
     <v>1969</v>
   </rv>
   <rv s="2">
@@ -5744,11 +5744,11 @@
     <v>Powered by Refinitiv</v>
     <v>170.9692</v>
     <v>93.77</v>
-    <v>1.5757000000000001</v>
-    <v>-3.09</v>
-    <v>-2.9470999999999997E-2</v>
-    <v>-0.8</v>
-    <v>-7.8620000000000009E-3</v>
+    <v>1.5775999999999999</v>
+    <v>0.67</v>
+    <v>6.7259999999999993E-3</v>
+    <v>0.22</v>
+    <v>2.1940000000000002E-3</v>
     <v>USD</v>
     <v>Axcelis Technologies, Inc. designs, manufactures and services ion implantation and other processing equipment used in the fabrication of semiconductor chips. The Company offers a complete line of high energy, high current and medium current implanters for all application requirements. In addition to equipment, the Company provides extensive aftermarket lifecycle products and services, including used tools, spare parts, equipment upgrades, maintenance services and customer training. Its Purion flagship systems are all based on a common platform, which enables a combination of implant purity, precision and productivity. Combining a single wafer end station, with advanced spot beam architectures (that ensures all points across the wafer see the same beam condition at the same beam angle), Purion products enable process control to optimize device performance and yield, at high productivity. The Company sells its products to semiconductor chip manufacturers around the world.</v>
     <v>1620</v>
@@ -5756,25 +5756,25 @@
     <v>XNAS</v>
     <v>XNAS</v>
     <v>108 Cherry Hill Dr, BEVERLY, MA, 01915 US</v>
-    <v>105</v>
+    <v>102.54</v>
     <v>Semiconductors &amp; Semiconductor Equipment</v>
     <v>Stock</v>
-    <v>45566.957719096878</v>
+    <v>45569.976284375</v>
     <v>59</v>
-    <v>99.385000000000005</v>
-    <v>3319165958</v>
+    <v>100.17</v>
+    <v>3270891925</v>
     <v>AXCELIS TECHNOLOGIES, INC.</v>
     <v>AXCELIS TECHNOLOGIES, INC.</v>
-    <v>104.99</v>
-    <v>14.0197</v>
-    <v>104.85</v>
-    <v>101.76</v>
-    <v>100.96</v>
+    <v>102.17</v>
+    <v>13.7235</v>
+    <v>99.61</v>
+    <v>100.28</v>
+    <v>100.5</v>
     <v>32617590</v>
     <v>ACLS</v>
     <v>AXCELIS TECHNOLOGIES, INC. (XNAS:ACLS)</v>
-    <v>517171</v>
-    <v>647845</v>
+    <v>448826</v>
+    <v>655003</v>
     <v>1995</v>
   </rv>
   <rv s="2">
@@ -5798,11 +5798,11 @@
     <v>Powered by Refinitiv</v>
     <v>179.7</v>
     <v>63.9</v>
-    <v>0.89410000000000001</v>
-    <v>-5.38</v>
-    <v>-4.5385999999999996E-2</v>
-    <v>-0.61</v>
-    <v>-5.391E-3</v>
+    <v>0.89510000000000001</v>
+    <v>4.75</v>
+    <v>4.1064999999999997E-2</v>
+    <v>-0.02</v>
+    <v>-1.661E-4</v>
     <v>USD</v>
     <v>Dell Technologies Inc. is engaged in designing, developing, manufacturing, marketing, selling, and supporting a wide range of comprehensive and integrated solutions, products, and services. The Company operates through two segments: Infrastructure Solutions Group (ISG) and Client Solutions Group (CSG). Its ISG segment enables the Company’s customer’s digital transformation with solutions that address artificial intelligence (AI), machine learning, data analytics, and multi cloud environments. Its comprehensive storage portfolio includes modern and traditional storage solutions, including all-flash arrays, scale-out file, object platforms, hyper-converged infrastructure, and software-defined storage. Its CSG segment offers branded personal computers (PCs) including notebooks, desktops, and workstations and branded peripherals that include displays, docking stations, keyboards, mice, and webcam and audio devices, as well as third-party software and peripherals.</v>
     <v>120000</v>
@@ -5810,25 +5810,25 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>ONE DELL WAY, ROUND ROCK, TX, 78682 US</v>
-    <v>117.78</v>
+    <v>120.84</v>
     <v>Computers, Phones &amp; Household Electronics</v>
     <v>Stock</v>
-    <v>45566.99978961797</v>
+    <v>45569.999740462503</v>
     <v>62</v>
-    <v>112.91</v>
-    <v>79437923940</v>
+    <v>117.06010000000001</v>
+    <v>84534418530</v>
     <v>DELL TECHNOLOGIES INC.</v>
     <v>DELL TECHNOLOGIES INC.</v>
-    <v>117.39</v>
-    <v>20.8217</v>
-    <v>118.54</v>
-    <v>113.16</v>
-    <v>112.55</v>
+    <v>117.5</v>
+    <v>22.157599999999999</v>
+    <v>115.67</v>
+    <v>120.42</v>
+    <v>120.4</v>
     <v>701996500</v>
     <v>DELL</v>
     <v>DELL TECHNOLOGIES INC. (XNYS:DELL)</v>
-    <v>9641850</v>
-    <v>14116347</v>
+    <v>8185053</v>
+    <v>14094510</v>
     <v>2013</v>
   </rv>
   <rv s="2">
@@ -5850,13 +5850,13 @@
     <v>268435456</v>
     <v>1</v>
     <v>Powered by Refinitiv</v>
-    <v>34.11</v>
+    <v>34.079900000000002</v>
     <v>25.2</v>
-    <v>0.6522</v>
-    <v>-0.27</v>
-    <v>-9.3299999999999998E-3</v>
-    <v>0</v>
-    <v>0</v>
+    <v>0.6492</v>
+    <v>0.24</v>
+    <v>8.4689999999999991E-3</v>
+    <v>0.05</v>
+    <v>1.7489999999999999E-3</v>
     <v>USD</v>
     <v>Pfizer Inc. is a research-based global biopharmaceutical company. The Company is engaged in the discovery, development, manufacture, marketing, sale and distribution of biopharmaceutical products worldwide. Its Biopharma segment is engaged in the science-based biopharmaceutical business. Its Biopharma segment includes the Pfizer Oncology Division, the Pfizer U.S. Commercial Division, and the Pfizer International Commercial Division. Its product categories include oncology, primary care and specialty care. Its Oncology products include Ibrance, Xtandi, Inlyta, Bosulif, Lorbrena, Braftovi, Mektovi, Padcev, Adcetris, Talzenna, Tukysa, Elrexfio and Tivdak. Its primary care products include Eliquis, Nurtec ODT/Vydura, Comirnaty, the Prevnar family, Abrysvo, FSME/IMMUN-TicoVac, Paxlovid and Lucira by Pfizer. Its specialty care products include Xeljanz, Enbrel (outside the U.S. and Canada), Inflectra, Cibinqo, Litfulo, Vyndaqel family, Genotropin, Sulperazon, Zavicefta, Medrol and Panzyga.</v>
     <v>88000</v>
@@ -5864,24 +5864,24 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>66 HUDSON BOULEVARD EAST, NEW YORK, NY, 10001-2192 US</v>
-    <v>29.08</v>
+    <v>28.59</v>
     <v>Pharmaceuticals</v>
     <v>Stock</v>
-    <v>45566.999642291405</v>
+    <v>45569.999953645311</v>
     <v>65</v>
-    <v>28.53</v>
-    <v>162464145650</v>
+    <v>28.24</v>
+    <v>161954143100</v>
     <v>PFIZER INC.</v>
     <v>PFIZER INC.</v>
-    <v>29.05</v>
-    <v>28.94</v>
-    <v>28.67</v>
-    <v>28.67</v>
+    <v>28.29</v>
+    <v>28.34</v>
+    <v>28.58</v>
+    <v>28.63</v>
     <v>5666695000</v>
     <v>PFE</v>
     <v>PFIZER INC. (XNYS:PFE)</v>
-    <v>30725106</v>
-    <v>28368037</v>
+    <v>28786884</v>
+    <v>29519892</v>
     <v>1942</v>
   </rv>
   <rv s="2">
@@ -5905,11 +5905,11 @@
     <v>Powered by Refinitiv</v>
     <v>30.32</v>
     <v>18.945</v>
-    <v>1.4074</v>
-    <v>-0.44</v>
-    <v>-2.1836000000000001E-2</v>
-    <v>0.04</v>
-    <v>2.029E-3</v>
+    <v>1.4095</v>
+    <v>0.33</v>
+    <v>1.6863E-2</v>
+    <v>0.05</v>
+    <v>2.513E-3</v>
     <v>USD</v>
     <v>Franklin Resources, Inc. is a global investment management company with subsidiaries operating as Franklin Templeton and serving clients in over 150 countries. It offers specialization on a global scale, bringing capabilities in fixed income, equity, alternatives and multi-asset solutions. The Company provides its investment management and related services to retail, institutional and high-net-worth investors in jurisdictions worldwide. Its investment products include sponsored funds, as well as institutional and high-net-worth separate accounts, retail separately managed account programs, sub-advised products, and other investment vehicles. Its funds include registered funds (including exchange-traded funds or ETFs) and unregistered funds. The Company offers its services and products under its various brand names, including Alcentra, K2, Benefit Street Partners, ClearBridge Investments, Martin Currie, O’Shaughnessy, and Lexington Partners. It also focuses on the retirement sector.</v>
     <v>10300</v>
@@ -5917,25 +5917,25 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>One Franklin Parkway, Building 920/2, SAN MATEO, CA, 94403 US</v>
-    <v>20.16</v>
+    <v>19.93</v>
     <v>Investment Banking &amp; Investment Services</v>
     <v>Stock</v>
-    <v>45566.997916596876</v>
+    <v>45569.991273760941</v>
     <v>68</v>
-    <v>19.7</v>
-    <v>10308298464</v>
+    <v>19.510100000000001</v>
+    <v>10407668160</v>
     <v>FRANKLIN RESOURCES, INC.</v>
     <v>FRANKLIN RESOURCES, INC.</v>
-    <v>20.11</v>
-    <v>12.308400000000001</v>
-    <v>20.149999999999999</v>
-    <v>19.71</v>
-    <v>19.75</v>
+    <v>19.8</v>
+    <v>12.4274</v>
+    <v>19.57</v>
+    <v>19.899999999999999</v>
+    <v>19.95</v>
     <v>522998400</v>
     <v>BEN</v>
     <v>FRANKLIN RESOURCES, INC. (XNYS:BEN)</v>
-    <v>4181229</v>
-    <v>4996892</v>
+    <v>3169543</v>
+    <v>4647003</v>
     <v>1969</v>
   </rv>
   <rv s="2">
@@ -5959,11 +5959,11 @@
     <v>Powered by Refinitiv</v>
     <v>26.15</v>
     <v>20.190000000000001</v>
-    <v>1.1435999999999999</v>
-    <v>-0.5</v>
-    <v>-1.9983999999999998E-2</v>
-    <v>0</v>
-    <v>0</v>
+    <v>1.1473</v>
+    <v>-0.01</v>
+    <v>-4.1369999999999997E-4</v>
+    <v>0.09</v>
+    <v>3.725E-3</v>
     <v>USD</v>
     <v>UGI Corporation is a holding company, which distributes, stores, transports and markets energy products and related services. In the United States, the Company owns and operates a retail propane marketing and distribution business, natural gas and electric distribution utilities, and energy marketing, midstream infrastructure, storage, natural gas gathering and processing, natural gas production, electricity generation and energy services businesses. In Europe, the Company markets and distributes propane and other liquified petroleum gas (LPG), and market other energy products and services. It operates through four segments: AmeriGas Propane, UGI International, Midstream &amp; Marketing, and Utilities. The AmeriGas Propane segment operates propane distribution business. The UGI International segment consists of LPG distribution businesses in Austria, Belgium, the Czech Republic, Denmark, Finland, France, Hungary, Italy, Luxembourg, the Netherlands, Norway, Poland, Romania and others.</v>
     <v>5160</v>
@@ -5971,25 +5971,25 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>500 N GULPH RD, P O BOX 858, KING OF PRUSSIA, PA, 19406 US</v>
-    <v>25.1</v>
+    <v>24.36</v>
     <v>Natural Gas Utilities</v>
     <v>Stock</v>
-    <v>45566.991050740624</v>
+    <v>45569.971942198441</v>
     <v>71</v>
-    <v>24.41</v>
-    <v>5264164472</v>
+    <v>24.01</v>
+    <v>5186876576</v>
     <v>UGI CORPORATION</v>
     <v>UGI CORPORATION</v>
-    <v>24.95</v>
-    <v>7.8066000000000004</v>
-    <v>25.02</v>
-    <v>24.52</v>
-    <v>24.52</v>
+    <v>24.17</v>
+    <v>7.6920999999999999</v>
+    <v>24.17</v>
+    <v>24.16</v>
+    <v>24.25</v>
     <v>214688600</v>
     <v>UGI</v>
     <v>UGI CORPORATION (XNYS:UGI)</v>
-    <v>1892121</v>
-    <v>2118867</v>
+    <v>1047760</v>
+    <v>2083774</v>
     <v>1991</v>
   </rv>
   <rv s="2">
@@ -6338,9 +6338,9 @@
       <v>at close</v>
       <v>from previous close</v>
       <v>from previous close</v>
-      <v>Source: Nasdaq Last Sale</v>
+      <v>Source: Nasdaq</v>
       <v>GMT</v>
-      <v>Real-Time Nasdaq Last Sale</v>
+      <v>Delayed 15 minutes</v>
       <v>from close</v>
       <v>from close</v>
     </spb>
@@ -7610,8 +7610,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X1011"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A87" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D117" sqref="D117"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A97" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D121" sqref="D121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -15338,38 +15338,38 @@
         <v>39</v>
       </c>
       <c r="C115" s="70">
-        <v>0</v>
+        <v>22834</v>
       </c>
       <c r="D115" s="93">
         <v>-588</v>
       </c>
       <c r="E115" s="70">
         <f t="shared" si="23"/>
-        <v>588</v>
+        <v>23422</v>
       </c>
       <c r="F115" s="81">
         <f t="shared" si="24"/>
-        <v>3.4227647113707063</v>
+        <v>136.34012766959981</v>
       </c>
       <c r="G115" s="80">
         <f t="shared" si="25"/>
-        <v>-3.6701247469453713</v>
+        <v>1.4579335758084485E-2</v>
       </c>
       <c r="H115" s="80">
         <f t="shared" si="29"/>
-        <v>-3.3747215663513037</v>
+        <v>0.30998251635215185</v>
       </c>
       <c r="I115" s="80">
         <f>(F115-MAX($F$2:F115))/MAX($F$2:F115)</f>
-        <v>-0.97472767539873384</v>
+        <v>0</v>
       </c>
       <c r="J115" s="80">
         <f>(F115-MAX($F$3:F115))/MIN($F$3:F115)</f>
-        <v>-38.568975777950449</v>
+        <v>0</v>
       </c>
       <c r="K115" s="80">
         <f>STDEV($G$4:G115)*SQRT(52)</f>
-        <v>2.5124988026412689</v>
+        <v>0.2224006427861763</v>
       </c>
       <c r="L115" s="82"/>
       <c r="M115" s="82"/>
@@ -15380,19 +15380,19 @@
       </c>
       <c r="P115" s="106">
         <f t="shared" si="26"/>
-        <v>-3.6707016700222943</v>
+        <v>1.4002412681161407E-2</v>
       </c>
       <c r="Q115" s="106">
         <f t="shared" si="27"/>
-        <v>-3.6707016700222943</v>
+        <v>0</v>
       </c>
       <c r="R115" s="107">
         <f t="shared" si="28"/>
-        <v>13.47405075030446</v>
+        <v>0</v>
       </c>
       <c r="S115" s="90">
         <f>AVERAGE($P$3:P115)/SQRT(AVERAGE($R$3:R115))</f>
-        <v>-8.7999171265827014E-2</v>
+        <v>0.10453387869513152</v>
       </c>
       <c r="T115" s="2"/>
       <c r="U115" s="3"/>
@@ -15406,38 +15406,38 @@
         <v>40</v>
       </c>
       <c r="C116" s="70">
-        <v>0</v>
+        <v>21434</v>
       </c>
       <c r="D116" s="93">
         <v>-1190</v>
       </c>
       <c r="E116" s="70">
         <f t="shared" si="23"/>
-        <v>1190</v>
-      </c>
-      <c r="F116" s="81" t="e">
+        <v>22624</v>
+      </c>
+      <c r="F116" s="81">
         <f t="shared" si="24"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G116" s="80" t="e">
+        <v>135.08623317846309</v>
+      </c>
+      <c r="G116" s="80">
         <f t="shared" si="25"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H116" s="80" t="e">
+        <v>-9.2393635399732246E-3</v>
+      </c>
+      <c r="H116" s="80">
         <f t="shared" si="29"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I116" s="80" t="e">
+        <v>0.30074315281217862</v>
+      </c>
+      <c r="I116" s="80">
         <f>(F116-MAX($F$2:F116))/MAX($F$2:F116)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J116" s="80" t="e">
+        <v>-9.1968117719190348E-3</v>
+      </c>
+      <c r="J116" s="80">
         <f>(F116-MAX($F$3:F116))/MIN($F$3:F116)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K116" s="80" t="e">
+        <v>-1.440451638744137E-2</v>
+      </c>
+      <c r="K116" s="80">
         <f>STDEV($G$4:G116)*SQRT(52)</f>
-        <v>#DIV/0!</v>
+        <v>0.2215577829785049</v>
       </c>
       <c r="L116" s="82"/>
       <c r="M116" s="82"/>
@@ -15446,21 +15446,21 @@
         <f t="shared" si="3"/>
         <v>5.7692307692307687E-4</v>
       </c>
-      <c r="P116" s="106" t="e">
+      <c r="P116" s="106">
         <f t="shared" si="26"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q116" s="106" t="e">
+        <v>-9.8162866168963019E-3</v>
+      </c>
+      <c r="Q116" s="106">
         <f t="shared" si="27"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R116" s="107" t="e">
+        <v>-9.8162866168963019E-3</v>
+      </c>
+      <c r="R116" s="107">
         <f t="shared" si="28"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S116" s="90" t="e">
+        <v>9.6359482945057443E-5</v>
+      </c>
+      <c r="S116" s="90">
         <f>AVERAGE($P$3:P116)/SQRT(AVERAGE($R$3:R116))</f>
-        <v>#DIV/0!</v>
+        <v>9.9801883455708534E-2</v>
       </c>
       <c r="T116" s="2"/>
       <c r="U116" s="3"/>
@@ -15481,21 +15481,21 @@
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
-      <c r="F117" s="81" t="e">
+      <c r="F117" s="81">
         <f t="shared" si="24"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="G117" s="80" t="e">
         <f t="shared" si="25"/>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="H117" s="80" t="e">
         <f t="shared" si="29"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I117" s="80" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="I117" s="80">
         <f>(F117-MAX($F$2:F117))/MAX($F$2:F117)</f>
-        <v>#DIV/0!</v>
+        <v>-1</v>
       </c>
       <c r="J117" s="80" t="e">
         <f>(F117-MAX($F$3:F117))/MIN($F$3:F117)</f>
@@ -15503,7 +15503,7 @@
       </c>
       <c r="K117" s="80" t="e">
         <f>STDEV($G$4:G117)*SQRT(52)</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="L117" s="82"/>
       <c r="M117" s="82"/>
@@ -15514,19 +15514,19 @@
       </c>
       <c r="P117" s="106" t="e">
         <f t="shared" si="26"/>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="Q117" s="106" t="e">
         <f t="shared" si="27"/>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="R117" s="107" t="e">
         <f t="shared" si="28"/>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="S117" s="90" t="e">
         <f>AVERAGE($P$3:P117)/SQRT(AVERAGE($R$3:R117))</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="T117" s="2"/>
       <c r="U117" s="3"/>
@@ -15557,7 +15557,7 @@
       </c>
       <c r="H118" s="80" t="e">
         <f t="shared" si="29"/>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="I118" s="80" t="e">
         <f>(F118-MAX($F$2:F118))/MAX($F$2:F118)</f>
@@ -15569,7 +15569,7 @@
       </c>
       <c r="K118" s="80" t="e">
         <f>STDEV($G$4:G118)*SQRT(52)</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="L118" s="82"/>
       <c r="M118" s="82"/>
@@ -15592,7 +15592,7 @@
       </c>
       <c r="S118" s="90" t="e">
         <f>AVERAGE($P$3:P118)/SQRT(AVERAGE($R$3:R118))</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="T118" s="2"/>
       <c r="U118" s="3"/>
@@ -15623,7 +15623,7 @@
       </c>
       <c r="H119" s="80" t="e">
         <f t="shared" si="29"/>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="I119" s="80" t="e">
         <f>(F119-MAX($F$2:F119))/MAX($F$2:F119)</f>
@@ -15635,7 +15635,7 @@
       </c>
       <c r="K119" s="80" t="e">
         <f>STDEV($G$4:G119)*SQRT(52)</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="L119" s="82"/>
       <c r="M119" s="82"/>
@@ -15658,7 +15658,7 @@
       </c>
       <c r="S119" s="90" t="e">
         <f>AVERAGE($P$3:P119)/SQRT(AVERAGE($R$3:R119))</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="T119" s="2"/>
       <c r="U119" s="3"/>
@@ -15689,7 +15689,7 @@
       </c>
       <c r="H120" s="80" t="e">
         <f t="shared" si="29"/>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="I120" s="80" t="e">
         <f>(F120-MAX($F$2:F120))/MAX($F$2:F120)</f>
@@ -15701,7 +15701,7 @@
       </c>
       <c r="K120" s="80" t="e">
         <f>STDEV($G$4:G120)*SQRT(52)</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="L120" s="82"/>
       <c r="M120" s="82"/>
@@ -15724,7 +15724,7 @@
       </c>
       <c r="S120" s="90" t="e">
         <f>AVERAGE($P$3:P120)/SQRT(AVERAGE($R$3:R120))</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="T120" s="2"/>
       <c r="U120" s="3"/>
@@ -15755,7 +15755,7 @@
       </c>
       <c r="H121" s="80" t="e">
         <f t="shared" si="29"/>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="I121" s="80" t="e">
         <f>(F121-MAX($F$2:F121))/MAX($F$2:F121)</f>
@@ -15767,7 +15767,7 @@
       </c>
       <c r="K121" s="80" t="e">
         <f>STDEV($G$4:G121)*SQRT(52)</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="L121" s="82"/>
       <c r="M121" s="82"/>
@@ -15790,7 +15790,7 @@
       </c>
       <c r="S121" s="90" t="e">
         <f>AVERAGE($P$3:P121)/SQRT(AVERAGE($R$3:R121))</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="T121" s="2"/>
       <c r="U121" s="3"/>
@@ -15821,7 +15821,7 @@
       </c>
       <c r="H122" s="80" t="e">
         <f t="shared" si="29"/>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="I122" s="80" t="e">
         <f>(F122-MAX($F$2:F122))/MAX($F$2:F122)</f>
@@ -15833,7 +15833,7 @@
       </c>
       <c r="K122" s="80" t="e">
         <f>STDEV($G$4:G122)*SQRT(52)</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="L122" s="82"/>
       <c r="M122" s="82"/>
@@ -15856,7 +15856,7 @@
       </c>
       <c r="S122" s="90" t="e">
         <f>AVERAGE($P$3:P122)/SQRT(AVERAGE($R$3:R122))</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="T122" s="2"/>
       <c r="U122" s="3"/>
@@ -15887,7 +15887,7 @@
       </c>
       <c r="H123" s="80" t="e">
         <f t="shared" si="29"/>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="I123" s="80" t="e">
         <f>(F123-MAX($F$2:F123))/MAX($F$2:F123)</f>
@@ -15899,7 +15899,7 @@
       </c>
       <c r="K123" s="80" t="e">
         <f>STDEV($G$4:G123)*SQRT(52)</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="L123" s="82"/>
       <c r="M123" s="82"/>
@@ -15922,7 +15922,7 @@
       </c>
       <c r="S123" s="90" t="e">
         <f>AVERAGE($P$3:P123)/SQRT(AVERAGE($R$3:R123))</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="T123" s="2"/>
       <c r="U123" s="3"/>
@@ -15953,7 +15953,7 @@
       </c>
       <c r="H124" s="80" t="e">
         <f t="shared" si="29"/>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="I124" s="80" t="e">
         <f>(F124-MAX($F$2:F124))/MAX($F$2:F124)</f>
@@ -15965,7 +15965,7 @@
       </c>
       <c r="K124" s="80" t="e">
         <f>STDEV($G$4:G124)*SQRT(52)</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="L124" s="82"/>
       <c r="M124" s="82"/>
@@ -15988,7 +15988,7 @@
       </c>
       <c r="S124" s="90" t="e">
         <f>AVERAGE($P$3:P124)/SQRT(AVERAGE($R$3:R124))</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="T124" s="2"/>
       <c r="U124" s="3"/>
@@ -16019,7 +16019,7 @@
       </c>
       <c r="H125" s="80" t="e">
         <f t="shared" si="29"/>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="I125" s="80" t="e">
         <f>(F125-MAX($F$2:F125))/MAX($F$2:F125)</f>
@@ -16031,7 +16031,7 @@
       </c>
       <c r="K125" s="80" t="e">
         <f>STDEV($G$4:G125)*SQRT(52)</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="L125" s="82"/>
       <c r="M125" s="82"/>
@@ -16054,7 +16054,7 @@
       </c>
       <c r="S125" s="90" t="e">
         <f>AVERAGE($P$3:P125)/SQRT(AVERAGE($R$3:R125))</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="T125" s="2"/>
       <c r="U125" s="3"/>
@@ -16085,7 +16085,7 @@
       </c>
       <c r="H126" s="80" t="e">
         <f t="shared" si="29"/>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="I126" s="80" t="e">
         <f>(F126-MAX($F$2:F126))/MAX($F$2:F126)</f>
@@ -16097,7 +16097,7 @@
       </c>
       <c r="K126" s="80" t="e">
         <f>STDEV($G$4:G126)*SQRT(52)</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="L126" s="82"/>
       <c r="M126" s="82"/>
@@ -16120,7 +16120,7 @@
       </c>
       <c r="S126" s="90" t="e">
         <f>AVERAGE($P$3:P126)/SQRT(AVERAGE($R$3:R126))</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="T126" s="2"/>
       <c r="U126" s="3"/>
@@ -16151,7 +16151,7 @@
       </c>
       <c r="H127" s="80" t="e">
         <f t="shared" si="29"/>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="I127" s="80" t="e">
         <f>(F127-MAX($F$2:F127))/MAX($F$2:F127)</f>
@@ -16163,7 +16163,7 @@
       </c>
       <c r="K127" s="80" t="e">
         <f>STDEV($G$4:G127)*SQRT(52)</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="L127" s="82"/>
       <c r="M127" s="82"/>
@@ -16186,7 +16186,7 @@
       </c>
       <c r="S127" s="90" t="e">
         <f>AVERAGE($P$3:P127)/SQRT(AVERAGE($R$3:R127))</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="T127" s="2"/>
       <c r="U127" s="3"/>
@@ -16217,7 +16217,7 @@
       </c>
       <c r="H128" s="80" t="e">
         <f t="shared" si="29"/>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="I128" s="80" t="e">
         <f>(F128-MAX($F$2:F128))/MAX($F$2:F128)</f>
@@ -16229,7 +16229,7 @@
       </c>
       <c r="K128" s="80" t="e">
         <f>STDEV($G$4:G128)*SQRT(52)</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="L128" s="82"/>
       <c r="M128" s="82"/>
@@ -16252,7 +16252,7 @@
       </c>
       <c r="S128" s="90" t="e">
         <f>AVERAGE($P$3:P128)/SQRT(AVERAGE($R$3:R128))</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="T128" s="2"/>
       <c r="U128" s="3"/>
@@ -16281,7 +16281,7 @@
       </c>
       <c r="H129" s="80" t="e">
         <f t="shared" si="29"/>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="I129" s="80" t="e">
         <f>(F129-MAX($F$2:F129))/MAX($F$2:F129)</f>
@@ -16293,7 +16293,7 @@
       </c>
       <c r="K129" s="80" t="e">
         <f>STDEV($G$4:G129)*SQRT(52)</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="L129" s="82"/>
       <c r="M129" s="82"/>
@@ -16316,7 +16316,7 @@
       </c>
       <c r="S129" s="90" t="e">
         <f>AVERAGE($P$3:P129)/SQRT(AVERAGE($R$3:R129))</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="T129" s="2"/>
       <c r="U129" s="3"/>
@@ -16345,7 +16345,7 @@
       </c>
       <c r="H130" s="80" t="e">
         <f t="shared" si="29"/>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="I130" s="80" t="e">
         <f>(F130-MAX($F$2:F130))/MAX($F$2:F130)</f>
@@ -16357,7 +16357,7 @@
       </c>
       <c r="K130" s="80" t="e">
         <f>STDEV($G$4:G130)*SQRT(52)</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="L130" s="82"/>
       <c r="M130" s="82"/>
@@ -16380,7 +16380,7 @@
       </c>
       <c r="S130" s="90" t="e">
         <f>AVERAGE($P$3:P130)/SQRT(AVERAGE($R$3:R130))</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="T130" s="2"/>
       <c r="U130" s="3"/>
@@ -16409,7 +16409,7 @@
       </c>
       <c r="H131" s="80" t="e">
         <f t="shared" si="29"/>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="I131" s="80" t="e">
         <f>(F131-MAX($F$2:F131))/MAX($F$2:F131)</f>
@@ -16421,7 +16421,7 @@
       </c>
       <c r="K131" s="80" t="e">
         <f>STDEV($G$4:G131)*SQRT(52)</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="L131" s="82"/>
       <c r="M131" s="82"/>
@@ -16444,7 +16444,7 @@
       </c>
       <c r="S131" s="90" t="e">
         <f>AVERAGE($P$3:P131)/SQRT(AVERAGE($R$3:R131))</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="T131" s="2"/>
       <c r="U131" s="3"/>
@@ -16473,7 +16473,7 @@
       </c>
       <c r="H132" s="80" t="e">
         <f t="shared" ref="H132:H163" si="36">H131+G132</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="I132" s="80" t="e">
         <f>(F132-MAX($F$2:F132))/MAX($F$2:F132)</f>
@@ -16485,7 +16485,7 @@
       </c>
       <c r="K132" s="80" t="e">
         <f>STDEV($G$4:G132)*SQRT(52)</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="L132" s="82"/>
       <c r="M132" s="82"/>
@@ -16508,7 +16508,7 @@
       </c>
       <c r="S132" s="90" t="e">
         <f>AVERAGE($P$3:P132)/SQRT(AVERAGE($R$3:R132))</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="T132" s="2"/>
       <c r="U132" s="3"/>
@@ -16537,7 +16537,7 @@
       </c>
       <c r="H133" s="80" t="e">
         <f t="shared" si="36"/>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="I133" s="80" t="e">
         <f>(F133-MAX($F$2:F133))/MAX($F$2:F133)</f>
@@ -16549,7 +16549,7 @@
       </c>
       <c r="K133" s="80" t="e">
         <f>STDEV($G$4:G133)*SQRT(52)</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="L133" s="82"/>
       <c r="M133" s="82"/>
@@ -16572,7 +16572,7 @@
       </c>
       <c r="S133" s="90" t="e">
         <f>AVERAGE($P$3:P133)/SQRT(AVERAGE($R$3:R133))</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="T133" s="2"/>
       <c r="U133" s="3"/>
@@ -16601,7 +16601,7 @@
       </c>
       <c r="H134" s="80" t="e">
         <f t="shared" si="36"/>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="I134" s="80" t="e">
         <f>(F134-MAX($F$2:F134))/MAX($F$2:F134)</f>
@@ -16613,7 +16613,7 @@
       </c>
       <c r="K134" s="80" t="e">
         <f>STDEV($G$4:G134)*SQRT(52)</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="L134" s="82"/>
       <c r="M134" s="82"/>
@@ -16636,7 +16636,7 @@
       </c>
       <c r="S134" s="90" t="e">
         <f>AVERAGE($P$3:P134)/SQRT(AVERAGE($R$3:R134))</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="T134" s="2"/>
       <c r="U134" s="3"/>
@@ -16665,7 +16665,7 @@
       </c>
       <c r="H135" s="80" t="e">
         <f t="shared" si="36"/>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="I135" s="80" t="e">
         <f>(F135-MAX($F$2:F135))/MAX($F$2:F135)</f>
@@ -16677,7 +16677,7 @@
       </c>
       <c r="K135" s="80" t="e">
         <f>STDEV($G$4:G135)*SQRT(52)</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="L135" s="82"/>
       <c r="M135" s="82"/>
@@ -16700,7 +16700,7 @@
       </c>
       <c r="S135" s="90" t="e">
         <f>AVERAGE($P$3:P135)/SQRT(AVERAGE($R$3:R135))</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="T135" s="2"/>
       <c r="U135" s="3"/>
@@ -16729,7 +16729,7 @@
       </c>
       <c r="H136" s="80" t="e">
         <f t="shared" si="36"/>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="I136" s="80" t="e">
         <f>(F136-MAX($F$2:F136))/MAX($F$2:F136)</f>
@@ -16741,7 +16741,7 @@
       </c>
       <c r="K136" s="80" t="e">
         <f>STDEV($G$4:G136)*SQRT(52)</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="L136" s="82"/>
       <c r="M136" s="82"/>
@@ -16764,7 +16764,7 @@
       </c>
       <c r="S136" s="90" t="e">
         <f>AVERAGE($P$3:P136)/SQRT(AVERAGE($R$3:R136))</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="T136" s="2"/>
       <c r="U136" s="3"/>
@@ -16793,7 +16793,7 @@
       </c>
       <c r="H137" s="80" t="e">
         <f t="shared" si="36"/>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="I137" s="80" t="e">
         <f>(F137-MAX($F$2:F137))/MAX($F$2:F137)</f>
@@ -16805,7 +16805,7 @@
       </c>
       <c r="K137" s="80" t="e">
         <f>STDEV($G$4:G137)*SQRT(52)</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="L137" s="82"/>
       <c r="M137" s="82"/>
@@ -16828,7 +16828,7 @@
       </c>
       <c r="S137" s="90" t="e">
         <f>AVERAGE($P$3:P137)/SQRT(AVERAGE($R$3:R137))</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="T137" s="2"/>
       <c r="U137" s="3"/>
@@ -16857,7 +16857,7 @@
       </c>
       <c r="H138" s="80" t="e">
         <f t="shared" si="36"/>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="I138" s="80" t="e">
         <f>(F138-MAX($F$2:F138))/MAX($F$2:F138)</f>
@@ -16869,7 +16869,7 @@
       </c>
       <c r="K138" s="80" t="e">
         <f>STDEV($G$4:G138)*SQRT(52)</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="L138" s="82"/>
       <c r="M138" s="82"/>
@@ -16892,7 +16892,7 @@
       </c>
       <c r="S138" s="90" t="e">
         <f>AVERAGE($P$3:P138)/SQRT(AVERAGE($R$3:R138))</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="T138" s="2"/>
       <c r="U138" s="3"/>
@@ -16921,7 +16921,7 @@
       </c>
       <c r="H139" s="80" t="e">
         <f t="shared" si="36"/>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="I139" s="80" t="e">
         <f>(F139-MAX($F$2:F139))/MAX($F$2:F139)</f>
@@ -16933,7 +16933,7 @@
       </c>
       <c r="K139" s="80" t="e">
         <f>STDEV($G$4:G139)*SQRT(52)</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="L139" s="82"/>
       <c r="M139" s="82"/>
@@ -16956,7 +16956,7 @@
       </c>
       <c r="S139" s="90" t="e">
         <f>AVERAGE($P$3:P139)/SQRT(AVERAGE($R$3:R139))</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="T139" s="2"/>
       <c r="U139" s="3"/>
@@ -16985,7 +16985,7 @@
       </c>
       <c r="H140" s="80" t="e">
         <f t="shared" si="36"/>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="I140" s="80" t="e">
         <f>(F140-MAX($F$2:F140))/MAX($F$2:F140)</f>
@@ -16997,7 +16997,7 @@
       </c>
       <c r="K140" s="80" t="e">
         <f>STDEV($G$4:G140)*SQRT(52)</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="L140" s="82"/>
       <c r="M140" s="82"/>
@@ -17020,7 +17020,7 @@
       </c>
       <c r="S140" s="90" t="e">
         <f>AVERAGE($P$3:P140)/SQRT(AVERAGE($R$3:R140))</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="T140" s="2"/>
       <c r="U140" s="3"/>
@@ -17049,7 +17049,7 @@
       </c>
       <c r="H141" s="80" t="e">
         <f t="shared" si="36"/>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="I141" s="80" t="e">
         <f>(F141-MAX($F$2:F141))/MAX($F$2:F141)</f>
@@ -17061,7 +17061,7 @@
       </c>
       <c r="K141" s="80" t="e">
         <f>STDEV($G$4:G141)*SQRT(52)</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="L141" s="82"/>
       <c r="M141" s="82"/>
@@ -17084,7 +17084,7 @@
       </c>
       <c r="S141" s="90" t="e">
         <f>AVERAGE($P$3:P141)/SQRT(AVERAGE($R$3:R141))</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="T141" s="2"/>
       <c r="U141" s="3"/>
@@ -17113,7 +17113,7 @@
       </c>
       <c r="H142" s="80" t="e">
         <f t="shared" si="36"/>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="I142" s="80" t="e">
         <f>(F142-MAX($F$2:F142))/MAX($F$2:F142)</f>
@@ -17125,7 +17125,7 @@
       </c>
       <c r="K142" s="80" t="e">
         <f>STDEV($G$4:G142)*SQRT(52)</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="L142" s="82"/>
       <c r="M142" s="82"/>
@@ -17148,7 +17148,7 @@
       </c>
       <c r="S142" s="90" t="e">
         <f>AVERAGE($P$3:P142)/SQRT(AVERAGE($R$3:R142))</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="T142" s="2"/>
       <c r="U142" s="3"/>
@@ -17177,7 +17177,7 @@
       </c>
       <c r="H143" s="80" t="e">
         <f t="shared" si="36"/>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="I143" s="80" t="e">
         <f>(F143-MAX($F$2:F143))/MAX($F$2:F143)</f>
@@ -17189,7 +17189,7 @@
       </c>
       <c r="K143" s="80" t="e">
         <f>STDEV($G$4:G143)*SQRT(52)</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="L143" s="82"/>
       <c r="M143" s="82"/>
@@ -17212,7 +17212,7 @@
       </c>
       <c r="S143" s="90" t="e">
         <f>AVERAGE($P$3:P143)/SQRT(AVERAGE($R$3:R143))</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="T143" s="2"/>
       <c r="U143" s="3"/>
@@ -17241,7 +17241,7 @@
       </c>
       <c r="H144" s="80" t="e">
         <f t="shared" si="36"/>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="I144" s="80" t="e">
         <f>(F144-MAX($F$2:F144))/MAX($F$2:F144)</f>
@@ -17253,7 +17253,7 @@
       </c>
       <c r="K144" s="80" t="e">
         <f>STDEV($G$4:G144)*SQRT(52)</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="L144" s="82"/>
       <c r="M144" s="82"/>
@@ -17276,7 +17276,7 @@
       </c>
       <c r="S144" s="90" t="e">
         <f>AVERAGE($P$3:P144)/SQRT(AVERAGE($R$3:R144))</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="T144" s="2"/>
       <c r="U144" s="3"/>
@@ -17305,7 +17305,7 @@
       </c>
       <c r="H145" s="80" t="e">
         <f t="shared" si="36"/>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="I145" s="80" t="e">
         <f>(F145-MAX($F$2:F145))/MAX($F$2:F145)</f>
@@ -17317,7 +17317,7 @@
       </c>
       <c r="K145" s="80" t="e">
         <f>STDEV($G$4:G145)*SQRT(52)</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="L145" s="82"/>
       <c r="M145" s="82"/>
@@ -17340,7 +17340,7 @@
       </c>
       <c r="S145" s="90" t="e">
         <f>AVERAGE($P$3:P145)/SQRT(AVERAGE($R$3:R145))</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="T145" s="2"/>
       <c r="U145" s="3"/>
@@ -17369,7 +17369,7 @@
       </c>
       <c r="H146" s="80" t="e">
         <f t="shared" si="36"/>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="I146" s="80" t="e">
         <f>(F146-MAX($F$2:F146))/MAX($F$2:F146)</f>
@@ -17381,7 +17381,7 @@
       </c>
       <c r="K146" s="80" t="e">
         <f>STDEV($G$4:G146)*SQRT(52)</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="L146" s="82"/>
       <c r="M146" s="82"/>
@@ -17404,7 +17404,7 @@
       </c>
       <c r="S146" s="90" t="e">
         <f>AVERAGE($P$3:P146)/SQRT(AVERAGE($R$3:R146))</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="T146" s="2"/>
       <c r="U146" s="3"/>
@@ -17433,7 +17433,7 @@
       </c>
       <c r="H147" s="80" t="e">
         <f t="shared" si="36"/>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="I147" s="80" t="e">
         <f>(F147-MAX($F$2:F147))/MAX($F$2:F147)</f>
@@ -17445,7 +17445,7 @@
       </c>
       <c r="K147" s="80" t="e">
         <f>STDEV($G$4:G147)*SQRT(52)</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="L147" s="82"/>
       <c r="M147" s="82"/>
@@ -17468,7 +17468,7 @@
       </c>
       <c r="S147" s="90" t="e">
         <f>AVERAGE($P$3:P147)/SQRT(AVERAGE($R$3:R147))</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="T147" s="2"/>
       <c r="U147" s="3"/>
@@ -17497,7 +17497,7 @@
       </c>
       <c r="H148" s="80" t="e">
         <f t="shared" si="36"/>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="I148" s="80" t="e">
         <f>(F148-MAX($F$2:F148))/MAX($F$2:F148)</f>
@@ -17509,7 +17509,7 @@
       </c>
       <c r="K148" s="80" t="e">
         <f>STDEV($G$4:G148)*SQRT(52)</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="L148" s="82"/>
       <c r="M148" s="82"/>
@@ -17532,7 +17532,7 @@
       </c>
       <c r="S148" s="90" t="e">
         <f>AVERAGE($P$3:P148)/SQRT(AVERAGE($R$3:R148))</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="T148" s="2"/>
       <c r="U148" s="3"/>
@@ -17561,7 +17561,7 @@
       </c>
       <c r="H149" s="80" t="e">
         <f t="shared" si="36"/>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="I149" s="80" t="e">
         <f>(F149-MAX($F$2:F149))/MAX($F$2:F149)</f>
@@ -17573,7 +17573,7 @@
       </c>
       <c r="K149" s="80" t="e">
         <f>STDEV($G$4:G149)*SQRT(52)</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="L149" s="82"/>
       <c r="M149" s="82"/>
@@ -17596,7 +17596,7 @@
       </c>
       <c r="S149" s="90" t="e">
         <f>AVERAGE($P$3:P149)/SQRT(AVERAGE($R$3:R149))</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="T149" s="2"/>
       <c r="U149" s="3"/>
@@ -17625,7 +17625,7 @@
       </c>
       <c r="H150" s="80" t="e">
         <f t="shared" si="36"/>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="I150" s="80" t="e">
         <f>(F150-MAX($F$2:F150))/MAX($F$2:F150)</f>
@@ -17637,7 +17637,7 @@
       </c>
       <c r="K150" s="80" t="e">
         <f>STDEV($G$4:G150)*SQRT(52)</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="L150" s="82"/>
       <c r="M150" s="82"/>
@@ -17660,7 +17660,7 @@
       </c>
       <c r="S150" s="90" t="e">
         <f>AVERAGE($P$3:P150)/SQRT(AVERAGE($R$3:R150))</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="T150" s="2"/>
       <c r="U150" s="3"/>
@@ -17689,7 +17689,7 @@
       </c>
       <c r="H151" s="80" t="e">
         <f t="shared" si="36"/>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="I151" s="80" t="e">
         <f>(F151-MAX($F$2:F151))/MAX($F$2:F151)</f>
@@ -17701,7 +17701,7 @@
       </c>
       <c r="K151" s="80" t="e">
         <f>STDEV($G$4:G151)*SQRT(52)</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="L151" s="82"/>
       <c r="M151" s="82"/>
@@ -17724,7 +17724,7 @@
       </c>
       <c r="S151" s="90" t="e">
         <f>AVERAGE($P$3:P151)/SQRT(AVERAGE($R$3:R151))</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="T151" s="2"/>
       <c r="U151" s="3"/>
@@ -17753,7 +17753,7 @@
       </c>
       <c r="H152" s="80" t="e">
         <f t="shared" si="36"/>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="I152" s="80" t="e">
         <f>(F152-MAX($F$2:F152))/MAX($F$2:F152)</f>
@@ -17765,7 +17765,7 @@
       </c>
       <c r="K152" s="80" t="e">
         <f>STDEV($G$4:G152)*SQRT(52)</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="L152" s="82"/>
       <c r="M152" s="82"/>
@@ -17788,7 +17788,7 @@
       </c>
       <c r="S152" s="90" t="e">
         <f>AVERAGE($P$3:P152)/SQRT(AVERAGE($R$3:R152))</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="T152" s="2"/>
       <c r="U152" s="3"/>
@@ -17817,7 +17817,7 @@
       </c>
       <c r="H153" s="80" t="e">
         <f t="shared" si="36"/>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="I153" s="80" t="e">
         <f>(F153-MAX($F$2:F153))/MAX($F$2:F153)</f>
@@ -17829,7 +17829,7 @@
       </c>
       <c r="K153" s="80" t="e">
         <f>STDEV($G$4:G153)*SQRT(52)</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="L153" s="82"/>
       <c r="M153" s="82"/>
@@ -17852,7 +17852,7 @@
       </c>
       <c r="S153" s="90" t="e">
         <f>AVERAGE($P$3:P153)/SQRT(AVERAGE($R$3:R153))</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="T153" s="2"/>
       <c r="U153" s="3"/>
@@ -17881,7 +17881,7 @@
       </c>
       <c r="H154" s="80" t="e">
         <f t="shared" si="36"/>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="I154" s="80" t="e">
         <f>(F154-MAX($F$2:F154))/MAX($F$2:F154)</f>
@@ -17893,7 +17893,7 @@
       </c>
       <c r="K154" s="80" t="e">
         <f>STDEV($G$4:G154)*SQRT(52)</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="L154" s="82"/>
       <c r="M154" s="82"/>
@@ -17916,7 +17916,7 @@
       </c>
       <c r="S154" s="90" t="e">
         <f>AVERAGE($P$3:P154)/SQRT(AVERAGE($R$3:R154))</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="T154" s="2"/>
       <c r="U154" s="3"/>
@@ -17945,7 +17945,7 @@
       </c>
       <c r="H155" s="80" t="e">
         <f t="shared" si="36"/>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="I155" s="80" t="e">
         <f>(F155-MAX($F$2:F155))/MAX($F$2:F155)</f>
@@ -17957,7 +17957,7 @@
       </c>
       <c r="K155" s="80" t="e">
         <f>STDEV($G$4:G155)*SQRT(52)</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="L155" s="82"/>
       <c r="M155" s="82"/>
@@ -17980,7 +17980,7 @@
       </c>
       <c r="S155" s="90" t="e">
         <f>AVERAGE($P$3:P155)/SQRT(AVERAGE($R$3:R155))</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="T155" s="2"/>
       <c r="U155" s="3"/>
@@ -18009,7 +18009,7 @@
       </c>
       <c r="H156" s="80" t="e">
         <f t="shared" si="36"/>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="I156" s="80" t="e">
         <f>(F156-MAX($F$2:F156))/MAX($F$2:F156)</f>
@@ -18021,7 +18021,7 @@
       </c>
       <c r="K156" s="80" t="e">
         <f>STDEV($G$4:G156)*SQRT(52)</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="L156" s="82"/>
       <c r="M156" s="82"/>
@@ -18044,7 +18044,7 @@
       </c>
       <c r="S156" s="90" t="e">
         <f>AVERAGE($P$3:P156)/SQRT(AVERAGE($R$3:R156))</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="T156" s="2"/>
       <c r="U156" s="3"/>
@@ -18073,7 +18073,7 @@
       </c>
       <c r="H157" s="80" t="e">
         <f t="shared" si="36"/>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="I157" s="80" t="e">
         <f>(F157-MAX($F$2:F157))/MAX($F$2:F157)</f>
@@ -18085,7 +18085,7 @@
       </c>
       <c r="K157" s="80" t="e">
         <f>STDEV($G$4:G157)*SQRT(52)</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="L157" s="82"/>
       <c r="M157" s="82"/>
@@ -18108,7 +18108,7 @@
       </c>
       <c r="S157" s="90" t="e">
         <f>AVERAGE($P$3:P157)/SQRT(AVERAGE($R$3:R157))</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="T157" s="2"/>
       <c r="U157" s="3"/>
@@ -18137,7 +18137,7 @@
       </c>
       <c r="H158" s="80" t="e">
         <f t="shared" si="36"/>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="I158" s="80" t="e">
         <f>(F158-MAX($F$2:F158))/MAX($F$2:F158)</f>
@@ -18149,7 +18149,7 @@
       </c>
       <c r="K158" s="80" t="e">
         <f>STDEV($G$4:G158)*SQRT(52)</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="L158" s="82"/>
       <c r="M158" s="82"/>
@@ -18172,7 +18172,7 @@
       </c>
       <c r="S158" s="90" t="e">
         <f>AVERAGE($P$3:P158)/SQRT(AVERAGE($R$3:R158))</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="T158" s="2"/>
       <c r="U158" s="3"/>
@@ -18201,7 +18201,7 @@
       </c>
       <c r="H159" s="80" t="e">
         <f t="shared" si="36"/>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="I159" s="80" t="e">
         <f>(F159-MAX($F$2:F159))/MAX($F$2:F159)</f>
@@ -18213,7 +18213,7 @@
       </c>
       <c r="K159" s="80" t="e">
         <f>STDEV($G$4:G159)*SQRT(52)</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="L159" s="82"/>
       <c r="M159" s="82"/>
@@ -18236,7 +18236,7 @@
       </c>
       <c r="S159" s="90" t="e">
         <f>AVERAGE($P$3:P159)/SQRT(AVERAGE($R$3:R159))</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="T159" s="2"/>
       <c r="U159" s="3"/>
@@ -18265,7 +18265,7 @@
       </c>
       <c r="H160" s="80" t="e">
         <f t="shared" si="36"/>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="I160" s="80" t="e">
         <f>(F160-MAX($F$2:F160))/MAX($F$2:F160)</f>
@@ -18277,7 +18277,7 @@
       </c>
       <c r="K160" s="80" t="e">
         <f>STDEV($G$4:G160)*SQRT(52)</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="L160" s="82"/>
       <c r="M160" s="82"/>
@@ -18300,7 +18300,7 @@
       </c>
       <c r="S160" s="90" t="e">
         <f>AVERAGE($P$3:P160)/SQRT(AVERAGE($R$3:R160))</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="T160" s="2"/>
       <c r="U160" s="3"/>
@@ -18329,7 +18329,7 @@
       </c>
       <c r="H161" s="80" t="e">
         <f t="shared" si="36"/>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="I161" s="80" t="e">
         <f>(F161-MAX($F$2:F161))/MAX($F$2:F161)</f>
@@ -18341,7 +18341,7 @@
       </c>
       <c r="K161" s="80" t="e">
         <f>STDEV($G$4:G161)*SQRT(52)</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="L161" s="82"/>
       <c r="M161" s="82"/>
@@ -18364,7 +18364,7 @@
       </c>
       <c r="S161" s="90" t="e">
         <f>AVERAGE($P$3:P161)/SQRT(AVERAGE($R$3:R161))</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="T161" s="2"/>
       <c r="U161" s="3"/>
@@ -18393,7 +18393,7 @@
       </c>
       <c r="H162" s="80" t="e">
         <f t="shared" si="36"/>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="I162" s="80" t="e">
         <f>(F162-MAX($F$2:F162))/MAX($F$2:F162)</f>
@@ -18405,7 +18405,7 @@
       </c>
       <c r="K162" s="80" t="e">
         <f>STDEV($G$4:G162)*SQRT(52)</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="L162" s="82"/>
       <c r="M162" s="82"/>
@@ -18428,7 +18428,7 @@
       </c>
       <c r="S162" s="90" t="e">
         <f>AVERAGE($P$3:P162)/SQRT(AVERAGE($R$3:R162))</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="T162" s="2"/>
       <c r="U162" s="3"/>
@@ -18457,7 +18457,7 @@
       </c>
       <c r="H163" s="80" t="e">
         <f t="shared" si="36"/>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="I163" s="80" t="e">
         <f>(F163-MAX($F$2:F163))/MAX($F$2:F163)</f>
@@ -18469,7 +18469,7 @@
       </c>
       <c r="K163" s="80" t="e">
         <f>STDEV($G$4:G163)*SQRT(52)</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="L163" s="82"/>
       <c r="M163" s="82"/>
@@ -18492,7 +18492,7 @@
       </c>
       <c r="S163" s="90" t="e">
         <f>AVERAGE($P$3:P163)/SQRT(AVERAGE($R$3:R163))</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="T163" s="2"/>
       <c r="U163" s="3"/>
@@ -18521,7 +18521,7 @@
       </c>
       <c r="H164" s="80" t="e">
         <f t="shared" ref="H164:H171" si="43">H163+G164</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="I164" s="80" t="e">
         <f>(F164-MAX($F$2:F164))/MAX($F$2:F164)</f>
@@ -18533,7 +18533,7 @@
       </c>
       <c r="K164" s="80" t="e">
         <f>STDEV($G$4:G164)*SQRT(52)</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="L164" s="82"/>
       <c r="M164" s="82"/>
@@ -18556,7 +18556,7 @@
       </c>
       <c r="S164" s="90" t="e">
         <f>AVERAGE($P$3:P164)/SQRT(AVERAGE($R$3:R164))</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="T164" s="2"/>
       <c r="U164" s="3"/>
@@ -18585,7 +18585,7 @@
       </c>
       <c r="H165" s="80" t="e">
         <f t="shared" si="43"/>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="I165" s="80" t="e">
         <f>(F165-MAX($F$2:F165))/MAX($F$2:F165)</f>
@@ -18597,7 +18597,7 @@
       </c>
       <c r="K165" s="80" t="e">
         <f>STDEV($G$4:G165)*SQRT(52)</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="L165" s="82"/>
       <c r="M165" s="82"/>
@@ -18620,7 +18620,7 @@
       </c>
       <c r="S165" s="90" t="e">
         <f>AVERAGE($P$3:P165)/SQRT(AVERAGE($R$3:R165))</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="T165" s="2"/>
       <c r="U165" s="3"/>
@@ -18649,7 +18649,7 @@
       </c>
       <c r="H166" s="80" t="e">
         <f t="shared" si="43"/>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="I166" s="80" t="e">
         <f>(F166-MAX($F$2:F166))/MAX($F$2:F166)</f>
@@ -18661,7 +18661,7 @@
       </c>
       <c r="K166" s="80" t="e">
         <f>STDEV($G$4:G166)*SQRT(52)</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="L166" s="82"/>
       <c r="M166" s="82"/>
@@ -18684,7 +18684,7 @@
       </c>
       <c r="S166" s="90" t="e">
         <f>AVERAGE($P$3:P166)/SQRT(AVERAGE($R$3:R166))</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="T166" s="2"/>
       <c r="U166" s="3"/>
@@ -18713,7 +18713,7 @@
       </c>
       <c r="H167" s="80" t="e">
         <f t="shared" si="43"/>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="I167" s="80" t="e">
         <f>(F167-MAX($F$2:F167))/MAX($F$2:F167)</f>
@@ -18725,7 +18725,7 @@
       </c>
       <c r="K167" s="80" t="e">
         <f>STDEV($G$4:G167)*SQRT(52)</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="L167" s="82"/>
       <c r="M167" s="82"/>
@@ -18748,7 +18748,7 @@
       </c>
       <c r="S167" s="90" t="e">
         <f>AVERAGE($P$3:P167)/SQRT(AVERAGE($R$3:R167))</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="T167" s="2"/>
       <c r="U167" s="3"/>
@@ -18777,7 +18777,7 @@
       </c>
       <c r="H168" s="80" t="e">
         <f t="shared" si="43"/>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="I168" s="80" t="e">
         <f>(F168-MAX($F$2:F168))/MAX($F$2:F168)</f>
@@ -18789,7 +18789,7 @@
       </c>
       <c r="K168" s="80" t="e">
         <f>STDEV($G$4:G168)*SQRT(52)</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="L168" s="82"/>
       <c r="M168" s="82"/>
@@ -18812,7 +18812,7 @@
       </c>
       <c r="S168" s="90" t="e">
         <f>AVERAGE($P$3:P168)/SQRT(AVERAGE($R$3:R168))</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="T168" s="2"/>
       <c r="U168" s="3"/>
@@ -18841,7 +18841,7 @@
       </c>
       <c r="H169" s="80" t="e">
         <f t="shared" si="43"/>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="I169" s="80" t="e">
         <f>(F169-MAX($F$2:F169))/MAX($F$2:F169)</f>
@@ -18853,7 +18853,7 @@
       </c>
       <c r="K169" s="80" t="e">
         <f>STDEV($G$4:G169)*SQRT(52)</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="L169" s="82"/>
       <c r="M169" s="82"/>
@@ -18876,7 +18876,7 @@
       </c>
       <c r="S169" s="90" t="e">
         <f>AVERAGE($P$3:P169)/SQRT(AVERAGE($R$3:R169))</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="T169" s="2"/>
       <c r="U169" s="3"/>
@@ -18905,7 +18905,7 @@
       </c>
       <c r="H170" s="80" t="e">
         <f t="shared" si="43"/>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="I170" s="80" t="e">
         <f>(F170-MAX($F$2:F170))/MAX($F$2:F170)</f>
@@ -18917,7 +18917,7 @@
       </c>
       <c r="K170" s="80" t="e">
         <f>STDEV($G$4:G170)*SQRT(52)</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="L170" s="82"/>
       <c r="M170" s="82"/>
@@ -18940,7 +18940,7 @@
       </c>
       <c r="S170" s="90" t="e">
         <f>AVERAGE($P$3:P170)/SQRT(AVERAGE($R$3:R170))</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="T170" s="2"/>
       <c r="U170" s="3"/>
@@ -18969,7 +18969,7 @@
       </c>
       <c r="H171" s="80" t="e">
         <f t="shared" si="43"/>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="I171" s="80" t="e">
         <f>(F171-MAX($F$2:F171))/MAX($F$2:F171)</f>
@@ -18981,7 +18981,7 @@
       </c>
       <c r="K171" s="80" t="e">
         <f>STDEV($G$4:G171)*SQRT(52)</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="L171" s="82"/>
       <c r="M171" s="82"/>
@@ -19004,7 +19004,7 @@
       </c>
       <c r="S171" s="90" t="e">
         <f>AVERAGE($P$3:P171)/SQRT(AVERAGE($R$3:R171))</f>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="T171" s="2"/>
       <c r="U171" s="3"/>
@@ -69976,15 +69976,15 @@
       </c>
       <c r="I3" s="149" cm="1">
         <f t="array" aca="1" ref="I3" ca="1">_FV(B3,"Price")</f>
-        <v>61.54</v>
+        <v>64.59</v>
       </c>
       <c r="J3" s="129">
         <f t="shared" ref="J3:J27" ca="1" si="0">((I3-F3)/F3)</f>
-        <v>-0.10487272727272728</v>
+        <v>-6.050909090909086E-2</v>
       </c>
       <c r="K3" s="170">
         <f t="shared" ref="K3:K27" ca="1" si="1">(I3*G3) - H3</f>
-        <v>-52.570327999999961</v>
+        <v>-30.345587999999964</v>
       </c>
       <c r="L3"/>
     </row>
@@ -70015,15 +70015,15 @@
       </c>
       <c r="I4" s="149" cm="1">
         <f t="array" aca="1" ref="I4" ca="1">_FV(B4,"Price")</f>
-        <v>141.63</v>
+        <v>141.93</v>
       </c>
       <c r="J4" s="129">
         <f t="shared" ca="1" si="0"/>
-        <v>0.41601679664067187</v>
+        <v>0.419016196760648</v>
       </c>
       <c r="K4" s="170">
         <f t="shared" ca="1" si="1"/>
-        <v>208.42466999999999</v>
+        <v>209.92737000000011</v>
       </c>
       <c r="L4"/>
     </row>
@@ -70054,15 +70054,15 @@
       </c>
       <c r="I5" s="149" cm="1">
         <f t="array" aca="1" ref="I5" ca="1">_FV(B5,"Price")</f>
-        <v>18.72</v>
+        <v>18.13</v>
       </c>
       <c r="J5" s="129">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.14128440366972486</v>
+        <v>-0.16834862385321109</v>
       </c>
       <c r="K5" s="170">
         <f t="shared" ca="1" si="1"/>
-        <v>-70.829376000000025</v>
+        <v>-84.387104000000022</v>
       </c>
       <c r="L5"/>
     </row>
@@ -70093,15 +70093,15 @@
       </c>
       <c r="I6" s="149" cm="1">
         <f t="array" aca="1" ref="I6" ca="1">_FV(B6,"Price")</f>
-        <v>21.61</v>
+        <v>21.58</v>
       </c>
       <c r="J6" s="129">
         <f t="shared" ca="1" si="0"/>
-        <v>0.23485714285714282</v>
+        <v>0.23314285714285704</v>
       </c>
       <c r="K6" s="170">
         <f t="shared" ca="1" si="1"/>
-        <v>131.23080399999992</v>
+        <v>130.3531119999999</v>
       </c>
       <c r="L6"/>
     </row>
@@ -70132,15 +70132,15 @@
       </c>
       <c r="I7" s="151" cm="1">
         <f t="array" aca="1" ref="I7" ca="1">_FV(B7,"Price")</f>
-        <v>226.21</v>
+        <v>226.8</v>
       </c>
       <c r="J7" s="129">
         <f t="shared" ca="1" si="0"/>
-        <v>0.28193358268162755</v>
+        <v>0.28527711662699762</v>
       </c>
       <c r="K7" s="170">
         <f t="shared" ca="1" si="1"/>
-        <v>141.25281100000007</v>
+        <v>142.92788000000007</v>
       </c>
       <c r="L7"/>
     </row>
@@ -70171,15 +70171,15 @@
       </c>
       <c r="I8" s="151" cm="1">
         <f t="array" aca="1" ref="I8" ca="1">_FV(B8,"Price")</f>
-        <v>97.46</v>
+        <v>99.05</v>
       </c>
       <c r="J8" s="129">
         <f t="shared" ca="1" si="0"/>
-        <v>0.73601710010687549</v>
+        <v>0.76433915211970072</v>
       </c>
       <c r="K8" s="170">
         <f t="shared" ca="1" si="1"/>
-        <v>368.67456400000003</v>
+        <v>382.86277000000007</v>
       </c>
       <c r="L8"/>
     </row>
@@ -70210,15 +70210,15 @@
       </c>
       <c r="I9" s="151" cm="1">
         <f t="array" aca="1" ref="I9" ca="1">_FV(B9,"Price")</f>
-        <v>17.53</v>
+        <v>18.97</v>
       </c>
       <c r="J9" s="129">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.47796307325789156</v>
+        <v>-0.43508040500297795</v>
       </c>
       <c r="K9" s="170">
         <f t="shared" ca="1" si="1"/>
-        <v>-239.436623</v>
+        <v>-217.95052700000002</v>
       </c>
       <c r="L9"/>
     </row>
@@ -70249,15 +70249,15 @@
       </c>
       <c r="I10" s="153" cm="1">
         <f t="array" aca="1" ref="I10" ca="1">_FV(B10,"Price")</f>
-        <v>62.7</v>
+        <v>65.72</v>
       </c>
       <c r="J10" s="129">
         <f t="shared" ca="1" si="0"/>
-        <v>7.7319587628865982E-2</v>
+        <v>0.12920962199312708</v>
       </c>
       <c r="K10" s="170">
         <f t="shared" ca="1" si="1"/>
-        <v>38.759219999999914</v>
+        <v>64.757191999999918</v>
       </c>
       <c r="L10"/>
     </row>
@@ -70288,15 +70288,15 @@
       </c>
       <c r="I11" s="153" cm="1">
         <f t="array" aca="1" ref="I11" ca="1">_FV(B11,"Price")</f>
-        <v>82.77</v>
+        <v>82.25</v>
       </c>
       <c r="J11" s="129">
         <f t="shared" ca="1" si="0"/>
-        <v>-9.313027281691684E-2</v>
+        <v>-9.8827654212775243E-2</v>
       </c>
       <c r="K11" s="170">
         <f t="shared" ca="1" si="1"/>
-        <v>-46.675470000000018</v>
+        <v>-49.529750000000035</v>
       </c>
       <c r="L11"/>
     </row>
@@ -70327,15 +70327,15 @@
       </c>
       <c r="I12" s="153" cm="1">
         <f t="array" aca="1" ref="I12" ca="1">_FV(B12,"Price")</f>
-        <v>102.99</v>
+        <v>104.57</v>
       </c>
       <c r="J12" s="129">
         <f t="shared" ca="1" si="0"/>
-        <v>0.23046594982078844</v>
+        <v>0.24934289127837503</v>
       </c>
       <c r="K12" s="170">
         <f t="shared" ca="1" si="1"/>
-        <v>115.44664499999999</v>
+        <v>124.90373499999998</v>
       </c>
       <c r="L12"/>
     </row>
@@ -70366,15 +70366,15 @@
       </c>
       <c r="I13" s="153" cm="1">
         <f t="array" aca="1" ref="I13" ca="1">_FV(B13,"Price")</f>
-        <v>98.5</v>
+        <v>97.45</v>
       </c>
       <c r="J13" s="129">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.15790373600068391</v>
+        <v>-0.1668803966829101</v>
       </c>
       <c r="K13" s="170">
         <f t="shared" ca="1" si="1"/>
-        <v>-79.114649999999983</v>
+        <v>-83.611904999999979</v>
       </c>
       <c r="L13"/>
     </row>
@@ -70405,15 +70405,15 @@
       </c>
       <c r="I14" s="155" cm="1">
         <f t="array" aca="1" ref="I14" ca="1">_FV(B14,"Price")</f>
-        <v>26.53</v>
+        <v>26.23</v>
       </c>
       <c r="J14" s="129">
         <f t="shared" ca="1" si="0"/>
-        <v>4.0800313848568172E-2</v>
+        <v>2.9030992546096587E-2</v>
       </c>
       <c r="K14" s="170">
         <f t="shared" ca="1" si="1"/>
-        <v>20.473679999999945</v>
+        <v>14.57687999999996</v>
       </c>
       <c r="L14"/>
     </row>
@@ -70444,15 +70444,15 @@
       </c>
       <c r="I15" s="155" cm="1">
         <f t="array" aca="1" ref="I15" ca="1">_FV(B15,"Price")</f>
-        <v>13.14</v>
+        <v>13.15</v>
       </c>
       <c r="J15" s="129">
         <f t="shared" ca="1" si="0"/>
-        <v>0.49828962371721791</v>
+        <v>0.49942987457240606</v>
       </c>
       <c r="K15" s="170">
         <f t="shared" ca="1" si="1"/>
-        <v>249.42671400000006</v>
+        <v>249.99781500000006</v>
       </c>
       <c r="L15"/>
     </row>
@@ -70483,15 +70483,15 @@
       </c>
       <c r="I16" s="157" cm="1">
         <f t="array" aca="1" ref="I16" ca="1">_FV(B16,"Price")</f>
-        <v>38.03</v>
+        <v>36.590000000000003</v>
       </c>
       <c r="J16" s="129">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.21619950535861504</v>
+        <v>-0.24587798845836767</v>
       </c>
       <c r="K16" s="170">
         <f t="shared" ca="1" si="1"/>
-        <v>-104.84999999999997</v>
+        <v>-119.24999999999994</v>
       </c>
       <c r="L16"/>
     </row>
@@ -70522,15 +70522,15 @@
       </c>
       <c r="I17" s="157" cm="1">
         <f t="array" aca="1" ref="I17" ca="1">_FV(B17,"Price")</f>
-        <v>77.48</v>
+        <v>77.959999999999994</v>
       </c>
       <c r="J17" s="129">
         <f t="shared" ca="1" si="0"/>
-        <v>0.10764832022873483</v>
+        <v>0.11451036454610422</v>
       </c>
       <c r="K17" s="170">
         <f t="shared" ca="1" si="1"/>
-        <v>52.720000000000027</v>
+        <v>56.079999999999927</v>
       </c>
       <c r="L17"/>
     </row>
@@ -70561,15 +70561,15 @@
       </c>
       <c r="I18" s="157" cm="1">
         <f t="array" aca="1" ref="I18" ca="1">_FV(B18,"Price")</f>
-        <v>59.86</v>
+        <v>61.99</v>
       </c>
       <c r="J18" s="129">
         <f t="shared" ca="1" si="0"/>
-        <v>-3.7311032486330012E-2</v>
+        <v>-3.05564490189768E-3</v>
       </c>
       <c r="K18" s="170">
         <f t="shared" ca="1" si="1"/>
-        <v>-18.560000000000002</v>
+        <v>-1.5199999999999818</v>
       </c>
       <c r="L18"/>
     </row>
@@ -70600,15 +70600,15 @@
       </c>
       <c r="I19" s="157" cm="1">
         <f t="array" aca="1" ref="I19" ca="1">_FV(B19,"Price")</f>
-        <v>9.67</v>
+        <v>9.7899999999999991</v>
       </c>
       <c r="J19" s="129">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.2783582089552239</v>
+        <v>-0.26940298507462695</v>
       </c>
       <c r="K19" s="170">
         <f t="shared" ca="1" si="1"/>
-        <v>-139.50638999999995</v>
+        <v>-135.02043000000003</v>
       </c>
       <c r="L19"/>
     </row>
@@ -70639,15 +70639,15 @@
       </c>
       <c r="I20" s="209" cm="1">
         <f t="array" aca="1" ref="I20" ca="1">_FV(B20,"Price")</f>
-        <v>379.13</v>
+        <v>381.8</v>
       </c>
       <c r="J20" s="129">
         <f t="shared" ca="1" si="0"/>
-        <v>-3.6273512963904381E-2</v>
+        <v>-2.9486527707168191E-2</v>
       </c>
       <c r="K20" s="170">
         <f t="shared" ca="1" si="1"/>
-        <v>-18.273599999999988</v>
+        <v>-14.855999999999995</v>
       </c>
       <c r="L20"/>
     </row>
@@ -70678,15 +70678,15 @@
       </c>
       <c r="I21" s="212" cm="1">
         <f t="array" aca="1" ref="I21" ca="1">_FV(B21,"Price")</f>
-        <v>20.98</v>
+        <v>20.78</v>
       </c>
       <c r="J21" s="129">
         <f t="shared" ca="1" si="0"/>
-        <v>-5.7502246181491509E-2</v>
+        <v>-6.6486972147349527E-2</v>
       </c>
       <c r="K21" s="170">
         <f t="shared" ca="1" si="1"/>
-        <v>-28.813629999999989</v>
+        <v>-33.314930000000004</v>
       </c>
     </row>
     <row r="22" spans="2:12">
@@ -70716,15 +70716,15 @@
       </c>
       <c r="I22" s="212" cm="1">
         <f t="array" aca="1" ref="I22" ca="1">_FV(B22,"Price")</f>
-        <v>69.260000000000005</v>
+        <v>66.680000000000007</v>
       </c>
       <c r="J22" s="129">
         <f t="shared" ca="1" si="0"/>
-        <v>-5.456634118322738E-3</v>
+        <v>-4.2504307869040692E-2</v>
       </c>
       <c r="K22" s="170">
         <f t="shared" ca="1" si="1"/>
-        <v>-1.2998779999999783</v>
+        <v>-19.913803999999971</v>
       </c>
     </row>
     <row r="23" spans="2:12">
@@ -70754,15 +70754,15 @@
       </c>
       <c r="I23" s="212" cm="1">
         <f t="array" aca="1" ref="I23" ca="1">_FV(B23,"Price")</f>
-        <v>101.76</v>
+        <v>100.28</v>
       </c>
       <c r="J23" s="129">
         <f t="shared" ca="1" si="0"/>
-        <v>6.2296054583210686E-3</v>
+        <v>-8.4050232374171304E-3</v>
       </c>
       <c r="K23" s="170">
         <f t="shared" ca="1" si="1"/>
-        <v>3.1392160000000331</v>
+        <v>-4.1928519999999594</v>
       </c>
     </row>
     <row r="24" spans="2:12">
@@ -70792,15 +70792,15 @@
       </c>
       <c r="I24" s="212" cm="1">
         <f t="array" aca="1" ref="I24" ca="1">_FV(B24,"Price")</f>
-        <v>113.16</v>
+        <v>120.42</v>
       </c>
       <c r="J24" s="129">
         <f t="shared" ca="1" si="0"/>
-        <v>-4.2477576578101285E-2</v>
+        <v>1.8954137755965432E-2</v>
       </c>
       <c r="K24" s="170">
         <f t="shared" ca="1" si="1"/>
-        <v>-21.269496000000061</v>
+        <v>9.508547999999962</v>
       </c>
     </row>
     <row r="25" spans="2:12">
@@ -70830,15 +70830,15 @@
       </c>
       <c r="I25" s="221" cm="1">
         <f t="array" aca="1" ref="I25" ca="1">_FV(B25,"Price")</f>
-        <v>28.67</v>
+        <v>28.58</v>
       </c>
       <c r="J25" s="129">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.8822724161533098E-2</v>
+        <v>-2.1902806297056831E-2</v>
       </c>
       <c r="K25" s="170">
         <f t="shared" ca="1" si="1"/>
-        <v>-9.4872540000000072</v>
+        <v>-11.030196000000046</v>
       </c>
     </row>
     <row r="26" spans="2:12">
@@ -70868,15 +70868,15 @@
       </c>
       <c r="I26" s="221" cm="1">
         <f t="array" aca="1" ref="I26" ca="1">_FV(B26,"Price")</f>
-        <v>19.71</v>
+        <v>19.899999999999999</v>
       </c>
       <c r="J26" s="129">
         <f t="shared" ca="1" si="0"/>
-        <v>-5.6937799043062093E-2</v>
+        <v>-4.784688995215311E-2</v>
       </c>
       <c r="K26" s="170">
         <f t="shared" ca="1" si="1"/>
-        <v>-28.506669999999986</v>
+        <v>-23.942300000000046</v>
       </c>
     </row>
     <row r="27" spans="2:12">
@@ -70906,21 +70906,21 @@
       </c>
       <c r="I27" s="221" cm="1">
         <f t="array" aca="1" ref="I27" ca="1">_FV(B27,"Price")</f>
-        <v>24.52</v>
+        <v>24.16</v>
       </c>
       <c r="J27" s="129">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.6840417000801994E-2</v>
+        <v>-3.1275060144346473E-2</v>
       </c>
       <c r="K27" s="170">
         <f t="shared" ca="1" si="1"/>
-        <v>-8.5329640000000495</v>
+        <v>-15.763312000000042</v>
       </c>
     </row>
     <row r="30" spans="2:12" ht="13">
       <c r="K30" s="169">
         <f ca="1">SUM(K3:K27)</f>
-        <v>461.8219949999999</v>
+        <v>541.26660400000014</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
vault backup: 2024-10-05 14:32:48
</commit_message>
<xml_diff>
--- a/_system/Attachments/Portfolio Management.xlsx
+++ b/_system/Attachments/Portfolio Management.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martin/repos/tomesink/obsidian/_system/Attachments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E11B357A-7188-7244-93B4-7A5D52B5DC9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59C6AB06-1E82-7640-BED3-A505E5F38AC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3860" yWindow="1520" windowWidth="34980" windowHeight="19340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3860" yWindow="1520" windowWidth="34980" windowHeight="19340" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Stocks Performance" sheetId="1" r:id="rId1"/>
@@ -7610,7 +7610,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X1011"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A97" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A97" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="D121" sqref="D121"/>
     </sheetView>
   </sheetViews>
@@ -40924,8 +40924,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:X1011"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A16" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A25" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -43505,35 +43505,37 @@
       <c r="B40" s="69">
         <v>39</v>
       </c>
-      <c r="C40" s="70"/>
+      <c r="C40" s="70">
+        <v>38710</v>
+      </c>
       <c r="D40" s="87"/>
       <c r="E40" s="70">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>38710</v>
       </c>
       <c r="F40" s="81">
         <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="G40" s="80" t="e">
+        <v>142.8175095857905</v>
+      </c>
+      <c r="G40" s="80">
         <f t="shared" si="10"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="H40" s="80" t="e">
+        <v>3.202373384173611E-2</v>
+      </c>
+      <c r="H40" s="80">
         <f t="shared" si="14"/>
-        <v>#NUM!</v>
+        <v>0.3563974725476402</v>
       </c>
       <c r="I40" s="80">
         <f>(F40-MAX($F$2:F40))/MAX($F$2:F40)</f>
-        <v>-1</v>
+        <v>-5.0128174338024301E-2</v>
       </c>
       <c r="J40" s="80">
         <f>(F40-MIN($F$2:F40))/MAX($F$2:F40)</f>
-        <v>0</v>
-      </c>
-      <c r="K40" s="80" t="e">
+        <v>0.30691842764929761</v>
+      </c>
+      <c r="K40" s="80">
         <f>STDEV($G$3:G40)*SQRT(52)</f>
-        <v>#NUM!</v>
+        <v>0.43274081379963042</v>
       </c>
       <c r="L40" s="82"/>
       <c r="M40" s="82"/>
@@ -43542,21 +43544,21 @@
         <f t="shared" si="3"/>
         <v>5.7692307692307687E-4</v>
       </c>
-      <c r="P40" s="88" t="e">
+      <c r="P40" s="88">
         <f t="shared" si="11"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="Q40" s="88" t="e">
+        <v>3.1446810764813031E-2</v>
+      </c>
+      <c r="Q40" s="88">
         <f t="shared" si="12"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="R40" s="89" t="e">
+        <v>0</v>
+      </c>
+      <c r="R40" s="89">
         <f t="shared" si="13"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="S40" s="90" t="e">
+        <v>0</v>
+      </c>
+      <c r="S40" s="90">
         <f>AVERAGE($P$3:P40)/SQRT(AVERAGE($R$3:R40))</f>
-        <v>#NUM!</v>
+        <v>0.23935661546120027</v>
       </c>
       <c r="T40" s="2"/>
       <c r="U40" s="3"/>
@@ -43569,35 +43571,37 @@
       <c r="B41" s="69">
         <v>40</v>
       </c>
-      <c r="C41" s="70"/>
+      <c r="C41" s="70">
+        <v>36814</v>
+      </c>
       <c r="D41" s="87"/>
       <c r="E41" s="70">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="F41" s="81" t="e">
+        <v>36814</v>
+      </c>
+      <c r="F41" s="81">
         <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G41" s="80" t="e">
+        <v>135.82236625913953</v>
+      </c>
+      <c r="G41" s="80">
         <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H41" s="80" t="e">
+        <v>-5.0219756979026454E-2</v>
+      </c>
+      <c r="H41" s="80">
         <f t="shared" si="14"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="I41" s="80" t="e">
+        <v>0.30617771556861373</v>
+      </c>
+      <c r="I41" s="80">
         <f>(F41-MAX($F$2:F41))/MAX($F$2:F41)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J41" s="80" t="e">
+        <v>-9.665250865616197E-2</v>
+      </c>
+      <c r="J41" s="80">
         <f>(F41-MIN($F$2:F41))/MAX($F$2:F41)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K41" s="80" t="e">
+        <v>0.26039409333115993</v>
+      </c>
+      <c r="K41" s="80">
         <f>STDEV($G$3:G41)*SQRT(52)</f>
-        <v>#NUM!</v>
+        <v>0.43251889284407968</v>
       </c>
       <c r="L41" s="82"/>
       <c r="M41" s="82"/>
@@ -43606,21 +43610,21 @@
         <f t="shared" si="3"/>
         <v>5.7692307692307687E-4</v>
       </c>
-      <c r="P41" s="88" t="e">
+      <c r="P41" s="88">
         <f t="shared" si="11"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q41" s="88" t="e">
+        <v>-5.0796680055949534E-2</v>
+      </c>
+      <c r="Q41" s="88">
         <f t="shared" si="12"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R41" s="89" t="e">
+        <v>-5.0796680055949534E-2</v>
+      </c>
+      <c r="R41" s="89">
         <f t="shared" si="13"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S41" s="90" t="e">
+        <v>2.5803027047065011E-3</v>
+      </c>
+      <c r="S41" s="90">
         <f>AVERAGE($P$3:P41)/SQRT(AVERAGE($R$3:R41))</f>
-        <v>#NUM!</v>
+        <v>0.195536799224094</v>
       </c>
       <c r="T41" s="2"/>
       <c r="U41" s="3"/>
@@ -43639,25 +43643,25 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="F42" s="81" t="e">
+      <c r="F42" s="81">
         <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="G42" s="80" t="e">
         <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="H42" s="80" t="e">
         <f t="shared" si="14"/>
         <v>#NUM!</v>
       </c>
-      <c r="I42" s="80" t="e">
+      <c r="I42" s="80">
         <f>(F42-MAX($F$2:F42))/MAX($F$2:F42)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J42" s="80" t="e">
+        <v>-1</v>
+      </c>
+      <c r="J42" s="80">
         <f>(F42-MIN($F$2:F42))/MAX($F$2:F42)</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="K42" s="80" t="e">
         <f>STDEV($G$3:G42)*SQRT(52)</f>
@@ -43672,15 +43676,15 @@
       </c>
       <c r="P42" s="88" t="e">
         <f t="shared" si="11"/>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="Q42" s="88" t="e">
         <f t="shared" si="12"/>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="R42" s="89" t="e">
         <f t="shared" si="13"/>
-        <v>#DIV/0!</v>
+        <v>#NUM!</v>
       </c>
       <c r="S42" s="90" t="e">
         <f>AVERAGE($P$3:P42)/SQRT(AVERAGE($R$3:R42))</f>
@@ -69617,7 +69621,7 @@
   <dimension ref="B1:K13"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.6640625" defaultRowHeight="21.75" customHeight="1"/>
@@ -69658,7 +69662,7 @@
         <v>25</v>
       </c>
       <c r="C3" s="20">
-        <v>29731</v>
+        <v>29347</v>
       </c>
       <c r="D3" s="21"/>
       <c r="E3" s="22">
@@ -69715,7 +69719,7 @@
         <v>169</v>
       </c>
       <c r="C6" s="25">
-        <v>4854</v>
+        <v>4700</v>
       </c>
       <c r="D6" s="26"/>
       <c r="E6" s="27">
@@ -69734,7 +69738,7 @@
         <v>29</v>
       </c>
       <c r="C7" s="20">
-        <v>2</v>
+        <v>218</v>
       </c>
       <c r="D7" s="21"/>
       <c r="E7" s="22">
@@ -69753,7 +69757,7 @@
         <v>132</v>
       </c>
       <c r="C8" s="62">
-        <v>802</v>
+        <v>744</v>
       </c>
       <c r="D8" s="63"/>
       <c r="E8" s="64"/>
@@ -69765,7 +69769,7 @@
         <v>30</v>
       </c>
       <c r="C9" s="31">
-        <v>2047</v>
+        <v>1751</v>
       </c>
       <c r="D9" s="32"/>
       <c r="E9" s="33">
@@ -69785,7 +69789,7 @@
       </c>
       <c r="C10" s="37">
         <f>SUM(C3:C9)</f>
-        <v>37490</v>
+        <v>36814</v>
       </c>
       <c r="D10" s="38">
         <f>SUM(D3:D9)</f>
@@ -69827,7 +69831,7 @@
       </c>
       <c r="K13" s="48">
         <f>C$10-$H13</f>
-        <v>10316</v>
+        <v>9640</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
vault backup: 2024-10-05 14:35:49
</commit_message>
<xml_diff>
--- a/_system/Attachments/Portfolio Management.xlsx
+++ b/_system/Attachments/Portfolio Management.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martin/repos/tomesink/obsidian/_system/Attachments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59C6AB06-1E82-7640-BED3-A505E5F38AC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E943E0A7-0BE9-D04D-9D15-88A55772BAC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3860" yWindow="1520" windowWidth="34980" windowHeight="19340" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3860" yWindow="1520" windowWidth="34980" windowHeight="19340" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Stocks Performance" sheetId="1" r:id="rId1"/>
@@ -40924,8 +40924,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:X1011"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A25" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="G42" sqref="G42"/>
+    <sheetView showGridLines="0" topLeftCell="A25" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -43572,36 +43572,36 @@
         <v>40</v>
       </c>
       <c r="C41" s="70">
-        <v>36814</v>
+        <v>36839</v>
       </c>
       <c r="D41" s="87"/>
       <c r="E41" s="70">
         <f t="shared" si="8"/>
-        <v>36814</v>
+        <v>36839</v>
       </c>
       <c r="F41" s="81">
         <f t="shared" si="9"/>
-        <v>135.82236625913953</v>
+        <v>135.91460179878419</v>
       </c>
       <c r="G41" s="80">
         <f t="shared" si="10"/>
-        <v>-5.0219756979026454E-2</v>
+        <v>-4.9540897979118675E-2</v>
       </c>
       <c r="H41" s="80">
         <f t="shared" si="14"/>
-        <v>0.30617771556861373</v>
+        <v>0.30685657456852156</v>
       </c>
       <c r="I41" s="80">
         <f>(F41-MAX($F$2:F41))/MAX($F$2:F41)</f>
-        <v>-9.665250865616197E-2</v>
+        <v>-9.6039054880870042E-2</v>
       </c>
       <c r="J41" s="80">
         <f>(F41-MIN($F$2:F41))/MAX($F$2:F41)</f>
-        <v>0.26039409333115993</v>
+        <v>0.26100754710645185</v>
       </c>
       <c r="K41" s="80">
         <f>STDEV($G$3:G41)*SQRT(52)</f>
-        <v>0.43251889284407968</v>
+        <v>0.43239486152742279</v>
       </c>
       <c r="L41" s="82"/>
       <c r="M41" s="82"/>
@@ -43612,19 +43612,19 @@
       </c>
       <c r="P41" s="88">
         <f t="shared" si="11"/>
-        <v>-5.0796680055949534E-2</v>
+        <v>-5.0117821056041754E-2</v>
       </c>
       <c r="Q41" s="88">
         <f t="shared" si="12"/>
-        <v>-5.0796680055949534E-2</v>
+        <v>-5.0117821056041754E-2</v>
       </c>
       <c r="R41" s="89">
         <f t="shared" si="13"/>
-        <v>2.5803027047065011E-3</v>
+        <v>2.5117959874054224E-3</v>
       </c>
       <c r="S41" s="90">
         <f>AVERAGE($P$3:P41)/SQRT(AVERAGE($R$3:R41))</f>
-        <v>0.195536799224094</v>
+        <v>0.19612925578939819</v>
       </c>
       <c r="T41" s="2"/>
       <c r="U41" s="3"/>
@@ -69322,8 +69322,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{960A98AA-C170-FD4F-A0A4-3255EEA67EE9}">
   <dimension ref="A1:M17"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -69460,7 +69460,7 @@
         <v>3.4200000000000001E-2</v>
       </c>
       <c r="D6" s="188">
-        <f t="shared" ref="D6:D11" si="0">D5+C6</f>
+        <f t="shared" ref="D6:D12" si="0">D5+C6</f>
         <v>7.3899999999999993E-2</v>
       </c>
       <c r="E6" s="184">
@@ -69542,30 +69542,38 @@
         <v>8</v>
       </c>
       <c r="C11" s="187">
-        <v>-3.49E-2</v>
+        <v>9.7000000000000003E-3</v>
       </c>
       <c r="D11" s="188">
         <f t="shared" si="0"/>
-        <v>9.5099999999999976E-2</v>
+        <v>0.13969999999999999</v>
       </c>
       <c r="E11" s="184">
         <f>STDEV($D$2:D11)*SQRT(52)</f>
-        <v>0.35429037180758316</v>
+        <v>0.39391794971936861</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="14">
       <c r="A12" s="189"/>
       <c r="B12" s="176">
-        <v>3</v>
-      </c>
-      <c r="C12" s="187"/>
-      <c r="D12" s="188"/>
-      <c r="E12" s="190"/>
+        <v>9</v>
+      </c>
+      <c r="C12" s="187">
+        <v>3.09E-2</v>
+      </c>
+      <c r="D12" s="188">
+        <f t="shared" si="0"/>
+        <v>0.1706</v>
+      </c>
+      <c r="E12" s="184">
+        <f>STDEV($D$2:D12)*SQRT(52)</f>
+        <v>0.44193308584404078</v>
+      </c>
     </row>
     <row r="13" spans="1:13" ht="14">
       <c r="A13" s="189"/>
       <c r="B13" s="176">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C13" s="187"/>
       <c r="D13" s="188"/>
@@ -69574,7 +69582,7 @@
     <row r="14" spans="1:13" ht="14">
       <c r="A14" s="189"/>
       <c r="B14" s="176">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C14" s="187"/>
       <c r="D14" s="188"/>
@@ -69583,7 +69591,7 @@
     <row r="15" spans="1:13" ht="14">
       <c r="A15" s="189"/>
       <c r="B15" s="176">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C15" s="187"/>
       <c r="D15" s="188"/>
@@ -69591,18 +69599,14 @@
     </row>
     <row r="16" spans="1:13" ht="14">
       <c r="A16" s="189"/>
-      <c r="B16" s="171">
-        <v>7</v>
-      </c>
+      <c r="B16" s="171"/>
       <c r="C16" s="187"/>
       <c r="D16" s="188"/>
       <c r="E16" s="190"/>
     </row>
     <row r="17" spans="1:5" ht="14">
       <c r="A17" s="189"/>
-      <c r="B17" s="171">
-        <v>8</v>
-      </c>
+      <c r="B17" s="171"/>
       <c r="C17" s="187"/>
       <c r="D17" s="188"/>
       <c r="E17" s="190"/>
@@ -69621,7 +69625,7 @@
   <dimension ref="B1:K13"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.6640625" defaultRowHeight="21.75" customHeight="1"/>
@@ -69757,7 +69761,7 @@
         <v>132</v>
       </c>
       <c r="C8" s="62">
-        <v>744</v>
+        <v>769</v>
       </c>
       <c r="D8" s="63"/>
       <c r="E8" s="64"/>
@@ -69789,7 +69793,7 @@
       </c>
       <c r="C10" s="37">
         <f>SUM(C3:C9)</f>
-        <v>36814</v>
+        <v>36839</v>
       </c>
       <c r="D10" s="38">
         <f>SUM(D3:D9)</f>
@@ -69831,7 +69835,7 @@
       </c>
       <c r="K13" s="48">
         <f>C$10-$H13</f>
-        <v>9640</v>
+        <v>9665</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
vault backup: 2024-10-05 14:36:48
</commit_message>
<xml_diff>
--- a/_system/Attachments/Portfolio Management.xlsx
+++ b/_system/Attachments/Portfolio Management.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martin/repos/tomesink/obsidian/_system/Attachments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E943E0A7-0BE9-D04D-9D15-88A55772BAC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76DFDA1A-1FEC-1341-86B4-0244A8BB0C2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3860" yWindow="1520" windowWidth="34980" windowHeight="19340" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2000" yWindow="1200" windowWidth="34980" windowHeight="19340" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Stocks Performance" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
vault backup: 2024-10-09 12:57:34
</commit_message>
<xml_diff>
--- a/_system/Attachments/Portfolio Management.xlsx
+++ b/_system/Attachments/Portfolio Management.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martin/repos/tomesink/obsidian/_system/Attachments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76DFDA1A-1FEC-1341-86B4-0244A8BB0C2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66C4BD7F-9043-8A45-85CE-D0782C686BA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2000" yWindow="1200" windowWidth="34980" windowHeight="19340" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2000" yWindow="1200" windowWidth="34980" windowHeight="19340" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Stocks Performance" sheetId="1" r:id="rId1"/>
@@ -319,7 +319,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="170">
   <si>
     <t>Year</t>
   </si>
@@ -4669,11 +4669,9 @@
     <v>Powered by Refinitiv</v>
     <v>83.25</v>
     <v>52.770499999999998</v>
-    <v>0.52700000000000002</v>
-    <v>1.67</v>
-    <v>2.6542E-2</v>
-    <v>-0.2</v>
-    <v>-3.0959999999999998E-3</v>
+    <v>0.52280000000000004</v>
+    <v>0.65</v>
+    <v>9.9620000000000004E-3</v>
     <v>USD</v>
     <v>CVS Health Corporation is a health solutions company. The Company operates in four segments: Health Care Benefits, Health Services, Pharmacy &amp; Consumer Wellness, and Corporate/Other. Its Health Care Benefits segment offer a range of traditional, voluntary and consumer-directed health insurance products and related services, including medical, pharmacy, dental and behavioral health plans, medical management capabilities, Medicare Advantage and Medicare supplement plans, and Medicaid health care management services. Its Health Services segment provides a full range of pharmacy benefit management solutions, delivers health care services in its medical clinics, virtually, and in the home, and offers provider enablement solutions. The Pharmacy &amp; Consumer Wellness segment dispenses prescriptions in its retail pharmacies and through its infusion operations, provides ancillary pharmacy services, including pharmacy patient care programs, diagnostic testing and vaccination administration.</v>
     <v>300000</v>
@@ -4681,25 +4679,24 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>1 Cvs Dr, WOONSOCKET, RI, 02895-6146 US</v>
-    <v>65.569999999999993</v>
+    <v>66.099999999999994</v>
     <v>Healthcare Providers &amp; Services</v>
     <v>Stock</v>
-    <v>45569.999667777345</v>
+    <v>45573.998909003909</v>
     <v>0</v>
-    <v>63.664299999999997</v>
-    <v>81252863610</v>
+    <v>64.95</v>
+    <v>82900816100</v>
     <v>CVS HEALTH CORPORATION</v>
     <v>CVS HEALTH CORPORATION</v>
-    <v>63.72</v>
-    <v>11.4941</v>
-    <v>62.92</v>
-    <v>64.59</v>
-    <v>64.39</v>
+    <v>65.3</v>
+    <v>11.7272</v>
+    <v>65.25</v>
+    <v>65.900000000000006</v>
     <v>1257979000</v>
     <v>CVS</v>
     <v>CVS HEALTH CORPORATION (XNYS:CVS)</v>
-    <v>16313877</v>
-    <v>9631744</v>
+    <v>747</v>
+    <v>10058342</v>
     <v>1996</v>
   </rv>
   <rv s="2">
@@ -4709,13 +4706,13 @@
     <v>https://www.bing.com/financeapi/forcetrigger?t=a1qclh&amp;q=XNAS%3aCROX&amp;form=skydnc</v>
     <v>Learn more on Bing</v>
   </rv>
-  <rv s="1">
-    <v>0</v>
+  <rv s="3">
+    <v>5</v>
     <v>CROCS, INC. (XNAS:CROX)</v>
     <v>2</v>
-    <v>3</v>
+    <v>6</v>
     <v>Finance</v>
-    <v>4</v>
+    <v>7</v>
     <v>en-GB</v>
     <v>a1qclh</v>
     <v>268435456</v>
@@ -4723,11 +4720,9 @@
     <v>Powered by Refinitiv</v>
     <v>165.32</v>
     <v>74</v>
-    <v>1.9844999999999999</v>
-    <v>3.94</v>
-    <v>2.8553000000000002E-2</v>
-    <v>-0.13</v>
-    <v>-9.1590000000000009E-4</v>
+    <v>1.9888999999999999</v>
+    <v>-0.93</v>
+    <v>-6.8110000000000002E-3</v>
     <v>USD</v>
     <v>Crocs, Inc. is engaged in the design, development, worldwide marketing, distribution, and sale of casual lifestyle footwear and accessories for women, men, and children. The Company’s segments include Crocs Brand and the HEYDUDE Brand. The Company’s Crocs Brand collection contains Croslite material, a molded footwear technology, delivering extraordinary comfort with each step. Its Croslite materials are formulated to create soft, comfortable, lightweight, non-marking, and odor-resistant footwear. The HEYDUDE Brand offers shoes with a versatile silhouette. It sells its products in more than 80 countries, through two distribution channels: wholesale and direct-to-consumer. Its wholesale channel includes domestic and international multi-brand retailers, mono-branded partner stores, e-tailers, and distributors; its direct-to-consumer channel includes Company-operated retail stores, Company-operated e-commerce sites, and third-party marketplaces.</v>
     <v>7030</v>
@@ -4735,25 +4730,25 @@
     <v>XNAS</v>
     <v>XNAS</v>
     <v>500 Eldorado Boulevard, Building 5, BROOMFIELD, CO, 80021 US</v>
-    <v>142.74</v>
+    <v>137.25</v>
     <v>Textiles &amp; Apparel</v>
     <v>Stock</v>
-    <v>45569.974103135937</v>
+    <v>45573.999516365628</v>
     <v>3</v>
-    <v>140.28</v>
-    <v>8428531500</v>
+    <v>134.63</v>
+    <v>8053217479</v>
     <v>CROCS, INC.</v>
     <v>CROCS, INC.</v>
-    <v>140.86000000000001</v>
-    <v>10.3779</v>
-    <v>137.99</v>
-    <v>141.93</v>
-    <v>141.80000000000001</v>
+    <v>135.74</v>
+    <v>10.1989</v>
+    <v>136.54</v>
+    <v>135.61000000000001</v>
+    <v>136.55000000000001</v>
     <v>59385130</v>
     <v>CROX</v>
     <v>CROCS, INC. (XNAS:CROX)</v>
-    <v>813650</v>
-    <v>972930</v>
+    <v>682</v>
+    <v>974515</v>
     <v>2005</v>
   </rv>
   <rv s="2">
@@ -4769,19 +4764,17 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>4</v>
+    <v>8</v>
     <v>en-GB</v>
     <v>a25yfr</v>
     <v>268435456</v>
     <v>1</v>
     <v>Powered by Refinitiv</v>
     <v>30.07</v>
-    <v>17.71</v>
-    <v>1.5218</v>
-    <v>-0.13</v>
-    <v>-7.1189999999999995E-3</v>
-    <v>0</v>
-    <v>0</v>
+    <v>17.68</v>
+    <v>1.5229999999999999</v>
+    <v>0.18</v>
+    <v>9.9670000000000002E-3</v>
     <v>USD</v>
     <v>Wabash National Corporation provides connected solutions for the transportation, logistics and distribution industries. The Company designs and manufactures products including dry freight and refrigerated trailers, platform trailers, tank trailers, dry and refrigerated truck bodies, structural composite panels and products, transportation, logistics, and distribution industry parts and services, and specialty food grade processing equipment. The Company’s Transportation Solutions (TS) segment comprises the design and manufacturing operations for the Company’s transportation-related equipment and products. This includes dry and refrigerated van trailers, platform trailers, tank trailers and truck-mounted tanks, truck-mounted dry and refrigerated truck bodies and EcoNex technology products. Its Parts &amp; Services (P&amp;S) segment is comprised of the Company’s parts and services businesses as well as the upfitting component of truck bodies business. It also includes DuraPlate composite panels.</v>
     <v>6700</v>
@@ -4789,25 +4782,24 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>3900 Mccarty Lane, LAFAYETTE, IN, 47905 US</v>
-    <v>18.66</v>
+    <v>18.309999999999999</v>
     <v>Machinery, Equipment &amp; Components</v>
     <v>Stock</v>
-    <v>45569.958333333336</v>
+    <v>45573.990293286719</v>
     <v>6</v>
-    <v>17.989999999999998</v>
-    <v>797706039</v>
+    <v>17.68</v>
+    <v>802545955</v>
     <v>WABASH NATIONAL CORPORATION</v>
     <v>WABASH NATIONAL CORPORATION</v>
-    <v>18.579999999999998</v>
-    <v>5.5614999999999997</v>
-    <v>18.260000000000002</v>
-    <v>18.13</v>
-    <v>18.13</v>
+    <v>18.05</v>
+    <v>5.5952000000000002</v>
+    <v>18.059999999999999</v>
+    <v>18.239999999999998</v>
     <v>43999230</v>
     <v>WNC</v>
     <v>WABASH NATIONAL CORPORATION (XNYS:WNC)</v>
-    <v>294144</v>
-    <v>598279</v>
+    <v>315998</v>
+    <v>586650</v>
     <v>1991</v>
   </rv>
   <rv s="2">
@@ -4831,11 +4823,9 @@
     <v>Powered by Refinitiv</v>
     <v>26.4</v>
     <v>16.12</v>
-    <v>1.0426</v>
-    <v>0.57999999999999996</v>
-    <v>2.7618999999999998E-2</v>
-    <v>0</v>
-    <v>0</v>
+    <v>1.0441</v>
+    <v>-0.1</v>
+    <v>-4.6839999999999998E-3</v>
     <v>USD</v>
     <v>Perdoceo Education Corporation, through its academic institutions, offers quality postsecondary education primarily online to a diverse student population, along with campus-based and blended learning programs. The Company's academic institutions include Colorado Technical University (CTU) and the American InterContinental University System (AIUS), which provides degree programs from the associate through doctoral level as well as non-degree seeking and professional development programs. Its academic institutions offer students industry-relevant and career-focused academic programs. CTU offers academic programs in the career-oriented disciplines of business and management, nursing, healthcare management, computer science, engineering, information systems and technology, project management, cybersecurity and criminal justice. AIUS offers academic programs in the career-oriented disciplines of business studies, information technologies, education, health sciences and criminal justice.</v>
     <v>2319</v>
@@ -4843,25 +4833,24 @@
     <v>XNAS</v>
     <v>XNAS</v>
     <v>1750 E. GOLF ROAD, SCHAUMBURG, IL, 60173 US</v>
-    <v>21.78</v>
+    <v>21.39</v>
     <v>Miscellaneous Educational Service Providers</v>
     <v>Stock</v>
-    <v>45569.834787939064</v>
+    <v>45573.835138089846</v>
     <v>9</v>
-    <v>21.27</v>
-    <v>1417232619</v>
+    <v>21.16</v>
+    <v>1395560387</v>
     <v>PERDOCEO EDUCATION CORPORATION</v>
     <v>PERDOCEO EDUCATION CORPORATION</v>
-    <v>21.28</v>
-    <v>10.320499999999999</v>
-    <v>21</v>
-    <v>21.58</v>
-    <v>21.58</v>
+    <v>21.37</v>
+    <v>10.4434</v>
+    <v>21.35</v>
+    <v>21.25</v>
     <v>65673430</v>
     <v>PRDO</v>
     <v>PERDOCEO EDUCATION CORPORATION (XNAS:PRDO)</v>
-    <v>342126</v>
-    <v>468802</v>
+    <v>178164</v>
+    <v>466975</v>
     <v>1994</v>
   </rv>
   <rv s="2">
@@ -4877,7 +4866,7 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>4</v>
+    <v>8</v>
     <v>en-GB</v>
     <v>a1mou2</v>
     <v>268435456</v>
@@ -4885,11 +4874,9 @@
     <v>Powered by Refinitiv</v>
     <v>237.23</v>
     <v>164.07499999999999</v>
-    <v>1.2384999999999999</v>
-    <v>1.1299999999999999</v>
-    <v>5.0070000000000002E-3</v>
-    <v>-0.38500000000000001</v>
-    <v>-1.6980000000000001E-3</v>
+    <v>1.2421</v>
+    <v>4.08</v>
+    <v>1.8404E-2</v>
     <v>USD</v>
     <v>Apple Inc. designs, manufactures and markets smartphones, personal computers, tablets, wearables and accessories, and sells a variety of related services. Its product categories include iPhone, Mac, iPad, and Wearables, Home and Accessories. Its software platforms include iOS, iPadOS, macOS, watchOS, and tvOS. Its services include advertising, AppleCare, cloud services, digital content and payment services. It operates various platforms, including the App Store, that allow customers to discover and download applications and digital content, such as books, music, video, games and podcasts. It also offers digital content through subscription-based services, including Apple Arcade, Apple Fitness+, Apple Music, Apple News+ and Apple TV+. Its products include iPhone 15 Pro, iPhone 15, iPhone 14, iPhone 13, MacBook Air, MacBook Pro, iMac, Mac mini, Mac Studio, Mac Pro, and others. It also provides DarwinAI, which specializes in visual quality inspection using its Explainable AI platform.</v>
     <v>161000</v>
@@ -4897,25 +4884,24 @@
     <v>XNAS</v>
     <v>XNAS</v>
     <v>One Apple Park Way, CUPERTINO, CA, 95014 US</v>
-    <v>228</v>
+    <v>225.98</v>
     <v>Computers, Phones &amp; Household Electronics</v>
     <v>Stock</v>
-    <v>45569.999978448439</v>
+    <v>45573.999981503905</v>
     <v>12</v>
-    <v>224.13</v>
-    <v>3448298952000</v>
+    <v>223.25</v>
+    <v>3432638687800</v>
     <v>APPLE INC.</v>
     <v>APPLE INC.</v>
-    <v>227.9</v>
-    <v>34.220999999999997</v>
-    <v>225.67</v>
-    <v>226.8</v>
-    <v>226.41499999999999</v>
+    <v>224.3</v>
+    <v>34.374699999999997</v>
+    <v>221.69</v>
+    <v>225.77</v>
     <v>15204140000</v>
     <v>AAPL</v>
     <v>APPLE INC. (XNAS:AAPL)</v>
-    <v>37345098</v>
-    <v>58699950</v>
+    <v>30674</v>
+    <v>58117502</v>
     <v>1977</v>
   </rv>
   <rv s="2">
@@ -4937,13 +4923,11 @@
     <v>268435456</v>
     <v>1</v>
     <v>Powered by Refinitiv</v>
-    <v>99.08</v>
+    <v>100.73</v>
     <v>50.134999999999998</v>
-    <v>0.99099999999999999</v>
-    <v>1.96</v>
-    <v>2.0187E-2</v>
-    <v>-3.2500000000000001E-2</v>
-    <v>-3.2810000000000001E-4</v>
+    <v>0.98750000000000004</v>
+    <v>-1.55</v>
+    <v>-1.5598000000000001E-2</v>
     <v>USD</v>
     <v>Allison Transmission Holdings, Inc. is a designer and manufacturer of propulsion solutions for commercial and defense vehicles. The Company is also a manufacturer of medium-and heavy-duty fully automatic transmissions. Its products are used in a variety of applications, including on-highway trucks, including distribution, refuse, construction, fire and emergency; buses, including school, transit and coach; motorhomes, off-highway vehicles, and equipment, including energy, mining and construction applications; and defense vehicles, including tactical wheeled and tracked. The Company operates in approximately 150 countries. The Company has manufacturing facilities in the United States, Hungary and India, as well as global engineering resources, including electrification engineering centers in Indianapolis, Indiana, Auburn Hills, Michigan and London in the United Kingdom. The Company also has approximately 1,600 independent distributor and dealer locations worldwide.</v>
     <v>3700</v>
@@ -4951,25 +4935,24 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>One Allison Way, INDIANAPOLIS, IN, 46222 US</v>
-    <v>99.08</v>
+    <v>98.94</v>
     <v>Machinery, Equipment &amp; Components</v>
     <v>Stock</v>
-    <v>45569.983881921093</v>
+    <v>45573.97539405078</v>
     <v>15</v>
-    <v>97.35</v>
-    <v>8631007014</v>
+    <v>97.170299999999997</v>
+    <v>8523827421</v>
     <v>ALLISON TRANSMISSION HOLDINGS, INC.</v>
     <v>ALLISON TRANSMISSION HOLDINGS, INC.</v>
-    <v>98.36</v>
-    <v>12.9518</v>
-    <v>97.09</v>
-    <v>99.05</v>
-    <v>99.017499999999998</v>
+    <v>98.94</v>
+    <v>12.791</v>
+    <v>99.37</v>
+    <v>97.82</v>
     <v>87137880</v>
     <v>ALSN</v>
     <v>ALLISON TRANSMISSION HOLDINGS, INC. (XNYS:ALSN)</v>
-    <v>385259</v>
-    <v>635069</v>
+    <v>607183</v>
+    <v>631715</v>
     <v>2007</v>
   </rv>
   <rv s="2">
@@ -4993,11 +4976,9 @@
     <v>Powered by Refinitiv</v>
     <v>40.695</v>
     <v>17.063600000000001</v>
-    <v>1.972</v>
-    <v>-0.35</v>
-    <v>-1.8116E-2</v>
-    <v>0</v>
-    <v>0</v>
+    <v>1.966</v>
+    <v>-1.08</v>
+    <v>-5.7754E-2</v>
     <v>USD</v>
     <v>Par Pacific Holdings, Inc. is an energy company, which provides both renewable and conventional fuels to the western United States. It owns and operates 125,000 barrels per day of combined refining capacity across three locations and an energy infrastructure network, including 7.6 million barrels of storage, and marine, rail, rack and pipeline assets. The Company has three segments. Refining segment owns and operates four refineries with total operating crude oil throughput capacity of 219 thousand barrels per day (Mbpd). Retail segment operates fuel retail outlets in Hawaii, Washington and Idaho. It operates convenience stores and fuel retail sites under Hele and nomnom brands, 76 branded fuel retail sites and other sites operated by third parties that sell gasoline, diesel, and retail merchandise, such as soft drinks, prepared foods, and other sundries. Logistics segment operates a multi-modal logistics network spanning the Pacific, the Northwest, and the Rocky Mountain regions.</v>
     <v>1814</v>
@@ -5005,25 +4986,24 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>825 Town and Country Ln Ste 1500, HOUSTON, TX, 77024-2235 US</v>
-    <v>19.71</v>
+    <v>18.510000000000002</v>
     <v>Oil &amp; Gas</v>
     <v>Stock</v>
-    <v>45569.958333356248</v>
+    <v>45573.958333378905</v>
     <v>18</v>
-    <v>18.64</v>
-    <v>1088312000</v>
+    <v>17.32</v>
+    <v>992549929</v>
     <v>PAR PACIFIC HOLDINGS, INC.</v>
     <v>PAR PACIFIC HOLDINGS, INC.</v>
-    <v>19.55</v>
-    <v>3.3052000000000001</v>
-    <v>19.32</v>
-    <v>18.97</v>
-    <v>18.97</v>
+    <v>18.510000000000002</v>
+    <v>3.0699000000000001</v>
+    <v>18.7</v>
+    <v>17.62</v>
     <v>56330870</v>
     <v>PARR</v>
     <v>PAR PACIFIC HOLDINGS, INC. (XNYS:PARR)</v>
-    <v>961414</v>
-    <v>1306497</v>
+    <v>973481</v>
+    <v>1287668</v>
     <v>2005</v>
   </rv>
   <rv s="2">
@@ -5039,7 +5019,7 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>4</v>
+    <v>8</v>
     <v>en-GB</v>
     <v>a1v177</v>
     <v>268435456</v>
@@ -5047,11 +5027,9 @@
     <v>Powered by Refinitiv</v>
     <v>84.44</v>
     <v>38.5</v>
-    <v>1.3087</v>
-    <v>3.38</v>
-    <v>5.4218999999999996E-2</v>
-    <v>0</v>
-    <v>0</v>
+    <v>1.3029999999999999</v>
+    <v>-1.36</v>
+    <v>-2.0438999999999999E-2</v>
     <v>USD</v>
     <v>Hyster-Yale, Inc., formerly Hyster-Yale Materials Handling, Inc., through its wholly owned operating subsidiary, Hyster-Yale Materials Handling, designs, engineers, manufactures, sells, and services a comprehensive line of lift trucks, attachments, aftermarket parts and technology solutions marketed globally primarily under the Hyster and Yale brand names. The Company's business segments include Lift Trucks, Attachments and Fuel Cells. The Hyster-Yale Maximal brand provides trucks for customers requiring fundamental lift truck performance. The Lift Truck segment is focused on fuel cell-powered battery box replacements and integrated fuel cell engine solutions. Hyster- Yale’s attachment subsidiary, Bolzoni S.p.A., is a producer of attachments, forks, and lift tables under the Bolzoni, Auramo and Meyer brand names. The Fuel Cell business, Nuvera Fuel Cells, is an alternative-power technology company focused on fuel cell stacks and engines.</v>
     <v>8600</v>
@@ -5059,25 +5037,24 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>5875 LANDERBROOK DRIVE, SUITE 300, CLEVELAND, OH, 44124 US</v>
-    <v>65.760000000000005</v>
+    <v>66.6357</v>
     <v>Machinery, Equipment &amp; Components</v>
     <v>Stock</v>
-    <v>45569.958333378905</v>
+    <v>45573.958333378905</v>
     <v>21</v>
-    <v>63.31</v>
-    <v>1091021000</v>
+    <v>64.306899999999999</v>
+    <v>1164526000</v>
     <v>HYSTER-YALE, INC.</v>
     <v>HYSTER-YALE, INC.</v>
-    <v>63.62</v>
-    <v>6.5719000000000003</v>
-    <v>62.34</v>
-    <v>65.72</v>
-    <v>65.72</v>
+    <v>66.2</v>
+    <v>6.5179</v>
+    <v>66.540000000000006</v>
+    <v>65.180000000000007</v>
     <v>17501150</v>
     <v>HY</v>
     <v>HYSTER-YALE, INC. (XNYS:HY)</v>
-    <v>83022</v>
-    <v>66357</v>
+    <v>69204</v>
+    <v>66539</v>
     <v>1999</v>
   </rv>
   <rv s="2">
@@ -5087,13 +5064,13 @@
     <v>https://www.bing.com/financeapi/forcetrigger?t=a1zvsm&amp;q=XNYS%3aPII&amp;form=skydnc</v>
     <v>Learn more on Bing</v>
   </rv>
-  <rv s="1">
-    <v>0</v>
+  <rv s="3">
+    <v>5</v>
     <v>Polaris Inc. (XNYS:PII)</v>
     <v>2</v>
-    <v>3</v>
+    <v>6</v>
     <v>Finance</v>
-    <v>4</v>
+    <v>7</v>
     <v>en-GB</v>
     <v>a1zvsm</v>
     <v>268435456</v>
@@ -5101,11 +5078,9 @@
     <v>Powered by Refinitiv</v>
     <v>100.91</v>
     <v>71.900000000000006</v>
-    <v>1.5028999999999999</v>
-    <v>0.4</v>
-    <v>4.8869999999999999E-3</v>
-    <v>0.39</v>
-    <v>4.7419999999999997E-3</v>
+    <v>1.5048999999999999</v>
+    <v>-0.55000000000000004</v>
+    <v>-6.8979999999999996E-3</v>
     <v>USD</v>
     <v>Polaris Inc. is engaged in designing, engineering, manufacturing and marketing of powersports vehicles. The Company also designs and manufactures or sources parts, garments and accessories (PG&amp;A), which includes aftermarket accessories and apparel. The Company operates through three segments: Off Road, On Road and Marine. The Off Road segment consists of off-road vehicles and snowmobiles. The On Road segment designs and manufactures motorcycles, moto-roadsters, light duty hauling, and passenger vehicles. The Marine segment designs and manufactures boats that are designed to compete in key segments of the recreational marine industry, specifically pontoon and deck boats. Its product line-up includes the RANGER, RZR and Polaris XPEDITION and GENERAL side-by-side off-road vehicles; Sportsman all-terrain off-road vehicles; military and commercial off-road vehicles; snowmobiles; Indian Motorcycle mid-size and heavyweight motorcycles; Slingshot moto-roadsters, and pontoon and deck boats.</v>
     <v>18500</v>
@@ -5113,25 +5088,25 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>2100 HIGHWAY 55, MEDINA, MN, 55340-9770 US</v>
-    <v>83.07</v>
+    <v>79.819999999999993</v>
     <v>Leisure Products</v>
     <v>Stock</v>
-    <v>45569.958333344533</v>
+    <v>45573.958333356248</v>
     <v>24</v>
-    <v>81.75</v>
-    <v>4585275467</v>
+    <v>78.72</v>
+    <v>4414129015</v>
     <v>Polaris Inc.</v>
     <v>Polaris Inc.</v>
-    <v>82.92</v>
-    <v>14.406599999999999</v>
-    <v>81.849999999999994</v>
-    <v>82.25</v>
-    <v>82.64</v>
+    <v>79.489999999999995</v>
+    <v>13.8687</v>
+    <v>79.73</v>
+    <v>79.180000000000007</v>
+    <v>79.099999999999994</v>
     <v>55748030</v>
     <v>PII</v>
     <v>Polaris Inc. (XNYS:PII)</v>
-    <v>347818</v>
-    <v>497431</v>
+    <v>2</v>
+    <v>496825</v>
     <v>1994</v>
   </rv>
   <rv s="2">
@@ -5155,11 +5130,9 @@
     <v>Powered by Refinitiv</v>
     <v>114.29989999999999</v>
     <v>75.430000000000007</v>
-    <v>1.7454000000000001</v>
-    <v>2.4500000000000002</v>
-    <v>2.3990999999999998E-2</v>
-    <v>-0.01</v>
-    <v>-9.5630000000000004E-5</v>
+    <v>1.7407999999999999</v>
+    <v>-1.99</v>
+    <v>-1.8488000000000001E-2</v>
     <v>USD</v>
     <v>CONSOL Energy Inc. is a producer and exporter of high-Btu bituminous thermal coal and metallurgical coal. It owns and operates longwall mining operations in the Northern Appalachian Basin. Its flagship operation is the Pennsylvania Mining Complex, located over 26 miles southwest of Pittsburgh, near the city of Washington and the borough of Waynesburg all in Pennsylvania, and consists of three deep longwall mining operations: the Bailey Mine, the Enlow Fork Mine and the Harvey Mine, as well as a centralized preparation plant. Its segments include the PAMC and the CONSOL Marine Terminal. The PAMC includes the Bailey Mine, the Enlow Fork Mine, the Harvey Mine and a centralized preparation plant. The PAMC segment's principal activities include the mining, preparation and marketing of bituminous coal, sold primarily to industrial end-users, metallurgical end-users and power generators. The CONSOL Marine Terminal segment provides coal export terminal services through the Port of Baltimore.</v>
     <v>2020</v>
@@ -5167,25 +5140,24 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>275 TECHNOLOGY DRIVE, SUITE #101, CANONSBURG, PA, 15317 US</v>
-    <v>105.1344</v>
+    <v>106.43</v>
     <v>Coal</v>
     <v>Stock</v>
-    <v>45569.969649536717</v>
+    <v>45573.973457835156</v>
     <v>27</v>
-    <v>102.51</v>
-    <v>3073650061</v>
+    <v>103.12</v>
+    <v>3105394749</v>
     <v>CONSOL ENERGY INC.</v>
     <v>CONSOL ENERGY INC.</v>
-    <v>103.03</v>
-    <v>7.8056999999999999</v>
-    <v>102.12</v>
-    <v>104.57</v>
-    <v>104.56</v>
+    <v>105.6</v>
+    <v>7.8863000000000003</v>
+    <v>107.64</v>
+    <v>105.65</v>
     <v>29393230</v>
     <v>CEIX</v>
     <v>CONSOL ENERGY INC. (XNYS:CEIX)</v>
-    <v>311631</v>
-    <v>424376</v>
+    <v>1</v>
+    <v>422716</v>
     <v>2017</v>
   </rv>
   <rv s="2">
@@ -5209,11 +5181,9 @@
     <v>Powered by Refinitiv</v>
     <v>127.3484</v>
     <v>84.35</v>
-    <v>1.2523</v>
-    <v>1.18</v>
-    <v>1.2257000000000001E-2</v>
-    <v>-1.31</v>
-    <v>-1.3443E-2</v>
+    <v>1.2513000000000001</v>
+    <v>-1.76</v>
+    <v>-1.8173999999999999E-2</v>
     <v>USD</v>
     <v>AGCO Corporation is a designer, manufacturer and distributor of agricultural machinery and precision agriculture technology. The Company sells a range of agricultural equipment, including tractors, combines, self-propelled sprayers, hay tools, forage equipment, seeding and tillage equipment, implements, and grain storage and protein production systems. It provides telemetry-based fleet management tools, including remote monitoring and diagnostics, which help farmers improve uptime, machine and yield optimization, mixed fleet optimization and decision support. The Company's Precision Planting, Headsight and Intelligent Ag Solutions brands provide retrofit solutions to upgrade farmers existing equipment to improve their planting, liquid application and harvest operations. The Company’s Precision Planting, Headsight, JCA and Intelligent Ag Solutions brands also sell precision agriculture solutions around the crop cycle to third party original equipment manufacturers (OEMs).</v>
     <v>27900</v>
@@ -5221,25 +5191,24 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>4205 River Green Pkway, DULUTH, GA, 30096 US</v>
-    <v>97.65</v>
+    <v>97.15</v>
     <v>Machinery, Equipment &amp; Components</v>
     <v>Stock</v>
-    <v>45569.999739073435</v>
+    <v>45573.958333367969</v>
     <v>30</v>
-    <v>96.65</v>
-    <v>7273892135</v>
+    <v>94.045000000000002</v>
+    <v>7096989884</v>
     <v>AGCO CORPORATION</v>
     <v>AGCO CORPORATION</v>
-    <v>97.52</v>
-    <v>17.359300000000001</v>
-    <v>96.27</v>
-    <v>97.45</v>
-    <v>96.14</v>
+    <v>96.13</v>
+    <v>16.9373</v>
+    <v>96.84</v>
+    <v>95.08</v>
     <v>74642300</v>
     <v>AGCO</v>
     <v>AGCO CORPORATION (XNYS:AGCO)</v>
-    <v>450825</v>
-    <v>743528</v>
+    <v>586739</v>
+    <v>720356</v>
     <v>1991</v>
   </rv>
   <rv s="2">
@@ -5264,10 +5233,8 @@
     <v>30.07</v>
     <v>24.01</v>
     <v>1.1493</v>
-    <v>0.2</v>
-    <v>7.6829999999999997E-3</v>
-    <v>0</v>
-    <v>0</v>
+    <v>-0.11</v>
+    <v>-4.1570000000000001E-3</v>
     <v>USD</v>
     <v>Ituran Location and Control Ltd. is a provider of location-based services, consisting of stolen vehicle recovery (SVR), fleet management services and other tracking services. The Company also provides wireless communication products used in connection with its location-based services and various other applications. Its operations consist of two segments: location-based services and wireless communications products. Its location-based services segment consists of its SVR and tracking services, fleet management and value-added services consisted of personal locater services and concierge services. Its wireless communications products segment consists of short and medium range two-way machine-to-machine wireless communications products that are used for various applications, including automatic vehicle location (AVL) and automatic vehicle identification. It primarily provides its services, as well as sells and leases its products in Israel, Brazil, Argentina and the United States.</v>
     <v>2841</v>
@@ -5275,25 +5242,24 @@
     <v>XNAS</v>
     <v>XNAS</v>
     <v>3 HASHIKMA, A.T AZUR, T.D 163, AZOR, 5800182 IL</v>
-    <v>26.234999999999999</v>
+    <v>26.57</v>
     <v>Communications &amp; Networking</v>
     <v>Stock</v>
-    <v>45569.833445775002</v>
+    <v>45573.859743020315</v>
     <v>33</v>
-    <v>25.864999999999998</v>
-    <v>521808603</v>
+    <v>26.26</v>
+    <v>524195833</v>
     <v>ITURAN LOCATION AND CONTROL LTD.</v>
     <v>ITURAN LOCATION AND CONTROL LTD.</v>
-    <v>26.13</v>
-    <v>10.273</v>
-    <v>26.03</v>
-    <v>26.23</v>
-    <v>26.23</v>
+    <v>26.46</v>
+    <v>10.319900000000001</v>
+    <v>26.46</v>
+    <v>26.35</v>
     <v>19893580</v>
     <v>ITRN</v>
     <v>ITURAN LOCATION AND CONTROL LTD. (XNAS:ITRN)</v>
-    <v>45013</v>
-    <v>73923</v>
+    <v>73311</v>
+    <v>73553</v>
     <v>1994</v>
   </rv>
   <rv s="2">
@@ -5317,11 +5283,9 @@
     <v>Powered by Refinitiv</v>
     <v>13.345000000000001</v>
     <v>6.37</v>
-    <v>2.1423999999999999</v>
+    <v>2.1389999999999998</v>
     <v>0</v>
     <v>0</v>
-    <v>-0.01</v>
-    <v>-7.6050000000000011E-4</v>
     <v>USD</v>
     <v>Everi Holdings Inc. develops and offers products and services that provide gaming entertainment, improve its customers’ patron engagement, and help its casino customers operate their businesses. It develops and supplies entertaining game content, gaming machines and gaming systems and services for land-based and iGaming operators. It operates through two segments: Games and Financial Technology Solutions (FinTech). The Games segment provides gaming operators with gaming technology and entertainment products and services, including gaming machines, primarily comprising Class II, Class III and Historic Horse Racing slot machines placed under participation and fixed-fee lease arrangements or sold to casino customers. The FinTech segment provides gaming operators with financial technology products and services, including financial access and related services supporting digital, cashless and physical cash options across mobile, assisted and self-service channels.</v>
     <v>2200</v>
@@ -5329,34 +5293,33 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>7250 S Tenaya Way Ste 100, LAS VEGAS, NV, 89113-2175 US</v>
-    <v>13.19</v>
+    <v>13.18</v>
     <v>Hotels &amp; Entertainment Services</v>
     <v>Stock</v>
-    <v>45569.98723153906</v>
+    <v>45573.958333367969</v>
     <v>36</v>
-    <v>13.14</v>
-    <v>1122005077</v>
+    <v>13.15</v>
+    <v>1131613782</v>
     <v>EVERI HOLDINGS INC.</v>
     <v>EVERI HOLDINGS INC.</v>
-    <v>13.19</v>
+    <v>13.17</v>
     <v>27.9312</v>
     <v>13.15</v>
     <v>13.15</v>
-    <v>13.14</v>
-    <v>85323580</v>
+    <v>86054280</v>
     <v>EVRI</v>
     <v>EVERI HOLDINGS INC. (XNYS:EVRI)</v>
-    <v>756393</v>
-    <v>852168</v>
+    <v>546556</v>
+    <v>845227</v>
     <v>2004</v>
   </rv>
   <rv s="2">
     <v>37</v>
   </rv>
-  <rv s="3">
-    <v>5</v>
+  <rv s="4">
+    <v>9</v>
     <v>NEXTRACKER INC. (XNAS:NXT)</v>
-    <v>6</v>
+    <v>10</v>
     <v>3</v>
     <v>Finance</v>
     <v>4</v>
@@ -5366,12 +5329,10 @@
     <v>1</v>
     <v>Powered by Refinitiv</v>
     <v>62.31</v>
-    <v>32.14</v>
+    <v>32.19</v>
     <v>2.1190000000000002</v>
-    <v>0.23</v>
-    <v>6.3260000000000009E-3</v>
-    <v>0.13</v>
-    <v>3.5530000000000002E-3</v>
+    <v>-0.84</v>
+    <v>-2.3353000000000002E-2</v>
     <v>USD</v>
     <v>Nextracker Inc. is a provider of integrated solar tracker and software solutions used in utility-scale and ground-mounted distributed generation solar projects. Its products enable solar panels in utility-scale power plants to follow the sun’s movement across the sky and optimize plant performance. Its products include NX Horizon, NX Gemini, TrueCapture, and NX Navigator. Its solutions include Bifacial PV modules, Large Format Modules, and First Solar Series 6 (FSLR6) Modules. NX Horizon is a one-in-portrait (1P) smart solar tracker system that delivers the lowest levelized cost of energy (LCOE). NX Gemini is its two-in-portrait (2P) format tracker which holds two rows of solar panels along the central support beam. TrueCapture is its flagship software offering, which is a self-adjusting tracker control system that uses machine learning to enhance solar power plant energy yield. It has operations in the United States, Brazil, Mexico, Spain, India, Australia, the Middle East and Brazil.</v>
     <v>1050</v>
@@ -5379,24 +5340,23 @@
     <v>XNAS</v>
     <v>XNAS</v>
     <v>6200 Paseo Padre Pkwy, FREMONT, CA, 94555 US</v>
-    <v>37.450000000000003</v>
+    <v>35.64</v>
     <v>Renewable Energy</v>
     <v>Stock</v>
-    <v>45569.998900821091</v>
-    <v>36.36</v>
-    <v>5318261366</v>
+    <v>45573.997946955467</v>
+    <v>34.9</v>
+    <v>5106054162</v>
     <v>NEXTRACKER INC.</v>
     <v>NEXTRACKER INC.</v>
-    <v>37.39</v>
-    <v>9.6498000000000008</v>
-    <v>36.36</v>
-    <v>36.590000000000003</v>
-    <v>36.72</v>
+    <v>35.520000000000003</v>
+    <v>9.3233999999999995</v>
+    <v>35.97</v>
+    <v>35.130000000000003</v>
     <v>145347400</v>
     <v>NXT</v>
     <v>NEXTRACKER INC. (XNAS:NXT)</v>
-    <v>1974573</v>
-    <v>3290102</v>
+    <v>356</v>
+    <v>3292096</v>
     <v>2022</v>
   </rv>
   <rv s="2">
@@ -5420,11 +5380,9 @@
     <v>Powered by Refinitiv</v>
     <v>80.22</v>
     <v>56.25</v>
-    <v>1.7453000000000001</v>
-    <v>0.86</v>
-    <v>1.1153999999999999E-2</v>
-    <v>-0.08</v>
-    <v>-1.026E-3</v>
+    <v>1.7467999999999999</v>
+    <v>-0.17</v>
+    <v>-2.2209999999999999E-3</v>
     <v>USD</v>
     <v>Monarch Casino &amp; Resort, Inc. owns and operates the Atlantis Casino Resort Spa, a hotel and casino in Reno, Nevada (the Atlantis) and the Monarch Casino Resort Spa Black Hawk (the Monarch Black Hawk), a hotel and casino in Black Hawk, Colorado. In addition, it owns separate parcels of land located next to the Atlantis and a parcel of land with an industrial warehouse located between Denver, Colorado, and Monarch Black Hawk. The Atlantis is located approximately three miles south of downtown, which features approximately 61,000 square feet of casino space; 817 guest rooms and suites; eight food outlets; two gourmet coffee and pastry bars and one snack bar; a 30,000 square-foot health spa and salon with an enclosed year-round pool. Monarch Black Hawk features approximately 60,000 square feet of casino space; approximately 1,000 slot machines; approximately 43 table games; a live poker room; a keno counter and a sports book. The resort also includes 10 bars and lounges.</v>
     <v>2900</v>
@@ -5432,25 +5390,24 @@
     <v>XNAS</v>
     <v>XNAS</v>
     <v>Executive Offices, 3800 S Virginia Street, RENO, NV, 89502 US</v>
-    <v>77.968999999999994</v>
+    <v>77.209999999999994</v>
     <v>Hotels &amp; Entertainment Services</v>
     <v>Stock</v>
-    <v>45569.888832661716</v>
+    <v>45573.847228356251</v>
     <v>41</v>
-    <v>76.95</v>
-    <v>1438527275</v>
+    <v>76.305000000000007</v>
+    <v>1409372925</v>
     <v>MONARCH CASINO &amp; RESORT, INC.</v>
     <v>MONARCH CASINO &amp; RESORT, INC.</v>
-    <v>77.78</v>
-    <v>18.017600000000002</v>
-    <v>77.099999999999994</v>
-    <v>77.959999999999994</v>
-    <v>77.88</v>
+    <v>76.599999999999994</v>
+    <v>17.849299999999999</v>
+    <v>76.55</v>
+    <v>76.38</v>
     <v>18452120</v>
     <v>MCRI</v>
     <v>MONARCH CASINO &amp; RESORT, INC. (XNAS:MCRI)</v>
-    <v>117758</v>
-    <v>156287</v>
+    <v>86166</v>
+    <v>156947</v>
     <v>1993</v>
   </rv>
   <rv s="2">
@@ -5466,7 +5423,7 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>4</v>
+    <v>8</v>
     <v>en-GB</v>
     <v>a1xqm7</v>
     <v>268435456</v>
@@ -5474,11 +5431,9 @@
     <v>Powered by Refinitiv</v>
     <v>69.75</v>
     <v>34.96</v>
-    <v>0.9647</v>
-    <v>0.15</v>
-    <v>2.4260000000000002E-3</v>
-    <v>0.04</v>
-    <v>6.4530000000000002E-4</v>
+    <v>0.96130000000000004</v>
+    <v>-0.21</v>
+    <v>-3.362E-3</v>
     <v>USD</v>
     <v>Miller Industries, Inc. is a manufacturer of towing and recovery equipment. The Company designs and manufactures bodies of car carriers and wreckers, which are installed on chassis manufactured by third parties, and sold to its customers. Its products are marketed and sold through a network of distributors that serve all 50 states, Canada, Mexico, and other foreign markets, and through prime contractors to governmental entities. In addition to selling its products, its independent distributors provide end-users with parts and service. Its product line includes car carriers, wreckers, and transport trailers. Car carriers are specialized flat-bed vehicles with hydraulic tilt mechanisms that enable a towing operator to drive or winch a vehicle onto the bed for transport. Its multi-vehicle transport trailers are specialized auto transport trailers with upper and lower decks and hydraulic ramps for loading vehicles. Its brands include Century, Vulcan, Chevron, Holmes, and Challenger.</v>
     <v>1821</v>
@@ -5486,25 +5441,24 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>Ste 100, 8503 Hilltop Dr, OOLTEWAH, TN, 37363 US</v>
-    <v>63.13</v>
+    <v>62.29</v>
     <v>Automobiles &amp; Auto Parts</v>
     <v>Stock</v>
-    <v>45569.960431250001</v>
+    <v>45573.958333367969</v>
     <v>44</v>
-    <v>61.52</v>
-    <v>710020442</v>
+    <v>61.02</v>
+    <v>712998427</v>
     <v>MILLER INDUSTRIES, INC.</v>
     <v>MILLER INDUSTRIES, INC.</v>
-    <v>63.13</v>
-    <v>9.9795999999999996</v>
-    <v>61.84</v>
-    <v>61.99</v>
-    <v>62.03</v>
+    <v>62.16</v>
+    <v>10.0214</v>
+    <v>62.46</v>
+    <v>62.25</v>
     <v>11453790</v>
     <v>MLR</v>
     <v>MILLER INDUSTRIES, INC. (XNYS:MLR)</v>
-    <v>68823</v>
-    <v>101679</v>
+    <v>75778</v>
+    <v>92641</v>
     <v>1994</v>
   </rv>
   <rv s="2">
@@ -5529,10 +5483,8 @@
     <v>15.86</v>
     <v>9.1649999999999991</v>
     <v>0.88660000000000005</v>
-    <v>0.18</v>
-    <v>1.873E-2</v>
-    <v>0.02</v>
-    <v>2.0430000000000001E-3</v>
+    <v>0.15</v>
+    <v>1.5290999999999999E-2</v>
     <v>USD</v>
     <v>Janus International Group, Inc. is a global manufacturer and supplier of turn-key self-storage, commercial and industrial building solutions. It operates through two geographic segments: Janus North America and Janus International. The Janus North America segment is comprised of all the other entities, including Janus International Group, LLC, Betco, Inc., Noke, Inc., Asta Industries, Inc., DBCI, LLC, Access Control Technologies, LLC, Janus Door, LLC, and Steel Door Depot.com, LLC. The Janus International segment is comprised of Janus International Europe Holdings Ltd. (UK). Its production and sales are in Europe and Australia. It provides facility and door automation and access control technologies, roll up and swing doors, hallway systems and relocatable storage moveable additional storage structures (MASS) units. It is comprised of three sales channels, including New Construction-Self-storage, R3-Self-storage, and Commercial and Other. It also provides terminal maintenance services.</v>
     <v>1956</v>
@@ -5540,25 +5492,24 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>135 Janus International Blvd., TEMPLE, GA, 30179 US</v>
-    <v>9.8149999999999995</v>
+    <v>10.02</v>
     <v>Homebuilding &amp; Construction Supplies</v>
     <v>Stock</v>
-    <v>45569.958333367969</v>
+    <v>45573.958333356248</v>
     <v>47</v>
-    <v>9.43</v>
-    <v>1396547000</v>
+    <v>9.69</v>
+    <v>1447409112</v>
     <v>JANUS INTERNATIONAL GROUP, INC.</v>
     <v>JANUS INTERNATIONAL GROUP, INC.</v>
-    <v>9.6999999999999993</v>
-    <v>10.9778</v>
-    <v>9.61</v>
-    <v>9.7899999999999991</v>
+    <v>9.82</v>
+    <v>11.1683</v>
     <v>9.81</v>
+    <v>9.9600000000000009</v>
     <v>145322200</v>
     <v>JBI</v>
     <v>JANUS INTERNATIONAL GROUP, INC. (XNYS:JBI)</v>
-    <v>1675210</v>
-    <v>2130654</v>
+    <v>1815743</v>
+    <v>2165648</v>
     <v>2020</v>
   </rv>
   <rv s="2">
@@ -5568,13 +5519,13 @@
     <v>https://www.bing.com/financeapi/forcetrigger?t=a24war&amp;q=XNAS%3aULTA&amp;form=skydnc</v>
     <v>Learn more on Bing</v>
   </rv>
-  <rv s="1">
-    <v>0</v>
+  <rv s="3">
+    <v>5</v>
     <v>ULTA BEAUTY, INC. (XNAS:ULTA)</v>
     <v>2</v>
-    <v>3</v>
+    <v>6</v>
     <v>Finance</v>
-    <v>4</v>
+    <v>7</v>
     <v>en-GB</v>
     <v>a24war</v>
     <v>268435456</v>
@@ -5582,11 +5533,9 @@
     <v>Powered by Refinitiv</v>
     <v>574.76</v>
     <v>318.17</v>
-    <v>1.3221000000000001</v>
-    <v>9.08</v>
-    <v>2.4361000000000001E-2</v>
-    <v>-11.86</v>
-    <v>-3.1063E-2</v>
+    <v>1.3254999999999999</v>
+    <v>-5.49</v>
+    <v>-1.4836999999999999E-2</v>
     <v>USD</v>
     <v>Ulta Beauty, Inc. is a beauty retailer. The Company's product categories include cosmetics, skincare, haircare products and styling tools, fragrance and bath, services, and accessories and other. The Company has one segment, which includes retail stores, salon services, and e-commerce. It offers a range of beauty services in its stores, focusing on hair, makeup, brow and skin services. Its skin services include a skin treatment room or dedicated skin treatment area on the sales floor. Its Ulta Beauty store prototype includes an open salon area, with most of its stores offering brow services on the salon floor. It offers a new way to shop for beauty - bringing together All Things Beauty, All in One Place. In addition to ship to home order fulfillment, it offers guests Buy Online, Pick-up in Store, Curbside Pickup, and Store 2 Door, which provides the ability for customers to order in-store and have products delivered to their homes. It operates over 1,350 retail stores across 50 states.</v>
     <v>20000</v>
@@ -5594,25 +5543,25 @@
     <v>XNAS</v>
     <v>XNAS</v>
     <v>1000 Remington Blvd, Suite 120, BOLINGBROOK, IL, 60440 US</v>
-    <v>384.61</v>
+    <v>371.9</v>
     <v>Specialty Retailers</v>
     <v>Stock</v>
-    <v>45569.998672001566</v>
+    <v>45573.99968850625</v>
     <v>50</v>
-    <v>377.01</v>
-    <v>17988403914</v>
+    <v>364.48</v>
+    <v>17174261379</v>
     <v>ULTA BEAUTY, INC.</v>
     <v>ULTA BEAUTY, INC.</v>
-    <v>380.59</v>
-    <v>15.2249</v>
-    <v>372.72</v>
-    <v>381.8</v>
-    <v>369.94</v>
+    <v>369.41</v>
+    <v>14.6371</v>
+    <v>370.01</v>
+    <v>364.52</v>
+    <v>365</v>
     <v>47114730</v>
     <v>ULTA</v>
     <v>ULTA BEAUTY, INC. (XNAS:ULTA)</v>
-    <v>1158971</v>
-    <v>1427579</v>
+    <v>687</v>
+    <v>1220125</v>
     <v>2016</v>
   </rv>
   <rv s="2">
@@ -5636,11 +5585,9 @@
     <v>Powered by Refinitiv</v>
     <v>31.85</v>
     <v>18.899999999999999</v>
-    <v>1.9713000000000001</v>
-    <v>0.17</v>
-    <v>8.2480000000000001E-3</v>
-    <v>0.04</v>
-    <v>1.9250000000000001E-3</v>
+    <v>1.9723999999999999</v>
+    <v>-0.18</v>
+    <v>-8.8319999999999996E-3</v>
     <v>USD</v>
     <v>International Game Technology PLC is a United Kingdom-based company, which is engaged in gaming. The Company operates and provides an integrated portfolio of gaming technology products and services, including online and instant lottery systems, iLottery, instant ticket printing, lottery management services, commercial services, gaming systems, electronic gaming machines, iGaming, and sports betting. The Company operates through three segments. The Global Lottery segment operates traditional lottery and iLottery businesses across the world, which includes sales, operations, product development, technology, and support, across the world. The Global Gaming segment operates a land-based gaming business across the world, which includes sales, product management, studios, global manufacturing, operation, and technology, across the world. The Digital &amp; Betting segment operates iGaming and sports betting activities across the world.</v>
     <v>11000</v>
@@ -5648,25 +5595,24 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>10 Finsbury Square, Third Floor, LONDON, UNITED KINGDOM-NA, EC2A 1AF GB</v>
-    <v>21.03</v>
+    <v>20.399999999999999</v>
     <v>Hotels &amp; Entertainment Services</v>
     <v>Stock</v>
-    <v>45569.958333356248</v>
+    <v>45573.958333356248</v>
     <v>53</v>
-    <v>20.73</v>
-    <v>4156000000</v>
+    <v>20.100000000000001</v>
+    <v>4040000000</v>
     <v>INTERNATIONAL GAME TECHNOLOGY PLC</v>
     <v>INTERNATIONAL GAME TECHNOLOGY PLC</v>
-    <v>20.98</v>
-    <v>20.104500000000002</v>
-    <v>20.61</v>
-    <v>20.78</v>
-    <v>20.82</v>
+    <v>20.399999999999999</v>
+    <v>19.543500000000002</v>
+    <v>20.38</v>
+    <v>20.2</v>
     <v>200000000</v>
     <v>IGT</v>
     <v>INTERNATIONAL GAME TECHNOLOGY PLC (XNYS:IGT)</v>
-    <v>559848</v>
-    <v>725396</v>
+    <v>568763</v>
+    <v>722184</v>
     <v>2014</v>
   </rv>
   <rv s="2">
@@ -5690,11 +5636,9 @@
     <v>Powered by Refinitiv</v>
     <v>87.32</v>
     <v>54.8</v>
-    <v>0.58860000000000001</v>
-    <v>0.92</v>
-    <v>1.3990000000000001E-2</v>
-    <v>0</v>
-    <v>0</v>
+    <v>0.5917</v>
+    <v>-1.1299999999999999</v>
+    <v>-1.7111000000000001E-2</v>
     <v>USD</v>
     <v>Oil-Dri Corporation of America is a manufacturer and supplier of specialty sorbent products for pet care, animal health and nutrition, fluid purification, agricultural ingredients, sports field, industrial and automotive markets. Its principal product is cat litter. The Company’s Retail and Wholesale Products Group segment customers include mass merchandisers, the farm and fleet channel, drugstore chains, pet specialty retail outlets, dollar stores, retail grocery stores, distributors of industrial cleanup and automotive products, environmental service companies, sports field product users and marketers of consumer products. Its Business to Business Products Group segment customers include processors and refiners of edible oils, renewable diesel, petroleum-based oils and biodiesel fuel; manufacturers of animal feed and agricultural chemicals; and distributors of animal health and nutrition products. It is also a supplier of silica gel-based crystal cat litter.</v>
     <v>884</v>
@@ -5702,25 +5646,24 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>SUITE 400, 410 NORTH MICHIGAN AVENUE, CHICAGO, IL, 60611 US</v>
-    <v>66.959999999999994</v>
+    <v>65.75</v>
     <v>Chemicals</v>
     <v>Stock</v>
-    <v>45569.958333344533</v>
+    <v>45573.958333356248</v>
     <v>56</v>
-    <v>66.25</v>
-    <v>479148600</v>
+    <v>64.290000000000006</v>
+    <v>481188800</v>
     <v>OIL-DRI CORPORATION OF AMERICA</v>
     <v>OIL-DRI CORPORATION OF AMERICA</v>
-    <v>66.75</v>
-    <v>13.6836</v>
-    <v>65.760000000000005</v>
-    <v>66.680000000000007</v>
-    <v>66.680000000000007</v>
+    <v>65.75</v>
+    <v>13.3203</v>
+    <v>66.040000000000006</v>
+    <v>64.91</v>
     <v>7286320</v>
     <v>ODC</v>
     <v>OIL-DRI CORPORATION OF AMERICA (XNYS:ODC)</v>
-    <v>14802</v>
-    <v>16359</v>
+    <v>10495</v>
+    <v>16196</v>
     <v>1969</v>
   </rv>
   <rv s="2">
@@ -5730,13 +5673,13 @@
     <v>https://www.bing.com/financeapi/forcetrigger?t=a1mt9c&amp;q=XNAS%3aACLS&amp;form=skydnc</v>
     <v>Learn more on Bing</v>
   </rv>
-  <rv s="1">
-    <v>0</v>
+  <rv s="3">
+    <v>5</v>
     <v>AXCELIS TECHNOLOGIES, INC. (XNAS:ACLS)</v>
     <v>2</v>
-    <v>3</v>
+    <v>6</v>
     <v>Finance</v>
-    <v>4</v>
+    <v>7</v>
     <v>en-GB</v>
     <v>a1mt9c</v>
     <v>268435456</v>
@@ -5744,11 +5687,9 @@
     <v>Powered by Refinitiv</v>
     <v>170.9692</v>
     <v>93.77</v>
-    <v>1.5775999999999999</v>
-    <v>0.67</v>
-    <v>6.7259999999999993E-3</v>
-    <v>0.22</v>
-    <v>2.1940000000000002E-3</v>
+    <v>1.5809</v>
+    <v>-0.44</v>
+    <v>-4.4469999999999996E-3</v>
     <v>USD</v>
     <v>Axcelis Technologies, Inc. designs, manufactures and services ion implantation and other processing equipment used in the fabrication of semiconductor chips. The Company offers a complete line of high energy, high current and medium current implanters for all application requirements. In addition to equipment, the Company provides extensive aftermarket lifecycle products and services, including used tools, spare parts, equipment upgrades, maintenance services and customer training. Its Purion flagship systems are all based on a common platform, which enables a combination of implant purity, precision and productivity. Combining a single wafer end station, with advanced spot beam architectures (that ensures all points across the wafer see the same beam condition at the same beam angle), Purion products enable process control to optimize device performance and yield, at high productivity. The Company sells its products to semiconductor chip manufacturers around the world.</v>
     <v>1620</v>
@@ -5756,25 +5697,25 @@
     <v>XNAS</v>
     <v>XNAS</v>
     <v>108 Cherry Hill Dr, BEVERLY, MA, 01915 US</v>
-    <v>102.54</v>
+    <v>98.95</v>
     <v>Semiconductors &amp; Semiconductor Equipment</v>
     <v>Stock</v>
-    <v>45569.976284375</v>
+    <v>45573.996179582813</v>
     <v>59</v>
-    <v>100.17</v>
-    <v>3270891925</v>
+    <v>96.72</v>
+    <v>3212832615</v>
     <v>AXCELIS TECHNOLOGIES, INC.</v>
     <v>AXCELIS TECHNOLOGIES, INC.</v>
-    <v>102.17</v>
-    <v>13.7235</v>
-    <v>99.61</v>
-    <v>100.28</v>
-    <v>100.5</v>
+    <v>98.95</v>
+    <v>13.570499999999999</v>
+    <v>98.94</v>
+    <v>98.5</v>
+    <v>99</v>
     <v>32617590</v>
     <v>ACLS</v>
     <v>AXCELIS TECHNOLOGIES, INC. (XNAS:ACLS)</v>
-    <v>448826</v>
-    <v>655003</v>
+    <v>368</v>
+    <v>658199</v>
     <v>1995</v>
   </rv>
   <rv s="2">
@@ -5784,13 +5725,13 @@
     <v>https://www.bing.com/financeapi/forcetrigger?t=a1retc&amp;q=XNYS%3aDELL&amp;form=skydnc</v>
     <v>Learn more on Bing</v>
   </rv>
-  <rv s="1">
-    <v>0</v>
+  <rv s="3">
+    <v>5</v>
     <v>DELL TECHNOLOGIES INC. (XNYS:DELL)</v>
     <v>2</v>
-    <v>3</v>
+    <v>6</v>
     <v>Finance</v>
-    <v>4</v>
+    <v>7</v>
     <v>en-GB</v>
     <v>a1retc</v>
     <v>268435456</v>
@@ -5798,11 +5739,9 @@
     <v>Powered by Refinitiv</v>
     <v>179.7</v>
     <v>63.9</v>
-    <v>0.89510000000000001</v>
-    <v>4.75</v>
-    <v>4.1064999999999997E-2</v>
-    <v>-0.02</v>
-    <v>-1.661E-4</v>
+    <v>0.89549999999999996</v>
+    <v>2.84</v>
+    <v>2.3847999999999998E-2</v>
     <v>USD</v>
     <v>Dell Technologies Inc. is engaged in designing, developing, manufacturing, marketing, selling, and supporting a wide range of comprehensive and integrated solutions, products, and services. The Company operates through two segments: Infrastructure Solutions Group (ISG) and Client Solutions Group (CSG). Its ISG segment enables the Company’s customer’s digital transformation with solutions that address artificial intelligence (AI), machine learning, data analytics, and multi cloud environments. Its comprehensive storage portfolio includes modern and traditional storage solutions, including all-flash arrays, scale-out file, object platforms, hyper-converged infrastructure, and software-defined storage. Its CSG segment offers branded personal computers (PCs) including notebooks, desktops, and workstations and branded peripherals that include displays, docking stations, keyboards, mice, and webcam and audio devices, as well as third-party software and peripherals.</v>
     <v>120000</v>
@@ -5810,25 +5749,25 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>ONE DELL WAY, ROUND ROCK, TX, 78682 US</v>
-    <v>120.84</v>
+    <v>121.94</v>
     <v>Computers, Phones &amp; Household Electronics</v>
     <v>Stock</v>
-    <v>45569.999740462503</v>
+    <v>45573.999278923438</v>
     <v>62</v>
-    <v>117.06010000000001</v>
-    <v>84534418530</v>
+    <v>118.7</v>
+    <v>85594433245</v>
     <v>DELL TECHNOLOGIES INC.</v>
     <v>DELL TECHNOLOGIES INC.</v>
-    <v>117.5</v>
-    <v>22.157599999999999</v>
-    <v>115.67</v>
-    <v>120.42</v>
-    <v>120.4</v>
+    <v>119.4</v>
+    <v>22.435400000000001</v>
+    <v>119.09</v>
+    <v>121.93</v>
+    <v>122.1</v>
     <v>701996500</v>
     <v>DELL</v>
     <v>DELL TECHNOLOGIES INC. (XNYS:DELL)</v>
-    <v>8185053</v>
-    <v>14094510</v>
+    <v>8278</v>
+    <v>13468448</v>
     <v>2013</v>
   </rv>
   <rv s="2">
@@ -5838,25 +5777,23 @@
     <v>https://www.bing.com/financeapi/forcetrigger?t=a1zqnm&amp;q=XNYS%3aPFE&amp;form=skydnc</v>
     <v>Learn more on Bing</v>
   </rv>
-  <rv s="4">
-    <v>7</v>
+  <rv s="5">
+    <v>11</v>
     <v>PFIZER INC. (XNYS:PFE)</v>
     <v>2</v>
+    <v>12</v>
+    <v>Finance</v>
     <v>8</v>
-    <v>Finance</v>
-    <v>4</v>
     <v>en-GB</v>
     <v>a1zqnm</v>
     <v>268435456</v>
     <v>1</v>
     <v>Powered by Refinitiv</v>
-    <v>34.079900000000002</v>
+    <v>33.92</v>
     <v>25.2</v>
-    <v>0.6492</v>
-    <v>0.24</v>
-    <v>8.4689999999999991E-3</v>
-    <v>0.05</v>
-    <v>1.7489999999999999E-3</v>
+    <v>0.64529999999999998</v>
+    <v>-0.02</v>
+    <v>-6.8490000000000001E-4</v>
     <v>USD</v>
     <v>Pfizer Inc. is a research-based global biopharmaceutical company. The Company is engaged in the discovery, development, manufacture, marketing, sale and distribution of biopharmaceutical products worldwide. Its Biopharma segment is engaged in the science-based biopharmaceutical business. Its Biopharma segment includes the Pfizer Oncology Division, the Pfizer U.S. Commercial Division, and the Pfizer International Commercial Division. Its product categories include oncology, primary care and specialty care. Its Oncology products include Ibrance, Xtandi, Inlyta, Bosulif, Lorbrena, Braftovi, Mektovi, Padcev, Adcetris, Talzenna, Tukysa, Elrexfio and Tivdak. Its primary care products include Eliquis, Nurtec ODT/Vydura, Comirnaty, the Prevnar family, Abrysvo, FSME/IMMUN-TicoVac, Paxlovid and Lucira by Pfizer. Its specialty care products include Xeljanz, Enbrel (outside the U.S. and Canada), Inflectra, Cibinqo, Litfulo, Vyndaqel family, Genotropin, Sulperazon, Zavicefta, Medrol and Panzyga.</v>
     <v>88000</v>
@@ -5864,24 +5801,23 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>66 HUDSON BOULEVARD EAST, NEW YORK, NY, 10001-2192 US</v>
-    <v>28.59</v>
+    <v>29.49</v>
     <v>Pharmaceuticals</v>
     <v>Stock</v>
-    <v>45569.999953645311</v>
+    <v>45573.999500439066</v>
     <v>65</v>
-    <v>28.24</v>
-    <v>161954143100</v>
+    <v>29</v>
+    <v>165354160100</v>
     <v>PFIZER INC.</v>
     <v>PFIZER INC.</v>
-    <v>28.29</v>
-    <v>28.34</v>
-    <v>28.58</v>
-    <v>28.63</v>
+    <v>29.21</v>
+    <v>29.2</v>
+    <v>29.18</v>
     <v>5666695000</v>
     <v>PFE</v>
     <v>PFIZER INC. (XNYS:PFE)</v>
-    <v>28786884</v>
-    <v>29519892</v>
+    <v>27485</v>
+    <v>29902174</v>
     <v>1942</v>
   </rv>
   <rv s="2">
@@ -5905,11 +5841,9 @@
     <v>Powered by Refinitiv</v>
     <v>30.32</v>
     <v>18.945</v>
-    <v>1.4095</v>
-    <v>0.33</v>
-    <v>1.6863E-2</v>
-    <v>0.05</v>
-    <v>2.513E-3</v>
+    <v>1.4094</v>
+    <v>-0.23</v>
+    <v>-1.1747E-2</v>
     <v>USD</v>
     <v>Franklin Resources, Inc. is a global investment management company with subsidiaries operating as Franklin Templeton and serving clients in over 150 countries. It offers specialization on a global scale, bringing capabilities in fixed income, equity, alternatives and multi-asset solutions. The Company provides its investment management and related services to retail, institutional and high-net-worth investors in jurisdictions worldwide. Its investment products include sponsored funds, as well as institutional and high-net-worth separate accounts, retail separately managed account programs, sub-advised products, and other investment vehicles. Its funds include registered funds (including exchange-traded funds or ETFs) and unregistered funds. The Company offers its services and products under its various brand names, including Alcentra, K2, Benefit Street Partners, ClearBridge Investments, Martin Currie, O’Shaughnessy, and Lexington Partners. It also focuses on the retirement sector.</v>
     <v>10300</v>
@@ -5917,25 +5851,24 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>One Franklin Parkway, Building 920/2, SAN MATEO, CA, 94403 US</v>
-    <v>19.93</v>
+    <v>19.64</v>
     <v>Investment Banking &amp; Investment Services</v>
     <v>Stock</v>
-    <v>45569.991273760941</v>
+    <v>45573.990230497657</v>
     <v>68</v>
-    <v>19.510100000000001</v>
-    <v>10407668160</v>
+    <v>19.28</v>
+    <v>10120019040</v>
     <v>FRANKLIN RESOURCES, INC.</v>
     <v>FRANKLIN RESOURCES, INC.</v>
-    <v>19.8</v>
-    <v>12.4274</v>
-    <v>19.57</v>
-    <v>19.899999999999999</v>
-    <v>19.95</v>
+    <v>19.579999999999998</v>
+    <v>12.083600000000001</v>
+    <v>19.579999999999998</v>
+    <v>19.350000000000001</v>
     <v>522998400</v>
     <v>BEN</v>
     <v>FRANKLIN RESOURCES, INC. (XNYS:BEN)</v>
-    <v>3169543</v>
-    <v>4647003</v>
+    <v>5</v>
+    <v>4544327</v>
     <v>1969</v>
   </rv>
   <rv s="2">
@@ -5959,11 +5892,9 @@
     <v>Powered by Refinitiv</v>
     <v>26.15</v>
     <v>20.190000000000001</v>
-    <v>1.1473</v>
-    <v>-0.01</v>
-    <v>-4.1369999999999997E-4</v>
-    <v>0.09</v>
-    <v>3.725E-3</v>
+    <v>1.1484000000000001</v>
+    <v>-0.05</v>
+    <v>-2.0999999999999999E-3</v>
     <v>USD</v>
     <v>UGI Corporation is a holding company, which distributes, stores, transports and markets energy products and related services. In the United States, the Company owns and operates a retail propane marketing and distribution business, natural gas and electric distribution utilities, and energy marketing, midstream infrastructure, storage, natural gas gathering and processing, natural gas production, electricity generation and energy services businesses. In Europe, the Company markets and distributes propane and other liquified petroleum gas (LPG), and market other energy products and services. It operates through four segments: AmeriGas Propane, UGI International, Midstream &amp; Marketing, and Utilities. The AmeriGas Propane segment operates propane distribution business. The UGI International segment consists of LPG distribution businesses in Austria, Belgium, the Czech Republic, Denmark, Finland, France, Hungary, Italy, Luxembourg, the Netherlands, Norway, Poland, Romania and others.</v>
     <v>5160</v>
@@ -5971,25 +5902,24 @@
     <v>XNYS</v>
     <v>XNYS</v>
     <v>500 N GULPH RD, P O BOX 858, KING OF PRUSSIA, PA, 19406 US</v>
-    <v>24.36</v>
+    <v>24.0166</v>
     <v>Natural Gas Utilities</v>
     <v>Stock</v>
-    <v>45569.971942198441</v>
+    <v>45573.958333344533</v>
     <v>71</v>
-    <v>24.01</v>
-    <v>5186876576</v>
+    <v>23.68</v>
+    <v>5101001136</v>
     <v>UGI CORPORATION</v>
     <v>UGI CORPORATION</v>
-    <v>24.17</v>
-    <v>7.6920999999999999</v>
-    <v>24.17</v>
-    <v>24.16</v>
-    <v>24.25</v>
+    <v>23.78</v>
+    <v>7.5646000000000004</v>
+    <v>23.81</v>
+    <v>23.76</v>
     <v>214688600</v>
     <v>UGI</v>
     <v>UGI CORPORATION (XNYS:UGI)</v>
-    <v>1047760</v>
-    <v>2083774</v>
+    <v>31</v>
+    <v>2084262</v>
     <v>1991</v>
   </rv>
   <rv s="2">
@@ -5999,7 +5929,7 @@
 </file>
 
 <file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
-<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="5">
+<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="6">
   <s t="_hyperlink">
     <k n="Address" t="s"/>
     <k n="Text" t="s"/>
@@ -6021,8 +5951,6 @@
     <k n="Beta"/>
     <k n="Change"/>
     <k n="Change (%)"/>
-    <k n="Change (Extended hours)"/>
-    <k n="Change % (Extended hours)"/>
     <k n="Currency" t="s"/>
     <k n="Description" t="s"/>
     <k n="Employees"/>
@@ -6043,7 +5971,6 @@
     <k n="P/E"/>
     <k n="Previous close"/>
     <k n="Price"/>
-    <k n="Price (Extended hours)"/>
     <k n="Shares outstanding"/>
     <k n="Ticker symbol" t="s"/>
     <k n="UniqueName" t="s"/>
@@ -6071,8 +5998,6 @@
     <k n="Beta"/>
     <k n="Change"/>
     <k n="Change (%)"/>
-    <k n="Change (Extended hours)"/>
-    <k n="Change % (Extended hours)"/>
     <k n="Currency" t="s"/>
     <k n="Description" t="s"/>
     <k n="Employees"/>
@@ -6084,6 +6009,7 @@
     <k n="Industry" t="s"/>
     <k n="Instrument type" t="s"/>
     <k n="Last trade time"/>
+    <k n="LearnMoreOnLink" t="r"/>
     <k n="Low"/>
     <k n="Market cap"/>
     <k n="Name" t="s"/>
@@ -6117,8 +6043,49 @@
     <k n="Beta"/>
     <k n="Change"/>
     <k n="Change (%)"/>
-    <k n="Change (Extended hours)"/>
-    <k n="Change % (Extended hours)"/>
+    <k n="Currency" t="s"/>
+    <k n="Description" t="s"/>
+    <k n="Employees"/>
+    <k n="Exchange" t="s"/>
+    <k n="Exchange abbreviation" t="s"/>
+    <k n="ExchangeID" t="s"/>
+    <k n="Headquarters" t="s"/>
+    <k n="High"/>
+    <k n="Industry" t="s"/>
+    <k n="Instrument type" t="s"/>
+    <k n="Last trade time"/>
+    <k n="Low"/>
+    <k n="Market cap"/>
+    <k n="Name" t="s"/>
+    <k n="Official name" t="s"/>
+    <k n="Open"/>
+    <k n="P/E"/>
+    <k n="Previous close"/>
+    <k n="Price"/>
+    <k n="Shares outstanding"/>
+    <k n="Ticker symbol" t="s"/>
+    <k n="UniqueName" t="s"/>
+    <k n="Volume"/>
+    <k n="Volume average"/>
+    <k n="Year incorporated"/>
+  </s>
+  <s t="_linkedentitycore">
+    <k n="_Display" t="spb"/>
+    <k n="_DisplayString" t="s"/>
+    <k n="_Flags" t="spb"/>
+    <k n="_Format" t="spb"/>
+    <k n="_Icon" t="s"/>
+    <k n="_SubLabel" t="spb"/>
+    <k n="%EntityCulture" t="s"/>
+    <k n="%EntityId" t="s"/>
+    <k n="%EntityServiceId"/>
+    <k n="%IsRefreshable" t="b"/>
+    <k n="%ProviderInfo" t="s"/>
+    <k n="52 week high"/>
+    <k n="52 week low"/>
+    <k n="Beta"/>
+    <k n="Change"/>
+    <k n="Change (%)"/>
     <k n="Currency" t="s"/>
     <k n="Description" t="s"/>
     <k n="Employees"/>
@@ -6138,7 +6105,6 @@
     <k n="Open"/>
     <k n="Previous close"/>
     <k n="Price"/>
-    <k n="Price (Extended hours)"/>
     <k n="Shares outstanding"/>
     <k n="Ticker symbol" t="s"/>
     <k n="UniqueName" t="s"/>
@@ -6151,8 +6117,8 @@
 
 <file path=xl/richData/rdsupportingpropertybag.xml><?xml version="1.0" encoding="utf-8"?>
 <supportingPropertyBags xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2">
-  <spbArrays count="3">
-    <a count="45">
+  <spbArrays count="4">
+    <a count="42">
       <v t="s">%EntityServiceId</v>
       <v t="s">_Format</v>
       <v t="s">%IsRefreshable</v>
@@ -6163,16 +6129,13 @@
       <v t="s">Name</v>
       <v t="s">_SubLabel</v>
       <v t="s">Price</v>
-      <v t="s">Price (Extended hours)</v>
       <v t="s">Exchange</v>
       <v t="s">Official name</v>
       <v t="s">Last trade time</v>
       <v t="s">Ticker symbol</v>
       <v t="s">Exchange abbreviation</v>
       <v t="s">Change</v>
-      <v t="s">Change (Extended hours)</v>
       <v t="s">Change (%)</v>
-      <v t="s">Change % (Extended hours)</v>
       <v t="s">Currency</v>
       <v t="s">Previous close</v>
       <v t="s">Open</v>
@@ -6199,7 +6162,7 @@
       <v t="s">ExchangeID</v>
       <v t="s">%ProviderInfo</v>
     </a>
-    <a count="44">
+    <a count="43">
       <v t="s">%EntityServiceId</v>
       <v t="s">_Format</v>
       <v t="s">%IsRefreshable</v>
@@ -6217,9 +6180,51 @@
       <v t="s">Ticker symbol</v>
       <v t="s">Exchange abbreviation</v>
       <v t="s">Change</v>
-      <v t="s">Change (Extended hours)</v>
       <v t="s">Change (%)</v>
-      <v t="s">Change % (Extended hours)</v>
+      <v t="s">Currency</v>
+      <v t="s">Previous close</v>
+      <v t="s">Open</v>
+      <v t="s">High</v>
+      <v t="s">Low</v>
+      <v t="s">52 week high</v>
+      <v t="s">52 week low</v>
+      <v t="s">Volume</v>
+      <v t="s">Volume average</v>
+      <v t="s">Market cap</v>
+      <v t="s">Beta</v>
+      <v t="s">P/E</v>
+      <v t="s">Shares outstanding</v>
+      <v t="s">Description</v>
+      <v t="s">Employees</v>
+      <v t="s">Headquarters</v>
+      <v t="s">Industry</v>
+      <v t="s">Instrument type</v>
+      <v t="s">Year incorporated</v>
+      <v t="s">_Flags</v>
+      <v t="s">UniqueName</v>
+      <v t="s">_DisplayString</v>
+      <v t="s">LearnMoreOnLink</v>
+      <v t="s">ExchangeID</v>
+      <v t="s">%ProviderInfo</v>
+    </a>
+    <a count="41">
+      <v t="s">%EntityServiceId</v>
+      <v t="s">_Format</v>
+      <v t="s">%IsRefreshable</v>
+      <v t="s">%EntityCulture</v>
+      <v t="s">%EntityId</v>
+      <v t="s">_Icon</v>
+      <v t="s">_Display</v>
+      <v t="s">Name</v>
+      <v t="s">_SubLabel</v>
+      <v t="s">Price</v>
+      <v t="s">Exchange</v>
+      <v t="s">Official name</v>
+      <v t="s">Last trade time</v>
+      <v t="s">Ticker symbol</v>
+      <v t="s">Exchange abbreviation</v>
+      <v t="s">Change</v>
+      <v t="s">Change (%)</v>
       <v t="s">Currency</v>
       <v t="s">Previous close</v>
       <v t="s">Open</v>
@@ -6245,7 +6250,7 @@
       <v t="s">ExchangeID</v>
       <v t="s">%ProviderInfo</v>
     </a>
-    <a count="44">
+    <a count="41">
       <v t="s">%EntityServiceId</v>
       <v t="s">_Format</v>
       <v t="s">%IsRefreshable</v>
@@ -6256,16 +6261,13 @@
       <v t="s">Name</v>
       <v t="s">_SubLabel</v>
       <v t="s">Price</v>
-      <v t="s">Price (Extended hours)</v>
       <v t="s">Exchange</v>
       <v t="s">Official name</v>
       <v t="s">Last trade time</v>
       <v t="s">Ticker symbol</v>
       <v t="s">Exchange abbreviation</v>
       <v t="s">Change</v>
-      <v t="s">Change (Extended hours)</v>
       <v t="s">Change (%)</v>
-      <v t="s">Change % (Extended hours)</v>
       <v t="s">Currency</v>
       <v t="s">Previous close</v>
       <v t="s">Open</v>
@@ -6292,7 +6294,7 @@
       <v t="s">%ProviderInfo</v>
     </a>
   </spbArrays>
-  <spbData count="9">
+  <spbData count="13">
     <spb s="0">
       <v>0</v>
       <v>Name</v>
@@ -6330,35 +6332,72 @@
       <v>8</v>
       <v>9</v>
       <v>4</v>
+    </spb>
+    <spb s="4">
+      <v>Delayed 15 minutes</v>
+      <v>from previous close</v>
+      <v>from previous close</v>
+      <v>Source: Nasdaq</v>
+      <v>GMT</v>
+    </spb>
+    <spb s="0">
+      <v>1</v>
+      <v>Name</v>
+      <v>LearnMoreOnLink</v>
+    </spb>
+    <spb s="5">
+      <v>1</v>
+      <v>2</v>
+      <v>2</v>
+      <v>1</v>
+      <v>3</v>
       <v>1</v>
       <v>1</v>
+      <v>1</v>
+      <v>4</v>
+      <v>4</v>
       <v>5</v>
+      <v>6</v>
+      <v>1</v>
+      <v>1</v>
+      <v>1</v>
+      <v>4</v>
+      <v>7</v>
+      <v>8</v>
+      <v>9</v>
+      <v>4</v>
+      <v>1</v>
     </spb>
-    <spb s="4">
+    <spb s="6">
       <v>at close</v>
       <v>from previous close</v>
       <v>from previous close</v>
       <v>Source: Nasdaq</v>
       <v>GMT</v>
       <v>Delayed 15 minutes</v>
-      <v>from close</v>
-      <v>from close</v>
     </spb>
-    <spb s="5">
-      <v>1</v>
+    <spb s="4">
+      <v>Real-Time Nasdaq Last Sale</v>
+      <v>from previous close</v>
+      <v>from previous close</v>
+      <v>Source: Nasdaq Last Sale</v>
+      <v>GMT</v>
+    </spb>
+    <spb s="7">
+      <v>2</v>
       <v>Name</v>
     </spb>
-    <spb s="6">
+    <spb s="8">
       <v>1</v>
       <v>1</v>
       <v>1</v>
     </spb>
     <spb s="0">
-      <v>2</v>
+      <v>3</v>
       <v>Name</v>
       <v>LearnMoreOnLink</v>
     </spb>
-    <spb s="7">
+    <spb s="9">
       <v>1</v>
       <v>2</v>
       <v>1</v>
@@ -6378,16 +6417,13 @@
       <v>8</v>
       <v>9</v>
       <v>4</v>
-      <v>1</v>
-      <v>1</v>
-      <v>5</v>
     </spb>
   </spbData>
 </supportingPropertyBags>
 </file>
 
 <file path=xl/richData/rdsupportingpropertybagstructure.xml><?xml version="1.0" encoding="utf-8"?>
-<spbStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" count="8">
+<spbStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" count="10">
   <s>
     <k n="^Order" t="spba"/>
     <k n="TitleProperty" t="s"/>
@@ -6425,9 +6461,36 @@
     <k n="Year incorporated" t="i"/>
     <k n="`%EntityServiceId" t="i"/>
     <k n="Shares outstanding" t="i"/>
+  </s>
+  <s>
+    <k n="Price" t="s"/>
+    <k n="Change" t="s"/>
+    <k n="Change (%)" t="s"/>
+    <k n="ExchangeID" t="s"/>
+    <k n="Last trade time" t="s"/>
+  </s>
+  <s>
+    <k n="Low" t="i"/>
+    <k n="P/E" t="i"/>
+    <k n="Beta" t="i"/>
+    <k n="High" t="i"/>
+    <k n="Name" t="i"/>
+    <k n="Open" t="i"/>
+    <k n="Price" t="i"/>
+    <k n="Change" t="i"/>
+    <k n="Volume" t="i"/>
+    <k n="Employees" t="i"/>
+    <k n="Change (%)" t="i"/>
+    <k n="Market cap" t="i"/>
+    <k n="52 week low" t="i"/>
+    <k n="52 week high" t="i"/>
+    <k n="Previous close" t="i"/>
+    <k n="Volume average" t="i"/>
+    <k n="Last trade time" t="i"/>
+    <k n="Year incorporated" t="i"/>
+    <k n="`%EntityServiceId" t="i"/>
+    <k n="Shares outstanding" t="i"/>
     <k n="Price (Extended hours)" t="i"/>
-    <k n="Change (Extended hours)" t="i"/>
-    <k n="Change % (Extended hours)" t="i"/>
   </s>
   <s>
     <k n="Price" t="s"/>
@@ -6436,8 +6499,6 @@
     <k n="ExchangeID" t="s"/>
     <k n="Last trade time" t="s"/>
     <k n="Price (Extended hours)" t="s"/>
-    <k n="Change (Extended hours)" t="s"/>
-    <k n="Change % (Extended hours)" t="s"/>
   </s>
   <s>
     <k n="^Order" t="spba"/>
@@ -6468,9 +6529,6 @@
     <k n="Year incorporated" t="i"/>
     <k n="`%EntityServiceId" t="i"/>
     <k n="Shares outstanding" t="i"/>
-    <k n="Price (Extended hours)" t="i"/>
-    <k n="Change (Extended hours)" t="i"/>
-    <k n="Change % (Extended hours)" t="i"/>
   </s>
 </spbStructures>
 </file>
@@ -69322,7 +69380,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{960A98AA-C170-FD4F-A0A4-3255EEA67EE9}">
   <dimension ref="A1:M17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
@@ -69849,10 +69907,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC8E6AFA-7BB7-D247-9FD7-C44546468350}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -69887,8 +69945,46 @@
         <v>168</v>
       </c>
     </row>
+    <row r="3" spans="1:6">
+      <c r="B3" s="225">
+        <v>45574</v>
+      </c>
+      <c r="C3" s="224" t="s">
+        <v>166</v>
+      </c>
+      <c r="D3" s="226">
+        <v>10120</v>
+      </c>
+      <c r="E3" s="224" t="s">
+        <v>167</v>
+      </c>
+      <c r="F3" s="224" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="D4" s="226"/>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="D5" s="226"/>
+    </row>
     <row r="6" spans="1:6">
-      <c r="D6" s="224"/>
+      <c r="D6" s="226"/>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="D7" s="226"/>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="D8" s="226"/>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="D9" s="226"/>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="D10" s="226"/>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="D11" s="226"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -69984,15 +70080,15 @@
       </c>
       <c r="I3" s="149" cm="1">
         <f t="array" aca="1" ref="I3" ca="1">_FV(B3,"Price")</f>
-        <v>64.59</v>
+        <v>65.900000000000006</v>
       </c>
       <c r="J3" s="129">
         <f t="shared" ref="J3:J27" ca="1" si="0">((I3-F3)/F3)</f>
-        <v>-6.050909090909086E-2</v>
+        <v>-4.1454545454545369E-2</v>
       </c>
       <c r="K3" s="170">
         <f t="shared" ref="K3:K27" ca="1" si="1">(I3*G3) - H3</f>
-        <v>-30.345587999999964</v>
+        <v>-20.799879999999916</v>
       </c>
       <c r="L3"/>
     </row>
@@ -70023,15 +70119,15 @@
       </c>
       <c r="I4" s="149" cm="1">
         <f t="array" aca="1" ref="I4" ca="1">_FV(B4,"Price")</f>
-        <v>141.93</v>
+        <v>135.61000000000001</v>
       </c>
       <c r="J4" s="129">
         <f t="shared" ca="1" si="0"/>
-        <v>0.419016196760648</v>
+        <v>0.35582883423315353</v>
       </c>
       <c r="K4" s="170">
         <f t="shared" ca="1" si="1"/>
-        <v>209.92737000000011</v>
+        <v>178.27049000000011</v>
       </c>
       <c r="L4"/>
     </row>
@@ -70062,15 +70158,15 @@
       </c>
       <c r="I5" s="149" cm="1">
         <f t="array" aca="1" ref="I5" ca="1">_FV(B5,"Price")</f>
-        <v>18.13</v>
+        <v>18.239999999999998</v>
       </c>
       <c r="J5" s="129">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.16834862385321109</v>
+        <v>-0.16330275229357807</v>
       </c>
       <c r="K5" s="170">
         <f t="shared" ca="1" si="1"/>
-        <v>-84.387104000000022</v>
+        <v>-81.859392000000071</v>
       </c>
       <c r="L5"/>
     </row>
@@ -70101,15 +70197,15 @@
       </c>
       <c r="I6" s="149" cm="1">
         <f t="array" aca="1" ref="I6" ca="1">_FV(B6,"Price")</f>
-        <v>21.58</v>
+        <v>21.25</v>
       </c>
       <c r="J6" s="129">
         <f t="shared" ca="1" si="0"/>
-        <v>0.23314285714285704</v>
+        <v>0.21428571428571427</v>
       </c>
       <c r="K6" s="170">
         <f t="shared" ca="1" si="1"/>
-        <v>130.3531119999999</v>
+        <v>120.69849999999997</v>
       </c>
       <c r="L6"/>
     </row>
@@ -70140,15 +70236,15 @@
       </c>
       <c r="I7" s="151" cm="1">
         <f t="array" aca="1" ref="I7" ca="1">_FV(B7,"Price")</f>
-        <v>226.8</v>
+        <v>225.77</v>
       </c>
       <c r="J7" s="129">
         <f t="shared" ca="1" si="0"/>
-        <v>0.28527711662699762</v>
+        <v>0.27944009973931772</v>
       </c>
       <c r="K7" s="170">
         <f t="shared" ca="1" si="1"/>
-        <v>142.92788000000007</v>
+        <v>140.0036070000001</v>
       </c>
       <c r="L7"/>
     </row>
@@ -70179,15 +70275,15 @@
       </c>
       <c r="I8" s="151" cm="1">
         <f t="array" aca="1" ref="I8" ca="1">_FV(B8,"Price")</f>
-        <v>99.05</v>
+        <v>97.82</v>
       </c>
       <c r="J8" s="129">
         <f t="shared" ca="1" si="0"/>
-        <v>0.76433915211970072</v>
+        <v>0.74242964018525104</v>
       </c>
       <c r="K8" s="170">
         <f t="shared" ca="1" si="1"/>
-        <v>382.86277000000007</v>
+        <v>371.88698799999997</v>
       </c>
       <c r="L8"/>
     </row>
@@ -70218,15 +70314,15 @@
       </c>
       <c r="I9" s="151" cm="1">
         <f t="array" aca="1" ref="I9" ca="1">_FV(B9,"Price")</f>
-        <v>18.97</v>
+        <v>17.62</v>
       </c>
       <c r="J9" s="129">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.43508040500297795</v>
+        <v>-0.47528290649195942</v>
       </c>
       <c r="K9" s="170">
         <f t="shared" ca="1" si="1"/>
-        <v>-217.95052700000002</v>
+        <v>-238.09374200000002</v>
       </c>
       <c r="L9"/>
     </row>
@@ -70257,15 +70353,15 @@
       </c>
       <c r="I10" s="153" cm="1">
         <f t="array" aca="1" ref="I10" ca="1">_FV(B10,"Price")</f>
-        <v>65.72</v>
+        <v>65.180000000000007</v>
       </c>
       <c r="J10" s="129">
         <f t="shared" ca="1" si="0"/>
-        <v>0.12920962199312708</v>
+        <v>0.11993127147766329</v>
       </c>
       <c r="K10" s="170">
         <f t="shared" ca="1" si="1"/>
-        <v>64.757191999999918</v>
+        <v>60.108548000000042</v>
       </c>
       <c r="L10"/>
     </row>
@@ -70296,15 +70392,15 @@
       </c>
       <c r="I11" s="153" cm="1">
         <f t="array" aca="1" ref="I11" ca="1">_FV(B11,"Price")</f>
-        <v>82.25</v>
+        <v>79.180000000000007</v>
       </c>
       <c r="J11" s="129">
         <f t="shared" ca="1" si="0"/>
-        <v>-9.8827654212775243E-2</v>
+        <v>-0.13246411745370867</v>
       </c>
       <c r="K11" s="170">
         <f t="shared" ca="1" si="1"/>
-        <v>-49.529750000000035</v>
+        <v>-66.380979999999965</v>
       </c>
       <c r="L11"/>
     </row>
@@ -70335,15 +70431,15 @@
       </c>
       <c r="I12" s="153" cm="1">
         <f t="array" aca="1" ref="I12" ca="1">_FV(B12,"Price")</f>
-        <v>104.57</v>
+        <v>105.65</v>
       </c>
       <c r="J12" s="129">
         <f t="shared" ca="1" si="0"/>
-        <v>0.24934289127837503</v>
+        <v>0.26224611708482681</v>
       </c>
       <c r="K12" s="170">
         <f t="shared" ca="1" si="1"/>
-        <v>124.90373499999998</v>
+        <v>131.36807500000009</v>
       </c>
       <c r="L12"/>
     </row>
@@ -70374,15 +70470,15 @@
       </c>
       <c r="I13" s="153" cm="1">
         <f t="array" aca="1" ref="I13" ca="1">_FV(B13,"Price")</f>
-        <v>97.45</v>
+        <v>95.08</v>
       </c>
       <c r="J13" s="129">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.1668803966829101</v>
+        <v>-0.18714200222279218</v>
       </c>
       <c r="K13" s="170">
         <f t="shared" ca="1" si="1"/>
-        <v>-83.611904999999979</v>
+        <v>-93.762852000000009</v>
       </c>
       <c r="L13"/>
     </row>
@@ -70413,15 +70509,15 @@
       </c>
       <c r="I14" s="155" cm="1">
         <f t="array" aca="1" ref="I14" ca="1">_FV(B14,"Price")</f>
-        <v>26.23</v>
+        <v>26.35</v>
       </c>
       <c r="J14" s="129">
         <f t="shared" ca="1" si="0"/>
-        <v>2.9030992546096587E-2</v>
+        <v>3.3738721067085253E-2</v>
       </c>
       <c r="K14" s="170">
         <f t="shared" ca="1" si="1"/>
-        <v>14.57687999999996</v>
+        <v>16.935600000000022</v>
       </c>
       <c r="L14"/>
     </row>
@@ -70491,15 +70587,15 @@
       </c>
       <c r="I16" s="157" cm="1">
         <f t="array" aca="1" ref="I16" ca="1">_FV(B16,"Price")</f>
-        <v>36.590000000000003</v>
+        <v>35.130000000000003</v>
       </c>
       <c r="J16" s="129">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.24587798845836767</v>
+        <v>-0.27596867271228359</v>
       </c>
       <c r="K16" s="170">
         <f t="shared" ca="1" si="1"/>
-        <v>-119.24999999999994</v>
+        <v>-133.84999999999997</v>
       </c>
       <c r="L16"/>
     </row>
@@ -70530,15 +70626,15 @@
       </c>
       <c r="I17" s="157" cm="1">
         <f t="array" aca="1" ref="I17" ca="1">_FV(B17,"Price")</f>
-        <v>77.959999999999994</v>
+        <v>76.38</v>
       </c>
       <c r="J17" s="129">
         <f t="shared" ca="1" si="0"/>
-        <v>0.11451036454610422</v>
+        <v>9.1922802001429479E-2</v>
       </c>
       <c r="K17" s="170">
         <f t="shared" ca="1" si="1"/>
-        <v>56.079999999999927</v>
+        <v>45.019999999999982</v>
       </c>
       <c r="L17"/>
     </row>
@@ -70569,15 +70665,15 @@
       </c>
       <c r="I18" s="157" cm="1">
         <f t="array" aca="1" ref="I18" ca="1">_FV(B18,"Price")</f>
-        <v>61.99</v>
+        <v>62.25</v>
       </c>
       <c r="J18" s="129">
         <f t="shared" ca="1" si="0"/>
-        <v>-3.05564490189768E-3</v>
+        <v>1.1257639112254791E-3</v>
       </c>
       <c r="K18" s="170">
         <f t="shared" ca="1" si="1"/>
-        <v>-1.5199999999999818</v>
+        <v>0.56000000000000227</v>
       </c>
       <c r="L18"/>
     </row>
@@ -70608,15 +70704,15 @@
       </c>
       <c r="I19" s="157" cm="1">
         <f t="array" aca="1" ref="I19" ca="1">_FV(B19,"Price")</f>
-        <v>9.7899999999999991</v>
+        <v>9.9600000000000009</v>
       </c>
       <c r="J19" s="129">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.26940298507462695</v>
+        <v>-0.25671641791044769</v>
       </c>
       <c r="K19" s="170">
         <f t="shared" ca="1" si="1"/>
-        <v>-135.02043000000003</v>
+        <v>-128.66531999999995</v>
       </c>
       <c r="L19"/>
     </row>
@@ -70647,15 +70743,15 @@
       </c>
       <c r="I20" s="209" cm="1">
         <f t="array" aca="1" ref="I20" ca="1">_FV(B20,"Price")</f>
-        <v>381.8</v>
+        <v>364.52</v>
       </c>
       <c r="J20" s="129">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.9486527707168191E-2</v>
+        <v>-7.3411286222674121E-2</v>
       </c>
       <c r="K20" s="170">
         <f t="shared" ca="1" si="1"/>
-        <v>-14.855999999999995</v>
+        <v>-36.974400000000003</v>
       </c>
       <c r="L20"/>
     </row>
@@ -70686,15 +70782,15 @@
       </c>
       <c r="I21" s="212" cm="1">
         <f t="array" aca="1" ref="I21" ca="1">_FV(B21,"Price")</f>
-        <v>20.78</v>
+        <v>20.2</v>
       </c>
       <c r="J21" s="129">
         <f t="shared" ca="1" si="0"/>
-        <v>-6.6486972147349527E-2</v>
+        <v>-9.2542677448337926E-2</v>
       </c>
       <c r="K21" s="170">
         <f t="shared" ca="1" si="1"/>
-        <v>-33.314930000000004</v>
+        <v>-46.368700000000047</v>
       </c>
     </row>
     <row r="22" spans="2:12">
@@ -70724,15 +70820,15 @@
       </c>
       <c r="I22" s="212" cm="1">
         <f t="array" aca="1" ref="I22" ca="1">_FV(B22,"Price")</f>
-        <v>66.680000000000007</v>
+        <v>64.91</v>
       </c>
       <c r="J22" s="129">
         <f t="shared" ca="1" si="0"/>
-        <v>-4.2504307869040692E-2</v>
+        <v>-6.7920735209649682E-2</v>
       </c>
       <c r="K22" s="170">
         <f t="shared" ca="1" si="1"/>
-        <v>-19.913803999999971</v>
+        <v>-32.683823000000075</v>
       </c>
     </row>
     <row r="23" spans="2:12">
@@ -70762,15 +70858,15 @@
       </c>
       <c r="I23" s="212" cm="1">
         <f t="array" aca="1" ref="I23" ca="1">_FV(B23,"Price")</f>
-        <v>100.28</v>
+        <v>98.5</v>
       </c>
       <c r="J23" s="129">
         <f t="shared" ca="1" si="0"/>
-        <v>-8.4050232374171304E-3</v>
+        <v>-2.6006130722831956E-2</v>
       </c>
       <c r="K23" s="170">
         <f t="shared" ca="1" si="1"/>
-        <v>-4.1928519999999594</v>
+        <v>-13.011149999999986</v>
       </c>
     </row>
     <row r="24" spans="2:12">
@@ -70800,15 +70896,15 @@
       </c>
       <c r="I24" s="212" cm="1">
         <f t="array" aca="1" ref="I24" ca="1">_FV(B24,"Price")</f>
-        <v>120.42</v>
+        <v>121.93</v>
       </c>
       <c r="J24" s="129">
         <f t="shared" ca="1" si="0"/>
-        <v>1.8954137755965432E-2</v>
+        <v>3.1731257403960059E-2</v>
       </c>
       <c r="K24" s="170">
         <f t="shared" ca="1" si="1"/>
-        <v>9.508547999999962</v>
+        <v>15.910041999999976</v>
       </c>
     </row>
     <row r="25" spans="2:12">
@@ -70838,15 +70934,15 @@
       </c>
       <c r="I25" s="221" cm="1">
         <f t="array" aca="1" ref="I25" ca="1">_FV(B25,"Price")</f>
-        <v>28.58</v>
+        <v>29.18</v>
       </c>
       <c r="J25" s="129">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.1902806297056831E-2</v>
+        <v>-1.3689253935660216E-3</v>
       </c>
       <c r="K25" s="170">
         <f t="shared" ca="1" si="1"/>
-        <v>-11.030196000000046</v>
+        <v>-0.7439160000000129</v>
       </c>
     </row>
     <row r="26" spans="2:12">
@@ -70876,15 +70972,15 @@
       </c>
       <c r="I26" s="221" cm="1">
         <f t="array" aca="1" ref="I26" ca="1">_FV(B26,"Price")</f>
-        <v>19.899999999999999</v>
+        <v>19.350000000000001</v>
       </c>
       <c r="J26" s="129">
         <f t="shared" ca="1" si="0"/>
-        <v>-4.784688995215311E-2</v>
+        <v>-7.4162679425837194E-2</v>
       </c>
       <c r="K26" s="170">
         <f t="shared" ca="1" si="1"/>
-        <v>-23.942300000000046</v>
+        <v>-37.154949999999985</v>
       </c>
     </row>
     <row r="27" spans="2:12">
@@ -70914,21 +71010,21 @@
       </c>
       <c r="I27" s="221" cm="1">
         <f t="array" aca="1" ref="I27" ca="1">_FV(B27,"Price")</f>
-        <v>24.16</v>
+        <v>23.76</v>
       </c>
       <c r="J27" s="129">
         <f t="shared" ca="1" si="0"/>
-        <v>-3.1275060144346473E-2</v>
+        <v>-4.7313552526062536E-2</v>
       </c>
       <c r="K27" s="170">
         <f t="shared" ca="1" si="1"/>
-        <v>-15.763312000000042</v>
+        <v>-23.797032000000002</v>
       </c>
     </row>
     <row r="30" spans="2:12" ht="13">
       <c r="K30" s="169">
         <f ca="1">SUM(K3:K27)</f>
-        <v>541.26660400000014</v>
+        <v>376.61352800000026</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
vault backup: 2024-10-09 12:58:34
</commit_message>
<xml_diff>
--- a/_system/Attachments/Portfolio Management.xlsx
+++ b/_system/Attachments/Portfolio Management.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martin/repos/tomesink/obsidian/_system/Attachments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66C4BD7F-9043-8A45-85CE-D0782C686BA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AD77512-948F-0840-B1F6-0F5AA5731634}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2000" yWindow="1200" windowWidth="34980" windowHeight="19340" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2000" yWindow="1200" windowWidth="34980" windowHeight="19340" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Stocks Performance" sheetId="1" r:id="rId1"/>
@@ -69909,7 +69909,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC8E6AFA-7BB7-D247-9FD7-C44546468350}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
@@ -69996,7 +69996,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F51CD2FE-0785-5E4C-91F5-512BDFA3DC54}">
   <dimension ref="B1:L30"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
vault backup: 2024-10-09 13:08:55
</commit_message>
<xml_diff>
--- a/_system/Attachments/Portfolio Management.xlsx
+++ b/_system/Attachments/Portfolio Management.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martin/repos/tomesink/obsidian/_system/Attachments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AD77512-948F-0840-B1F6-0F5AA5731634}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3557154-5150-854A-81A0-A3F3F821DF9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2000" yWindow="1200" windowWidth="34980" windowHeight="19340" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4669,7 +4669,7 @@
     <v>Powered by Refinitiv</v>
     <v>83.25</v>
     <v>52.770499999999998</v>
-    <v>0.52280000000000004</v>
+    <v>0.5252</v>
     <v>0.65</v>
     <v>9.9620000000000004E-3</v>
     <v>USD</v>
@@ -4706,13 +4706,13 @@
     <v>https://www.bing.com/financeapi/forcetrigger?t=a1qclh&amp;q=XNAS%3aCROX&amp;form=skydnc</v>
     <v>Learn more on Bing</v>
   </rv>
-  <rv s="3">
-    <v>5</v>
+  <rv s="1">
+    <v>0</v>
     <v>CROCS, INC. (XNAS:CROX)</v>
     <v>2</v>
-    <v>6</v>
+    <v>3</v>
     <v>Finance</v>
-    <v>7</v>
+    <v>5</v>
     <v>en-GB</v>
     <v>a1qclh</v>
     <v>268435456</v>
@@ -4720,7 +4720,7 @@
     <v>Powered by Refinitiv</v>
     <v>165.32</v>
     <v>74</v>
-    <v>1.9888999999999999</v>
+    <v>1.9883</v>
     <v>-0.93</v>
     <v>-6.8110000000000002E-3</v>
     <v>USD</v>
@@ -4743,11 +4743,10 @@
     <v>10.1989</v>
     <v>136.54</v>
     <v>135.61000000000001</v>
-    <v>136.55000000000001</v>
     <v>59385130</v>
     <v>CROX</v>
     <v>CROCS, INC. (XNAS:CROX)</v>
-    <v>682</v>
+    <v>938</v>
     <v>974515</v>
     <v>2005</v>
   </rv>
@@ -4764,7 +4763,7 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>8</v>
+    <v>5</v>
     <v>en-GB</v>
     <v>a25yfr</v>
     <v>268435456</v>
@@ -4823,7 +4822,7 @@
     <v>Powered by Refinitiv</v>
     <v>26.4</v>
     <v>16.12</v>
-    <v>1.0441</v>
+    <v>1.0448</v>
     <v>-0.1</v>
     <v>-4.6839999999999998E-3</v>
     <v>USD</v>
@@ -4866,7 +4865,7 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>8</v>
+    <v>5</v>
     <v>en-GB</v>
     <v>a1mou2</v>
     <v>268435456</v>
@@ -4874,7 +4873,7 @@
     <v>Powered by Refinitiv</v>
     <v>237.23</v>
     <v>164.07499999999999</v>
-    <v>1.2421</v>
+    <v>1.2388999999999999</v>
     <v>4.08</v>
     <v>1.8404E-2</v>
     <v>USD</v>
@@ -4900,7 +4899,7 @@
     <v>15204140000</v>
     <v>AAPL</v>
     <v>APPLE INC. (XNAS:AAPL)</v>
-    <v>30674</v>
+    <v>36076</v>
     <v>58117502</v>
     <v>1977</v>
   </rv>
@@ -4917,7 +4916,7 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>4</v>
+    <v>5</v>
     <v>en-GB</v>
     <v>a1ncgh</v>
     <v>268435456</v>
@@ -4925,7 +4924,7 @@
     <v>Powered by Refinitiv</v>
     <v>100.73</v>
     <v>50.134999999999998</v>
-    <v>0.98750000000000004</v>
+    <v>0.99209999999999998</v>
     <v>-1.55</v>
     <v>-1.5598000000000001E-2</v>
     <v>USD</v>
@@ -4968,7 +4967,7 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>4</v>
+    <v>5</v>
     <v>en-GB</v>
     <v>az23tc</v>
     <v>268435456</v>
@@ -5019,7 +5018,7 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>8</v>
+    <v>5</v>
     <v>en-GB</v>
     <v>a1v177</v>
     <v>268435456</v>
@@ -5027,7 +5026,7 @@
     <v>Powered by Refinitiv</v>
     <v>84.44</v>
     <v>38.5</v>
-    <v>1.3029999999999999</v>
+    <v>1.3095000000000001</v>
     <v>-1.36</v>
     <v>-2.0438999999999999E-2</v>
     <v>USD</v>
@@ -5065,12 +5064,12 @@
     <v>Learn more on Bing</v>
   </rv>
   <rv s="3">
-    <v>5</v>
+    <v>6</v>
     <v>Polaris Inc. (XNYS:PII)</v>
     <v>2</v>
-    <v>6</v>
+    <v>7</v>
     <v>Finance</v>
-    <v>7</v>
+    <v>8</v>
     <v>en-GB</v>
     <v>a1zvsm</v>
     <v>268435456</v>
@@ -5078,7 +5077,7 @@
     <v>Powered by Refinitiv</v>
     <v>100.91</v>
     <v>71.900000000000006</v>
-    <v>1.5048999999999999</v>
+    <v>1.5061</v>
     <v>-0.55000000000000004</v>
     <v>-6.8979999999999996E-3</v>
     <v>USD</v>
@@ -5173,7 +5172,7 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>4</v>
+    <v>5</v>
     <v>en-GB</v>
     <v>a1n1r7</v>
     <v>268435456</v>
@@ -5181,7 +5180,7 @@
     <v>Powered by Refinitiv</v>
     <v>127.3484</v>
     <v>84.35</v>
-    <v>1.2513000000000001</v>
+    <v>1.2544</v>
     <v>-1.76</v>
     <v>-1.8173999999999999E-2</v>
     <v>USD</v>
@@ -5224,7 +5223,7 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>4</v>
+    <v>5</v>
     <v>en-GB</v>
     <v>a1vuw7</v>
     <v>268435456</v>
@@ -5232,7 +5231,7 @@
     <v>Powered by Refinitiv</v>
     <v>30.07</v>
     <v>24.01</v>
-    <v>1.1493</v>
+    <v>1.1501999999999999</v>
     <v>-0.11</v>
     <v>-4.1570000000000001E-3</v>
     <v>USD</v>
@@ -5283,7 +5282,7 @@
     <v>Powered by Refinitiv</v>
     <v>13.345000000000001</v>
     <v>6.37</v>
-    <v>2.1389999999999998</v>
+    <v>2.1423999999999999</v>
     <v>0</v>
     <v>0</v>
     <v>USD</v>
@@ -5380,7 +5379,7 @@
     <v>Powered by Refinitiv</v>
     <v>80.22</v>
     <v>56.25</v>
-    <v>1.7467999999999999</v>
+    <v>1.7464999999999999</v>
     <v>-0.17</v>
     <v>-2.2209999999999999E-3</v>
     <v>USD</v>
@@ -5423,7 +5422,7 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>8</v>
+    <v>5</v>
     <v>en-GB</v>
     <v>a1xqm7</v>
     <v>268435456</v>
@@ -5431,7 +5430,7 @@
     <v>Powered by Refinitiv</v>
     <v>69.75</v>
     <v>34.96</v>
-    <v>0.96130000000000004</v>
+    <v>0.96440000000000003</v>
     <v>-0.21</v>
     <v>-3.362E-3</v>
     <v>USD</v>
@@ -5519,13 +5518,13 @@
     <v>https://www.bing.com/financeapi/forcetrigger?t=a24war&amp;q=XNAS%3aULTA&amp;form=skydnc</v>
     <v>Learn more on Bing</v>
   </rv>
-  <rv s="3">
-    <v>5</v>
+  <rv s="1">
+    <v>0</v>
     <v>ULTA BEAUTY, INC. (XNAS:ULTA)</v>
     <v>2</v>
-    <v>6</v>
+    <v>3</v>
     <v>Finance</v>
-    <v>7</v>
+    <v>5</v>
     <v>en-GB</v>
     <v>a24war</v>
     <v>268435456</v>
@@ -5533,7 +5532,7 @@
     <v>Powered by Refinitiv</v>
     <v>574.76</v>
     <v>318.17</v>
-    <v>1.3254999999999999</v>
+    <v>1.3259000000000001</v>
     <v>-5.49</v>
     <v>-1.4836999999999999E-2</v>
     <v>USD</v>
@@ -5556,11 +5555,10 @@
     <v>14.6371</v>
     <v>370.01</v>
     <v>364.52</v>
-    <v>365</v>
     <v>47114730</v>
     <v>ULTA</v>
     <v>ULTA BEAUTY, INC. (XNAS:ULTA)</v>
-    <v>687</v>
+    <v>917</v>
     <v>1220125</v>
     <v>2016</v>
   </rv>
@@ -5577,7 +5575,7 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>4</v>
+    <v>5</v>
     <v>en-GB</v>
     <v>a1vehw</v>
     <v>268435456</v>
@@ -5585,7 +5583,7 @@
     <v>Powered by Refinitiv</v>
     <v>31.85</v>
     <v>18.899999999999999</v>
-    <v>1.9723999999999999</v>
+    <v>1.9737</v>
     <v>-0.18</v>
     <v>-8.8319999999999996E-3</v>
     <v>USD</v>
@@ -5628,7 +5626,7 @@
     <v>2</v>
     <v>3</v>
     <v>Finance</v>
-    <v>4</v>
+    <v>5</v>
     <v>en-GB</v>
     <v>a1z3ec</v>
     <v>268435456</v>
@@ -5636,7 +5634,7 @@
     <v>Powered by Refinitiv</v>
     <v>87.32</v>
     <v>54.8</v>
-    <v>0.5917</v>
+    <v>0.59089999999999998</v>
     <v>-1.1299999999999999</v>
     <v>-1.7111000000000001E-2</v>
     <v>USD</v>
@@ -5673,13 +5671,13 @@
     <v>https://www.bing.com/financeapi/forcetrigger?t=a1mt9c&amp;q=XNAS%3aACLS&amp;form=skydnc</v>
     <v>Learn more on Bing</v>
   </rv>
-  <rv s="3">
-    <v>5</v>
+  <rv s="1">
+    <v>0</v>
     <v>AXCELIS TECHNOLOGIES, INC. (XNAS:ACLS)</v>
     <v>2</v>
-    <v>6</v>
+    <v>3</v>
     <v>Finance</v>
-    <v>7</v>
+    <v>5</v>
     <v>en-GB</v>
     <v>a1mt9c</v>
     <v>268435456</v>
@@ -5687,7 +5685,7 @@
     <v>Powered by Refinitiv</v>
     <v>170.9692</v>
     <v>93.77</v>
-    <v>1.5809</v>
+    <v>1.5790999999999999</v>
     <v>-0.44</v>
     <v>-4.4469999999999996E-3</v>
     <v>USD</v>
@@ -5710,11 +5708,10 @@
     <v>13.570499999999999</v>
     <v>98.94</v>
     <v>98.5</v>
-    <v>99</v>
     <v>32617590</v>
     <v>ACLS</v>
     <v>AXCELIS TECHNOLOGIES, INC. (XNAS:ACLS)</v>
-    <v>368</v>
+    <v>383</v>
     <v>658199</v>
     <v>1995</v>
   </rv>
@@ -5725,13 +5722,13 @@
     <v>https://www.bing.com/financeapi/forcetrigger?t=a1retc&amp;q=XNYS%3aDELL&amp;form=skydnc</v>
     <v>Learn more on Bing</v>
   </rv>
-  <rv s="3">
-    <v>5</v>
+  <rv s="1">
+    <v>0</v>
     <v>DELL TECHNOLOGIES INC. (XNYS:DELL)</v>
     <v>2</v>
-    <v>6</v>
+    <v>3</v>
     <v>Finance</v>
-    <v>7</v>
+    <v>5</v>
     <v>en-GB</v>
     <v>a1retc</v>
     <v>268435456</v>
@@ -5739,7 +5736,7 @@
     <v>Powered by Refinitiv</v>
     <v>179.7</v>
     <v>63.9</v>
-    <v>0.89549999999999996</v>
+    <v>0.89400000000000002</v>
     <v>2.84</v>
     <v>2.3847999999999998E-2</v>
     <v>USD</v>
@@ -5762,11 +5759,10 @@
     <v>22.435400000000001</v>
     <v>119.09</v>
     <v>121.93</v>
-    <v>122.1</v>
     <v>701996500</v>
     <v>DELL</v>
     <v>DELL TECHNOLOGIES INC. (XNYS:DELL)</v>
-    <v>8278</v>
+    <v>10143</v>
     <v>13468448</v>
     <v>2013</v>
   </rv>
@@ -5783,7 +5779,7 @@
     <v>2</v>
     <v>12</v>
     <v>Finance</v>
-    <v>8</v>
+    <v>5</v>
     <v>en-GB</v>
     <v>a1zqnm</v>
     <v>268435456</v>
@@ -5791,7 +5787,7 @@
     <v>Powered by Refinitiv</v>
     <v>33.92</v>
     <v>25.2</v>
-    <v>0.64529999999999998</v>
+    <v>0.64739999999999998</v>
     <v>-0.02</v>
     <v>-6.8490000000000001E-4</v>
     <v>USD</v>
@@ -5816,7 +5812,7 @@
     <v>5666695000</v>
     <v>PFE</v>
     <v>PFIZER INC. (XNYS:PFE)</v>
-    <v>27485</v>
+    <v>31140</v>
     <v>29902174</v>
     <v>1942</v>
   </rv>
@@ -5841,7 +5837,7 @@
     <v>Powered by Refinitiv</v>
     <v>30.32</v>
     <v>18.945</v>
-    <v>1.4094</v>
+    <v>1.4118999999999999</v>
     <v>-0.23</v>
     <v>-1.1747E-2</v>
     <v>USD</v>
@@ -5892,7 +5888,7 @@
     <v>Powered by Refinitiv</v>
     <v>26.15</v>
     <v>20.190000000000001</v>
-    <v>1.1484000000000001</v>
+    <v>1.1487000000000001</v>
     <v>-0.05</v>
     <v>-2.0999999999999999E-3</v>
     <v>USD</v>
@@ -6340,6 +6336,13 @@
       <v>Source: Nasdaq</v>
       <v>GMT</v>
     </spb>
+    <spb s="4">
+      <v>Real-Time Nasdaq Last Sale</v>
+      <v>from previous close</v>
+      <v>from previous close</v>
+      <v>Source: Nasdaq Last Sale</v>
+      <v>GMT</v>
+    </spb>
     <spb s="0">
       <v>1</v>
       <v>Name</v>
@@ -6375,13 +6378,6 @@
       <v>Source: Nasdaq</v>
       <v>GMT</v>
       <v>Delayed 15 minutes</v>
-    </spb>
-    <spb s="4">
-      <v>Real-Time Nasdaq Last Sale</v>
-      <v>from previous close</v>
-      <v>from previous close</v>
-      <v>Source: Nasdaq Last Sale</v>
-      <v>GMT</v>
     </spb>
     <spb s="7">
       <v>2</v>
@@ -69997,7 +69993,7 @@
   <dimension ref="B1:L30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="J33" sqref="J33"/>
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>

</xml_diff>